<commit_message>
implemented movimients controller sendEmail methodo +
</commit_message>
<xml_diff>
--- a/WSafe/WSafe.Web/SG-SST/2. HACER/2022/3.1.1/PERFIL SOCIODEMOGRAFICO 2022.xlsx
+++ b/WSafe/WSafe.Web/SG-SST/2. HACER/2022/3.1.1/PERFIL SOCIODEMOGRAFICO 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WSafe\WSafe.Web\SG-SST\2. HACER\2022\3.1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9046E31C-1F97-4300-B2C2-90B06F327403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2889337-D703-4FF0-BB0D-417550233AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="624" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PERFIL SOCIODEMOGRAFICO" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="130">
   <si>
     <t>CÉDULA</t>
   </si>
@@ -424,32 +424,17 @@
  COCINA CAFÉ Y PAN</t>
   </si>
   <si>
-    <t>Francisco Puerta Cardona</t>
-  </si>
-  <si>
-    <t>Ingeniero de sistemas</t>
-  </si>
-  <si>
-    <t>Olga Patricia Bernal</t>
-  </si>
-  <si>
-    <t>flpuertacardon@gmail.com</t>
-  </si>
-  <si>
-    <t>Calle 58 sur # 42-99</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>deporte, entrenamiento en SST</t>
+    <t>FRANCISCO PUERTA</t>
+  </si>
+  <si>
+    <t>INGENIERO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,6 +536,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -721,7 +712,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -789,6 +780,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -814,13 +808,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -828,7 +825,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -844,7 +841,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -868,23 +865,23 @@
     <xf numFmtId="3" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="16" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -899,7 +896,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -933,6 +930,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -943,15 +949,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1134,10 +1131,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2365,7 +2362,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2377,7 +2374,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2716,10 +2713,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3024,7 +3021,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3214,10 +3211,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5386,8 +5383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC238"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6560,49 +6557,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72"/>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
+      <c r="A1" s="74"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
       <c r="N1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="O1" s="39">
+      <c r="O1" s="41">
         <f ca="1">TODAY()</f>
-        <v>44884</v>
+        <v>44895</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="5" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="77"/>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="78"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="80"/>
     </row>
     <row r="3" spans="1:29" s="8" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -6697,16 +6694,36 @@
       <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="31">
+        <v>71579486</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="24">
+        <v>22011</v>
+      </c>
+      <c r="F4" s="25">
+        <v>44895</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="L4" s="9"/>
       <c r="M4" s="26"/>
       <c r="N4" s="26"/>
@@ -6718,27 +6735,27 @@
       <c r="T4" s="26"/>
       <c r="U4" s="11"/>
       <c r="V4" s="11"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="65"/>
-      <c r="Y4" s="27"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="28"/>
       <c r="Z4" s="9"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
     </row>
     <row r="5" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>2</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="30"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="23"/>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="26"/>
@@ -6751,27 +6768,27 @@
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
       <c r="V5" s="11"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="27"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="68"/>
+      <c r="Y5" s="28"/>
       <c r="Z5" s="9"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="67"/>
+      <c r="AA5" s="36"/>
+      <c r="AB5" s="36"/>
+      <c r="AC5" s="69"/>
     </row>
     <row r="6" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>3</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="30"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="23"/>
       <c r="E6" s="24"/>
       <c r="F6" s="25"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="32"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="33"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="26"/>
@@ -6784,27 +6801,27 @@
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="27"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="28"/>
       <c r="Z6" s="9"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="67"/>
+      <c r="AA6" s="36"/>
+      <c r="AB6" s="36"/>
+      <c r="AC6" s="69"/>
     </row>
     <row r="7" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>4</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="57"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="58"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="33"/>
+      <c r="J7" s="34"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="11"/>
@@ -6817,27 +6834,27 @@
       <c r="T7" s="11"/>
       <c r="U7" s="11"/>
       <c r="V7" s="11"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="68"/>
-      <c r="Y7" s="33"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="70"/>
+      <c r="Y7" s="34"/>
       <c r="Z7" s="9"/>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="35"/>
-      <c r="AC7" s="67"/>
+      <c r="AA7" s="36"/>
+      <c r="AB7" s="36"/>
+      <c r="AC7" s="69"/>
     </row>
     <row r="8" spans="1:29" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>5</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="37"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="56"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="25"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="26"/>
@@ -6850,27 +6867,27 @@
       <c r="T8" s="26"/>
       <c r="U8" s="11"/>
       <c r="V8" s="11"/>
-      <c r="W8" s="34"/>
-      <c r="X8" s="65"/>
-      <c r="Y8" s="27"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="28"/>
       <c r="Z8" s="9"/>
-      <c r="AA8" s="35"/>
-      <c r="AB8" s="35"/>
-      <c r="AC8" s="67"/>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="69"/>
     </row>
     <row r="9" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>6</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="37"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="56"/>
+      <c r="E9" s="58"/>
       <c r="F9" s="25"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="26"/>
@@ -6883,27 +6900,27 @@
       <c r="T9" s="26"/>
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
-      <c r="W9" s="34"/>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="27"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="28"/>
       <c r="Z9" s="9"/>
-      <c r="AA9" s="35"/>
-      <c r="AB9" s="35"/>
-      <c r="AC9" s="67"/>
+      <c r="AA9" s="36"/>
+      <c r="AB9" s="36"/>
+      <c r="AC9" s="69"/>
     </row>
     <row r="10" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>7</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="37"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="56"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="25"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="26"/>
@@ -6916,27 +6933,27 @@
       <c r="T10" s="26"/>
       <c r="U10" s="11"/>
       <c r="V10" s="11"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="27"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="28"/>
       <c r="Z10" s="9"/>
-      <c r="AA10" s="35"/>
-      <c r="AB10" s="35"/>
-      <c r="AC10" s="67"/>
+      <c r="AA10" s="36"/>
+      <c r="AB10" s="36"/>
+      <c r="AC10" s="69"/>
     </row>
     <row r="11" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>8</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="57"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="64"/>
+      <c r="E11" s="66"/>
       <c r="F11" s="10"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="33"/>
+      <c r="J11" s="34"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="11"/>
@@ -6949,27 +6966,27 @@
       <c r="T11" s="11"/>
       <c r="U11" s="11"/>
       <c r="V11" s="11"/>
-      <c r="W11" s="31"/>
+      <c r="W11" s="32"/>
       <c r="X11" s="11"/>
-      <c r="Y11" s="33"/>
+      <c r="Y11" s="34"/>
       <c r="Z11" s="9"/>
-      <c r="AA11" s="67"/>
-      <c r="AB11" s="35"/>
-      <c r="AC11" s="67"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="36"/>
+      <c r="AC11" s="69"/>
     </row>
     <row r="12" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>9</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="57"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="64"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="10"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="33"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="11"/>
@@ -6982,23 +6999,23 @@
       <c r="T12" s="11"/>
       <c r="U12" s="11"/>
       <c r="V12" s="11"/>
-      <c r="W12" s="31"/>
-      <c r="X12" s="68"/>
-      <c r="Y12" s="33"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="70"/>
+      <c r="Y12" s="34"/>
       <c r="Z12" s="9"/>
-      <c r="AA12" s="70"/>
+      <c r="AA12" s="72"/>
       <c r="AB12" s="12"/>
-      <c r="AC12" s="70"/>
+      <c r="AC12" s="72"/>
     </row>
     <row r="13" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>10</v>
       </c>
       <c r="B13" s="9"/>
-      <c r="C13" s="57"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="58"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -7011,13 +7028,13 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
-      <c r="S13" s="33"/>
+      <c r="S13" s="34"/>
       <c r="T13" s="11"/>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="68"/>
-      <c r="Y13" s="33"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="70"/>
+      <c r="Y13" s="34"/>
       <c r="Z13" s="9"/>
       <c r="AA13" s="12"/>
       <c r="AB13" s="12"/>
@@ -7028,10 +7045,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="57"/>
+      <c r="C14" s="59"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -7048,9 +7065,9 @@
       <c r="T14" s="11"/>
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
-      <c r="W14" s="31"/>
+      <c r="W14" s="32"/>
       <c r="X14" s="11"/>
-      <c r="Y14" s="33"/>
+      <c r="Y14" s="34"/>
       <c r="Z14" s="9"/>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
@@ -7061,10 +7078,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="57"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -7081,9 +7098,9 @@
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
-      <c r="W15" s="31"/>
+      <c r="W15" s="32"/>
       <c r="X15" s="11"/>
-      <c r="Y15" s="33"/>
+      <c r="Y15" s="34"/>
       <c r="Z15" s="9"/>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
@@ -7094,10 +7111,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="9"/>
-      <c r="C16" s="57"/>
+      <c r="C16" s="59"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -7114,9 +7131,9 @@
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="68"/>
-      <c r="Y16" s="33"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="70"/>
+      <c r="Y16" s="34"/>
       <c r="Z16" s="9"/>
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
@@ -7127,10 +7144,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="57"/>
+      <c r="C17" s="59"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -7147,9 +7164,9 @@
       <c r="T17" s="11"/>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="71"/>
-      <c r="Y17" s="33"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="73"/>
+      <c r="Y17" s="34"/>
       <c r="Z17" s="9"/>
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
@@ -7160,10 +7177,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="9"/>
-      <c r="C18" s="57"/>
+      <c r="C18" s="59"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -7180,9 +7197,9 @@
       <c r="T18" s="11"/>
       <c r="U18" s="11"/>
       <c r="V18" s="11"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="68"/>
-      <c r="Y18" s="33"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="70"/>
+      <c r="Y18" s="34"/>
       <c r="Z18" s="9"/>
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
@@ -7193,14 +7210,14 @@
         <v>16</v>
       </c>
       <c r="B19" s="9"/>
-      <c r="C19" s="30"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="23"/>
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="26"/>
@@ -7213,13 +7230,13 @@
       <c r="T19" s="11"/>
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
-      <c r="W19" s="34"/>
-      <c r="X19" s="55"/>
-      <c r="Y19" s="27"/>
+      <c r="W19" s="35"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="28"/>
       <c r="Z19" s="9"/>
-      <c r="AA19" s="35"/>
-      <c r="AB19" s="35"/>
-      <c r="AC19" s="67"/>
+      <c r="AA19" s="36"/>
+      <c r="AB19" s="36"/>
+      <c r="AC19" s="69"/>
     </row>
     <row r="20" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
@@ -7251,89 +7268,89 @@
       <c r="AA20" s="14"/>
     </row>
     <row r="21" spans="1:29" ht="15" x14ac:dyDescent="0.25">
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="79">
+      <c r="D21" s="76"/>
+      <c r="E21" s="81">
         <v>43614</v>
       </c>
-      <c r="F21" s="80"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
-      <c r="N21" s="75"/>
+      <c r="F21" s="82"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="77"/>
+      <c r="N21" s="77"/>
       <c r="AA21" s="4"/>
     </row>
     <row r="22" spans="1:29" ht="15" x14ac:dyDescent="0.25">
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="79">
+      <c r="D22" s="76"/>
+      <c r="E22" s="81">
         <v>44046</v>
       </c>
-      <c r="F22" s="80"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="75"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="75"/>
+      <c r="F22" s="82"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="77"/>
+      <c r="M22" s="77"/>
+      <c r="N22" s="77"/>
       <c r="AA22" s="4"/>
     </row>
     <row r="147" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E147" s="48" t="s">
+      <c r="E147" s="50" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="148" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E148" s="48" t="s">
+      <c r="E148" s="50" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="149" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E149" s="48" t="s">
+      <c r="E149" s="50" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="150" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E150" s="48" t="s">
+      <c r="E150" s="50" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="151" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E151" s="48" t="s">
+      <c r="E151" s="50" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="152" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E152" s="48" t="s">
+      <c r="E152" s="50" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="153" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E153" s="48" t="s">
+      <c r="E153" s="50" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="156" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E156" s="47" t="s">
+      <c r="E156" s="49" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="157" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E157" s="47" t="s">
+      <c r="E157" s="49" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="158" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E158" s="47" t="s">
+      <c r="E158" s="49" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="159" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E159" s="47" t="s">
+      <c r="E159" s="49" t="s">
         <v>110</v>
       </c>
     </row>
@@ -7341,32 +7358,32 @@
       <c r="E160" s="15"/>
     </row>
     <row r="161" spans="5:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="E161" s="50" t="s">
+      <c r="E161" s="52" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="162" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E162" s="50" t="s">
+      <c r="E162" s="52" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="163" spans="5:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="E163" s="51" t="s">
+      <c r="E163" s="53" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="164" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E164" s="50" t="s">
+      <c r="E164" s="52" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="165" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E165" s="50" t="s">
+      <c r="E165" s="52" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="166" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E166" s="47" t="s">
+      <c r="E166" s="49" t="s">
         <v>115</v>
       </c>
     </row>
@@ -7374,27 +7391,27 @@
       <c r="E167" s="15"/>
     </row>
     <row r="168" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E168" s="48" t="s">
+      <c r="E168" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="169" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E169" s="48" t="s">
+      <c r="E169" s="50" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="170" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E170" s="48" t="s">
+      <c r="E170" s="50" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="171" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E171" s="48" t="s">
+      <c r="E171" s="50" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="172" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E172" s="48" t="s">
+      <c r="E172" s="50" t="s">
         <v>42</v>
       </c>
     </row>
@@ -7402,17 +7419,17 @@
       <c r="E173" s="15"/>
     </row>
     <row r="174" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E174" s="48" t="s">
+      <c r="E174" s="50" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="175" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E175" s="48" t="s">
+      <c r="E175" s="50" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="176" spans="5:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="E176" s="48" t="s">
+      <c r="E176" s="50" t="s">
         <v>45</v>
       </c>
     </row>
@@ -7420,37 +7437,37 @@
       <c r="E177" s="15"/>
     </row>
     <row r="178" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E178" s="52" t="s">
+      <c r="E178" s="54" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="179" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E179" s="52" t="s">
+      <c r="E179" s="54" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="180" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E180" s="52" t="s">
+      <c r="E180" s="54" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="181" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E181" s="48" t="s">
+      <c r="E181" s="50" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="182" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E182" s="52" t="s">
+      <c r="E182" s="54" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="183" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E183" s="52" t="s">
+      <c r="E183" s="54" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="184" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E184" s="52" t="s">
+      <c r="E184" s="54" t="s">
         <v>104</v>
       </c>
     </row>
@@ -7458,22 +7475,22 @@
       <c r="E185" s="15"/>
     </row>
     <row r="186" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E186" s="48" t="s">
+      <c r="E186" s="50" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="187" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E187" s="48" t="s">
+      <c r="E187" s="50" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="188" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E188" s="48" t="s">
+      <c r="E188" s="50" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="189" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E189" s="52" t="s">
+      <c r="E189" s="54" t="s">
         <v>105</v>
       </c>
     </row>
@@ -7481,32 +7498,32 @@
       <c r="E190" s="15"/>
     </row>
     <row r="191" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E191" s="48" t="s">
+      <c r="E191" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="192" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E192" s="48" t="s">
+      <c r="E192" s="50" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="193" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E193" s="48" t="s">
+      <c r="E193" s="50" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="194" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E194" s="48" t="s">
+      <c r="E194" s="50" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="195" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E195" s="48" t="s">
+      <c r="E195" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="196" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E196" s="48" t="s">
+      <c r="E196" s="50" t="s">
         <v>57</v>
       </c>
     </row>
@@ -7514,42 +7531,42 @@
       <c r="E197" s="15"/>
     </row>
     <row r="198" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E198" s="48" t="s">
+      <c r="E198" s="50" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="199" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E199" s="48" t="s">
+      <c r="E199" s="50" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="200" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E200" s="48" t="s">
+      <c r="E200" s="50" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="201" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E201" s="48" t="s">
+      <c r="E201" s="50" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="202" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E202" s="48" t="s">
+      <c r="E202" s="50" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="203" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E203" s="48" t="s">
+      <c r="E203" s="50" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="204" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E204" s="48" t="s">
+      <c r="E204" s="50" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="205" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E205" s="48" t="s">
+      <c r="E205" s="50" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7557,22 +7574,22 @@
       <c r="E206" s="15"/>
     </row>
     <row r="207" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E207" s="48" t="s">
+      <c r="E207" s="50" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="208" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E208" s="48" t="s">
+      <c r="E208" s="50" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="209" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E209" s="48" t="s">
+      <c r="E209" s="50" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="210" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E210" s="48" t="s">
+      <c r="E210" s="50" t="s">
         <v>70</v>
       </c>
     </row>
@@ -7580,22 +7597,22 @@
       <c r="E211" s="15"/>
     </row>
     <row r="212" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E212" s="48" t="s">
+      <c r="E212" s="50" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="213" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E213" s="48" t="s">
+      <c r="E213" s="50" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="214" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E214" s="48" t="s">
+      <c r="E214" s="50" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="215" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E215" s="48" t="s">
+      <c r="E215" s="50" t="s">
         <v>78</v>
       </c>
     </row>
@@ -7603,37 +7620,37 @@
       <c r="E216" s="15"/>
     </row>
     <row r="217" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E217" s="48" t="s">
+      <c r="E217" s="50" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="218" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E218" s="48" t="s">
+      <c r="E218" s="50" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="219" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E219" s="48" t="s">
+      <c r="E219" s="50" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="220" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E220" s="48" t="s">
+      <c r="E220" s="50" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="221" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E221" s="48" t="s">
+      <c r="E221" s="50" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="222" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E222" s="48" t="s">
+      <c r="E222" s="50" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="223" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E223" s="48" t="s">
+      <c r="E223" s="50" t="s">
         <v>84</v>
       </c>
     </row>
@@ -7641,32 +7658,32 @@
       <c r="E224" s="15"/>
     </row>
     <row r="225" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E225" s="53" t="s">
+      <c r="E225" s="55" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="226" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E226" s="53" t="s">
+      <c r="E226" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="227" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E227" s="53" t="s">
+      <c r="E227" s="55" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="228" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E228" s="53" t="s">
+      <c r="E228" s="55" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="229" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E229" s="53" t="s">
+      <c r="E229" s="55" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="230" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E230" s="53" t="s">
+      <c r="E230" s="55" t="s">
         <v>116</v>
       </c>
     </row>
@@ -7674,17 +7691,17 @@
       <c r="E231" s="15"/>
     </row>
     <row r="232" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E232" s="48" t="s">
+      <c r="E232" s="50" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="233" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E233" s="48" t="s">
+      <c r="E233" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="234" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E234" s="48" t="s">
+      <c r="E234" s="50" t="s">
         <v>90</v>
       </c>
     </row>
@@ -7692,17 +7709,17 @@
       <c r="E235" s="15"/>
     </row>
     <row r="236" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E236" s="48" t="s">
+      <c r="E236" s="50" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="237" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E237" s="48" t="s">
+      <c r="E237" s="50" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="238" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E238" s="48" t="s">
+      <c r="E238" s="50" t="s">
         <v>48</v>
       </c>
     </row>
@@ -7861,99 +7878,99 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28" style="40" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="11.42578125" style="40"/>
-    <col min="10" max="10" width="39.42578125" style="40" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="40" customWidth="1"/>
-    <col min="12" max="16" width="11.42578125" style="40"/>
-    <col min="17" max="17" width="29.42578125" style="40" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" style="40" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="40"/>
+    <col min="1" max="1" width="28" style="42" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="11.42578125" style="42"/>
+    <col min="10" max="10" width="39.42578125" style="42" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="42" customWidth="1"/>
+    <col min="12" max="16" width="11.42578125" style="42"/>
+    <col min="17" max="17" width="29.42578125" style="42" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" style="42" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="42"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="83" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="84"/>
-      <c r="R3" s="46"/>
+      <c r="K3" s="89"/>
+      <c r="R3" s="48"/>
     </row>
     <row r="4" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
       <c r="J4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z32,'GENERO Y CENTRO Y AREA TRABAJO'!J4)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="47"/>
+      <c r="R4" s="49"/>
     </row>
     <row r="5" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z19,'GENERO Y CENTRO Y AREA TRABAJO'!A5)</f>
         <v>0</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z33,'GENERO Y CENTRO Y AREA TRABAJO'!J5)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="47"/>
+      <c r="R5" s="49"/>
     </row>
     <row r="6" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z20,'GENERO Y CENTRO Y AREA TRABAJO'!A6)</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z34,'GENERO Y CENTRO Y AREA TRABAJO'!J6)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="47"/>
+      <c r="R6" s="49"/>
     </row>
     <row r="7" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
@@ -7961,206 +7978,206 @@
       </c>
       <c r="B7" s="22">
         <f>SUM(B5:B6)</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
       <c r="J7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z35,'GENERO Y CENTRO Y AREA TRABAJO'!J7)</f>
         <v>0</v>
       </c>
-      <c r="R7" s="47"/>
+      <c r="R7" s="49"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
       <c r="J8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z36,'GENERO Y CENTRO Y AREA TRABAJO'!J8)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="47"/>
+      <c r="R8" s="49"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z37,'GENERO Y CENTRO Y AREA TRABAJO'!J9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z38,'GENERO Y CENTRO Y AREA TRABAJO'!J10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K11" s="22">
         <f>SUM(K4:K10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J15" s="81" t="s">
+      <c r="J15" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="K15" s="81"/>
+      <c r="K15" s="86"/>
     </row>
     <row r="16" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="81"/>
-      <c r="J16" s="42" t="s">
+      <c r="B16" s="86"/>
+      <c r="J16" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z44,'GENERO Y CENTRO Y AREA TRABAJO'!J16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z31,'GENERO Y CENTRO Y AREA TRABAJO'!A17)</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z45,'GENERO Y CENTRO Y AREA TRABAJO'!J17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z32,'GENERO Y CENTRO Y AREA TRABAJO'!A18)</f>
         <v>0</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z46,'GENERO Y CENTRO Y AREA TRABAJO'!J18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z33,'GENERO Y CENTRO Y AREA TRABAJO'!A19)</f>
         <v>0</v>
       </c>
-      <c r="J19" s="42" t="s">
+      <c r="J19" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="K19" s="28">
+      <c r="K19" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z47,'GENERO Y CENTRO Y AREA TRABAJO'!J19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z34,'GENERO Y CENTRO Y AREA TRABAJO'!A20)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="42" t="s">
+      <c r="J20" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="K20" s="28">
+      <c r="K20" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z48,'GENERO Y CENTRO Y AREA TRABAJO'!J20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="J21" s="28" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="J21" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="K21" s="28">
+      <c r="K21" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z49,'GENERO Y CENTRO Y AREA TRABAJO'!J21)</f>
         <v>0</v>
       </c>
@@ -8171,22 +8188,22 @@
       </c>
       <c r="B22" s="22">
         <f>SUM(B17:B21)</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J25" s="28"/>
-      <c r="K25" s="28">
+      <c r="J25" s="29"/>
+      <c r="K25" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z53,'GENERO Y CENTRO Y AREA TRABAJO'!J25)</f>
         <v>0</v>
       </c>
@@ -8197,24 +8214,24 @@
       </c>
       <c r="K26" s="22">
         <f>SUM(K16:K25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J28" s="81" t="s">
+      <c r="J28" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="K28" s="81"/>
+      <c r="K28" s="86"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="81" t="s">
+      <c r="A29" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="81"/>
+      <c r="B29" s="86"/>
       <c r="J29" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K29" s="28">
+      <c r="K29" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA43,'GENERO Y CENTRO Y AREA TRABAJO'!J29)</f>
         <v>0</v>
       </c>
@@ -8223,14 +8240,14 @@
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z44,'GENERO Y CENTRO Y AREA TRABAJO'!A30)</f>
         <v>0</v>
       </c>
       <c r="J30" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K30" s="28">
+      <c r="K30" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA44,'GENERO Y CENTRO Y AREA TRABAJO'!J30)</f>
         <v>0</v>
       </c>
@@ -8239,14 +8256,14 @@
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B31" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z45,'GENERO Y CENTRO Y AREA TRABAJO'!A31)</f>
         <v>0</v>
       </c>
       <c r="J31" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K31" s="28">
+      <c r="K31" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA45,'GENERO Y CENTRO Y AREA TRABAJO'!J31)</f>
         <v>0</v>
       </c>
@@ -8255,7 +8272,7 @@
       <c r="A32" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z46,'GENERO Y CENTRO Y AREA TRABAJO'!A32)</f>
         <v>0</v>
       </c>
@@ -8271,7 +8288,7 @@
       <c r="A33" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="28">
+      <c r="B33" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z47,'GENERO Y CENTRO Y AREA TRABAJO'!A33)</f>
         <v>0</v>
       </c>
@@ -8280,9 +8297,9 @@
       <c r="A34" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="28">
+      <c r="B34" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z48,'GENERO Y CENTRO Y AREA TRABAJO'!A34)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -8291,63 +8308,63 @@
       </c>
       <c r="B35" s="22">
         <f>SUM(B30:B34)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="81" t="s">
+      <c r="A45" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="81"/>
-      <c r="J45" s="81" t="s">
+      <c r="B45" s="86"/>
+      <c r="J45" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="K45" s="81"/>
+      <c r="K45" s="86"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z58,'GENERO Y CENTRO Y AREA TRABAJO'!A46)</f>
         <v>0</v>
       </c>
       <c r="J46" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="K46" s="28">
+      <c r="K46" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA60,'GENERO Y CENTRO Y AREA TRABAJO'!J46)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="28">
+      <c r="B47" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z59,'GENERO Y CENTRO Y AREA TRABAJO'!A47)</f>
         <v>0</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K47" s="28">
+      <c r="K47" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA61,'GENERO Y CENTRO Y AREA TRABAJO'!J47)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="28">
+      <c r="B48" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z60,'GENERO Y CENTRO Y AREA TRABAJO'!A48)</f>
         <v>0</v>
       </c>
       <c r="J48" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K48" s="28">
+      <c r="K48" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA62,'GENERO Y CENTRO Y AREA TRABAJO'!J48)</f>
         <v>0</v>
       </c>
@@ -8356,23 +8373,23 @@
       <c r="A49" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="28">
+      <c r="B49" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z61,'GENERO Y CENTRO Y AREA TRABAJO'!A49)</f>
         <v>0</v>
       </c>
-      <c r="J49" s="29" t="s">
+      <c r="J49" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="K49" s="28">
+      <c r="K49" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA63,'GENERO Y CENTRO Y AREA TRABAJO'!J49)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="28">
+      <c r="B50" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z62,'GENERO Y CENTRO Y AREA TRABAJO'!A50)</f>
         <v>0</v>
       </c>
@@ -8385,19 +8402,19 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="28">
+      <c r="B51" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z63,'GENERO Y CENTRO Y AREA TRABAJO'!A51)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="28">
+      <c r="B52" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z64,'GENERO Y CENTRO Y AREA TRABAJO'!A52)</f>
         <v>0</v>
       </c>
@@ -8412,27 +8429,27 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="81" t="s">
+      <c r="A61" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="81"/>
-      <c r="J61" s="81" t="s">
+      <c r="B61" s="86"/>
+      <c r="J61" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="K61" s="81"/>
+      <c r="K61" s="86"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B62" s="28">
+      <c r="B62" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z74,'GENERO Y CENTRO Y AREA TRABAJO'!A62)</f>
         <v>0</v>
       </c>
       <c r="J62" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="K62" s="28">
+      <c r="K62" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA74,'GENERO Y CENTRO Y AREA TRABAJO'!J62)</f>
         <v>0</v>
       </c>
@@ -8441,14 +8458,14 @@
       <c r="A63" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B63" s="28">
+      <c r="B63" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z75,'GENERO Y CENTRO Y AREA TRABAJO'!A63)</f>
         <v>0</v>
       </c>
       <c r="J63" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="K63" s="28">
+      <c r="K63" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA75,'GENERO Y CENTRO Y AREA TRABAJO'!J63)</f>
         <v>0</v>
       </c>
@@ -8457,14 +8474,14 @@
       <c r="A64" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="28">
+      <c r="B64" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z76,'GENERO Y CENTRO Y AREA TRABAJO'!A64)</f>
         <v>0</v>
       </c>
       <c r="J64" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="K64" s="28">
+      <c r="K64" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA76,'GENERO Y CENTRO Y AREA TRABAJO'!J64)</f>
         <v>0</v>
       </c>
@@ -8473,14 +8490,14 @@
       <c r="A65" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="28">
+      <c r="B65" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z77,'GENERO Y CENTRO Y AREA TRABAJO'!A65)</f>
         <v>0</v>
       </c>
       <c r="J65" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="K65" s="28">
+      <c r="K65" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA77,'GENERO Y CENTRO Y AREA TRABAJO'!J65)</f>
         <v>0</v>
       </c>
@@ -8489,14 +8506,14 @@
       <c r="A66" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B66" s="28">
+      <c r="B66" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z78,'GENERO Y CENTRO Y AREA TRABAJO'!A66)</f>
         <v>0</v>
       </c>
       <c r="J66" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K66" s="28">
+      <c r="K66" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA78,'GENERO Y CENTRO Y AREA TRABAJO'!J66)</f>
         <v>0</v>
       </c>
@@ -8505,14 +8522,14 @@
       <c r="A67" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="28">
+      <c r="B67" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z79,'GENERO Y CENTRO Y AREA TRABAJO'!A67)</f>
         <v>0</v>
       </c>
       <c r="J67" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K67" s="28">
+      <c r="K67" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA79,'GENERO Y CENTRO Y AREA TRABAJO'!J67)</f>
         <v>0</v>
       </c>
@@ -8528,7 +8545,7 @@
       <c r="J68" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="K68" s="28">
+      <c r="K68" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA80,'GENERO Y CENTRO Y AREA TRABAJO'!J68)</f>
         <v>0</v>
       </c>
@@ -8537,7 +8554,7 @@
       <c r="J69" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="K69" s="28">
+      <c r="K69" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA81,'GENERO Y CENTRO Y AREA TRABAJO'!J69)</f>
         <v>0</v>
       </c>
@@ -8552,20 +8569,20 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J77" s="85" t="s">
+      <c r="J77" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="K77" s="85"/>
+      <c r="K77" s="83"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" s="81" t="s">
+      <c r="A78" s="86" t="s">
         <v>122</v>
       </c>
-      <c r="B78" s="81"/>
-      <c r="J78" s="43" t="s">
+      <c r="B78" s="86"/>
+      <c r="J78" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="K78" s="28">
+      <c r="K78" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA90,'GENERO Y CENTRO Y AREA TRABAJO'!J78)</f>
         <v>0</v>
       </c>
@@ -8574,14 +8591,14 @@
       <c r="A79" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B79" s="28">
+      <c r="B79" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z91,'GENERO Y CENTRO Y AREA TRABAJO'!A79)</f>
         <v>0</v>
       </c>
-      <c r="J79" s="43" t="s">
+      <c r="J79" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="K79" s="28">
+      <c r="K79" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA91,'GENERO Y CENTRO Y AREA TRABAJO'!J79)</f>
         <v>0</v>
       </c>
@@ -8590,14 +8607,14 @@
       <c r="A80" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B80" s="28">
+      <c r="B80" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z92,'GENERO Y CENTRO Y AREA TRABAJO'!A80)</f>
         <v>0</v>
       </c>
-      <c r="J80" s="43" t="s">
+      <c r="J80" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="K80" s="28">
+      <c r="K80" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA92,'GENERO Y CENTRO Y AREA TRABAJO'!J80)</f>
         <v>0</v>
       </c>
@@ -8606,14 +8623,14 @@
       <c r="A81" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B81" s="28">
+      <c r="B81" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z93,'GENERO Y CENTRO Y AREA TRABAJO'!A81)</f>
         <v>0</v>
       </c>
-      <c r="J81" s="43" t="s">
+      <c r="J81" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="K81" s="28">
+      <c r="K81" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA93,'GENERO Y CENTRO Y AREA TRABAJO'!J81)</f>
         <v>0</v>
       </c>
@@ -8622,7 +8639,7 @@
       <c r="A82" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B82" s="28">
+      <c r="B82" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z94,'GENERO Y CENTRO Y AREA TRABAJO'!A82)</f>
         <v>0</v>
       </c>
@@ -8635,129 +8652,129 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A83" s="44" t="s">
+      <c r="A83" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="44">
+      <c r="B83" s="46">
         <f>SUM(B79:B82)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="85" t="s">
+      <c r="A92" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="85"/>
-      <c r="J92" s="86" t="s">
+      <c r="B92" s="83"/>
+      <c r="J92" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="K92" s="87"/>
+      <c r="K92" s="85"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A93" s="49">
+      <c r="A93" s="51">
         <v>28</v>
       </c>
-      <c r="B93" s="28">
+      <c r="B93" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z105,'GENERO Y CENTRO Y AREA TRABAJO'!A93)</f>
         <v>0</v>
       </c>
-      <c r="J93" s="49">
+      <c r="J93" s="51">
         <v>36</v>
       </c>
-      <c r="K93" s="28">
+      <c r="K93" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA106,'GENERO Y CENTRO Y AREA TRABAJO'!J93)</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A94" s="49">
+      <c r="A94" s="51">
         <v>30</v>
       </c>
-      <c r="B94" s="28">
+      <c r="B94" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z106,'GENERO Y CENTRO Y AREA TRABAJO'!A94)</f>
         <v>0</v>
       </c>
-      <c r="J94" s="49">
+      <c r="J94" s="51">
         <v>28</v>
       </c>
-      <c r="K94" s="28">
+      <c r="K94" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA107,'GENERO Y CENTRO Y AREA TRABAJO'!J94)</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A95" s="49">
+      <c r="A95" s="51">
         <v>32</v>
       </c>
-      <c r="B95" s="28">
+      <c r="B95" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z107,'GENERO Y CENTRO Y AREA TRABAJO'!A95)</f>
         <v>0</v>
       </c>
-      <c r="J95" s="49">
+      <c r="J95" s="51">
         <v>39</v>
       </c>
-      <c r="K95" s="28">
+      <c r="K95" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA108,'GENERO Y CENTRO Y AREA TRABAJO'!J95)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A96" s="49">
+      <c r="A96" s="51">
         <v>34</v>
       </c>
-      <c r="B96" s="28">
+      <c r="B96" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z108,'GENERO Y CENTRO Y AREA TRABAJO'!A96)</f>
         <v>0</v>
       </c>
-      <c r="J96" s="49">
+      <c r="J96" s="51">
         <v>40</v>
       </c>
-      <c r="K96" s="28">
+      <c r="K96" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA109,'GENERO Y CENTRO Y AREA TRABAJO'!J96)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A97" s="49">
+      <c r="A97" s="51">
         <v>36</v>
       </c>
-      <c r="B97" s="28">
+      <c r="B97" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z109,'GENERO Y CENTRO Y AREA TRABAJO'!A97)</f>
         <v>0</v>
       </c>
-      <c r="J97" s="49">
+      <c r="J97" s="51">
         <v>41</v>
       </c>
-      <c r="K97" s="28">
+      <c r="K97" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA110,'GENERO Y CENTRO Y AREA TRABAJO'!J97)</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A98" s="49">
+      <c r="A98" s="51">
         <v>38</v>
       </c>
-      <c r="B98" s="28">
+      <c r="B98" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z110,'GENERO Y CENTRO Y AREA TRABAJO'!A98)</f>
         <v>0</v>
       </c>
-      <c r="J98" s="49">
+      <c r="J98" s="51">
         <v>42</v>
       </c>
-      <c r="K98" s="28">
+      <c r="K98" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA111,'GENERO Y CENTRO Y AREA TRABAJO'!J98)</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A99" s="45" t="s">
+      <c r="A99" s="47" t="s">
         <v>87</v>
       </c>
       <c r="B99" s="22">
         <f>SUM(B93:B98)</f>
         <v>0</v>
       </c>
-      <c r="J99" s="45" t="s">
+      <c r="J99" s="47" t="s">
         <v>87</v>
       </c>
       <c r="K99" s="22">
@@ -8766,36 +8783,36 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A109" s="85" t="s">
+      <c r="A109" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B109" s="85"/>
+      <c r="B109" s="83"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B110" s="28">
+      <c r="B110" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z122,'GENERO Y CENTRO Y AREA TRABAJO'!A110)</f>
         <v>0</v>
       </c>
-      <c r="J110" s="85" t="s">
+      <c r="J110" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="K110" s="85"/>
+      <c r="K110" s="83"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B111" s="28">
+      <c r="B111" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z123,'GENERO Y CENTRO Y AREA TRABAJO'!A111)</f>
         <v>0</v>
       </c>
       <c r="J111" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="K111" s="28">
+      <c r="K111" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA123,'GENERO Y CENTRO Y AREA TRABAJO'!J111)</f>
         <v>0</v>
       </c>
@@ -8804,14 +8821,14 @@
       <c r="A112" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B112" s="28">
+      <c r="B112" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z124,'GENERO Y CENTRO Y AREA TRABAJO'!A112)</f>
         <v>0</v>
       </c>
       <c r="J112" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="K112" s="28">
+      <c r="K112" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA124,'GENERO Y CENTRO Y AREA TRABAJO'!J112)</f>
         <v>0</v>
       </c>
@@ -8820,14 +8837,14 @@
       <c r="A113" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B113" s="28">
+      <c r="B113" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z125,'GENERO Y CENTRO Y AREA TRABAJO'!A113)</f>
         <v>0</v>
       </c>
       <c r="J113" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="K113" s="28">
+      <c r="K113" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA125,'GENERO Y CENTRO Y AREA TRABAJO'!J113)</f>
         <v>0</v>
       </c>
@@ -8843,7 +8860,7 @@
       <c r="J114" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="K114" s="28">
+      <c r="K114" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA126,'GENERO Y CENTRO Y AREA TRABAJO'!J114)</f>
         <v>0</v>
       </c>
@@ -8852,7 +8869,7 @@
       <c r="J115" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="K115" s="28">
+      <c r="K115" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA127,'GENERO Y CENTRO Y AREA TRABAJO'!J115)</f>
         <v>0</v>
       </c>
@@ -8861,7 +8878,7 @@
       <c r="J116" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="K116" s="28">
+      <c r="K116" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA128,'GENERO Y CENTRO Y AREA TRABAJO'!J116)</f>
         <v>0</v>
       </c>
@@ -8870,7 +8887,7 @@
       <c r="J117" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="K117" s="28">
+      <c r="K117" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA129,'GENERO Y CENTRO Y AREA TRABAJO'!J117)</f>
         <v>0</v>
       </c>
@@ -8885,77 +8902,77 @@
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A126" s="85" t="s">
+      <c r="A126" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="B126" s="85"/>
+      <c r="B126" s="83"/>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A127" s="33" t="s">
+      <c r="A127" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B127" s="28">
+      <c r="B127" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z139,'GENERO Y CENTRO Y AREA TRABAJO'!A127)</f>
         <v>0</v>
       </c>
-      <c r="J127" s="85" t="s">
+      <c r="J127" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="K127" s="85"/>
+      <c r="K127" s="83"/>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A128" s="33" t="s">
+      <c r="A128" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B128" s="28">
+      <c r="B128" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z140,'GENERO Y CENTRO Y AREA TRABAJO'!A128)</f>
         <v>0</v>
       </c>
       <c r="J128" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="K128" s="28">
+      <c r="K128" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA140,'GENERO Y CENTRO Y AREA TRABAJO'!J128)</f>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A129" s="33" t="s">
+      <c r="A129" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B129" s="28">
+      <c r="B129" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z141,'GENERO Y CENTRO Y AREA TRABAJO'!A129)</f>
         <v>0</v>
       </c>
       <c r="J129" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K129" s="28">
+      <c r="K129" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA141,'GENERO Y CENTRO Y AREA TRABAJO'!J129)</f>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A130" s="33" t="s">
+      <c r="A130" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B130" s="28">
+      <c r="B130" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z142,'GENERO Y CENTRO Y AREA TRABAJO'!A130)</f>
         <v>0</v>
       </c>
       <c r="J130" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="K130" s="28">
+      <c r="K130" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!I$4:AA142,'GENERO Y CENTRO Y AREA TRABAJO'!J130)</f>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A131" s="33" t="s">
+      <c r="A131" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="B131" s="28">
+      <c r="B131" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z143,'GENERO Y CENTRO Y AREA TRABAJO'!A131)</f>
         <v>0</v>
       </c>
@@ -8968,10 +8985,10 @@
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A132" s="33" t="s">
+      <c r="A132" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="B132" s="28">
+      <c r="B132" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z144,'GENERO Y CENTRO Y AREA TRABAJO'!A132)</f>
         <v>0</v>
       </c>
@@ -8986,16 +9003,16 @@
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A142" s="85" t="s">
+      <c r="A142" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B142" s="85"/>
+      <c r="B142" s="83"/>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B143" s="28">
+      <c r="B143" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z155,'GENERO Y CENTRO Y AREA TRABAJO'!A143)</f>
         <v>0</v>
       </c>
@@ -9004,7 +9021,7 @@
       <c r="A144" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B144" s="28">
+      <c r="B144" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z156,'GENERO Y CENTRO Y AREA TRABAJO'!A144)</f>
         <v>0</v>
       </c>
@@ -9013,7 +9030,7 @@
       <c r="A145" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B145" s="28">
+      <c r="B145" s="29">
         <f>COUNTIF('PERFIL SOCIODEMOGRAFICO'!B$4:Z157,'GENERO Y CENTRO Y AREA TRABAJO'!#REF!)</f>
         <v>0</v>
       </c>
@@ -9029,6 +9046,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J28:K28"/>
     <mergeCell ref="A92:B92"/>
     <mergeCell ref="J92:K92"/>
     <mergeCell ref="A29:B29"/>
@@ -9043,11 +9065,6 @@
     <mergeCell ref="J61:K61"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="J77:K77"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J28:K28"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J33" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -9067,38 +9084,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AC239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="54" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="54" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="56" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="56" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="48.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="54" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" style="54" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="56" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" style="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="56" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="54" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="56" customWidth="1"/>
     <col min="13" max="13" width="18.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="54"/>
-    <col min="16" max="16" width="14.28515625" style="54" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="54" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" style="54" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="54" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" style="54" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" style="54" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" style="54" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="43.85546875" style="54" customWidth="1"/>
-    <col min="25" max="25" width="62" style="54" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.140625" style="54" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="56"/>
+    <col min="16" max="16" width="14.28515625" style="56" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" style="56" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" style="56" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" style="56" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" style="56" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" style="56" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="43.85546875" style="56" customWidth="1"/>
+    <col min="25" max="25" width="62" style="56" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" style="56" customWidth="1"/>
     <col min="27" max="27" width="19.140625" style="3" customWidth="1"/>
     <col min="28" max="28" width="19.140625" style="4" customWidth="1"/>
     <col min="29" max="29" width="213" style="4" bestFit="1" customWidth="1"/>
@@ -10244,43 +10261,43 @@
       <c r="N1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="O1" s="39">
+      <c r="O1" s="41">
         <f ca="1">TODAY()</f>
-        <v>44884</v>
+        <v>44895</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="5" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="77"/>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="78"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="80"/>
     </row>
     <row r="3" spans="1:29" s="8" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -10371,450 +10388,180 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="30">
-        <v>71579486</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="24">
-        <v>22011</v>
-      </c>
-      <c r="F4" s="25">
-        <v>40664</v>
-      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="T4" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="V4" s="11">
-        <v>3112363842</v>
-      </c>
-      <c r="W4" s="34">
-        <v>3112363842</v>
-      </c>
-      <c r="X4" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y4" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z4" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA4" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB4" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC4" s="35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+    </row>
+    <row r="5" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="30">
-        <v>71579486</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="24">
-        <v>22011</v>
-      </c>
-      <c r="F5" s="25">
-        <v>40664</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="M5" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="T5" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="V5" s="11">
-        <v>3112363842</v>
-      </c>
-      <c r="W5" s="34">
-        <v>3112363842</v>
-      </c>
-      <c r="X5" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y5" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z5" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA5" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB5" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC5" s="35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="36"/>
+      <c r="AB5" s="36"/>
+      <c r="AC5" s="36"/>
+    </row>
+    <row r="6" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <v>1</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="30">
-        <v>71579486</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="24">
-        <v>22011</v>
-      </c>
-      <c r="F6" s="25">
-        <v>40664</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="60"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J6" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="M6" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="T6" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="V6" s="11">
-        <v>3112363842</v>
-      </c>
-      <c r="W6" s="34">
-        <v>3112363842</v>
-      </c>
-      <c r="X6" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y6" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z6" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA6" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB6" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC6" s="35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+    </row>
+    <row r="7" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
-        <v>1</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="30">
-        <v>71579486</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="24">
-        <v>22011</v>
-      </c>
-      <c r="F7" s="25">
-        <v>40664</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J7" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="M7" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="T7" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="V7" s="11">
-        <v>3112363842</v>
-      </c>
-      <c r="W7" s="34">
-        <v>3112363842</v>
-      </c>
-      <c r="X7" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y7" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z7" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA7" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB7" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC7" s="35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="H7" s="9"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="68"/>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="36"/>
+      <c r="AB7" s="36"/>
+      <c r="AC7" s="36"/>
+    </row>
+    <row r="8" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
-        <v>1</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="30">
-        <v>71579486</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="24">
-        <v>22011</v>
-      </c>
-      <c r="F8" s="25">
-        <v>40664</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="M8" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="T8" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="U8" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="V8" s="11">
-        <v>3112363842</v>
-      </c>
-      <c r="W8" s="34">
-        <v>3112363842</v>
-      </c>
-      <c r="X8" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y8" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z8" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA8" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB8" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC8" s="35" t="s">
-        <v>134</v>
-      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="69"/>
     </row>
     <row r="9" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>6</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="57"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -10833,7 +10580,7 @@
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
       <c r="X9" s="11"/>
-      <c r="Y9" s="33"/>
+      <c r="Y9" s="34"/>
       <c r="Z9" s="9"/>
       <c r="AA9" s="12"/>
       <c r="AB9" s="12"/>
@@ -10843,44 +10590,44 @@
       <c r="A10" s="11">
         <v>7</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="59"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="61"/>
       <c r="N10" s="26"/>
       <c r="O10" s="9"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="59"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="59"/>
-      <c r="W10" s="61"/>
-      <c r="X10" s="59"/>
-      <c r="Y10" s="62"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="63"/>
-      <c r="AB10" s="63"/>
-      <c r="AC10" s="67"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="61"/>
+      <c r="U10" s="61"/>
+      <c r="V10" s="61"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="64"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="65"/>
+      <c r="AB10" s="65"/>
+      <c r="AC10" s="69"/>
     </row>
     <row r="11" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>8</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="57"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="61"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -10897,9 +10644,9 @@
       <c r="T11" s="11"/>
       <c r="U11" s="11"/>
       <c r="V11" s="11"/>
-      <c r="W11" s="31"/>
-      <c r="X11" s="68"/>
-      <c r="Y11" s="33"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="70"/>
+      <c r="Y11" s="34"/>
       <c r="Z11" s="9"/>
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
@@ -10908,14 +10655,14 @@
     <row r="12" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="31"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="9"/>
       <c r="E12" s="13"/>
       <c r="F12" s="10"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="33"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
@@ -10939,14 +10686,14 @@
     <row r="13" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="31"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="9"/>
       <c r="E13" s="13"/>
       <c r="F13" s="10"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="33"/>
+      <c r="J13" s="34"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
@@ -10970,14 +10717,14 @@
     <row r="14" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="31"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="9"/>
       <c r="E14" s="13"/>
       <c r="F14" s="10"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="33"/>
+      <c r="J14" s="34"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -11001,7 +10748,7 @@
     <row r="15" spans="1:29" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="31"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="9"/>
       <c r="E15" s="13"/>
       <c r="F15" s="10"/>
@@ -11214,458 +10961,458 @@
       <c r="AA21" s="14"/>
     </row>
     <row r="22" spans="1:29" ht="15" x14ac:dyDescent="0.25">
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="79">
+      <c r="D22" s="76"/>
+      <c r="E22" s="81">
         <v>43516</v>
       </c>
-      <c r="F22" s="80"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="75"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="75"/>
+      <c r="F22" s="82"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="77"/>
+      <c r="M22" s="77"/>
+      <c r="N22" s="77"/>
       <c r="AA22" s="4"/>
     </row>
     <row r="23" spans="1:29" ht="15" x14ac:dyDescent="0.25">
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="79">
+      <c r="D23" s="76"/>
+      <c r="E23" s="81">
         <v>44046</v>
       </c>
-      <c r="F23" s="80"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="75"/>
+      <c r="F23" s="82"/>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="77"/>
       <c r="AA23" s="4"/>
     </row>
     <row r="148" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E148" s="48" t="s">
+      <c r="E148" s="50" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="149" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E149" s="48" t="s">
+      <c r="E149" s="50" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="150" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E150" s="48" t="s">
+      <c r="E150" s="50" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="151" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E151" s="48" t="s">
+      <c r="E151" s="50" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="152" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E152" s="48" t="s">
+      <c r="E152" s="50" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="153" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E153" s="48" t="s">
+      <c r="E153" s="50" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="154" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E154" s="48" t="s">
+      <c r="E154" s="50" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="157" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E157" s="47" t="s">
+      <c r="E157" s="49" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="158" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E158" s="47" t="s">
+      <c r="E158" s="49" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="159" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E159" s="47" t="s">
+      <c r="E159" s="49" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="160" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E160" s="47" t="s">
+      <c r="E160" s="49" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="161" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E161" s="54"/>
+      <c r="E161" s="56"/>
     </row>
     <row r="162" spans="5:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="E162" s="50" t="s">
+      <c r="E162" s="52" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="163" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E163" s="50" t="s">
+      <c r="E163" s="52" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="164" spans="5:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="E164" s="51" t="s">
+      <c r="E164" s="53" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="165" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E165" s="50" t="s">
+      <c r="E165" s="52" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="166" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E166" s="50" t="s">
+      <c r="E166" s="52" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="167" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E167" s="47" t="s">
+      <c r="E167" s="49" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="168" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E168" s="54"/>
+      <c r="E168" s="56"/>
     </row>
     <row r="169" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E169" s="48" t="s">
+      <c r="E169" s="50" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="170" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E170" s="48" t="s">
+      <c r="E170" s="50" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="171" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E171" s="48" t="s">
+      <c r="E171" s="50" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="172" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E172" s="48" t="s">
+      <c r="E172" s="50" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="173" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E173" s="48" t="s">
+      <c r="E173" s="50" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="174" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E174" s="54"/>
+      <c r="E174" s="56"/>
     </row>
     <row r="175" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E175" s="48" t="s">
+      <c r="E175" s="50" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="176" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E176" s="48" t="s">
+      <c r="E176" s="50" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="177" spans="5:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="E177" s="48" t="s">
+      <c r="E177" s="50" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="178" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E178" s="54"/>
+      <c r="E178" s="56"/>
     </row>
     <row r="179" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E179" s="52" t="s">
+      <c r="E179" s="54" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="180" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E180" s="52" t="s">
+      <c r="E180" s="54" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="181" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E181" s="52" t="s">
+      <c r="E181" s="54" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="182" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E182" s="48" t="s">
+      <c r="E182" s="50" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="183" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E183" s="52" t="s">
+      <c r="E183" s="54" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="184" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E184" s="52" t="s">
+      <c r="E184" s="54" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="185" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E185" s="52" t="s">
+      <c r="E185" s="54" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="186" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E186" s="54"/>
+      <c r="E186" s="56"/>
     </row>
     <row r="187" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E187" s="48" t="s">
+      <c r="E187" s="50" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="188" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E188" s="48" t="s">
+      <c r="E188" s="50" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="189" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E189" s="48" t="s">
+      <c r="E189" s="50" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="190" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E190" s="52" t="s">
+      <c r="E190" s="54" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="191" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E191" s="54"/>
+      <c r="E191" s="56"/>
     </row>
     <row r="192" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E192" s="48" t="s">
+      <c r="E192" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="193" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E193" s="48" t="s">
+      <c r="E193" s="50" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="194" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E194" s="48" t="s">
+      <c r="E194" s="50" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="195" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E195" s="48" t="s">
+      <c r="E195" s="50" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="196" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E196" s="48" t="s">
+      <c r="E196" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="197" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E197" s="48" t="s">
+      <c r="E197" s="50" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="198" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E198" s="54"/>
+      <c r="E198" s="56"/>
     </row>
     <row r="199" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E199" s="48" t="s">
+      <c r="E199" s="50" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="200" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E200" s="48" t="s">
+      <c r="E200" s="50" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="201" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E201" s="48" t="s">
+      <c r="E201" s="50" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="202" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E202" s="48" t="s">
+      <c r="E202" s="50" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="203" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E203" s="48" t="s">
+      <c r="E203" s="50" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="204" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E204" s="48" t="s">
+      <c r="E204" s="50" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="205" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E205" s="48" t="s">
+      <c r="E205" s="50" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="206" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E206" s="48" t="s">
+      <c r="E206" s="50" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="207" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E207" s="54"/>
+      <c r="E207" s="56"/>
     </row>
     <row r="208" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E208" s="48" t="s">
+      <c r="E208" s="50" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="209" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E209" s="48" t="s">
+      <c r="E209" s="50" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="210" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E210" s="48" t="s">
+      <c r="E210" s="50" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="211" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E211" s="48" t="s">
+      <c r="E211" s="50" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="212" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E212" s="54"/>
+      <c r="E212" s="56"/>
     </row>
     <row r="213" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E213" s="48" t="s">
+      <c r="E213" s="50" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="214" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E214" s="48" t="s">
+      <c r="E214" s="50" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="215" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E215" s="48" t="s">
+      <c r="E215" s="50" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="216" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E216" s="48" t="s">
+      <c r="E216" s="50" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="217" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E217" s="54"/>
+      <c r="E217" s="56"/>
     </row>
     <row r="218" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E218" s="48" t="s">
+      <c r="E218" s="50" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="219" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E219" s="48" t="s">
+      <c r="E219" s="50" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="220" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E220" s="48" t="s">
+      <c r="E220" s="50" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="221" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E221" s="48" t="s">
+      <c r="E221" s="50" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="222" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E222" s="48" t="s">
+      <c r="E222" s="50" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="223" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E223" s="48" t="s">
+      <c r="E223" s="50" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="224" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E224" s="48" t="s">
+      <c r="E224" s="50" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="225" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E225" s="54"/>
+      <c r="E225" s="56"/>
     </row>
     <row r="226" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E226" s="53" t="s">
+      <c r="E226" s="55" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="227" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E227" s="53" t="s">
+      <c r="E227" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="228" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E228" s="53" t="s">
+      <c r="E228" s="55" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="229" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E229" s="53" t="s">
+      <c r="E229" s="55" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="230" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E230" s="53" t="s">
+      <c r="E230" s="55" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="231" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E231" s="53" t="s">
+      <c r="E231" s="55" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="232" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E232" s="54"/>
+      <c r="E232" s="56"/>
     </row>
     <row r="233" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E233" s="48" t="s">
+      <c r="E233" s="50" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="234" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E234" s="48" t="s">
+      <c r="E234" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="235" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E235" s="48" t="s">
+      <c r="E235" s="50" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="236" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E236" s="54"/>
+      <c r="E236" s="56"/>
     </row>
     <row r="237" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E237" s="48" t="s">
+      <c r="E237" s="50" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="238" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E238" s="48" t="s">
+      <c r="E238" s="50" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="239" spans="5:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E239" s="48" t="s">
+      <c r="E239" s="50" t="s">
         <v>48</v>
       </c>
     </row>
@@ -11679,104 +11426,113 @@
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="J23:N23"/>
   </mergeCells>
-  <dataValidations count="36">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11:G20" xr:uid="{00000000-0002-0000-0200-000000000000}">
+  <dataValidations count="39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7 G11:G20" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$E$148:$E$154</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E183:E184 E179:E181" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>$B$31:$B$35</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M20" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M6 M9:M20" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"CAFESALUD,SURA,COOMEVA,CONFENALCO,NUEVA EPS, CAOLSANITAS, SALUD TOTAL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N12:N20" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N6 N12:N20" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"PROTECCION, PORVENIR,COLFONDOS, SEGURO SOCIAL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVW983019:WVW983049 JK65515:JK65545 TG65515:TG65545 ADC65515:ADC65545 AMY65515:AMY65545 AWU65515:AWU65545 BGQ65515:BGQ65545 BQM65515:BQM65545 CAI65515:CAI65545 CKE65515:CKE65545 CUA65515:CUA65545 DDW65515:DDW65545 DNS65515:DNS65545 DXO65515:DXO65545 EHK65515:EHK65545 ERG65515:ERG65545 FBC65515:FBC65545 FKY65515:FKY65545 FUU65515:FUU65545 GEQ65515:GEQ65545 GOM65515:GOM65545 GYI65515:GYI65545 HIE65515:HIE65545 HSA65515:HSA65545 IBW65515:IBW65545 ILS65515:ILS65545 IVO65515:IVO65545 JFK65515:JFK65545 JPG65515:JPG65545 JZC65515:JZC65545 KIY65515:KIY65545 KSU65515:KSU65545 LCQ65515:LCQ65545 LMM65515:LMM65545 LWI65515:LWI65545 MGE65515:MGE65545 MQA65515:MQA65545 MZW65515:MZW65545 NJS65515:NJS65545 NTO65515:NTO65545 ODK65515:ODK65545 ONG65515:ONG65545 OXC65515:OXC65545 PGY65515:PGY65545 PQU65515:PQU65545 QAQ65515:QAQ65545 QKM65515:QKM65545 QUI65515:QUI65545 REE65515:REE65545 ROA65515:ROA65545 RXW65515:RXW65545 SHS65515:SHS65545 SRO65515:SRO65545 TBK65515:TBK65545 TLG65515:TLG65545 TVC65515:TVC65545 UEY65515:UEY65545 UOU65515:UOU65545 UYQ65515:UYQ65545 VIM65515:VIM65545 VSI65515:VSI65545 WCE65515:WCE65545 WMA65515:WMA65545 WVW65515:WVW65545 JK131051:JK131081 TG131051:TG131081 ADC131051:ADC131081 AMY131051:AMY131081 AWU131051:AWU131081 BGQ131051:BGQ131081 BQM131051:BQM131081 CAI131051:CAI131081 CKE131051:CKE131081 CUA131051:CUA131081 DDW131051:DDW131081 DNS131051:DNS131081 DXO131051:DXO131081 EHK131051:EHK131081 ERG131051:ERG131081 FBC131051:FBC131081 FKY131051:FKY131081 FUU131051:FUU131081 GEQ131051:GEQ131081 GOM131051:GOM131081 GYI131051:GYI131081 HIE131051:HIE131081 HSA131051:HSA131081 IBW131051:IBW131081 ILS131051:ILS131081 IVO131051:IVO131081 JFK131051:JFK131081 JPG131051:JPG131081 JZC131051:JZC131081 KIY131051:KIY131081 KSU131051:KSU131081 LCQ131051:LCQ131081 LMM131051:LMM131081 LWI131051:LWI131081 MGE131051:MGE131081 MQA131051:MQA131081 MZW131051:MZW131081 NJS131051:NJS131081 NTO131051:NTO131081 ODK131051:ODK131081 ONG131051:ONG131081 OXC131051:OXC131081 PGY131051:PGY131081 PQU131051:PQU131081 QAQ131051:QAQ131081 QKM131051:QKM131081 QUI131051:QUI131081 REE131051:REE131081 ROA131051:ROA131081 RXW131051:RXW131081 SHS131051:SHS131081 SRO131051:SRO131081 TBK131051:TBK131081 TLG131051:TLG131081 TVC131051:TVC131081 UEY131051:UEY131081 UOU131051:UOU131081 UYQ131051:UYQ131081 VIM131051:VIM131081 VSI131051:VSI131081 WCE131051:WCE131081 WMA131051:WMA131081 WVW131051:WVW131081 JK196587:JK196617 TG196587:TG196617 ADC196587:ADC196617 AMY196587:AMY196617 AWU196587:AWU196617 BGQ196587:BGQ196617 BQM196587:BQM196617 CAI196587:CAI196617 CKE196587:CKE196617 CUA196587:CUA196617 DDW196587:DDW196617 DNS196587:DNS196617 DXO196587:DXO196617 EHK196587:EHK196617 ERG196587:ERG196617 FBC196587:FBC196617 FKY196587:FKY196617 FUU196587:FUU196617 GEQ196587:GEQ196617 GOM196587:GOM196617 GYI196587:GYI196617 HIE196587:HIE196617 HSA196587:HSA196617 IBW196587:IBW196617 ILS196587:ILS196617 IVO196587:IVO196617 JFK196587:JFK196617 JPG196587:JPG196617 JZC196587:JZC196617 KIY196587:KIY196617 KSU196587:KSU196617 LCQ196587:LCQ196617 LMM196587:LMM196617 LWI196587:LWI196617 MGE196587:MGE196617 MQA196587:MQA196617 MZW196587:MZW196617 NJS196587:NJS196617 NTO196587:NTO196617 ODK196587:ODK196617 ONG196587:ONG196617 OXC196587:OXC196617 PGY196587:PGY196617 PQU196587:PQU196617 QAQ196587:QAQ196617 QKM196587:QKM196617 QUI196587:QUI196617 REE196587:REE196617 ROA196587:ROA196617 RXW196587:RXW196617 SHS196587:SHS196617 SRO196587:SRO196617 TBK196587:TBK196617 TLG196587:TLG196617 TVC196587:TVC196617 UEY196587:UEY196617 UOU196587:UOU196617 UYQ196587:UYQ196617 VIM196587:VIM196617 VSI196587:VSI196617 WCE196587:WCE196617 WMA196587:WMA196617 WVW196587:WVW196617 JK262123:JK262153 TG262123:TG262153 ADC262123:ADC262153 AMY262123:AMY262153 AWU262123:AWU262153 BGQ262123:BGQ262153 BQM262123:BQM262153 CAI262123:CAI262153 CKE262123:CKE262153 CUA262123:CUA262153 DDW262123:DDW262153 DNS262123:DNS262153 DXO262123:DXO262153 EHK262123:EHK262153 ERG262123:ERG262153 FBC262123:FBC262153 FKY262123:FKY262153 FUU262123:FUU262153 GEQ262123:GEQ262153 GOM262123:GOM262153 GYI262123:GYI262153 HIE262123:HIE262153 HSA262123:HSA262153 IBW262123:IBW262153 ILS262123:ILS262153 IVO262123:IVO262153 JFK262123:JFK262153 JPG262123:JPG262153 JZC262123:JZC262153 KIY262123:KIY262153 KSU262123:KSU262153 LCQ262123:LCQ262153 LMM262123:LMM262153 LWI262123:LWI262153 MGE262123:MGE262153 MQA262123:MQA262153 MZW262123:MZW262153 NJS262123:NJS262153 NTO262123:NTO262153 ODK262123:ODK262153 ONG262123:ONG262153 OXC262123:OXC262153 PGY262123:PGY262153 PQU262123:PQU262153 QAQ262123:QAQ262153 QKM262123:QKM262153 QUI262123:QUI262153 REE262123:REE262153 ROA262123:ROA262153 RXW262123:RXW262153 SHS262123:SHS262153 SRO262123:SRO262153 TBK262123:TBK262153 TLG262123:TLG262153 TVC262123:TVC262153 UEY262123:UEY262153 UOU262123:UOU262153 UYQ262123:UYQ262153 VIM262123:VIM262153 VSI262123:VSI262153 WCE262123:WCE262153 WMA262123:WMA262153 WVW262123:WVW262153 JK327659:JK327689 TG327659:TG327689 ADC327659:ADC327689 AMY327659:AMY327689 AWU327659:AWU327689 BGQ327659:BGQ327689 BQM327659:BQM327689 CAI327659:CAI327689 CKE327659:CKE327689 CUA327659:CUA327689 DDW327659:DDW327689 DNS327659:DNS327689 DXO327659:DXO327689 EHK327659:EHK327689 ERG327659:ERG327689 FBC327659:FBC327689 FKY327659:FKY327689 FUU327659:FUU327689 GEQ327659:GEQ327689 GOM327659:GOM327689 GYI327659:GYI327689 HIE327659:HIE327689 HSA327659:HSA327689 IBW327659:IBW327689 ILS327659:ILS327689 IVO327659:IVO327689 JFK327659:JFK327689 JPG327659:JPG327689 JZC327659:JZC327689 KIY327659:KIY327689 KSU327659:KSU327689 LCQ327659:LCQ327689 LMM327659:LMM327689 LWI327659:LWI327689 MGE327659:MGE327689 MQA327659:MQA327689 MZW327659:MZW327689 NJS327659:NJS327689 NTO327659:NTO327689 ODK327659:ODK327689 ONG327659:ONG327689 OXC327659:OXC327689 PGY327659:PGY327689 PQU327659:PQU327689 QAQ327659:QAQ327689 QKM327659:QKM327689 QUI327659:QUI327689 REE327659:REE327689 ROA327659:ROA327689 RXW327659:RXW327689 SHS327659:SHS327689 SRO327659:SRO327689 TBK327659:TBK327689 TLG327659:TLG327689 TVC327659:TVC327689 UEY327659:UEY327689 UOU327659:UOU327689 UYQ327659:UYQ327689 VIM327659:VIM327689 VSI327659:VSI327689 WCE327659:WCE327689 WMA327659:WMA327689 WVW327659:WVW327689 JK393195:JK393225 TG393195:TG393225 ADC393195:ADC393225 AMY393195:AMY393225 AWU393195:AWU393225 BGQ393195:BGQ393225 BQM393195:BQM393225 CAI393195:CAI393225 CKE393195:CKE393225 CUA393195:CUA393225 DDW393195:DDW393225 DNS393195:DNS393225 DXO393195:DXO393225 EHK393195:EHK393225 ERG393195:ERG393225 FBC393195:FBC393225 FKY393195:FKY393225 FUU393195:FUU393225 GEQ393195:GEQ393225 GOM393195:GOM393225 GYI393195:GYI393225 HIE393195:HIE393225 HSA393195:HSA393225 IBW393195:IBW393225 ILS393195:ILS393225 IVO393195:IVO393225 JFK393195:JFK393225 JPG393195:JPG393225 JZC393195:JZC393225 KIY393195:KIY393225 KSU393195:KSU393225 LCQ393195:LCQ393225 LMM393195:LMM393225 LWI393195:LWI393225 MGE393195:MGE393225 MQA393195:MQA393225 MZW393195:MZW393225 NJS393195:NJS393225 NTO393195:NTO393225 ODK393195:ODK393225 ONG393195:ONG393225 OXC393195:OXC393225 PGY393195:PGY393225 PQU393195:PQU393225 QAQ393195:QAQ393225 QKM393195:QKM393225 QUI393195:QUI393225 REE393195:REE393225 ROA393195:ROA393225 RXW393195:RXW393225 SHS393195:SHS393225 SRO393195:SRO393225 TBK393195:TBK393225 TLG393195:TLG393225 TVC393195:TVC393225 UEY393195:UEY393225 UOU393195:UOU393225 UYQ393195:UYQ393225 VIM393195:VIM393225 VSI393195:VSI393225 WCE393195:WCE393225 WMA393195:WMA393225 WVW393195:WVW393225 JK458731:JK458761 TG458731:TG458761 ADC458731:ADC458761 AMY458731:AMY458761 AWU458731:AWU458761 BGQ458731:BGQ458761 BQM458731:BQM458761 CAI458731:CAI458761 CKE458731:CKE458761 CUA458731:CUA458761 DDW458731:DDW458761 DNS458731:DNS458761 DXO458731:DXO458761 EHK458731:EHK458761 ERG458731:ERG458761 FBC458731:FBC458761 FKY458731:FKY458761 FUU458731:FUU458761 GEQ458731:GEQ458761 GOM458731:GOM458761 GYI458731:GYI458761 HIE458731:HIE458761 HSA458731:HSA458761 IBW458731:IBW458761 ILS458731:ILS458761 IVO458731:IVO458761 JFK458731:JFK458761 JPG458731:JPG458761 JZC458731:JZC458761 KIY458731:KIY458761 KSU458731:KSU458761 LCQ458731:LCQ458761 LMM458731:LMM458761 LWI458731:LWI458761 MGE458731:MGE458761 MQA458731:MQA458761 MZW458731:MZW458761 NJS458731:NJS458761 NTO458731:NTO458761 ODK458731:ODK458761 ONG458731:ONG458761 OXC458731:OXC458761 PGY458731:PGY458761 PQU458731:PQU458761 QAQ458731:QAQ458761 QKM458731:QKM458761 QUI458731:QUI458761 REE458731:REE458761 ROA458731:ROA458761 RXW458731:RXW458761 SHS458731:SHS458761 SRO458731:SRO458761 TBK458731:TBK458761 TLG458731:TLG458761 TVC458731:TVC458761 UEY458731:UEY458761 UOU458731:UOU458761 UYQ458731:UYQ458761 VIM458731:VIM458761 VSI458731:VSI458761 WCE458731:WCE458761 WMA458731:WMA458761 WVW458731:WVW458761 JK524267:JK524297 TG524267:TG524297 ADC524267:ADC524297 AMY524267:AMY524297 AWU524267:AWU524297 BGQ524267:BGQ524297 BQM524267:BQM524297 CAI524267:CAI524297 CKE524267:CKE524297 CUA524267:CUA524297 DDW524267:DDW524297 DNS524267:DNS524297 DXO524267:DXO524297 EHK524267:EHK524297 ERG524267:ERG524297 FBC524267:FBC524297 FKY524267:FKY524297 FUU524267:FUU524297 GEQ524267:GEQ524297 GOM524267:GOM524297 GYI524267:GYI524297 HIE524267:HIE524297 HSA524267:HSA524297 IBW524267:IBW524297 ILS524267:ILS524297 IVO524267:IVO524297 JFK524267:JFK524297 JPG524267:JPG524297 JZC524267:JZC524297 KIY524267:KIY524297 KSU524267:KSU524297 LCQ524267:LCQ524297 LMM524267:LMM524297 LWI524267:LWI524297 MGE524267:MGE524297 MQA524267:MQA524297 MZW524267:MZW524297 NJS524267:NJS524297 NTO524267:NTO524297 ODK524267:ODK524297 ONG524267:ONG524297 OXC524267:OXC524297 PGY524267:PGY524297 PQU524267:PQU524297 QAQ524267:QAQ524297 QKM524267:QKM524297 QUI524267:QUI524297 REE524267:REE524297 ROA524267:ROA524297 RXW524267:RXW524297 SHS524267:SHS524297 SRO524267:SRO524297 TBK524267:TBK524297 TLG524267:TLG524297 TVC524267:TVC524297 UEY524267:UEY524297 UOU524267:UOU524297 UYQ524267:UYQ524297 VIM524267:VIM524297 VSI524267:VSI524297 WCE524267:WCE524297 WMA524267:WMA524297 WVW524267:WVW524297 JK589803:JK589833 TG589803:TG589833 ADC589803:ADC589833 AMY589803:AMY589833 AWU589803:AWU589833 BGQ589803:BGQ589833 BQM589803:BQM589833 CAI589803:CAI589833 CKE589803:CKE589833 CUA589803:CUA589833 DDW589803:DDW589833 DNS589803:DNS589833 DXO589803:DXO589833 EHK589803:EHK589833 ERG589803:ERG589833 FBC589803:FBC589833 FKY589803:FKY589833 FUU589803:FUU589833 GEQ589803:GEQ589833 GOM589803:GOM589833 GYI589803:GYI589833 HIE589803:HIE589833 HSA589803:HSA589833 IBW589803:IBW589833 ILS589803:ILS589833 IVO589803:IVO589833 JFK589803:JFK589833 JPG589803:JPG589833 JZC589803:JZC589833 KIY589803:KIY589833 KSU589803:KSU589833 LCQ589803:LCQ589833 LMM589803:LMM589833 LWI589803:LWI589833 MGE589803:MGE589833 MQA589803:MQA589833 MZW589803:MZW589833 NJS589803:NJS589833 NTO589803:NTO589833 ODK589803:ODK589833 ONG589803:ONG589833 OXC589803:OXC589833 PGY589803:PGY589833 PQU589803:PQU589833 QAQ589803:QAQ589833 QKM589803:QKM589833 QUI589803:QUI589833 REE589803:REE589833 ROA589803:ROA589833 RXW589803:RXW589833 SHS589803:SHS589833 SRO589803:SRO589833 TBK589803:TBK589833 TLG589803:TLG589833 TVC589803:TVC589833 UEY589803:UEY589833 UOU589803:UOU589833 UYQ589803:UYQ589833 VIM589803:VIM589833 VSI589803:VSI589833 WCE589803:WCE589833 WMA589803:WMA589833 WVW589803:WVW589833 JK655339:JK655369 TG655339:TG655369 ADC655339:ADC655369 AMY655339:AMY655369 AWU655339:AWU655369 BGQ655339:BGQ655369 BQM655339:BQM655369 CAI655339:CAI655369 CKE655339:CKE655369 CUA655339:CUA655369 DDW655339:DDW655369 DNS655339:DNS655369 DXO655339:DXO655369 EHK655339:EHK655369 ERG655339:ERG655369 FBC655339:FBC655369 FKY655339:FKY655369 FUU655339:FUU655369 GEQ655339:GEQ655369 GOM655339:GOM655369 GYI655339:GYI655369 HIE655339:HIE655369 HSA655339:HSA655369 IBW655339:IBW655369 ILS655339:ILS655369 IVO655339:IVO655369 JFK655339:JFK655369 JPG655339:JPG655369 JZC655339:JZC655369 KIY655339:KIY655369 KSU655339:KSU655369 LCQ655339:LCQ655369 LMM655339:LMM655369 LWI655339:LWI655369 MGE655339:MGE655369 MQA655339:MQA655369 MZW655339:MZW655369 NJS655339:NJS655369 NTO655339:NTO655369 ODK655339:ODK655369 ONG655339:ONG655369 OXC655339:OXC655369 PGY655339:PGY655369 PQU655339:PQU655369 QAQ655339:QAQ655369 QKM655339:QKM655369 QUI655339:QUI655369 REE655339:REE655369 ROA655339:ROA655369 RXW655339:RXW655369 SHS655339:SHS655369 SRO655339:SRO655369 TBK655339:TBK655369 TLG655339:TLG655369 TVC655339:TVC655369 UEY655339:UEY655369 UOU655339:UOU655369 UYQ655339:UYQ655369 VIM655339:VIM655369 VSI655339:VSI655369 WCE655339:WCE655369 WMA655339:WMA655369 WVW655339:WVW655369 JK720875:JK720905 TG720875:TG720905 ADC720875:ADC720905 AMY720875:AMY720905 AWU720875:AWU720905 BGQ720875:BGQ720905 BQM720875:BQM720905 CAI720875:CAI720905 CKE720875:CKE720905 CUA720875:CUA720905 DDW720875:DDW720905 DNS720875:DNS720905 DXO720875:DXO720905 EHK720875:EHK720905 ERG720875:ERG720905 FBC720875:FBC720905 FKY720875:FKY720905 FUU720875:FUU720905 GEQ720875:GEQ720905 GOM720875:GOM720905 GYI720875:GYI720905 HIE720875:HIE720905 HSA720875:HSA720905 IBW720875:IBW720905 ILS720875:ILS720905 IVO720875:IVO720905 JFK720875:JFK720905 JPG720875:JPG720905 JZC720875:JZC720905 KIY720875:KIY720905 KSU720875:KSU720905 LCQ720875:LCQ720905 LMM720875:LMM720905 LWI720875:LWI720905 MGE720875:MGE720905 MQA720875:MQA720905 MZW720875:MZW720905 NJS720875:NJS720905 NTO720875:NTO720905 ODK720875:ODK720905 ONG720875:ONG720905 OXC720875:OXC720905 PGY720875:PGY720905 PQU720875:PQU720905 QAQ720875:QAQ720905 QKM720875:QKM720905 QUI720875:QUI720905 REE720875:REE720905 ROA720875:ROA720905 RXW720875:RXW720905 SHS720875:SHS720905 SRO720875:SRO720905 TBK720875:TBK720905 TLG720875:TLG720905 TVC720875:TVC720905 UEY720875:UEY720905 UOU720875:UOU720905 UYQ720875:UYQ720905 VIM720875:VIM720905 VSI720875:VSI720905 WCE720875:WCE720905 WMA720875:WMA720905 WVW720875:WVW720905 JK786411:JK786441 TG786411:TG786441 ADC786411:ADC786441 AMY786411:AMY786441 AWU786411:AWU786441 BGQ786411:BGQ786441 BQM786411:BQM786441 CAI786411:CAI786441 CKE786411:CKE786441 CUA786411:CUA786441 DDW786411:DDW786441 DNS786411:DNS786441 DXO786411:DXO786441 EHK786411:EHK786441 ERG786411:ERG786441 FBC786411:FBC786441 FKY786411:FKY786441 FUU786411:FUU786441 GEQ786411:GEQ786441 GOM786411:GOM786441 GYI786411:GYI786441 HIE786411:HIE786441 HSA786411:HSA786441 IBW786411:IBW786441 ILS786411:ILS786441 IVO786411:IVO786441 JFK786411:JFK786441 JPG786411:JPG786441 JZC786411:JZC786441 KIY786411:KIY786441 KSU786411:KSU786441 LCQ786411:LCQ786441 LMM786411:LMM786441 LWI786411:LWI786441 MGE786411:MGE786441 MQA786411:MQA786441 MZW786411:MZW786441 NJS786411:NJS786441 NTO786411:NTO786441 ODK786411:ODK786441 ONG786411:ONG786441 OXC786411:OXC786441 PGY786411:PGY786441 PQU786411:PQU786441 QAQ786411:QAQ786441 QKM786411:QKM786441 QUI786411:QUI786441 REE786411:REE786441 ROA786411:ROA786441 RXW786411:RXW786441 SHS786411:SHS786441 SRO786411:SRO786441 TBK786411:TBK786441 TLG786411:TLG786441 TVC786411:TVC786441 UEY786411:UEY786441 UOU786411:UOU786441 UYQ786411:UYQ786441 VIM786411:VIM786441 VSI786411:VSI786441 WCE786411:WCE786441 WMA786411:WMA786441 WVW786411:WVW786441 JK851947:JK851977 TG851947:TG851977 ADC851947:ADC851977 AMY851947:AMY851977 AWU851947:AWU851977 BGQ851947:BGQ851977 BQM851947:BQM851977 CAI851947:CAI851977 CKE851947:CKE851977 CUA851947:CUA851977 DDW851947:DDW851977 DNS851947:DNS851977 DXO851947:DXO851977 EHK851947:EHK851977 ERG851947:ERG851977 FBC851947:FBC851977 FKY851947:FKY851977 FUU851947:FUU851977 GEQ851947:GEQ851977 GOM851947:GOM851977 GYI851947:GYI851977 HIE851947:HIE851977 HSA851947:HSA851977 IBW851947:IBW851977 ILS851947:ILS851977 IVO851947:IVO851977 JFK851947:JFK851977 JPG851947:JPG851977 JZC851947:JZC851977 KIY851947:KIY851977 KSU851947:KSU851977 LCQ851947:LCQ851977 LMM851947:LMM851977 LWI851947:LWI851977 MGE851947:MGE851977 MQA851947:MQA851977 MZW851947:MZW851977 NJS851947:NJS851977 NTO851947:NTO851977 ODK851947:ODK851977 ONG851947:ONG851977 OXC851947:OXC851977 PGY851947:PGY851977 PQU851947:PQU851977 QAQ851947:QAQ851977 QKM851947:QKM851977 QUI851947:QUI851977 REE851947:REE851977 ROA851947:ROA851977 RXW851947:RXW851977 SHS851947:SHS851977 SRO851947:SRO851977 TBK851947:TBK851977 TLG851947:TLG851977 TVC851947:TVC851977 UEY851947:UEY851977 UOU851947:UOU851977 UYQ851947:UYQ851977 VIM851947:VIM851977 VSI851947:VSI851977 WCE851947:WCE851977 WMA851947:WMA851977 WVW851947:WVW851977 JK917483:JK917513 TG917483:TG917513 ADC917483:ADC917513 AMY917483:AMY917513 AWU917483:AWU917513 BGQ917483:BGQ917513 BQM917483:BQM917513 CAI917483:CAI917513 CKE917483:CKE917513 CUA917483:CUA917513 DDW917483:DDW917513 DNS917483:DNS917513 DXO917483:DXO917513 EHK917483:EHK917513 ERG917483:ERG917513 FBC917483:FBC917513 FKY917483:FKY917513 FUU917483:FUU917513 GEQ917483:GEQ917513 GOM917483:GOM917513 GYI917483:GYI917513 HIE917483:HIE917513 HSA917483:HSA917513 IBW917483:IBW917513 ILS917483:ILS917513 IVO917483:IVO917513 JFK917483:JFK917513 JPG917483:JPG917513 JZC917483:JZC917513 KIY917483:KIY917513 KSU917483:KSU917513 LCQ917483:LCQ917513 LMM917483:LMM917513 LWI917483:LWI917513 MGE917483:MGE917513 MQA917483:MQA917513 MZW917483:MZW917513 NJS917483:NJS917513 NTO917483:NTO917513 ODK917483:ODK917513 ONG917483:ONG917513 OXC917483:OXC917513 PGY917483:PGY917513 PQU917483:PQU917513 QAQ917483:QAQ917513 QKM917483:QKM917513 QUI917483:QUI917513 REE917483:REE917513 ROA917483:ROA917513 RXW917483:RXW917513 SHS917483:SHS917513 SRO917483:SRO917513 TBK917483:TBK917513 TLG917483:TLG917513 TVC917483:TVC917513 UEY917483:UEY917513 UOU917483:UOU917513 UYQ917483:UYQ917513 VIM917483:VIM917513 VSI917483:VSI917513 WCE917483:WCE917513 WMA917483:WMA917513 WVW917483:WVW917513 JK983019:JK983049 TG983019:TG983049 ADC983019:ADC983049 AMY983019:AMY983049 AWU983019:AWU983049 BGQ983019:BGQ983049 BQM983019:BQM983049 CAI983019:CAI983049 CKE983019:CKE983049 CUA983019:CUA983049 DDW983019:DDW983049 DNS983019:DNS983049 DXO983019:DXO983049 EHK983019:EHK983049 ERG983019:ERG983049 FBC983019:FBC983049 FKY983019:FKY983049 FUU983019:FUU983049 GEQ983019:GEQ983049 GOM983019:GOM983049 GYI983019:GYI983049 HIE983019:HIE983049 HSA983019:HSA983049 IBW983019:IBW983049 ILS983019:ILS983049 IVO983019:IVO983049 JFK983019:JFK983049 JPG983019:JPG983049 JZC983019:JZC983049 KIY983019:KIY983049 KSU983019:KSU983049 LCQ983019:LCQ983049 LMM983019:LMM983049 LWI983019:LWI983049 MGE983019:MGE983049 MQA983019:MQA983049 MZW983019:MZW983049 NJS983019:NJS983049 NTO983019:NTO983049 ODK983019:ODK983049 ONG983019:ONG983049 OXC983019:OXC983049 PGY983019:PGY983049 PQU983019:PQU983049 QAQ983019:QAQ983049 QKM983019:QKM983049 QUI983019:QUI983049 REE983019:REE983049 ROA983019:ROA983049 RXW983019:RXW983049 SHS983019:SHS983049 SRO983019:SRO983049 TBK983019:TBK983049 TLG983019:TLG983049 TVC983019:TVC983049 UEY983019:UEY983049 UOU983019:UOU983049 UYQ983019:UYQ983049 VIM983019:VIM983049 VSI983019:VSI983049 WCE983019:WCE983049 WMA983019:WMA983049 WVW4:WVW20 WMA4:WMA20 WCE4:WCE20 VSI4:VSI20 VIM4:VIM20 UYQ4:UYQ20 UOU4:UOU20 UEY4:UEY20 TVC4:TVC20 TLG4:TLG20 TBK4:TBK20 SRO4:SRO20 SHS4:SHS20 RXW4:RXW20 ROA4:ROA20 REE4:REE20 QUI4:QUI20 QKM4:QKM20 QAQ4:QAQ20 PQU4:PQU20 PGY4:PGY20 OXC4:OXC20 ONG4:ONG20 ODK4:ODK20 NTO4:NTO20 NJS4:NJS20 MZW4:MZW20 MQA4:MQA20 MGE4:MGE20 LWI4:LWI20 LMM4:LMM20 LCQ4:LCQ20 KSU4:KSU20 KIY4:KIY20 JZC4:JZC20 JPG4:JPG20 JFK4:JFK20 IVO4:IVO20 ILS4:ILS20 IBW4:IBW20 HSA4:HSA20 HIE4:HIE20 GYI4:GYI20 GOM4:GOM20 GEQ4:GEQ20 FUU4:FUU20 FKY4:FKY20 FBC4:FBC20 ERG4:ERG20 EHK4:EHK20 DXO4:DXO20 DNS4:DNS20 DDW4:DDW20 CUA4:CUA20 CKE4:CKE20 CAI4:CAI20 BQM4:BQM20 BGQ4:BGQ20 AWU4:AWU20 AMY4:AMY20 ADC4:ADC20 TG4:TG20 JK4:JK20" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVW983019:WVW983049 JK65515:JK65545 TG65515:TG65545 ADC65515:ADC65545 AMY65515:AMY65545 AWU65515:AWU65545 BGQ65515:BGQ65545 BQM65515:BQM65545 CAI65515:CAI65545 CKE65515:CKE65545 CUA65515:CUA65545 DDW65515:DDW65545 DNS65515:DNS65545 DXO65515:DXO65545 EHK65515:EHK65545 ERG65515:ERG65545 FBC65515:FBC65545 FKY65515:FKY65545 FUU65515:FUU65545 GEQ65515:GEQ65545 GOM65515:GOM65545 GYI65515:GYI65545 HIE65515:HIE65545 HSA65515:HSA65545 IBW65515:IBW65545 ILS65515:ILS65545 IVO65515:IVO65545 JFK65515:JFK65545 JPG65515:JPG65545 JZC65515:JZC65545 KIY65515:KIY65545 KSU65515:KSU65545 LCQ65515:LCQ65545 LMM65515:LMM65545 LWI65515:LWI65545 MGE65515:MGE65545 MQA65515:MQA65545 MZW65515:MZW65545 NJS65515:NJS65545 NTO65515:NTO65545 ODK65515:ODK65545 ONG65515:ONG65545 OXC65515:OXC65545 PGY65515:PGY65545 PQU65515:PQU65545 QAQ65515:QAQ65545 QKM65515:QKM65545 QUI65515:QUI65545 REE65515:REE65545 ROA65515:ROA65545 RXW65515:RXW65545 SHS65515:SHS65545 SRO65515:SRO65545 TBK65515:TBK65545 TLG65515:TLG65545 TVC65515:TVC65545 UEY65515:UEY65545 UOU65515:UOU65545 UYQ65515:UYQ65545 VIM65515:VIM65545 VSI65515:VSI65545 WCE65515:WCE65545 WMA65515:WMA65545 WVW65515:WVW65545 JK131051:JK131081 TG131051:TG131081 ADC131051:ADC131081 AMY131051:AMY131081 AWU131051:AWU131081 BGQ131051:BGQ131081 BQM131051:BQM131081 CAI131051:CAI131081 CKE131051:CKE131081 CUA131051:CUA131081 DDW131051:DDW131081 DNS131051:DNS131081 DXO131051:DXO131081 EHK131051:EHK131081 ERG131051:ERG131081 FBC131051:FBC131081 FKY131051:FKY131081 FUU131051:FUU131081 GEQ131051:GEQ131081 GOM131051:GOM131081 GYI131051:GYI131081 HIE131051:HIE131081 HSA131051:HSA131081 IBW131051:IBW131081 ILS131051:ILS131081 IVO131051:IVO131081 JFK131051:JFK131081 JPG131051:JPG131081 JZC131051:JZC131081 KIY131051:KIY131081 KSU131051:KSU131081 LCQ131051:LCQ131081 LMM131051:LMM131081 LWI131051:LWI131081 MGE131051:MGE131081 MQA131051:MQA131081 MZW131051:MZW131081 NJS131051:NJS131081 NTO131051:NTO131081 ODK131051:ODK131081 ONG131051:ONG131081 OXC131051:OXC131081 PGY131051:PGY131081 PQU131051:PQU131081 QAQ131051:QAQ131081 QKM131051:QKM131081 QUI131051:QUI131081 REE131051:REE131081 ROA131051:ROA131081 RXW131051:RXW131081 SHS131051:SHS131081 SRO131051:SRO131081 TBK131051:TBK131081 TLG131051:TLG131081 TVC131051:TVC131081 UEY131051:UEY131081 UOU131051:UOU131081 UYQ131051:UYQ131081 VIM131051:VIM131081 VSI131051:VSI131081 WCE131051:WCE131081 WMA131051:WMA131081 WVW131051:WVW131081 JK196587:JK196617 TG196587:TG196617 ADC196587:ADC196617 AMY196587:AMY196617 AWU196587:AWU196617 BGQ196587:BGQ196617 BQM196587:BQM196617 CAI196587:CAI196617 CKE196587:CKE196617 CUA196587:CUA196617 DDW196587:DDW196617 DNS196587:DNS196617 DXO196587:DXO196617 EHK196587:EHK196617 ERG196587:ERG196617 FBC196587:FBC196617 FKY196587:FKY196617 FUU196587:FUU196617 GEQ196587:GEQ196617 GOM196587:GOM196617 GYI196587:GYI196617 HIE196587:HIE196617 HSA196587:HSA196617 IBW196587:IBW196617 ILS196587:ILS196617 IVO196587:IVO196617 JFK196587:JFK196617 JPG196587:JPG196617 JZC196587:JZC196617 KIY196587:KIY196617 KSU196587:KSU196617 LCQ196587:LCQ196617 LMM196587:LMM196617 LWI196587:LWI196617 MGE196587:MGE196617 MQA196587:MQA196617 MZW196587:MZW196617 NJS196587:NJS196617 NTO196587:NTO196617 ODK196587:ODK196617 ONG196587:ONG196617 OXC196587:OXC196617 PGY196587:PGY196617 PQU196587:PQU196617 QAQ196587:QAQ196617 QKM196587:QKM196617 QUI196587:QUI196617 REE196587:REE196617 ROA196587:ROA196617 RXW196587:RXW196617 SHS196587:SHS196617 SRO196587:SRO196617 TBK196587:TBK196617 TLG196587:TLG196617 TVC196587:TVC196617 UEY196587:UEY196617 UOU196587:UOU196617 UYQ196587:UYQ196617 VIM196587:VIM196617 VSI196587:VSI196617 WCE196587:WCE196617 WMA196587:WMA196617 WVW196587:WVW196617 JK262123:JK262153 TG262123:TG262153 ADC262123:ADC262153 AMY262123:AMY262153 AWU262123:AWU262153 BGQ262123:BGQ262153 BQM262123:BQM262153 CAI262123:CAI262153 CKE262123:CKE262153 CUA262123:CUA262153 DDW262123:DDW262153 DNS262123:DNS262153 DXO262123:DXO262153 EHK262123:EHK262153 ERG262123:ERG262153 FBC262123:FBC262153 FKY262123:FKY262153 FUU262123:FUU262153 GEQ262123:GEQ262153 GOM262123:GOM262153 GYI262123:GYI262153 HIE262123:HIE262153 HSA262123:HSA262153 IBW262123:IBW262153 ILS262123:ILS262153 IVO262123:IVO262153 JFK262123:JFK262153 JPG262123:JPG262153 JZC262123:JZC262153 KIY262123:KIY262153 KSU262123:KSU262153 LCQ262123:LCQ262153 LMM262123:LMM262153 LWI262123:LWI262153 MGE262123:MGE262153 MQA262123:MQA262153 MZW262123:MZW262153 NJS262123:NJS262153 NTO262123:NTO262153 ODK262123:ODK262153 ONG262123:ONG262153 OXC262123:OXC262153 PGY262123:PGY262153 PQU262123:PQU262153 QAQ262123:QAQ262153 QKM262123:QKM262153 QUI262123:QUI262153 REE262123:REE262153 ROA262123:ROA262153 RXW262123:RXW262153 SHS262123:SHS262153 SRO262123:SRO262153 TBK262123:TBK262153 TLG262123:TLG262153 TVC262123:TVC262153 UEY262123:UEY262153 UOU262123:UOU262153 UYQ262123:UYQ262153 VIM262123:VIM262153 VSI262123:VSI262153 WCE262123:WCE262153 WMA262123:WMA262153 WVW262123:WVW262153 JK327659:JK327689 TG327659:TG327689 ADC327659:ADC327689 AMY327659:AMY327689 AWU327659:AWU327689 BGQ327659:BGQ327689 BQM327659:BQM327689 CAI327659:CAI327689 CKE327659:CKE327689 CUA327659:CUA327689 DDW327659:DDW327689 DNS327659:DNS327689 DXO327659:DXO327689 EHK327659:EHK327689 ERG327659:ERG327689 FBC327659:FBC327689 FKY327659:FKY327689 FUU327659:FUU327689 GEQ327659:GEQ327689 GOM327659:GOM327689 GYI327659:GYI327689 HIE327659:HIE327689 HSA327659:HSA327689 IBW327659:IBW327689 ILS327659:ILS327689 IVO327659:IVO327689 JFK327659:JFK327689 JPG327659:JPG327689 JZC327659:JZC327689 KIY327659:KIY327689 KSU327659:KSU327689 LCQ327659:LCQ327689 LMM327659:LMM327689 LWI327659:LWI327689 MGE327659:MGE327689 MQA327659:MQA327689 MZW327659:MZW327689 NJS327659:NJS327689 NTO327659:NTO327689 ODK327659:ODK327689 ONG327659:ONG327689 OXC327659:OXC327689 PGY327659:PGY327689 PQU327659:PQU327689 QAQ327659:QAQ327689 QKM327659:QKM327689 QUI327659:QUI327689 REE327659:REE327689 ROA327659:ROA327689 RXW327659:RXW327689 SHS327659:SHS327689 SRO327659:SRO327689 TBK327659:TBK327689 TLG327659:TLG327689 TVC327659:TVC327689 UEY327659:UEY327689 UOU327659:UOU327689 UYQ327659:UYQ327689 VIM327659:VIM327689 VSI327659:VSI327689 WCE327659:WCE327689 WMA327659:WMA327689 WVW327659:WVW327689 JK393195:JK393225 TG393195:TG393225 ADC393195:ADC393225 AMY393195:AMY393225 AWU393195:AWU393225 BGQ393195:BGQ393225 BQM393195:BQM393225 CAI393195:CAI393225 CKE393195:CKE393225 CUA393195:CUA393225 DDW393195:DDW393225 DNS393195:DNS393225 DXO393195:DXO393225 EHK393195:EHK393225 ERG393195:ERG393225 FBC393195:FBC393225 FKY393195:FKY393225 FUU393195:FUU393225 GEQ393195:GEQ393225 GOM393195:GOM393225 GYI393195:GYI393225 HIE393195:HIE393225 HSA393195:HSA393225 IBW393195:IBW393225 ILS393195:ILS393225 IVO393195:IVO393225 JFK393195:JFK393225 JPG393195:JPG393225 JZC393195:JZC393225 KIY393195:KIY393225 KSU393195:KSU393225 LCQ393195:LCQ393225 LMM393195:LMM393225 LWI393195:LWI393225 MGE393195:MGE393225 MQA393195:MQA393225 MZW393195:MZW393225 NJS393195:NJS393225 NTO393195:NTO393225 ODK393195:ODK393225 ONG393195:ONG393225 OXC393195:OXC393225 PGY393195:PGY393225 PQU393195:PQU393225 QAQ393195:QAQ393225 QKM393195:QKM393225 QUI393195:QUI393225 REE393195:REE393225 ROA393195:ROA393225 RXW393195:RXW393225 SHS393195:SHS393225 SRO393195:SRO393225 TBK393195:TBK393225 TLG393195:TLG393225 TVC393195:TVC393225 UEY393195:UEY393225 UOU393195:UOU393225 UYQ393195:UYQ393225 VIM393195:VIM393225 VSI393195:VSI393225 WCE393195:WCE393225 WMA393195:WMA393225 WVW393195:WVW393225 JK458731:JK458761 TG458731:TG458761 ADC458731:ADC458761 AMY458731:AMY458761 AWU458731:AWU458761 BGQ458731:BGQ458761 BQM458731:BQM458761 CAI458731:CAI458761 CKE458731:CKE458761 CUA458731:CUA458761 DDW458731:DDW458761 DNS458731:DNS458761 DXO458731:DXO458761 EHK458731:EHK458761 ERG458731:ERG458761 FBC458731:FBC458761 FKY458731:FKY458761 FUU458731:FUU458761 GEQ458731:GEQ458761 GOM458731:GOM458761 GYI458731:GYI458761 HIE458731:HIE458761 HSA458731:HSA458761 IBW458731:IBW458761 ILS458731:ILS458761 IVO458731:IVO458761 JFK458731:JFK458761 JPG458731:JPG458761 JZC458731:JZC458761 KIY458731:KIY458761 KSU458731:KSU458761 LCQ458731:LCQ458761 LMM458731:LMM458761 LWI458731:LWI458761 MGE458731:MGE458761 MQA458731:MQA458761 MZW458731:MZW458761 NJS458731:NJS458761 NTO458731:NTO458761 ODK458731:ODK458761 ONG458731:ONG458761 OXC458731:OXC458761 PGY458731:PGY458761 PQU458731:PQU458761 QAQ458731:QAQ458761 QKM458731:QKM458761 QUI458731:QUI458761 REE458731:REE458761 ROA458731:ROA458761 RXW458731:RXW458761 SHS458731:SHS458761 SRO458731:SRO458761 TBK458731:TBK458761 TLG458731:TLG458761 TVC458731:TVC458761 UEY458731:UEY458761 UOU458731:UOU458761 UYQ458731:UYQ458761 VIM458731:VIM458761 VSI458731:VSI458761 WCE458731:WCE458761 WMA458731:WMA458761 WVW458731:WVW458761 JK524267:JK524297 TG524267:TG524297 ADC524267:ADC524297 AMY524267:AMY524297 AWU524267:AWU524297 BGQ524267:BGQ524297 BQM524267:BQM524297 CAI524267:CAI524297 CKE524267:CKE524297 CUA524267:CUA524297 DDW524267:DDW524297 DNS524267:DNS524297 DXO524267:DXO524297 EHK524267:EHK524297 ERG524267:ERG524297 FBC524267:FBC524297 FKY524267:FKY524297 FUU524267:FUU524297 GEQ524267:GEQ524297 GOM524267:GOM524297 GYI524267:GYI524297 HIE524267:HIE524297 HSA524267:HSA524297 IBW524267:IBW524297 ILS524267:ILS524297 IVO524267:IVO524297 JFK524267:JFK524297 JPG524267:JPG524297 JZC524267:JZC524297 KIY524267:KIY524297 KSU524267:KSU524297 LCQ524267:LCQ524297 LMM524267:LMM524297 LWI524267:LWI524297 MGE524267:MGE524297 MQA524267:MQA524297 MZW524267:MZW524297 NJS524267:NJS524297 NTO524267:NTO524297 ODK524267:ODK524297 ONG524267:ONG524297 OXC524267:OXC524297 PGY524267:PGY524297 PQU524267:PQU524297 QAQ524267:QAQ524297 QKM524267:QKM524297 QUI524267:QUI524297 REE524267:REE524297 ROA524267:ROA524297 RXW524267:RXW524297 SHS524267:SHS524297 SRO524267:SRO524297 TBK524267:TBK524297 TLG524267:TLG524297 TVC524267:TVC524297 UEY524267:UEY524297 UOU524267:UOU524297 UYQ524267:UYQ524297 VIM524267:VIM524297 VSI524267:VSI524297 WCE524267:WCE524297 WMA524267:WMA524297 WVW524267:WVW524297 JK589803:JK589833 TG589803:TG589833 ADC589803:ADC589833 AMY589803:AMY589833 AWU589803:AWU589833 BGQ589803:BGQ589833 BQM589803:BQM589833 CAI589803:CAI589833 CKE589803:CKE589833 CUA589803:CUA589833 DDW589803:DDW589833 DNS589803:DNS589833 DXO589803:DXO589833 EHK589803:EHK589833 ERG589803:ERG589833 FBC589803:FBC589833 FKY589803:FKY589833 FUU589803:FUU589833 GEQ589803:GEQ589833 GOM589803:GOM589833 GYI589803:GYI589833 HIE589803:HIE589833 HSA589803:HSA589833 IBW589803:IBW589833 ILS589803:ILS589833 IVO589803:IVO589833 JFK589803:JFK589833 JPG589803:JPG589833 JZC589803:JZC589833 KIY589803:KIY589833 KSU589803:KSU589833 LCQ589803:LCQ589833 LMM589803:LMM589833 LWI589803:LWI589833 MGE589803:MGE589833 MQA589803:MQA589833 MZW589803:MZW589833 NJS589803:NJS589833 NTO589803:NTO589833 ODK589803:ODK589833 ONG589803:ONG589833 OXC589803:OXC589833 PGY589803:PGY589833 PQU589803:PQU589833 QAQ589803:QAQ589833 QKM589803:QKM589833 QUI589803:QUI589833 REE589803:REE589833 ROA589803:ROA589833 RXW589803:RXW589833 SHS589803:SHS589833 SRO589803:SRO589833 TBK589803:TBK589833 TLG589803:TLG589833 TVC589803:TVC589833 UEY589803:UEY589833 UOU589803:UOU589833 UYQ589803:UYQ589833 VIM589803:VIM589833 VSI589803:VSI589833 WCE589803:WCE589833 WMA589803:WMA589833 WVW589803:WVW589833 JK655339:JK655369 TG655339:TG655369 ADC655339:ADC655369 AMY655339:AMY655369 AWU655339:AWU655369 BGQ655339:BGQ655369 BQM655339:BQM655369 CAI655339:CAI655369 CKE655339:CKE655369 CUA655339:CUA655369 DDW655339:DDW655369 DNS655339:DNS655369 DXO655339:DXO655369 EHK655339:EHK655369 ERG655339:ERG655369 FBC655339:FBC655369 FKY655339:FKY655369 FUU655339:FUU655369 GEQ655339:GEQ655369 GOM655339:GOM655369 GYI655339:GYI655369 HIE655339:HIE655369 HSA655339:HSA655369 IBW655339:IBW655369 ILS655339:ILS655369 IVO655339:IVO655369 JFK655339:JFK655369 JPG655339:JPG655369 JZC655339:JZC655369 KIY655339:KIY655369 KSU655339:KSU655369 LCQ655339:LCQ655369 LMM655339:LMM655369 LWI655339:LWI655369 MGE655339:MGE655369 MQA655339:MQA655369 MZW655339:MZW655369 NJS655339:NJS655369 NTO655339:NTO655369 ODK655339:ODK655369 ONG655339:ONG655369 OXC655339:OXC655369 PGY655339:PGY655369 PQU655339:PQU655369 QAQ655339:QAQ655369 QKM655339:QKM655369 QUI655339:QUI655369 REE655339:REE655369 ROA655339:ROA655369 RXW655339:RXW655369 SHS655339:SHS655369 SRO655339:SRO655369 TBK655339:TBK655369 TLG655339:TLG655369 TVC655339:TVC655369 UEY655339:UEY655369 UOU655339:UOU655369 UYQ655339:UYQ655369 VIM655339:VIM655369 VSI655339:VSI655369 WCE655339:WCE655369 WMA655339:WMA655369 WVW655339:WVW655369 JK720875:JK720905 TG720875:TG720905 ADC720875:ADC720905 AMY720875:AMY720905 AWU720875:AWU720905 BGQ720875:BGQ720905 BQM720875:BQM720905 CAI720875:CAI720905 CKE720875:CKE720905 CUA720875:CUA720905 DDW720875:DDW720905 DNS720875:DNS720905 DXO720875:DXO720905 EHK720875:EHK720905 ERG720875:ERG720905 FBC720875:FBC720905 FKY720875:FKY720905 FUU720875:FUU720905 GEQ720875:GEQ720905 GOM720875:GOM720905 GYI720875:GYI720905 HIE720875:HIE720905 HSA720875:HSA720905 IBW720875:IBW720905 ILS720875:ILS720905 IVO720875:IVO720905 JFK720875:JFK720905 JPG720875:JPG720905 JZC720875:JZC720905 KIY720875:KIY720905 KSU720875:KSU720905 LCQ720875:LCQ720905 LMM720875:LMM720905 LWI720875:LWI720905 MGE720875:MGE720905 MQA720875:MQA720905 MZW720875:MZW720905 NJS720875:NJS720905 NTO720875:NTO720905 ODK720875:ODK720905 ONG720875:ONG720905 OXC720875:OXC720905 PGY720875:PGY720905 PQU720875:PQU720905 QAQ720875:QAQ720905 QKM720875:QKM720905 QUI720875:QUI720905 REE720875:REE720905 ROA720875:ROA720905 RXW720875:RXW720905 SHS720875:SHS720905 SRO720875:SRO720905 TBK720875:TBK720905 TLG720875:TLG720905 TVC720875:TVC720905 UEY720875:UEY720905 UOU720875:UOU720905 UYQ720875:UYQ720905 VIM720875:VIM720905 VSI720875:VSI720905 WCE720875:WCE720905 WMA720875:WMA720905 WVW720875:WVW720905 JK786411:JK786441 TG786411:TG786441 ADC786411:ADC786441 AMY786411:AMY786441 AWU786411:AWU786441 BGQ786411:BGQ786441 BQM786411:BQM786441 CAI786411:CAI786441 CKE786411:CKE786441 CUA786411:CUA786441 DDW786411:DDW786441 DNS786411:DNS786441 DXO786411:DXO786441 EHK786411:EHK786441 ERG786411:ERG786441 FBC786411:FBC786441 FKY786411:FKY786441 FUU786411:FUU786441 GEQ786411:GEQ786441 GOM786411:GOM786441 GYI786411:GYI786441 HIE786411:HIE786441 HSA786411:HSA786441 IBW786411:IBW786441 ILS786411:ILS786441 IVO786411:IVO786441 JFK786411:JFK786441 JPG786411:JPG786441 JZC786411:JZC786441 KIY786411:KIY786441 KSU786411:KSU786441 LCQ786411:LCQ786441 LMM786411:LMM786441 LWI786411:LWI786441 MGE786411:MGE786441 MQA786411:MQA786441 MZW786411:MZW786441 NJS786411:NJS786441 NTO786411:NTO786441 ODK786411:ODK786441 ONG786411:ONG786441 OXC786411:OXC786441 PGY786411:PGY786441 PQU786411:PQU786441 QAQ786411:QAQ786441 QKM786411:QKM786441 QUI786411:QUI786441 REE786411:REE786441 ROA786411:ROA786441 RXW786411:RXW786441 SHS786411:SHS786441 SRO786411:SRO786441 TBK786411:TBK786441 TLG786411:TLG786441 TVC786411:TVC786441 UEY786411:UEY786441 UOU786411:UOU786441 UYQ786411:UYQ786441 VIM786411:VIM786441 VSI786411:VSI786441 WCE786411:WCE786441 WMA786411:WMA786441 WVW786411:WVW786441 JK851947:JK851977 TG851947:TG851977 ADC851947:ADC851977 AMY851947:AMY851977 AWU851947:AWU851977 BGQ851947:BGQ851977 BQM851947:BQM851977 CAI851947:CAI851977 CKE851947:CKE851977 CUA851947:CUA851977 DDW851947:DDW851977 DNS851947:DNS851977 DXO851947:DXO851977 EHK851947:EHK851977 ERG851947:ERG851977 FBC851947:FBC851977 FKY851947:FKY851977 FUU851947:FUU851977 GEQ851947:GEQ851977 GOM851947:GOM851977 GYI851947:GYI851977 HIE851947:HIE851977 HSA851947:HSA851977 IBW851947:IBW851977 ILS851947:ILS851977 IVO851947:IVO851977 JFK851947:JFK851977 JPG851947:JPG851977 JZC851947:JZC851977 KIY851947:KIY851977 KSU851947:KSU851977 LCQ851947:LCQ851977 LMM851947:LMM851977 LWI851947:LWI851977 MGE851947:MGE851977 MQA851947:MQA851977 MZW851947:MZW851977 NJS851947:NJS851977 NTO851947:NTO851977 ODK851947:ODK851977 ONG851947:ONG851977 OXC851947:OXC851977 PGY851947:PGY851977 PQU851947:PQU851977 QAQ851947:QAQ851977 QKM851947:QKM851977 QUI851947:QUI851977 REE851947:REE851977 ROA851947:ROA851977 RXW851947:RXW851977 SHS851947:SHS851977 SRO851947:SRO851977 TBK851947:TBK851977 TLG851947:TLG851977 TVC851947:TVC851977 UEY851947:UEY851977 UOU851947:UOU851977 UYQ851947:UYQ851977 VIM851947:VIM851977 VSI851947:VSI851977 WCE851947:WCE851977 WMA851947:WMA851977 WVW851947:WVW851977 JK917483:JK917513 TG917483:TG917513 ADC917483:ADC917513 AMY917483:AMY917513 AWU917483:AWU917513 BGQ917483:BGQ917513 BQM917483:BQM917513 CAI917483:CAI917513 CKE917483:CKE917513 CUA917483:CUA917513 DDW917483:DDW917513 DNS917483:DNS917513 DXO917483:DXO917513 EHK917483:EHK917513 ERG917483:ERG917513 FBC917483:FBC917513 FKY917483:FKY917513 FUU917483:FUU917513 GEQ917483:GEQ917513 GOM917483:GOM917513 GYI917483:GYI917513 HIE917483:HIE917513 HSA917483:HSA917513 IBW917483:IBW917513 ILS917483:ILS917513 IVO917483:IVO917513 JFK917483:JFK917513 JPG917483:JPG917513 JZC917483:JZC917513 KIY917483:KIY917513 KSU917483:KSU917513 LCQ917483:LCQ917513 LMM917483:LMM917513 LWI917483:LWI917513 MGE917483:MGE917513 MQA917483:MQA917513 MZW917483:MZW917513 NJS917483:NJS917513 NTO917483:NTO917513 ODK917483:ODK917513 ONG917483:ONG917513 OXC917483:OXC917513 PGY917483:PGY917513 PQU917483:PQU917513 QAQ917483:QAQ917513 QKM917483:QKM917513 QUI917483:QUI917513 REE917483:REE917513 ROA917483:ROA917513 RXW917483:RXW917513 SHS917483:SHS917513 SRO917483:SRO917513 TBK917483:TBK917513 TLG917483:TLG917513 TVC917483:TVC917513 UEY917483:UEY917513 UOU917483:UOU917513 UYQ917483:UYQ917513 VIM917483:VIM917513 VSI917483:VSI917513 WCE917483:WCE917513 WMA917483:WMA917513 WVW917483:WVW917513 JK983019:JK983049 TG983019:TG983049 ADC983019:ADC983049 AMY983019:AMY983049 AWU983019:AWU983049 BGQ983019:BGQ983049 BQM983019:BQM983049 CAI983019:CAI983049 CKE983019:CKE983049 CUA983019:CUA983049 DDW983019:DDW983049 DNS983019:DNS983049 DXO983019:DXO983049 EHK983019:EHK983049 ERG983019:ERG983049 FBC983019:FBC983049 FKY983019:FKY983049 FUU983019:FUU983049 GEQ983019:GEQ983049 GOM983019:GOM983049 GYI983019:GYI983049 HIE983019:HIE983049 HSA983019:HSA983049 IBW983019:IBW983049 ILS983019:ILS983049 IVO983019:IVO983049 JFK983019:JFK983049 JPG983019:JPG983049 JZC983019:JZC983049 KIY983019:KIY983049 KSU983019:KSU983049 LCQ983019:LCQ983049 LMM983019:LMM983049 LWI983019:LWI983049 MGE983019:MGE983049 MQA983019:MQA983049 MZW983019:MZW983049 NJS983019:NJS983049 NTO983019:NTO983049 ODK983019:ODK983049 ONG983019:ONG983049 OXC983019:OXC983049 PGY983019:PGY983049 PQU983019:PQU983049 QAQ983019:QAQ983049 QKM983019:QKM983049 QUI983019:QUI983049 REE983019:REE983049 ROA983019:ROA983049 RXW983019:RXW983049 SHS983019:SHS983049 SRO983019:SRO983049 TBK983019:TBK983049 TLG983019:TLG983049 TVC983019:TVC983049 UEY983019:UEY983049 UOU983019:UOU983049 UYQ983019:UYQ983049 VIM983019:VIM983049 VSI983019:VSI983049 WCE983019:WCE983049 WMA983019:WMA983049 JK4:JK20 TG4:TG20 ADC4:ADC20 AMY4:AMY20 AWU4:AWU20 BGQ4:BGQ20 BQM4:BQM20 CAI4:CAI20 CKE4:CKE20 CUA4:CUA20 DDW4:DDW20 DNS4:DNS20 DXO4:DXO20 EHK4:EHK20 ERG4:ERG20 FBC4:FBC20 FKY4:FKY20 FUU4:FUU20 GEQ4:GEQ20 GOM4:GOM20 GYI4:GYI20 HIE4:HIE20 HSA4:HSA20 IBW4:IBW20 ILS4:ILS20 IVO4:IVO20 JFK4:JFK20 JPG4:JPG20 JZC4:JZC20 KIY4:KIY20 KSU4:KSU20 LCQ4:LCQ20 LMM4:LMM20 LWI4:LWI20 MGE4:MGE20 MQA4:MQA20 MZW4:MZW20 NJS4:NJS20 NTO4:NTO20 ODK4:ODK20 ONG4:ONG20 OXC4:OXC20 PGY4:PGY20 PQU4:PQU20 QAQ4:QAQ20 QKM4:QKM20 QUI4:QUI20 REE4:REE20 ROA4:ROA20 RXW4:RXW20 SHS4:SHS20 SRO4:SRO20 TBK4:TBK20 TLG4:TLG20 TVC4:TVC20 UEY4:UEY20 UOU4:UOU20 UYQ4:UYQ20 VIM4:VIM20 VSI4:VSI20 WCE4:WCE20 WMA4:WMA20 WVW4:WVW20" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"Medellín, Rionegro, Bogotá"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JB65515:JB65545 SX65515:SX65545 ACT65515:ACT65545 AMP65515:AMP65545 AWL65515:AWL65545 BGH65515:BGH65545 BQD65515:BQD65545 BZZ65515:BZZ65545 CJV65515:CJV65545 CTR65515:CTR65545 DDN65515:DDN65545 DNJ65515:DNJ65545 DXF65515:DXF65545 EHB65515:EHB65545 EQX65515:EQX65545 FAT65515:FAT65545 FKP65515:FKP65545 FUL65515:FUL65545 GEH65515:GEH65545 GOD65515:GOD65545 GXZ65515:GXZ65545 HHV65515:HHV65545 HRR65515:HRR65545 IBN65515:IBN65545 ILJ65515:ILJ65545 IVF65515:IVF65545 JFB65515:JFB65545 JOX65515:JOX65545 JYT65515:JYT65545 KIP65515:KIP65545 KSL65515:KSL65545 LCH65515:LCH65545 LMD65515:LMD65545 LVZ65515:LVZ65545 MFV65515:MFV65545 MPR65515:MPR65545 MZN65515:MZN65545 NJJ65515:NJJ65545 NTF65515:NTF65545 ODB65515:ODB65545 OMX65515:OMX65545 OWT65515:OWT65545 PGP65515:PGP65545 PQL65515:PQL65545 QAH65515:QAH65545 QKD65515:QKD65545 QTZ65515:QTZ65545 RDV65515:RDV65545 RNR65515:RNR65545 RXN65515:RXN65545 SHJ65515:SHJ65545 SRF65515:SRF65545 TBB65515:TBB65545 TKX65515:TKX65545 TUT65515:TUT65545 UEP65515:UEP65545 UOL65515:UOL65545 UYH65515:UYH65545 VID65515:VID65545 VRZ65515:VRZ65545 WBV65515:WBV65545 WLR65515:WLR65545 WVN65515:WVN65545 JB131051:JB131081 SX131051:SX131081 ACT131051:ACT131081 AMP131051:AMP131081 AWL131051:AWL131081 BGH131051:BGH131081 BQD131051:BQD131081 BZZ131051:BZZ131081 CJV131051:CJV131081 CTR131051:CTR131081 DDN131051:DDN131081 DNJ131051:DNJ131081 DXF131051:DXF131081 EHB131051:EHB131081 EQX131051:EQX131081 FAT131051:FAT131081 FKP131051:FKP131081 FUL131051:FUL131081 GEH131051:GEH131081 GOD131051:GOD131081 GXZ131051:GXZ131081 HHV131051:HHV131081 HRR131051:HRR131081 IBN131051:IBN131081 ILJ131051:ILJ131081 IVF131051:IVF131081 JFB131051:JFB131081 JOX131051:JOX131081 JYT131051:JYT131081 KIP131051:KIP131081 KSL131051:KSL131081 LCH131051:LCH131081 LMD131051:LMD131081 LVZ131051:LVZ131081 MFV131051:MFV131081 MPR131051:MPR131081 MZN131051:MZN131081 NJJ131051:NJJ131081 NTF131051:NTF131081 ODB131051:ODB131081 OMX131051:OMX131081 OWT131051:OWT131081 PGP131051:PGP131081 PQL131051:PQL131081 QAH131051:QAH131081 QKD131051:QKD131081 QTZ131051:QTZ131081 RDV131051:RDV131081 RNR131051:RNR131081 RXN131051:RXN131081 SHJ131051:SHJ131081 SRF131051:SRF131081 TBB131051:TBB131081 TKX131051:TKX131081 TUT131051:TUT131081 UEP131051:UEP131081 UOL131051:UOL131081 UYH131051:UYH131081 VID131051:VID131081 VRZ131051:VRZ131081 WBV131051:WBV131081 WLR131051:WLR131081 WVN131051:WVN131081 JB196587:JB196617 SX196587:SX196617 ACT196587:ACT196617 AMP196587:AMP196617 AWL196587:AWL196617 BGH196587:BGH196617 BQD196587:BQD196617 BZZ196587:BZZ196617 CJV196587:CJV196617 CTR196587:CTR196617 DDN196587:DDN196617 DNJ196587:DNJ196617 DXF196587:DXF196617 EHB196587:EHB196617 EQX196587:EQX196617 FAT196587:FAT196617 FKP196587:FKP196617 FUL196587:FUL196617 GEH196587:GEH196617 GOD196587:GOD196617 GXZ196587:GXZ196617 HHV196587:HHV196617 HRR196587:HRR196617 IBN196587:IBN196617 ILJ196587:ILJ196617 IVF196587:IVF196617 JFB196587:JFB196617 JOX196587:JOX196617 JYT196587:JYT196617 KIP196587:KIP196617 KSL196587:KSL196617 LCH196587:LCH196617 LMD196587:LMD196617 LVZ196587:LVZ196617 MFV196587:MFV196617 MPR196587:MPR196617 MZN196587:MZN196617 NJJ196587:NJJ196617 NTF196587:NTF196617 ODB196587:ODB196617 OMX196587:OMX196617 OWT196587:OWT196617 PGP196587:PGP196617 PQL196587:PQL196617 QAH196587:QAH196617 QKD196587:QKD196617 QTZ196587:QTZ196617 RDV196587:RDV196617 RNR196587:RNR196617 RXN196587:RXN196617 SHJ196587:SHJ196617 SRF196587:SRF196617 TBB196587:TBB196617 TKX196587:TKX196617 TUT196587:TUT196617 UEP196587:UEP196617 UOL196587:UOL196617 UYH196587:UYH196617 VID196587:VID196617 VRZ196587:VRZ196617 WBV196587:WBV196617 WLR196587:WLR196617 WVN196587:WVN196617 JB262123:JB262153 SX262123:SX262153 ACT262123:ACT262153 AMP262123:AMP262153 AWL262123:AWL262153 BGH262123:BGH262153 BQD262123:BQD262153 BZZ262123:BZZ262153 CJV262123:CJV262153 CTR262123:CTR262153 DDN262123:DDN262153 DNJ262123:DNJ262153 DXF262123:DXF262153 EHB262123:EHB262153 EQX262123:EQX262153 FAT262123:FAT262153 FKP262123:FKP262153 FUL262123:FUL262153 GEH262123:GEH262153 GOD262123:GOD262153 GXZ262123:GXZ262153 HHV262123:HHV262153 HRR262123:HRR262153 IBN262123:IBN262153 ILJ262123:ILJ262153 IVF262123:IVF262153 JFB262123:JFB262153 JOX262123:JOX262153 JYT262123:JYT262153 KIP262123:KIP262153 KSL262123:KSL262153 LCH262123:LCH262153 LMD262123:LMD262153 LVZ262123:LVZ262153 MFV262123:MFV262153 MPR262123:MPR262153 MZN262123:MZN262153 NJJ262123:NJJ262153 NTF262123:NTF262153 ODB262123:ODB262153 OMX262123:OMX262153 OWT262123:OWT262153 PGP262123:PGP262153 PQL262123:PQL262153 QAH262123:QAH262153 QKD262123:QKD262153 QTZ262123:QTZ262153 RDV262123:RDV262153 RNR262123:RNR262153 RXN262123:RXN262153 SHJ262123:SHJ262153 SRF262123:SRF262153 TBB262123:TBB262153 TKX262123:TKX262153 TUT262123:TUT262153 UEP262123:UEP262153 UOL262123:UOL262153 UYH262123:UYH262153 VID262123:VID262153 VRZ262123:VRZ262153 WBV262123:WBV262153 WLR262123:WLR262153 WVN262123:WVN262153 JB327659:JB327689 SX327659:SX327689 ACT327659:ACT327689 AMP327659:AMP327689 AWL327659:AWL327689 BGH327659:BGH327689 BQD327659:BQD327689 BZZ327659:BZZ327689 CJV327659:CJV327689 CTR327659:CTR327689 DDN327659:DDN327689 DNJ327659:DNJ327689 DXF327659:DXF327689 EHB327659:EHB327689 EQX327659:EQX327689 FAT327659:FAT327689 FKP327659:FKP327689 FUL327659:FUL327689 GEH327659:GEH327689 GOD327659:GOD327689 GXZ327659:GXZ327689 HHV327659:HHV327689 HRR327659:HRR327689 IBN327659:IBN327689 ILJ327659:ILJ327689 IVF327659:IVF327689 JFB327659:JFB327689 JOX327659:JOX327689 JYT327659:JYT327689 KIP327659:KIP327689 KSL327659:KSL327689 LCH327659:LCH327689 LMD327659:LMD327689 LVZ327659:LVZ327689 MFV327659:MFV327689 MPR327659:MPR327689 MZN327659:MZN327689 NJJ327659:NJJ327689 NTF327659:NTF327689 ODB327659:ODB327689 OMX327659:OMX327689 OWT327659:OWT327689 PGP327659:PGP327689 PQL327659:PQL327689 QAH327659:QAH327689 QKD327659:QKD327689 QTZ327659:QTZ327689 RDV327659:RDV327689 RNR327659:RNR327689 RXN327659:RXN327689 SHJ327659:SHJ327689 SRF327659:SRF327689 TBB327659:TBB327689 TKX327659:TKX327689 TUT327659:TUT327689 UEP327659:UEP327689 UOL327659:UOL327689 UYH327659:UYH327689 VID327659:VID327689 VRZ327659:VRZ327689 WBV327659:WBV327689 WLR327659:WLR327689 WVN327659:WVN327689 JB393195:JB393225 SX393195:SX393225 ACT393195:ACT393225 AMP393195:AMP393225 AWL393195:AWL393225 BGH393195:BGH393225 BQD393195:BQD393225 BZZ393195:BZZ393225 CJV393195:CJV393225 CTR393195:CTR393225 DDN393195:DDN393225 DNJ393195:DNJ393225 DXF393195:DXF393225 EHB393195:EHB393225 EQX393195:EQX393225 FAT393195:FAT393225 FKP393195:FKP393225 FUL393195:FUL393225 GEH393195:GEH393225 GOD393195:GOD393225 GXZ393195:GXZ393225 HHV393195:HHV393225 HRR393195:HRR393225 IBN393195:IBN393225 ILJ393195:ILJ393225 IVF393195:IVF393225 JFB393195:JFB393225 JOX393195:JOX393225 JYT393195:JYT393225 KIP393195:KIP393225 KSL393195:KSL393225 LCH393195:LCH393225 LMD393195:LMD393225 LVZ393195:LVZ393225 MFV393195:MFV393225 MPR393195:MPR393225 MZN393195:MZN393225 NJJ393195:NJJ393225 NTF393195:NTF393225 ODB393195:ODB393225 OMX393195:OMX393225 OWT393195:OWT393225 PGP393195:PGP393225 PQL393195:PQL393225 QAH393195:QAH393225 QKD393195:QKD393225 QTZ393195:QTZ393225 RDV393195:RDV393225 RNR393195:RNR393225 RXN393195:RXN393225 SHJ393195:SHJ393225 SRF393195:SRF393225 TBB393195:TBB393225 TKX393195:TKX393225 TUT393195:TUT393225 UEP393195:UEP393225 UOL393195:UOL393225 UYH393195:UYH393225 VID393195:VID393225 VRZ393195:VRZ393225 WBV393195:WBV393225 WLR393195:WLR393225 WVN393195:WVN393225 JB458731:JB458761 SX458731:SX458761 ACT458731:ACT458761 AMP458731:AMP458761 AWL458731:AWL458761 BGH458731:BGH458761 BQD458731:BQD458761 BZZ458731:BZZ458761 CJV458731:CJV458761 CTR458731:CTR458761 DDN458731:DDN458761 DNJ458731:DNJ458761 DXF458731:DXF458761 EHB458731:EHB458761 EQX458731:EQX458761 FAT458731:FAT458761 FKP458731:FKP458761 FUL458731:FUL458761 GEH458731:GEH458761 GOD458731:GOD458761 GXZ458731:GXZ458761 HHV458731:HHV458761 HRR458731:HRR458761 IBN458731:IBN458761 ILJ458731:ILJ458761 IVF458731:IVF458761 JFB458731:JFB458761 JOX458731:JOX458761 JYT458731:JYT458761 KIP458731:KIP458761 KSL458731:KSL458761 LCH458731:LCH458761 LMD458731:LMD458761 LVZ458731:LVZ458761 MFV458731:MFV458761 MPR458731:MPR458761 MZN458731:MZN458761 NJJ458731:NJJ458761 NTF458731:NTF458761 ODB458731:ODB458761 OMX458731:OMX458761 OWT458731:OWT458761 PGP458731:PGP458761 PQL458731:PQL458761 QAH458731:QAH458761 QKD458731:QKD458761 QTZ458731:QTZ458761 RDV458731:RDV458761 RNR458731:RNR458761 RXN458731:RXN458761 SHJ458731:SHJ458761 SRF458731:SRF458761 TBB458731:TBB458761 TKX458731:TKX458761 TUT458731:TUT458761 UEP458731:UEP458761 UOL458731:UOL458761 UYH458731:UYH458761 VID458731:VID458761 VRZ458731:VRZ458761 WBV458731:WBV458761 WLR458731:WLR458761 WVN458731:WVN458761 JB524267:JB524297 SX524267:SX524297 ACT524267:ACT524297 AMP524267:AMP524297 AWL524267:AWL524297 BGH524267:BGH524297 BQD524267:BQD524297 BZZ524267:BZZ524297 CJV524267:CJV524297 CTR524267:CTR524297 DDN524267:DDN524297 DNJ524267:DNJ524297 DXF524267:DXF524297 EHB524267:EHB524297 EQX524267:EQX524297 FAT524267:FAT524297 FKP524267:FKP524297 FUL524267:FUL524297 GEH524267:GEH524297 GOD524267:GOD524297 GXZ524267:GXZ524297 HHV524267:HHV524297 HRR524267:HRR524297 IBN524267:IBN524297 ILJ524267:ILJ524297 IVF524267:IVF524297 JFB524267:JFB524297 JOX524267:JOX524297 JYT524267:JYT524297 KIP524267:KIP524297 KSL524267:KSL524297 LCH524267:LCH524297 LMD524267:LMD524297 LVZ524267:LVZ524297 MFV524267:MFV524297 MPR524267:MPR524297 MZN524267:MZN524297 NJJ524267:NJJ524297 NTF524267:NTF524297 ODB524267:ODB524297 OMX524267:OMX524297 OWT524267:OWT524297 PGP524267:PGP524297 PQL524267:PQL524297 QAH524267:QAH524297 QKD524267:QKD524297 QTZ524267:QTZ524297 RDV524267:RDV524297 RNR524267:RNR524297 RXN524267:RXN524297 SHJ524267:SHJ524297 SRF524267:SRF524297 TBB524267:TBB524297 TKX524267:TKX524297 TUT524267:TUT524297 UEP524267:UEP524297 UOL524267:UOL524297 UYH524267:UYH524297 VID524267:VID524297 VRZ524267:VRZ524297 WBV524267:WBV524297 WLR524267:WLR524297 WVN524267:WVN524297 JB589803:JB589833 SX589803:SX589833 ACT589803:ACT589833 AMP589803:AMP589833 AWL589803:AWL589833 BGH589803:BGH589833 BQD589803:BQD589833 BZZ589803:BZZ589833 CJV589803:CJV589833 CTR589803:CTR589833 DDN589803:DDN589833 DNJ589803:DNJ589833 DXF589803:DXF589833 EHB589803:EHB589833 EQX589803:EQX589833 FAT589803:FAT589833 FKP589803:FKP589833 FUL589803:FUL589833 GEH589803:GEH589833 GOD589803:GOD589833 GXZ589803:GXZ589833 HHV589803:HHV589833 HRR589803:HRR589833 IBN589803:IBN589833 ILJ589803:ILJ589833 IVF589803:IVF589833 JFB589803:JFB589833 JOX589803:JOX589833 JYT589803:JYT589833 KIP589803:KIP589833 KSL589803:KSL589833 LCH589803:LCH589833 LMD589803:LMD589833 LVZ589803:LVZ589833 MFV589803:MFV589833 MPR589803:MPR589833 MZN589803:MZN589833 NJJ589803:NJJ589833 NTF589803:NTF589833 ODB589803:ODB589833 OMX589803:OMX589833 OWT589803:OWT589833 PGP589803:PGP589833 PQL589803:PQL589833 QAH589803:QAH589833 QKD589803:QKD589833 QTZ589803:QTZ589833 RDV589803:RDV589833 RNR589803:RNR589833 RXN589803:RXN589833 SHJ589803:SHJ589833 SRF589803:SRF589833 TBB589803:TBB589833 TKX589803:TKX589833 TUT589803:TUT589833 UEP589803:UEP589833 UOL589803:UOL589833 UYH589803:UYH589833 VID589803:VID589833 VRZ589803:VRZ589833 WBV589803:WBV589833 WLR589803:WLR589833 WVN589803:WVN589833 JB655339:JB655369 SX655339:SX655369 ACT655339:ACT655369 AMP655339:AMP655369 AWL655339:AWL655369 BGH655339:BGH655369 BQD655339:BQD655369 BZZ655339:BZZ655369 CJV655339:CJV655369 CTR655339:CTR655369 DDN655339:DDN655369 DNJ655339:DNJ655369 DXF655339:DXF655369 EHB655339:EHB655369 EQX655339:EQX655369 FAT655339:FAT655369 FKP655339:FKP655369 FUL655339:FUL655369 GEH655339:GEH655369 GOD655339:GOD655369 GXZ655339:GXZ655369 HHV655339:HHV655369 HRR655339:HRR655369 IBN655339:IBN655369 ILJ655339:ILJ655369 IVF655339:IVF655369 JFB655339:JFB655369 JOX655339:JOX655369 JYT655339:JYT655369 KIP655339:KIP655369 KSL655339:KSL655369 LCH655339:LCH655369 LMD655339:LMD655369 LVZ655339:LVZ655369 MFV655339:MFV655369 MPR655339:MPR655369 MZN655339:MZN655369 NJJ655339:NJJ655369 NTF655339:NTF655369 ODB655339:ODB655369 OMX655339:OMX655369 OWT655339:OWT655369 PGP655339:PGP655369 PQL655339:PQL655369 QAH655339:QAH655369 QKD655339:QKD655369 QTZ655339:QTZ655369 RDV655339:RDV655369 RNR655339:RNR655369 RXN655339:RXN655369 SHJ655339:SHJ655369 SRF655339:SRF655369 TBB655339:TBB655369 TKX655339:TKX655369 TUT655339:TUT655369 UEP655339:UEP655369 UOL655339:UOL655369 UYH655339:UYH655369 VID655339:VID655369 VRZ655339:VRZ655369 WBV655339:WBV655369 WLR655339:WLR655369 WVN655339:WVN655369 JB720875:JB720905 SX720875:SX720905 ACT720875:ACT720905 AMP720875:AMP720905 AWL720875:AWL720905 BGH720875:BGH720905 BQD720875:BQD720905 BZZ720875:BZZ720905 CJV720875:CJV720905 CTR720875:CTR720905 DDN720875:DDN720905 DNJ720875:DNJ720905 DXF720875:DXF720905 EHB720875:EHB720905 EQX720875:EQX720905 FAT720875:FAT720905 FKP720875:FKP720905 FUL720875:FUL720905 GEH720875:GEH720905 GOD720875:GOD720905 GXZ720875:GXZ720905 HHV720875:HHV720905 HRR720875:HRR720905 IBN720875:IBN720905 ILJ720875:ILJ720905 IVF720875:IVF720905 JFB720875:JFB720905 JOX720875:JOX720905 JYT720875:JYT720905 KIP720875:KIP720905 KSL720875:KSL720905 LCH720875:LCH720905 LMD720875:LMD720905 LVZ720875:LVZ720905 MFV720875:MFV720905 MPR720875:MPR720905 MZN720875:MZN720905 NJJ720875:NJJ720905 NTF720875:NTF720905 ODB720875:ODB720905 OMX720875:OMX720905 OWT720875:OWT720905 PGP720875:PGP720905 PQL720875:PQL720905 QAH720875:QAH720905 QKD720875:QKD720905 QTZ720875:QTZ720905 RDV720875:RDV720905 RNR720875:RNR720905 RXN720875:RXN720905 SHJ720875:SHJ720905 SRF720875:SRF720905 TBB720875:TBB720905 TKX720875:TKX720905 TUT720875:TUT720905 UEP720875:UEP720905 UOL720875:UOL720905 UYH720875:UYH720905 VID720875:VID720905 VRZ720875:VRZ720905 WBV720875:WBV720905 WLR720875:WLR720905 WVN720875:WVN720905 JB786411:JB786441 SX786411:SX786441 ACT786411:ACT786441 AMP786411:AMP786441 AWL786411:AWL786441 BGH786411:BGH786441 BQD786411:BQD786441 BZZ786411:BZZ786441 CJV786411:CJV786441 CTR786411:CTR786441 DDN786411:DDN786441 DNJ786411:DNJ786441 DXF786411:DXF786441 EHB786411:EHB786441 EQX786411:EQX786441 FAT786411:FAT786441 FKP786411:FKP786441 FUL786411:FUL786441 GEH786411:GEH786441 GOD786411:GOD786441 GXZ786411:GXZ786441 HHV786411:HHV786441 HRR786411:HRR786441 IBN786411:IBN786441 ILJ786411:ILJ786441 IVF786411:IVF786441 JFB786411:JFB786441 JOX786411:JOX786441 JYT786411:JYT786441 KIP786411:KIP786441 KSL786411:KSL786441 LCH786411:LCH786441 LMD786411:LMD786441 LVZ786411:LVZ786441 MFV786411:MFV786441 MPR786411:MPR786441 MZN786411:MZN786441 NJJ786411:NJJ786441 NTF786411:NTF786441 ODB786411:ODB786441 OMX786411:OMX786441 OWT786411:OWT786441 PGP786411:PGP786441 PQL786411:PQL786441 QAH786411:QAH786441 QKD786411:QKD786441 QTZ786411:QTZ786441 RDV786411:RDV786441 RNR786411:RNR786441 RXN786411:RXN786441 SHJ786411:SHJ786441 SRF786411:SRF786441 TBB786411:TBB786441 TKX786411:TKX786441 TUT786411:TUT786441 UEP786411:UEP786441 UOL786411:UOL786441 UYH786411:UYH786441 VID786411:VID786441 VRZ786411:VRZ786441 WBV786411:WBV786441 WLR786411:WLR786441 WVN786411:WVN786441 JB851947:JB851977 SX851947:SX851977 ACT851947:ACT851977 AMP851947:AMP851977 AWL851947:AWL851977 BGH851947:BGH851977 BQD851947:BQD851977 BZZ851947:BZZ851977 CJV851947:CJV851977 CTR851947:CTR851977 DDN851947:DDN851977 DNJ851947:DNJ851977 DXF851947:DXF851977 EHB851947:EHB851977 EQX851947:EQX851977 FAT851947:FAT851977 FKP851947:FKP851977 FUL851947:FUL851977 GEH851947:GEH851977 GOD851947:GOD851977 GXZ851947:GXZ851977 HHV851947:HHV851977 HRR851947:HRR851977 IBN851947:IBN851977 ILJ851947:ILJ851977 IVF851947:IVF851977 JFB851947:JFB851977 JOX851947:JOX851977 JYT851947:JYT851977 KIP851947:KIP851977 KSL851947:KSL851977 LCH851947:LCH851977 LMD851947:LMD851977 LVZ851947:LVZ851977 MFV851947:MFV851977 MPR851947:MPR851977 MZN851947:MZN851977 NJJ851947:NJJ851977 NTF851947:NTF851977 ODB851947:ODB851977 OMX851947:OMX851977 OWT851947:OWT851977 PGP851947:PGP851977 PQL851947:PQL851977 QAH851947:QAH851977 QKD851947:QKD851977 QTZ851947:QTZ851977 RDV851947:RDV851977 RNR851947:RNR851977 RXN851947:RXN851977 SHJ851947:SHJ851977 SRF851947:SRF851977 TBB851947:TBB851977 TKX851947:TKX851977 TUT851947:TUT851977 UEP851947:UEP851977 UOL851947:UOL851977 UYH851947:UYH851977 VID851947:VID851977 VRZ851947:VRZ851977 WBV851947:WBV851977 WLR851947:WLR851977 WVN851947:WVN851977 JB917483:JB917513 SX917483:SX917513 ACT917483:ACT917513 AMP917483:AMP917513 AWL917483:AWL917513 BGH917483:BGH917513 BQD917483:BQD917513 BZZ917483:BZZ917513 CJV917483:CJV917513 CTR917483:CTR917513 DDN917483:DDN917513 DNJ917483:DNJ917513 DXF917483:DXF917513 EHB917483:EHB917513 EQX917483:EQX917513 FAT917483:FAT917513 FKP917483:FKP917513 FUL917483:FUL917513 GEH917483:GEH917513 GOD917483:GOD917513 GXZ917483:GXZ917513 HHV917483:HHV917513 HRR917483:HRR917513 IBN917483:IBN917513 ILJ917483:ILJ917513 IVF917483:IVF917513 JFB917483:JFB917513 JOX917483:JOX917513 JYT917483:JYT917513 KIP917483:KIP917513 KSL917483:KSL917513 LCH917483:LCH917513 LMD917483:LMD917513 LVZ917483:LVZ917513 MFV917483:MFV917513 MPR917483:MPR917513 MZN917483:MZN917513 NJJ917483:NJJ917513 NTF917483:NTF917513 ODB917483:ODB917513 OMX917483:OMX917513 OWT917483:OWT917513 PGP917483:PGP917513 PQL917483:PQL917513 QAH917483:QAH917513 QKD917483:QKD917513 QTZ917483:QTZ917513 RDV917483:RDV917513 RNR917483:RNR917513 RXN917483:RXN917513 SHJ917483:SHJ917513 SRF917483:SRF917513 TBB917483:TBB917513 TKX917483:TKX917513 TUT917483:TUT917513 UEP917483:UEP917513 UOL917483:UOL917513 UYH917483:UYH917513 VID917483:VID917513 VRZ917483:VRZ917513 WBV917483:WBV917513 WLR917483:WLR917513 WVN917483:WVN917513 JB983019:JB983049 SX983019:SX983049 ACT983019:ACT983049 AMP983019:AMP983049 AWL983019:AWL983049 BGH983019:BGH983049 BQD983019:BQD983049 BZZ983019:BZZ983049 CJV983019:CJV983049 CTR983019:CTR983049 DDN983019:DDN983049 DNJ983019:DNJ983049 DXF983019:DXF983049 EHB983019:EHB983049 EQX983019:EQX983049 FAT983019:FAT983049 FKP983019:FKP983049 FUL983019:FUL983049 GEH983019:GEH983049 GOD983019:GOD983049 GXZ983019:GXZ983049 HHV983019:HHV983049 HRR983019:HRR983049 IBN983019:IBN983049 ILJ983019:ILJ983049 IVF983019:IVF983049 JFB983019:JFB983049 JOX983019:JOX983049 JYT983019:JYT983049 KIP983019:KIP983049 KSL983019:KSL983049 LCH983019:LCH983049 LMD983019:LMD983049 LVZ983019:LVZ983049 MFV983019:MFV983049 MPR983019:MPR983049 MZN983019:MZN983049 NJJ983019:NJJ983049 NTF983019:NTF983049 ODB983019:ODB983049 OMX983019:OMX983049 OWT983019:OWT983049 PGP983019:PGP983049 PQL983019:PQL983049 QAH983019:QAH983049 QKD983019:QKD983049 QTZ983019:QTZ983049 RDV983019:RDV983049 RNR983019:RNR983049 RXN983019:RXN983049 SHJ983019:SHJ983049 SRF983019:SRF983049 TBB983019:TBB983049 TKX983019:TKX983049 TUT983019:TUT983049 UEP983019:UEP983049 UOL983019:UOL983049 UYH983019:UYH983049 VID983019:VID983049 VRZ983019:VRZ983049 WBV983019:WBV983049 WLR983019:WLR983049 WVN983019:WVN983049 I983019:I983049 I65515:I65545 I131051:I131081 I196587:I196617 I262123:I262153 I327659:I327689 I393195:I393225 I458731:I458761 I524267:I524297 I589803:I589833 I655339:I655369 I720875:I720905 I786411:I786441 I851947:I851977 I917483:I917513 WVN4:WVN20 WLR4:WLR20 WBV4:WBV20 VRZ4:VRZ20 VID4:VID20 UYH4:UYH20 UOL4:UOL20 UEP4:UEP20 TUT4:TUT20 TKX4:TKX20 TBB4:TBB20 SRF4:SRF20 SHJ4:SHJ20 RXN4:RXN20 RNR4:RNR20 RDV4:RDV20 QTZ4:QTZ20 QKD4:QKD20 QAH4:QAH20 PQL4:PQL20 PGP4:PGP20 OWT4:OWT20 OMX4:OMX20 ODB4:ODB20 NTF4:NTF20 NJJ4:NJJ20 MZN4:MZN20 MPR4:MPR20 MFV4:MFV20 LVZ4:LVZ20 LMD4:LMD20 LCH4:LCH20 KSL4:KSL20 KIP4:KIP20 JYT4:JYT20 JOX4:JOX20 JFB4:JFB20 IVF4:IVF20 ILJ4:ILJ20 IBN4:IBN20 HRR4:HRR20 HHV4:HHV20 GXZ4:GXZ20 GOD4:GOD20 GEH4:GEH20 FUL4:FUL20 FKP4:FKP20 FAT4:FAT20 EQX4:EQX20 EHB4:EHB20 DXF4:DXF20 DNJ4:DNJ20 DDN4:DDN20 CTR4:CTR20 CJV4:CJV20 BZZ4:BZZ20 BQD4:BQD20 BGH4:BGH20 AWL4:AWL20 AMP4:AMP20 ACT4:ACT20 SX4:SX20 JB4:JB20" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JB65515:JB65545 SX65515:SX65545 ACT65515:ACT65545 AMP65515:AMP65545 AWL65515:AWL65545 BGH65515:BGH65545 BQD65515:BQD65545 BZZ65515:BZZ65545 CJV65515:CJV65545 CTR65515:CTR65545 DDN65515:DDN65545 DNJ65515:DNJ65545 DXF65515:DXF65545 EHB65515:EHB65545 EQX65515:EQX65545 FAT65515:FAT65545 FKP65515:FKP65545 FUL65515:FUL65545 GEH65515:GEH65545 GOD65515:GOD65545 GXZ65515:GXZ65545 HHV65515:HHV65545 HRR65515:HRR65545 IBN65515:IBN65545 ILJ65515:ILJ65545 IVF65515:IVF65545 JFB65515:JFB65545 JOX65515:JOX65545 JYT65515:JYT65545 KIP65515:KIP65545 KSL65515:KSL65545 LCH65515:LCH65545 LMD65515:LMD65545 LVZ65515:LVZ65545 MFV65515:MFV65545 MPR65515:MPR65545 MZN65515:MZN65545 NJJ65515:NJJ65545 NTF65515:NTF65545 ODB65515:ODB65545 OMX65515:OMX65545 OWT65515:OWT65545 PGP65515:PGP65545 PQL65515:PQL65545 QAH65515:QAH65545 QKD65515:QKD65545 QTZ65515:QTZ65545 RDV65515:RDV65545 RNR65515:RNR65545 RXN65515:RXN65545 SHJ65515:SHJ65545 SRF65515:SRF65545 TBB65515:TBB65545 TKX65515:TKX65545 TUT65515:TUT65545 UEP65515:UEP65545 UOL65515:UOL65545 UYH65515:UYH65545 VID65515:VID65545 VRZ65515:VRZ65545 WBV65515:WBV65545 WLR65515:WLR65545 WVN65515:WVN65545 JB131051:JB131081 SX131051:SX131081 ACT131051:ACT131081 AMP131051:AMP131081 AWL131051:AWL131081 BGH131051:BGH131081 BQD131051:BQD131081 BZZ131051:BZZ131081 CJV131051:CJV131081 CTR131051:CTR131081 DDN131051:DDN131081 DNJ131051:DNJ131081 DXF131051:DXF131081 EHB131051:EHB131081 EQX131051:EQX131081 FAT131051:FAT131081 FKP131051:FKP131081 FUL131051:FUL131081 GEH131051:GEH131081 GOD131051:GOD131081 GXZ131051:GXZ131081 HHV131051:HHV131081 HRR131051:HRR131081 IBN131051:IBN131081 ILJ131051:ILJ131081 IVF131051:IVF131081 JFB131051:JFB131081 JOX131051:JOX131081 JYT131051:JYT131081 KIP131051:KIP131081 KSL131051:KSL131081 LCH131051:LCH131081 LMD131051:LMD131081 LVZ131051:LVZ131081 MFV131051:MFV131081 MPR131051:MPR131081 MZN131051:MZN131081 NJJ131051:NJJ131081 NTF131051:NTF131081 ODB131051:ODB131081 OMX131051:OMX131081 OWT131051:OWT131081 PGP131051:PGP131081 PQL131051:PQL131081 QAH131051:QAH131081 QKD131051:QKD131081 QTZ131051:QTZ131081 RDV131051:RDV131081 RNR131051:RNR131081 RXN131051:RXN131081 SHJ131051:SHJ131081 SRF131051:SRF131081 TBB131051:TBB131081 TKX131051:TKX131081 TUT131051:TUT131081 UEP131051:UEP131081 UOL131051:UOL131081 UYH131051:UYH131081 VID131051:VID131081 VRZ131051:VRZ131081 WBV131051:WBV131081 WLR131051:WLR131081 WVN131051:WVN131081 JB196587:JB196617 SX196587:SX196617 ACT196587:ACT196617 AMP196587:AMP196617 AWL196587:AWL196617 BGH196587:BGH196617 BQD196587:BQD196617 BZZ196587:BZZ196617 CJV196587:CJV196617 CTR196587:CTR196617 DDN196587:DDN196617 DNJ196587:DNJ196617 DXF196587:DXF196617 EHB196587:EHB196617 EQX196587:EQX196617 FAT196587:FAT196617 FKP196587:FKP196617 FUL196587:FUL196617 GEH196587:GEH196617 GOD196587:GOD196617 GXZ196587:GXZ196617 HHV196587:HHV196617 HRR196587:HRR196617 IBN196587:IBN196617 ILJ196587:ILJ196617 IVF196587:IVF196617 JFB196587:JFB196617 JOX196587:JOX196617 JYT196587:JYT196617 KIP196587:KIP196617 KSL196587:KSL196617 LCH196587:LCH196617 LMD196587:LMD196617 LVZ196587:LVZ196617 MFV196587:MFV196617 MPR196587:MPR196617 MZN196587:MZN196617 NJJ196587:NJJ196617 NTF196587:NTF196617 ODB196587:ODB196617 OMX196587:OMX196617 OWT196587:OWT196617 PGP196587:PGP196617 PQL196587:PQL196617 QAH196587:QAH196617 QKD196587:QKD196617 QTZ196587:QTZ196617 RDV196587:RDV196617 RNR196587:RNR196617 RXN196587:RXN196617 SHJ196587:SHJ196617 SRF196587:SRF196617 TBB196587:TBB196617 TKX196587:TKX196617 TUT196587:TUT196617 UEP196587:UEP196617 UOL196587:UOL196617 UYH196587:UYH196617 VID196587:VID196617 VRZ196587:VRZ196617 WBV196587:WBV196617 WLR196587:WLR196617 WVN196587:WVN196617 JB262123:JB262153 SX262123:SX262153 ACT262123:ACT262153 AMP262123:AMP262153 AWL262123:AWL262153 BGH262123:BGH262153 BQD262123:BQD262153 BZZ262123:BZZ262153 CJV262123:CJV262153 CTR262123:CTR262153 DDN262123:DDN262153 DNJ262123:DNJ262153 DXF262123:DXF262153 EHB262123:EHB262153 EQX262123:EQX262153 FAT262123:FAT262153 FKP262123:FKP262153 FUL262123:FUL262153 GEH262123:GEH262153 GOD262123:GOD262153 GXZ262123:GXZ262153 HHV262123:HHV262153 HRR262123:HRR262153 IBN262123:IBN262153 ILJ262123:ILJ262153 IVF262123:IVF262153 JFB262123:JFB262153 JOX262123:JOX262153 JYT262123:JYT262153 KIP262123:KIP262153 KSL262123:KSL262153 LCH262123:LCH262153 LMD262123:LMD262153 LVZ262123:LVZ262153 MFV262123:MFV262153 MPR262123:MPR262153 MZN262123:MZN262153 NJJ262123:NJJ262153 NTF262123:NTF262153 ODB262123:ODB262153 OMX262123:OMX262153 OWT262123:OWT262153 PGP262123:PGP262153 PQL262123:PQL262153 QAH262123:QAH262153 QKD262123:QKD262153 QTZ262123:QTZ262153 RDV262123:RDV262153 RNR262123:RNR262153 RXN262123:RXN262153 SHJ262123:SHJ262153 SRF262123:SRF262153 TBB262123:TBB262153 TKX262123:TKX262153 TUT262123:TUT262153 UEP262123:UEP262153 UOL262123:UOL262153 UYH262123:UYH262153 VID262123:VID262153 VRZ262123:VRZ262153 WBV262123:WBV262153 WLR262123:WLR262153 WVN262123:WVN262153 JB327659:JB327689 SX327659:SX327689 ACT327659:ACT327689 AMP327659:AMP327689 AWL327659:AWL327689 BGH327659:BGH327689 BQD327659:BQD327689 BZZ327659:BZZ327689 CJV327659:CJV327689 CTR327659:CTR327689 DDN327659:DDN327689 DNJ327659:DNJ327689 DXF327659:DXF327689 EHB327659:EHB327689 EQX327659:EQX327689 FAT327659:FAT327689 FKP327659:FKP327689 FUL327659:FUL327689 GEH327659:GEH327689 GOD327659:GOD327689 GXZ327659:GXZ327689 HHV327659:HHV327689 HRR327659:HRR327689 IBN327659:IBN327689 ILJ327659:ILJ327689 IVF327659:IVF327689 JFB327659:JFB327689 JOX327659:JOX327689 JYT327659:JYT327689 KIP327659:KIP327689 KSL327659:KSL327689 LCH327659:LCH327689 LMD327659:LMD327689 LVZ327659:LVZ327689 MFV327659:MFV327689 MPR327659:MPR327689 MZN327659:MZN327689 NJJ327659:NJJ327689 NTF327659:NTF327689 ODB327659:ODB327689 OMX327659:OMX327689 OWT327659:OWT327689 PGP327659:PGP327689 PQL327659:PQL327689 QAH327659:QAH327689 QKD327659:QKD327689 QTZ327659:QTZ327689 RDV327659:RDV327689 RNR327659:RNR327689 RXN327659:RXN327689 SHJ327659:SHJ327689 SRF327659:SRF327689 TBB327659:TBB327689 TKX327659:TKX327689 TUT327659:TUT327689 UEP327659:UEP327689 UOL327659:UOL327689 UYH327659:UYH327689 VID327659:VID327689 VRZ327659:VRZ327689 WBV327659:WBV327689 WLR327659:WLR327689 WVN327659:WVN327689 JB393195:JB393225 SX393195:SX393225 ACT393195:ACT393225 AMP393195:AMP393225 AWL393195:AWL393225 BGH393195:BGH393225 BQD393195:BQD393225 BZZ393195:BZZ393225 CJV393195:CJV393225 CTR393195:CTR393225 DDN393195:DDN393225 DNJ393195:DNJ393225 DXF393195:DXF393225 EHB393195:EHB393225 EQX393195:EQX393225 FAT393195:FAT393225 FKP393195:FKP393225 FUL393195:FUL393225 GEH393195:GEH393225 GOD393195:GOD393225 GXZ393195:GXZ393225 HHV393195:HHV393225 HRR393195:HRR393225 IBN393195:IBN393225 ILJ393195:ILJ393225 IVF393195:IVF393225 JFB393195:JFB393225 JOX393195:JOX393225 JYT393195:JYT393225 KIP393195:KIP393225 KSL393195:KSL393225 LCH393195:LCH393225 LMD393195:LMD393225 LVZ393195:LVZ393225 MFV393195:MFV393225 MPR393195:MPR393225 MZN393195:MZN393225 NJJ393195:NJJ393225 NTF393195:NTF393225 ODB393195:ODB393225 OMX393195:OMX393225 OWT393195:OWT393225 PGP393195:PGP393225 PQL393195:PQL393225 QAH393195:QAH393225 QKD393195:QKD393225 QTZ393195:QTZ393225 RDV393195:RDV393225 RNR393195:RNR393225 RXN393195:RXN393225 SHJ393195:SHJ393225 SRF393195:SRF393225 TBB393195:TBB393225 TKX393195:TKX393225 TUT393195:TUT393225 UEP393195:UEP393225 UOL393195:UOL393225 UYH393195:UYH393225 VID393195:VID393225 VRZ393195:VRZ393225 WBV393195:WBV393225 WLR393195:WLR393225 WVN393195:WVN393225 JB458731:JB458761 SX458731:SX458761 ACT458731:ACT458761 AMP458731:AMP458761 AWL458731:AWL458761 BGH458731:BGH458761 BQD458731:BQD458761 BZZ458731:BZZ458761 CJV458731:CJV458761 CTR458731:CTR458761 DDN458731:DDN458761 DNJ458731:DNJ458761 DXF458731:DXF458761 EHB458731:EHB458761 EQX458731:EQX458761 FAT458731:FAT458761 FKP458731:FKP458761 FUL458731:FUL458761 GEH458731:GEH458761 GOD458731:GOD458761 GXZ458731:GXZ458761 HHV458731:HHV458761 HRR458731:HRR458761 IBN458731:IBN458761 ILJ458731:ILJ458761 IVF458731:IVF458761 JFB458731:JFB458761 JOX458731:JOX458761 JYT458731:JYT458761 KIP458731:KIP458761 KSL458731:KSL458761 LCH458731:LCH458761 LMD458731:LMD458761 LVZ458731:LVZ458761 MFV458731:MFV458761 MPR458731:MPR458761 MZN458731:MZN458761 NJJ458731:NJJ458761 NTF458731:NTF458761 ODB458731:ODB458761 OMX458731:OMX458761 OWT458731:OWT458761 PGP458731:PGP458761 PQL458731:PQL458761 QAH458731:QAH458761 QKD458731:QKD458761 QTZ458731:QTZ458761 RDV458731:RDV458761 RNR458731:RNR458761 RXN458731:RXN458761 SHJ458731:SHJ458761 SRF458731:SRF458761 TBB458731:TBB458761 TKX458731:TKX458761 TUT458731:TUT458761 UEP458731:UEP458761 UOL458731:UOL458761 UYH458731:UYH458761 VID458731:VID458761 VRZ458731:VRZ458761 WBV458731:WBV458761 WLR458731:WLR458761 WVN458731:WVN458761 JB524267:JB524297 SX524267:SX524297 ACT524267:ACT524297 AMP524267:AMP524297 AWL524267:AWL524297 BGH524267:BGH524297 BQD524267:BQD524297 BZZ524267:BZZ524297 CJV524267:CJV524297 CTR524267:CTR524297 DDN524267:DDN524297 DNJ524267:DNJ524297 DXF524267:DXF524297 EHB524267:EHB524297 EQX524267:EQX524297 FAT524267:FAT524297 FKP524267:FKP524297 FUL524267:FUL524297 GEH524267:GEH524297 GOD524267:GOD524297 GXZ524267:GXZ524297 HHV524267:HHV524297 HRR524267:HRR524297 IBN524267:IBN524297 ILJ524267:ILJ524297 IVF524267:IVF524297 JFB524267:JFB524297 JOX524267:JOX524297 JYT524267:JYT524297 KIP524267:KIP524297 KSL524267:KSL524297 LCH524267:LCH524297 LMD524267:LMD524297 LVZ524267:LVZ524297 MFV524267:MFV524297 MPR524267:MPR524297 MZN524267:MZN524297 NJJ524267:NJJ524297 NTF524267:NTF524297 ODB524267:ODB524297 OMX524267:OMX524297 OWT524267:OWT524297 PGP524267:PGP524297 PQL524267:PQL524297 QAH524267:QAH524297 QKD524267:QKD524297 QTZ524267:QTZ524297 RDV524267:RDV524297 RNR524267:RNR524297 RXN524267:RXN524297 SHJ524267:SHJ524297 SRF524267:SRF524297 TBB524267:TBB524297 TKX524267:TKX524297 TUT524267:TUT524297 UEP524267:UEP524297 UOL524267:UOL524297 UYH524267:UYH524297 VID524267:VID524297 VRZ524267:VRZ524297 WBV524267:WBV524297 WLR524267:WLR524297 WVN524267:WVN524297 JB589803:JB589833 SX589803:SX589833 ACT589803:ACT589833 AMP589803:AMP589833 AWL589803:AWL589833 BGH589803:BGH589833 BQD589803:BQD589833 BZZ589803:BZZ589833 CJV589803:CJV589833 CTR589803:CTR589833 DDN589803:DDN589833 DNJ589803:DNJ589833 DXF589803:DXF589833 EHB589803:EHB589833 EQX589803:EQX589833 FAT589803:FAT589833 FKP589803:FKP589833 FUL589803:FUL589833 GEH589803:GEH589833 GOD589803:GOD589833 GXZ589803:GXZ589833 HHV589803:HHV589833 HRR589803:HRR589833 IBN589803:IBN589833 ILJ589803:ILJ589833 IVF589803:IVF589833 JFB589803:JFB589833 JOX589803:JOX589833 JYT589803:JYT589833 KIP589803:KIP589833 KSL589803:KSL589833 LCH589803:LCH589833 LMD589803:LMD589833 LVZ589803:LVZ589833 MFV589803:MFV589833 MPR589803:MPR589833 MZN589803:MZN589833 NJJ589803:NJJ589833 NTF589803:NTF589833 ODB589803:ODB589833 OMX589803:OMX589833 OWT589803:OWT589833 PGP589803:PGP589833 PQL589803:PQL589833 QAH589803:QAH589833 QKD589803:QKD589833 QTZ589803:QTZ589833 RDV589803:RDV589833 RNR589803:RNR589833 RXN589803:RXN589833 SHJ589803:SHJ589833 SRF589803:SRF589833 TBB589803:TBB589833 TKX589803:TKX589833 TUT589803:TUT589833 UEP589803:UEP589833 UOL589803:UOL589833 UYH589803:UYH589833 VID589803:VID589833 VRZ589803:VRZ589833 WBV589803:WBV589833 WLR589803:WLR589833 WVN589803:WVN589833 JB655339:JB655369 SX655339:SX655369 ACT655339:ACT655369 AMP655339:AMP655369 AWL655339:AWL655369 BGH655339:BGH655369 BQD655339:BQD655369 BZZ655339:BZZ655369 CJV655339:CJV655369 CTR655339:CTR655369 DDN655339:DDN655369 DNJ655339:DNJ655369 DXF655339:DXF655369 EHB655339:EHB655369 EQX655339:EQX655369 FAT655339:FAT655369 FKP655339:FKP655369 FUL655339:FUL655369 GEH655339:GEH655369 GOD655339:GOD655369 GXZ655339:GXZ655369 HHV655339:HHV655369 HRR655339:HRR655369 IBN655339:IBN655369 ILJ655339:ILJ655369 IVF655339:IVF655369 JFB655339:JFB655369 JOX655339:JOX655369 JYT655339:JYT655369 KIP655339:KIP655369 KSL655339:KSL655369 LCH655339:LCH655369 LMD655339:LMD655369 LVZ655339:LVZ655369 MFV655339:MFV655369 MPR655339:MPR655369 MZN655339:MZN655369 NJJ655339:NJJ655369 NTF655339:NTF655369 ODB655339:ODB655369 OMX655339:OMX655369 OWT655339:OWT655369 PGP655339:PGP655369 PQL655339:PQL655369 QAH655339:QAH655369 QKD655339:QKD655369 QTZ655339:QTZ655369 RDV655339:RDV655369 RNR655339:RNR655369 RXN655339:RXN655369 SHJ655339:SHJ655369 SRF655339:SRF655369 TBB655339:TBB655369 TKX655339:TKX655369 TUT655339:TUT655369 UEP655339:UEP655369 UOL655339:UOL655369 UYH655339:UYH655369 VID655339:VID655369 VRZ655339:VRZ655369 WBV655339:WBV655369 WLR655339:WLR655369 WVN655339:WVN655369 JB720875:JB720905 SX720875:SX720905 ACT720875:ACT720905 AMP720875:AMP720905 AWL720875:AWL720905 BGH720875:BGH720905 BQD720875:BQD720905 BZZ720875:BZZ720905 CJV720875:CJV720905 CTR720875:CTR720905 DDN720875:DDN720905 DNJ720875:DNJ720905 DXF720875:DXF720905 EHB720875:EHB720905 EQX720875:EQX720905 FAT720875:FAT720905 FKP720875:FKP720905 FUL720875:FUL720905 GEH720875:GEH720905 GOD720875:GOD720905 GXZ720875:GXZ720905 HHV720875:HHV720905 HRR720875:HRR720905 IBN720875:IBN720905 ILJ720875:ILJ720905 IVF720875:IVF720905 JFB720875:JFB720905 JOX720875:JOX720905 JYT720875:JYT720905 KIP720875:KIP720905 KSL720875:KSL720905 LCH720875:LCH720905 LMD720875:LMD720905 LVZ720875:LVZ720905 MFV720875:MFV720905 MPR720875:MPR720905 MZN720875:MZN720905 NJJ720875:NJJ720905 NTF720875:NTF720905 ODB720875:ODB720905 OMX720875:OMX720905 OWT720875:OWT720905 PGP720875:PGP720905 PQL720875:PQL720905 QAH720875:QAH720905 QKD720875:QKD720905 QTZ720875:QTZ720905 RDV720875:RDV720905 RNR720875:RNR720905 RXN720875:RXN720905 SHJ720875:SHJ720905 SRF720875:SRF720905 TBB720875:TBB720905 TKX720875:TKX720905 TUT720875:TUT720905 UEP720875:UEP720905 UOL720875:UOL720905 UYH720875:UYH720905 VID720875:VID720905 VRZ720875:VRZ720905 WBV720875:WBV720905 WLR720875:WLR720905 WVN720875:WVN720905 JB786411:JB786441 SX786411:SX786441 ACT786411:ACT786441 AMP786411:AMP786441 AWL786411:AWL786441 BGH786411:BGH786441 BQD786411:BQD786441 BZZ786411:BZZ786441 CJV786411:CJV786441 CTR786411:CTR786441 DDN786411:DDN786441 DNJ786411:DNJ786441 DXF786411:DXF786441 EHB786411:EHB786441 EQX786411:EQX786441 FAT786411:FAT786441 FKP786411:FKP786441 FUL786411:FUL786441 GEH786411:GEH786441 GOD786411:GOD786441 GXZ786411:GXZ786441 HHV786411:HHV786441 HRR786411:HRR786441 IBN786411:IBN786441 ILJ786411:ILJ786441 IVF786411:IVF786441 JFB786411:JFB786441 JOX786411:JOX786441 JYT786411:JYT786441 KIP786411:KIP786441 KSL786411:KSL786441 LCH786411:LCH786441 LMD786411:LMD786441 LVZ786411:LVZ786441 MFV786411:MFV786441 MPR786411:MPR786441 MZN786411:MZN786441 NJJ786411:NJJ786441 NTF786411:NTF786441 ODB786411:ODB786441 OMX786411:OMX786441 OWT786411:OWT786441 PGP786411:PGP786441 PQL786411:PQL786441 QAH786411:QAH786441 QKD786411:QKD786441 QTZ786411:QTZ786441 RDV786411:RDV786441 RNR786411:RNR786441 RXN786411:RXN786441 SHJ786411:SHJ786441 SRF786411:SRF786441 TBB786411:TBB786441 TKX786411:TKX786441 TUT786411:TUT786441 UEP786411:UEP786441 UOL786411:UOL786441 UYH786411:UYH786441 VID786411:VID786441 VRZ786411:VRZ786441 WBV786411:WBV786441 WLR786411:WLR786441 WVN786411:WVN786441 JB851947:JB851977 SX851947:SX851977 ACT851947:ACT851977 AMP851947:AMP851977 AWL851947:AWL851977 BGH851947:BGH851977 BQD851947:BQD851977 BZZ851947:BZZ851977 CJV851947:CJV851977 CTR851947:CTR851977 DDN851947:DDN851977 DNJ851947:DNJ851977 DXF851947:DXF851977 EHB851947:EHB851977 EQX851947:EQX851977 FAT851947:FAT851977 FKP851947:FKP851977 FUL851947:FUL851977 GEH851947:GEH851977 GOD851947:GOD851977 GXZ851947:GXZ851977 HHV851947:HHV851977 HRR851947:HRR851977 IBN851947:IBN851977 ILJ851947:ILJ851977 IVF851947:IVF851977 JFB851947:JFB851977 JOX851947:JOX851977 JYT851947:JYT851977 KIP851947:KIP851977 KSL851947:KSL851977 LCH851947:LCH851977 LMD851947:LMD851977 LVZ851947:LVZ851977 MFV851947:MFV851977 MPR851947:MPR851977 MZN851947:MZN851977 NJJ851947:NJJ851977 NTF851947:NTF851977 ODB851947:ODB851977 OMX851947:OMX851977 OWT851947:OWT851977 PGP851947:PGP851977 PQL851947:PQL851977 QAH851947:QAH851977 QKD851947:QKD851977 QTZ851947:QTZ851977 RDV851947:RDV851977 RNR851947:RNR851977 RXN851947:RXN851977 SHJ851947:SHJ851977 SRF851947:SRF851977 TBB851947:TBB851977 TKX851947:TKX851977 TUT851947:TUT851977 UEP851947:UEP851977 UOL851947:UOL851977 UYH851947:UYH851977 VID851947:VID851977 VRZ851947:VRZ851977 WBV851947:WBV851977 WLR851947:WLR851977 WVN851947:WVN851977 JB917483:JB917513 SX917483:SX917513 ACT917483:ACT917513 AMP917483:AMP917513 AWL917483:AWL917513 BGH917483:BGH917513 BQD917483:BQD917513 BZZ917483:BZZ917513 CJV917483:CJV917513 CTR917483:CTR917513 DDN917483:DDN917513 DNJ917483:DNJ917513 DXF917483:DXF917513 EHB917483:EHB917513 EQX917483:EQX917513 FAT917483:FAT917513 FKP917483:FKP917513 FUL917483:FUL917513 GEH917483:GEH917513 GOD917483:GOD917513 GXZ917483:GXZ917513 HHV917483:HHV917513 HRR917483:HRR917513 IBN917483:IBN917513 ILJ917483:ILJ917513 IVF917483:IVF917513 JFB917483:JFB917513 JOX917483:JOX917513 JYT917483:JYT917513 KIP917483:KIP917513 KSL917483:KSL917513 LCH917483:LCH917513 LMD917483:LMD917513 LVZ917483:LVZ917513 MFV917483:MFV917513 MPR917483:MPR917513 MZN917483:MZN917513 NJJ917483:NJJ917513 NTF917483:NTF917513 ODB917483:ODB917513 OMX917483:OMX917513 OWT917483:OWT917513 PGP917483:PGP917513 PQL917483:PQL917513 QAH917483:QAH917513 QKD917483:QKD917513 QTZ917483:QTZ917513 RDV917483:RDV917513 RNR917483:RNR917513 RXN917483:RXN917513 SHJ917483:SHJ917513 SRF917483:SRF917513 TBB917483:TBB917513 TKX917483:TKX917513 TUT917483:TUT917513 UEP917483:UEP917513 UOL917483:UOL917513 UYH917483:UYH917513 VID917483:VID917513 VRZ917483:VRZ917513 WBV917483:WBV917513 WLR917483:WLR917513 WVN917483:WVN917513 JB983019:JB983049 SX983019:SX983049 ACT983019:ACT983049 AMP983019:AMP983049 AWL983019:AWL983049 BGH983019:BGH983049 BQD983019:BQD983049 BZZ983019:BZZ983049 CJV983019:CJV983049 CTR983019:CTR983049 DDN983019:DDN983049 DNJ983019:DNJ983049 DXF983019:DXF983049 EHB983019:EHB983049 EQX983019:EQX983049 FAT983019:FAT983049 FKP983019:FKP983049 FUL983019:FUL983049 GEH983019:GEH983049 GOD983019:GOD983049 GXZ983019:GXZ983049 HHV983019:HHV983049 HRR983019:HRR983049 IBN983019:IBN983049 ILJ983019:ILJ983049 IVF983019:IVF983049 JFB983019:JFB983049 JOX983019:JOX983049 JYT983019:JYT983049 KIP983019:KIP983049 KSL983019:KSL983049 LCH983019:LCH983049 LMD983019:LMD983049 LVZ983019:LVZ983049 MFV983019:MFV983049 MPR983019:MPR983049 MZN983019:MZN983049 NJJ983019:NJJ983049 NTF983019:NTF983049 ODB983019:ODB983049 OMX983019:OMX983049 OWT983019:OWT983049 PGP983019:PGP983049 PQL983019:PQL983049 QAH983019:QAH983049 QKD983019:QKD983049 QTZ983019:QTZ983049 RDV983019:RDV983049 RNR983019:RNR983049 RXN983019:RXN983049 SHJ983019:SHJ983049 SRF983019:SRF983049 TBB983019:TBB983049 TKX983019:TKX983049 TUT983019:TUT983049 UEP983019:UEP983049 UOL983019:UOL983049 UYH983019:UYH983049 VID983019:VID983049 VRZ983019:VRZ983049 WBV983019:WBV983049 WLR983019:WLR983049 WVN983019:WVN983049 I983019:I983049 I65515:I65545 I131051:I131081 I196587:I196617 I262123:I262153 I327659:I327689 I393195:I393225 I458731:I458761 I524267:I524297 I589803:I589833 I655339:I655369 I720875:I720905 I786411:I786441 I851947:I851977 I917483:I917513 JB4:JB20 SX4:SX20 ACT4:ACT20 AMP4:AMP20 AWL4:AWL20 BGH4:BGH20 BQD4:BQD20 BZZ4:BZZ20 CJV4:CJV20 CTR4:CTR20 DDN4:DDN20 DNJ4:DNJ20 DXF4:DXF20 EHB4:EHB20 EQX4:EQX20 FAT4:FAT20 FKP4:FKP20 FUL4:FUL20 GEH4:GEH20 GOD4:GOD20 GXZ4:GXZ20 HHV4:HHV20 HRR4:HRR20 IBN4:IBN20 ILJ4:ILJ20 IVF4:IVF20 JFB4:JFB20 JOX4:JOX20 JYT4:JYT20 KIP4:KIP20 KSL4:KSL20 LCH4:LCH20 LMD4:LMD20 LVZ4:LVZ20 MFV4:MFV20 MPR4:MPR20 MZN4:MZN20 NJJ4:NJJ20 NTF4:NTF20 ODB4:ODB20 OMX4:OMX20 OWT4:OWT20 PGP4:PGP20 PQL4:PQL20 QAH4:QAH20 QKD4:QKD20 QTZ4:QTZ20 RDV4:RDV20 RNR4:RNR20 RXN4:RXN20 SHJ4:SHJ20 SRF4:SRF20 TBB4:TBB20 TKX4:TKX20 TUT4:TUT20 UEP4:UEP20 UOL4:UOL20 UYH4:UYH20 VID4:VID20 VRZ4:VRZ20 WBV4:WBV20 WLR4:WLR20 WVN4:WVN20" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Administrativa, Apoyo logistico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVQ983019:WVQ983049 P65515:P65545 JE65515:JE65545 TA65515:TA65545 ACW65515:ACW65545 AMS65515:AMS65545 AWO65515:AWO65545 BGK65515:BGK65545 BQG65515:BQG65545 CAC65515:CAC65545 CJY65515:CJY65545 CTU65515:CTU65545 DDQ65515:DDQ65545 DNM65515:DNM65545 DXI65515:DXI65545 EHE65515:EHE65545 ERA65515:ERA65545 FAW65515:FAW65545 FKS65515:FKS65545 FUO65515:FUO65545 GEK65515:GEK65545 GOG65515:GOG65545 GYC65515:GYC65545 HHY65515:HHY65545 HRU65515:HRU65545 IBQ65515:IBQ65545 ILM65515:ILM65545 IVI65515:IVI65545 JFE65515:JFE65545 JPA65515:JPA65545 JYW65515:JYW65545 KIS65515:KIS65545 KSO65515:KSO65545 LCK65515:LCK65545 LMG65515:LMG65545 LWC65515:LWC65545 MFY65515:MFY65545 MPU65515:MPU65545 MZQ65515:MZQ65545 NJM65515:NJM65545 NTI65515:NTI65545 ODE65515:ODE65545 ONA65515:ONA65545 OWW65515:OWW65545 PGS65515:PGS65545 PQO65515:PQO65545 QAK65515:QAK65545 QKG65515:QKG65545 QUC65515:QUC65545 RDY65515:RDY65545 RNU65515:RNU65545 RXQ65515:RXQ65545 SHM65515:SHM65545 SRI65515:SRI65545 TBE65515:TBE65545 TLA65515:TLA65545 TUW65515:TUW65545 UES65515:UES65545 UOO65515:UOO65545 UYK65515:UYK65545 VIG65515:VIG65545 VSC65515:VSC65545 WBY65515:WBY65545 WLU65515:WLU65545 WVQ65515:WVQ65545 P131051:P131081 JE131051:JE131081 TA131051:TA131081 ACW131051:ACW131081 AMS131051:AMS131081 AWO131051:AWO131081 BGK131051:BGK131081 BQG131051:BQG131081 CAC131051:CAC131081 CJY131051:CJY131081 CTU131051:CTU131081 DDQ131051:DDQ131081 DNM131051:DNM131081 DXI131051:DXI131081 EHE131051:EHE131081 ERA131051:ERA131081 FAW131051:FAW131081 FKS131051:FKS131081 FUO131051:FUO131081 GEK131051:GEK131081 GOG131051:GOG131081 GYC131051:GYC131081 HHY131051:HHY131081 HRU131051:HRU131081 IBQ131051:IBQ131081 ILM131051:ILM131081 IVI131051:IVI131081 JFE131051:JFE131081 JPA131051:JPA131081 JYW131051:JYW131081 KIS131051:KIS131081 KSO131051:KSO131081 LCK131051:LCK131081 LMG131051:LMG131081 LWC131051:LWC131081 MFY131051:MFY131081 MPU131051:MPU131081 MZQ131051:MZQ131081 NJM131051:NJM131081 NTI131051:NTI131081 ODE131051:ODE131081 ONA131051:ONA131081 OWW131051:OWW131081 PGS131051:PGS131081 PQO131051:PQO131081 QAK131051:QAK131081 QKG131051:QKG131081 QUC131051:QUC131081 RDY131051:RDY131081 RNU131051:RNU131081 RXQ131051:RXQ131081 SHM131051:SHM131081 SRI131051:SRI131081 TBE131051:TBE131081 TLA131051:TLA131081 TUW131051:TUW131081 UES131051:UES131081 UOO131051:UOO131081 UYK131051:UYK131081 VIG131051:VIG131081 VSC131051:VSC131081 WBY131051:WBY131081 WLU131051:WLU131081 WVQ131051:WVQ131081 P196587:P196617 JE196587:JE196617 TA196587:TA196617 ACW196587:ACW196617 AMS196587:AMS196617 AWO196587:AWO196617 BGK196587:BGK196617 BQG196587:BQG196617 CAC196587:CAC196617 CJY196587:CJY196617 CTU196587:CTU196617 DDQ196587:DDQ196617 DNM196587:DNM196617 DXI196587:DXI196617 EHE196587:EHE196617 ERA196587:ERA196617 FAW196587:FAW196617 FKS196587:FKS196617 FUO196587:FUO196617 GEK196587:GEK196617 GOG196587:GOG196617 GYC196587:GYC196617 HHY196587:HHY196617 HRU196587:HRU196617 IBQ196587:IBQ196617 ILM196587:ILM196617 IVI196587:IVI196617 JFE196587:JFE196617 JPA196587:JPA196617 JYW196587:JYW196617 KIS196587:KIS196617 KSO196587:KSO196617 LCK196587:LCK196617 LMG196587:LMG196617 LWC196587:LWC196617 MFY196587:MFY196617 MPU196587:MPU196617 MZQ196587:MZQ196617 NJM196587:NJM196617 NTI196587:NTI196617 ODE196587:ODE196617 ONA196587:ONA196617 OWW196587:OWW196617 PGS196587:PGS196617 PQO196587:PQO196617 QAK196587:QAK196617 QKG196587:QKG196617 QUC196587:QUC196617 RDY196587:RDY196617 RNU196587:RNU196617 RXQ196587:RXQ196617 SHM196587:SHM196617 SRI196587:SRI196617 TBE196587:TBE196617 TLA196587:TLA196617 TUW196587:TUW196617 UES196587:UES196617 UOO196587:UOO196617 UYK196587:UYK196617 VIG196587:VIG196617 VSC196587:VSC196617 WBY196587:WBY196617 WLU196587:WLU196617 WVQ196587:WVQ196617 P262123:P262153 JE262123:JE262153 TA262123:TA262153 ACW262123:ACW262153 AMS262123:AMS262153 AWO262123:AWO262153 BGK262123:BGK262153 BQG262123:BQG262153 CAC262123:CAC262153 CJY262123:CJY262153 CTU262123:CTU262153 DDQ262123:DDQ262153 DNM262123:DNM262153 DXI262123:DXI262153 EHE262123:EHE262153 ERA262123:ERA262153 FAW262123:FAW262153 FKS262123:FKS262153 FUO262123:FUO262153 GEK262123:GEK262153 GOG262123:GOG262153 GYC262123:GYC262153 HHY262123:HHY262153 HRU262123:HRU262153 IBQ262123:IBQ262153 ILM262123:ILM262153 IVI262123:IVI262153 JFE262123:JFE262153 JPA262123:JPA262153 JYW262123:JYW262153 KIS262123:KIS262153 KSO262123:KSO262153 LCK262123:LCK262153 LMG262123:LMG262153 LWC262123:LWC262153 MFY262123:MFY262153 MPU262123:MPU262153 MZQ262123:MZQ262153 NJM262123:NJM262153 NTI262123:NTI262153 ODE262123:ODE262153 ONA262123:ONA262153 OWW262123:OWW262153 PGS262123:PGS262153 PQO262123:PQO262153 QAK262123:QAK262153 QKG262123:QKG262153 QUC262123:QUC262153 RDY262123:RDY262153 RNU262123:RNU262153 RXQ262123:RXQ262153 SHM262123:SHM262153 SRI262123:SRI262153 TBE262123:TBE262153 TLA262123:TLA262153 TUW262123:TUW262153 UES262123:UES262153 UOO262123:UOO262153 UYK262123:UYK262153 VIG262123:VIG262153 VSC262123:VSC262153 WBY262123:WBY262153 WLU262123:WLU262153 WVQ262123:WVQ262153 P327659:P327689 JE327659:JE327689 TA327659:TA327689 ACW327659:ACW327689 AMS327659:AMS327689 AWO327659:AWO327689 BGK327659:BGK327689 BQG327659:BQG327689 CAC327659:CAC327689 CJY327659:CJY327689 CTU327659:CTU327689 DDQ327659:DDQ327689 DNM327659:DNM327689 DXI327659:DXI327689 EHE327659:EHE327689 ERA327659:ERA327689 FAW327659:FAW327689 FKS327659:FKS327689 FUO327659:FUO327689 GEK327659:GEK327689 GOG327659:GOG327689 GYC327659:GYC327689 HHY327659:HHY327689 HRU327659:HRU327689 IBQ327659:IBQ327689 ILM327659:ILM327689 IVI327659:IVI327689 JFE327659:JFE327689 JPA327659:JPA327689 JYW327659:JYW327689 KIS327659:KIS327689 KSO327659:KSO327689 LCK327659:LCK327689 LMG327659:LMG327689 LWC327659:LWC327689 MFY327659:MFY327689 MPU327659:MPU327689 MZQ327659:MZQ327689 NJM327659:NJM327689 NTI327659:NTI327689 ODE327659:ODE327689 ONA327659:ONA327689 OWW327659:OWW327689 PGS327659:PGS327689 PQO327659:PQO327689 QAK327659:QAK327689 QKG327659:QKG327689 QUC327659:QUC327689 RDY327659:RDY327689 RNU327659:RNU327689 RXQ327659:RXQ327689 SHM327659:SHM327689 SRI327659:SRI327689 TBE327659:TBE327689 TLA327659:TLA327689 TUW327659:TUW327689 UES327659:UES327689 UOO327659:UOO327689 UYK327659:UYK327689 VIG327659:VIG327689 VSC327659:VSC327689 WBY327659:WBY327689 WLU327659:WLU327689 WVQ327659:WVQ327689 P393195:P393225 JE393195:JE393225 TA393195:TA393225 ACW393195:ACW393225 AMS393195:AMS393225 AWO393195:AWO393225 BGK393195:BGK393225 BQG393195:BQG393225 CAC393195:CAC393225 CJY393195:CJY393225 CTU393195:CTU393225 DDQ393195:DDQ393225 DNM393195:DNM393225 DXI393195:DXI393225 EHE393195:EHE393225 ERA393195:ERA393225 FAW393195:FAW393225 FKS393195:FKS393225 FUO393195:FUO393225 GEK393195:GEK393225 GOG393195:GOG393225 GYC393195:GYC393225 HHY393195:HHY393225 HRU393195:HRU393225 IBQ393195:IBQ393225 ILM393195:ILM393225 IVI393195:IVI393225 JFE393195:JFE393225 JPA393195:JPA393225 JYW393195:JYW393225 KIS393195:KIS393225 KSO393195:KSO393225 LCK393195:LCK393225 LMG393195:LMG393225 LWC393195:LWC393225 MFY393195:MFY393225 MPU393195:MPU393225 MZQ393195:MZQ393225 NJM393195:NJM393225 NTI393195:NTI393225 ODE393195:ODE393225 ONA393195:ONA393225 OWW393195:OWW393225 PGS393195:PGS393225 PQO393195:PQO393225 QAK393195:QAK393225 QKG393195:QKG393225 QUC393195:QUC393225 RDY393195:RDY393225 RNU393195:RNU393225 RXQ393195:RXQ393225 SHM393195:SHM393225 SRI393195:SRI393225 TBE393195:TBE393225 TLA393195:TLA393225 TUW393195:TUW393225 UES393195:UES393225 UOO393195:UOO393225 UYK393195:UYK393225 VIG393195:VIG393225 VSC393195:VSC393225 WBY393195:WBY393225 WLU393195:WLU393225 WVQ393195:WVQ393225 P458731:P458761 JE458731:JE458761 TA458731:TA458761 ACW458731:ACW458761 AMS458731:AMS458761 AWO458731:AWO458761 BGK458731:BGK458761 BQG458731:BQG458761 CAC458731:CAC458761 CJY458731:CJY458761 CTU458731:CTU458761 DDQ458731:DDQ458761 DNM458731:DNM458761 DXI458731:DXI458761 EHE458731:EHE458761 ERA458731:ERA458761 FAW458731:FAW458761 FKS458731:FKS458761 FUO458731:FUO458761 GEK458731:GEK458761 GOG458731:GOG458761 GYC458731:GYC458761 HHY458731:HHY458761 HRU458731:HRU458761 IBQ458731:IBQ458761 ILM458731:ILM458761 IVI458731:IVI458761 JFE458731:JFE458761 JPA458731:JPA458761 JYW458731:JYW458761 KIS458731:KIS458761 KSO458731:KSO458761 LCK458731:LCK458761 LMG458731:LMG458761 LWC458731:LWC458761 MFY458731:MFY458761 MPU458731:MPU458761 MZQ458731:MZQ458761 NJM458731:NJM458761 NTI458731:NTI458761 ODE458731:ODE458761 ONA458731:ONA458761 OWW458731:OWW458761 PGS458731:PGS458761 PQO458731:PQO458761 QAK458731:QAK458761 QKG458731:QKG458761 QUC458731:QUC458761 RDY458731:RDY458761 RNU458731:RNU458761 RXQ458731:RXQ458761 SHM458731:SHM458761 SRI458731:SRI458761 TBE458731:TBE458761 TLA458731:TLA458761 TUW458731:TUW458761 UES458731:UES458761 UOO458731:UOO458761 UYK458731:UYK458761 VIG458731:VIG458761 VSC458731:VSC458761 WBY458731:WBY458761 WLU458731:WLU458761 WVQ458731:WVQ458761 P524267:P524297 JE524267:JE524297 TA524267:TA524297 ACW524267:ACW524297 AMS524267:AMS524297 AWO524267:AWO524297 BGK524267:BGK524297 BQG524267:BQG524297 CAC524267:CAC524297 CJY524267:CJY524297 CTU524267:CTU524297 DDQ524267:DDQ524297 DNM524267:DNM524297 DXI524267:DXI524297 EHE524267:EHE524297 ERA524267:ERA524297 FAW524267:FAW524297 FKS524267:FKS524297 FUO524267:FUO524297 GEK524267:GEK524297 GOG524267:GOG524297 GYC524267:GYC524297 HHY524267:HHY524297 HRU524267:HRU524297 IBQ524267:IBQ524297 ILM524267:ILM524297 IVI524267:IVI524297 JFE524267:JFE524297 JPA524267:JPA524297 JYW524267:JYW524297 KIS524267:KIS524297 KSO524267:KSO524297 LCK524267:LCK524297 LMG524267:LMG524297 LWC524267:LWC524297 MFY524267:MFY524297 MPU524267:MPU524297 MZQ524267:MZQ524297 NJM524267:NJM524297 NTI524267:NTI524297 ODE524267:ODE524297 ONA524267:ONA524297 OWW524267:OWW524297 PGS524267:PGS524297 PQO524267:PQO524297 QAK524267:QAK524297 QKG524267:QKG524297 QUC524267:QUC524297 RDY524267:RDY524297 RNU524267:RNU524297 RXQ524267:RXQ524297 SHM524267:SHM524297 SRI524267:SRI524297 TBE524267:TBE524297 TLA524267:TLA524297 TUW524267:TUW524297 UES524267:UES524297 UOO524267:UOO524297 UYK524267:UYK524297 VIG524267:VIG524297 VSC524267:VSC524297 WBY524267:WBY524297 WLU524267:WLU524297 WVQ524267:WVQ524297 P589803:P589833 JE589803:JE589833 TA589803:TA589833 ACW589803:ACW589833 AMS589803:AMS589833 AWO589803:AWO589833 BGK589803:BGK589833 BQG589803:BQG589833 CAC589803:CAC589833 CJY589803:CJY589833 CTU589803:CTU589833 DDQ589803:DDQ589833 DNM589803:DNM589833 DXI589803:DXI589833 EHE589803:EHE589833 ERA589803:ERA589833 FAW589803:FAW589833 FKS589803:FKS589833 FUO589803:FUO589833 GEK589803:GEK589833 GOG589803:GOG589833 GYC589803:GYC589833 HHY589803:HHY589833 HRU589803:HRU589833 IBQ589803:IBQ589833 ILM589803:ILM589833 IVI589803:IVI589833 JFE589803:JFE589833 JPA589803:JPA589833 JYW589803:JYW589833 KIS589803:KIS589833 KSO589803:KSO589833 LCK589803:LCK589833 LMG589803:LMG589833 LWC589803:LWC589833 MFY589803:MFY589833 MPU589803:MPU589833 MZQ589803:MZQ589833 NJM589803:NJM589833 NTI589803:NTI589833 ODE589803:ODE589833 ONA589803:ONA589833 OWW589803:OWW589833 PGS589803:PGS589833 PQO589803:PQO589833 QAK589803:QAK589833 QKG589803:QKG589833 QUC589803:QUC589833 RDY589803:RDY589833 RNU589803:RNU589833 RXQ589803:RXQ589833 SHM589803:SHM589833 SRI589803:SRI589833 TBE589803:TBE589833 TLA589803:TLA589833 TUW589803:TUW589833 UES589803:UES589833 UOO589803:UOO589833 UYK589803:UYK589833 VIG589803:VIG589833 VSC589803:VSC589833 WBY589803:WBY589833 WLU589803:WLU589833 WVQ589803:WVQ589833 P655339:P655369 JE655339:JE655369 TA655339:TA655369 ACW655339:ACW655369 AMS655339:AMS655369 AWO655339:AWO655369 BGK655339:BGK655369 BQG655339:BQG655369 CAC655339:CAC655369 CJY655339:CJY655369 CTU655339:CTU655369 DDQ655339:DDQ655369 DNM655339:DNM655369 DXI655339:DXI655369 EHE655339:EHE655369 ERA655339:ERA655369 FAW655339:FAW655369 FKS655339:FKS655369 FUO655339:FUO655369 GEK655339:GEK655369 GOG655339:GOG655369 GYC655339:GYC655369 HHY655339:HHY655369 HRU655339:HRU655369 IBQ655339:IBQ655369 ILM655339:ILM655369 IVI655339:IVI655369 JFE655339:JFE655369 JPA655339:JPA655369 JYW655339:JYW655369 KIS655339:KIS655369 KSO655339:KSO655369 LCK655339:LCK655369 LMG655339:LMG655369 LWC655339:LWC655369 MFY655339:MFY655369 MPU655339:MPU655369 MZQ655339:MZQ655369 NJM655339:NJM655369 NTI655339:NTI655369 ODE655339:ODE655369 ONA655339:ONA655369 OWW655339:OWW655369 PGS655339:PGS655369 PQO655339:PQO655369 QAK655339:QAK655369 QKG655339:QKG655369 QUC655339:QUC655369 RDY655339:RDY655369 RNU655339:RNU655369 RXQ655339:RXQ655369 SHM655339:SHM655369 SRI655339:SRI655369 TBE655339:TBE655369 TLA655339:TLA655369 TUW655339:TUW655369 UES655339:UES655369 UOO655339:UOO655369 UYK655339:UYK655369 VIG655339:VIG655369 VSC655339:VSC655369 WBY655339:WBY655369 WLU655339:WLU655369 WVQ655339:WVQ655369 P720875:P720905 JE720875:JE720905 TA720875:TA720905 ACW720875:ACW720905 AMS720875:AMS720905 AWO720875:AWO720905 BGK720875:BGK720905 BQG720875:BQG720905 CAC720875:CAC720905 CJY720875:CJY720905 CTU720875:CTU720905 DDQ720875:DDQ720905 DNM720875:DNM720905 DXI720875:DXI720905 EHE720875:EHE720905 ERA720875:ERA720905 FAW720875:FAW720905 FKS720875:FKS720905 FUO720875:FUO720905 GEK720875:GEK720905 GOG720875:GOG720905 GYC720875:GYC720905 HHY720875:HHY720905 HRU720875:HRU720905 IBQ720875:IBQ720905 ILM720875:ILM720905 IVI720875:IVI720905 JFE720875:JFE720905 JPA720875:JPA720905 JYW720875:JYW720905 KIS720875:KIS720905 KSO720875:KSO720905 LCK720875:LCK720905 LMG720875:LMG720905 LWC720875:LWC720905 MFY720875:MFY720905 MPU720875:MPU720905 MZQ720875:MZQ720905 NJM720875:NJM720905 NTI720875:NTI720905 ODE720875:ODE720905 ONA720875:ONA720905 OWW720875:OWW720905 PGS720875:PGS720905 PQO720875:PQO720905 QAK720875:QAK720905 QKG720875:QKG720905 QUC720875:QUC720905 RDY720875:RDY720905 RNU720875:RNU720905 RXQ720875:RXQ720905 SHM720875:SHM720905 SRI720875:SRI720905 TBE720875:TBE720905 TLA720875:TLA720905 TUW720875:TUW720905 UES720875:UES720905 UOO720875:UOO720905 UYK720875:UYK720905 VIG720875:VIG720905 VSC720875:VSC720905 WBY720875:WBY720905 WLU720875:WLU720905 WVQ720875:WVQ720905 P786411:P786441 JE786411:JE786441 TA786411:TA786441 ACW786411:ACW786441 AMS786411:AMS786441 AWO786411:AWO786441 BGK786411:BGK786441 BQG786411:BQG786441 CAC786411:CAC786441 CJY786411:CJY786441 CTU786411:CTU786441 DDQ786411:DDQ786441 DNM786411:DNM786441 DXI786411:DXI786441 EHE786411:EHE786441 ERA786411:ERA786441 FAW786411:FAW786441 FKS786411:FKS786441 FUO786411:FUO786441 GEK786411:GEK786441 GOG786411:GOG786441 GYC786411:GYC786441 HHY786411:HHY786441 HRU786411:HRU786441 IBQ786411:IBQ786441 ILM786411:ILM786441 IVI786411:IVI786441 JFE786411:JFE786441 JPA786411:JPA786441 JYW786411:JYW786441 KIS786411:KIS786441 KSO786411:KSO786441 LCK786411:LCK786441 LMG786411:LMG786441 LWC786411:LWC786441 MFY786411:MFY786441 MPU786411:MPU786441 MZQ786411:MZQ786441 NJM786411:NJM786441 NTI786411:NTI786441 ODE786411:ODE786441 ONA786411:ONA786441 OWW786411:OWW786441 PGS786411:PGS786441 PQO786411:PQO786441 QAK786411:QAK786441 QKG786411:QKG786441 QUC786411:QUC786441 RDY786411:RDY786441 RNU786411:RNU786441 RXQ786411:RXQ786441 SHM786411:SHM786441 SRI786411:SRI786441 TBE786411:TBE786441 TLA786411:TLA786441 TUW786411:TUW786441 UES786411:UES786441 UOO786411:UOO786441 UYK786411:UYK786441 VIG786411:VIG786441 VSC786411:VSC786441 WBY786411:WBY786441 WLU786411:WLU786441 WVQ786411:WVQ786441 P851947:P851977 JE851947:JE851977 TA851947:TA851977 ACW851947:ACW851977 AMS851947:AMS851977 AWO851947:AWO851977 BGK851947:BGK851977 BQG851947:BQG851977 CAC851947:CAC851977 CJY851947:CJY851977 CTU851947:CTU851977 DDQ851947:DDQ851977 DNM851947:DNM851977 DXI851947:DXI851977 EHE851947:EHE851977 ERA851947:ERA851977 FAW851947:FAW851977 FKS851947:FKS851977 FUO851947:FUO851977 GEK851947:GEK851977 GOG851947:GOG851977 GYC851947:GYC851977 HHY851947:HHY851977 HRU851947:HRU851977 IBQ851947:IBQ851977 ILM851947:ILM851977 IVI851947:IVI851977 JFE851947:JFE851977 JPA851947:JPA851977 JYW851947:JYW851977 KIS851947:KIS851977 KSO851947:KSO851977 LCK851947:LCK851977 LMG851947:LMG851977 LWC851947:LWC851977 MFY851947:MFY851977 MPU851947:MPU851977 MZQ851947:MZQ851977 NJM851947:NJM851977 NTI851947:NTI851977 ODE851947:ODE851977 ONA851947:ONA851977 OWW851947:OWW851977 PGS851947:PGS851977 PQO851947:PQO851977 QAK851947:QAK851977 QKG851947:QKG851977 QUC851947:QUC851977 RDY851947:RDY851977 RNU851947:RNU851977 RXQ851947:RXQ851977 SHM851947:SHM851977 SRI851947:SRI851977 TBE851947:TBE851977 TLA851947:TLA851977 TUW851947:TUW851977 UES851947:UES851977 UOO851947:UOO851977 UYK851947:UYK851977 VIG851947:VIG851977 VSC851947:VSC851977 WBY851947:WBY851977 WLU851947:WLU851977 WVQ851947:WVQ851977 P917483:P917513 JE917483:JE917513 TA917483:TA917513 ACW917483:ACW917513 AMS917483:AMS917513 AWO917483:AWO917513 BGK917483:BGK917513 BQG917483:BQG917513 CAC917483:CAC917513 CJY917483:CJY917513 CTU917483:CTU917513 DDQ917483:DDQ917513 DNM917483:DNM917513 DXI917483:DXI917513 EHE917483:EHE917513 ERA917483:ERA917513 FAW917483:FAW917513 FKS917483:FKS917513 FUO917483:FUO917513 GEK917483:GEK917513 GOG917483:GOG917513 GYC917483:GYC917513 HHY917483:HHY917513 HRU917483:HRU917513 IBQ917483:IBQ917513 ILM917483:ILM917513 IVI917483:IVI917513 JFE917483:JFE917513 JPA917483:JPA917513 JYW917483:JYW917513 KIS917483:KIS917513 KSO917483:KSO917513 LCK917483:LCK917513 LMG917483:LMG917513 LWC917483:LWC917513 MFY917483:MFY917513 MPU917483:MPU917513 MZQ917483:MZQ917513 NJM917483:NJM917513 NTI917483:NTI917513 ODE917483:ODE917513 ONA917483:ONA917513 OWW917483:OWW917513 PGS917483:PGS917513 PQO917483:PQO917513 QAK917483:QAK917513 QKG917483:QKG917513 QUC917483:QUC917513 RDY917483:RDY917513 RNU917483:RNU917513 RXQ917483:RXQ917513 SHM917483:SHM917513 SRI917483:SRI917513 TBE917483:TBE917513 TLA917483:TLA917513 TUW917483:TUW917513 UES917483:UES917513 UOO917483:UOO917513 UYK917483:UYK917513 VIG917483:VIG917513 VSC917483:VSC917513 WBY917483:WBY917513 WLU917483:WLU917513 WVQ917483:WVQ917513 P983019:P983049 JE983019:JE983049 TA983019:TA983049 ACW983019:ACW983049 AMS983019:AMS983049 AWO983019:AWO983049 BGK983019:BGK983049 BQG983019:BQG983049 CAC983019:CAC983049 CJY983019:CJY983049 CTU983019:CTU983049 DDQ983019:DDQ983049 DNM983019:DNM983049 DXI983019:DXI983049 EHE983019:EHE983049 ERA983019:ERA983049 FAW983019:FAW983049 FKS983019:FKS983049 FUO983019:FUO983049 GEK983019:GEK983049 GOG983019:GOG983049 GYC983019:GYC983049 HHY983019:HHY983049 HRU983019:HRU983049 IBQ983019:IBQ983049 ILM983019:ILM983049 IVI983019:IVI983049 JFE983019:JFE983049 JPA983019:JPA983049 JYW983019:JYW983049 KIS983019:KIS983049 KSO983019:KSO983049 LCK983019:LCK983049 LMG983019:LMG983049 LWC983019:LWC983049 MFY983019:MFY983049 MPU983019:MPU983049 MZQ983019:MZQ983049 NJM983019:NJM983049 NTI983019:NTI983049 ODE983019:ODE983049 ONA983019:ONA983049 OWW983019:OWW983049 PGS983019:PGS983049 PQO983019:PQO983049 QAK983019:QAK983049 QKG983019:QKG983049 QUC983019:QUC983049 RDY983019:RDY983049 RNU983019:RNU983049 RXQ983019:RXQ983049 SHM983019:SHM983049 SRI983019:SRI983049 TBE983019:TBE983049 TLA983019:TLA983049 TUW983019:TUW983049 UES983019:UES983049 UOO983019:UOO983049 UYK983019:UYK983049 VIG983019:VIG983049 VSC983019:VSC983049 WBY983019:WBY983049 WLU983019:WLU983049 WVQ4:WVQ20 WLU4:WLU20 WBY4:WBY20 VSC4:VSC20 VIG4:VIG20 UYK4:UYK20 UOO4:UOO20 UES4:UES20 TUW4:TUW20 TLA4:TLA20 TBE4:TBE20 SRI4:SRI20 SHM4:SHM20 RXQ4:RXQ20 RNU4:RNU20 RDY4:RDY20 QUC4:QUC20 QKG4:QKG20 QAK4:QAK20 PQO4:PQO20 PGS4:PGS20 OWW4:OWW20 ONA4:ONA20 ODE4:ODE20 NTI4:NTI20 NJM4:NJM20 MZQ4:MZQ20 MPU4:MPU20 MFY4:MFY20 LWC4:LWC20 LMG4:LMG20 LCK4:LCK20 KSO4:KSO20 KIS4:KIS20 JYW4:JYW20 JPA4:JPA20 JFE4:JFE20 IVI4:IVI20 ILM4:ILM20 IBQ4:IBQ20 HRU4:HRU20 HHY4:HHY20 GYC4:GYC20 GOG4:GOG20 GEK4:GEK20 FUO4:FUO20 FKS4:FKS20 FAW4:FAW20 ERA4:ERA20 EHE4:EHE20 DXI4:DXI20 DNM4:DNM20 DDQ4:DDQ20 CTU4:CTU20 CJY4:CJY20 CAC4:CAC20 BQG4:BQG20 BGK4:BGK20 AWO4:AWO20 AMS4:AMS20 ACW4:ACW20 TA4:TA20 JE4:JE20" xr:uid="{00000000-0002-0000-0200-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVQ983019:WVQ983049 P65515:P65545 JE65515:JE65545 TA65515:TA65545 ACW65515:ACW65545 AMS65515:AMS65545 AWO65515:AWO65545 BGK65515:BGK65545 BQG65515:BQG65545 CAC65515:CAC65545 CJY65515:CJY65545 CTU65515:CTU65545 DDQ65515:DDQ65545 DNM65515:DNM65545 DXI65515:DXI65545 EHE65515:EHE65545 ERA65515:ERA65545 FAW65515:FAW65545 FKS65515:FKS65545 FUO65515:FUO65545 GEK65515:GEK65545 GOG65515:GOG65545 GYC65515:GYC65545 HHY65515:HHY65545 HRU65515:HRU65545 IBQ65515:IBQ65545 ILM65515:ILM65545 IVI65515:IVI65545 JFE65515:JFE65545 JPA65515:JPA65545 JYW65515:JYW65545 KIS65515:KIS65545 KSO65515:KSO65545 LCK65515:LCK65545 LMG65515:LMG65545 LWC65515:LWC65545 MFY65515:MFY65545 MPU65515:MPU65545 MZQ65515:MZQ65545 NJM65515:NJM65545 NTI65515:NTI65545 ODE65515:ODE65545 ONA65515:ONA65545 OWW65515:OWW65545 PGS65515:PGS65545 PQO65515:PQO65545 QAK65515:QAK65545 QKG65515:QKG65545 QUC65515:QUC65545 RDY65515:RDY65545 RNU65515:RNU65545 RXQ65515:RXQ65545 SHM65515:SHM65545 SRI65515:SRI65545 TBE65515:TBE65545 TLA65515:TLA65545 TUW65515:TUW65545 UES65515:UES65545 UOO65515:UOO65545 UYK65515:UYK65545 VIG65515:VIG65545 VSC65515:VSC65545 WBY65515:WBY65545 WLU65515:WLU65545 WVQ65515:WVQ65545 P131051:P131081 JE131051:JE131081 TA131051:TA131081 ACW131051:ACW131081 AMS131051:AMS131081 AWO131051:AWO131081 BGK131051:BGK131081 BQG131051:BQG131081 CAC131051:CAC131081 CJY131051:CJY131081 CTU131051:CTU131081 DDQ131051:DDQ131081 DNM131051:DNM131081 DXI131051:DXI131081 EHE131051:EHE131081 ERA131051:ERA131081 FAW131051:FAW131081 FKS131051:FKS131081 FUO131051:FUO131081 GEK131051:GEK131081 GOG131051:GOG131081 GYC131051:GYC131081 HHY131051:HHY131081 HRU131051:HRU131081 IBQ131051:IBQ131081 ILM131051:ILM131081 IVI131051:IVI131081 JFE131051:JFE131081 JPA131051:JPA131081 JYW131051:JYW131081 KIS131051:KIS131081 KSO131051:KSO131081 LCK131051:LCK131081 LMG131051:LMG131081 LWC131051:LWC131081 MFY131051:MFY131081 MPU131051:MPU131081 MZQ131051:MZQ131081 NJM131051:NJM131081 NTI131051:NTI131081 ODE131051:ODE131081 ONA131051:ONA131081 OWW131051:OWW131081 PGS131051:PGS131081 PQO131051:PQO131081 QAK131051:QAK131081 QKG131051:QKG131081 QUC131051:QUC131081 RDY131051:RDY131081 RNU131051:RNU131081 RXQ131051:RXQ131081 SHM131051:SHM131081 SRI131051:SRI131081 TBE131051:TBE131081 TLA131051:TLA131081 TUW131051:TUW131081 UES131051:UES131081 UOO131051:UOO131081 UYK131051:UYK131081 VIG131051:VIG131081 VSC131051:VSC131081 WBY131051:WBY131081 WLU131051:WLU131081 WVQ131051:WVQ131081 P196587:P196617 JE196587:JE196617 TA196587:TA196617 ACW196587:ACW196617 AMS196587:AMS196617 AWO196587:AWO196617 BGK196587:BGK196617 BQG196587:BQG196617 CAC196587:CAC196617 CJY196587:CJY196617 CTU196587:CTU196617 DDQ196587:DDQ196617 DNM196587:DNM196617 DXI196587:DXI196617 EHE196587:EHE196617 ERA196587:ERA196617 FAW196587:FAW196617 FKS196587:FKS196617 FUO196587:FUO196617 GEK196587:GEK196617 GOG196587:GOG196617 GYC196587:GYC196617 HHY196587:HHY196617 HRU196587:HRU196617 IBQ196587:IBQ196617 ILM196587:ILM196617 IVI196587:IVI196617 JFE196587:JFE196617 JPA196587:JPA196617 JYW196587:JYW196617 KIS196587:KIS196617 KSO196587:KSO196617 LCK196587:LCK196617 LMG196587:LMG196617 LWC196587:LWC196617 MFY196587:MFY196617 MPU196587:MPU196617 MZQ196587:MZQ196617 NJM196587:NJM196617 NTI196587:NTI196617 ODE196587:ODE196617 ONA196587:ONA196617 OWW196587:OWW196617 PGS196587:PGS196617 PQO196587:PQO196617 QAK196587:QAK196617 QKG196587:QKG196617 QUC196587:QUC196617 RDY196587:RDY196617 RNU196587:RNU196617 RXQ196587:RXQ196617 SHM196587:SHM196617 SRI196587:SRI196617 TBE196587:TBE196617 TLA196587:TLA196617 TUW196587:TUW196617 UES196587:UES196617 UOO196587:UOO196617 UYK196587:UYK196617 VIG196587:VIG196617 VSC196587:VSC196617 WBY196587:WBY196617 WLU196587:WLU196617 WVQ196587:WVQ196617 P262123:P262153 JE262123:JE262153 TA262123:TA262153 ACW262123:ACW262153 AMS262123:AMS262153 AWO262123:AWO262153 BGK262123:BGK262153 BQG262123:BQG262153 CAC262123:CAC262153 CJY262123:CJY262153 CTU262123:CTU262153 DDQ262123:DDQ262153 DNM262123:DNM262153 DXI262123:DXI262153 EHE262123:EHE262153 ERA262123:ERA262153 FAW262123:FAW262153 FKS262123:FKS262153 FUO262123:FUO262153 GEK262123:GEK262153 GOG262123:GOG262153 GYC262123:GYC262153 HHY262123:HHY262153 HRU262123:HRU262153 IBQ262123:IBQ262153 ILM262123:ILM262153 IVI262123:IVI262153 JFE262123:JFE262153 JPA262123:JPA262153 JYW262123:JYW262153 KIS262123:KIS262153 KSO262123:KSO262153 LCK262123:LCK262153 LMG262123:LMG262153 LWC262123:LWC262153 MFY262123:MFY262153 MPU262123:MPU262153 MZQ262123:MZQ262153 NJM262123:NJM262153 NTI262123:NTI262153 ODE262123:ODE262153 ONA262123:ONA262153 OWW262123:OWW262153 PGS262123:PGS262153 PQO262123:PQO262153 QAK262123:QAK262153 QKG262123:QKG262153 QUC262123:QUC262153 RDY262123:RDY262153 RNU262123:RNU262153 RXQ262123:RXQ262153 SHM262123:SHM262153 SRI262123:SRI262153 TBE262123:TBE262153 TLA262123:TLA262153 TUW262123:TUW262153 UES262123:UES262153 UOO262123:UOO262153 UYK262123:UYK262153 VIG262123:VIG262153 VSC262123:VSC262153 WBY262123:WBY262153 WLU262123:WLU262153 WVQ262123:WVQ262153 P327659:P327689 JE327659:JE327689 TA327659:TA327689 ACW327659:ACW327689 AMS327659:AMS327689 AWO327659:AWO327689 BGK327659:BGK327689 BQG327659:BQG327689 CAC327659:CAC327689 CJY327659:CJY327689 CTU327659:CTU327689 DDQ327659:DDQ327689 DNM327659:DNM327689 DXI327659:DXI327689 EHE327659:EHE327689 ERA327659:ERA327689 FAW327659:FAW327689 FKS327659:FKS327689 FUO327659:FUO327689 GEK327659:GEK327689 GOG327659:GOG327689 GYC327659:GYC327689 HHY327659:HHY327689 HRU327659:HRU327689 IBQ327659:IBQ327689 ILM327659:ILM327689 IVI327659:IVI327689 JFE327659:JFE327689 JPA327659:JPA327689 JYW327659:JYW327689 KIS327659:KIS327689 KSO327659:KSO327689 LCK327659:LCK327689 LMG327659:LMG327689 LWC327659:LWC327689 MFY327659:MFY327689 MPU327659:MPU327689 MZQ327659:MZQ327689 NJM327659:NJM327689 NTI327659:NTI327689 ODE327659:ODE327689 ONA327659:ONA327689 OWW327659:OWW327689 PGS327659:PGS327689 PQO327659:PQO327689 QAK327659:QAK327689 QKG327659:QKG327689 QUC327659:QUC327689 RDY327659:RDY327689 RNU327659:RNU327689 RXQ327659:RXQ327689 SHM327659:SHM327689 SRI327659:SRI327689 TBE327659:TBE327689 TLA327659:TLA327689 TUW327659:TUW327689 UES327659:UES327689 UOO327659:UOO327689 UYK327659:UYK327689 VIG327659:VIG327689 VSC327659:VSC327689 WBY327659:WBY327689 WLU327659:WLU327689 WVQ327659:WVQ327689 P393195:P393225 JE393195:JE393225 TA393195:TA393225 ACW393195:ACW393225 AMS393195:AMS393225 AWO393195:AWO393225 BGK393195:BGK393225 BQG393195:BQG393225 CAC393195:CAC393225 CJY393195:CJY393225 CTU393195:CTU393225 DDQ393195:DDQ393225 DNM393195:DNM393225 DXI393195:DXI393225 EHE393195:EHE393225 ERA393195:ERA393225 FAW393195:FAW393225 FKS393195:FKS393225 FUO393195:FUO393225 GEK393195:GEK393225 GOG393195:GOG393225 GYC393195:GYC393225 HHY393195:HHY393225 HRU393195:HRU393225 IBQ393195:IBQ393225 ILM393195:ILM393225 IVI393195:IVI393225 JFE393195:JFE393225 JPA393195:JPA393225 JYW393195:JYW393225 KIS393195:KIS393225 KSO393195:KSO393225 LCK393195:LCK393225 LMG393195:LMG393225 LWC393195:LWC393225 MFY393195:MFY393225 MPU393195:MPU393225 MZQ393195:MZQ393225 NJM393195:NJM393225 NTI393195:NTI393225 ODE393195:ODE393225 ONA393195:ONA393225 OWW393195:OWW393225 PGS393195:PGS393225 PQO393195:PQO393225 QAK393195:QAK393225 QKG393195:QKG393225 QUC393195:QUC393225 RDY393195:RDY393225 RNU393195:RNU393225 RXQ393195:RXQ393225 SHM393195:SHM393225 SRI393195:SRI393225 TBE393195:TBE393225 TLA393195:TLA393225 TUW393195:TUW393225 UES393195:UES393225 UOO393195:UOO393225 UYK393195:UYK393225 VIG393195:VIG393225 VSC393195:VSC393225 WBY393195:WBY393225 WLU393195:WLU393225 WVQ393195:WVQ393225 P458731:P458761 JE458731:JE458761 TA458731:TA458761 ACW458731:ACW458761 AMS458731:AMS458761 AWO458731:AWO458761 BGK458731:BGK458761 BQG458731:BQG458761 CAC458731:CAC458761 CJY458731:CJY458761 CTU458731:CTU458761 DDQ458731:DDQ458761 DNM458731:DNM458761 DXI458731:DXI458761 EHE458731:EHE458761 ERA458731:ERA458761 FAW458731:FAW458761 FKS458731:FKS458761 FUO458731:FUO458761 GEK458731:GEK458761 GOG458731:GOG458761 GYC458731:GYC458761 HHY458731:HHY458761 HRU458731:HRU458761 IBQ458731:IBQ458761 ILM458731:ILM458761 IVI458731:IVI458761 JFE458731:JFE458761 JPA458731:JPA458761 JYW458731:JYW458761 KIS458731:KIS458761 KSO458731:KSO458761 LCK458731:LCK458761 LMG458731:LMG458761 LWC458731:LWC458761 MFY458731:MFY458761 MPU458731:MPU458761 MZQ458731:MZQ458761 NJM458731:NJM458761 NTI458731:NTI458761 ODE458731:ODE458761 ONA458731:ONA458761 OWW458731:OWW458761 PGS458731:PGS458761 PQO458731:PQO458761 QAK458731:QAK458761 QKG458731:QKG458761 QUC458731:QUC458761 RDY458731:RDY458761 RNU458731:RNU458761 RXQ458731:RXQ458761 SHM458731:SHM458761 SRI458731:SRI458761 TBE458731:TBE458761 TLA458731:TLA458761 TUW458731:TUW458761 UES458731:UES458761 UOO458731:UOO458761 UYK458731:UYK458761 VIG458731:VIG458761 VSC458731:VSC458761 WBY458731:WBY458761 WLU458731:WLU458761 WVQ458731:WVQ458761 P524267:P524297 JE524267:JE524297 TA524267:TA524297 ACW524267:ACW524297 AMS524267:AMS524297 AWO524267:AWO524297 BGK524267:BGK524297 BQG524267:BQG524297 CAC524267:CAC524297 CJY524267:CJY524297 CTU524267:CTU524297 DDQ524267:DDQ524297 DNM524267:DNM524297 DXI524267:DXI524297 EHE524267:EHE524297 ERA524267:ERA524297 FAW524267:FAW524297 FKS524267:FKS524297 FUO524267:FUO524297 GEK524267:GEK524297 GOG524267:GOG524297 GYC524267:GYC524297 HHY524267:HHY524297 HRU524267:HRU524297 IBQ524267:IBQ524297 ILM524267:ILM524297 IVI524267:IVI524297 JFE524267:JFE524297 JPA524267:JPA524297 JYW524267:JYW524297 KIS524267:KIS524297 KSO524267:KSO524297 LCK524267:LCK524297 LMG524267:LMG524297 LWC524267:LWC524297 MFY524267:MFY524297 MPU524267:MPU524297 MZQ524267:MZQ524297 NJM524267:NJM524297 NTI524267:NTI524297 ODE524267:ODE524297 ONA524267:ONA524297 OWW524267:OWW524297 PGS524267:PGS524297 PQO524267:PQO524297 QAK524267:QAK524297 QKG524267:QKG524297 QUC524267:QUC524297 RDY524267:RDY524297 RNU524267:RNU524297 RXQ524267:RXQ524297 SHM524267:SHM524297 SRI524267:SRI524297 TBE524267:TBE524297 TLA524267:TLA524297 TUW524267:TUW524297 UES524267:UES524297 UOO524267:UOO524297 UYK524267:UYK524297 VIG524267:VIG524297 VSC524267:VSC524297 WBY524267:WBY524297 WLU524267:WLU524297 WVQ524267:WVQ524297 P589803:P589833 JE589803:JE589833 TA589803:TA589833 ACW589803:ACW589833 AMS589803:AMS589833 AWO589803:AWO589833 BGK589803:BGK589833 BQG589803:BQG589833 CAC589803:CAC589833 CJY589803:CJY589833 CTU589803:CTU589833 DDQ589803:DDQ589833 DNM589803:DNM589833 DXI589803:DXI589833 EHE589803:EHE589833 ERA589803:ERA589833 FAW589803:FAW589833 FKS589803:FKS589833 FUO589803:FUO589833 GEK589803:GEK589833 GOG589803:GOG589833 GYC589803:GYC589833 HHY589803:HHY589833 HRU589803:HRU589833 IBQ589803:IBQ589833 ILM589803:ILM589833 IVI589803:IVI589833 JFE589803:JFE589833 JPA589803:JPA589833 JYW589803:JYW589833 KIS589803:KIS589833 KSO589803:KSO589833 LCK589803:LCK589833 LMG589803:LMG589833 LWC589803:LWC589833 MFY589803:MFY589833 MPU589803:MPU589833 MZQ589803:MZQ589833 NJM589803:NJM589833 NTI589803:NTI589833 ODE589803:ODE589833 ONA589803:ONA589833 OWW589803:OWW589833 PGS589803:PGS589833 PQO589803:PQO589833 QAK589803:QAK589833 QKG589803:QKG589833 QUC589803:QUC589833 RDY589803:RDY589833 RNU589803:RNU589833 RXQ589803:RXQ589833 SHM589803:SHM589833 SRI589803:SRI589833 TBE589803:TBE589833 TLA589803:TLA589833 TUW589803:TUW589833 UES589803:UES589833 UOO589803:UOO589833 UYK589803:UYK589833 VIG589803:VIG589833 VSC589803:VSC589833 WBY589803:WBY589833 WLU589803:WLU589833 WVQ589803:WVQ589833 P655339:P655369 JE655339:JE655369 TA655339:TA655369 ACW655339:ACW655369 AMS655339:AMS655369 AWO655339:AWO655369 BGK655339:BGK655369 BQG655339:BQG655369 CAC655339:CAC655369 CJY655339:CJY655369 CTU655339:CTU655369 DDQ655339:DDQ655369 DNM655339:DNM655369 DXI655339:DXI655369 EHE655339:EHE655369 ERA655339:ERA655369 FAW655339:FAW655369 FKS655339:FKS655369 FUO655339:FUO655369 GEK655339:GEK655369 GOG655339:GOG655369 GYC655339:GYC655369 HHY655339:HHY655369 HRU655339:HRU655369 IBQ655339:IBQ655369 ILM655339:ILM655369 IVI655339:IVI655369 JFE655339:JFE655369 JPA655339:JPA655369 JYW655339:JYW655369 KIS655339:KIS655369 KSO655339:KSO655369 LCK655339:LCK655369 LMG655339:LMG655369 LWC655339:LWC655369 MFY655339:MFY655369 MPU655339:MPU655369 MZQ655339:MZQ655369 NJM655339:NJM655369 NTI655339:NTI655369 ODE655339:ODE655369 ONA655339:ONA655369 OWW655339:OWW655369 PGS655339:PGS655369 PQO655339:PQO655369 QAK655339:QAK655369 QKG655339:QKG655369 QUC655339:QUC655369 RDY655339:RDY655369 RNU655339:RNU655369 RXQ655339:RXQ655369 SHM655339:SHM655369 SRI655339:SRI655369 TBE655339:TBE655369 TLA655339:TLA655369 TUW655339:TUW655369 UES655339:UES655369 UOO655339:UOO655369 UYK655339:UYK655369 VIG655339:VIG655369 VSC655339:VSC655369 WBY655339:WBY655369 WLU655339:WLU655369 WVQ655339:WVQ655369 P720875:P720905 JE720875:JE720905 TA720875:TA720905 ACW720875:ACW720905 AMS720875:AMS720905 AWO720875:AWO720905 BGK720875:BGK720905 BQG720875:BQG720905 CAC720875:CAC720905 CJY720875:CJY720905 CTU720875:CTU720905 DDQ720875:DDQ720905 DNM720875:DNM720905 DXI720875:DXI720905 EHE720875:EHE720905 ERA720875:ERA720905 FAW720875:FAW720905 FKS720875:FKS720905 FUO720875:FUO720905 GEK720875:GEK720905 GOG720875:GOG720905 GYC720875:GYC720905 HHY720875:HHY720905 HRU720875:HRU720905 IBQ720875:IBQ720905 ILM720875:ILM720905 IVI720875:IVI720905 JFE720875:JFE720905 JPA720875:JPA720905 JYW720875:JYW720905 KIS720875:KIS720905 KSO720875:KSO720905 LCK720875:LCK720905 LMG720875:LMG720905 LWC720875:LWC720905 MFY720875:MFY720905 MPU720875:MPU720905 MZQ720875:MZQ720905 NJM720875:NJM720905 NTI720875:NTI720905 ODE720875:ODE720905 ONA720875:ONA720905 OWW720875:OWW720905 PGS720875:PGS720905 PQO720875:PQO720905 QAK720875:QAK720905 QKG720875:QKG720905 QUC720875:QUC720905 RDY720875:RDY720905 RNU720875:RNU720905 RXQ720875:RXQ720905 SHM720875:SHM720905 SRI720875:SRI720905 TBE720875:TBE720905 TLA720875:TLA720905 TUW720875:TUW720905 UES720875:UES720905 UOO720875:UOO720905 UYK720875:UYK720905 VIG720875:VIG720905 VSC720875:VSC720905 WBY720875:WBY720905 WLU720875:WLU720905 WVQ720875:WVQ720905 P786411:P786441 JE786411:JE786441 TA786411:TA786441 ACW786411:ACW786441 AMS786411:AMS786441 AWO786411:AWO786441 BGK786411:BGK786441 BQG786411:BQG786441 CAC786411:CAC786441 CJY786411:CJY786441 CTU786411:CTU786441 DDQ786411:DDQ786441 DNM786411:DNM786441 DXI786411:DXI786441 EHE786411:EHE786441 ERA786411:ERA786441 FAW786411:FAW786441 FKS786411:FKS786441 FUO786411:FUO786441 GEK786411:GEK786441 GOG786411:GOG786441 GYC786411:GYC786441 HHY786411:HHY786441 HRU786411:HRU786441 IBQ786411:IBQ786441 ILM786411:ILM786441 IVI786411:IVI786441 JFE786411:JFE786441 JPA786411:JPA786441 JYW786411:JYW786441 KIS786411:KIS786441 KSO786411:KSO786441 LCK786411:LCK786441 LMG786411:LMG786441 LWC786411:LWC786441 MFY786411:MFY786441 MPU786411:MPU786441 MZQ786411:MZQ786441 NJM786411:NJM786441 NTI786411:NTI786441 ODE786411:ODE786441 ONA786411:ONA786441 OWW786411:OWW786441 PGS786411:PGS786441 PQO786411:PQO786441 QAK786411:QAK786441 QKG786411:QKG786441 QUC786411:QUC786441 RDY786411:RDY786441 RNU786411:RNU786441 RXQ786411:RXQ786441 SHM786411:SHM786441 SRI786411:SRI786441 TBE786411:TBE786441 TLA786411:TLA786441 TUW786411:TUW786441 UES786411:UES786441 UOO786411:UOO786441 UYK786411:UYK786441 VIG786411:VIG786441 VSC786411:VSC786441 WBY786411:WBY786441 WLU786411:WLU786441 WVQ786411:WVQ786441 P851947:P851977 JE851947:JE851977 TA851947:TA851977 ACW851947:ACW851977 AMS851947:AMS851977 AWO851947:AWO851977 BGK851947:BGK851977 BQG851947:BQG851977 CAC851947:CAC851977 CJY851947:CJY851977 CTU851947:CTU851977 DDQ851947:DDQ851977 DNM851947:DNM851977 DXI851947:DXI851977 EHE851947:EHE851977 ERA851947:ERA851977 FAW851947:FAW851977 FKS851947:FKS851977 FUO851947:FUO851977 GEK851947:GEK851977 GOG851947:GOG851977 GYC851947:GYC851977 HHY851947:HHY851977 HRU851947:HRU851977 IBQ851947:IBQ851977 ILM851947:ILM851977 IVI851947:IVI851977 JFE851947:JFE851977 JPA851947:JPA851977 JYW851947:JYW851977 KIS851947:KIS851977 KSO851947:KSO851977 LCK851947:LCK851977 LMG851947:LMG851977 LWC851947:LWC851977 MFY851947:MFY851977 MPU851947:MPU851977 MZQ851947:MZQ851977 NJM851947:NJM851977 NTI851947:NTI851977 ODE851947:ODE851977 ONA851947:ONA851977 OWW851947:OWW851977 PGS851947:PGS851977 PQO851947:PQO851977 QAK851947:QAK851977 QKG851947:QKG851977 QUC851947:QUC851977 RDY851947:RDY851977 RNU851947:RNU851977 RXQ851947:RXQ851977 SHM851947:SHM851977 SRI851947:SRI851977 TBE851947:TBE851977 TLA851947:TLA851977 TUW851947:TUW851977 UES851947:UES851977 UOO851947:UOO851977 UYK851947:UYK851977 VIG851947:VIG851977 VSC851947:VSC851977 WBY851947:WBY851977 WLU851947:WLU851977 WVQ851947:WVQ851977 P917483:P917513 JE917483:JE917513 TA917483:TA917513 ACW917483:ACW917513 AMS917483:AMS917513 AWO917483:AWO917513 BGK917483:BGK917513 BQG917483:BQG917513 CAC917483:CAC917513 CJY917483:CJY917513 CTU917483:CTU917513 DDQ917483:DDQ917513 DNM917483:DNM917513 DXI917483:DXI917513 EHE917483:EHE917513 ERA917483:ERA917513 FAW917483:FAW917513 FKS917483:FKS917513 FUO917483:FUO917513 GEK917483:GEK917513 GOG917483:GOG917513 GYC917483:GYC917513 HHY917483:HHY917513 HRU917483:HRU917513 IBQ917483:IBQ917513 ILM917483:ILM917513 IVI917483:IVI917513 JFE917483:JFE917513 JPA917483:JPA917513 JYW917483:JYW917513 KIS917483:KIS917513 KSO917483:KSO917513 LCK917483:LCK917513 LMG917483:LMG917513 LWC917483:LWC917513 MFY917483:MFY917513 MPU917483:MPU917513 MZQ917483:MZQ917513 NJM917483:NJM917513 NTI917483:NTI917513 ODE917483:ODE917513 ONA917483:ONA917513 OWW917483:OWW917513 PGS917483:PGS917513 PQO917483:PQO917513 QAK917483:QAK917513 QKG917483:QKG917513 QUC917483:QUC917513 RDY917483:RDY917513 RNU917483:RNU917513 RXQ917483:RXQ917513 SHM917483:SHM917513 SRI917483:SRI917513 TBE917483:TBE917513 TLA917483:TLA917513 TUW917483:TUW917513 UES917483:UES917513 UOO917483:UOO917513 UYK917483:UYK917513 VIG917483:VIG917513 VSC917483:VSC917513 WBY917483:WBY917513 WLU917483:WLU917513 WVQ917483:WVQ917513 P983019:P983049 JE983019:JE983049 TA983019:TA983049 ACW983019:ACW983049 AMS983019:AMS983049 AWO983019:AWO983049 BGK983019:BGK983049 BQG983019:BQG983049 CAC983019:CAC983049 CJY983019:CJY983049 CTU983019:CTU983049 DDQ983019:DDQ983049 DNM983019:DNM983049 DXI983019:DXI983049 EHE983019:EHE983049 ERA983019:ERA983049 FAW983019:FAW983049 FKS983019:FKS983049 FUO983019:FUO983049 GEK983019:GEK983049 GOG983019:GOG983049 GYC983019:GYC983049 HHY983019:HHY983049 HRU983019:HRU983049 IBQ983019:IBQ983049 ILM983019:ILM983049 IVI983019:IVI983049 JFE983019:JFE983049 JPA983019:JPA983049 JYW983019:JYW983049 KIS983019:KIS983049 KSO983019:KSO983049 LCK983019:LCK983049 LMG983019:LMG983049 LWC983019:LWC983049 MFY983019:MFY983049 MPU983019:MPU983049 MZQ983019:MZQ983049 NJM983019:NJM983049 NTI983019:NTI983049 ODE983019:ODE983049 ONA983019:ONA983049 OWW983019:OWW983049 PGS983019:PGS983049 PQO983019:PQO983049 QAK983019:QAK983049 QKG983019:QKG983049 QUC983019:QUC983049 RDY983019:RDY983049 RNU983019:RNU983049 RXQ983019:RXQ983049 SHM983019:SHM983049 SRI983019:SRI983049 TBE983019:TBE983049 TLA983019:TLA983049 TUW983019:TUW983049 UES983019:UES983049 UOO983019:UOO983049 UYK983019:UYK983049 VIG983019:VIG983049 VSC983019:VSC983049 WBY983019:WBY983049 WLU983019:WLU983049 JE4:JE20 TA4:TA20 ACW4:ACW20 AMS4:AMS20 AWO4:AWO20 BGK4:BGK20 BQG4:BQG20 CAC4:CAC20 CJY4:CJY20 CTU4:CTU20 DDQ4:DDQ20 DNM4:DNM20 DXI4:DXI20 EHE4:EHE20 ERA4:ERA20 FAW4:FAW20 FKS4:FKS20 FUO4:FUO20 GEK4:GEK20 GOG4:GOG20 GYC4:GYC20 HHY4:HHY20 HRU4:HRU20 IBQ4:IBQ20 ILM4:ILM20 IVI4:IVI20 JFE4:JFE20 JPA4:JPA20 JYW4:JYW20 KIS4:KIS20 KSO4:KSO20 LCK4:LCK20 LMG4:LMG20 LWC4:LWC20 MFY4:MFY20 MPU4:MPU20 MZQ4:MZQ20 NJM4:NJM20 NTI4:NTI20 ODE4:ODE20 ONA4:ONA20 OWW4:OWW20 PGS4:PGS20 PQO4:PQO20 QAK4:QAK20 QKG4:QKG20 QUC4:QUC20 RDY4:RDY20 RNU4:RNU20 RXQ4:RXQ20 SHM4:SHM20 SRI4:SRI20 TBE4:TBE20 TLA4:TLA20 TUW4:TUW20 UES4:UES20 UOO4:UOO20 UYK4:UYK20 VIG4:VIG20 VSC4:VSC20 WBY4:WBY20 WLU4:WLU20 WVQ4:WVQ20" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"Mestizo, Raizal, Negro, Indio, Blanco, Amarillo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVZ983019:WVZ983049 Z65515:Z65545 JN65515:JN65545 TJ65515:TJ65545 ADF65515:ADF65545 ANB65515:ANB65545 AWX65515:AWX65545 BGT65515:BGT65545 BQP65515:BQP65545 CAL65515:CAL65545 CKH65515:CKH65545 CUD65515:CUD65545 DDZ65515:DDZ65545 DNV65515:DNV65545 DXR65515:DXR65545 EHN65515:EHN65545 ERJ65515:ERJ65545 FBF65515:FBF65545 FLB65515:FLB65545 FUX65515:FUX65545 GET65515:GET65545 GOP65515:GOP65545 GYL65515:GYL65545 HIH65515:HIH65545 HSD65515:HSD65545 IBZ65515:IBZ65545 ILV65515:ILV65545 IVR65515:IVR65545 JFN65515:JFN65545 JPJ65515:JPJ65545 JZF65515:JZF65545 KJB65515:KJB65545 KSX65515:KSX65545 LCT65515:LCT65545 LMP65515:LMP65545 LWL65515:LWL65545 MGH65515:MGH65545 MQD65515:MQD65545 MZZ65515:MZZ65545 NJV65515:NJV65545 NTR65515:NTR65545 ODN65515:ODN65545 ONJ65515:ONJ65545 OXF65515:OXF65545 PHB65515:PHB65545 PQX65515:PQX65545 QAT65515:QAT65545 QKP65515:QKP65545 QUL65515:QUL65545 REH65515:REH65545 ROD65515:ROD65545 RXZ65515:RXZ65545 SHV65515:SHV65545 SRR65515:SRR65545 TBN65515:TBN65545 TLJ65515:TLJ65545 TVF65515:TVF65545 UFB65515:UFB65545 UOX65515:UOX65545 UYT65515:UYT65545 VIP65515:VIP65545 VSL65515:VSL65545 WCH65515:WCH65545 WMD65515:WMD65545 WVZ65515:WVZ65545 Z131051:Z131081 JN131051:JN131081 TJ131051:TJ131081 ADF131051:ADF131081 ANB131051:ANB131081 AWX131051:AWX131081 BGT131051:BGT131081 BQP131051:BQP131081 CAL131051:CAL131081 CKH131051:CKH131081 CUD131051:CUD131081 DDZ131051:DDZ131081 DNV131051:DNV131081 DXR131051:DXR131081 EHN131051:EHN131081 ERJ131051:ERJ131081 FBF131051:FBF131081 FLB131051:FLB131081 FUX131051:FUX131081 GET131051:GET131081 GOP131051:GOP131081 GYL131051:GYL131081 HIH131051:HIH131081 HSD131051:HSD131081 IBZ131051:IBZ131081 ILV131051:ILV131081 IVR131051:IVR131081 JFN131051:JFN131081 JPJ131051:JPJ131081 JZF131051:JZF131081 KJB131051:KJB131081 KSX131051:KSX131081 LCT131051:LCT131081 LMP131051:LMP131081 LWL131051:LWL131081 MGH131051:MGH131081 MQD131051:MQD131081 MZZ131051:MZZ131081 NJV131051:NJV131081 NTR131051:NTR131081 ODN131051:ODN131081 ONJ131051:ONJ131081 OXF131051:OXF131081 PHB131051:PHB131081 PQX131051:PQX131081 QAT131051:QAT131081 QKP131051:QKP131081 QUL131051:QUL131081 REH131051:REH131081 ROD131051:ROD131081 RXZ131051:RXZ131081 SHV131051:SHV131081 SRR131051:SRR131081 TBN131051:TBN131081 TLJ131051:TLJ131081 TVF131051:TVF131081 UFB131051:UFB131081 UOX131051:UOX131081 UYT131051:UYT131081 VIP131051:VIP131081 VSL131051:VSL131081 WCH131051:WCH131081 WMD131051:WMD131081 WVZ131051:WVZ131081 Z196587:Z196617 JN196587:JN196617 TJ196587:TJ196617 ADF196587:ADF196617 ANB196587:ANB196617 AWX196587:AWX196617 BGT196587:BGT196617 BQP196587:BQP196617 CAL196587:CAL196617 CKH196587:CKH196617 CUD196587:CUD196617 DDZ196587:DDZ196617 DNV196587:DNV196617 DXR196587:DXR196617 EHN196587:EHN196617 ERJ196587:ERJ196617 FBF196587:FBF196617 FLB196587:FLB196617 FUX196587:FUX196617 GET196587:GET196617 GOP196587:GOP196617 GYL196587:GYL196617 HIH196587:HIH196617 HSD196587:HSD196617 IBZ196587:IBZ196617 ILV196587:ILV196617 IVR196587:IVR196617 JFN196587:JFN196617 JPJ196587:JPJ196617 JZF196587:JZF196617 KJB196587:KJB196617 KSX196587:KSX196617 LCT196587:LCT196617 LMP196587:LMP196617 LWL196587:LWL196617 MGH196587:MGH196617 MQD196587:MQD196617 MZZ196587:MZZ196617 NJV196587:NJV196617 NTR196587:NTR196617 ODN196587:ODN196617 ONJ196587:ONJ196617 OXF196587:OXF196617 PHB196587:PHB196617 PQX196587:PQX196617 QAT196587:QAT196617 QKP196587:QKP196617 QUL196587:QUL196617 REH196587:REH196617 ROD196587:ROD196617 RXZ196587:RXZ196617 SHV196587:SHV196617 SRR196587:SRR196617 TBN196587:TBN196617 TLJ196587:TLJ196617 TVF196587:TVF196617 UFB196587:UFB196617 UOX196587:UOX196617 UYT196587:UYT196617 VIP196587:VIP196617 VSL196587:VSL196617 WCH196587:WCH196617 WMD196587:WMD196617 WVZ196587:WVZ196617 Z262123:Z262153 JN262123:JN262153 TJ262123:TJ262153 ADF262123:ADF262153 ANB262123:ANB262153 AWX262123:AWX262153 BGT262123:BGT262153 BQP262123:BQP262153 CAL262123:CAL262153 CKH262123:CKH262153 CUD262123:CUD262153 DDZ262123:DDZ262153 DNV262123:DNV262153 DXR262123:DXR262153 EHN262123:EHN262153 ERJ262123:ERJ262153 FBF262123:FBF262153 FLB262123:FLB262153 FUX262123:FUX262153 GET262123:GET262153 GOP262123:GOP262153 GYL262123:GYL262153 HIH262123:HIH262153 HSD262123:HSD262153 IBZ262123:IBZ262153 ILV262123:ILV262153 IVR262123:IVR262153 JFN262123:JFN262153 JPJ262123:JPJ262153 JZF262123:JZF262153 KJB262123:KJB262153 KSX262123:KSX262153 LCT262123:LCT262153 LMP262123:LMP262153 LWL262123:LWL262153 MGH262123:MGH262153 MQD262123:MQD262153 MZZ262123:MZZ262153 NJV262123:NJV262153 NTR262123:NTR262153 ODN262123:ODN262153 ONJ262123:ONJ262153 OXF262123:OXF262153 PHB262123:PHB262153 PQX262123:PQX262153 QAT262123:QAT262153 QKP262123:QKP262153 QUL262123:QUL262153 REH262123:REH262153 ROD262123:ROD262153 RXZ262123:RXZ262153 SHV262123:SHV262153 SRR262123:SRR262153 TBN262123:TBN262153 TLJ262123:TLJ262153 TVF262123:TVF262153 UFB262123:UFB262153 UOX262123:UOX262153 UYT262123:UYT262153 VIP262123:VIP262153 VSL262123:VSL262153 WCH262123:WCH262153 WMD262123:WMD262153 WVZ262123:WVZ262153 Z327659:Z327689 JN327659:JN327689 TJ327659:TJ327689 ADF327659:ADF327689 ANB327659:ANB327689 AWX327659:AWX327689 BGT327659:BGT327689 BQP327659:BQP327689 CAL327659:CAL327689 CKH327659:CKH327689 CUD327659:CUD327689 DDZ327659:DDZ327689 DNV327659:DNV327689 DXR327659:DXR327689 EHN327659:EHN327689 ERJ327659:ERJ327689 FBF327659:FBF327689 FLB327659:FLB327689 FUX327659:FUX327689 GET327659:GET327689 GOP327659:GOP327689 GYL327659:GYL327689 HIH327659:HIH327689 HSD327659:HSD327689 IBZ327659:IBZ327689 ILV327659:ILV327689 IVR327659:IVR327689 JFN327659:JFN327689 JPJ327659:JPJ327689 JZF327659:JZF327689 KJB327659:KJB327689 KSX327659:KSX327689 LCT327659:LCT327689 LMP327659:LMP327689 LWL327659:LWL327689 MGH327659:MGH327689 MQD327659:MQD327689 MZZ327659:MZZ327689 NJV327659:NJV327689 NTR327659:NTR327689 ODN327659:ODN327689 ONJ327659:ONJ327689 OXF327659:OXF327689 PHB327659:PHB327689 PQX327659:PQX327689 QAT327659:QAT327689 QKP327659:QKP327689 QUL327659:QUL327689 REH327659:REH327689 ROD327659:ROD327689 RXZ327659:RXZ327689 SHV327659:SHV327689 SRR327659:SRR327689 TBN327659:TBN327689 TLJ327659:TLJ327689 TVF327659:TVF327689 UFB327659:UFB327689 UOX327659:UOX327689 UYT327659:UYT327689 VIP327659:VIP327689 VSL327659:VSL327689 WCH327659:WCH327689 WMD327659:WMD327689 WVZ327659:WVZ327689 Z393195:Z393225 JN393195:JN393225 TJ393195:TJ393225 ADF393195:ADF393225 ANB393195:ANB393225 AWX393195:AWX393225 BGT393195:BGT393225 BQP393195:BQP393225 CAL393195:CAL393225 CKH393195:CKH393225 CUD393195:CUD393225 DDZ393195:DDZ393225 DNV393195:DNV393225 DXR393195:DXR393225 EHN393195:EHN393225 ERJ393195:ERJ393225 FBF393195:FBF393225 FLB393195:FLB393225 FUX393195:FUX393225 GET393195:GET393225 GOP393195:GOP393225 GYL393195:GYL393225 HIH393195:HIH393225 HSD393195:HSD393225 IBZ393195:IBZ393225 ILV393195:ILV393225 IVR393195:IVR393225 JFN393195:JFN393225 JPJ393195:JPJ393225 JZF393195:JZF393225 KJB393195:KJB393225 KSX393195:KSX393225 LCT393195:LCT393225 LMP393195:LMP393225 LWL393195:LWL393225 MGH393195:MGH393225 MQD393195:MQD393225 MZZ393195:MZZ393225 NJV393195:NJV393225 NTR393195:NTR393225 ODN393195:ODN393225 ONJ393195:ONJ393225 OXF393195:OXF393225 PHB393195:PHB393225 PQX393195:PQX393225 QAT393195:QAT393225 QKP393195:QKP393225 QUL393195:QUL393225 REH393195:REH393225 ROD393195:ROD393225 RXZ393195:RXZ393225 SHV393195:SHV393225 SRR393195:SRR393225 TBN393195:TBN393225 TLJ393195:TLJ393225 TVF393195:TVF393225 UFB393195:UFB393225 UOX393195:UOX393225 UYT393195:UYT393225 VIP393195:VIP393225 VSL393195:VSL393225 WCH393195:WCH393225 WMD393195:WMD393225 WVZ393195:WVZ393225 Z458731:Z458761 JN458731:JN458761 TJ458731:TJ458761 ADF458731:ADF458761 ANB458731:ANB458761 AWX458731:AWX458761 BGT458731:BGT458761 BQP458731:BQP458761 CAL458731:CAL458761 CKH458731:CKH458761 CUD458731:CUD458761 DDZ458731:DDZ458761 DNV458731:DNV458761 DXR458731:DXR458761 EHN458731:EHN458761 ERJ458731:ERJ458761 FBF458731:FBF458761 FLB458731:FLB458761 FUX458731:FUX458761 GET458731:GET458761 GOP458731:GOP458761 GYL458731:GYL458761 HIH458731:HIH458761 HSD458731:HSD458761 IBZ458731:IBZ458761 ILV458731:ILV458761 IVR458731:IVR458761 JFN458731:JFN458761 JPJ458731:JPJ458761 JZF458731:JZF458761 KJB458731:KJB458761 KSX458731:KSX458761 LCT458731:LCT458761 LMP458731:LMP458761 LWL458731:LWL458761 MGH458731:MGH458761 MQD458731:MQD458761 MZZ458731:MZZ458761 NJV458731:NJV458761 NTR458731:NTR458761 ODN458731:ODN458761 ONJ458731:ONJ458761 OXF458731:OXF458761 PHB458731:PHB458761 PQX458731:PQX458761 QAT458731:QAT458761 QKP458731:QKP458761 QUL458731:QUL458761 REH458731:REH458761 ROD458731:ROD458761 RXZ458731:RXZ458761 SHV458731:SHV458761 SRR458731:SRR458761 TBN458731:TBN458761 TLJ458731:TLJ458761 TVF458731:TVF458761 UFB458731:UFB458761 UOX458731:UOX458761 UYT458731:UYT458761 VIP458731:VIP458761 VSL458731:VSL458761 WCH458731:WCH458761 WMD458731:WMD458761 WVZ458731:WVZ458761 Z524267:Z524297 JN524267:JN524297 TJ524267:TJ524297 ADF524267:ADF524297 ANB524267:ANB524297 AWX524267:AWX524297 BGT524267:BGT524297 BQP524267:BQP524297 CAL524267:CAL524297 CKH524267:CKH524297 CUD524267:CUD524297 DDZ524267:DDZ524297 DNV524267:DNV524297 DXR524267:DXR524297 EHN524267:EHN524297 ERJ524267:ERJ524297 FBF524267:FBF524297 FLB524267:FLB524297 FUX524267:FUX524297 GET524267:GET524297 GOP524267:GOP524297 GYL524267:GYL524297 HIH524267:HIH524297 HSD524267:HSD524297 IBZ524267:IBZ524297 ILV524267:ILV524297 IVR524267:IVR524297 JFN524267:JFN524297 JPJ524267:JPJ524297 JZF524267:JZF524297 KJB524267:KJB524297 KSX524267:KSX524297 LCT524267:LCT524297 LMP524267:LMP524297 LWL524267:LWL524297 MGH524267:MGH524297 MQD524267:MQD524297 MZZ524267:MZZ524297 NJV524267:NJV524297 NTR524267:NTR524297 ODN524267:ODN524297 ONJ524267:ONJ524297 OXF524267:OXF524297 PHB524267:PHB524297 PQX524267:PQX524297 QAT524267:QAT524297 QKP524267:QKP524297 QUL524267:QUL524297 REH524267:REH524297 ROD524267:ROD524297 RXZ524267:RXZ524297 SHV524267:SHV524297 SRR524267:SRR524297 TBN524267:TBN524297 TLJ524267:TLJ524297 TVF524267:TVF524297 UFB524267:UFB524297 UOX524267:UOX524297 UYT524267:UYT524297 VIP524267:VIP524297 VSL524267:VSL524297 WCH524267:WCH524297 WMD524267:WMD524297 WVZ524267:WVZ524297 Z589803:Z589833 JN589803:JN589833 TJ589803:TJ589833 ADF589803:ADF589833 ANB589803:ANB589833 AWX589803:AWX589833 BGT589803:BGT589833 BQP589803:BQP589833 CAL589803:CAL589833 CKH589803:CKH589833 CUD589803:CUD589833 DDZ589803:DDZ589833 DNV589803:DNV589833 DXR589803:DXR589833 EHN589803:EHN589833 ERJ589803:ERJ589833 FBF589803:FBF589833 FLB589803:FLB589833 FUX589803:FUX589833 GET589803:GET589833 GOP589803:GOP589833 GYL589803:GYL589833 HIH589803:HIH589833 HSD589803:HSD589833 IBZ589803:IBZ589833 ILV589803:ILV589833 IVR589803:IVR589833 JFN589803:JFN589833 JPJ589803:JPJ589833 JZF589803:JZF589833 KJB589803:KJB589833 KSX589803:KSX589833 LCT589803:LCT589833 LMP589803:LMP589833 LWL589803:LWL589833 MGH589803:MGH589833 MQD589803:MQD589833 MZZ589803:MZZ589833 NJV589803:NJV589833 NTR589803:NTR589833 ODN589803:ODN589833 ONJ589803:ONJ589833 OXF589803:OXF589833 PHB589803:PHB589833 PQX589803:PQX589833 QAT589803:QAT589833 QKP589803:QKP589833 QUL589803:QUL589833 REH589803:REH589833 ROD589803:ROD589833 RXZ589803:RXZ589833 SHV589803:SHV589833 SRR589803:SRR589833 TBN589803:TBN589833 TLJ589803:TLJ589833 TVF589803:TVF589833 UFB589803:UFB589833 UOX589803:UOX589833 UYT589803:UYT589833 VIP589803:VIP589833 VSL589803:VSL589833 WCH589803:WCH589833 WMD589803:WMD589833 WVZ589803:WVZ589833 Z655339:Z655369 JN655339:JN655369 TJ655339:TJ655369 ADF655339:ADF655369 ANB655339:ANB655369 AWX655339:AWX655369 BGT655339:BGT655369 BQP655339:BQP655369 CAL655339:CAL655369 CKH655339:CKH655369 CUD655339:CUD655369 DDZ655339:DDZ655369 DNV655339:DNV655369 DXR655339:DXR655369 EHN655339:EHN655369 ERJ655339:ERJ655369 FBF655339:FBF655369 FLB655339:FLB655369 FUX655339:FUX655369 GET655339:GET655369 GOP655339:GOP655369 GYL655339:GYL655369 HIH655339:HIH655369 HSD655339:HSD655369 IBZ655339:IBZ655369 ILV655339:ILV655369 IVR655339:IVR655369 JFN655339:JFN655369 JPJ655339:JPJ655369 JZF655339:JZF655369 KJB655339:KJB655369 KSX655339:KSX655369 LCT655339:LCT655369 LMP655339:LMP655369 LWL655339:LWL655369 MGH655339:MGH655369 MQD655339:MQD655369 MZZ655339:MZZ655369 NJV655339:NJV655369 NTR655339:NTR655369 ODN655339:ODN655369 ONJ655339:ONJ655369 OXF655339:OXF655369 PHB655339:PHB655369 PQX655339:PQX655369 QAT655339:QAT655369 QKP655339:QKP655369 QUL655339:QUL655369 REH655339:REH655369 ROD655339:ROD655369 RXZ655339:RXZ655369 SHV655339:SHV655369 SRR655339:SRR655369 TBN655339:TBN655369 TLJ655339:TLJ655369 TVF655339:TVF655369 UFB655339:UFB655369 UOX655339:UOX655369 UYT655339:UYT655369 VIP655339:VIP655369 VSL655339:VSL655369 WCH655339:WCH655369 WMD655339:WMD655369 WVZ655339:WVZ655369 Z720875:Z720905 JN720875:JN720905 TJ720875:TJ720905 ADF720875:ADF720905 ANB720875:ANB720905 AWX720875:AWX720905 BGT720875:BGT720905 BQP720875:BQP720905 CAL720875:CAL720905 CKH720875:CKH720905 CUD720875:CUD720905 DDZ720875:DDZ720905 DNV720875:DNV720905 DXR720875:DXR720905 EHN720875:EHN720905 ERJ720875:ERJ720905 FBF720875:FBF720905 FLB720875:FLB720905 FUX720875:FUX720905 GET720875:GET720905 GOP720875:GOP720905 GYL720875:GYL720905 HIH720875:HIH720905 HSD720875:HSD720905 IBZ720875:IBZ720905 ILV720875:ILV720905 IVR720875:IVR720905 JFN720875:JFN720905 JPJ720875:JPJ720905 JZF720875:JZF720905 KJB720875:KJB720905 KSX720875:KSX720905 LCT720875:LCT720905 LMP720875:LMP720905 LWL720875:LWL720905 MGH720875:MGH720905 MQD720875:MQD720905 MZZ720875:MZZ720905 NJV720875:NJV720905 NTR720875:NTR720905 ODN720875:ODN720905 ONJ720875:ONJ720905 OXF720875:OXF720905 PHB720875:PHB720905 PQX720875:PQX720905 QAT720875:QAT720905 QKP720875:QKP720905 QUL720875:QUL720905 REH720875:REH720905 ROD720875:ROD720905 RXZ720875:RXZ720905 SHV720875:SHV720905 SRR720875:SRR720905 TBN720875:TBN720905 TLJ720875:TLJ720905 TVF720875:TVF720905 UFB720875:UFB720905 UOX720875:UOX720905 UYT720875:UYT720905 VIP720875:VIP720905 VSL720875:VSL720905 WCH720875:WCH720905 WMD720875:WMD720905 WVZ720875:WVZ720905 Z786411:Z786441 JN786411:JN786441 TJ786411:TJ786441 ADF786411:ADF786441 ANB786411:ANB786441 AWX786411:AWX786441 BGT786411:BGT786441 BQP786411:BQP786441 CAL786411:CAL786441 CKH786411:CKH786441 CUD786411:CUD786441 DDZ786411:DDZ786441 DNV786411:DNV786441 DXR786411:DXR786441 EHN786411:EHN786441 ERJ786411:ERJ786441 FBF786411:FBF786441 FLB786411:FLB786441 FUX786411:FUX786441 GET786411:GET786441 GOP786411:GOP786441 GYL786411:GYL786441 HIH786411:HIH786441 HSD786411:HSD786441 IBZ786411:IBZ786441 ILV786411:ILV786441 IVR786411:IVR786441 JFN786411:JFN786441 JPJ786411:JPJ786441 JZF786411:JZF786441 KJB786411:KJB786441 KSX786411:KSX786441 LCT786411:LCT786441 LMP786411:LMP786441 LWL786411:LWL786441 MGH786411:MGH786441 MQD786411:MQD786441 MZZ786411:MZZ786441 NJV786411:NJV786441 NTR786411:NTR786441 ODN786411:ODN786441 ONJ786411:ONJ786441 OXF786411:OXF786441 PHB786411:PHB786441 PQX786411:PQX786441 QAT786411:QAT786441 QKP786411:QKP786441 QUL786411:QUL786441 REH786411:REH786441 ROD786411:ROD786441 RXZ786411:RXZ786441 SHV786411:SHV786441 SRR786411:SRR786441 TBN786411:TBN786441 TLJ786411:TLJ786441 TVF786411:TVF786441 UFB786411:UFB786441 UOX786411:UOX786441 UYT786411:UYT786441 VIP786411:VIP786441 VSL786411:VSL786441 WCH786411:WCH786441 WMD786411:WMD786441 WVZ786411:WVZ786441 Z851947:Z851977 JN851947:JN851977 TJ851947:TJ851977 ADF851947:ADF851977 ANB851947:ANB851977 AWX851947:AWX851977 BGT851947:BGT851977 BQP851947:BQP851977 CAL851947:CAL851977 CKH851947:CKH851977 CUD851947:CUD851977 DDZ851947:DDZ851977 DNV851947:DNV851977 DXR851947:DXR851977 EHN851947:EHN851977 ERJ851947:ERJ851977 FBF851947:FBF851977 FLB851947:FLB851977 FUX851947:FUX851977 GET851947:GET851977 GOP851947:GOP851977 GYL851947:GYL851977 HIH851947:HIH851977 HSD851947:HSD851977 IBZ851947:IBZ851977 ILV851947:ILV851977 IVR851947:IVR851977 JFN851947:JFN851977 JPJ851947:JPJ851977 JZF851947:JZF851977 KJB851947:KJB851977 KSX851947:KSX851977 LCT851947:LCT851977 LMP851947:LMP851977 LWL851947:LWL851977 MGH851947:MGH851977 MQD851947:MQD851977 MZZ851947:MZZ851977 NJV851947:NJV851977 NTR851947:NTR851977 ODN851947:ODN851977 ONJ851947:ONJ851977 OXF851947:OXF851977 PHB851947:PHB851977 PQX851947:PQX851977 QAT851947:QAT851977 QKP851947:QKP851977 QUL851947:QUL851977 REH851947:REH851977 ROD851947:ROD851977 RXZ851947:RXZ851977 SHV851947:SHV851977 SRR851947:SRR851977 TBN851947:TBN851977 TLJ851947:TLJ851977 TVF851947:TVF851977 UFB851947:UFB851977 UOX851947:UOX851977 UYT851947:UYT851977 VIP851947:VIP851977 VSL851947:VSL851977 WCH851947:WCH851977 WMD851947:WMD851977 WVZ851947:WVZ851977 Z917483:Z917513 JN917483:JN917513 TJ917483:TJ917513 ADF917483:ADF917513 ANB917483:ANB917513 AWX917483:AWX917513 BGT917483:BGT917513 BQP917483:BQP917513 CAL917483:CAL917513 CKH917483:CKH917513 CUD917483:CUD917513 DDZ917483:DDZ917513 DNV917483:DNV917513 DXR917483:DXR917513 EHN917483:EHN917513 ERJ917483:ERJ917513 FBF917483:FBF917513 FLB917483:FLB917513 FUX917483:FUX917513 GET917483:GET917513 GOP917483:GOP917513 GYL917483:GYL917513 HIH917483:HIH917513 HSD917483:HSD917513 IBZ917483:IBZ917513 ILV917483:ILV917513 IVR917483:IVR917513 JFN917483:JFN917513 JPJ917483:JPJ917513 JZF917483:JZF917513 KJB917483:KJB917513 KSX917483:KSX917513 LCT917483:LCT917513 LMP917483:LMP917513 LWL917483:LWL917513 MGH917483:MGH917513 MQD917483:MQD917513 MZZ917483:MZZ917513 NJV917483:NJV917513 NTR917483:NTR917513 ODN917483:ODN917513 ONJ917483:ONJ917513 OXF917483:OXF917513 PHB917483:PHB917513 PQX917483:PQX917513 QAT917483:QAT917513 QKP917483:QKP917513 QUL917483:QUL917513 REH917483:REH917513 ROD917483:ROD917513 RXZ917483:RXZ917513 SHV917483:SHV917513 SRR917483:SRR917513 TBN917483:TBN917513 TLJ917483:TLJ917513 TVF917483:TVF917513 UFB917483:UFB917513 UOX917483:UOX917513 UYT917483:UYT917513 VIP917483:VIP917513 VSL917483:VSL917513 WCH917483:WCH917513 WMD917483:WMD917513 WVZ917483:WVZ917513 Z983019:Z983049 JN983019:JN983049 TJ983019:TJ983049 ADF983019:ADF983049 ANB983019:ANB983049 AWX983019:AWX983049 BGT983019:BGT983049 BQP983019:BQP983049 CAL983019:CAL983049 CKH983019:CKH983049 CUD983019:CUD983049 DDZ983019:DDZ983049 DNV983019:DNV983049 DXR983019:DXR983049 EHN983019:EHN983049 ERJ983019:ERJ983049 FBF983019:FBF983049 FLB983019:FLB983049 FUX983019:FUX983049 GET983019:GET983049 GOP983019:GOP983049 GYL983019:GYL983049 HIH983019:HIH983049 HSD983019:HSD983049 IBZ983019:IBZ983049 ILV983019:ILV983049 IVR983019:IVR983049 JFN983019:JFN983049 JPJ983019:JPJ983049 JZF983019:JZF983049 KJB983019:KJB983049 KSX983019:KSX983049 LCT983019:LCT983049 LMP983019:LMP983049 LWL983019:LWL983049 MGH983019:MGH983049 MQD983019:MQD983049 MZZ983019:MZZ983049 NJV983019:NJV983049 NTR983019:NTR983049 ODN983019:ODN983049 ONJ983019:ONJ983049 OXF983019:OXF983049 PHB983019:PHB983049 PQX983019:PQX983049 QAT983019:QAT983049 QKP983019:QKP983049 QUL983019:QUL983049 REH983019:REH983049 ROD983019:ROD983049 RXZ983019:RXZ983049 SHV983019:SHV983049 SRR983019:SRR983049 TBN983019:TBN983049 TLJ983019:TLJ983049 TVF983019:TVF983049 UFB983019:UFB983049 UOX983019:UOX983049 UYT983019:UYT983049 VIP983019:VIP983049 VSL983019:VSL983049 WCH983019:WCH983049 WMD983019:WMD983049 Z4:Z20 WVZ4:WVZ20 WMD4:WMD20 WCH4:WCH20 VSL4:VSL20 VIP4:VIP20 UYT4:UYT20 UOX4:UOX20 UFB4:UFB20 TVF4:TVF20 TLJ4:TLJ20 TBN4:TBN20 SRR4:SRR20 SHV4:SHV20 RXZ4:RXZ20 ROD4:ROD20 REH4:REH20 QUL4:QUL20 QKP4:QKP20 QAT4:QAT20 PQX4:PQX20 PHB4:PHB20 OXF4:OXF20 ONJ4:ONJ20 ODN4:ODN20 NTR4:NTR20 NJV4:NJV20 MZZ4:MZZ20 MQD4:MQD20 MGH4:MGH20 LWL4:LWL20 LMP4:LMP20 LCT4:LCT20 KSX4:KSX20 KJB4:KJB20 JZF4:JZF20 JPJ4:JPJ20 JFN4:JFN20 IVR4:IVR20 ILV4:ILV20 IBZ4:IBZ20 HSD4:HSD20 HIH4:HIH20 GYL4:GYL20 GOP4:GOP20 GET4:GET20 FUX4:FUX20 FLB4:FLB20 FBF4:FBF20 ERJ4:ERJ20 EHN4:EHN20 DXR4:DXR20 DNV4:DNV20 DDZ4:DDZ20 CUD4:CUD20 CKH4:CKH20 CAL4:CAL20 BQP4:BQP20 BGT4:BGT20 AWX4:AWX20 ANB4:ANB20 ADF4:ADF20 TJ4:TJ20 JN4:JN20" xr:uid="{00000000-0002-0000-0200-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVZ983019:WVZ983049 Z65515:Z65545 JN65515:JN65545 TJ65515:TJ65545 ADF65515:ADF65545 ANB65515:ANB65545 AWX65515:AWX65545 BGT65515:BGT65545 BQP65515:BQP65545 CAL65515:CAL65545 CKH65515:CKH65545 CUD65515:CUD65545 DDZ65515:DDZ65545 DNV65515:DNV65545 DXR65515:DXR65545 EHN65515:EHN65545 ERJ65515:ERJ65545 FBF65515:FBF65545 FLB65515:FLB65545 FUX65515:FUX65545 GET65515:GET65545 GOP65515:GOP65545 GYL65515:GYL65545 HIH65515:HIH65545 HSD65515:HSD65545 IBZ65515:IBZ65545 ILV65515:ILV65545 IVR65515:IVR65545 JFN65515:JFN65545 JPJ65515:JPJ65545 JZF65515:JZF65545 KJB65515:KJB65545 KSX65515:KSX65545 LCT65515:LCT65545 LMP65515:LMP65545 LWL65515:LWL65545 MGH65515:MGH65545 MQD65515:MQD65545 MZZ65515:MZZ65545 NJV65515:NJV65545 NTR65515:NTR65545 ODN65515:ODN65545 ONJ65515:ONJ65545 OXF65515:OXF65545 PHB65515:PHB65545 PQX65515:PQX65545 QAT65515:QAT65545 QKP65515:QKP65545 QUL65515:QUL65545 REH65515:REH65545 ROD65515:ROD65545 RXZ65515:RXZ65545 SHV65515:SHV65545 SRR65515:SRR65545 TBN65515:TBN65545 TLJ65515:TLJ65545 TVF65515:TVF65545 UFB65515:UFB65545 UOX65515:UOX65545 UYT65515:UYT65545 VIP65515:VIP65545 VSL65515:VSL65545 WCH65515:WCH65545 WMD65515:WMD65545 WVZ65515:WVZ65545 Z131051:Z131081 JN131051:JN131081 TJ131051:TJ131081 ADF131051:ADF131081 ANB131051:ANB131081 AWX131051:AWX131081 BGT131051:BGT131081 BQP131051:BQP131081 CAL131051:CAL131081 CKH131051:CKH131081 CUD131051:CUD131081 DDZ131051:DDZ131081 DNV131051:DNV131081 DXR131051:DXR131081 EHN131051:EHN131081 ERJ131051:ERJ131081 FBF131051:FBF131081 FLB131051:FLB131081 FUX131051:FUX131081 GET131051:GET131081 GOP131051:GOP131081 GYL131051:GYL131081 HIH131051:HIH131081 HSD131051:HSD131081 IBZ131051:IBZ131081 ILV131051:ILV131081 IVR131051:IVR131081 JFN131051:JFN131081 JPJ131051:JPJ131081 JZF131051:JZF131081 KJB131051:KJB131081 KSX131051:KSX131081 LCT131051:LCT131081 LMP131051:LMP131081 LWL131051:LWL131081 MGH131051:MGH131081 MQD131051:MQD131081 MZZ131051:MZZ131081 NJV131051:NJV131081 NTR131051:NTR131081 ODN131051:ODN131081 ONJ131051:ONJ131081 OXF131051:OXF131081 PHB131051:PHB131081 PQX131051:PQX131081 QAT131051:QAT131081 QKP131051:QKP131081 QUL131051:QUL131081 REH131051:REH131081 ROD131051:ROD131081 RXZ131051:RXZ131081 SHV131051:SHV131081 SRR131051:SRR131081 TBN131051:TBN131081 TLJ131051:TLJ131081 TVF131051:TVF131081 UFB131051:UFB131081 UOX131051:UOX131081 UYT131051:UYT131081 VIP131051:VIP131081 VSL131051:VSL131081 WCH131051:WCH131081 WMD131051:WMD131081 WVZ131051:WVZ131081 Z196587:Z196617 JN196587:JN196617 TJ196587:TJ196617 ADF196587:ADF196617 ANB196587:ANB196617 AWX196587:AWX196617 BGT196587:BGT196617 BQP196587:BQP196617 CAL196587:CAL196617 CKH196587:CKH196617 CUD196587:CUD196617 DDZ196587:DDZ196617 DNV196587:DNV196617 DXR196587:DXR196617 EHN196587:EHN196617 ERJ196587:ERJ196617 FBF196587:FBF196617 FLB196587:FLB196617 FUX196587:FUX196617 GET196587:GET196617 GOP196587:GOP196617 GYL196587:GYL196617 HIH196587:HIH196617 HSD196587:HSD196617 IBZ196587:IBZ196617 ILV196587:ILV196617 IVR196587:IVR196617 JFN196587:JFN196617 JPJ196587:JPJ196617 JZF196587:JZF196617 KJB196587:KJB196617 KSX196587:KSX196617 LCT196587:LCT196617 LMP196587:LMP196617 LWL196587:LWL196617 MGH196587:MGH196617 MQD196587:MQD196617 MZZ196587:MZZ196617 NJV196587:NJV196617 NTR196587:NTR196617 ODN196587:ODN196617 ONJ196587:ONJ196617 OXF196587:OXF196617 PHB196587:PHB196617 PQX196587:PQX196617 QAT196587:QAT196617 QKP196587:QKP196617 QUL196587:QUL196617 REH196587:REH196617 ROD196587:ROD196617 RXZ196587:RXZ196617 SHV196587:SHV196617 SRR196587:SRR196617 TBN196587:TBN196617 TLJ196587:TLJ196617 TVF196587:TVF196617 UFB196587:UFB196617 UOX196587:UOX196617 UYT196587:UYT196617 VIP196587:VIP196617 VSL196587:VSL196617 WCH196587:WCH196617 WMD196587:WMD196617 WVZ196587:WVZ196617 Z262123:Z262153 JN262123:JN262153 TJ262123:TJ262153 ADF262123:ADF262153 ANB262123:ANB262153 AWX262123:AWX262153 BGT262123:BGT262153 BQP262123:BQP262153 CAL262123:CAL262153 CKH262123:CKH262153 CUD262123:CUD262153 DDZ262123:DDZ262153 DNV262123:DNV262153 DXR262123:DXR262153 EHN262123:EHN262153 ERJ262123:ERJ262153 FBF262123:FBF262153 FLB262123:FLB262153 FUX262123:FUX262153 GET262123:GET262153 GOP262123:GOP262153 GYL262123:GYL262153 HIH262123:HIH262153 HSD262123:HSD262153 IBZ262123:IBZ262153 ILV262123:ILV262153 IVR262123:IVR262153 JFN262123:JFN262153 JPJ262123:JPJ262153 JZF262123:JZF262153 KJB262123:KJB262153 KSX262123:KSX262153 LCT262123:LCT262153 LMP262123:LMP262153 LWL262123:LWL262153 MGH262123:MGH262153 MQD262123:MQD262153 MZZ262123:MZZ262153 NJV262123:NJV262153 NTR262123:NTR262153 ODN262123:ODN262153 ONJ262123:ONJ262153 OXF262123:OXF262153 PHB262123:PHB262153 PQX262123:PQX262153 QAT262123:QAT262153 QKP262123:QKP262153 QUL262123:QUL262153 REH262123:REH262153 ROD262123:ROD262153 RXZ262123:RXZ262153 SHV262123:SHV262153 SRR262123:SRR262153 TBN262123:TBN262153 TLJ262123:TLJ262153 TVF262123:TVF262153 UFB262123:UFB262153 UOX262123:UOX262153 UYT262123:UYT262153 VIP262123:VIP262153 VSL262123:VSL262153 WCH262123:WCH262153 WMD262123:WMD262153 WVZ262123:WVZ262153 Z327659:Z327689 JN327659:JN327689 TJ327659:TJ327689 ADF327659:ADF327689 ANB327659:ANB327689 AWX327659:AWX327689 BGT327659:BGT327689 BQP327659:BQP327689 CAL327659:CAL327689 CKH327659:CKH327689 CUD327659:CUD327689 DDZ327659:DDZ327689 DNV327659:DNV327689 DXR327659:DXR327689 EHN327659:EHN327689 ERJ327659:ERJ327689 FBF327659:FBF327689 FLB327659:FLB327689 FUX327659:FUX327689 GET327659:GET327689 GOP327659:GOP327689 GYL327659:GYL327689 HIH327659:HIH327689 HSD327659:HSD327689 IBZ327659:IBZ327689 ILV327659:ILV327689 IVR327659:IVR327689 JFN327659:JFN327689 JPJ327659:JPJ327689 JZF327659:JZF327689 KJB327659:KJB327689 KSX327659:KSX327689 LCT327659:LCT327689 LMP327659:LMP327689 LWL327659:LWL327689 MGH327659:MGH327689 MQD327659:MQD327689 MZZ327659:MZZ327689 NJV327659:NJV327689 NTR327659:NTR327689 ODN327659:ODN327689 ONJ327659:ONJ327689 OXF327659:OXF327689 PHB327659:PHB327689 PQX327659:PQX327689 QAT327659:QAT327689 QKP327659:QKP327689 QUL327659:QUL327689 REH327659:REH327689 ROD327659:ROD327689 RXZ327659:RXZ327689 SHV327659:SHV327689 SRR327659:SRR327689 TBN327659:TBN327689 TLJ327659:TLJ327689 TVF327659:TVF327689 UFB327659:UFB327689 UOX327659:UOX327689 UYT327659:UYT327689 VIP327659:VIP327689 VSL327659:VSL327689 WCH327659:WCH327689 WMD327659:WMD327689 WVZ327659:WVZ327689 Z393195:Z393225 JN393195:JN393225 TJ393195:TJ393225 ADF393195:ADF393225 ANB393195:ANB393225 AWX393195:AWX393225 BGT393195:BGT393225 BQP393195:BQP393225 CAL393195:CAL393225 CKH393195:CKH393225 CUD393195:CUD393225 DDZ393195:DDZ393225 DNV393195:DNV393225 DXR393195:DXR393225 EHN393195:EHN393225 ERJ393195:ERJ393225 FBF393195:FBF393225 FLB393195:FLB393225 FUX393195:FUX393225 GET393195:GET393225 GOP393195:GOP393225 GYL393195:GYL393225 HIH393195:HIH393225 HSD393195:HSD393225 IBZ393195:IBZ393225 ILV393195:ILV393225 IVR393195:IVR393225 JFN393195:JFN393225 JPJ393195:JPJ393225 JZF393195:JZF393225 KJB393195:KJB393225 KSX393195:KSX393225 LCT393195:LCT393225 LMP393195:LMP393225 LWL393195:LWL393225 MGH393195:MGH393225 MQD393195:MQD393225 MZZ393195:MZZ393225 NJV393195:NJV393225 NTR393195:NTR393225 ODN393195:ODN393225 ONJ393195:ONJ393225 OXF393195:OXF393225 PHB393195:PHB393225 PQX393195:PQX393225 QAT393195:QAT393225 QKP393195:QKP393225 QUL393195:QUL393225 REH393195:REH393225 ROD393195:ROD393225 RXZ393195:RXZ393225 SHV393195:SHV393225 SRR393195:SRR393225 TBN393195:TBN393225 TLJ393195:TLJ393225 TVF393195:TVF393225 UFB393195:UFB393225 UOX393195:UOX393225 UYT393195:UYT393225 VIP393195:VIP393225 VSL393195:VSL393225 WCH393195:WCH393225 WMD393195:WMD393225 WVZ393195:WVZ393225 Z458731:Z458761 JN458731:JN458761 TJ458731:TJ458761 ADF458731:ADF458761 ANB458731:ANB458761 AWX458731:AWX458761 BGT458731:BGT458761 BQP458731:BQP458761 CAL458731:CAL458761 CKH458731:CKH458761 CUD458731:CUD458761 DDZ458731:DDZ458761 DNV458731:DNV458761 DXR458731:DXR458761 EHN458731:EHN458761 ERJ458731:ERJ458761 FBF458731:FBF458761 FLB458731:FLB458761 FUX458731:FUX458761 GET458731:GET458761 GOP458731:GOP458761 GYL458731:GYL458761 HIH458731:HIH458761 HSD458731:HSD458761 IBZ458731:IBZ458761 ILV458731:ILV458761 IVR458731:IVR458761 JFN458731:JFN458761 JPJ458731:JPJ458761 JZF458731:JZF458761 KJB458731:KJB458761 KSX458731:KSX458761 LCT458731:LCT458761 LMP458731:LMP458761 LWL458731:LWL458761 MGH458731:MGH458761 MQD458731:MQD458761 MZZ458731:MZZ458761 NJV458731:NJV458761 NTR458731:NTR458761 ODN458731:ODN458761 ONJ458731:ONJ458761 OXF458731:OXF458761 PHB458731:PHB458761 PQX458731:PQX458761 QAT458731:QAT458761 QKP458731:QKP458761 QUL458731:QUL458761 REH458731:REH458761 ROD458731:ROD458761 RXZ458731:RXZ458761 SHV458731:SHV458761 SRR458731:SRR458761 TBN458731:TBN458761 TLJ458731:TLJ458761 TVF458731:TVF458761 UFB458731:UFB458761 UOX458731:UOX458761 UYT458731:UYT458761 VIP458731:VIP458761 VSL458731:VSL458761 WCH458731:WCH458761 WMD458731:WMD458761 WVZ458731:WVZ458761 Z524267:Z524297 JN524267:JN524297 TJ524267:TJ524297 ADF524267:ADF524297 ANB524267:ANB524297 AWX524267:AWX524297 BGT524267:BGT524297 BQP524267:BQP524297 CAL524267:CAL524297 CKH524267:CKH524297 CUD524267:CUD524297 DDZ524267:DDZ524297 DNV524267:DNV524297 DXR524267:DXR524297 EHN524267:EHN524297 ERJ524267:ERJ524297 FBF524267:FBF524297 FLB524267:FLB524297 FUX524267:FUX524297 GET524267:GET524297 GOP524267:GOP524297 GYL524267:GYL524297 HIH524267:HIH524297 HSD524267:HSD524297 IBZ524267:IBZ524297 ILV524267:ILV524297 IVR524267:IVR524297 JFN524267:JFN524297 JPJ524267:JPJ524297 JZF524267:JZF524297 KJB524267:KJB524297 KSX524267:KSX524297 LCT524267:LCT524297 LMP524267:LMP524297 LWL524267:LWL524297 MGH524267:MGH524297 MQD524267:MQD524297 MZZ524267:MZZ524297 NJV524267:NJV524297 NTR524267:NTR524297 ODN524267:ODN524297 ONJ524267:ONJ524297 OXF524267:OXF524297 PHB524267:PHB524297 PQX524267:PQX524297 QAT524267:QAT524297 QKP524267:QKP524297 QUL524267:QUL524297 REH524267:REH524297 ROD524267:ROD524297 RXZ524267:RXZ524297 SHV524267:SHV524297 SRR524267:SRR524297 TBN524267:TBN524297 TLJ524267:TLJ524297 TVF524267:TVF524297 UFB524267:UFB524297 UOX524267:UOX524297 UYT524267:UYT524297 VIP524267:VIP524297 VSL524267:VSL524297 WCH524267:WCH524297 WMD524267:WMD524297 WVZ524267:WVZ524297 Z589803:Z589833 JN589803:JN589833 TJ589803:TJ589833 ADF589803:ADF589833 ANB589803:ANB589833 AWX589803:AWX589833 BGT589803:BGT589833 BQP589803:BQP589833 CAL589803:CAL589833 CKH589803:CKH589833 CUD589803:CUD589833 DDZ589803:DDZ589833 DNV589803:DNV589833 DXR589803:DXR589833 EHN589803:EHN589833 ERJ589803:ERJ589833 FBF589803:FBF589833 FLB589803:FLB589833 FUX589803:FUX589833 GET589803:GET589833 GOP589803:GOP589833 GYL589803:GYL589833 HIH589803:HIH589833 HSD589803:HSD589833 IBZ589803:IBZ589833 ILV589803:ILV589833 IVR589803:IVR589833 JFN589803:JFN589833 JPJ589803:JPJ589833 JZF589803:JZF589833 KJB589803:KJB589833 KSX589803:KSX589833 LCT589803:LCT589833 LMP589803:LMP589833 LWL589803:LWL589833 MGH589803:MGH589833 MQD589803:MQD589833 MZZ589803:MZZ589833 NJV589803:NJV589833 NTR589803:NTR589833 ODN589803:ODN589833 ONJ589803:ONJ589833 OXF589803:OXF589833 PHB589803:PHB589833 PQX589803:PQX589833 QAT589803:QAT589833 QKP589803:QKP589833 QUL589803:QUL589833 REH589803:REH589833 ROD589803:ROD589833 RXZ589803:RXZ589833 SHV589803:SHV589833 SRR589803:SRR589833 TBN589803:TBN589833 TLJ589803:TLJ589833 TVF589803:TVF589833 UFB589803:UFB589833 UOX589803:UOX589833 UYT589803:UYT589833 VIP589803:VIP589833 VSL589803:VSL589833 WCH589803:WCH589833 WMD589803:WMD589833 WVZ589803:WVZ589833 Z655339:Z655369 JN655339:JN655369 TJ655339:TJ655369 ADF655339:ADF655369 ANB655339:ANB655369 AWX655339:AWX655369 BGT655339:BGT655369 BQP655339:BQP655369 CAL655339:CAL655369 CKH655339:CKH655369 CUD655339:CUD655369 DDZ655339:DDZ655369 DNV655339:DNV655369 DXR655339:DXR655369 EHN655339:EHN655369 ERJ655339:ERJ655369 FBF655339:FBF655369 FLB655339:FLB655369 FUX655339:FUX655369 GET655339:GET655369 GOP655339:GOP655369 GYL655339:GYL655369 HIH655339:HIH655369 HSD655339:HSD655369 IBZ655339:IBZ655369 ILV655339:ILV655369 IVR655339:IVR655369 JFN655339:JFN655369 JPJ655339:JPJ655369 JZF655339:JZF655369 KJB655339:KJB655369 KSX655339:KSX655369 LCT655339:LCT655369 LMP655339:LMP655369 LWL655339:LWL655369 MGH655339:MGH655369 MQD655339:MQD655369 MZZ655339:MZZ655369 NJV655339:NJV655369 NTR655339:NTR655369 ODN655339:ODN655369 ONJ655339:ONJ655369 OXF655339:OXF655369 PHB655339:PHB655369 PQX655339:PQX655369 QAT655339:QAT655369 QKP655339:QKP655369 QUL655339:QUL655369 REH655339:REH655369 ROD655339:ROD655369 RXZ655339:RXZ655369 SHV655339:SHV655369 SRR655339:SRR655369 TBN655339:TBN655369 TLJ655339:TLJ655369 TVF655339:TVF655369 UFB655339:UFB655369 UOX655339:UOX655369 UYT655339:UYT655369 VIP655339:VIP655369 VSL655339:VSL655369 WCH655339:WCH655369 WMD655339:WMD655369 WVZ655339:WVZ655369 Z720875:Z720905 JN720875:JN720905 TJ720875:TJ720905 ADF720875:ADF720905 ANB720875:ANB720905 AWX720875:AWX720905 BGT720875:BGT720905 BQP720875:BQP720905 CAL720875:CAL720905 CKH720875:CKH720905 CUD720875:CUD720905 DDZ720875:DDZ720905 DNV720875:DNV720905 DXR720875:DXR720905 EHN720875:EHN720905 ERJ720875:ERJ720905 FBF720875:FBF720905 FLB720875:FLB720905 FUX720875:FUX720905 GET720875:GET720905 GOP720875:GOP720905 GYL720875:GYL720905 HIH720875:HIH720905 HSD720875:HSD720905 IBZ720875:IBZ720905 ILV720875:ILV720905 IVR720875:IVR720905 JFN720875:JFN720905 JPJ720875:JPJ720905 JZF720875:JZF720905 KJB720875:KJB720905 KSX720875:KSX720905 LCT720875:LCT720905 LMP720875:LMP720905 LWL720875:LWL720905 MGH720875:MGH720905 MQD720875:MQD720905 MZZ720875:MZZ720905 NJV720875:NJV720905 NTR720875:NTR720905 ODN720875:ODN720905 ONJ720875:ONJ720905 OXF720875:OXF720905 PHB720875:PHB720905 PQX720875:PQX720905 QAT720875:QAT720905 QKP720875:QKP720905 QUL720875:QUL720905 REH720875:REH720905 ROD720875:ROD720905 RXZ720875:RXZ720905 SHV720875:SHV720905 SRR720875:SRR720905 TBN720875:TBN720905 TLJ720875:TLJ720905 TVF720875:TVF720905 UFB720875:UFB720905 UOX720875:UOX720905 UYT720875:UYT720905 VIP720875:VIP720905 VSL720875:VSL720905 WCH720875:WCH720905 WMD720875:WMD720905 WVZ720875:WVZ720905 Z786411:Z786441 JN786411:JN786441 TJ786411:TJ786441 ADF786411:ADF786441 ANB786411:ANB786441 AWX786411:AWX786441 BGT786411:BGT786441 BQP786411:BQP786441 CAL786411:CAL786441 CKH786411:CKH786441 CUD786411:CUD786441 DDZ786411:DDZ786441 DNV786411:DNV786441 DXR786411:DXR786441 EHN786411:EHN786441 ERJ786411:ERJ786441 FBF786411:FBF786441 FLB786411:FLB786441 FUX786411:FUX786441 GET786411:GET786441 GOP786411:GOP786441 GYL786411:GYL786441 HIH786411:HIH786441 HSD786411:HSD786441 IBZ786411:IBZ786441 ILV786411:ILV786441 IVR786411:IVR786441 JFN786411:JFN786441 JPJ786411:JPJ786441 JZF786411:JZF786441 KJB786411:KJB786441 KSX786411:KSX786441 LCT786411:LCT786441 LMP786411:LMP786441 LWL786411:LWL786441 MGH786411:MGH786441 MQD786411:MQD786441 MZZ786411:MZZ786441 NJV786411:NJV786441 NTR786411:NTR786441 ODN786411:ODN786441 ONJ786411:ONJ786441 OXF786411:OXF786441 PHB786411:PHB786441 PQX786411:PQX786441 QAT786411:QAT786441 QKP786411:QKP786441 QUL786411:QUL786441 REH786411:REH786441 ROD786411:ROD786441 RXZ786411:RXZ786441 SHV786411:SHV786441 SRR786411:SRR786441 TBN786411:TBN786441 TLJ786411:TLJ786441 TVF786411:TVF786441 UFB786411:UFB786441 UOX786411:UOX786441 UYT786411:UYT786441 VIP786411:VIP786441 VSL786411:VSL786441 WCH786411:WCH786441 WMD786411:WMD786441 WVZ786411:WVZ786441 Z851947:Z851977 JN851947:JN851977 TJ851947:TJ851977 ADF851947:ADF851977 ANB851947:ANB851977 AWX851947:AWX851977 BGT851947:BGT851977 BQP851947:BQP851977 CAL851947:CAL851977 CKH851947:CKH851977 CUD851947:CUD851977 DDZ851947:DDZ851977 DNV851947:DNV851977 DXR851947:DXR851977 EHN851947:EHN851977 ERJ851947:ERJ851977 FBF851947:FBF851977 FLB851947:FLB851977 FUX851947:FUX851977 GET851947:GET851977 GOP851947:GOP851977 GYL851947:GYL851977 HIH851947:HIH851977 HSD851947:HSD851977 IBZ851947:IBZ851977 ILV851947:ILV851977 IVR851947:IVR851977 JFN851947:JFN851977 JPJ851947:JPJ851977 JZF851947:JZF851977 KJB851947:KJB851977 KSX851947:KSX851977 LCT851947:LCT851977 LMP851947:LMP851977 LWL851947:LWL851977 MGH851947:MGH851977 MQD851947:MQD851977 MZZ851947:MZZ851977 NJV851947:NJV851977 NTR851947:NTR851977 ODN851947:ODN851977 ONJ851947:ONJ851977 OXF851947:OXF851977 PHB851947:PHB851977 PQX851947:PQX851977 QAT851947:QAT851977 QKP851947:QKP851977 QUL851947:QUL851977 REH851947:REH851977 ROD851947:ROD851977 RXZ851947:RXZ851977 SHV851947:SHV851977 SRR851947:SRR851977 TBN851947:TBN851977 TLJ851947:TLJ851977 TVF851947:TVF851977 UFB851947:UFB851977 UOX851947:UOX851977 UYT851947:UYT851977 VIP851947:VIP851977 VSL851947:VSL851977 WCH851947:WCH851977 WMD851947:WMD851977 WVZ851947:WVZ851977 Z917483:Z917513 JN917483:JN917513 TJ917483:TJ917513 ADF917483:ADF917513 ANB917483:ANB917513 AWX917483:AWX917513 BGT917483:BGT917513 BQP917483:BQP917513 CAL917483:CAL917513 CKH917483:CKH917513 CUD917483:CUD917513 DDZ917483:DDZ917513 DNV917483:DNV917513 DXR917483:DXR917513 EHN917483:EHN917513 ERJ917483:ERJ917513 FBF917483:FBF917513 FLB917483:FLB917513 FUX917483:FUX917513 GET917483:GET917513 GOP917483:GOP917513 GYL917483:GYL917513 HIH917483:HIH917513 HSD917483:HSD917513 IBZ917483:IBZ917513 ILV917483:ILV917513 IVR917483:IVR917513 JFN917483:JFN917513 JPJ917483:JPJ917513 JZF917483:JZF917513 KJB917483:KJB917513 KSX917483:KSX917513 LCT917483:LCT917513 LMP917483:LMP917513 LWL917483:LWL917513 MGH917483:MGH917513 MQD917483:MQD917513 MZZ917483:MZZ917513 NJV917483:NJV917513 NTR917483:NTR917513 ODN917483:ODN917513 ONJ917483:ONJ917513 OXF917483:OXF917513 PHB917483:PHB917513 PQX917483:PQX917513 QAT917483:QAT917513 QKP917483:QKP917513 QUL917483:QUL917513 REH917483:REH917513 ROD917483:ROD917513 RXZ917483:RXZ917513 SHV917483:SHV917513 SRR917483:SRR917513 TBN917483:TBN917513 TLJ917483:TLJ917513 TVF917483:TVF917513 UFB917483:UFB917513 UOX917483:UOX917513 UYT917483:UYT917513 VIP917483:VIP917513 VSL917483:VSL917513 WCH917483:WCH917513 WMD917483:WMD917513 WVZ917483:WVZ917513 Z983019:Z983049 JN983019:JN983049 TJ983019:TJ983049 ADF983019:ADF983049 ANB983019:ANB983049 AWX983019:AWX983049 BGT983019:BGT983049 BQP983019:BQP983049 CAL983019:CAL983049 CKH983019:CKH983049 CUD983019:CUD983049 DDZ983019:DDZ983049 DNV983019:DNV983049 DXR983019:DXR983049 EHN983019:EHN983049 ERJ983019:ERJ983049 FBF983019:FBF983049 FLB983019:FLB983049 FUX983019:FUX983049 GET983019:GET983049 GOP983019:GOP983049 GYL983019:GYL983049 HIH983019:HIH983049 HSD983019:HSD983049 IBZ983019:IBZ983049 ILV983019:ILV983049 IVR983019:IVR983049 JFN983019:JFN983049 JPJ983019:JPJ983049 JZF983019:JZF983049 KJB983019:KJB983049 KSX983019:KSX983049 LCT983019:LCT983049 LMP983019:LMP983049 LWL983019:LWL983049 MGH983019:MGH983049 MQD983019:MQD983049 MZZ983019:MZZ983049 NJV983019:NJV983049 NTR983019:NTR983049 ODN983019:ODN983049 ONJ983019:ONJ983049 OXF983019:OXF983049 PHB983019:PHB983049 PQX983019:PQX983049 QAT983019:QAT983049 QKP983019:QKP983049 QUL983019:QUL983049 REH983019:REH983049 ROD983019:ROD983049 RXZ983019:RXZ983049 SHV983019:SHV983049 SRR983019:SRR983049 TBN983019:TBN983049 TLJ983019:TLJ983049 TVF983019:TVF983049 UFB983019:UFB983049 UOX983019:UOX983049 UYT983019:UYT983049 VIP983019:VIP983049 VSL983019:VSL983049 WCH983019:WCH983049 WMD983019:WMD983049 JN4:JN20 TJ4:TJ20 ADF4:ADF20 ANB4:ANB20 AWX4:AWX20 BGT4:BGT20 BQP4:BQP20 CAL4:CAL20 CKH4:CKH20 CUD4:CUD20 DDZ4:DDZ20 DNV4:DNV20 DXR4:DXR20 EHN4:EHN20 ERJ4:ERJ20 FBF4:FBF20 FLB4:FLB20 FUX4:FUX20 GET4:GET20 GOP4:GOP20 GYL4:GYL20 HIH4:HIH20 HSD4:HSD20 IBZ4:IBZ20 ILV4:ILV20 IVR4:IVR20 JFN4:JFN20 JPJ4:JPJ20 JZF4:JZF20 KJB4:KJB20 KSX4:KSX20 LCT4:LCT20 LMP4:LMP20 LWL4:LWL20 MGH4:MGH20 MQD4:MQD20 MZZ4:MZZ20 NJV4:NJV20 NTR4:NTR20 ODN4:ODN20 ONJ4:ONJ20 OXF4:OXF20 PHB4:PHB20 PQX4:PQX20 QAT4:QAT20 QKP4:QKP20 QUL4:QUL20 REH4:REH20 ROD4:ROD20 RXZ4:RXZ20 SHV4:SHV20 SRR4:SRR20 TBN4:TBN20 TLJ4:TLJ20 TVF4:TVF20 UFB4:UFB20 UOX4:UOX20 UYT4:UYT20 VIP4:VIP20 VSL4:VSL20 WCH4:WCH20 WMD4:WMD20 WVZ4:WVZ20 Z4:Z20" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"Propia, Arrendada, Familiar "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JH65515:JH65545 TD65515:TD65545 ACZ65515:ACZ65545 AMV65515:AMV65545 AWR65515:AWR65545 BGN65515:BGN65545 BQJ65515:BQJ65545 CAF65515:CAF65545 CKB65515:CKB65545 CTX65515:CTX65545 DDT65515:DDT65545 DNP65515:DNP65545 DXL65515:DXL65545 EHH65515:EHH65545 ERD65515:ERD65545 FAZ65515:FAZ65545 FKV65515:FKV65545 FUR65515:FUR65545 GEN65515:GEN65545 GOJ65515:GOJ65545 GYF65515:GYF65545 HIB65515:HIB65545 HRX65515:HRX65545 IBT65515:IBT65545 ILP65515:ILP65545 IVL65515:IVL65545 JFH65515:JFH65545 JPD65515:JPD65545 JYZ65515:JYZ65545 KIV65515:KIV65545 KSR65515:KSR65545 LCN65515:LCN65545 LMJ65515:LMJ65545 LWF65515:LWF65545 MGB65515:MGB65545 MPX65515:MPX65545 MZT65515:MZT65545 NJP65515:NJP65545 NTL65515:NTL65545 ODH65515:ODH65545 OND65515:OND65545 OWZ65515:OWZ65545 PGV65515:PGV65545 PQR65515:PQR65545 QAN65515:QAN65545 QKJ65515:QKJ65545 QUF65515:QUF65545 REB65515:REB65545 RNX65515:RNX65545 RXT65515:RXT65545 SHP65515:SHP65545 SRL65515:SRL65545 TBH65515:TBH65545 TLD65515:TLD65545 TUZ65515:TUZ65545 UEV65515:UEV65545 UOR65515:UOR65545 UYN65515:UYN65545 VIJ65515:VIJ65545 VSF65515:VSF65545 WCB65515:WCB65545 WLX65515:WLX65545 WVT65515:WVT65545 JH131051:JH131081 TD131051:TD131081 ACZ131051:ACZ131081 AMV131051:AMV131081 AWR131051:AWR131081 BGN131051:BGN131081 BQJ131051:BQJ131081 CAF131051:CAF131081 CKB131051:CKB131081 CTX131051:CTX131081 DDT131051:DDT131081 DNP131051:DNP131081 DXL131051:DXL131081 EHH131051:EHH131081 ERD131051:ERD131081 FAZ131051:FAZ131081 FKV131051:FKV131081 FUR131051:FUR131081 GEN131051:GEN131081 GOJ131051:GOJ131081 GYF131051:GYF131081 HIB131051:HIB131081 HRX131051:HRX131081 IBT131051:IBT131081 ILP131051:ILP131081 IVL131051:IVL131081 JFH131051:JFH131081 JPD131051:JPD131081 JYZ131051:JYZ131081 KIV131051:KIV131081 KSR131051:KSR131081 LCN131051:LCN131081 LMJ131051:LMJ131081 LWF131051:LWF131081 MGB131051:MGB131081 MPX131051:MPX131081 MZT131051:MZT131081 NJP131051:NJP131081 NTL131051:NTL131081 ODH131051:ODH131081 OND131051:OND131081 OWZ131051:OWZ131081 PGV131051:PGV131081 PQR131051:PQR131081 QAN131051:QAN131081 QKJ131051:QKJ131081 QUF131051:QUF131081 REB131051:REB131081 RNX131051:RNX131081 RXT131051:RXT131081 SHP131051:SHP131081 SRL131051:SRL131081 TBH131051:TBH131081 TLD131051:TLD131081 TUZ131051:TUZ131081 UEV131051:UEV131081 UOR131051:UOR131081 UYN131051:UYN131081 VIJ131051:VIJ131081 VSF131051:VSF131081 WCB131051:WCB131081 WLX131051:WLX131081 WVT131051:WVT131081 JH196587:JH196617 TD196587:TD196617 ACZ196587:ACZ196617 AMV196587:AMV196617 AWR196587:AWR196617 BGN196587:BGN196617 BQJ196587:BQJ196617 CAF196587:CAF196617 CKB196587:CKB196617 CTX196587:CTX196617 DDT196587:DDT196617 DNP196587:DNP196617 DXL196587:DXL196617 EHH196587:EHH196617 ERD196587:ERD196617 FAZ196587:FAZ196617 FKV196587:FKV196617 FUR196587:FUR196617 GEN196587:GEN196617 GOJ196587:GOJ196617 GYF196587:GYF196617 HIB196587:HIB196617 HRX196587:HRX196617 IBT196587:IBT196617 ILP196587:ILP196617 IVL196587:IVL196617 JFH196587:JFH196617 JPD196587:JPD196617 JYZ196587:JYZ196617 KIV196587:KIV196617 KSR196587:KSR196617 LCN196587:LCN196617 LMJ196587:LMJ196617 LWF196587:LWF196617 MGB196587:MGB196617 MPX196587:MPX196617 MZT196587:MZT196617 NJP196587:NJP196617 NTL196587:NTL196617 ODH196587:ODH196617 OND196587:OND196617 OWZ196587:OWZ196617 PGV196587:PGV196617 PQR196587:PQR196617 QAN196587:QAN196617 QKJ196587:QKJ196617 QUF196587:QUF196617 REB196587:REB196617 RNX196587:RNX196617 RXT196587:RXT196617 SHP196587:SHP196617 SRL196587:SRL196617 TBH196587:TBH196617 TLD196587:TLD196617 TUZ196587:TUZ196617 UEV196587:UEV196617 UOR196587:UOR196617 UYN196587:UYN196617 VIJ196587:VIJ196617 VSF196587:VSF196617 WCB196587:WCB196617 WLX196587:WLX196617 WVT196587:WVT196617 JH262123:JH262153 TD262123:TD262153 ACZ262123:ACZ262153 AMV262123:AMV262153 AWR262123:AWR262153 BGN262123:BGN262153 BQJ262123:BQJ262153 CAF262123:CAF262153 CKB262123:CKB262153 CTX262123:CTX262153 DDT262123:DDT262153 DNP262123:DNP262153 DXL262123:DXL262153 EHH262123:EHH262153 ERD262123:ERD262153 FAZ262123:FAZ262153 FKV262123:FKV262153 FUR262123:FUR262153 GEN262123:GEN262153 GOJ262123:GOJ262153 GYF262123:GYF262153 HIB262123:HIB262153 HRX262123:HRX262153 IBT262123:IBT262153 ILP262123:ILP262153 IVL262123:IVL262153 JFH262123:JFH262153 JPD262123:JPD262153 JYZ262123:JYZ262153 KIV262123:KIV262153 KSR262123:KSR262153 LCN262123:LCN262153 LMJ262123:LMJ262153 LWF262123:LWF262153 MGB262123:MGB262153 MPX262123:MPX262153 MZT262123:MZT262153 NJP262123:NJP262153 NTL262123:NTL262153 ODH262123:ODH262153 OND262123:OND262153 OWZ262123:OWZ262153 PGV262123:PGV262153 PQR262123:PQR262153 QAN262123:QAN262153 QKJ262123:QKJ262153 QUF262123:QUF262153 REB262123:REB262153 RNX262123:RNX262153 RXT262123:RXT262153 SHP262123:SHP262153 SRL262123:SRL262153 TBH262123:TBH262153 TLD262123:TLD262153 TUZ262123:TUZ262153 UEV262123:UEV262153 UOR262123:UOR262153 UYN262123:UYN262153 VIJ262123:VIJ262153 VSF262123:VSF262153 WCB262123:WCB262153 WLX262123:WLX262153 WVT262123:WVT262153 JH327659:JH327689 TD327659:TD327689 ACZ327659:ACZ327689 AMV327659:AMV327689 AWR327659:AWR327689 BGN327659:BGN327689 BQJ327659:BQJ327689 CAF327659:CAF327689 CKB327659:CKB327689 CTX327659:CTX327689 DDT327659:DDT327689 DNP327659:DNP327689 DXL327659:DXL327689 EHH327659:EHH327689 ERD327659:ERD327689 FAZ327659:FAZ327689 FKV327659:FKV327689 FUR327659:FUR327689 GEN327659:GEN327689 GOJ327659:GOJ327689 GYF327659:GYF327689 HIB327659:HIB327689 HRX327659:HRX327689 IBT327659:IBT327689 ILP327659:ILP327689 IVL327659:IVL327689 JFH327659:JFH327689 JPD327659:JPD327689 JYZ327659:JYZ327689 KIV327659:KIV327689 KSR327659:KSR327689 LCN327659:LCN327689 LMJ327659:LMJ327689 LWF327659:LWF327689 MGB327659:MGB327689 MPX327659:MPX327689 MZT327659:MZT327689 NJP327659:NJP327689 NTL327659:NTL327689 ODH327659:ODH327689 OND327659:OND327689 OWZ327659:OWZ327689 PGV327659:PGV327689 PQR327659:PQR327689 QAN327659:QAN327689 QKJ327659:QKJ327689 QUF327659:QUF327689 REB327659:REB327689 RNX327659:RNX327689 RXT327659:RXT327689 SHP327659:SHP327689 SRL327659:SRL327689 TBH327659:TBH327689 TLD327659:TLD327689 TUZ327659:TUZ327689 UEV327659:UEV327689 UOR327659:UOR327689 UYN327659:UYN327689 VIJ327659:VIJ327689 VSF327659:VSF327689 WCB327659:WCB327689 WLX327659:WLX327689 WVT327659:WVT327689 JH393195:JH393225 TD393195:TD393225 ACZ393195:ACZ393225 AMV393195:AMV393225 AWR393195:AWR393225 BGN393195:BGN393225 BQJ393195:BQJ393225 CAF393195:CAF393225 CKB393195:CKB393225 CTX393195:CTX393225 DDT393195:DDT393225 DNP393195:DNP393225 DXL393195:DXL393225 EHH393195:EHH393225 ERD393195:ERD393225 FAZ393195:FAZ393225 FKV393195:FKV393225 FUR393195:FUR393225 GEN393195:GEN393225 GOJ393195:GOJ393225 GYF393195:GYF393225 HIB393195:HIB393225 HRX393195:HRX393225 IBT393195:IBT393225 ILP393195:ILP393225 IVL393195:IVL393225 JFH393195:JFH393225 JPD393195:JPD393225 JYZ393195:JYZ393225 KIV393195:KIV393225 KSR393195:KSR393225 LCN393195:LCN393225 LMJ393195:LMJ393225 LWF393195:LWF393225 MGB393195:MGB393225 MPX393195:MPX393225 MZT393195:MZT393225 NJP393195:NJP393225 NTL393195:NTL393225 ODH393195:ODH393225 OND393195:OND393225 OWZ393195:OWZ393225 PGV393195:PGV393225 PQR393195:PQR393225 QAN393195:QAN393225 QKJ393195:QKJ393225 QUF393195:QUF393225 REB393195:REB393225 RNX393195:RNX393225 RXT393195:RXT393225 SHP393195:SHP393225 SRL393195:SRL393225 TBH393195:TBH393225 TLD393195:TLD393225 TUZ393195:TUZ393225 UEV393195:UEV393225 UOR393195:UOR393225 UYN393195:UYN393225 VIJ393195:VIJ393225 VSF393195:VSF393225 WCB393195:WCB393225 WLX393195:WLX393225 WVT393195:WVT393225 JH458731:JH458761 TD458731:TD458761 ACZ458731:ACZ458761 AMV458731:AMV458761 AWR458731:AWR458761 BGN458731:BGN458761 BQJ458731:BQJ458761 CAF458731:CAF458761 CKB458731:CKB458761 CTX458731:CTX458761 DDT458731:DDT458761 DNP458731:DNP458761 DXL458731:DXL458761 EHH458731:EHH458761 ERD458731:ERD458761 FAZ458731:FAZ458761 FKV458731:FKV458761 FUR458731:FUR458761 GEN458731:GEN458761 GOJ458731:GOJ458761 GYF458731:GYF458761 HIB458731:HIB458761 HRX458731:HRX458761 IBT458731:IBT458761 ILP458731:ILP458761 IVL458731:IVL458761 JFH458731:JFH458761 JPD458731:JPD458761 JYZ458731:JYZ458761 KIV458731:KIV458761 KSR458731:KSR458761 LCN458731:LCN458761 LMJ458731:LMJ458761 LWF458731:LWF458761 MGB458731:MGB458761 MPX458731:MPX458761 MZT458731:MZT458761 NJP458731:NJP458761 NTL458731:NTL458761 ODH458731:ODH458761 OND458731:OND458761 OWZ458731:OWZ458761 PGV458731:PGV458761 PQR458731:PQR458761 QAN458731:QAN458761 QKJ458731:QKJ458761 QUF458731:QUF458761 REB458731:REB458761 RNX458731:RNX458761 RXT458731:RXT458761 SHP458731:SHP458761 SRL458731:SRL458761 TBH458731:TBH458761 TLD458731:TLD458761 TUZ458731:TUZ458761 UEV458731:UEV458761 UOR458731:UOR458761 UYN458731:UYN458761 VIJ458731:VIJ458761 VSF458731:VSF458761 WCB458731:WCB458761 WLX458731:WLX458761 WVT458731:WVT458761 JH524267:JH524297 TD524267:TD524297 ACZ524267:ACZ524297 AMV524267:AMV524297 AWR524267:AWR524297 BGN524267:BGN524297 BQJ524267:BQJ524297 CAF524267:CAF524297 CKB524267:CKB524297 CTX524267:CTX524297 DDT524267:DDT524297 DNP524267:DNP524297 DXL524267:DXL524297 EHH524267:EHH524297 ERD524267:ERD524297 FAZ524267:FAZ524297 FKV524267:FKV524297 FUR524267:FUR524297 GEN524267:GEN524297 GOJ524267:GOJ524297 GYF524267:GYF524297 HIB524267:HIB524297 HRX524267:HRX524297 IBT524267:IBT524297 ILP524267:ILP524297 IVL524267:IVL524297 JFH524267:JFH524297 JPD524267:JPD524297 JYZ524267:JYZ524297 KIV524267:KIV524297 KSR524267:KSR524297 LCN524267:LCN524297 LMJ524267:LMJ524297 LWF524267:LWF524297 MGB524267:MGB524297 MPX524267:MPX524297 MZT524267:MZT524297 NJP524267:NJP524297 NTL524267:NTL524297 ODH524267:ODH524297 OND524267:OND524297 OWZ524267:OWZ524297 PGV524267:PGV524297 PQR524267:PQR524297 QAN524267:QAN524297 QKJ524267:QKJ524297 QUF524267:QUF524297 REB524267:REB524297 RNX524267:RNX524297 RXT524267:RXT524297 SHP524267:SHP524297 SRL524267:SRL524297 TBH524267:TBH524297 TLD524267:TLD524297 TUZ524267:TUZ524297 UEV524267:UEV524297 UOR524267:UOR524297 UYN524267:UYN524297 VIJ524267:VIJ524297 VSF524267:VSF524297 WCB524267:WCB524297 WLX524267:WLX524297 WVT524267:WVT524297 JH589803:JH589833 TD589803:TD589833 ACZ589803:ACZ589833 AMV589803:AMV589833 AWR589803:AWR589833 BGN589803:BGN589833 BQJ589803:BQJ589833 CAF589803:CAF589833 CKB589803:CKB589833 CTX589803:CTX589833 DDT589803:DDT589833 DNP589803:DNP589833 DXL589803:DXL589833 EHH589803:EHH589833 ERD589803:ERD589833 FAZ589803:FAZ589833 FKV589803:FKV589833 FUR589803:FUR589833 GEN589803:GEN589833 GOJ589803:GOJ589833 GYF589803:GYF589833 HIB589803:HIB589833 HRX589803:HRX589833 IBT589803:IBT589833 ILP589803:ILP589833 IVL589803:IVL589833 JFH589803:JFH589833 JPD589803:JPD589833 JYZ589803:JYZ589833 KIV589803:KIV589833 KSR589803:KSR589833 LCN589803:LCN589833 LMJ589803:LMJ589833 LWF589803:LWF589833 MGB589803:MGB589833 MPX589803:MPX589833 MZT589803:MZT589833 NJP589803:NJP589833 NTL589803:NTL589833 ODH589803:ODH589833 OND589803:OND589833 OWZ589803:OWZ589833 PGV589803:PGV589833 PQR589803:PQR589833 QAN589803:QAN589833 QKJ589803:QKJ589833 QUF589803:QUF589833 REB589803:REB589833 RNX589803:RNX589833 RXT589803:RXT589833 SHP589803:SHP589833 SRL589803:SRL589833 TBH589803:TBH589833 TLD589803:TLD589833 TUZ589803:TUZ589833 UEV589803:UEV589833 UOR589803:UOR589833 UYN589803:UYN589833 VIJ589803:VIJ589833 VSF589803:VSF589833 WCB589803:WCB589833 WLX589803:WLX589833 WVT589803:WVT589833 JH655339:JH655369 TD655339:TD655369 ACZ655339:ACZ655369 AMV655339:AMV655369 AWR655339:AWR655369 BGN655339:BGN655369 BQJ655339:BQJ655369 CAF655339:CAF655369 CKB655339:CKB655369 CTX655339:CTX655369 DDT655339:DDT655369 DNP655339:DNP655369 DXL655339:DXL655369 EHH655339:EHH655369 ERD655339:ERD655369 FAZ655339:FAZ655369 FKV655339:FKV655369 FUR655339:FUR655369 GEN655339:GEN655369 GOJ655339:GOJ655369 GYF655339:GYF655369 HIB655339:HIB655369 HRX655339:HRX655369 IBT655339:IBT655369 ILP655339:ILP655369 IVL655339:IVL655369 JFH655339:JFH655369 JPD655339:JPD655369 JYZ655339:JYZ655369 KIV655339:KIV655369 KSR655339:KSR655369 LCN655339:LCN655369 LMJ655339:LMJ655369 LWF655339:LWF655369 MGB655339:MGB655369 MPX655339:MPX655369 MZT655339:MZT655369 NJP655339:NJP655369 NTL655339:NTL655369 ODH655339:ODH655369 OND655339:OND655369 OWZ655339:OWZ655369 PGV655339:PGV655369 PQR655339:PQR655369 QAN655339:QAN655369 QKJ655339:QKJ655369 QUF655339:QUF655369 REB655339:REB655369 RNX655339:RNX655369 RXT655339:RXT655369 SHP655339:SHP655369 SRL655339:SRL655369 TBH655339:TBH655369 TLD655339:TLD655369 TUZ655339:TUZ655369 UEV655339:UEV655369 UOR655339:UOR655369 UYN655339:UYN655369 VIJ655339:VIJ655369 VSF655339:VSF655369 WCB655339:WCB655369 WLX655339:WLX655369 WVT655339:WVT655369 JH720875:JH720905 TD720875:TD720905 ACZ720875:ACZ720905 AMV720875:AMV720905 AWR720875:AWR720905 BGN720875:BGN720905 BQJ720875:BQJ720905 CAF720875:CAF720905 CKB720875:CKB720905 CTX720875:CTX720905 DDT720875:DDT720905 DNP720875:DNP720905 DXL720875:DXL720905 EHH720875:EHH720905 ERD720875:ERD720905 FAZ720875:FAZ720905 FKV720875:FKV720905 FUR720875:FUR720905 GEN720875:GEN720905 GOJ720875:GOJ720905 GYF720875:GYF720905 HIB720875:HIB720905 HRX720875:HRX720905 IBT720875:IBT720905 ILP720875:ILP720905 IVL720875:IVL720905 JFH720875:JFH720905 JPD720875:JPD720905 JYZ720875:JYZ720905 KIV720875:KIV720905 KSR720875:KSR720905 LCN720875:LCN720905 LMJ720875:LMJ720905 LWF720875:LWF720905 MGB720875:MGB720905 MPX720875:MPX720905 MZT720875:MZT720905 NJP720875:NJP720905 NTL720875:NTL720905 ODH720875:ODH720905 OND720875:OND720905 OWZ720875:OWZ720905 PGV720875:PGV720905 PQR720875:PQR720905 QAN720875:QAN720905 QKJ720875:QKJ720905 QUF720875:QUF720905 REB720875:REB720905 RNX720875:RNX720905 RXT720875:RXT720905 SHP720875:SHP720905 SRL720875:SRL720905 TBH720875:TBH720905 TLD720875:TLD720905 TUZ720875:TUZ720905 UEV720875:UEV720905 UOR720875:UOR720905 UYN720875:UYN720905 VIJ720875:VIJ720905 VSF720875:VSF720905 WCB720875:WCB720905 WLX720875:WLX720905 WVT720875:WVT720905 JH786411:JH786441 TD786411:TD786441 ACZ786411:ACZ786441 AMV786411:AMV786441 AWR786411:AWR786441 BGN786411:BGN786441 BQJ786411:BQJ786441 CAF786411:CAF786441 CKB786411:CKB786441 CTX786411:CTX786441 DDT786411:DDT786441 DNP786411:DNP786441 DXL786411:DXL786441 EHH786411:EHH786441 ERD786411:ERD786441 FAZ786411:FAZ786441 FKV786411:FKV786441 FUR786411:FUR786441 GEN786411:GEN786441 GOJ786411:GOJ786441 GYF786411:GYF786441 HIB786411:HIB786441 HRX786411:HRX786441 IBT786411:IBT786441 ILP786411:ILP786441 IVL786411:IVL786441 JFH786411:JFH786441 JPD786411:JPD786441 JYZ786411:JYZ786441 KIV786411:KIV786441 KSR786411:KSR786441 LCN786411:LCN786441 LMJ786411:LMJ786441 LWF786411:LWF786441 MGB786411:MGB786441 MPX786411:MPX786441 MZT786411:MZT786441 NJP786411:NJP786441 NTL786411:NTL786441 ODH786411:ODH786441 OND786411:OND786441 OWZ786411:OWZ786441 PGV786411:PGV786441 PQR786411:PQR786441 QAN786411:QAN786441 QKJ786411:QKJ786441 QUF786411:QUF786441 REB786411:REB786441 RNX786411:RNX786441 RXT786411:RXT786441 SHP786411:SHP786441 SRL786411:SRL786441 TBH786411:TBH786441 TLD786411:TLD786441 TUZ786411:TUZ786441 UEV786411:UEV786441 UOR786411:UOR786441 UYN786411:UYN786441 VIJ786411:VIJ786441 VSF786411:VSF786441 WCB786411:WCB786441 WLX786411:WLX786441 WVT786411:WVT786441 JH851947:JH851977 TD851947:TD851977 ACZ851947:ACZ851977 AMV851947:AMV851977 AWR851947:AWR851977 BGN851947:BGN851977 BQJ851947:BQJ851977 CAF851947:CAF851977 CKB851947:CKB851977 CTX851947:CTX851977 DDT851947:DDT851977 DNP851947:DNP851977 DXL851947:DXL851977 EHH851947:EHH851977 ERD851947:ERD851977 FAZ851947:FAZ851977 FKV851947:FKV851977 FUR851947:FUR851977 GEN851947:GEN851977 GOJ851947:GOJ851977 GYF851947:GYF851977 HIB851947:HIB851977 HRX851947:HRX851977 IBT851947:IBT851977 ILP851947:ILP851977 IVL851947:IVL851977 JFH851947:JFH851977 JPD851947:JPD851977 JYZ851947:JYZ851977 KIV851947:KIV851977 KSR851947:KSR851977 LCN851947:LCN851977 LMJ851947:LMJ851977 LWF851947:LWF851977 MGB851947:MGB851977 MPX851947:MPX851977 MZT851947:MZT851977 NJP851947:NJP851977 NTL851947:NTL851977 ODH851947:ODH851977 OND851947:OND851977 OWZ851947:OWZ851977 PGV851947:PGV851977 PQR851947:PQR851977 QAN851947:QAN851977 QKJ851947:QKJ851977 QUF851947:QUF851977 REB851947:REB851977 RNX851947:RNX851977 RXT851947:RXT851977 SHP851947:SHP851977 SRL851947:SRL851977 TBH851947:TBH851977 TLD851947:TLD851977 TUZ851947:TUZ851977 UEV851947:UEV851977 UOR851947:UOR851977 UYN851947:UYN851977 VIJ851947:VIJ851977 VSF851947:VSF851977 WCB851947:WCB851977 WLX851947:WLX851977 WVT851947:WVT851977 JH917483:JH917513 TD917483:TD917513 ACZ917483:ACZ917513 AMV917483:AMV917513 AWR917483:AWR917513 BGN917483:BGN917513 BQJ917483:BQJ917513 CAF917483:CAF917513 CKB917483:CKB917513 CTX917483:CTX917513 DDT917483:DDT917513 DNP917483:DNP917513 DXL917483:DXL917513 EHH917483:EHH917513 ERD917483:ERD917513 FAZ917483:FAZ917513 FKV917483:FKV917513 FUR917483:FUR917513 GEN917483:GEN917513 GOJ917483:GOJ917513 GYF917483:GYF917513 HIB917483:HIB917513 HRX917483:HRX917513 IBT917483:IBT917513 ILP917483:ILP917513 IVL917483:IVL917513 JFH917483:JFH917513 JPD917483:JPD917513 JYZ917483:JYZ917513 KIV917483:KIV917513 KSR917483:KSR917513 LCN917483:LCN917513 LMJ917483:LMJ917513 LWF917483:LWF917513 MGB917483:MGB917513 MPX917483:MPX917513 MZT917483:MZT917513 NJP917483:NJP917513 NTL917483:NTL917513 ODH917483:ODH917513 OND917483:OND917513 OWZ917483:OWZ917513 PGV917483:PGV917513 PQR917483:PQR917513 QAN917483:QAN917513 QKJ917483:QKJ917513 QUF917483:QUF917513 REB917483:REB917513 RNX917483:RNX917513 RXT917483:RXT917513 SHP917483:SHP917513 SRL917483:SRL917513 TBH917483:TBH917513 TLD917483:TLD917513 TUZ917483:TUZ917513 UEV917483:UEV917513 UOR917483:UOR917513 UYN917483:UYN917513 VIJ917483:VIJ917513 VSF917483:VSF917513 WCB917483:WCB917513 WLX917483:WLX917513 WVT917483:WVT917513 JH983019:JH983049 TD983019:TD983049 ACZ983019:ACZ983049 AMV983019:AMV983049 AWR983019:AWR983049 BGN983019:BGN983049 BQJ983019:BQJ983049 CAF983019:CAF983049 CKB983019:CKB983049 CTX983019:CTX983049 DDT983019:DDT983049 DNP983019:DNP983049 DXL983019:DXL983049 EHH983019:EHH983049 ERD983019:ERD983049 FAZ983019:FAZ983049 FKV983019:FKV983049 FUR983019:FUR983049 GEN983019:GEN983049 GOJ983019:GOJ983049 GYF983019:GYF983049 HIB983019:HIB983049 HRX983019:HRX983049 IBT983019:IBT983049 ILP983019:ILP983049 IVL983019:IVL983049 JFH983019:JFH983049 JPD983019:JPD983049 JYZ983019:JYZ983049 KIV983019:KIV983049 KSR983019:KSR983049 LCN983019:LCN983049 LMJ983019:LMJ983049 LWF983019:LWF983049 MGB983019:MGB983049 MPX983019:MPX983049 MZT983019:MZT983049 NJP983019:NJP983049 NTL983019:NTL983049 ODH983019:ODH983049 OND983019:OND983049 OWZ983019:OWZ983049 PGV983019:PGV983049 PQR983019:PQR983049 QAN983019:QAN983049 QKJ983019:QKJ983049 QUF983019:QUF983049 REB983019:REB983049 RNX983019:RNX983049 RXT983019:RXT983049 SHP983019:SHP983049 SRL983019:SRL983049 TBH983019:TBH983049 TLD983019:TLD983049 TUZ983019:TUZ983049 UEV983019:UEV983049 UOR983019:UOR983049 UYN983019:UYN983049 VIJ983019:VIJ983049 VSF983019:VSF983049 WCB983019:WCB983049 WLX983019:WLX983049 WVT983019:WVT983049 L983019:L983049 L65515:L65545 L131051:L131081 L196587:L196617 L262123:L262153 L327659:L327689 L393195:L393225 L458731:L458761 L524267:L524297 L589803:L589833 L655339:L655369 L720875:L720905 L786411:L786441 L851947:L851977 L917483:L917513 WVT4:WVT20 WLX4:WLX20 WCB4:WCB20 VSF4:VSF20 VIJ4:VIJ20 UYN4:UYN20 UOR4:UOR20 UEV4:UEV20 TUZ4:TUZ20 TLD4:TLD20 TBH4:TBH20 SRL4:SRL20 SHP4:SHP20 RXT4:RXT20 RNX4:RNX20 REB4:REB20 QUF4:QUF20 QKJ4:QKJ20 QAN4:QAN20 PQR4:PQR20 PGV4:PGV20 OWZ4:OWZ20 OND4:OND20 ODH4:ODH20 NTL4:NTL20 NJP4:NJP20 MZT4:MZT20 MPX4:MPX20 MGB4:MGB20 LWF4:LWF20 LMJ4:LMJ20 LCN4:LCN20 KSR4:KSR20 KIV4:KIV20 JYZ4:JYZ20 JPD4:JPD20 JFH4:JFH20 IVL4:IVL20 ILP4:ILP20 IBT4:IBT20 HRX4:HRX20 HIB4:HIB20 GYF4:GYF20 GOJ4:GOJ20 GEN4:GEN20 FUR4:FUR20 FKV4:FKV20 FAZ4:FAZ20 ERD4:ERD20 EHH4:EHH20 DXL4:DXL20 DNP4:DNP20 DDT4:DDT20 CTX4:CTX20 CKB4:CKB20 CAF4:CAF20 BQJ4:BQJ20 BGN4:BGN20 AWR4:AWR20 AMV4:AMV20 ACZ4:ACZ20 TD4:TD20 JH4:JH20" xr:uid="{00000000-0002-0000-0200-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JH65515:JH65545 TD65515:TD65545 ACZ65515:ACZ65545 AMV65515:AMV65545 AWR65515:AWR65545 BGN65515:BGN65545 BQJ65515:BQJ65545 CAF65515:CAF65545 CKB65515:CKB65545 CTX65515:CTX65545 DDT65515:DDT65545 DNP65515:DNP65545 DXL65515:DXL65545 EHH65515:EHH65545 ERD65515:ERD65545 FAZ65515:FAZ65545 FKV65515:FKV65545 FUR65515:FUR65545 GEN65515:GEN65545 GOJ65515:GOJ65545 GYF65515:GYF65545 HIB65515:HIB65545 HRX65515:HRX65545 IBT65515:IBT65545 ILP65515:ILP65545 IVL65515:IVL65545 JFH65515:JFH65545 JPD65515:JPD65545 JYZ65515:JYZ65545 KIV65515:KIV65545 KSR65515:KSR65545 LCN65515:LCN65545 LMJ65515:LMJ65545 LWF65515:LWF65545 MGB65515:MGB65545 MPX65515:MPX65545 MZT65515:MZT65545 NJP65515:NJP65545 NTL65515:NTL65545 ODH65515:ODH65545 OND65515:OND65545 OWZ65515:OWZ65545 PGV65515:PGV65545 PQR65515:PQR65545 QAN65515:QAN65545 QKJ65515:QKJ65545 QUF65515:QUF65545 REB65515:REB65545 RNX65515:RNX65545 RXT65515:RXT65545 SHP65515:SHP65545 SRL65515:SRL65545 TBH65515:TBH65545 TLD65515:TLD65545 TUZ65515:TUZ65545 UEV65515:UEV65545 UOR65515:UOR65545 UYN65515:UYN65545 VIJ65515:VIJ65545 VSF65515:VSF65545 WCB65515:WCB65545 WLX65515:WLX65545 WVT65515:WVT65545 JH131051:JH131081 TD131051:TD131081 ACZ131051:ACZ131081 AMV131051:AMV131081 AWR131051:AWR131081 BGN131051:BGN131081 BQJ131051:BQJ131081 CAF131051:CAF131081 CKB131051:CKB131081 CTX131051:CTX131081 DDT131051:DDT131081 DNP131051:DNP131081 DXL131051:DXL131081 EHH131051:EHH131081 ERD131051:ERD131081 FAZ131051:FAZ131081 FKV131051:FKV131081 FUR131051:FUR131081 GEN131051:GEN131081 GOJ131051:GOJ131081 GYF131051:GYF131081 HIB131051:HIB131081 HRX131051:HRX131081 IBT131051:IBT131081 ILP131051:ILP131081 IVL131051:IVL131081 JFH131051:JFH131081 JPD131051:JPD131081 JYZ131051:JYZ131081 KIV131051:KIV131081 KSR131051:KSR131081 LCN131051:LCN131081 LMJ131051:LMJ131081 LWF131051:LWF131081 MGB131051:MGB131081 MPX131051:MPX131081 MZT131051:MZT131081 NJP131051:NJP131081 NTL131051:NTL131081 ODH131051:ODH131081 OND131051:OND131081 OWZ131051:OWZ131081 PGV131051:PGV131081 PQR131051:PQR131081 QAN131051:QAN131081 QKJ131051:QKJ131081 QUF131051:QUF131081 REB131051:REB131081 RNX131051:RNX131081 RXT131051:RXT131081 SHP131051:SHP131081 SRL131051:SRL131081 TBH131051:TBH131081 TLD131051:TLD131081 TUZ131051:TUZ131081 UEV131051:UEV131081 UOR131051:UOR131081 UYN131051:UYN131081 VIJ131051:VIJ131081 VSF131051:VSF131081 WCB131051:WCB131081 WLX131051:WLX131081 WVT131051:WVT131081 JH196587:JH196617 TD196587:TD196617 ACZ196587:ACZ196617 AMV196587:AMV196617 AWR196587:AWR196617 BGN196587:BGN196617 BQJ196587:BQJ196617 CAF196587:CAF196617 CKB196587:CKB196617 CTX196587:CTX196617 DDT196587:DDT196617 DNP196587:DNP196617 DXL196587:DXL196617 EHH196587:EHH196617 ERD196587:ERD196617 FAZ196587:FAZ196617 FKV196587:FKV196617 FUR196587:FUR196617 GEN196587:GEN196617 GOJ196587:GOJ196617 GYF196587:GYF196617 HIB196587:HIB196617 HRX196587:HRX196617 IBT196587:IBT196617 ILP196587:ILP196617 IVL196587:IVL196617 JFH196587:JFH196617 JPD196587:JPD196617 JYZ196587:JYZ196617 KIV196587:KIV196617 KSR196587:KSR196617 LCN196587:LCN196617 LMJ196587:LMJ196617 LWF196587:LWF196617 MGB196587:MGB196617 MPX196587:MPX196617 MZT196587:MZT196617 NJP196587:NJP196617 NTL196587:NTL196617 ODH196587:ODH196617 OND196587:OND196617 OWZ196587:OWZ196617 PGV196587:PGV196617 PQR196587:PQR196617 QAN196587:QAN196617 QKJ196587:QKJ196617 QUF196587:QUF196617 REB196587:REB196617 RNX196587:RNX196617 RXT196587:RXT196617 SHP196587:SHP196617 SRL196587:SRL196617 TBH196587:TBH196617 TLD196587:TLD196617 TUZ196587:TUZ196617 UEV196587:UEV196617 UOR196587:UOR196617 UYN196587:UYN196617 VIJ196587:VIJ196617 VSF196587:VSF196617 WCB196587:WCB196617 WLX196587:WLX196617 WVT196587:WVT196617 JH262123:JH262153 TD262123:TD262153 ACZ262123:ACZ262153 AMV262123:AMV262153 AWR262123:AWR262153 BGN262123:BGN262153 BQJ262123:BQJ262153 CAF262123:CAF262153 CKB262123:CKB262153 CTX262123:CTX262153 DDT262123:DDT262153 DNP262123:DNP262153 DXL262123:DXL262153 EHH262123:EHH262153 ERD262123:ERD262153 FAZ262123:FAZ262153 FKV262123:FKV262153 FUR262123:FUR262153 GEN262123:GEN262153 GOJ262123:GOJ262153 GYF262123:GYF262153 HIB262123:HIB262153 HRX262123:HRX262153 IBT262123:IBT262153 ILP262123:ILP262153 IVL262123:IVL262153 JFH262123:JFH262153 JPD262123:JPD262153 JYZ262123:JYZ262153 KIV262123:KIV262153 KSR262123:KSR262153 LCN262123:LCN262153 LMJ262123:LMJ262153 LWF262123:LWF262153 MGB262123:MGB262153 MPX262123:MPX262153 MZT262123:MZT262153 NJP262123:NJP262153 NTL262123:NTL262153 ODH262123:ODH262153 OND262123:OND262153 OWZ262123:OWZ262153 PGV262123:PGV262153 PQR262123:PQR262153 QAN262123:QAN262153 QKJ262123:QKJ262153 QUF262123:QUF262153 REB262123:REB262153 RNX262123:RNX262153 RXT262123:RXT262153 SHP262123:SHP262153 SRL262123:SRL262153 TBH262123:TBH262153 TLD262123:TLD262153 TUZ262123:TUZ262153 UEV262123:UEV262153 UOR262123:UOR262153 UYN262123:UYN262153 VIJ262123:VIJ262153 VSF262123:VSF262153 WCB262123:WCB262153 WLX262123:WLX262153 WVT262123:WVT262153 JH327659:JH327689 TD327659:TD327689 ACZ327659:ACZ327689 AMV327659:AMV327689 AWR327659:AWR327689 BGN327659:BGN327689 BQJ327659:BQJ327689 CAF327659:CAF327689 CKB327659:CKB327689 CTX327659:CTX327689 DDT327659:DDT327689 DNP327659:DNP327689 DXL327659:DXL327689 EHH327659:EHH327689 ERD327659:ERD327689 FAZ327659:FAZ327689 FKV327659:FKV327689 FUR327659:FUR327689 GEN327659:GEN327689 GOJ327659:GOJ327689 GYF327659:GYF327689 HIB327659:HIB327689 HRX327659:HRX327689 IBT327659:IBT327689 ILP327659:ILP327689 IVL327659:IVL327689 JFH327659:JFH327689 JPD327659:JPD327689 JYZ327659:JYZ327689 KIV327659:KIV327689 KSR327659:KSR327689 LCN327659:LCN327689 LMJ327659:LMJ327689 LWF327659:LWF327689 MGB327659:MGB327689 MPX327659:MPX327689 MZT327659:MZT327689 NJP327659:NJP327689 NTL327659:NTL327689 ODH327659:ODH327689 OND327659:OND327689 OWZ327659:OWZ327689 PGV327659:PGV327689 PQR327659:PQR327689 QAN327659:QAN327689 QKJ327659:QKJ327689 QUF327659:QUF327689 REB327659:REB327689 RNX327659:RNX327689 RXT327659:RXT327689 SHP327659:SHP327689 SRL327659:SRL327689 TBH327659:TBH327689 TLD327659:TLD327689 TUZ327659:TUZ327689 UEV327659:UEV327689 UOR327659:UOR327689 UYN327659:UYN327689 VIJ327659:VIJ327689 VSF327659:VSF327689 WCB327659:WCB327689 WLX327659:WLX327689 WVT327659:WVT327689 JH393195:JH393225 TD393195:TD393225 ACZ393195:ACZ393225 AMV393195:AMV393225 AWR393195:AWR393225 BGN393195:BGN393225 BQJ393195:BQJ393225 CAF393195:CAF393225 CKB393195:CKB393225 CTX393195:CTX393225 DDT393195:DDT393225 DNP393195:DNP393225 DXL393195:DXL393225 EHH393195:EHH393225 ERD393195:ERD393225 FAZ393195:FAZ393225 FKV393195:FKV393225 FUR393195:FUR393225 GEN393195:GEN393225 GOJ393195:GOJ393225 GYF393195:GYF393225 HIB393195:HIB393225 HRX393195:HRX393225 IBT393195:IBT393225 ILP393195:ILP393225 IVL393195:IVL393225 JFH393195:JFH393225 JPD393195:JPD393225 JYZ393195:JYZ393225 KIV393195:KIV393225 KSR393195:KSR393225 LCN393195:LCN393225 LMJ393195:LMJ393225 LWF393195:LWF393225 MGB393195:MGB393225 MPX393195:MPX393225 MZT393195:MZT393225 NJP393195:NJP393225 NTL393195:NTL393225 ODH393195:ODH393225 OND393195:OND393225 OWZ393195:OWZ393225 PGV393195:PGV393225 PQR393195:PQR393225 QAN393195:QAN393225 QKJ393195:QKJ393225 QUF393195:QUF393225 REB393195:REB393225 RNX393195:RNX393225 RXT393195:RXT393225 SHP393195:SHP393225 SRL393195:SRL393225 TBH393195:TBH393225 TLD393195:TLD393225 TUZ393195:TUZ393225 UEV393195:UEV393225 UOR393195:UOR393225 UYN393195:UYN393225 VIJ393195:VIJ393225 VSF393195:VSF393225 WCB393195:WCB393225 WLX393195:WLX393225 WVT393195:WVT393225 JH458731:JH458761 TD458731:TD458761 ACZ458731:ACZ458761 AMV458731:AMV458761 AWR458731:AWR458761 BGN458731:BGN458761 BQJ458731:BQJ458761 CAF458731:CAF458761 CKB458731:CKB458761 CTX458731:CTX458761 DDT458731:DDT458761 DNP458731:DNP458761 DXL458731:DXL458761 EHH458731:EHH458761 ERD458731:ERD458761 FAZ458731:FAZ458761 FKV458731:FKV458761 FUR458731:FUR458761 GEN458731:GEN458761 GOJ458731:GOJ458761 GYF458731:GYF458761 HIB458731:HIB458761 HRX458731:HRX458761 IBT458731:IBT458761 ILP458731:ILP458761 IVL458731:IVL458761 JFH458731:JFH458761 JPD458731:JPD458761 JYZ458731:JYZ458761 KIV458731:KIV458761 KSR458731:KSR458761 LCN458731:LCN458761 LMJ458731:LMJ458761 LWF458731:LWF458761 MGB458731:MGB458761 MPX458731:MPX458761 MZT458731:MZT458761 NJP458731:NJP458761 NTL458731:NTL458761 ODH458731:ODH458761 OND458731:OND458761 OWZ458731:OWZ458761 PGV458731:PGV458761 PQR458731:PQR458761 QAN458731:QAN458761 QKJ458731:QKJ458761 QUF458731:QUF458761 REB458731:REB458761 RNX458731:RNX458761 RXT458731:RXT458761 SHP458731:SHP458761 SRL458731:SRL458761 TBH458731:TBH458761 TLD458731:TLD458761 TUZ458731:TUZ458761 UEV458731:UEV458761 UOR458731:UOR458761 UYN458731:UYN458761 VIJ458731:VIJ458761 VSF458731:VSF458761 WCB458731:WCB458761 WLX458731:WLX458761 WVT458731:WVT458761 JH524267:JH524297 TD524267:TD524297 ACZ524267:ACZ524297 AMV524267:AMV524297 AWR524267:AWR524297 BGN524267:BGN524297 BQJ524267:BQJ524297 CAF524267:CAF524297 CKB524267:CKB524297 CTX524267:CTX524297 DDT524267:DDT524297 DNP524267:DNP524297 DXL524267:DXL524297 EHH524267:EHH524297 ERD524267:ERD524297 FAZ524267:FAZ524297 FKV524267:FKV524297 FUR524267:FUR524297 GEN524267:GEN524297 GOJ524267:GOJ524297 GYF524267:GYF524297 HIB524267:HIB524297 HRX524267:HRX524297 IBT524267:IBT524297 ILP524267:ILP524297 IVL524267:IVL524297 JFH524267:JFH524297 JPD524267:JPD524297 JYZ524267:JYZ524297 KIV524267:KIV524297 KSR524267:KSR524297 LCN524267:LCN524297 LMJ524267:LMJ524297 LWF524267:LWF524297 MGB524267:MGB524297 MPX524267:MPX524297 MZT524267:MZT524297 NJP524267:NJP524297 NTL524267:NTL524297 ODH524267:ODH524297 OND524267:OND524297 OWZ524267:OWZ524297 PGV524267:PGV524297 PQR524267:PQR524297 QAN524267:QAN524297 QKJ524267:QKJ524297 QUF524267:QUF524297 REB524267:REB524297 RNX524267:RNX524297 RXT524267:RXT524297 SHP524267:SHP524297 SRL524267:SRL524297 TBH524267:TBH524297 TLD524267:TLD524297 TUZ524267:TUZ524297 UEV524267:UEV524297 UOR524267:UOR524297 UYN524267:UYN524297 VIJ524267:VIJ524297 VSF524267:VSF524297 WCB524267:WCB524297 WLX524267:WLX524297 WVT524267:WVT524297 JH589803:JH589833 TD589803:TD589833 ACZ589803:ACZ589833 AMV589803:AMV589833 AWR589803:AWR589833 BGN589803:BGN589833 BQJ589803:BQJ589833 CAF589803:CAF589833 CKB589803:CKB589833 CTX589803:CTX589833 DDT589803:DDT589833 DNP589803:DNP589833 DXL589803:DXL589833 EHH589803:EHH589833 ERD589803:ERD589833 FAZ589803:FAZ589833 FKV589803:FKV589833 FUR589803:FUR589833 GEN589803:GEN589833 GOJ589803:GOJ589833 GYF589803:GYF589833 HIB589803:HIB589833 HRX589803:HRX589833 IBT589803:IBT589833 ILP589803:ILP589833 IVL589803:IVL589833 JFH589803:JFH589833 JPD589803:JPD589833 JYZ589803:JYZ589833 KIV589803:KIV589833 KSR589803:KSR589833 LCN589803:LCN589833 LMJ589803:LMJ589833 LWF589803:LWF589833 MGB589803:MGB589833 MPX589803:MPX589833 MZT589803:MZT589833 NJP589803:NJP589833 NTL589803:NTL589833 ODH589803:ODH589833 OND589803:OND589833 OWZ589803:OWZ589833 PGV589803:PGV589833 PQR589803:PQR589833 QAN589803:QAN589833 QKJ589803:QKJ589833 QUF589803:QUF589833 REB589803:REB589833 RNX589803:RNX589833 RXT589803:RXT589833 SHP589803:SHP589833 SRL589803:SRL589833 TBH589803:TBH589833 TLD589803:TLD589833 TUZ589803:TUZ589833 UEV589803:UEV589833 UOR589803:UOR589833 UYN589803:UYN589833 VIJ589803:VIJ589833 VSF589803:VSF589833 WCB589803:WCB589833 WLX589803:WLX589833 WVT589803:WVT589833 JH655339:JH655369 TD655339:TD655369 ACZ655339:ACZ655369 AMV655339:AMV655369 AWR655339:AWR655369 BGN655339:BGN655369 BQJ655339:BQJ655369 CAF655339:CAF655369 CKB655339:CKB655369 CTX655339:CTX655369 DDT655339:DDT655369 DNP655339:DNP655369 DXL655339:DXL655369 EHH655339:EHH655369 ERD655339:ERD655369 FAZ655339:FAZ655369 FKV655339:FKV655369 FUR655339:FUR655369 GEN655339:GEN655369 GOJ655339:GOJ655369 GYF655339:GYF655369 HIB655339:HIB655369 HRX655339:HRX655369 IBT655339:IBT655369 ILP655339:ILP655369 IVL655339:IVL655369 JFH655339:JFH655369 JPD655339:JPD655369 JYZ655339:JYZ655369 KIV655339:KIV655369 KSR655339:KSR655369 LCN655339:LCN655369 LMJ655339:LMJ655369 LWF655339:LWF655369 MGB655339:MGB655369 MPX655339:MPX655369 MZT655339:MZT655369 NJP655339:NJP655369 NTL655339:NTL655369 ODH655339:ODH655369 OND655339:OND655369 OWZ655339:OWZ655369 PGV655339:PGV655369 PQR655339:PQR655369 QAN655339:QAN655369 QKJ655339:QKJ655369 QUF655339:QUF655369 REB655339:REB655369 RNX655339:RNX655369 RXT655339:RXT655369 SHP655339:SHP655369 SRL655339:SRL655369 TBH655339:TBH655369 TLD655339:TLD655369 TUZ655339:TUZ655369 UEV655339:UEV655369 UOR655339:UOR655369 UYN655339:UYN655369 VIJ655339:VIJ655369 VSF655339:VSF655369 WCB655339:WCB655369 WLX655339:WLX655369 WVT655339:WVT655369 JH720875:JH720905 TD720875:TD720905 ACZ720875:ACZ720905 AMV720875:AMV720905 AWR720875:AWR720905 BGN720875:BGN720905 BQJ720875:BQJ720905 CAF720875:CAF720905 CKB720875:CKB720905 CTX720875:CTX720905 DDT720875:DDT720905 DNP720875:DNP720905 DXL720875:DXL720905 EHH720875:EHH720905 ERD720875:ERD720905 FAZ720875:FAZ720905 FKV720875:FKV720905 FUR720875:FUR720905 GEN720875:GEN720905 GOJ720875:GOJ720905 GYF720875:GYF720905 HIB720875:HIB720905 HRX720875:HRX720905 IBT720875:IBT720905 ILP720875:ILP720905 IVL720875:IVL720905 JFH720875:JFH720905 JPD720875:JPD720905 JYZ720875:JYZ720905 KIV720875:KIV720905 KSR720875:KSR720905 LCN720875:LCN720905 LMJ720875:LMJ720905 LWF720875:LWF720905 MGB720875:MGB720905 MPX720875:MPX720905 MZT720875:MZT720905 NJP720875:NJP720905 NTL720875:NTL720905 ODH720875:ODH720905 OND720875:OND720905 OWZ720875:OWZ720905 PGV720875:PGV720905 PQR720875:PQR720905 QAN720875:QAN720905 QKJ720875:QKJ720905 QUF720875:QUF720905 REB720875:REB720905 RNX720875:RNX720905 RXT720875:RXT720905 SHP720875:SHP720905 SRL720875:SRL720905 TBH720875:TBH720905 TLD720875:TLD720905 TUZ720875:TUZ720905 UEV720875:UEV720905 UOR720875:UOR720905 UYN720875:UYN720905 VIJ720875:VIJ720905 VSF720875:VSF720905 WCB720875:WCB720905 WLX720875:WLX720905 WVT720875:WVT720905 JH786411:JH786441 TD786411:TD786441 ACZ786411:ACZ786441 AMV786411:AMV786441 AWR786411:AWR786441 BGN786411:BGN786441 BQJ786411:BQJ786441 CAF786411:CAF786441 CKB786411:CKB786441 CTX786411:CTX786441 DDT786411:DDT786441 DNP786411:DNP786441 DXL786411:DXL786441 EHH786411:EHH786441 ERD786411:ERD786441 FAZ786411:FAZ786441 FKV786411:FKV786441 FUR786411:FUR786441 GEN786411:GEN786441 GOJ786411:GOJ786441 GYF786411:GYF786441 HIB786411:HIB786441 HRX786411:HRX786441 IBT786411:IBT786441 ILP786411:ILP786441 IVL786411:IVL786441 JFH786411:JFH786441 JPD786411:JPD786441 JYZ786411:JYZ786441 KIV786411:KIV786441 KSR786411:KSR786441 LCN786411:LCN786441 LMJ786411:LMJ786441 LWF786411:LWF786441 MGB786411:MGB786441 MPX786411:MPX786441 MZT786411:MZT786441 NJP786411:NJP786441 NTL786411:NTL786441 ODH786411:ODH786441 OND786411:OND786441 OWZ786411:OWZ786441 PGV786411:PGV786441 PQR786411:PQR786441 QAN786411:QAN786441 QKJ786411:QKJ786441 QUF786411:QUF786441 REB786411:REB786441 RNX786411:RNX786441 RXT786411:RXT786441 SHP786411:SHP786441 SRL786411:SRL786441 TBH786411:TBH786441 TLD786411:TLD786441 TUZ786411:TUZ786441 UEV786411:UEV786441 UOR786411:UOR786441 UYN786411:UYN786441 VIJ786411:VIJ786441 VSF786411:VSF786441 WCB786411:WCB786441 WLX786411:WLX786441 WVT786411:WVT786441 JH851947:JH851977 TD851947:TD851977 ACZ851947:ACZ851977 AMV851947:AMV851977 AWR851947:AWR851977 BGN851947:BGN851977 BQJ851947:BQJ851977 CAF851947:CAF851977 CKB851947:CKB851977 CTX851947:CTX851977 DDT851947:DDT851977 DNP851947:DNP851977 DXL851947:DXL851977 EHH851947:EHH851977 ERD851947:ERD851977 FAZ851947:FAZ851977 FKV851947:FKV851977 FUR851947:FUR851977 GEN851947:GEN851977 GOJ851947:GOJ851977 GYF851947:GYF851977 HIB851947:HIB851977 HRX851947:HRX851977 IBT851947:IBT851977 ILP851947:ILP851977 IVL851947:IVL851977 JFH851947:JFH851977 JPD851947:JPD851977 JYZ851947:JYZ851977 KIV851947:KIV851977 KSR851947:KSR851977 LCN851947:LCN851977 LMJ851947:LMJ851977 LWF851947:LWF851977 MGB851947:MGB851977 MPX851947:MPX851977 MZT851947:MZT851977 NJP851947:NJP851977 NTL851947:NTL851977 ODH851947:ODH851977 OND851947:OND851977 OWZ851947:OWZ851977 PGV851947:PGV851977 PQR851947:PQR851977 QAN851947:QAN851977 QKJ851947:QKJ851977 QUF851947:QUF851977 REB851947:REB851977 RNX851947:RNX851977 RXT851947:RXT851977 SHP851947:SHP851977 SRL851947:SRL851977 TBH851947:TBH851977 TLD851947:TLD851977 TUZ851947:TUZ851977 UEV851947:UEV851977 UOR851947:UOR851977 UYN851947:UYN851977 VIJ851947:VIJ851977 VSF851947:VSF851977 WCB851947:WCB851977 WLX851947:WLX851977 WVT851947:WVT851977 JH917483:JH917513 TD917483:TD917513 ACZ917483:ACZ917513 AMV917483:AMV917513 AWR917483:AWR917513 BGN917483:BGN917513 BQJ917483:BQJ917513 CAF917483:CAF917513 CKB917483:CKB917513 CTX917483:CTX917513 DDT917483:DDT917513 DNP917483:DNP917513 DXL917483:DXL917513 EHH917483:EHH917513 ERD917483:ERD917513 FAZ917483:FAZ917513 FKV917483:FKV917513 FUR917483:FUR917513 GEN917483:GEN917513 GOJ917483:GOJ917513 GYF917483:GYF917513 HIB917483:HIB917513 HRX917483:HRX917513 IBT917483:IBT917513 ILP917483:ILP917513 IVL917483:IVL917513 JFH917483:JFH917513 JPD917483:JPD917513 JYZ917483:JYZ917513 KIV917483:KIV917513 KSR917483:KSR917513 LCN917483:LCN917513 LMJ917483:LMJ917513 LWF917483:LWF917513 MGB917483:MGB917513 MPX917483:MPX917513 MZT917483:MZT917513 NJP917483:NJP917513 NTL917483:NTL917513 ODH917483:ODH917513 OND917483:OND917513 OWZ917483:OWZ917513 PGV917483:PGV917513 PQR917483:PQR917513 QAN917483:QAN917513 QKJ917483:QKJ917513 QUF917483:QUF917513 REB917483:REB917513 RNX917483:RNX917513 RXT917483:RXT917513 SHP917483:SHP917513 SRL917483:SRL917513 TBH917483:TBH917513 TLD917483:TLD917513 TUZ917483:TUZ917513 UEV917483:UEV917513 UOR917483:UOR917513 UYN917483:UYN917513 VIJ917483:VIJ917513 VSF917483:VSF917513 WCB917483:WCB917513 WLX917483:WLX917513 WVT917483:WVT917513 JH983019:JH983049 TD983019:TD983049 ACZ983019:ACZ983049 AMV983019:AMV983049 AWR983019:AWR983049 BGN983019:BGN983049 BQJ983019:BQJ983049 CAF983019:CAF983049 CKB983019:CKB983049 CTX983019:CTX983049 DDT983019:DDT983049 DNP983019:DNP983049 DXL983019:DXL983049 EHH983019:EHH983049 ERD983019:ERD983049 FAZ983019:FAZ983049 FKV983019:FKV983049 FUR983019:FUR983049 GEN983019:GEN983049 GOJ983019:GOJ983049 GYF983019:GYF983049 HIB983019:HIB983049 HRX983019:HRX983049 IBT983019:IBT983049 ILP983019:ILP983049 IVL983019:IVL983049 JFH983019:JFH983049 JPD983019:JPD983049 JYZ983019:JYZ983049 KIV983019:KIV983049 KSR983019:KSR983049 LCN983019:LCN983049 LMJ983019:LMJ983049 LWF983019:LWF983049 MGB983019:MGB983049 MPX983019:MPX983049 MZT983019:MZT983049 NJP983019:NJP983049 NTL983019:NTL983049 ODH983019:ODH983049 OND983019:OND983049 OWZ983019:OWZ983049 PGV983019:PGV983049 PQR983019:PQR983049 QAN983019:QAN983049 QKJ983019:QKJ983049 QUF983019:QUF983049 REB983019:REB983049 RNX983019:RNX983049 RXT983019:RXT983049 SHP983019:SHP983049 SRL983019:SRL983049 TBH983019:TBH983049 TLD983019:TLD983049 TUZ983019:TUZ983049 UEV983019:UEV983049 UOR983019:UOR983049 UYN983019:UYN983049 VIJ983019:VIJ983049 VSF983019:VSF983049 WCB983019:WCB983049 WLX983019:WLX983049 WVT983019:WVT983049 L983019:L983049 L65515:L65545 L131051:L131081 L196587:L196617 L262123:L262153 L327659:L327689 L393195:L393225 L458731:L458761 L524267:L524297 L589803:L589833 L655339:L655369 L720875:L720905 L786411:L786441 L851947:L851977 L917483:L917513 JH4:JH20 TD4:TD20 ACZ4:ACZ20 AMV4:AMV20 AWR4:AWR20 BGN4:BGN20 BQJ4:BQJ20 CAF4:CAF20 CKB4:CKB20 CTX4:CTX20 DDT4:DDT20 DNP4:DNP20 DXL4:DXL20 EHH4:EHH20 ERD4:ERD20 FAZ4:FAZ20 FKV4:FKV20 FUR4:FUR20 GEN4:GEN20 GOJ4:GOJ20 GYF4:GYF20 HIB4:HIB20 HRX4:HRX20 IBT4:IBT20 ILP4:ILP20 IVL4:IVL20 JFH4:JFH20 JPD4:JPD20 JYZ4:JYZ20 KIV4:KIV20 KSR4:KSR20 LCN4:LCN20 LMJ4:LMJ20 LWF4:LWF20 MGB4:MGB20 MPX4:MPX20 MZT4:MZT20 NJP4:NJP20 NTL4:NTL20 ODH4:ODH20 OND4:OND20 OWZ4:OWZ20 PGV4:PGV20 PQR4:PQR20 QAN4:QAN20 QKJ4:QKJ20 QUF4:QUF20 REB4:REB20 RNX4:RNX20 RXT4:RXT20 SHP4:SHP20 SRL4:SRL20 TBH4:TBH20 TLD4:TLD20 TUZ4:TUZ20 UEV4:UEV20 UOR4:UOR20 UYN4:UYN20 VIJ4:VIJ20 VSF4:VSF20 WCB4:WCB20 WLX4:WLX20 WVT4:WVT20" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>"Diurna, Nocturna, Rotativa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVS983019:WVS983049 Q65515:Q65545 JG65515:JG65545 TC65515:TC65545 ACY65515:ACY65545 AMU65515:AMU65545 AWQ65515:AWQ65545 BGM65515:BGM65545 BQI65515:BQI65545 CAE65515:CAE65545 CKA65515:CKA65545 CTW65515:CTW65545 DDS65515:DDS65545 DNO65515:DNO65545 DXK65515:DXK65545 EHG65515:EHG65545 ERC65515:ERC65545 FAY65515:FAY65545 FKU65515:FKU65545 FUQ65515:FUQ65545 GEM65515:GEM65545 GOI65515:GOI65545 GYE65515:GYE65545 HIA65515:HIA65545 HRW65515:HRW65545 IBS65515:IBS65545 ILO65515:ILO65545 IVK65515:IVK65545 JFG65515:JFG65545 JPC65515:JPC65545 JYY65515:JYY65545 KIU65515:KIU65545 KSQ65515:KSQ65545 LCM65515:LCM65545 LMI65515:LMI65545 LWE65515:LWE65545 MGA65515:MGA65545 MPW65515:MPW65545 MZS65515:MZS65545 NJO65515:NJO65545 NTK65515:NTK65545 ODG65515:ODG65545 ONC65515:ONC65545 OWY65515:OWY65545 PGU65515:PGU65545 PQQ65515:PQQ65545 QAM65515:QAM65545 QKI65515:QKI65545 QUE65515:QUE65545 REA65515:REA65545 RNW65515:RNW65545 RXS65515:RXS65545 SHO65515:SHO65545 SRK65515:SRK65545 TBG65515:TBG65545 TLC65515:TLC65545 TUY65515:TUY65545 UEU65515:UEU65545 UOQ65515:UOQ65545 UYM65515:UYM65545 VII65515:VII65545 VSE65515:VSE65545 WCA65515:WCA65545 WLW65515:WLW65545 WVS65515:WVS65545 Q131051:Q131081 JG131051:JG131081 TC131051:TC131081 ACY131051:ACY131081 AMU131051:AMU131081 AWQ131051:AWQ131081 BGM131051:BGM131081 BQI131051:BQI131081 CAE131051:CAE131081 CKA131051:CKA131081 CTW131051:CTW131081 DDS131051:DDS131081 DNO131051:DNO131081 DXK131051:DXK131081 EHG131051:EHG131081 ERC131051:ERC131081 FAY131051:FAY131081 FKU131051:FKU131081 FUQ131051:FUQ131081 GEM131051:GEM131081 GOI131051:GOI131081 GYE131051:GYE131081 HIA131051:HIA131081 HRW131051:HRW131081 IBS131051:IBS131081 ILO131051:ILO131081 IVK131051:IVK131081 JFG131051:JFG131081 JPC131051:JPC131081 JYY131051:JYY131081 KIU131051:KIU131081 KSQ131051:KSQ131081 LCM131051:LCM131081 LMI131051:LMI131081 LWE131051:LWE131081 MGA131051:MGA131081 MPW131051:MPW131081 MZS131051:MZS131081 NJO131051:NJO131081 NTK131051:NTK131081 ODG131051:ODG131081 ONC131051:ONC131081 OWY131051:OWY131081 PGU131051:PGU131081 PQQ131051:PQQ131081 QAM131051:QAM131081 QKI131051:QKI131081 QUE131051:QUE131081 REA131051:REA131081 RNW131051:RNW131081 RXS131051:RXS131081 SHO131051:SHO131081 SRK131051:SRK131081 TBG131051:TBG131081 TLC131051:TLC131081 TUY131051:TUY131081 UEU131051:UEU131081 UOQ131051:UOQ131081 UYM131051:UYM131081 VII131051:VII131081 VSE131051:VSE131081 WCA131051:WCA131081 WLW131051:WLW131081 WVS131051:WVS131081 Q196587:Q196617 JG196587:JG196617 TC196587:TC196617 ACY196587:ACY196617 AMU196587:AMU196617 AWQ196587:AWQ196617 BGM196587:BGM196617 BQI196587:BQI196617 CAE196587:CAE196617 CKA196587:CKA196617 CTW196587:CTW196617 DDS196587:DDS196617 DNO196587:DNO196617 DXK196587:DXK196617 EHG196587:EHG196617 ERC196587:ERC196617 FAY196587:FAY196617 FKU196587:FKU196617 FUQ196587:FUQ196617 GEM196587:GEM196617 GOI196587:GOI196617 GYE196587:GYE196617 HIA196587:HIA196617 HRW196587:HRW196617 IBS196587:IBS196617 ILO196587:ILO196617 IVK196587:IVK196617 JFG196587:JFG196617 JPC196587:JPC196617 JYY196587:JYY196617 KIU196587:KIU196617 KSQ196587:KSQ196617 LCM196587:LCM196617 LMI196587:LMI196617 LWE196587:LWE196617 MGA196587:MGA196617 MPW196587:MPW196617 MZS196587:MZS196617 NJO196587:NJO196617 NTK196587:NTK196617 ODG196587:ODG196617 ONC196587:ONC196617 OWY196587:OWY196617 PGU196587:PGU196617 PQQ196587:PQQ196617 QAM196587:QAM196617 QKI196587:QKI196617 QUE196587:QUE196617 REA196587:REA196617 RNW196587:RNW196617 RXS196587:RXS196617 SHO196587:SHO196617 SRK196587:SRK196617 TBG196587:TBG196617 TLC196587:TLC196617 TUY196587:TUY196617 UEU196587:UEU196617 UOQ196587:UOQ196617 UYM196587:UYM196617 VII196587:VII196617 VSE196587:VSE196617 WCA196587:WCA196617 WLW196587:WLW196617 WVS196587:WVS196617 Q262123:Q262153 JG262123:JG262153 TC262123:TC262153 ACY262123:ACY262153 AMU262123:AMU262153 AWQ262123:AWQ262153 BGM262123:BGM262153 BQI262123:BQI262153 CAE262123:CAE262153 CKA262123:CKA262153 CTW262123:CTW262153 DDS262123:DDS262153 DNO262123:DNO262153 DXK262123:DXK262153 EHG262123:EHG262153 ERC262123:ERC262153 FAY262123:FAY262153 FKU262123:FKU262153 FUQ262123:FUQ262153 GEM262123:GEM262153 GOI262123:GOI262153 GYE262123:GYE262153 HIA262123:HIA262153 HRW262123:HRW262153 IBS262123:IBS262153 ILO262123:ILO262153 IVK262123:IVK262153 JFG262123:JFG262153 JPC262123:JPC262153 JYY262123:JYY262153 KIU262123:KIU262153 KSQ262123:KSQ262153 LCM262123:LCM262153 LMI262123:LMI262153 LWE262123:LWE262153 MGA262123:MGA262153 MPW262123:MPW262153 MZS262123:MZS262153 NJO262123:NJO262153 NTK262123:NTK262153 ODG262123:ODG262153 ONC262123:ONC262153 OWY262123:OWY262153 PGU262123:PGU262153 PQQ262123:PQQ262153 QAM262123:QAM262153 QKI262123:QKI262153 QUE262123:QUE262153 REA262123:REA262153 RNW262123:RNW262153 RXS262123:RXS262153 SHO262123:SHO262153 SRK262123:SRK262153 TBG262123:TBG262153 TLC262123:TLC262153 TUY262123:TUY262153 UEU262123:UEU262153 UOQ262123:UOQ262153 UYM262123:UYM262153 VII262123:VII262153 VSE262123:VSE262153 WCA262123:WCA262153 WLW262123:WLW262153 WVS262123:WVS262153 Q327659:Q327689 JG327659:JG327689 TC327659:TC327689 ACY327659:ACY327689 AMU327659:AMU327689 AWQ327659:AWQ327689 BGM327659:BGM327689 BQI327659:BQI327689 CAE327659:CAE327689 CKA327659:CKA327689 CTW327659:CTW327689 DDS327659:DDS327689 DNO327659:DNO327689 DXK327659:DXK327689 EHG327659:EHG327689 ERC327659:ERC327689 FAY327659:FAY327689 FKU327659:FKU327689 FUQ327659:FUQ327689 GEM327659:GEM327689 GOI327659:GOI327689 GYE327659:GYE327689 HIA327659:HIA327689 HRW327659:HRW327689 IBS327659:IBS327689 ILO327659:ILO327689 IVK327659:IVK327689 JFG327659:JFG327689 JPC327659:JPC327689 JYY327659:JYY327689 KIU327659:KIU327689 KSQ327659:KSQ327689 LCM327659:LCM327689 LMI327659:LMI327689 LWE327659:LWE327689 MGA327659:MGA327689 MPW327659:MPW327689 MZS327659:MZS327689 NJO327659:NJO327689 NTK327659:NTK327689 ODG327659:ODG327689 ONC327659:ONC327689 OWY327659:OWY327689 PGU327659:PGU327689 PQQ327659:PQQ327689 QAM327659:QAM327689 QKI327659:QKI327689 QUE327659:QUE327689 REA327659:REA327689 RNW327659:RNW327689 RXS327659:RXS327689 SHO327659:SHO327689 SRK327659:SRK327689 TBG327659:TBG327689 TLC327659:TLC327689 TUY327659:TUY327689 UEU327659:UEU327689 UOQ327659:UOQ327689 UYM327659:UYM327689 VII327659:VII327689 VSE327659:VSE327689 WCA327659:WCA327689 WLW327659:WLW327689 WVS327659:WVS327689 Q393195:Q393225 JG393195:JG393225 TC393195:TC393225 ACY393195:ACY393225 AMU393195:AMU393225 AWQ393195:AWQ393225 BGM393195:BGM393225 BQI393195:BQI393225 CAE393195:CAE393225 CKA393195:CKA393225 CTW393195:CTW393225 DDS393195:DDS393225 DNO393195:DNO393225 DXK393195:DXK393225 EHG393195:EHG393225 ERC393195:ERC393225 FAY393195:FAY393225 FKU393195:FKU393225 FUQ393195:FUQ393225 GEM393195:GEM393225 GOI393195:GOI393225 GYE393195:GYE393225 HIA393195:HIA393225 HRW393195:HRW393225 IBS393195:IBS393225 ILO393195:ILO393225 IVK393195:IVK393225 JFG393195:JFG393225 JPC393195:JPC393225 JYY393195:JYY393225 KIU393195:KIU393225 KSQ393195:KSQ393225 LCM393195:LCM393225 LMI393195:LMI393225 LWE393195:LWE393225 MGA393195:MGA393225 MPW393195:MPW393225 MZS393195:MZS393225 NJO393195:NJO393225 NTK393195:NTK393225 ODG393195:ODG393225 ONC393195:ONC393225 OWY393195:OWY393225 PGU393195:PGU393225 PQQ393195:PQQ393225 QAM393195:QAM393225 QKI393195:QKI393225 QUE393195:QUE393225 REA393195:REA393225 RNW393195:RNW393225 RXS393195:RXS393225 SHO393195:SHO393225 SRK393195:SRK393225 TBG393195:TBG393225 TLC393195:TLC393225 TUY393195:TUY393225 UEU393195:UEU393225 UOQ393195:UOQ393225 UYM393195:UYM393225 VII393195:VII393225 VSE393195:VSE393225 WCA393195:WCA393225 WLW393195:WLW393225 WVS393195:WVS393225 Q458731:Q458761 JG458731:JG458761 TC458731:TC458761 ACY458731:ACY458761 AMU458731:AMU458761 AWQ458731:AWQ458761 BGM458731:BGM458761 BQI458731:BQI458761 CAE458731:CAE458761 CKA458731:CKA458761 CTW458731:CTW458761 DDS458731:DDS458761 DNO458731:DNO458761 DXK458731:DXK458761 EHG458731:EHG458761 ERC458731:ERC458761 FAY458731:FAY458761 FKU458731:FKU458761 FUQ458731:FUQ458761 GEM458731:GEM458761 GOI458731:GOI458761 GYE458731:GYE458761 HIA458731:HIA458761 HRW458731:HRW458761 IBS458731:IBS458761 ILO458731:ILO458761 IVK458731:IVK458761 JFG458731:JFG458761 JPC458731:JPC458761 JYY458731:JYY458761 KIU458731:KIU458761 KSQ458731:KSQ458761 LCM458731:LCM458761 LMI458731:LMI458761 LWE458731:LWE458761 MGA458731:MGA458761 MPW458731:MPW458761 MZS458731:MZS458761 NJO458731:NJO458761 NTK458731:NTK458761 ODG458731:ODG458761 ONC458731:ONC458761 OWY458731:OWY458761 PGU458731:PGU458761 PQQ458731:PQQ458761 QAM458731:QAM458761 QKI458731:QKI458761 QUE458731:QUE458761 REA458731:REA458761 RNW458731:RNW458761 RXS458731:RXS458761 SHO458731:SHO458761 SRK458731:SRK458761 TBG458731:TBG458761 TLC458731:TLC458761 TUY458731:TUY458761 UEU458731:UEU458761 UOQ458731:UOQ458761 UYM458731:UYM458761 VII458731:VII458761 VSE458731:VSE458761 WCA458731:WCA458761 WLW458731:WLW458761 WVS458731:WVS458761 Q524267:Q524297 JG524267:JG524297 TC524267:TC524297 ACY524267:ACY524297 AMU524267:AMU524297 AWQ524267:AWQ524297 BGM524267:BGM524297 BQI524267:BQI524297 CAE524267:CAE524297 CKA524267:CKA524297 CTW524267:CTW524297 DDS524267:DDS524297 DNO524267:DNO524297 DXK524267:DXK524297 EHG524267:EHG524297 ERC524267:ERC524297 FAY524267:FAY524297 FKU524267:FKU524297 FUQ524267:FUQ524297 GEM524267:GEM524297 GOI524267:GOI524297 GYE524267:GYE524297 HIA524267:HIA524297 HRW524267:HRW524297 IBS524267:IBS524297 ILO524267:ILO524297 IVK524267:IVK524297 JFG524267:JFG524297 JPC524267:JPC524297 JYY524267:JYY524297 KIU524267:KIU524297 KSQ524267:KSQ524297 LCM524267:LCM524297 LMI524267:LMI524297 LWE524267:LWE524297 MGA524267:MGA524297 MPW524267:MPW524297 MZS524267:MZS524297 NJO524267:NJO524297 NTK524267:NTK524297 ODG524267:ODG524297 ONC524267:ONC524297 OWY524267:OWY524297 PGU524267:PGU524297 PQQ524267:PQQ524297 QAM524267:QAM524297 QKI524267:QKI524297 QUE524267:QUE524297 REA524267:REA524297 RNW524267:RNW524297 RXS524267:RXS524297 SHO524267:SHO524297 SRK524267:SRK524297 TBG524267:TBG524297 TLC524267:TLC524297 TUY524267:TUY524297 UEU524267:UEU524297 UOQ524267:UOQ524297 UYM524267:UYM524297 VII524267:VII524297 VSE524267:VSE524297 WCA524267:WCA524297 WLW524267:WLW524297 WVS524267:WVS524297 Q589803:Q589833 JG589803:JG589833 TC589803:TC589833 ACY589803:ACY589833 AMU589803:AMU589833 AWQ589803:AWQ589833 BGM589803:BGM589833 BQI589803:BQI589833 CAE589803:CAE589833 CKA589803:CKA589833 CTW589803:CTW589833 DDS589803:DDS589833 DNO589803:DNO589833 DXK589803:DXK589833 EHG589803:EHG589833 ERC589803:ERC589833 FAY589803:FAY589833 FKU589803:FKU589833 FUQ589803:FUQ589833 GEM589803:GEM589833 GOI589803:GOI589833 GYE589803:GYE589833 HIA589803:HIA589833 HRW589803:HRW589833 IBS589803:IBS589833 ILO589803:ILO589833 IVK589803:IVK589833 JFG589803:JFG589833 JPC589803:JPC589833 JYY589803:JYY589833 KIU589803:KIU589833 KSQ589803:KSQ589833 LCM589803:LCM589833 LMI589803:LMI589833 LWE589803:LWE589833 MGA589803:MGA589833 MPW589803:MPW589833 MZS589803:MZS589833 NJO589803:NJO589833 NTK589803:NTK589833 ODG589803:ODG589833 ONC589803:ONC589833 OWY589803:OWY589833 PGU589803:PGU589833 PQQ589803:PQQ589833 QAM589803:QAM589833 QKI589803:QKI589833 QUE589803:QUE589833 REA589803:REA589833 RNW589803:RNW589833 RXS589803:RXS589833 SHO589803:SHO589833 SRK589803:SRK589833 TBG589803:TBG589833 TLC589803:TLC589833 TUY589803:TUY589833 UEU589803:UEU589833 UOQ589803:UOQ589833 UYM589803:UYM589833 VII589803:VII589833 VSE589803:VSE589833 WCA589803:WCA589833 WLW589803:WLW589833 WVS589803:WVS589833 Q655339:Q655369 JG655339:JG655369 TC655339:TC655369 ACY655339:ACY655369 AMU655339:AMU655369 AWQ655339:AWQ655369 BGM655339:BGM655369 BQI655339:BQI655369 CAE655339:CAE655369 CKA655339:CKA655369 CTW655339:CTW655369 DDS655339:DDS655369 DNO655339:DNO655369 DXK655339:DXK655369 EHG655339:EHG655369 ERC655339:ERC655369 FAY655339:FAY655369 FKU655339:FKU655369 FUQ655339:FUQ655369 GEM655339:GEM655369 GOI655339:GOI655369 GYE655339:GYE655369 HIA655339:HIA655369 HRW655339:HRW655369 IBS655339:IBS655369 ILO655339:ILO655369 IVK655339:IVK655369 JFG655339:JFG655369 JPC655339:JPC655369 JYY655339:JYY655369 KIU655339:KIU655369 KSQ655339:KSQ655369 LCM655339:LCM655369 LMI655339:LMI655369 LWE655339:LWE655369 MGA655339:MGA655369 MPW655339:MPW655369 MZS655339:MZS655369 NJO655339:NJO655369 NTK655339:NTK655369 ODG655339:ODG655369 ONC655339:ONC655369 OWY655339:OWY655369 PGU655339:PGU655369 PQQ655339:PQQ655369 QAM655339:QAM655369 QKI655339:QKI655369 QUE655339:QUE655369 REA655339:REA655369 RNW655339:RNW655369 RXS655339:RXS655369 SHO655339:SHO655369 SRK655339:SRK655369 TBG655339:TBG655369 TLC655339:TLC655369 TUY655339:TUY655369 UEU655339:UEU655369 UOQ655339:UOQ655369 UYM655339:UYM655369 VII655339:VII655369 VSE655339:VSE655369 WCA655339:WCA655369 WLW655339:WLW655369 WVS655339:WVS655369 Q720875:Q720905 JG720875:JG720905 TC720875:TC720905 ACY720875:ACY720905 AMU720875:AMU720905 AWQ720875:AWQ720905 BGM720875:BGM720905 BQI720875:BQI720905 CAE720875:CAE720905 CKA720875:CKA720905 CTW720875:CTW720905 DDS720875:DDS720905 DNO720875:DNO720905 DXK720875:DXK720905 EHG720875:EHG720905 ERC720875:ERC720905 FAY720875:FAY720905 FKU720875:FKU720905 FUQ720875:FUQ720905 GEM720875:GEM720905 GOI720875:GOI720905 GYE720875:GYE720905 HIA720875:HIA720905 HRW720875:HRW720905 IBS720875:IBS720905 ILO720875:ILO720905 IVK720875:IVK720905 JFG720875:JFG720905 JPC720875:JPC720905 JYY720875:JYY720905 KIU720875:KIU720905 KSQ720875:KSQ720905 LCM720875:LCM720905 LMI720875:LMI720905 LWE720875:LWE720905 MGA720875:MGA720905 MPW720875:MPW720905 MZS720875:MZS720905 NJO720875:NJO720905 NTK720875:NTK720905 ODG720875:ODG720905 ONC720875:ONC720905 OWY720875:OWY720905 PGU720875:PGU720905 PQQ720875:PQQ720905 QAM720875:QAM720905 QKI720875:QKI720905 QUE720875:QUE720905 REA720875:REA720905 RNW720875:RNW720905 RXS720875:RXS720905 SHO720875:SHO720905 SRK720875:SRK720905 TBG720875:TBG720905 TLC720875:TLC720905 TUY720875:TUY720905 UEU720875:UEU720905 UOQ720875:UOQ720905 UYM720875:UYM720905 VII720875:VII720905 VSE720875:VSE720905 WCA720875:WCA720905 WLW720875:WLW720905 WVS720875:WVS720905 Q786411:Q786441 JG786411:JG786441 TC786411:TC786441 ACY786411:ACY786441 AMU786411:AMU786441 AWQ786411:AWQ786441 BGM786411:BGM786441 BQI786411:BQI786441 CAE786411:CAE786441 CKA786411:CKA786441 CTW786411:CTW786441 DDS786411:DDS786441 DNO786411:DNO786441 DXK786411:DXK786441 EHG786411:EHG786441 ERC786411:ERC786441 FAY786411:FAY786441 FKU786411:FKU786441 FUQ786411:FUQ786441 GEM786411:GEM786441 GOI786411:GOI786441 GYE786411:GYE786441 HIA786411:HIA786441 HRW786411:HRW786441 IBS786411:IBS786441 ILO786411:ILO786441 IVK786411:IVK786441 JFG786411:JFG786441 JPC786411:JPC786441 JYY786411:JYY786441 KIU786411:KIU786441 KSQ786411:KSQ786441 LCM786411:LCM786441 LMI786411:LMI786441 LWE786411:LWE786441 MGA786411:MGA786441 MPW786411:MPW786441 MZS786411:MZS786441 NJO786411:NJO786441 NTK786411:NTK786441 ODG786411:ODG786441 ONC786411:ONC786441 OWY786411:OWY786441 PGU786411:PGU786441 PQQ786411:PQQ786441 QAM786411:QAM786441 QKI786411:QKI786441 QUE786411:QUE786441 REA786411:REA786441 RNW786411:RNW786441 RXS786411:RXS786441 SHO786411:SHO786441 SRK786411:SRK786441 TBG786411:TBG786441 TLC786411:TLC786441 TUY786411:TUY786441 UEU786411:UEU786441 UOQ786411:UOQ786441 UYM786411:UYM786441 VII786411:VII786441 VSE786411:VSE786441 WCA786411:WCA786441 WLW786411:WLW786441 WVS786411:WVS786441 Q851947:Q851977 JG851947:JG851977 TC851947:TC851977 ACY851947:ACY851977 AMU851947:AMU851977 AWQ851947:AWQ851977 BGM851947:BGM851977 BQI851947:BQI851977 CAE851947:CAE851977 CKA851947:CKA851977 CTW851947:CTW851977 DDS851947:DDS851977 DNO851947:DNO851977 DXK851947:DXK851977 EHG851947:EHG851977 ERC851947:ERC851977 FAY851947:FAY851977 FKU851947:FKU851977 FUQ851947:FUQ851977 GEM851947:GEM851977 GOI851947:GOI851977 GYE851947:GYE851977 HIA851947:HIA851977 HRW851947:HRW851977 IBS851947:IBS851977 ILO851947:ILO851977 IVK851947:IVK851977 JFG851947:JFG851977 JPC851947:JPC851977 JYY851947:JYY851977 KIU851947:KIU851977 KSQ851947:KSQ851977 LCM851947:LCM851977 LMI851947:LMI851977 LWE851947:LWE851977 MGA851947:MGA851977 MPW851947:MPW851977 MZS851947:MZS851977 NJO851947:NJO851977 NTK851947:NTK851977 ODG851947:ODG851977 ONC851947:ONC851977 OWY851947:OWY851977 PGU851947:PGU851977 PQQ851947:PQQ851977 QAM851947:QAM851977 QKI851947:QKI851977 QUE851947:QUE851977 REA851947:REA851977 RNW851947:RNW851977 RXS851947:RXS851977 SHO851947:SHO851977 SRK851947:SRK851977 TBG851947:TBG851977 TLC851947:TLC851977 TUY851947:TUY851977 UEU851947:UEU851977 UOQ851947:UOQ851977 UYM851947:UYM851977 VII851947:VII851977 VSE851947:VSE851977 WCA851947:WCA851977 WLW851947:WLW851977 WVS851947:WVS851977 Q917483:Q917513 JG917483:JG917513 TC917483:TC917513 ACY917483:ACY917513 AMU917483:AMU917513 AWQ917483:AWQ917513 BGM917483:BGM917513 BQI917483:BQI917513 CAE917483:CAE917513 CKA917483:CKA917513 CTW917483:CTW917513 DDS917483:DDS917513 DNO917483:DNO917513 DXK917483:DXK917513 EHG917483:EHG917513 ERC917483:ERC917513 FAY917483:FAY917513 FKU917483:FKU917513 FUQ917483:FUQ917513 GEM917483:GEM917513 GOI917483:GOI917513 GYE917483:GYE917513 HIA917483:HIA917513 HRW917483:HRW917513 IBS917483:IBS917513 ILO917483:ILO917513 IVK917483:IVK917513 JFG917483:JFG917513 JPC917483:JPC917513 JYY917483:JYY917513 KIU917483:KIU917513 KSQ917483:KSQ917513 LCM917483:LCM917513 LMI917483:LMI917513 LWE917483:LWE917513 MGA917483:MGA917513 MPW917483:MPW917513 MZS917483:MZS917513 NJO917483:NJO917513 NTK917483:NTK917513 ODG917483:ODG917513 ONC917483:ONC917513 OWY917483:OWY917513 PGU917483:PGU917513 PQQ917483:PQQ917513 QAM917483:QAM917513 QKI917483:QKI917513 QUE917483:QUE917513 REA917483:REA917513 RNW917483:RNW917513 RXS917483:RXS917513 SHO917483:SHO917513 SRK917483:SRK917513 TBG917483:TBG917513 TLC917483:TLC917513 TUY917483:TUY917513 UEU917483:UEU917513 UOQ917483:UOQ917513 UYM917483:UYM917513 VII917483:VII917513 VSE917483:VSE917513 WCA917483:WCA917513 WLW917483:WLW917513 WVS917483:WVS917513 Q983019:Q983049 JG983019:JG983049 TC983019:TC983049 ACY983019:ACY983049 AMU983019:AMU983049 AWQ983019:AWQ983049 BGM983019:BGM983049 BQI983019:BQI983049 CAE983019:CAE983049 CKA983019:CKA983049 CTW983019:CTW983049 DDS983019:DDS983049 DNO983019:DNO983049 DXK983019:DXK983049 EHG983019:EHG983049 ERC983019:ERC983049 FAY983019:FAY983049 FKU983019:FKU983049 FUQ983019:FUQ983049 GEM983019:GEM983049 GOI983019:GOI983049 GYE983019:GYE983049 HIA983019:HIA983049 HRW983019:HRW983049 IBS983019:IBS983049 ILO983019:ILO983049 IVK983019:IVK983049 JFG983019:JFG983049 JPC983019:JPC983049 JYY983019:JYY983049 KIU983019:KIU983049 KSQ983019:KSQ983049 LCM983019:LCM983049 LMI983019:LMI983049 LWE983019:LWE983049 MGA983019:MGA983049 MPW983019:MPW983049 MZS983019:MZS983049 NJO983019:NJO983049 NTK983019:NTK983049 ODG983019:ODG983049 ONC983019:ONC983049 OWY983019:OWY983049 PGU983019:PGU983049 PQQ983019:PQQ983049 QAM983019:QAM983049 QKI983019:QKI983049 QUE983019:QUE983049 REA983019:REA983049 RNW983019:RNW983049 RXS983019:RXS983049 SHO983019:SHO983049 SRK983019:SRK983049 TBG983019:TBG983049 TLC983019:TLC983049 TUY983019:TUY983049 UEU983019:UEU983049 UOQ983019:UOQ983049 UYM983019:UYM983049 VII983019:VII983049 VSE983019:VSE983049 WCA983019:WCA983049 WLW983019:WLW983049 Q4:Q20 WVS4:WVS20 WLW4:WLW20 WCA4:WCA20 VSE4:VSE20 VII4:VII20 UYM4:UYM20 UOQ4:UOQ20 UEU4:UEU20 TUY4:TUY20 TLC4:TLC20 TBG4:TBG20 SRK4:SRK20 SHO4:SHO20 RXS4:RXS20 RNW4:RNW20 REA4:REA20 QUE4:QUE20 QKI4:QKI20 QAM4:QAM20 PQQ4:PQQ20 PGU4:PGU20 OWY4:OWY20 ONC4:ONC20 ODG4:ODG20 NTK4:NTK20 NJO4:NJO20 MZS4:MZS20 MPW4:MPW20 MGA4:MGA20 LWE4:LWE20 LMI4:LMI20 LCM4:LCM20 KSQ4:KSQ20 KIU4:KIU20 JYY4:JYY20 JPC4:JPC20 JFG4:JFG20 IVK4:IVK20 ILO4:ILO20 IBS4:IBS20 HRW4:HRW20 HIA4:HIA20 GYE4:GYE20 GOI4:GOI20 GEM4:GEM20 FUQ4:FUQ20 FKU4:FKU20 FAY4:FAY20 ERC4:ERC20 EHG4:EHG20 DXK4:DXK20 DNO4:DNO20 DDS4:DDS20 CTW4:CTW20 CKA4:CKA20 CAE4:CAE20 BQI4:BQI20 BGM4:BGM20 AWQ4:AWQ20 AMU4:AMU20 ACY4:ACY20 TC4:TC20 JG4:JG20" xr:uid="{00000000-0002-0000-0200-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVS983019:WVS983049 Q65515:Q65545 JG65515:JG65545 TC65515:TC65545 ACY65515:ACY65545 AMU65515:AMU65545 AWQ65515:AWQ65545 BGM65515:BGM65545 BQI65515:BQI65545 CAE65515:CAE65545 CKA65515:CKA65545 CTW65515:CTW65545 DDS65515:DDS65545 DNO65515:DNO65545 DXK65515:DXK65545 EHG65515:EHG65545 ERC65515:ERC65545 FAY65515:FAY65545 FKU65515:FKU65545 FUQ65515:FUQ65545 GEM65515:GEM65545 GOI65515:GOI65545 GYE65515:GYE65545 HIA65515:HIA65545 HRW65515:HRW65545 IBS65515:IBS65545 ILO65515:ILO65545 IVK65515:IVK65545 JFG65515:JFG65545 JPC65515:JPC65545 JYY65515:JYY65545 KIU65515:KIU65545 KSQ65515:KSQ65545 LCM65515:LCM65545 LMI65515:LMI65545 LWE65515:LWE65545 MGA65515:MGA65545 MPW65515:MPW65545 MZS65515:MZS65545 NJO65515:NJO65545 NTK65515:NTK65545 ODG65515:ODG65545 ONC65515:ONC65545 OWY65515:OWY65545 PGU65515:PGU65545 PQQ65515:PQQ65545 QAM65515:QAM65545 QKI65515:QKI65545 QUE65515:QUE65545 REA65515:REA65545 RNW65515:RNW65545 RXS65515:RXS65545 SHO65515:SHO65545 SRK65515:SRK65545 TBG65515:TBG65545 TLC65515:TLC65545 TUY65515:TUY65545 UEU65515:UEU65545 UOQ65515:UOQ65545 UYM65515:UYM65545 VII65515:VII65545 VSE65515:VSE65545 WCA65515:WCA65545 WLW65515:WLW65545 WVS65515:WVS65545 Q131051:Q131081 JG131051:JG131081 TC131051:TC131081 ACY131051:ACY131081 AMU131051:AMU131081 AWQ131051:AWQ131081 BGM131051:BGM131081 BQI131051:BQI131081 CAE131051:CAE131081 CKA131051:CKA131081 CTW131051:CTW131081 DDS131051:DDS131081 DNO131051:DNO131081 DXK131051:DXK131081 EHG131051:EHG131081 ERC131051:ERC131081 FAY131051:FAY131081 FKU131051:FKU131081 FUQ131051:FUQ131081 GEM131051:GEM131081 GOI131051:GOI131081 GYE131051:GYE131081 HIA131051:HIA131081 HRW131051:HRW131081 IBS131051:IBS131081 ILO131051:ILO131081 IVK131051:IVK131081 JFG131051:JFG131081 JPC131051:JPC131081 JYY131051:JYY131081 KIU131051:KIU131081 KSQ131051:KSQ131081 LCM131051:LCM131081 LMI131051:LMI131081 LWE131051:LWE131081 MGA131051:MGA131081 MPW131051:MPW131081 MZS131051:MZS131081 NJO131051:NJO131081 NTK131051:NTK131081 ODG131051:ODG131081 ONC131051:ONC131081 OWY131051:OWY131081 PGU131051:PGU131081 PQQ131051:PQQ131081 QAM131051:QAM131081 QKI131051:QKI131081 QUE131051:QUE131081 REA131051:REA131081 RNW131051:RNW131081 RXS131051:RXS131081 SHO131051:SHO131081 SRK131051:SRK131081 TBG131051:TBG131081 TLC131051:TLC131081 TUY131051:TUY131081 UEU131051:UEU131081 UOQ131051:UOQ131081 UYM131051:UYM131081 VII131051:VII131081 VSE131051:VSE131081 WCA131051:WCA131081 WLW131051:WLW131081 WVS131051:WVS131081 Q196587:Q196617 JG196587:JG196617 TC196587:TC196617 ACY196587:ACY196617 AMU196587:AMU196617 AWQ196587:AWQ196617 BGM196587:BGM196617 BQI196587:BQI196617 CAE196587:CAE196617 CKA196587:CKA196617 CTW196587:CTW196617 DDS196587:DDS196617 DNO196587:DNO196617 DXK196587:DXK196617 EHG196587:EHG196617 ERC196587:ERC196617 FAY196587:FAY196617 FKU196587:FKU196617 FUQ196587:FUQ196617 GEM196587:GEM196617 GOI196587:GOI196617 GYE196587:GYE196617 HIA196587:HIA196617 HRW196587:HRW196617 IBS196587:IBS196617 ILO196587:ILO196617 IVK196587:IVK196617 JFG196587:JFG196617 JPC196587:JPC196617 JYY196587:JYY196617 KIU196587:KIU196617 KSQ196587:KSQ196617 LCM196587:LCM196617 LMI196587:LMI196617 LWE196587:LWE196617 MGA196587:MGA196617 MPW196587:MPW196617 MZS196587:MZS196617 NJO196587:NJO196617 NTK196587:NTK196617 ODG196587:ODG196617 ONC196587:ONC196617 OWY196587:OWY196617 PGU196587:PGU196617 PQQ196587:PQQ196617 QAM196587:QAM196617 QKI196587:QKI196617 QUE196587:QUE196617 REA196587:REA196617 RNW196587:RNW196617 RXS196587:RXS196617 SHO196587:SHO196617 SRK196587:SRK196617 TBG196587:TBG196617 TLC196587:TLC196617 TUY196587:TUY196617 UEU196587:UEU196617 UOQ196587:UOQ196617 UYM196587:UYM196617 VII196587:VII196617 VSE196587:VSE196617 WCA196587:WCA196617 WLW196587:WLW196617 WVS196587:WVS196617 Q262123:Q262153 JG262123:JG262153 TC262123:TC262153 ACY262123:ACY262153 AMU262123:AMU262153 AWQ262123:AWQ262153 BGM262123:BGM262153 BQI262123:BQI262153 CAE262123:CAE262153 CKA262123:CKA262153 CTW262123:CTW262153 DDS262123:DDS262153 DNO262123:DNO262153 DXK262123:DXK262153 EHG262123:EHG262153 ERC262123:ERC262153 FAY262123:FAY262153 FKU262123:FKU262153 FUQ262123:FUQ262153 GEM262123:GEM262153 GOI262123:GOI262153 GYE262123:GYE262153 HIA262123:HIA262153 HRW262123:HRW262153 IBS262123:IBS262153 ILO262123:ILO262153 IVK262123:IVK262153 JFG262123:JFG262153 JPC262123:JPC262153 JYY262123:JYY262153 KIU262123:KIU262153 KSQ262123:KSQ262153 LCM262123:LCM262153 LMI262123:LMI262153 LWE262123:LWE262153 MGA262123:MGA262153 MPW262123:MPW262153 MZS262123:MZS262153 NJO262123:NJO262153 NTK262123:NTK262153 ODG262123:ODG262153 ONC262123:ONC262153 OWY262123:OWY262153 PGU262123:PGU262153 PQQ262123:PQQ262153 QAM262123:QAM262153 QKI262123:QKI262153 QUE262123:QUE262153 REA262123:REA262153 RNW262123:RNW262153 RXS262123:RXS262153 SHO262123:SHO262153 SRK262123:SRK262153 TBG262123:TBG262153 TLC262123:TLC262153 TUY262123:TUY262153 UEU262123:UEU262153 UOQ262123:UOQ262153 UYM262123:UYM262153 VII262123:VII262153 VSE262123:VSE262153 WCA262123:WCA262153 WLW262123:WLW262153 WVS262123:WVS262153 Q327659:Q327689 JG327659:JG327689 TC327659:TC327689 ACY327659:ACY327689 AMU327659:AMU327689 AWQ327659:AWQ327689 BGM327659:BGM327689 BQI327659:BQI327689 CAE327659:CAE327689 CKA327659:CKA327689 CTW327659:CTW327689 DDS327659:DDS327689 DNO327659:DNO327689 DXK327659:DXK327689 EHG327659:EHG327689 ERC327659:ERC327689 FAY327659:FAY327689 FKU327659:FKU327689 FUQ327659:FUQ327689 GEM327659:GEM327689 GOI327659:GOI327689 GYE327659:GYE327689 HIA327659:HIA327689 HRW327659:HRW327689 IBS327659:IBS327689 ILO327659:ILO327689 IVK327659:IVK327689 JFG327659:JFG327689 JPC327659:JPC327689 JYY327659:JYY327689 KIU327659:KIU327689 KSQ327659:KSQ327689 LCM327659:LCM327689 LMI327659:LMI327689 LWE327659:LWE327689 MGA327659:MGA327689 MPW327659:MPW327689 MZS327659:MZS327689 NJO327659:NJO327689 NTK327659:NTK327689 ODG327659:ODG327689 ONC327659:ONC327689 OWY327659:OWY327689 PGU327659:PGU327689 PQQ327659:PQQ327689 QAM327659:QAM327689 QKI327659:QKI327689 QUE327659:QUE327689 REA327659:REA327689 RNW327659:RNW327689 RXS327659:RXS327689 SHO327659:SHO327689 SRK327659:SRK327689 TBG327659:TBG327689 TLC327659:TLC327689 TUY327659:TUY327689 UEU327659:UEU327689 UOQ327659:UOQ327689 UYM327659:UYM327689 VII327659:VII327689 VSE327659:VSE327689 WCA327659:WCA327689 WLW327659:WLW327689 WVS327659:WVS327689 Q393195:Q393225 JG393195:JG393225 TC393195:TC393225 ACY393195:ACY393225 AMU393195:AMU393225 AWQ393195:AWQ393225 BGM393195:BGM393225 BQI393195:BQI393225 CAE393195:CAE393225 CKA393195:CKA393225 CTW393195:CTW393225 DDS393195:DDS393225 DNO393195:DNO393225 DXK393195:DXK393225 EHG393195:EHG393225 ERC393195:ERC393225 FAY393195:FAY393225 FKU393195:FKU393225 FUQ393195:FUQ393225 GEM393195:GEM393225 GOI393195:GOI393225 GYE393195:GYE393225 HIA393195:HIA393225 HRW393195:HRW393225 IBS393195:IBS393225 ILO393195:ILO393225 IVK393195:IVK393225 JFG393195:JFG393225 JPC393195:JPC393225 JYY393195:JYY393225 KIU393195:KIU393225 KSQ393195:KSQ393225 LCM393195:LCM393225 LMI393195:LMI393225 LWE393195:LWE393225 MGA393195:MGA393225 MPW393195:MPW393225 MZS393195:MZS393225 NJO393195:NJO393225 NTK393195:NTK393225 ODG393195:ODG393225 ONC393195:ONC393225 OWY393195:OWY393225 PGU393195:PGU393225 PQQ393195:PQQ393225 QAM393195:QAM393225 QKI393195:QKI393225 QUE393195:QUE393225 REA393195:REA393225 RNW393195:RNW393225 RXS393195:RXS393225 SHO393195:SHO393225 SRK393195:SRK393225 TBG393195:TBG393225 TLC393195:TLC393225 TUY393195:TUY393225 UEU393195:UEU393225 UOQ393195:UOQ393225 UYM393195:UYM393225 VII393195:VII393225 VSE393195:VSE393225 WCA393195:WCA393225 WLW393195:WLW393225 WVS393195:WVS393225 Q458731:Q458761 JG458731:JG458761 TC458731:TC458761 ACY458731:ACY458761 AMU458731:AMU458761 AWQ458731:AWQ458761 BGM458731:BGM458761 BQI458731:BQI458761 CAE458731:CAE458761 CKA458731:CKA458761 CTW458731:CTW458761 DDS458731:DDS458761 DNO458731:DNO458761 DXK458731:DXK458761 EHG458731:EHG458761 ERC458731:ERC458761 FAY458731:FAY458761 FKU458731:FKU458761 FUQ458731:FUQ458761 GEM458731:GEM458761 GOI458731:GOI458761 GYE458731:GYE458761 HIA458731:HIA458761 HRW458731:HRW458761 IBS458731:IBS458761 ILO458731:ILO458761 IVK458731:IVK458761 JFG458731:JFG458761 JPC458731:JPC458761 JYY458731:JYY458761 KIU458731:KIU458761 KSQ458731:KSQ458761 LCM458731:LCM458761 LMI458731:LMI458761 LWE458731:LWE458761 MGA458731:MGA458761 MPW458731:MPW458761 MZS458731:MZS458761 NJO458731:NJO458761 NTK458731:NTK458761 ODG458731:ODG458761 ONC458731:ONC458761 OWY458731:OWY458761 PGU458731:PGU458761 PQQ458731:PQQ458761 QAM458731:QAM458761 QKI458731:QKI458761 QUE458731:QUE458761 REA458731:REA458761 RNW458731:RNW458761 RXS458731:RXS458761 SHO458731:SHO458761 SRK458731:SRK458761 TBG458731:TBG458761 TLC458731:TLC458761 TUY458731:TUY458761 UEU458731:UEU458761 UOQ458731:UOQ458761 UYM458731:UYM458761 VII458731:VII458761 VSE458731:VSE458761 WCA458731:WCA458761 WLW458731:WLW458761 WVS458731:WVS458761 Q524267:Q524297 JG524267:JG524297 TC524267:TC524297 ACY524267:ACY524297 AMU524267:AMU524297 AWQ524267:AWQ524297 BGM524267:BGM524297 BQI524267:BQI524297 CAE524267:CAE524297 CKA524267:CKA524297 CTW524267:CTW524297 DDS524267:DDS524297 DNO524267:DNO524297 DXK524267:DXK524297 EHG524267:EHG524297 ERC524267:ERC524297 FAY524267:FAY524297 FKU524267:FKU524297 FUQ524267:FUQ524297 GEM524267:GEM524297 GOI524267:GOI524297 GYE524267:GYE524297 HIA524267:HIA524297 HRW524267:HRW524297 IBS524267:IBS524297 ILO524267:ILO524297 IVK524267:IVK524297 JFG524267:JFG524297 JPC524267:JPC524297 JYY524267:JYY524297 KIU524267:KIU524297 KSQ524267:KSQ524297 LCM524267:LCM524297 LMI524267:LMI524297 LWE524267:LWE524297 MGA524267:MGA524297 MPW524267:MPW524297 MZS524267:MZS524297 NJO524267:NJO524297 NTK524267:NTK524297 ODG524267:ODG524297 ONC524267:ONC524297 OWY524267:OWY524297 PGU524267:PGU524297 PQQ524267:PQQ524297 QAM524267:QAM524297 QKI524267:QKI524297 QUE524267:QUE524297 REA524267:REA524297 RNW524267:RNW524297 RXS524267:RXS524297 SHO524267:SHO524297 SRK524267:SRK524297 TBG524267:TBG524297 TLC524267:TLC524297 TUY524267:TUY524297 UEU524267:UEU524297 UOQ524267:UOQ524297 UYM524267:UYM524297 VII524267:VII524297 VSE524267:VSE524297 WCA524267:WCA524297 WLW524267:WLW524297 WVS524267:WVS524297 Q589803:Q589833 JG589803:JG589833 TC589803:TC589833 ACY589803:ACY589833 AMU589803:AMU589833 AWQ589803:AWQ589833 BGM589803:BGM589833 BQI589803:BQI589833 CAE589803:CAE589833 CKA589803:CKA589833 CTW589803:CTW589833 DDS589803:DDS589833 DNO589803:DNO589833 DXK589803:DXK589833 EHG589803:EHG589833 ERC589803:ERC589833 FAY589803:FAY589833 FKU589803:FKU589833 FUQ589803:FUQ589833 GEM589803:GEM589833 GOI589803:GOI589833 GYE589803:GYE589833 HIA589803:HIA589833 HRW589803:HRW589833 IBS589803:IBS589833 ILO589803:ILO589833 IVK589803:IVK589833 JFG589803:JFG589833 JPC589803:JPC589833 JYY589803:JYY589833 KIU589803:KIU589833 KSQ589803:KSQ589833 LCM589803:LCM589833 LMI589803:LMI589833 LWE589803:LWE589833 MGA589803:MGA589833 MPW589803:MPW589833 MZS589803:MZS589833 NJO589803:NJO589833 NTK589803:NTK589833 ODG589803:ODG589833 ONC589803:ONC589833 OWY589803:OWY589833 PGU589803:PGU589833 PQQ589803:PQQ589833 QAM589803:QAM589833 QKI589803:QKI589833 QUE589803:QUE589833 REA589803:REA589833 RNW589803:RNW589833 RXS589803:RXS589833 SHO589803:SHO589833 SRK589803:SRK589833 TBG589803:TBG589833 TLC589803:TLC589833 TUY589803:TUY589833 UEU589803:UEU589833 UOQ589803:UOQ589833 UYM589803:UYM589833 VII589803:VII589833 VSE589803:VSE589833 WCA589803:WCA589833 WLW589803:WLW589833 WVS589803:WVS589833 Q655339:Q655369 JG655339:JG655369 TC655339:TC655369 ACY655339:ACY655369 AMU655339:AMU655369 AWQ655339:AWQ655369 BGM655339:BGM655369 BQI655339:BQI655369 CAE655339:CAE655369 CKA655339:CKA655369 CTW655339:CTW655369 DDS655339:DDS655369 DNO655339:DNO655369 DXK655339:DXK655369 EHG655339:EHG655369 ERC655339:ERC655369 FAY655339:FAY655369 FKU655339:FKU655369 FUQ655339:FUQ655369 GEM655339:GEM655369 GOI655339:GOI655369 GYE655339:GYE655369 HIA655339:HIA655369 HRW655339:HRW655369 IBS655339:IBS655369 ILO655339:ILO655369 IVK655339:IVK655369 JFG655339:JFG655369 JPC655339:JPC655369 JYY655339:JYY655369 KIU655339:KIU655369 KSQ655339:KSQ655369 LCM655339:LCM655369 LMI655339:LMI655369 LWE655339:LWE655369 MGA655339:MGA655369 MPW655339:MPW655369 MZS655339:MZS655369 NJO655339:NJO655369 NTK655339:NTK655369 ODG655339:ODG655369 ONC655339:ONC655369 OWY655339:OWY655369 PGU655339:PGU655369 PQQ655339:PQQ655369 QAM655339:QAM655369 QKI655339:QKI655369 QUE655339:QUE655369 REA655339:REA655369 RNW655339:RNW655369 RXS655339:RXS655369 SHO655339:SHO655369 SRK655339:SRK655369 TBG655339:TBG655369 TLC655339:TLC655369 TUY655339:TUY655369 UEU655339:UEU655369 UOQ655339:UOQ655369 UYM655339:UYM655369 VII655339:VII655369 VSE655339:VSE655369 WCA655339:WCA655369 WLW655339:WLW655369 WVS655339:WVS655369 Q720875:Q720905 JG720875:JG720905 TC720875:TC720905 ACY720875:ACY720905 AMU720875:AMU720905 AWQ720875:AWQ720905 BGM720875:BGM720905 BQI720875:BQI720905 CAE720875:CAE720905 CKA720875:CKA720905 CTW720875:CTW720905 DDS720875:DDS720905 DNO720875:DNO720905 DXK720875:DXK720905 EHG720875:EHG720905 ERC720875:ERC720905 FAY720875:FAY720905 FKU720875:FKU720905 FUQ720875:FUQ720905 GEM720875:GEM720905 GOI720875:GOI720905 GYE720875:GYE720905 HIA720875:HIA720905 HRW720875:HRW720905 IBS720875:IBS720905 ILO720875:ILO720905 IVK720875:IVK720905 JFG720875:JFG720905 JPC720875:JPC720905 JYY720875:JYY720905 KIU720875:KIU720905 KSQ720875:KSQ720905 LCM720875:LCM720905 LMI720875:LMI720905 LWE720875:LWE720905 MGA720875:MGA720905 MPW720875:MPW720905 MZS720875:MZS720905 NJO720875:NJO720905 NTK720875:NTK720905 ODG720875:ODG720905 ONC720875:ONC720905 OWY720875:OWY720905 PGU720875:PGU720905 PQQ720875:PQQ720905 QAM720875:QAM720905 QKI720875:QKI720905 QUE720875:QUE720905 REA720875:REA720905 RNW720875:RNW720905 RXS720875:RXS720905 SHO720875:SHO720905 SRK720875:SRK720905 TBG720875:TBG720905 TLC720875:TLC720905 TUY720875:TUY720905 UEU720875:UEU720905 UOQ720875:UOQ720905 UYM720875:UYM720905 VII720875:VII720905 VSE720875:VSE720905 WCA720875:WCA720905 WLW720875:WLW720905 WVS720875:WVS720905 Q786411:Q786441 JG786411:JG786441 TC786411:TC786441 ACY786411:ACY786441 AMU786411:AMU786441 AWQ786411:AWQ786441 BGM786411:BGM786441 BQI786411:BQI786441 CAE786411:CAE786441 CKA786411:CKA786441 CTW786411:CTW786441 DDS786411:DDS786441 DNO786411:DNO786441 DXK786411:DXK786441 EHG786411:EHG786441 ERC786411:ERC786441 FAY786411:FAY786441 FKU786411:FKU786441 FUQ786411:FUQ786441 GEM786411:GEM786441 GOI786411:GOI786441 GYE786411:GYE786441 HIA786411:HIA786441 HRW786411:HRW786441 IBS786411:IBS786441 ILO786411:ILO786441 IVK786411:IVK786441 JFG786411:JFG786441 JPC786411:JPC786441 JYY786411:JYY786441 KIU786411:KIU786441 KSQ786411:KSQ786441 LCM786411:LCM786441 LMI786411:LMI786441 LWE786411:LWE786441 MGA786411:MGA786441 MPW786411:MPW786441 MZS786411:MZS786441 NJO786411:NJO786441 NTK786411:NTK786441 ODG786411:ODG786441 ONC786411:ONC786441 OWY786411:OWY786441 PGU786411:PGU786441 PQQ786411:PQQ786441 QAM786411:QAM786441 QKI786411:QKI786441 QUE786411:QUE786441 REA786411:REA786441 RNW786411:RNW786441 RXS786411:RXS786441 SHO786411:SHO786441 SRK786411:SRK786441 TBG786411:TBG786441 TLC786411:TLC786441 TUY786411:TUY786441 UEU786411:UEU786441 UOQ786411:UOQ786441 UYM786411:UYM786441 VII786411:VII786441 VSE786411:VSE786441 WCA786411:WCA786441 WLW786411:WLW786441 WVS786411:WVS786441 Q851947:Q851977 JG851947:JG851977 TC851947:TC851977 ACY851947:ACY851977 AMU851947:AMU851977 AWQ851947:AWQ851977 BGM851947:BGM851977 BQI851947:BQI851977 CAE851947:CAE851977 CKA851947:CKA851977 CTW851947:CTW851977 DDS851947:DDS851977 DNO851947:DNO851977 DXK851947:DXK851977 EHG851947:EHG851977 ERC851947:ERC851977 FAY851947:FAY851977 FKU851947:FKU851977 FUQ851947:FUQ851977 GEM851947:GEM851977 GOI851947:GOI851977 GYE851947:GYE851977 HIA851947:HIA851977 HRW851947:HRW851977 IBS851947:IBS851977 ILO851947:ILO851977 IVK851947:IVK851977 JFG851947:JFG851977 JPC851947:JPC851977 JYY851947:JYY851977 KIU851947:KIU851977 KSQ851947:KSQ851977 LCM851947:LCM851977 LMI851947:LMI851977 LWE851947:LWE851977 MGA851947:MGA851977 MPW851947:MPW851977 MZS851947:MZS851977 NJO851947:NJO851977 NTK851947:NTK851977 ODG851947:ODG851977 ONC851947:ONC851977 OWY851947:OWY851977 PGU851947:PGU851977 PQQ851947:PQQ851977 QAM851947:QAM851977 QKI851947:QKI851977 QUE851947:QUE851977 REA851947:REA851977 RNW851947:RNW851977 RXS851947:RXS851977 SHO851947:SHO851977 SRK851947:SRK851977 TBG851947:TBG851977 TLC851947:TLC851977 TUY851947:TUY851977 UEU851947:UEU851977 UOQ851947:UOQ851977 UYM851947:UYM851977 VII851947:VII851977 VSE851947:VSE851977 WCA851947:WCA851977 WLW851947:WLW851977 WVS851947:WVS851977 Q917483:Q917513 JG917483:JG917513 TC917483:TC917513 ACY917483:ACY917513 AMU917483:AMU917513 AWQ917483:AWQ917513 BGM917483:BGM917513 BQI917483:BQI917513 CAE917483:CAE917513 CKA917483:CKA917513 CTW917483:CTW917513 DDS917483:DDS917513 DNO917483:DNO917513 DXK917483:DXK917513 EHG917483:EHG917513 ERC917483:ERC917513 FAY917483:FAY917513 FKU917483:FKU917513 FUQ917483:FUQ917513 GEM917483:GEM917513 GOI917483:GOI917513 GYE917483:GYE917513 HIA917483:HIA917513 HRW917483:HRW917513 IBS917483:IBS917513 ILO917483:ILO917513 IVK917483:IVK917513 JFG917483:JFG917513 JPC917483:JPC917513 JYY917483:JYY917513 KIU917483:KIU917513 KSQ917483:KSQ917513 LCM917483:LCM917513 LMI917483:LMI917513 LWE917483:LWE917513 MGA917483:MGA917513 MPW917483:MPW917513 MZS917483:MZS917513 NJO917483:NJO917513 NTK917483:NTK917513 ODG917483:ODG917513 ONC917483:ONC917513 OWY917483:OWY917513 PGU917483:PGU917513 PQQ917483:PQQ917513 QAM917483:QAM917513 QKI917483:QKI917513 QUE917483:QUE917513 REA917483:REA917513 RNW917483:RNW917513 RXS917483:RXS917513 SHO917483:SHO917513 SRK917483:SRK917513 TBG917483:TBG917513 TLC917483:TLC917513 TUY917483:TUY917513 UEU917483:UEU917513 UOQ917483:UOQ917513 UYM917483:UYM917513 VII917483:VII917513 VSE917483:VSE917513 WCA917483:WCA917513 WLW917483:WLW917513 WVS917483:WVS917513 Q983019:Q983049 JG983019:JG983049 TC983019:TC983049 ACY983019:ACY983049 AMU983019:AMU983049 AWQ983019:AWQ983049 BGM983019:BGM983049 BQI983019:BQI983049 CAE983019:CAE983049 CKA983019:CKA983049 CTW983019:CTW983049 DDS983019:DDS983049 DNO983019:DNO983049 DXK983019:DXK983049 EHG983019:EHG983049 ERC983019:ERC983049 FAY983019:FAY983049 FKU983019:FKU983049 FUQ983019:FUQ983049 GEM983019:GEM983049 GOI983019:GOI983049 GYE983019:GYE983049 HIA983019:HIA983049 HRW983019:HRW983049 IBS983019:IBS983049 ILO983019:ILO983049 IVK983019:IVK983049 JFG983019:JFG983049 JPC983019:JPC983049 JYY983019:JYY983049 KIU983019:KIU983049 KSQ983019:KSQ983049 LCM983019:LCM983049 LMI983019:LMI983049 LWE983019:LWE983049 MGA983019:MGA983049 MPW983019:MPW983049 MZS983019:MZS983049 NJO983019:NJO983049 NTK983019:NTK983049 ODG983019:ODG983049 ONC983019:ONC983049 OWY983019:OWY983049 PGU983019:PGU983049 PQQ983019:PQQ983049 QAM983019:QAM983049 QKI983019:QKI983049 QUE983019:QUE983049 REA983019:REA983049 RNW983019:RNW983049 RXS983019:RXS983049 SHO983019:SHO983049 SRK983019:SRK983049 TBG983019:TBG983049 TLC983019:TLC983049 TUY983019:TUY983049 UEU983019:UEU983049 UOQ983019:UOQ983049 UYM983019:UYM983049 VII983019:VII983049 VSE983019:VSE983049 WCA983019:WCA983049 WLW983019:WLW983049 JG4:JG20 TC4:TC20 ACY4:ACY20 AMU4:AMU20 AWQ4:AWQ20 BGM4:BGM20 BQI4:BQI20 CAE4:CAE20 CKA4:CKA20 CTW4:CTW20 DDS4:DDS20 DNO4:DNO20 DXK4:DXK20 EHG4:EHG20 ERC4:ERC20 FAY4:FAY20 FKU4:FKU20 FUQ4:FUQ20 GEM4:GEM20 GOI4:GOI20 GYE4:GYE20 HIA4:HIA20 HRW4:HRW20 IBS4:IBS20 ILO4:ILO20 IVK4:IVK20 JFG4:JFG20 JPC4:JPC20 JYY4:JYY20 KIU4:KIU20 KSQ4:KSQ20 LCM4:LCM20 LMI4:LMI20 LWE4:LWE20 MGA4:MGA20 MPW4:MPW20 MZS4:MZS20 NJO4:NJO20 NTK4:NTK20 ODG4:ODG20 ONC4:ONC20 OWY4:OWY20 PGU4:PGU20 PQQ4:PQQ20 QAM4:QAM20 QKI4:QKI20 QUE4:QUE20 REA4:REA20 RNW4:RNW20 RXS4:RXS20 SHO4:SHO20 SRK4:SRK20 TBG4:TBG20 TLC4:TLC20 TUY4:TUY20 UEU4:UEU20 UOQ4:UOQ20 UYM4:UYM20 VII4:VII20 VSE4:VSE20 WCA4:WCA20 WLW4:WLW20 WVS4:WVS20 Q4:Q20" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"Menos de 1 año, 1 a 5 años, 6 a 10 años, 11 a 20 años, mas de 20 años"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JM65515:JM65545 TI65515:TI65545 ADE65515:ADE65545 ANA65515:ANA65545 AWW65515:AWW65545 BGS65515:BGS65545 BQO65515:BQO65545 CAK65515:CAK65545 CKG65515:CKG65545 CUC65515:CUC65545 DDY65515:DDY65545 DNU65515:DNU65545 DXQ65515:DXQ65545 EHM65515:EHM65545 ERI65515:ERI65545 FBE65515:FBE65545 FLA65515:FLA65545 FUW65515:FUW65545 GES65515:GES65545 GOO65515:GOO65545 GYK65515:GYK65545 HIG65515:HIG65545 HSC65515:HSC65545 IBY65515:IBY65545 ILU65515:ILU65545 IVQ65515:IVQ65545 JFM65515:JFM65545 JPI65515:JPI65545 JZE65515:JZE65545 KJA65515:KJA65545 KSW65515:KSW65545 LCS65515:LCS65545 LMO65515:LMO65545 LWK65515:LWK65545 MGG65515:MGG65545 MQC65515:MQC65545 MZY65515:MZY65545 NJU65515:NJU65545 NTQ65515:NTQ65545 ODM65515:ODM65545 ONI65515:ONI65545 OXE65515:OXE65545 PHA65515:PHA65545 PQW65515:PQW65545 QAS65515:QAS65545 QKO65515:QKO65545 QUK65515:QUK65545 REG65515:REG65545 ROC65515:ROC65545 RXY65515:RXY65545 SHU65515:SHU65545 SRQ65515:SRQ65545 TBM65515:TBM65545 TLI65515:TLI65545 TVE65515:TVE65545 UFA65515:UFA65545 UOW65515:UOW65545 UYS65515:UYS65545 VIO65515:VIO65545 VSK65515:VSK65545 WCG65515:WCG65545 WMC65515:WMC65545 WVY65515:WVY65545 JM131051:JM131081 TI131051:TI131081 ADE131051:ADE131081 ANA131051:ANA131081 AWW131051:AWW131081 BGS131051:BGS131081 BQO131051:BQO131081 CAK131051:CAK131081 CKG131051:CKG131081 CUC131051:CUC131081 DDY131051:DDY131081 DNU131051:DNU131081 DXQ131051:DXQ131081 EHM131051:EHM131081 ERI131051:ERI131081 FBE131051:FBE131081 FLA131051:FLA131081 FUW131051:FUW131081 GES131051:GES131081 GOO131051:GOO131081 GYK131051:GYK131081 HIG131051:HIG131081 HSC131051:HSC131081 IBY131051:IBY131081 ILU131051:ILU131081 IVQ131051:IVQ131081 JFM131051:JFM131081 JPI131051:JPI131081 JZE131051:JZE131081 KJA131051:KJA131081 KSW131051:KSW131081 LCS131051:LCS131081 LMO131051:LMO131081 LWK131051:LWK131081 MGG131051:MGG131081 MQC131051:MQC131081 MZY131051:MZY131081 NJU131051:NJU131081 NTQ131051:NTQ131081 ODM131051:ODM131081 ONI131051:ONI131081 OXE131051:OXE131081 PHA131051:PHA131081 PQW131051:PQW131081 QAS131051:QAS131081 QKO131051:QKO131081 QUK131051:QUK131081 REG131051:REG131081 ROC131051:ROC131081 RXY131051:RXY131081 SHU131051:SHU131081 SRQ131051:SRQ131081 TBM131051:TBM131081 TLI131051:TLI131081 TVE131051:TVE131081 UFA131051:UFA131081 UOW131051:UOW131081 UYS131051:UYS131081 VIO131051:VIO131081 VSK131051:VSK131081 WCG131051:WCG131081 WMC131051:WMC131081 WVY131051:WVY131081 JM196587:JM196617 TI196587:TI196617 ADE196587:ADE196617 ANA196587:ANA196617 AWW196587:AWW196617 BGS196587:BGS196617 BQO196587:BQO196617 CAK196587:CAK196617 CKG196587:CKG196617 CUC196587:CUC196617 DDY196587:DDY196617 DNU196587:DNU196617 DXQ196587:DXQ196617 EHM196587:EHM196617 ERI196587:ERI196617 FBE196587:FBE196617 FLA196587:FLA196617 FUW196587:FUW196617 GES196587:GES196617 GOO196587:GOO196617 GYK196587:GYK196617 HIG196587:HIG196617 HSC196587:HSC196617 IBY196587:IBY196617 ILU196587:ILU196617 IVQ196587:IVQ196617 JFM196587:JFM196617 JPI196587:JPI196617 JZE196587:JZE196617 KJA196587:KJA196617 KSW196587:KSW196617 LCS196587:LCS196617 LMO196587:LMO196617 LWK196587:LWK196617 MGG196587:MGG196617 MQC196587:MQC196617 MZY196587:MZY196617 NJU196587:NJU196617 NTQ196587:NTQ196617 ODM196587:ODM196617 ONI196587:ONI196617 OXE196587:OXE196617 PHA196587:PHA196617 PQW196587:PQW196617 QAS196587:QAS196617 QKO196587:QKO196617 QUK196587:QUK196617 REG196587:REG196617 ROC196587:ROC196617 RXY196587:RXY196617 SHU196587:SHU196617 SRQ196587:SRQ196617 TBM196587:TBM196617 TLI196587:TLI196617 TVE196587:TVE196617 UFA196587:UFA196617 UOW196587:UOW196617 UYS196587:UYS196617 VIO196587:VIO196617 VSK196587:VSK196617 WCG196587:WCG196617 WMC196587:WMC196617 WVY196587:WVY196617 JM262123:JM262153 TI262123:TI262153 ADE262123:ADE262153 ANA262123:ANA262153 AWW262123:AWW262153 BGS262123:BGS262153 BQO262123:BQO262153 CAK262123:CAK262153 CKG262123:CKG262153 CUC262123:CUC262153 DDY262123:DDY262153 DNU262123:DNU262153 DXQ262123:DXQ262153 EHM262123:EHM262153 ERI262123:ERI262153 FBE262123:FBE262153 FLA262123:FLA262153 FUW262123:FUW262153 GES262123:GES262153 GOO262123:GOO262153 GYK262123:GYK262153 HIG262123:HIG262153 HSC262123:HSC262153 IBY262123:IBY262153 ILU262123:ILU262153 IVQ262123:IVQ262153 JFM262123:JFM262153 JPI262123:JPI262153 JZE262123:JZE262153 KJA262123:KJA262153 KSW262123:KSW262153 LCS262123:LCS262153 LMO262123:LMO262153 LWK262123:LWK262153 MGG262123:MGG262153 MQC262123:MQC262153 MZY262123:MZY262153 NJU262123:NJU262153 NTQ262123:NTQ262153 ODM262123:ODM262153 ONI262123:ONI262153 OXE262123:OXE262153 PHA262123:PHA262153 PQW262123:PQW262153 QAS262123:QAS262153 QKO262123:QKO262153 QUK262123:QUK262153 REG262123:REG262153 ROC262123:ROC262153 RXY262123:RXY262153 SHU262123:SHU262153 SRQ262123:SRQ262153 TBM262123:TBM262153 TLI262123:TLI262153 TVE262123:TVE262153 UFA262123:UFA262153 UOW262123:UOW262153 UYS262123:UYS262153 VIO262123:VIO262153 VSK262123:VSK262153 WCG262123:WCG262153 WMC262123:WMC262153 WVY262123:WVY262153 JM327659:JM327689 TI327659:TI327689 ADE327659:ADE327689 ANA327659:ANA327689 AWW327659:AWW327689 BGS327659:BGS327689 BQO327659:BQO327689 CAK327659:CAK327689 CKG327659:CKG327689 CUC327659:CUC327689 DDY327659:DDY327689 DNU327659:DNU327689 DXQ327659:DXQ327689 EHM327659:EHM327689 ERI327659:ERI327689 FBE327659:FBE327689 FLA327659:FLA327689 FUW327659:FUW327689 GES327659:GES327689 GOO327659:GOO327689 GYK327659:GYK327689 HIG327659:HIG327689 HSC327659:HSC327689 IBY327659:IBY327689 ILU327659:ILU327689 IVQ327659:IVQ327689 JFM327659:JFM327689 JPI327659:JPI327689 JZE327659:JZE327689 KJA327659:KJA327689 KSW327659:KSW327689 LCS327659:LCS327689 LMO327659:LMO327689 LWK327659:LWK327689 MGG327659:MGG327689 MQC327659:MQC327689 MZY327659:MZY327689 NJU327659:NJU327689 NTQ327659:NTQ327689 ODM327659:ODM327689 ONI327659:ONI327689 OXE327659:OXE327689 PHA327659:PHA327689 PQW327659:PQW327689 QAS327659:QAS327689 QKO327659:QKO327689 QUK327659:QUK327689 REG327659:REG327689 ROC327659:ROC327689 RXY327659:RXY327689 SHU327659:SHU327689 SRQ327659:SRQ327689 TBM327659:TBM327689 TLI327659:TLI327689 TVE327659:TVE327689 UFA327659:UFA327689 UOW327659:UOW327689 UYS327659:UYS327689 VIO327659:VIO327689 VSK327659:VSK327689 WCG327659:WCG327689 WMC327659:WMC327689 WVY327659:WVY327689 JM393195:JM393225 TI393195:TI393225 ADE393195:ADE393225 ANA393195:ANA393225 AWW393195:AWW393225 BGS393195:BGS393225 BQO393195:BQO393225 CAK393195:CAK393225 CKG393195:CKG393225 CUC393195:CUC393225 DDY393195:DDY393225 DNU393195:DNU393225 DXQ393195:DXQ393225 EHM393195:EHM393225 ERI393195:ERI393225 FBE393195:FBE393225 FLA393195:FLA393225 FUW393195:FUW393225 GES393195:GES393225 GOO393195:GOO393225 GYK393195:GYK393225 HIG393195:HIG393225 HSC393195:HSC393225 IBY393195:IBY393225 ILU393195:ILU393225 IVQ393195:IVQ393225 JFM393195:JFM393225 JPI393195:JPI393225 JZE393195:JZE393225 KJA393195:KJA393225 KSW393195:KSW393225 LCS393195:LCS393225 LMO393195:LMO393225 LWK393195:LWK393225 MGG393195:MGG393225 MQC393195:MQC393225 MZY393195:MZY393225 NJU393195:NJU393225 NTQ393195:NTQ393225 ODM393195:ODM393225 ONI393195:ONI393225 OXE393195:OXE393225 PHA393195:PHA393225 PQW393195:PQW393225 QAS393195:QAS393225 QKO393195:QKO393225 QUK393195:QUK393225 REG393195:REG393225 ROC393195:ROC393225 RXY393195:RXY393225 SHU393195:SHU393225 SRQ393195:SRQ393225 TBM393195:TBM393225 TLI393195:TLI393225 TVE393195:TVE393225 UFA393195:UFA393225 UOW393195:UOW393225 UYS393195:UYS393225 VIO393195:VIO393225 VSK393195:VSK393225 WCG393195:WCG393225 WMC393195:WMC393225 WVY393195:WVY393225 JM458731:JM458761 TI458731:TI458761 ADE458731:ADE458761 ANA458731:ANA458761 AWW458731:AWW458761 BGS458731:BGS458761 BQO458731:BQO458761 CAK458731:CAK458761 CKG458731:CKG458761 CUC458731:CUC458761 DDY458731:DDY458761 DNU458731:DNU458761 DXQ458731:DXQ458761 EHM458731:EHM458761 ERI458731:ERI458761 FBE458731:FBE458761 FLA458731:FLA458761 FUW458731:FUW458761 GES458731:GES458761 GOO458731:GOO458761 GYK458731:GYK458761 HIG458731:HIG458761 HSC458731:HSC458761 IBY458731:IBY458761 ILU458731:ILU458761 IVQ458731:IVQ458761 JFM458731:JFM458761 JPI458731:JPI458761 JZE458731:JZE458761 KJA458731:KJA458761 KSW458731:KSW458761 LCS458731:LCS458761 LMO458731:LMO458761 LWK458731:LWK458761 MGG458731:MGG458761 MQC458731:MQC458761 MZY458731:MZY458761 NJU458731:NJU458761 NTQ458731:NTQ458761 ODM458731:ODM458761 ONI458731:ONI458761 OXE458731:OXE458761 PHA458731:PHA458761 PQW458731:PQW458761 QAS458731:QAS458761 QKO458731:QKO458761 QUK458731:QUK458761 REG458731:REG458761 ROC458731:ROC458761 RXY458731:RXY458761 SHU458731:SHU458761 SRQ458731:SRQ458761 TBM458731:TBM458761 TLI458731:TLI458761 TVE458731:TVE458761 UFA458731:UFA458761 UOW458731:UOW458761 UYS458731:UYS458761 VIO458731:VIO458761 VSK458731:VSK458761 WCG458731:WCG458761 WMC458731:WMC458761 WVY458731:WVY458761 JM524267:JM524297 TI524267:TI524297 ADE524267:ADE524297 ANA524267:ANA524297 AWW524267:AWW524297 BGS524267:BGS524297 BQO524267:BQO524297 CAK524267:CAK524297 CKG524267:CKG524297 CUC524267:CUC524297 DDY524267:DDY524297 DNU524267:DNU524297 DXQ524267:DXQ524297 EHM524267:EHM524297 ERI524267:ERI524297 FBE524267:FBE524297 FLA524267:FLA524297 FUW524267:FUW524297 GES524267:GES524297 GOO524267:GOO524297 GYK524267:GYK524297 HIG524267:HIG524297 HSC524267:HSC524297 IBY524267:IBY524297 ILU524267:ILU524297 IVQ524267:IVQ524297 JFM524267:JFM524297 JPI524267:JPI524297 JZE524267:JZE524297 KJA524267:KJA524297 KSW524267:KSW524297 LCS524267:LCS524297 LMO524267:LMO524297 LWK524267:LWK524297 MGG524267:MGG524297 MQC524267:MQC524297 MZY524267:MZY524297 NJU524267:NJU524297 NTQ524267:NTQ524297 ODM524267:ODM524297 ONI524267:ONI524297 OXE524267:OXE524297 PHA524267:PHA524297 PQW524267:PQW524297 QAS524267:QAS524297 QKO524267:QKO524297 QUK524267:QUK524297 REG524267:REG524297 ROC524267:ROC524297 RXY524267:RXY524297 SHU524267:SHU524297 SRQ524267:SRQ524297 TBM524267:TBM524297 TLI524267:TLI524297 TVE524267:TVE524297 UFA524267:UFA524297 UOW524267:UOW524297 UYS524267:UYS524297 VIO524267:VIO524297 VSK524267:VSK524297 WCG524267:WCG524297 WMC524267:WMC524297 WVY524267:WVY524297 JM589803:JM589833 TI589803:TI589833 ADE589803:ADE589833 ANA589803:ANA589833 AWW589803:AWW589833 BGS589803:BGS589833 BQO589803:BQO589833 CAK589803:CAK589833 CKG589803:CKG589833 CUC589803:CUC589833 DDY589803:DDY589833 DNU589803:DNU589833 DXQ589803:DXQ589833 EHM589803:EHM589833 ERI589803:ERI589833 FBE589803:FBE589833 FLA589803:FLA589833 FUW589803:FUW589833 GES589803:GES589833 GOO589803:GOO589833 GYK589803:GYK589833 HIG589803:HIG589833 HSC589803:HSC589833 IBY589803:IBY589833 ILU589803:ILU589833 IVQ589803:IVQ589833 JFM589803:JFM589833 JPI589803:JPI589833 JZE589803:JZE589833 KJA589803:KJA589833 KSW589803:KSW589833 LCS589803:LCS589833 LMO589803:LMO589833 LWK589803:LWK589833 MGG589803:MGG589833 MQC589803:MQC589833 MZY589803:MZY589833 NJU589803:NJU589833 NTQ589803:NTQ589833 ODM589803:ODM589833 ONI589803:ONI589833 OXE589803:OXE589833 PHA589803:PHA589833 PQW589803:PQW589833 QAS589803:QAS589833 QKO589803:QKO589833 QUK589803:QUK589833 REG589803:REG589833 ROC589803:ROC589833 RXY589803:RXY589833 SHU589803:SHU589833 SRQ589803:SRQ589833 TBM589803:TBM589833 TLI589803:TLI589833 TVE589803:TVE589833 UFA589803:UFA589833 UOW589803:UOW589833 UYS589803:UYS589833 VIO589803:VIO589833 VSK589803:VSK589833 WCG589803:WCG589833 WMC589803:WMC589833 WVY589803:WVY589833 JM655339:JM655369 TI655339:TI655369 ADE655339:ADE655369 ANA655339:ANA655369 AWW655339:AWW655369 BGS655339:BGS655369 BQO655339:BQO655369 CAK655339:CAK655369 CKG655339:CKG655369 CUC655339:CUC655369 DDY655339:DDY655369 DNU655339:DNU655369 DXQ655339:DXQ655369 EHM655339:EHM655369 ERI655339:ERI655369 FBE655339:FBE655369 FLA655339:FLA655369 FUW655339:FUW655369 GES655339:GES655369 GOO655339:GOO655369 GYK655339:GYK655369 HIG655339:HIG655369 HSC655339:HSC655369 IBY655339:IBY655369 ILU655339:ILU655369 IVQ655339:IVQ655369 JFM655339:JFM655369 JPI655339:JPI655369 JZE655339:JZE655369 KJA655339:KJA655369 KSW655339:KSW655369 LCS655339:LCS655369 LMO655339:LMO655369 LWK655339:LWK655369 MGG655339:MGG655369 MQC655339:MQC655369 MZY655339:MZY655369 NJU655339:NJU655369 NTQ655339:NTQ655369 ODM655339:ODM655369 ONI655339:ONI655369 OXE655339:OXE655369 PHA655339:PHA655369 PQW655339:PQW655369 QAS655339:QAS655369 QKO655339:QKO655369 QUK655339:QUK655369 REG655339:REG655369 ROC655339:ROC655369 RXY655339:RXY655369 SHU655339:SHU655369 SRQ655339:SRQ655369 TBM655339:TBM655369 TLI655339:TLI655369 TVE655339:TVE655369 UFA655339:UFA655369 UOW655339:UOW655369 UYS655339:UYS655369 VIO655339:VIO655369 VSK655339:VSK655369 WCG655339:WCG655369 WMC655339:WMC655369 WVY655339:WVY655369 JM720875:JM720905 TI720875:TI720905 ADE720875:ADE720905 ANA720875:ANA720905 AWW720875:AWW720905 BGS720875:BGS720905 BQO720875:BQO720905 CAK720875:CAK720905 CKG720875:CKG720905 CUC720875:CUC720905 DDY720875:DDY720905 DNU720875:DNU720905 DXQ720875:DXQ720905 EHM720875:EHM720905 ERI720875:ERI720905 FBE720875:FBE720905 FLA720875:FLA720905 FUW720875:FUW720905 GES720875:GES720905 GOO720875:GOO720905 GYK720875:GYK720905 HIG720875:HIG720905 HSC720875:HSC720905 IBY720875:IBY720905 ILU720875:ILU720905 IVQ720875:IVQ720905 JFM720875:JFM720905 JPI720875:JPI720905 JZE720875:JZE720905 KJA720875:KJA720905 KSW720875:KSW720905 LCS720875:LCS720905 LMO720875:LMO720905 LWK720875:LWK720905 MGG720875:MGG720905 MQC720875:MQC720905 MZY720875:MZY720905 NJU720875:NJU720905 NTQ720875:NTQ720905 ODM720875:ODM720905 ONI720875:ONI720905 OXE720875:OXE720905 PHA720875:PHA720905 PQW720875:PQW720905 QAS720875:QAS720905 QKO720875:QKO720905 QUK720875:QUK720905 REG720875:REG720905 ROC720875:ROC720905 RXY720875:RXY720905 SHU720875:SHU720905 SRQ720875:SRQ720905 TBM720875:TBM720905 TLI720875:TLI720905 TVE720875:TVE720905 UFA720875:UFA720905 UOW720875:UOW720905 UYS720875:UYS720905 VIO720875:VIO720905 VSK720875:VSK720905 WCG720875:WCG720905 WMC720875:WMC720905 WVY720875:WVY720905 JM786411:JM786441 TI786411:TI786441 ADE786411:ADE786441 ANA786411:ANA786441 AWW786411:AWW786441 BGS786411:BGS786441 BQO786411:BQO786441 CAK786411:CAK786441 CKG786411:CKG786441 CUC786411:CUC786441 DDY786411:DDY786441 DNU786411:DNU786441 DXQ786411:DXQ786441 EHM786411:EHM786441 ERI786411:ERI786441 FBE786411:FBE786441 FLA786411:FLA786441 FUW786411:FUW786441 GES786411:GES786441 GOO786411:GOO786441 GYK786411:GYK786441 HIG786411:HIG786441 HSC786411:HSC786441 IBY786411:IBY786441 ILU786411:ILU786441 IVQ786411:IVQ786441 JFM786411:JFM786441 JPI786411:JPI786441 JZE786411:JZE786441 KJA786411:KJA786441 KSW786411:KSW786441 LCS786411:LCS786441 LMO786411:LMO786441 LWK786411:LWK786441 MGG786411:MGG786441 MQC786411:MQC786441 MZY786411:MZY786441 NJU786411:NJU786441 NTQ786411:NTQ786441 ODM786411:ODM786441 ONI786411:ONI786441 OXE786411:OXE786441 PHA786411:PHA786441 PQW786411:PQW786441 QAS786411:QAS786441 QKO786411:QKO786441 QUK786411:QUK786441 REG786411:REG786441 ROC786411:ROC786441 RXY786411:RXY786441 SHU786411:SHU786441 SRQ786411:SRQ786441 TBM786411:TBM786441 TLI786411:TLI786441 TVE786411:TVE786441 UFA786411:UFA786441 UOW786411:UOW786441 UYS786411:UYS786441 VIO786411:VIO786441 VSK786411:VSK786441 WCG786411:WCG786441 WMC786411:WMC786441 WVY786411:WVY786441 JM851947:JM851977 TI851947:TI851977 ADE851947:ADE851977 ANA851947:ANA851977 AWW851947:AWW851977 BGS851947:BGS851977 BQO851947:BQO851977 CAK851947:CAK851977 CKG851947:CKG851977 CUC851947:CUC851977 DDY851947:DDY851977 DNU851947:DNU851977 DXQ851947:DXQ851977 EHM851947:EHM851977 ERI851947:ERI851977 FBE851947:FBE851977 FLA851947:FLA851977 FUW851947:FUW851977 GES851947:GES851977 GOO851947:GOO851977 GYK851947:GYK851977 HIG851947:HIG851977 HSC851947:HSC851977 IBY851947:IBY851977 ILU851947:ILU851977 IVQ851947:IVQ851977 JFM851947:JFM851977 JPI851947:JPI851977 JZE851947:JZE851977 KJA851947:KJA851977 KSW851947:KSW851977 LCS851947:LCS851977 LMO851947:LMO851977 LWK851947:LWK851977 MGG851947:MGG851977 MQC851947:MQC851977 MZY851947:MZY851977 NJU851947:NJU851977 NTQ851947:NTQ851977 ODM851947:ODM851977 ONI851947:ONI851977 OXE851947:OXE851977 PHA851947:PHA851977 PQW851947:PQW851977 QAS851947:QAS851977 QKO851947:QKO851977 QUK851947:QUK851977 REG851947:REG851977 ROC851947:ROC851977 RXY851947:RXY851977 SHU851947:SHU851977 SRQ851947:SRQ851977 TBM851947:TBM851977 TLI851947:TLI851977 TVE851947:TVE851977 UFA851947:UFA851977 UOW851947:UOW851977 UYS851947:UYS851977 VIO851947:VIO851977 VSK851947:VSK851977 WCG851947:WCG851977 WMC851947:WMC851977 WVY851947:WVY851977 JM917483:JM917513 TI917483:TI917513 ADE917483:ADE917513 ANA917483:ANA917513 AWW917483:AWW917513 BGS917483:BGS917513 BQO917483:BQO917513 CAK917483:CAK917513 CKG917483:CKG917513 CUC917483:CUC917513 DDY917483:DDY917513 DNU917483:DNU917513 DXQ917483:DXQ917513 EHM917483:EHM917513 ERI917483:ERI917513 FBE917483:FBE917513 FLA917483:FLA917513 FUW917483:FUW917513 GES917483:GES917513 GOO917483:GOO917513 GYK917483:GYK917513 HIG917483:HIG917513 HSC917483:HSC917513 IBY917483:IBY917513 ILU917483:ILU917513 IVQ917483:IVQ917513 JFM917483:JFM917513 JPI917483:JPI917513 JZE917483:JZE917513 KJA917483:KJA917513 KSW917483:KSW917513 LCS917483:LCS917513 LMO917483:LMO917513 LWK917483:LWK917513 MGG917483:MGG917513 MQC917483:MQC917513 MZY917483:MZY917513 NJU917483:NJU917513 NTQ917483:NTQ917513 ODM917483:ODM917513 ONI917483:ONI917513 OXE917483:OXE917513 PHA917483:PHA917513 PQW917483:PQW917513 QAS917483:QAS917513 QKO917483:QKO917513 QUK917483:QUK917513 REG917483:REG917513 ROC917483:ROC917513 RXY917483:RXY917513 SHU917483:SHU917513 SRQ917483:SRQ917513 TBM917483:TBM917513 TLI917483:TLI917513 TVE917483:TVE917513 UFA917483:UFA917513 UOW917483:UOW917513 UYS917483:UYS917513 VIO917483:VIO917513 VSK917483:VSK917513 WCG917483:WCG917513 WMC917483:WMC917513 WVY917483:WVY917513 JM983019:JM983049 TI983019:TI983049 ADE983019:ADE983049 ANA983019:ANA983049 AWW983019:AWW983049 BGS983019:BGS983049 BQO983019:BQO983049 CAK983019:CAK983049 CKG983019:CKG983049 CUC983019:CUC983049 DDY983019:DDY983049 DNU983019:DNU983049 DXQ983019:DXQ983049 EHM983019:EHM983049 ERI983019:ERI983049 FBE983019:FBE983049 FLA983019:FLA983049 FUW983019:FUW983049 GES983019:GES983049 GOO983019:GOO983049 GYK983019:GYK983049 HIG983019:HIG983049 HSC983019:HSC983049 IBY983019:IBY983049 ILU983019:ILU983049 IVQ983019:IVQ983049 JFM983019:JFM983049 JPI983019:JPI983049 JZE983019:JZE983049 KJA983019:KJA983049 KSW983019:KSW983049 LCS983019:LCS983049 LMO983019:LMO983049 LWK983019:LWK983049 MGG983019:MGG983049 MQC983019:MQC983049 MZY983019:MZY983049 NJU983019:NJU983049 NTQ983019:NTQ983049 ODM983019:ODM983049 ONI983019:ONI983049 OXE983019:OXE983049 PHA983019:PHA983049 PQW983019:PQW983049 QAS983019:QAS983049 QKO983019:QKO983049 QUK983019:QUK983049 REG983019:REG983049 ROC983019:ROC983049 RXY983019:RXY983049 SHU983019:SHU983049 SRQ983019:SRQ983049 TBM983019:TBM983049 TLI983019:TLI983049 TVE983019:TVE983049 UFA983019:UFA983049 UOW983019:UOW983049 UYS983019:UYS983049 VIO983019:VIO983049 VSK983019:VSK983049 WCG983019:WCG983049 WMC983019:WMC983049 WVY983019:WVY983049 WVY4:WVY20 WMC4:WMC20 WCG4:WCG20 VSK4:VSK20 VIO4:VIO20 UYS4:UYS20 UOW4:UOW20 UFA4:UFA20 TVE4:TVE20 TLI4:TLI20 TBM4:TBM20 SRQ4:SRQ20 SHU4:SHU20 RXY4:RXY20 ROC4:ROC20 REG4:REG20 QUK4:QUK20 QKO4:QKO20 QAS4:QAS20 PQW4:PQW20 PHA4:PHA20 OXE4:OXE20 ONI4:ONI20 ODM4:ODM20 NTQ4:NTQ20 NJU4:NJU20 MZY4:MZY20 MQC4:MQC20 MGG4:MGG20 LWK4:LWK20 LMO4:LMO20 LCS4:LCS20 KSW4:KSW20 KJA4:KJA20 JZE4:JZE20 JPI4:JPI20 JFM4:JFM20 IVQ4:IVQ20 ILU4:ILU20 IBY4:IBY20 HSC4:HSC20 HIG4:HIG20 GYK4:GYK20 GOO4:GOO20 GES4:GES20 FUW4:FUW20 FLA4:FLA20 FBE4:FBE20 ERI4:ERI20 EHM4:EHM20 DXQ4:DXQ20 DNU4:DNU20 DDY4:DDY20 CUC4:CUC20 CKG4:CKG20 CAK4:CAK20 BQO4:BQO20 BGS4:BGS20 AWW4:AWW20 ANA4:ANA20 ADE4:ADE20 TI4:TI20 JM4:JM20" xr:uid="{00000000-0002-0000-0200-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JM65515:JM65545 TI65515:TI65545 ADE65515:ADE65545 ANA65515:ANA65545 AWW65515:AWW65545 BGS65515:BGS65545 BQO65515:BQO65545 CAK65515:CAK65545 CKG65515:CKG65545 CUC65515:CUC65545 DDY65515:DDY65545 DNU65515:DNU65545 DXQ65515:DXQ65545 EHM65515:EHM65545 ERI65515:ERI65545 FBE65515:FBE65545 FLA65515:FLA65545 FUW65515:FUW65545 GES65515:GES65545 GOO65515:GOO65545 GYK65515:GYK65545 HIG65515:HIG65545 HSC65515:HSC65545 IBY65515:IBY65545 ILU65515:ILU65545 IVQ65515:IVQ65545 JFM65515:JFM65545 JPI65515:JPI65545 JZE65515:JZE65545 KJA65515:KJA65545 KSW65515:KSW65545 LCS65515:LCS65545 LMO65515:LMO65545 LWK65515:LWK65545 MGG65515:MGG65545 MQC65515:MQC65545 MZY65515:MZY65545 NJU65515:NJU65545 NTQ65515:NTQ65545 ODM65515:ODM65545 ONI65515:ONI65545 OXE65515:OXE65545 PHA65515:PHA65545 PQW65515:PQW65545 QAS65515:QAS65545 QKO65515:QKO65545 QUK65515:QUK65545 REG65515:REG65545 ROC65515:ROC65545 RXY65515:RXY65545 SHU65515:SHU65545 SRQ65515:SRQ65545 TBM65515:TBM65545 TLI65515:TLI65545 TVE65515:TVE65545 UFA65515:UFA65545 UOW65515:UOW65545 UYS65515:UYS65545 VIO65515:VIO65545 VSK65515:VSK65545 WCG65515:WCG65545 WMC65515:WMC65545 WVY65515:WVY65545 JM131051:JM131081 TI131051:TI131081 ADE131051:ADE131081 ANA131051:ANA131081 AWW131051:AWW131081 BGS131051:BGS131081 BQO131051:BQO131081 CAK131051:CAK131081 CKG131051:CKG131081 CUC131051:CUC131081 DDY131051:DDY131081 DNU131051:DNU131081 DXQ131051:DXQ131081 EHM131051:EHM131081 ERI131051:ERI131081 FBE131051:FBE131081 FLA131051:FLA131081 FUW131051:FUW131081 GES131051:GES131081 GOO131051:GOO131081 GYK131051:GYK131081 HIG131051:HIG131081 HSC131051:HSC131081 IBY131051:IBY131081 ILU131051:ILU131081 IVQ131051:IVQ131081 JFM131051:JFM131081 JPI131051:JPI131081 JZE131051:JZE131081 KJA131051:KJA131081 KSW131051:KSW131081 LCS131051:LCS131081 LMO131051:LMO131081 LWK131051:LWK131081 MGG131051:MGG131081 MQC131051:MQC131081 MZY131051:MZY131081 NJU131051:NJU131081 NTQ131051:NTQ131081 ODM131051:ODM131081 ONI131051:ONI131081 OXE131051:OXE131081 PHA131051:PHA131081 PQW131051:PQW131081 QAS131051:QAS131081 QKO131051:QKO131081 QUK131051:QUK131081 REG131051:REG131081 ROC131051:ROC131081 RXY131051:RXY131081 SHU131051:SHU131081 SRQ131051:SRQ131081 TBM131051:TBM131081 TLI131051:TLI131081 TVE131051:TVE131081 UFA131051:UFA131081 UOW131051:UOW131081 UYS131051:UYS131081 VIO131051:VIO131081 VSK131051:VSK131081 WCG131051:WCG131081 WMC131051:WMC131081 WVY131051:WVY131081 JM196587:JM196617 TI196587:TI196617 ADE196587:ADE196617 ANA196587:ANA196617 AWW196587:AWW196617 BGS196587:BGS196617 BQO196587:BQO196617 CAK196587:CAK196617 CKG196587:CKG196617 CUC196587:CUC196617 DDY196587:DDY196617 DNU196587:DNU196617 DXQ196587:DXQ196617 EHM196587:EHM196617 ERI196587:ERI196617 FBE196587:FBE196617 FLA196587:FLA196617 FUW196587:FUW196617 GES196587:GES196617 GOO196587:GOO196617 GYK196587:GYK196617 HIG196587:HIG196617 HSC196587:HSC196617 IBY196587:IBY196617 ILU196587:ILU196617 IVQ196587:IVQ196617 JFM196587:JFM196617 JPI196587:JPI196617 JZE196587:JZE196617 KJA196587:KJA196617 KSW196587:KSW196617 LCS196587:LCS196617 LMO196587:LMO196617 LWK196587:LWK196617 MGG196587:MGG196617 MQC196587:MQC196617 MZY196587:MZY196617 NJU196587:NJU196617 NTQ196587:NTQ196617 ODM196587:ODM196617 ONI196587:ONI196617 OXE196587:OXE196617 PHA196587:PHA196617 PQW196587:PQW196617 QAS196587:QAS196617 QKO196587:QKO196617 QUK196587:QUK196617 REG196587:REG196617 ROC196587:ROC196617 RXY196587:RXY196617 SHU196587:SHU196617 SRQ196587:SRQ196617 TBM196587:TBM196617 TLI196587:TLI196617 TVE196587:TVE196617 UFA196587:UFA196617 UOW196587:UOW196617 UYS196587:UYS196617 VIO196587:VIO196617 VSK196587:VSK196617 WCG196587:WCG196617 WMC196587:WMC196617 WVY196587:WVY196617 JM262123:JM262153 TI262123:TI262153 ADE262123:ADE262153 ANA262123:ANA262153 AWW262123:AWW262153 BGS262123:BGS262153 BQO262123:BQO262153 CAK262123:CAK262153 CKG262123:CKG262153 CUC262123:CUC262153 DDY262123:DDY262153 DNU262123:DNU262153 DXQ262123:DXQ262153 EHM262123:EHM262153 ERI262123:ERI262153 FBE262123:FBE262153 FLA262123:FLA262153 FUW262123:FUW262153 GES262123:GES262153 GOO262123:GOO262153 GYK262123:GYK262153 HIG262123:HIG262153 HSC262123:HSC262153 IBY262123:IBY262153 ILU262123:ILU262153 IVQ262123:IVQ262153 JFM262123:JFM262153 JPI262123:JPI262153 JZE262123:JZE262153 KJA262123:KJA262153 KSW262123:KSW262153 LCS262123:LCS262153 LMO262123:LMO262153 LWK262123:LWK262153 MGG262123:MGG262153 MQC262123:MQC262153 MZY262123:MZY262153 NJU262123:NJU262153 NTQ262123:NTQ262153 ODM262123:ODM262153 ONI262123:ONI262153 OXE262123:OXE262153 PHA262123:PHA262153 PQW262123:PQW262153 QAS262123:QAS262153 QKO262123:QKO262153 QUK262123:QUK262153 REG262123:REG262153 ROC262123:ROC262153 RXY262123:RXY262153 SHU262123:SHU262153 SRQ262123:SRQ262153 TBM262123:TBM262153 TLI262123:TLI262153 TVE262123:TVE262153 UFA262123:UFA262153 UOW262123:UOW262153 UYS262123:UYS262153 VIO262123:VIO262153 VSK262123:VSK262153 WCG262123:WCG262153 WMC262123:WMC262153 WVY262123:WVY262153 JM327659:JM327689 TI327659:TI327689 ADE327659:ADE327689 ANA327659:ANA327689 AWW327659:AWW327689 BGS327659:BGS327689 BQO327659:BQO327689 CAK327659:CAK327689 CKG327659:CKG327689 CUC327659:CUC327689 DDY327659:DDY327689 DNU327659:DNU327689 DXQ327659:DXQ327689 EHM327659:EHM327689 ERI327659:ERI327689 FBE327659:FBE327689 FLA327659:FLA327689 FUW327659:FUW327689 GES327659:GES327689 GOO327659:GOO327689 GYK327659:GYK327689 HIG327659:HIG327689 HSC327659:HSC327689 IBY327659:IBY327689 ILU327659:ILU327689 IVQ327659:IVQ327689 JFM327659:JFM327689 JPI327659:JPI327689 JZE327659:JZE327689 KJA327659:KJA327689 KSW327659:KSW327689 LCS327659:LCS327689 LMO327659:LMO327689 LWK327659:LWK327689 MGG327659:MGG327689 MQC327659:MQC327689 MZY327659:MZY327689 NJU327659:NJU327689 NTQ327659:NTQ327689 ODM327659:ODM327689 ONI327659:ONI327689 OXE327659:OXE327689 PHA327659:PHA327689 PQW327659:PQW327689 QAS327659:QAS327689 QKO327659:QKO327689 QUK327659:QUK327689 REG327659:REG327689 ROC327659:ROC327689 RXY327659:RXY327689 SHU327659:SHU327689 SRQ327659:SRQ327689 TBM327659:TBM327689 TLI327659:TLI327689 TVE327659:TVE327689 UFA327659:UFA327689 UOW327659:UOW327689 UYS327659:UYS327689 VIO327659:VIO327689 VSK327659:VSK327689 WCG327659:WCG327689 WMC327659:WMC327689 WVY327659:WVY327689 JM393195:JM393225 TI393195:TI393225 ADE393195:ADE393225 ANA393195:ANA393225 AWW393195:AWW393225 BGS393195:BGS393225 BQO393195:BQO393225 CAK393195:CAK393225 CKG393195:CKG393225 CUC393195:CUC393225 DDY393195:DDY393225 DNU393195:DNU393225 DXQ393195:DXQ393225 EHM393195:EHM393225 ERI393195:ERI393225 FBE393195:FBE393225 FLA393195:FLA393225 FUW393195:FUW393225 GES393195:GES393225 GOO393195:GOO393225 GYK393195:GYK393225 HIG393195:HIG393225 HSC393195:HSC393225 IBY393195:IBY393225 ILU393195:ILU393225 IVQ393195:IVQ393225 JFM393195:JFM393225 JPI393195:JPI393225 JZE393195:JZE393225 KJA393195:KJA393225 KSW393195:KSW393225 LCS393195:LCS393225 LMO393195:LMO393225 LWK393195:LWK393225 MGG393195:MGG393225 MQC393195:MQC393225 MZY393195:MZY393225 NJU393195:NJU393225 NTQ393195:NTQ393225 ODM393195:ODM393225 ONI393195:ONI393225 OXE393195:OXE393225 PHA393195:PHA393225 PQW393195:PQW393225 QAS393195:QAS393225 QKO393195:QKO393225 QUK393195:QUK393225 REG393195:REG393225 ROC393195:ROC393225 RXY393195:RXY393225 SHU393195:SHU393225 SRQ393195:SRQ393225 TBM393195:TBM393225 TLI393195:TLI393225 TVE393195:TVE393225 UFA393195:UFA393225 UOW393195:UOW393225 UYS393195:UYS393225 VIO393195:VIO393225 VSK393195:VSK393225 WCG393195:WCG393225 WMC393195:WMC393225 WVY393195:WVY393225 JM458731:JM458761 TI458731:TI458761 ADE458731:ADE458761 ANA458731:ANA458761 AWW458731:AWW458761 BGS458731:BGS458761 BQO458731:BQO458761 CAK458731:CAK458761 CKG458731:CKG458761 CUC458731:CUC458761 DDY458731:DDY458761 DNU458731:DNU458761 DXQ458731:DXQ458761 EHM458731:EHM458761 ERI458731:ERI458761 FBE458731:FBE458761 FLA458731:FLA458761 FUW458731:FUW458761 GES458731:GES458761 GOO458731:GOO458761 GYK458731:GYK458761 HIG458731:HIG458761 HSC458731:HSC458761 IBY458731:IBY458761 ILU458731:ILU458761 IVQ458731:IVQ458761 JFM458731:JFM458761 JPI458731:JPI458761 JZE458731:JZE458761 KJA458731:KJA458761 KSW458731:KSW458761 LCS458731:LCS458761 LMO458731:LMO458761 LWK458731:LWK458761 MGG458731:MGG458761 MQC458731:MQC458761 MZY458731:MZY458761 NJU458731:NJU458761 NTQ458731:NTQ458761 ODM458731:ODM458761 ONI458731:ONI458761 OXE458731:OXE458761 PHA458731:PHA458761 PQW458731:PQW458761 QAS458731:QAS458761 QKO458731:QKO458761 QUK458731:QUK458761 REG458731:REG458761 ROC458731:ROC458761 RXY458731:RXY458761 SHU458731:SHU458761 SRQ458731:SRQ458761 TBM458731:TBM458761 TLI458731:TLI458761 TVE458731:TVE458761 UFA458731:UFA458761 UOW458731:UOW458761 UYS458731:UYS458761 VIO458731:VIO458761 VSK458731:VSK458761 WCG458731:WCG458761 WMC458731:WMC458761 WVY458731:WVY458761 JM524267:JM524297 TI524267:TI524297 ADE524267:ADE524297 ANA524267:ANA524297 AWW524267:AWW524297 BGS524267:BGS524297 BQO524267:BQO524297 CAK524267:CAK524297 CKG524267:CKG524297 CUC524267:CUC524297 DDY524267:DDY524297 DNU524267:DNU524297 DXQ524267:DXQ524297 EHM524267:EHM524297 ERI524267:ERI524297 FBE524267:FBE524297 FLA524267:FLA524297 FUW524267:FUW524297 GES524267:GES524297 GOO524267:GOO524297 GYK524267:GYK524297 HIG524267:HIG524297 HSC524267:HSC524297 IBY524267:IBY524297 ILU524267:ILU524297 IVQ524267:IVQ524297 JFM524267:JFM524297 JPI524267:JPI524297 JZE524267:JZE524297 KJA524267:KJA524297 KSW524267:KSW524297 LCS524267:LCS524297 LMO524267:LMO524297 LWK524267:LWK524297 MGG524267:MGG524297 MQC524267:MQC524297 MZY524267:MZY524297 NJU524267:NJU524297 NTQ524267:NTQ524297 ODM524267:ODM524297 ONI524267:ONI524297 OXE524267:OXE524297 PHA524267:PHA524297 PQW524267:PQW524297 QAS524267:QAS524297 QKO524267:QKO524297 QUK524267:QUK524297 REG524267:REG524297 ROC524267:ROC524297 RXY524267:RXY524297 SHU524267:SHU524297 SRQ524267:SRQ524297 TBM524267:TBM524297 TLI524267:TLI524297 TVE524267:TVE524297 UFA524267:UFA524297 UOW524267:UOW524297 UYS524267:UYS524297 VIO524267:VIO524297 VSK524267:VSK524297 WCG524267:WCG524297 WMC524267:WMC524297 WVY524267:WVY524297 JM589803:JM589833 TI589803:TI589833 ADE589803:ADE589833 ANA589803:ANA589833 AWW589803:AWW589833 BGS589803:BGS589833 BQO589803:BQO589833 CAK589803:CAK589833 CKG589803:CKG589833 CUC589803:CUC589833 DDY589803:DDY589833 DNU589803:DNU589833 DXQ589803:DXQ589833 EHM589803:EHM589833 ERI589803:ERI589833 FBE589803:FBE589833 FLA589803:FLA589833 FUW589803:FUW589833 GES589803:GES589833 GOO589803:GOO589833 GYK589803:GYK589833 HIG589803:HIG589833 HSC589803:HSC589833 IBY589803:IBY589833 ILU589803:ILU589833 IVQ589803:IVQ589833 JFM589803:JFM589833 JPI589803:JPI589833 JZE589803:JZE589833 KJA589803:KJA589833 KSW589803:KSW589833 LCS589803:LCS589833 LMO589803:LMO589833 LWK589803:LWK589833 MGG589803:MGG589833 MQC589803:MQC589833 MZY589803:MZY589833 NJU589803:NJU589833 NTQ589803:NTQ589833 ODM589803:ODM589833 ONI589803:ONI589833 OXE589803:OXE589833 PHA589803:PHA589833 PQW589803:PQW589833 QAS589803:QAS589833 QKO589803:QKO589833 QUK589803:QUK589833 REG589803:REG589833 ROC589803:ROC589833 RXY589803:RXY589833 SHU589803:SHU589833 SRQ589803:SRQ589833 TBM589803:TBM589833 TLI589803:TLI589833 TVE589803:TVE589833 UFA589803:UFA589833 UOW589803:UOW589833 UYS589803:UYS589833 VIO589803:VIO589833 VSK589803:VSK589833 WCG589803:WCG589833 WMC589803:WMC589833 WVY589803:WVY589833 JM655339:JM655369 TI655339:TI655369 ADE655339:ADE655369 ANA655339:ANA655369 AWW655339:AWW655369 BGS655339:BGS655369 BQO655339:BQO655369 CAK655339:CAK655369 CKG655339:CKG655369 CUC655339:CUC655369 DDY655339:DDY655369 DNU655339:DNU655369 DXQ655339:DXQ655369 EHM655339:EHM655369 ERI655339:ERI655369 FBE655339:FBE655369 FLA655339:FLA655369 FUW655339:FUW655369 GES655339:GES655369 GOO655339:GOO655369 GYK655339:GYK655369 HIG655339:HIG655369 HSC655339:HSC655369 IBY655339:IBY655369 ILU655339:ILU655369 IVQ655339:IVQ655369 JFM655339:JFM655369 JPI655339:JPI655369 JZE655339:JZE655369 KJA655339:KJA655369 KSW655339:KSW655369 LCS655339:LCS655369 LMO655339:LMO655369 LWK655339:LWK655369 MGG655339:MGG655369 MQC655339:MQC655369 MZY655339:MZY655369 NJU655339:NJU655369 NTQ655339:NTQ655369 ODM655339:ODM655369 ONI655339:ONI655369 OXE655339:OXE655369 PHA655339:PHA655369 PQW655339:PQW655369 QAS655339:QAS655369 QKO655339:QKO655369 QUK655339:QUK655369 REG655339:REG655369 ROC655339:ROC655369 RXY655339:RXY655369 SHU655339:SHU655369 SRQ655339:SRQ655369 TBM655339:TBM655369 TLI655339:TLI655369 TVE655339:TVE655369 UFA655339:UFA655369 UOW655339:UOW655369 UYS655339:UYS655369 VIO655339:VIO655369 VSK655339:VSK655369 WCG655339:WCG655369 WMC655339:WMC655369 WVY655339:WVY655369 JM720875:JM720905 TI720875:TI720905 ADE720875:ADE720905 ANA720875:ANA720905 AWW720875:AWW720905 BGS720875:BGS720905 BQO720875:BQO720905 CAK720875:CAK720905 CKG720875:CKG720905 CUC720875:CUC720905 DDY720875:DDY720905 DNU720875:DNU720905 DXQ720875:DXQ720905 EHM720875:EHM720905 ERI720875:ERI720905 FBE720875:FBE720905 FLA720875:FLA720905 FUW720875:FUW720905 GES720875:GES720905 GOO720875:GOO720905 GYK720875:GYK720905 HIG720875:HIG720905 HSC720875:HSC720905 IBY720875:IBY720905 ILU720875:ILU720905 IVQ720875:IVQ720905 JFM720875:JFM720905 JPI720875:JPI720905 JZE720875:JZE720905 KJA720875:KJA720905 KSW720875:KSW720905 LCS720875:LCS720905 LMO720875:LMO720905 LWK720875:LWK720905 MGG720875:MGG720905 MQC720875:MQC720905 MZY720875:MZY720905 NJU720875:NJU720905 NTQ720875:NTQ720905 ODM720875:ODM720905 ONI720875:ONI720905 OXE720875:OXE720905 PHA720875:PHA720905 PQW720875:PQW720905 QAS720875:QAS720905 QKO720875:QKO720905 QUK720875:QUK720905 REG720875:REG720905 ROC720875:ROC720905 RXY720875:RXY720905 SHU720875:SHU720905 SRQ720875:SRQ720905 TBM720875:TBM720905 TLI720875:TLI720905 TVE720875:TVE720905 UFA720875:UFA720905 UOW720875:UOW720905 UYS720875:UYS720905 VIO720875:VIO720905 VSK720875:VSK720905 WCG720875:WCG720905 WMC720875:WMC720905 WVY720875:WVY720905 JM786411:JM786441 TI786411:TI786441 ADE786411:ADE786441 ANA786411:ANA786441 AWW786411:AWW786441 BGS786411:BGS786441 BQO786411:BQO786441 CAK786411:CAK786441 CKG786411:CKG786441 CUC786411:CUC786441 DDY786411:DDY786441 DNU786411:DNU786441 DXQ786411:DXQ786441 EHM786411:EHM786441 ERI786411:ERI786441 FBE786411:FBE786441 FLA786411:FLA786441 FUW786411:FUW786441 GES786411:GES786441 GOO786411:GOO786441 GYK786411:GYK786441 HIG786411:HIG786441 HSC786411:HSC786441 IBY786411:IBY786441 ILU786411:ILU786441 IVQ786411:IVQ786441 JFM786411:JFM786441 JPI786411:JPI786441 JZE786411:JZE786441 KJA786411:KJA786441 KSW786411:KSW786441 LCS786411:LCS786441 LMO786411:LMO786441 LWK786411:LWK786441 MGG786411:MGG786441 MQC786411:MQC786441 MZY786411:MZY786441 NJU786411:NJU786441 NTQ786411:NTQ786441 ODM786411:ODM786441 ONI786411:ONI786441 OXE786411:OXE786441 PHA786411:PHA786441 PQW786411:PQW786441 QAS786411:QAS786441 QKO786411:QKO786441 QUK786411:QUK786441 REG786411:REG786441 ROC786411:ROC786441 RXY786411:RXY786441 SHU786411:SHU786441 SRQ786411:SRQ786441 TBM786411:TBM786441 TLI786411:TLI786441 TVE786411:TVE786441 UFA786411:UFA786441 UOW786411:UOW786441 UYS786411:UYS786441 VIO786411:VIO786441 VSK786411:VSK786441 WCG786411:WCG786441 WMC786411:WMC786441 WVY786411:WVY786441 JM851947:JM851977 TI851947:TI851977 ADE851947:ADE851977 ANA851947:ANA851977 AWW851947:AWW851977 BGS851947:BGS851977 BQO851947:BQO851977 CAK851947:CAK851977 CKG851947:CKG851977 CUC851947:CUC851977 DDY851947:DDY851977 DNU851947:DNU851977 DXQ851947:DXQ851977 EHM851947:EHM851977 ERI851947:ERI851977 FBE851947:FBE851977 FLA851947:FLA851977 FUW851947:FUW851977 GES851947:GES851977 GOO851947:GOO851977 GYK851947:GYK851977 HIG851947:HIG851977 HSC851947:HSC851977 IBY851947:IBY851977 ILU851947:ILU851977 IVQ851947:IVQ851977 JFM851947:JFM851977 JPI851947:JPI851977 JZE851947:JZE851977 KJA851947:KJA851977 KSW851947:KSW851977 LCS851947:LCS851977 LMO851947:LMO851977 LWK851947:LWK851977 MGG851947:MGG851977 MQC851947:MQC851977 MZY851947:MZY851977 NJU851947:NJU851977 NTQ851947:NTQ851977 ODM851947:ODM851977 ONI851947:ONI851977 OXE851947:OXE851977 PHA851947:PHA851977 PQW851947:PQW851977 QAS851947:QAS851977 QKO851947:QKO851977 QUK851947:QUK851977 REG851947:REG851977 ROC851947:ROC851977 RXY851947:RXY851977 SHU851947:SHU851977 SRQ851947:SRQ851977 TBM851947:TBM851977 TLI851947:TLI851977 TVE851947:TVE851977 UFA851947:UFA851977 UOW851947:UOW851977 UYS851947:UYS851977 VIO851947:VIO851977 VSK851947:VSK851977 WCG851947:WCG851977 WMC851947:WMC851977 WVY851947:WVY851977 JM917483:JM917513 TI917483:TI917513 ADE917483:ADE917513 ANA917483:ANA917513 AWW917483:AWW917513 BGS917483:BGS917513 BQO917483:BQO917513 CAK917483:CAK917513 CKG917483:CKG917513 CUC917483:CUC917513 DDY917483:DDY917513 DNU917483:DNU917513 DXQ917483:DXQ917513 EHM917483:EHM917513 ERI917483:ERI917513 FBE917483:FBE917513 FLA917483:FLA917513 FUW917483:FUW917513 GES917483:GES917513 GOO917483:GOO917513 GYK917483:GYK917513 HIG917483:HIG917513 HSC917483:HSC917513 IBY917483:IBY917513 ILU917483:ILU917513 IVQ917483:IVQ917513 JFM917483:JFM917513 JPI917483:JPI917513 JZE917483:JZE917513 KJA917483:KJA917513 KSW917483:KSW917513 LCS917483:LCS917513 LMO917483:LMO917513 LWK917483:LWK917513 MGG917483:MGG917513 MQC917483:MQC917513 MZY917483:MZY917513 NJU917483:NJU917513 NTQ917483:NTQ917513 ODM917483:ODM917513 ONI917483:ONI917513 OXE917483:OXE917513 PHA917483:PHA917513 PQW917483:PQW917513 QAS917483:QAS917513 QKO917483:QKO917513 QUK917483:QUK917513 REG917483:REG917513 ROC917483:ROC917513 RXY917483:RXY917513 SHU917483:SHU917513 SRQ917483:SRQ917513 TBM917483:TBM917513 TLI917483:TLI917513 TVE917483:TVE917513 UFA917483:UFA917513 UOW917483:UOW917513 UYS917483:UYS917513 VIO917483:VIO917513 VSK917483:VSK917513 WCG917483:WCG917513 WMC917483:WMC917513 WVY917483:WVY917513 JM983019:JM983049 TI983019:TI983049 ADE983019:ADE983049 ANA983019:ANA983049 AWW983019:AWW983049 BGS983019:BGS983049 BQO983019:BQO983049 CAK983019:CAK983049 CKG983019:CKG983049 CUC983019:CUC983049 DDY983019:DDY983049 DNU983019:DNU983049 DXQ983019:DXQ983049 EHM983019:EHM983049 ERI983019:ERI983049 FBE983019:FBE983049 FLA983019:FLA983049 FUW983019:FUW983049 GES983019:GES983049 GOO983019:GOO983049 GYK983019:GYK983049 HIG983019:HIG983049 HSC983019:HSC983049 IBY983019:IBY983049 ILU983019:ILU983049 IVQ983019:IVQ983049 JFM983019:JFM983049 JPI983019:JPI983049 JZE983019:JZE983049 KJA983019:KJA983049 KSW983019:KSW983049 LCS983019:LCS983049 LMO983019:LMO983049 LWK983019:LWK983049 MGG983019:MGG983049 MQC983019:MQC983049 MZY983019:MZY983049 NJU983019:NJU983049 NTQ983019:NTQ983049 ODM983019:ODM983049 ONI983019:ONI983049 OXE983019:OXE983049 PHA983019:PHA983049 PQW983019:PQW983049 QAS983019:QAS983049 QKO983019:QKO983049 QUK983019:QUK983049 REG983019:REG983049 ROC983019:ROC983049 RXY983019:RXY983049 SHU983019:SHU983049 SRQ983019:SRQ983049 TBM983019:TBM983049 TLI983019:TLI983049 TVE983019:TVE983049 UFA983019:UFA983049 UOW983019:UOW983049 UYS983019:UYS983049 VIO983019:VIO983049 VSK983019:VSK983049 WCG983019:WCG983049 WMC983019:WMC983049 WVY983019:WVY983049 JM4:JM20 TI4:TI20 ADE4:ADE20 ANA4:ANA20 AWW4:AWW20 BGS4:BGS20 BQO4:BQO20 CAK4:CAK20 CKG4:CKG20 CUC4:CUC20 DDY4:DDY20 DNU4:DNU20 DXQ4:DXQ20 EHM4:EHM20 ERI4:ERI20 FBE4:FBE20 FLA4:FLA20 FUW4:FUW20 GES4:GES20 GOO4:GOO20 GYK4:GYK20 HIG4:HIG20 HSC4:HSC20 IBY4:IBY20 ILU4:ILU20 IVQ4:IVQ20 JFM4:JFM20 JPI4:JPI20 JZE4:JZE20 KJA4:KJA20 KSW4:KSW20 LCS4:LCS20 LMO4:LMO20 LWK4:LWK20 MGG4:MGG20 MQC4:MQC20 MZY4:MZY20 NJU4:NJU20 NTQ4:NTQ20 ODM4:ODM20 ONI4:ONI20 OXE4:OXE20 PHA4:PHA20 PQW4:PQW20 QAS4:QAS20 QKO4:QKO20 QUK4:QUK20 REG4:REG20 ROC4:ROC20 RXY4:RXY20 SHU4:SHU20 SRQ4:SRQ20 TBM4:TBM20 TLI4:TLI20 TVE4:TVE20 UFA4:UFA20 UOW4:UOW20 UYS4:UYS20 VIO4:VIO20 VSK4:VSK20 WCG4:WCG20 WMC4:WMC20 WVY4:WVY20" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"1 salario minimo, 1 a 3 salarios minimos, mas de 3 salarios minimos"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U65515:Y65545 U131051:Y131081 JL65515:JL65545 TH65515:TH65545 ADD65515:ADD65545 AMZ65515:AMZ65545 AWV65515:AWV65545 BGR65515:BGR65545 BQN65515:BQN65545 CAJ65515:CAJ65545 CKF65515:CKF65545 CUB65515:CUB65545 DDX65515:DDX65545 DNT65515:DNT65545 DXP65515:DXP65545 EHL65515:EHL65545 ERH65515:ERH65545 FBD65515:FBD65545 FKZ65515:FKZ65545 FUV65515:FUV65545 GER65515:GER65545 GON65515:GON65545 GYJ65515:GYJ65545 HIF65515:HIF65545 HSB65515:HSB65545 IBX65515:IBX65545 ILT65515:ILT65545 IVP65515:IVP65545 JFL65515:JFL65545 JPH65515:JPH65545 JZD65515:JZD65545 KIZ65515:KIZ65545 KSV65515:KSV65545 LCR65515:LCR65545 LMN65515:LMN65545 LWJ65515:LWJ65545 MGF65515:MGF65545 MQB65515:MQB65545 MZX65515:MZX65545 NJT65515:NJT65545 NTP65515:NTP65545 ODL65515:ODL65545 ONH65515:ONH65545 OXD65515:OXD65545 PGZ65515:PGZ65545 PQV65515:PQV65545 QAR65515:QAR65545 QKN65515:QKN65545 QUJ65515:QUJ65545 REF65515:REF65545 ROB65515:ROB65545 RXX65515:RXX65545 SHT65515:SHT65545 SRP65515:SRP65545 TBL65515:TBL65545 TLH65515:TLH65545 TVD65515:TVD65545 UEZ65515:UEZ65545 UOV65515:UOV65545 UYR65515:UYR65545 VIN65515:VIN65545 VSJ65515:VSJ65545 WCF65515:WCF65545 WMB65515:WMB65545 WVX65515:WVX65545 U196587:Y196617 JL131051:JL131081 TH131051:TH131081 ADD131051:ADD131081 AMZ131051:AMZ131081 AWV131051:AWV131081 BGR131051:BGR131081 BQN131051:BQN131081 CAJ131051:CAJ131081 CKF131051:CKF131081 CUB131051:CUB131081 DDX131051:DDX131081 DNT131051:DNT131081 DXP131051:DXP131081 EHL131051:EHL131081 ERH131051:ERH131081 FBD131051:FBD131081 FKZ131051:FKZ131081 FUV131051:FUV131081 GER131051:GER131081 GON131051:GON131081 GYJ131051:GYJ131081 HIF131051:HIF131081 HSB131051:HSB131081 IBX131051:IBX131081 ILT131051:ILT131081 IVP131051:IVP131081 JFL131051:JFL131081 JPH131051:JPH131081 JZD131051:JZD131081 KIZ131051:KIZ131081 KSV131051:KSV131081 LCR131051:LCR131081 LMN131051:LMN131081 LWJ131051:LWJ131081 MGF131051:MGF131081 MQB131051:MQB131081 MZX131051:MZX131081 NJT131051:NJT131081 NTP131051:NTP131081 ODL131051:ODL131081 ONH131051:ONH131081 OXD131051:OXD131081 PGZ131051:PGZ131081 PQV131051:PQV131081 QAR131051:QAR131081 QKN131051:QKN131081 QUJ131051:QUJ131081 REF131051:REF131081 ROB131051:ROB131081 RXX131051:RXX131081 SHT131051:SHT131081 SRP131051:SRP131081 TBL131051:TBL131081 TLH131051:TLH131081 TVD131051:TVD131081 UEZ131051:UEZ131081 UOV131051:UOV131081 UYR131051:UYR131081 VIN131051:VIN131081 VSJ131051:VSJ131081 WCF131051:WCF131081 WMB131051:WMB131081 WVX131051:WVX131081 U262123:Y262153 JL196587:JL196617 TH196587:TH196617 ADD196587:ADD196617 AMZ196587:AMZ196617 AWV196587:AWV196617 BGR196587:BGR196617 BQN196587:BQN196617 CAJ196587:CAJ196617 CKF196587:CKF196617 CUB196587:CUB196617 DDX196587:DDX196617 DNT196587:DNT196617 DXP196587:DXP196617 EHL196587:EHL196617 ERH196587:ERH196617 FBD196587:FBD196617 FKZ196587:FKZ196617 FUV196587:FUV196617 GER196587:GER196617 GON196587:GON196617 GYJ196587:GYJ196617 HIF196587:HIF196617 HSB196587:HSB196617 IBX196587:IBX196617 ILT196587:ILT196617 IVP196587:IVP196617 JFL196587:JFL196617 JPH196587:JPH196617 JZD196587:JZD196617 KIZ196587:KIZ196617 KSV196587:KSV196617 LCR196587:LCR196617 LMN196587:LMN196617 LWJ196587:LWJ196617 MGF196587:MGF196617 MQB196587:MQB196617 MZX196587:MZX196617 NJT196587:NJT196617 NTP196587:NTP196617 ODL196587:ODL196617 ONH196587:ONH196617 OXD196587:OXD196617 PGZ196587:PGZ196617 PQV196587:PQV196617 QAR196587:QAR196617 QKN196587:QKN196617 QUJ196587:QUJ196617 REF196587:REF196617 ROB196587:ROB196617 RXX196587:RXX196617 SHT196587:SHT196617 SRP196587:SRP196617 TBL196587:TBL196617 TLH196587:TLH196617 TVD196587:TVD196617 UEZ196587:UEZ196617 UOV196587:UOV196617 UYR196587:UYR196617 VIN196587:VIN196617 VSJ196587:VSJ196617 WCF196587:WCF196617 WMB196587:WMB196617 WVX196587:WVX196617 U327659:Y327689 JL262123:JL262153 TH262123:TH262153 ADD262123:ADD262153 AMZ262123:AMZ262153 AWV262123:AWV262153 BGR262123:BGR262153 BQN262123:BQN262153 CAJ262123:CAJ262153 CKF262123:CKF262153 CUB262123:CUB262153 DDX262123:DDX262153 DNT262123:DNT262153 DXP262123:DXP262153 EHL262123:EHL262153 ERH262123:ERH262153 FBD262123:FBD262153 FKZ262123:FKZ262153 FUV262123:FUV262153 GER262123:GER262153 GON262123:GON262153 GYJ262123:GYJ262153 HIF262123:HIF262153 HSB262123:HSB262153 IBX262123:IBX262153 ILT262123:ILT262153 IVP262123:IVP262153 JFL262123:JFL262153 JPH262123:JPH262153 JZD262123:JZD262153 KIZ262123:KIZ262153 KSV262123:KSV262153 LCR262123:LCR262153 LMN262123:LMN262153 LWJ262123:LWJ262153 MGF262123:MGF262153 MQB262123:MQB262153 MZX262123:MZX262153 NJT262123:NJT262153 NTP262123:NTP262153 ODL262123:ODL262153 ONH262123:ONH262153 OXD262123:OXD262153 PGZ262123:PGZ262153 PQV262123:PQV262153 QAR262123:QAR262153 QKN262123:QKN262153 QUJ262123:QUJ262153 REF262123:REF262153 ROB262123:ROB262153 RXX262123:RXX262153 SHT262123:SHT262153 SRP262123:SRP262153 TBL262123:TBL262153 TLH262123:TLH262153 TVD262123:TVD262153 UEZ262123:UEZ262153 UOV262123:UOV262153 UYR262123:UYR262153 VIN262123:VIN262153 VSJ262123:VSJ262153 WCF262123:WCF262153 WMB262123:WMB262153 WVX262123:WVX262153 U393195:Y393225 JL327659:JL327689 TH327659:TH327689 ADD327659:ADD327689 AMZ327659:AMZ327689 AWV327659:AWV327689 BGR327659:BGR327689 BQN327659:BQN327689 CAJ327659:CAJ327689 CKF327659:CKF327689 CUB327659:CUB327689 DDX327659:DDX327689 DNT327659:DNT327689 DXP327659:DXP327689 EHL327659:EHL327689 ERH327659:ERH327689 FBD327659:FBD327689 FKZ327659:FKZ327689 FUV327659:FUV327689 GER327659:GER327689 GON327659:GON327689 GYJ327659:GYJ327689 HIF327659:HIF327689 HSB327659:HSB327689 IBX327659:IBX327689 ILT327659:ILT327689 IVP327659:IVP327689 JFL327659:JFL327689 JPH327659:JPH327689 JZD327659:JZD327689 KIZ327659:KIZ327689 KSV327659:KSV327689 LCR327659:LCR327689 LMN327659:LMN327689 LWJ327659:LWJ327689 MGF327659:MGF327689 MQB327659:MQB327689 MZX327659:MZX327689 NJT327659:NJT327689 NTP327659:NTP327689 ODL327659:ODL327689 ONH327659:ONH327689 OXD327659:OXD327689 PGZ327659:PGZ327689 PQV327659:PQV327689 QAR327659:QAR327689 QKN327659:QKN327689 QUJ327659:QUJ327689 REF327659:REF327689 ROB327659:ROB327689 RXX327659:RXX327689 SHT327659:SHT327689 SRP327659:SRP327689 TBL327659:TBL327689 TLH327659:TLH327689 TVD327659:TVD327689 UEZ327659:UEZ327689 UOV327659:UOV327689 UYR327659:UYR327689 VIN327659:VIN327689 VSJ327659:VSJ327689 WCF327659:WCF327689 WMB327659:WMB327689 WVX327659:WVX327689 U458731:Y458761 JL393195:JL393225 TH393195:TH393225 ADD393195:ADD393225 AMZ393195:AMZ393225 AWV393195:AWV393225 BGR393195:BGR393225 BQN393195:BQN393225 CAJ393195:CAJ393225 CKF393195:CKF393225 CUB393195:CUB393225 DDX393195:DDX393225 DNT393195:DNT393225 DXP393195:DXP393225 EHL393195:EHL393225 ERH393195:ERH393225 FBD393195:FBD393225 FKZ393195:FKZ393225 FUV393195:FUV393225 GER393195:GER393225 GON393195:GON393225 GYJ393195:GYJ393225 HIF393195:HIF393225 HSB393195:HSB393225 IBX393195:IBX393225 ILT393195:ILT393225 IVP393195:IVP393225 JFL393195:JFL393225 JPH393195:JPH393225 JZD393195:JZD393225 KIZ393195:KIZ393225 KSV393195:KSV393225 LCR393195:LCR393225 LMN393195:LMN393225 LWJ393195:LWJ393225 MGF393195:MGF393225 MQB393195:MQB393225 MZX393195:MZX393225 NJT393195:NJT393225 NTP393195:NTP393225 ODL393195:ODL393225 ONH393195:ONH393225 OXD393195:OXD393225 PGZ393195:PGZ393225 PQV393195:PQV393225 QAR393195:QAR393225 QKN393195:QKN393225 QUJ393195:QUJ393225 REF393195:REF393225 ROB393195:ROB393225 RXX393195:RXX393225 SHT393195:SHT393225 SRP393195:SRP393225 TBL393195:TBL393225 TLH393195:TLH393225 TVD393195:TVD393225 UEZ393195:UEZ393225 UOV393195:UOV393225 UYR393195:UYR393225 VIN393195:VIN393225 VSJ393195:VSJ393225 WCF393195:WCF393225 WMB393195:WMB393225 WVX393195:WVX393225 U524267:Y524297 JL458731:JL458761 TH458731:TH458761 ADD458731:ADD458761 AMZ458731:AMZ458761 AWV458731:AWV458761 BGR458731:BGR458761 BQN458731:BQN458761 CAJ458731:CAJ458761 CKF458731:CKF458761 CUB458731:CUB458761 DDX458731:DDX458761 DNT458731:DNT458761 DXP458731:DXP458761 EHL458731:EHL458761 ERH458731:ERH458761 FBD458731:FBD458761 FKZ458731:FKZ458761 FUV458731:FUV458761 GER458731:GER458761 GON458731:GON458761 GYJ458731:GYJ458761 HIF458731:HIF458761 HSB458731:HSB458761 IBX458731:IBX458761 ILT458731:ILT458761 IVP458731:IVP458761 JFL458731:JFL458761 JPH458731:JPH458761 JZD458731:JZD458761 KIZ458731:KIZ458761 KSV458731:KSV458761 LCR458731:LCR458761 LMN458731:LMN458761 LWJ458731:LWJ458761 MGF458731:MGF458761 MQB458731:MQB458761 MZX458731:MZX458761 NJT458731:NJT458761 NTP458731:NTP458761 ODL458731:ODL458761 ONH458731:ONH458761 OXD458731:OXD458761 PGZ458731:PGZ458761 PQV458731:PQV458761 QAR458731:QAR458761 QKN458731:QKN458761 QUJ458731:QUJ458761 REF458731:REF458761 ROB458731:ROB458761 RXX458731:RXX458761 SHT458731:SHT458761 SRP458731:SRP458761 TBL458731:TBL458761 TLH458731:TLH458761 TVD458731:TVD458761 UEZ458731:UEZ458761 UOV458731:UOV458761 UYR458731:UYR458761 VIN458731:VIN458761 VSJ458731:VSJ458761 WCF458731:WCF458761 WMB458731:WMB458761 WVX458731:WVX458761 U589803:Y589833 JL524267:JL524297 TH524267:TH524297 ADD524267:ADD524297 AMZ524267:AMZ524297 AWV524267:AWV524297 BGR524267:BGR524297 BQN524267:BQN524297 CAJ524267:CAJ524297 CKF524267:CKF524297 CUB524267:CUB524297 DDX524267:DDX524297 DNT524267:DNT524297 DXP524267:DXP524297 EHL524267:EHL524297 ERH524267:ERH524297 FBD524267:FBD524297 FKZ524267:FKZ524297 FUV524267:FUV524297 GER524267:GER524297 GON524267:GON524297 GYJ524267:GYJ524297 HIF524267:HIF524297 HSB524267:HSB524297 IBX524267:IBX524297 ILT524267:ILT524297 IVP524267:IVP524297 JFL524267:JFL524297 JPH524267:JPH524297 JZD524267:JZD524297 KIZ524267:KIZ524297 KSV524267:KSV524297 LCR524267:LCR524297 LMN524267:LMN524297 LWJ524267:LWJ524297 MGF524267:MGF524297 MQB524267:MQB524297 MZX524267:MZX524297 NJT524267:NJT524297 NTP524267:NTP524297 ODL524267:ODL524297 ONH524267:ONH524297 OXD524267:OXD524297 PGZ524267:PGZ524297 PQV524267:PQV524297 QAR524267:QAR524297 QKN524267:QKN524297 QUJ524267:QUJ524297 REF524267:REF524297 ROB524267:ROB524297 RXX524267:RXX524297 SHT524267:SHT524297 SRP524267:SRP524297 TBL524267:TBL524297 TLH524267:TLH524297 TVD524267:TVD524297 UEZ524267:UEZ524297 UOV524267:UOV524297 UYR524267:UYR524297 VIN524267:VIN524297 VSJ524267:VSJ524297 WCF524267:WCF524297 WMB524267:WMB524297 WVX524267:WVX524297 U655339:Y655369 JL589803:JL589833 TH589803:TH589833 ADD589803:ADD589833 AMZ589803:AMZ589833 AWV589803:AWV589833 BGR589803:BGR589833 BQN589803:BQN589833 CAJ589803:CAJ589833 CKF589803:CKF589833 CUB589803:CUB589833 DDX589803:DDX589833 DNT589803:DNT589833 DXP589803:DXP589833 EHL589803:EHL589833 ERH589803:ERH589833 FBD589803:FBD589833 FKZ589803:FKZ589833 FUV589803:FUV589833 GER589803:GER589833 GON589803:GON589833 GYJ589803:GYJ589833 HIF589803:HIF589833 HSB589803:HSB589833 IBX589803:IBX589833 ILT589803:ILT589833 IVP589803:IVP589833 JFL589803:JFL589833 JPH589803:JPH589833 JZD589803:JZD589833 KIZ589803:KIZ589833 KSV589803:KSV589833 LCR589803:LCR589833 LMN589803:LMN589833 LWJ589803:LWJ589833 MGF589803:MGF589833 MQB589803:MQB589833 MZX589803:MZX589833 NJT589803:NJT589833 NTP589803:NTP589833 ODL589803:ODL589833 ONH589803:ONH589833 OXD589803:OXD589833 PGZ589803:PGZ589833 PQV589803:PQV589833 QAR589803:QAR589833 QKN589803:QKN589833 QUJ589803:QUJ589833 REF589803:REF589833 ROB589803:ROB589833 RXX589803:RXX589833 SHT589803:SHT589833 SRP589803:SRP589833 TBL589803:TBL589833 TLH589803:TLH589833 TVD589803:TVD589833 UEZ589803:UEZ589833 UOV589803:UOV589833 UYR589803:UYR589833 VIN589803:VIN589833 VSJ589803:VSJ589833 WCF589803:WCF589833 WMB589803:WMB589833 WVX589803:WVX589833 U720875:Y720905 JL655339:JL655369 TH655339:TH655369 ADD655339:ADD655369 AMZ655339:AMZ655369 AWV655339:AWV655369 BGR655339:BGR655369 BQN655339:BQN655369 CAJ655339:CAJ655369 CKF655339:CKF655369 CUB655339:CUB655369 DDX655339:DDX655369 DNT655339:DNT655369 DXP655339:DXP655369 EHL655339:EHL655369 ERH655339:ERH655369 FBD655339:FBD655369 FKZ655339:FKZ655369 FUV655339:FUV655369 GER655339:GER655369 GON655339:GON655369 GYJ655339:GYJ655369 HIF655339:HIF655369 HSB655339:HSB655369 IBX655339:IBX655369 ILT655339:ILT655369 IVP655339:IVP655369 JFL655339:JFL655369 JPH655339:JPH655369 JZD655339:JZD655369 KIZ655339:KIZ655369 KSV655339:KSV655369 LCR655339:LCR655369 LMN655339:LMN655369 LWJ655339:LWJ655369 MGF655339:MGF655369 MQB655339:MQB655369 MZX655339:MZX655369 NJT655339:NJT655369 NTP655339:NTP655369 ODL655339:ODL655369 ONH655339:ONH655369 OXD655339:OXD655369 PGZ655339:PGZ655369 PQV655339:PQV655369 QAR655339:QAR655369 QKN655339:QKN655369 QUJ655339:QUJ655369 REF655339:REF655369 ROB655339:ROB655369 RXX655339:RXX655369 SHT655339:SHT655369 SRP655339:SRP655369 TBL655339:TBL655369 TLH655339:TLH655369 TVD655339:TVD655369 UEZ655339:UEZ655369 UOV655339:UOV655369 UYR655339:UYR655369 VIN655339:VIN655369 VSJ655339:VSJ655369 WCF655339:WCF655369 WMB655339:WMB655369 WVX655339:WVX655369 U786411:Y786441 JL720875:JL720905 TH720875:TH720905 ADD720875:ADD720905 AMZ720875:AMZ720905 AWV720875:AWV720905 BGR720875:BGR720905 BQN720875:BQN720905 CAJ720875:CAJ720905 CKF720875:CKF720905 CUB720875:CUB720905 DDX720875:DDX720905 DNT720875:DNT720905 DXP720875:DXP720905 EHL720875:EHL720905 ERH720875:ERH720905 FBD720875:FBD720905 FKZ720875:FKZ720905 FUV720875:FUV720905 GER720875:GER720905 GON720875:GON720905 GYJ720875:GYJ720905 HIF720875:HIF720905 HSB720875:HSB720905 IBX720875:IBX720905 ILT720875:ILT720905 IVP720875:IVP720905 JFL720875:JFL720905 JPH720875:JPH720905 JZD720875:JZD720905 KIZ720875:KIZ720905 KSV720875:KSV720905 LCR720875:LCR720905 LMN720875:LMN720905 LWJ720875:LWJ720905 MGF720875:MGF720905 MQB720875:MQB720905 MZX720875:MZX720905 NJT720875:NJT720905 NTP720875:NTP720905 ODL720875:ODL720905 ONH720875:ONH720905 OXD720875:OXD720905 PGZ720875:PGZ720905 PQV720875:PQV720905 QAR720875:QAR720905 QKN720875:QKN720905 QUJ720875:QUJ720905 REF720875:REF720905 ROB720875:ROB720905 RXX720875:RXX720905 SHT720875:SHT720905 SRP720875:SRP720905 TBL720875:TBL720905 TLH720875:TLH720905 TVD720875:TVD720905 UEZ720875:UEZ720905 UOV720875:UOV720905 UYR720875:UYR720905 VIN720875:VIN720905 VSJ720875:VSJ720905 WCF720875:WCF720905 WMB720875:WMB720905 WVX720875:WVX720905 U851947:Y851977 JL786411:JL786441 TH786411:TH786441 ADD786411:ADD786441 AMZ786411:AMZ786441 AWV786411:AWV786441 BGR786411:BGR786441 BQN786411:BQN786441 CAJ786411:CAJ786441 CKF786411:CKF786441 CUB786411:CUB786441 DDX786411:DDX786441 DNT786411:DNT786441 DXP786411:DXP786441 EHL786411:EHL786441 ERH786411:ERH786441 FBD786411:FBD786441 FKZ786411:FKZ786441 FUV786411:FUV786441 GER786411:GER786441 GON786411:GON786441 GYJ786411:GYJ786441 HIF786411:HIF786441 HSB786411:HSB786441 IBX786411:IBX786441 ILT786411:ILT786441 IVP786411:IVP786441 JFL786411:JFL786441 JPH786411:JPH786441 JZD786411:JZD786441 KIZ786411:KIZ786441 KSV786411:KSV786441 LCR786411:LCR786441 LMN786411:LMN786441 LWJ786411:LWJ786441 MGF786411:MGF786441 MQB786411:MQB786441 MZX786411:MZX786441 NJT786411:NJT786441 NTP786411:NTP786441 ODL786411:ODL786441 ONH786411:ONH786441 OXD786411:OXD786441 PGZ786411:PGZ786441 PQV786411:PQV786441 QAR786411:QAR786441 QKN786411:QKN786441 QUJ786411:QUJ786441 REF786411:REF786441 ROB786411:ROB786441 RXX786411:RXX786441 SHT786411:SHT786441 SRP786411:SRP786441 TBL786411:TBL786441 TLH786411:TLH786441 TVD786411:TVD786441 UEZ786411:UEZ786441 UOV786411:UOV786441 UYR786411:UYR786441 VIN786411:VIN786441 VSJ786411:VSJ786441 WCF786411:WCF786441 WMB786411:WMB786441 WVX786411:WVX786441 U917483:Y917513 JL851947:JL851977 TH851947:TH851977 ADD851947:ADD851977 AMZ851947:AMZ851977 AWV851947:AWV851977 BGR851947:BGR851977 BQN851947:BQN851977 CAJ851947:CAJ851977 CKF851947:CKF851977 CUB851947:CUB851977 DDX851947:DDX851977 DNT851947:DNT851977 DXP851947:DXP851977 EHL851947:EHL851977 ERH851947:ERH851977 FBD851947:FBD851977 FKZ851947:FKZ851977 FUV851947:FUV851977 GER851947:GER851977 GON851947:GON851977 GYJ851947:GYJ851977 HIF851947:HIF851977 HSB851947:HSB851977 IBX851947:IBX851977 ILT851947:ILT851977 IVP851947:IVP851977 JFL851947:JFL851977 JPH851947:JPH851977 JZD851947:JZD851977 KIZ851947:KIZ851977 KSV851947:KSV851977 LCR851947:LCR851977 LMN851947:LMN851977 LWJ851947:LWJ851977 MGF851947:MGF851977 MQB851947:MQB851977 MZX851947:MZX851977 NJT851947:NJT851977 NTP851947:NTP851977 ODL851947:ODL851977 ONH851947:ONH851977 OXD851947:OXD851977 PGZ851947:PGZ851977 PQV851947:PQV851977 QAR851947:QAR851977 QKN851947:QKN851977 QUJ851947:QUJ851977 REF851947:REF851977 ROB851947:ROB851977 RXX851947:RXX851977 SHT851947:SHT851977 SRP851947:SRP851977 TBL851947:TBL851977 TLH851947:TLH851977 TVD851947:TVD851977 UEZ851947:UEZ851977 UOV851947:UOV851977 UYR851947:UYR851977 VIN851947:VIN851977 VSJ851947:VSJ851977 WCF851947:WCF851977 WMB851947:WMB851977 WVX851947:WVX851977 U983019:Y983049 JL917483:JL917513 TH917483:TH917513 ADD917483:ADD917513 AMZ917483:AMZ917513 AWV917483:AWV917513 BGR917483:BGR917513 BQN917483:BQN917513 CAJ917483:CAJ917513 CKF917483:CKF917513 CUB917483:CUB917513 DDX917483:DDX917513 DNT917483:DNT917513 DXP917483:DXP917513 EHL917483:EHL917513 ERH917483:ERH917513 FBD917483:FBD917513 FKZ917483:FKZ917513 FUV917483:FUV917513 GER917483:GER917513 GON917483:GON917513 GYJ917483:GYJ917513 HIF917483:HIF917513 HSB917483:HSB917513 IBX917483:IBX917513 ILT917483:ILT917513 IVP917483:IVP917513 JFL917483:JFL917513 JPH917483:JPH917513 JZD917483:JZD917513 KIZ917483:KIZ917513 KSV917483:KSV917513 LCR917483:LCR917513 LMN917483:LMN917513 LWJ917483:LWJ917513 MGF917483:MGF917513 MQB917483:MQB917513 MZX917483:MZX917513 NJT917483:NJT917513 NTP917483:NTP917513 ODL917483:ODL917513 ONH917483:ONH917513 OXD917483:OXD917513 PGZ917483:PGZ917513 PQV917483:PQV917513 QAR917483:QAR917513 QKN917483:QKN917513 QUJ917483:QUJ917513 REF917483:REF917513 ROB917483:ROB917513 RXX917483:RXX917513 SHT917483:SHT917513 SRP917483:SRP917513 TBL917483:TBL917513 TLH917483:TLH917513 TVD917483:TVD917513 UEZ917483:UEZ917513 UOV917483:UOV917513 UYR917483:UYR917513 VIN917483:VIN917513 VSJ917483:VSJ917513 WCF917483:WCF917513 WMB917483:WMB917513 WVX917483:WVX917513 WVX983019:WVX983049 JL983019:JL983049 TH983019:TH983049 ADD983019:ADD983049 AMZ983019:AMZ983049 AWV983019:AWV983049 BGR983019:BGR983049 BQN983019:BQN983049 CAJ983019:CAJ983049 CKF983019:CKF983049 CUB983019:CUB983049 DDX983019:DDX983049 DNT983019:DNT983049 DXP983019:DXP983049 EHL983019:EHL983049 ERH983019:ERH983049 FBD983019:FBD983049 FKZ983019:FKZ983049 FUV983019:FUV983049 GER983019:GER983049 GON983019:GON983049 GYJ983019:GYJ983049 HIF983019:HIF983049 HSB983019:HSB983049 IBX983019:IBX983049 ILT983019:ILT983049 IVP983019:IVP983049 JFL983019:JFL983049 JPH983019:JPH983049 JZD983019:JZD983049 KIZ983019:KIZ983049 KSV983019:KSV983049 LCR983019:LCR983049 LMN983019:LMN983049 LWJ983019:LWJ983049 MGF983019:MGF983049 MQB983019:MQB983049 MZX983019:MZX983049 NJT983019:NJT983049 NTP983019:NTP983049 ODL983019:ODL983049 ONH983019:ONH983049 OXD983019:OXD983049 PGZ983019:PGZ983049 PQV983019:PQV983049 QAR983019:QAR983049 QKN983019:QKN983049 QUJ983019:QUJ983049 REF983019:REF983049 ROB983019:ROB983049 RXX983019:RXX983049 SHT983019:SHT983049 SRP983019:SRP983049 TBL983019:TBL983049 TLH983019:TLH983049 TVD983019:TVD983049 UEZ983019:UEZ983049 UOV983019:UOV983049 UYR983019:UYR983049 VIN983019:VIN983049 VSJ983019:VSJ983049 WCF983019:WCF983049 WMB983019:WMB983049 WVX4:WVX20 WMB4:WMB20 WCF4:WCF20 VSJ4:VSJ20 VIN4:VIN20 UYR4:UYR20 UOV4:UOV20 UEZ4:UEZ20 TVD4:TVD20 TLH4:TLH20 TBL4:TBL20 SRP4:SRP20 SHT4:SHT20 RXX4:RXX20 ROB4:ROB20 REF4:REF20 QUJ4:QUJ20 QKN4:QKN20 QAR4:QAR20 PQV4:PQV20 PGZ4:PGZ20 OXD4:OXD20 ONH4:ONH20 ODL4:ODL20 NTP4:NTP20 NJT4:NJT20 MZX4:MZX20 MQB4:MQB20 MGF4:MGF20 LWJ4:LWJ20 LMN4:LMN20 LCR4:LCR20 KSV4:KSV20 KIZ4:KIZ20 JZD4:JZD20 JPH4:JPH20 JFL4:JFL20 IVP4:IVP20 ILT4:ILT20 IBX4:IBX20 HSB4:HSB20 HIF4:HIF20 GYJ4:GYJ20 GON4:GON20 GER4:GER20 FUV4:FUV20 FKZ4:FKZ20 FBD4:FBD20 ERH4:ERH20 EHL4:EHL20 DXP4:DXP20 DNT4:DNT20 DDX4:DDX20 CUB4:CUB20 CKF4:CKF20 CAJ4:CAJ20 BQN4:BQN20 BGR4:BGR20 AWV4:AWV20 AMZ4:AMZ20 ADD4:ADD20 TH4:TH20 JL4:JL20" xr:uid="{00000000-0002-0000-0200-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U65515:Y65545 U131051:Y131081 JL65515:JL65545 TH65515:TH65545 ADD65515:ADD65545 AMZ65515:AMZ65545 AWV65515:AWV65545 BGR65515:BGR65545 BQN65515:BQN65545 CAJ65515:CAJ65545 CKF65515:CKF65545 CUB65515:CUB65545 DDX65515:DDX65545 DNT65515:DNT65545 DXP65515:DXP65545 EHL65515:EHL65545 ERH65515:ERH65545 FBD65515:FBD65545 FKZ65515:FKZ65545 FUV65515:FUV65545 GER65515:GER65545 GON65515:GON65545 GYJ65515:GYJ65545 HIF65515:HIF65545 HSB65515:HSB65545 IBX65515:IBX65545 ILT65515:ILT65545 IVP65515:IVP65545 JFL65515:JFL65545 JPH65515:JPH65545 JZD65515:JZD65545 KIZ65515:KIZ65545 KSV65515:KSV65545 LCR65515:LCR65545 LMN65515:LMN65545 LWJ65515:LWJ65545 MGF65515:MGF65545 MQB65515:MQB65545 MZX65515:MZX65545 NJT65515:NJT65545 NTP65515:NTP65545 ODL65515:ODL65545 ONH65515:ONH65545 OXD65515:OXD65545 PGZ65515:PGZ65545 PQV65515:PQV65545 QAR65515:QAR65545 QKN65515:QKN65545 QUJ65515:QUJ65545 REF65515:REF65545 ROB65515:ROB65545 RXX65515:RXX65545 SHT65515:SHT65545 SRP65515:SRP65545 TBL65515:TBL65545 TLH65515:TLH65545 TVD65515:TVD65545 UEZ65515:UEZ65545 UOV65515:UOV65545 UYR65515:UYR65545 VIN65515:VIN65545 VSJ65515:VSJ65545 WCF65515:WCF65545 WMB65515:WMB65545 WVX65515:WVX65545 U196587:Y196617 JL131051:JL131081 TH131051:TH131081 ADD131051:ADD131081 AMZ131051:AMZ131081 AWV131051:AWV131081 BGR131051:BGR131081 BQN131051:BQN131081 CAJ131051:CAJ131081 CKF131051:CKF131081 CUB131051:CUB131081 DDX131051:DDX131081 DNT131051:DNT131081 DXP131051:DXP131081 EHL131051:EHL131081 ERH131051:ERH131081 FBD131051:FBD131081 FKZ131051:FKZ131081 FUV131051:FUV131081 GER131051:GER131081 GON131051:GON131081 GYJ131051:GYJ131081 HIF131051:HIF131081 HSB131051:HSB131081 IBX131051:IBX131081 ILT131051:ILT131081 IVP131051:IVP131081 JFL131051:JFL131081 JPH131051:JPH131081 JZD131051:JZD131081 KIZ131051:KIZ131081 KSV131051:KSV131081 LCR131051:LCR131081 LMN131051:LMN131081 LWJ131051:LWJ131081 MGF131051:MGF131081 MQB131051:MQB131081 MZX131051:MZX131081 NJT131051:NJT131081 NTP131051:NTP131081 ODL131051:ODL131081 ONH131051:ONH131081 OXD131051:OXD131081 PGZ131051:PGZ131081 PQV131051:PQV131081 QAR131051:QAR131081 QKN131051:QKN131081 QUJ131051:QUJ131081 REF131051:REF131081 ROB131051:ROB131081 RXX131051:RXX131081 SHT131051:SHT131081 SRP131051:SRP131081 TBL131051:TBL131081 TLH131051:TLH131081 TVD131051:TVD131081 UEZ131051:UEZ131081 UOV131051:UOV131081 UYR131051:UYR131081 VIN131051:VIN131081 VSJ131051:VSJ131081 WCF131051:WCF131081 WMB131051:WMB131081 WVX131051:WVX131081 U262123:Y262153 JL196587:JL196617 TH196587:TH196617 ADD196587:ADD196617 AMZ196587:AMZ196617 AWV196587:AWV196617 BGR196587:BGR196617 BQN196587:BQN196617 CAJ196587:CAJ196617 CKF196587:CKF196617 CUB196587:CUB196617 DDX196587:DDX196617 DNT196587:DNT196617 DXP196587:DXP196617 EHL196587:EHL196617 ERH196587:ERH196617 FBD196587:FBD196617 FKZ196587:FKZ196617 FUV196587:FUV196617 GER196587:GER196617 GON196587:GON196617 GYJ196587:GYJ196617 HIF196587:HIF196617 HSB196587:HSB196617 IBX196587:IBX196617 ILT196587:ILT196617 IVP196587:IVP196617 JFL196587:JFL196617 JPH196587:JPH196617 JZD196587:JZD196617 KIZ196587:KIZ196617 KSV196587:KSV196617 LCR196587:LCR196617 LMN196587:LMN196617 LWJ196587:LWJ196617 MGF196587:MGF196617 MQB196587:MQB196617 MZX196587:MZX196617 NJT196587:NJT196617 NTP196587:NTP196617 ODL196587:ODL196617 ONH196587:ONH196617 OXD196587:OXD196617 PGZ196587:PGZ196617 PQV196587:PQV196617 QAR196587:QAR196617 QKN196587:QKN196617 QUJ196587:QUJ196617 REF196587:REF196617 ROB196587:ROB196617 RXX196587:RXX196617 SHT196587:SHT196617 SRP196587:SRP196617 TBL196587:TBL196617 TLH196587:TLH196617 TVD196587:TVD196617 UEZ196587:UEZ196617 UOV196587:UOV196617 UYR196587:UYR196617 VIN196587:VIN196617 VSJ196587:VSJ196617 WCF196587:WCF196617 WMB196587:WMB196617 WVX196587:WVX196617 U327659:Y327689 JL262123:JL262153 TH262123:TH262153 ADD262123:ADD262153 AMZ262123:AMZ262153 AWV262123:AWV262153 BGR262123:BGR262153 BQN262123:BQN262153 CAJ262123:CAJ262153 CKF262123:CKF262153 CUB262123:CUB262153 DDX262123:DDX262153 DNT262123:DNT262153 DXP262123:DXP262153 EHL262123:EHL262153 ERH262123:ERH262153 FBD262123:FBD262153 FKZ262123:FKZ262153 FUV262123:FUV262153 GER262123:GER262153 GON262123:GON262153 GYJ262123:GYJ262153 HIF262123:HIF262153 HSB262123:HSB262153 IBX262123:IBX262153 ILT262123:ILT262153 IVP262123:IVP262153 JFL262123:JFL262153 JPH262123:JPH262153 JZD262123:JZD262153 KIZ262123:KIZ262153 KSV262123:KSV262153 LCR262123:LCR262153 LMN262123:LMN262153 LWJ262123:LWJ262153 MGF262123:MGF262153 MQB262123:MQB262153 MZX262123:MZX262153 NJT262123:NJT262153 NTP262123:NTP262153 ODL262123:ODL262153 ONH262123:ONH262153 OXD262123:OXD262153 PGZ262123:PGZ262153 PQV262123:PQV262153 QAR262123:QAR262153 QKN262123:QKN262153 QUJ262123:QUJ262153 REF262123:REF262153 ROB262123:ROB262153 RXX262123:RXX262153 SHT262123:SHT262153 SRP262123:SRP262153 TBL262123:TBL262153 TLH262123:TLH262153 TVD262123:TVD262153 UEZ262123:UEZ262153 UOV262123:UOV262153 UYR262123:UYR262153 VIN262123:VIN262153 VSJ262123:VSJ262153 WCF262123:WCF262153 WMB262123:WMB262153 WVX262123:WVX262153 U393195:Y393225 JL327659:JL327689 TH327659:TH327689 ADD327659:ADD327689 AMZ327659:AMZ327689 AWV327659:AWV327689 BGR327659:BGR327689 BQN327659:BQN327689 CAJ327659:CAJ327689 CKF327659:CKF327689 CUB327659:CUB327689 DDX327659:DDX327689 DNT327659:DNT327689 DXP327659:DXP327689 EHL327659:EHL327689 ERH327659:ERH327689 FBD327659:FBD327689 FKZ327659:FKZ327689 FUV327659:FUV327689 GER327659:GER327689 GON327659:GON327689 GYJ327659:GYJ327689 HIF327659:HIF327689 HSB327659:HSB327689 IBX327659:IBX327689 ILT327659:ILT327689 IVP327659:IVP327689 JFL327659:JFL327689 JPH327659:JPH327689 JZD327659:JZD327689 KIZ327659:KIZ327689 KSV327659:KSV327689 LCR327659:LCR327689 LMN327659:LMN327689 LWJ327659:LWJ327689 MGF327659:MGF327689 MQB327659:MQB327689 MZX327659:MZX327689 NJT327659:NJT327689 NTP327659:NTP327689 ODL327659:ODL327689 ONH327659:ONH327689 OXD327659:OXD327689 PGZ327659:PGZ327689 PQV327659:PQV327689 QAR327659:QAR327689 QKN327659:QKN327689 QUJ327659:QUJ327689 REF327659:REF327689 ROB327659:ROB327689 RXX327659:RXX327689 SHT327659:SHT327689 SRP327659:SRP327689 TBL327659:TBL327689 TLH327659:TLH327689 TVD327659:TVD327689 UEZ327659:UEZ327689 UOV327659:UOV327689 UYR327659:UYR327689 VIN327659:VIN327689 VSJ327659:VSJ327689 WCF327659:WCF327689 WMB327659:WMB327689 WVX327659:WVX327689 U458731:Y458761 JL393195:JL393225 TH393195:TH393225 ADD393195:ADD393225 AMZ393195:AMZ393225 AWV393195:AWV393225 BGR393195:BGR393225 BQN393195:BQN393225 CAJ393195:CAJ393225 CKF393195:CKF393225 CUB393195:CUB393225 DDX393195:DDX393225 DNT393195:DNT393225 DXP393195:DXP393225 EHL393195:EHL393225 ERH393195:ERH393225 FBD393195:FBD393225 FKZ393195:FKZ393225 FUV393195:FUV393225 GER393195:GER393225 GON393195:GON393225 GYJ393195:GYJ393225 HIF393195:HIF393225 HSB393195:HSB393225 IBX393195:IBX393225 ILT393195:ILT393225 IVP393195:IVP393225 JFL393195:JFL393225 JPH393195:JPH393225 JZD393195:JZD393225 KIZ393195:KIZ393225 KSV393195:KSV393225 LCR393195:LCR393225 LMN393195:LMN393225 LWJ393195:LWJ393225 MGF393195:MGF393225 MQB393195:MQB393225 MZX393195:MZX393225 NJT393195:NJT393225 NTP393195:NTP393225 ODL393195:ODL393225 ONH393195:ONH393225 OXD393195:OXD393225 PGZ393195:PGZ393225 PQV393195:PQV393225 QAR393195:QAR393225 QKN393195:QKN393225 QUJ393195:QUJ393225 REF393195:REF393225 ROB393195:ROB393225 RXX393195:RXX393225 SHT393195:SHT393225 SRP393195:SRP393225 TBL393195:TBL393225 TLH393195:TLH393225 TVD393195:TVD393225 UEZ393195:UEZ393225 UOV393195:UOV393225 UYR393195:UYR393225 VIN393195:VIN393225 VSJ393195:VSJ393225 WCF393195:WCF393225 WMB393195:WMB393225 WVX393195:WVX393225 U524267:Y524297 JL458731:JL458761 TH458731:TH458761 ADD458731:ADD458761 AMZ458731:AMZ458761 AWV458731:AWV458761 BGR458731:BGR458761 BQN458731:BQN458761 CAJ458731:CAJ458761 CKF458731:CKF458761 CUB458731:CUB458761 DDX458731:DDX458761 DNT458731:DNT458761 DXP458731:DXP458761 EHL458731:EHL458761 ERH458731:ERH458761 FBD458731:FBD458761 FKZ458731:FKZ458761 FUV458731:FUV458761 GER458731:GER458761 GON458731:GON458761 GYJ458731:GYJ458761 HIF458731:HIF458761 HSB458731:HSB458761 IBX458731:IBX458761 ILT458731:ILT458761 IVP458731:IVP458761 JFL458731:JFL458761 JPH458731:JPH458761 JZD458731:JZD458761 KIZ458731:KIZ458761 KSV458731:KSV458761 LCR458731:LCR458761 LMN458731:LMN458761 LWJ458731:LWJ458761 MGF458731:MGF458761 MQB458731:MQB458761 MZX458731:MZX458761 NJT458731:NJT458761 NTP458731:NTP458761 ODL458731:ODL458761 ONH458731:ONH458761 OXD458731:OXD458761 PGZ458731:PGZ458761 PQV458731:PQV458761 QAR458731:QAR458761 QKN458731:QKN458761 QUJ458731:QUJ458761 REF458731:REF458761 ROB458731:ROB458761 RXX458731:RXX458761 SHT458731:SHT458761 SRP458731:SRP458761 TBL458731:TBL458761 TLH458731:TLH458761 TVD458731:TVD458761 UEZ458731:UEZ458761 UOV458731:UOV458761 UYR458731:UYR458761 VIN458731:VIN458761 VSJ458731:VSJ458761 WCF458731:WCF458761 WMB458731:WMB458761 WVX458731:WVX458761 U589803:Y589833 JL524267:JL524297 TH524267:TH524297 ADD524267:ADD524297 AMZ524267:AMZ524297 AWV524267:AWV524297 BGR524267:BGR524297 BQN524267:BQN524297 CAJ524267:CAJ524297 CKF524267:CKF524297 CUB524267:CUB524297 DDX524267:DDX524297 DNT524267:DNT524297 DXP524267:DXP524297 EHL524267:EHL524297 ERH524267:ERH524297 FBD524267:FBD524297 FKZ524267:FKZ524297 FUV524267:FUV524297 GER524267:GER524297 GON524267:GON524297 GYJ524267:GYJ524297 HIF524267:HIF524297 HSB524267:HSB524297 IBX524267:IBX524297 ILT524267:ILT524297 IVP524267:IVP524297 JFL524267:JFL524297 JPH524267:JPH524297 JZD524267:JZD524297 KIZ524267:KIZ524297 KSV524267:KSV524297 LCR524267:LCR524297 LMN524267:LMN524297 LWJ524267:LWJ524297 MGF524267:MGF524297 MQB524267:MQB524297 MZX524267:MZX524297 NJT524267:NJT524297 NTP524267:NTP524297 ODL524267:ODL524297 ONH524267:ONH524297 OXD524267:OXD524297 PGZ524267:PGZ524297 PQV524267:PQV524297 QAR524267:QAR524297 QKN524267:QKN524297 QUJ524267:QUJ524297 REF524267:REF524297 ROB524267:ROB524297 RXX524267:RXX524297 SHT524267:SHT524297 SRP524267:SRP524297 TBL524267:TBL524297 TLH524267:TLH524297 TVD524267:TVD524297 UEZ524267:UEZ524297 UOV524267:UOV524297 UYR524267:UYR524297 VIN524267:VIN524297 VSJ524267:VSJ524297 WCF524267:WCF524297 WMB524267:WMB524297 WVX524267:WVX524297 U655339:Y655369 JL589803:JL589833 TH589803:TH589833 ADD589803:ADD589833 AMZ589803:AMZ589833 AWV589803:AWV589833 BGR589803:BGR589833 BQN589803:BQN589833 CAJ589803:CAJ589833 CKF589803:CKF589833 CUB589803:CUB589833 DDX589803:DDX589833 DNT589803:DNT589833 DXP589803:DXP589833 EHL589803:EHL589833 ERH589803:ERH589833 FBD589803:FBD589833 FKZ589803:FKZ589833 FUV589803:FUV589833 GER589803:GER589833 GON589803:GON589833 GYJ589803:GYJ589833 HIF589803:HIF589833 HSB589803:HSB589833 IBX589803:IBX589833 ILT589803:ILT589833 IVP589803:IVP589833 JFL589803:JFL589833 JPH589803:JPH589833 JZD589803:JZD589833 KIZ589803:KIZ589833 KSV589803:KSV589833 LCR589803:LCR589833 LMN589803:LMN589833 LWJ589803:LWJ589833 MGF589803:MGF589833 MQB589803:MQB589833 MZX589803:MZX589833 NJT589803:NJT589833 NTP589803:NTP589833 ODL589803:ODL589833 ONH589803:ONH589833 OXD589803:OXD589833 PGZ589803:PGZ589833 PQV589803:PQV589833 QAR589803:QAR589833 QKN589803:QKN589833 QUJ589803:QUJ589833 REF589803:REF589833 ROB589803:ROB589833 RXX589803:RXX589833 SHT589803:SHT589833 SRP589803:SRP589833 TBL589803:TBL589833 TLH589803:TLH589833 TVD589803:TVD589833 UEZ589803:UEZ589833 UOV589803:UOV589833 UYR589803:UYR589833 VIN589803:VIN589833 VSJ589803:VSJ589833 WCF589803:WCF589833 WMB589803:WMB589833 WVX589803:WVX589833 U720875:Y720905 JL655339:JL655369 TH655339:TH655369 ADD655339:ADD655369 AMZ655339:AMZ655369 AWV655339:AWV655369 BGR655339:BGR655369 BQN655339:BQN655369 CAJ655339:CAJ655369 CKF655339:CKF655369 CUB655339:CUB655369 DDX655339:DDX655369 DNT655339:DNT655369 DXP655339:DXP655369 EHL655339:EHL655369 ERH655339:ERH655369 FBD655339:FBD655369 FKZ655339:FKZ655369 FUV655339:FUV655369 GER655339:GER655369 GON655339:GON655369 GYJ655339:GYJ655369 HIF655339:HIF655369 HSB655339:HSB655369 IBX655339:IBX655369 ILT655339:ILT655369 IVP655339:IVP655369 JFL655339:JFL655369 JPH655339:JPH655369 JZD655339:JZD655369 KIZ655339:KIZ655369 KSV655339:KSV655369 LCR655339:LCR655369 LMN655339:LMN655369 LWJ655339:LWJ655369 MGF655339:MGF655369 MQB655339:MQB655369 MZX655339:MZX655369 NJT655339:NJT655369 NTP655339:NTP655369 ODL655339:ODL655369 ONH655339:ONH655369 OXD655339:OXD655369 PGZ655339:PGZ655369 PQV655339:PQV655369 QAR655339:QAR655369 QKN655339:QKN655369 QUJ655339:QUJ655369 REF655339:REF655369 ROB655339:ROB655369 RXX655339:RXX655369 SHT655339:SHT655369 SRP655339:SRP655369 TBL655339:TBL655369 TLH655339:TLH655369 TVD655339:TVD655369 UEZ655339:UEZ655369 UOV655339:UOV655369 UYR655339:UYR655369 VIN655339:VIN655369 VSJ655339:VSJ655369 WCF655339:WCF655369 WMB655339:WMB655369 WVX655339:WVX655369 U786411:Y786441 JL720875:JL720905 TH720875:TH720905 ADD720875:ADD720905 AMZ720875:AMZ720905 AWV720875:AWV720905 BGR720875:BGR720905 BQN720875:BQN720905 CAJ720875:CAJ720905 CKF720875:CKF720905 CUB720875:CUB720905 DDX720875:DDX720905 DNT720875:DNT720905 DXP720875:DXP720905 EHL720875:EHL720905 ERH720875:ERH720905 FBD720875:FBD720905 FKZ720875:FKZ720905 FUV720875:FUV720905 GER720875:GER720905 GON720875:GON720905 GYJ720875:GYJ720905 HIF720875:HIF720905 HSB720875:HSB720905 IBX720875:IBX720905 ILT720875:ILT720905 IVP720875:IVP720905 JFL720875:JFL720905 JPH720875:JPH720905 JZD720875:JZD720905 KIZ720875:KIZ720905 KSV720875:KSV720905 LCR720875:LCR720905 LMN720875:LMN720905 LWJ720875:LWJ720905 MGF720875:MGF720905 MQB720875:MQB720905 MZX720875:MZX720905 NJT720875:NJT720905 NTP720875:NTP720905 ODL720875:ODL720905 ONH720875:ONH720905 OXD720875:OXD720905 PGZ720875:PGZ720905 PQV720875:PQV720905 QAR720875:QAR720905 QKN720875:QKN720905 QUJ720875:QUJ720905 REF720875:REF720905 ROB720875:ROB720905 RXX720875:RXX720905 SHT720875:SHT720905 SRP720875:SRP720905 TBL720875:TBL720905 TLH720875:TLH720905 TVD720875:TVD720905 UEZ720875:UEZ720905 UOV720875:UOV720905 UYR720875:UYR720905 VIN720875:VIN720905 VSJ720875:VSJ720905 WCF720875:WCF720905 WMB720875:WMB720905 WVX720875:WVX720905 U851947:Y851977 JL786411:JL786441 TH786411:TH786441 ADD786411:ADD786441 AMZ786411:AMZ786441 AWV786411:AWV786441 BGR786411:BGR786441 BQN786411:BQN786441 CAJ786411:CAJ786441 CKF786411:CKF786441 CUB786411:CUB786441 DDX786411:DDX786441 DNT786411:DNT786441 DXP786411:DXP786441 EHL786411:EHL786441 ERH786411:ERH786441 FBD786411:FBD786441 FKZ786411:FKZ786441 FUV786411:FUV786441 GER786411:GER786441 GON786411:GON786441 GYJ786411:GYJ786441 HIF786411:HIF786441 HSB786411:HSB786441 IBX786411:IBX786441 ILT786411:ILT786441 IVP786411:IVP786441 JFL786411:JFL786441 JPH786411:JPH786441 JZD786411:JZD786441 KIZ786411:KIZ786441 KSV786411:KSV786441 LCR786411:LCR786441 LMN786411:LMN786441 LWJ786411:LWJ786441 MGF786411:MGF786441 MQB786411:MQB786441 MZX786411:MZX786441 NJT786411:NJT786441 NTP786411:NTP786441 ODL786411:ODL786441 ONH786411:ONH786441 OXD786411:OXD786441 PGZ786411:PGZ786441 PQV786411:PQV786441 QAR786411:QAR786441 QKN786411:QKN786441 QUJ786411:QUJ786441 REF786411:REF786441 ROB786411:ROB786441 RXX786411:RXX786441 SHT786411:SHT786441 SRP786411:SRP786441 TBL786411:TBL786441 TLH786411:TLH786441 TVD786411:TVD786441 UEZ786411:UEZ786441 UOV786411:UOV786441 UYR786411:UYR786441 VIN786411:VIN786441 VSJ786411:VSJ786441 WCF786411:WCF786441 WMB786411:WMB786441 WVX786411:WVX786441 U917483:Y917513 JL851947:JL851977 TH851947:TH851977 ADD851947:ADD851977 AMZ851947:AMZ851977 AWV851947:AWV851977 BGR851947:BGR851977 BQN851947:BQN851977 CAJ851947:CAJ851977 CKF851947:CKF851977 CUB851947:CUB851977 DDX851947:DDX851977 DNT851947:DNT851977 DXP851947:DXP851977 EHL851947:EHL851977 ERH851947:ERH851977 FBD851947:FBD851977 FKZ851947:FKZ851977 FUV851947:FUV851977 GER851947:GER851977 GON851947:GON851977 GYJ851947:GYJ851977 HIF851947:HIF851977 HSB851947:HSB851977 IBX851947:IBX851977 ILT851947:ILT851977 IVP851947:IVP851977 JFL851947:JFL851977 JPH851947:JPH851977 JZD851947:JZD851977 KIZ851947:KIZ851977 KSV851947:KSV851977 LCR851947:LCR851977 LMN851947:LMN851977 LWJ851947:LWJ851977 MGF851947:MGF851977 MQB851947:MQB851977 MZX851947:MZX851977 NJT851947:NJT851977 NTP851947:NTP851977 ODL851947:ODL851977 ONH851947:ONH851977 OXD851947:OXD851977 PGZ851947:PGZ851977 PQV851947:PQV851977 QAR851947:QAR851977 QKN851947:QKN851977 QUJ851947:QUJ851977 REF851947:REF851977 ROB851947:ROB851977 RXX851947:RXX851977 SHT851947:SHT851977 SRP851947:SRP851977 TBL851947:TBL851977 TLH851947:TLH851977 TVD851947:TVD851977 UEZ851947:UEZ851977 UOV851947:UOV851977 UYR851947:UYR851977 VIN851947:VIN851977 VSJ851947:VSJ851977 WCF851947:WCF851977 WMB851947:WMB851977 WVX851947:WVX851977 U983019:Y983049 JL917483:JL917513 TH917483:TH917513 ADD917483:ADD917513 AMZ917483:AMZ917513 AWV917483:AWV917513 BGR917483:BGR917513 BQN917483:BQN917513 CAJ917483:CAJ917513 CKF917483:CKF917513 CUB917483:CUB917513 DDX917483:DDX917513 DNT917483:DNT917513 DXP917483:DXP917513 EHL917483:EHL917513 ERH917483:ERH917513 FBD917483:FBD917513 FKZ917483:FKZ917513 FUV917483:FUV917513 GER917483:GER917513 GON917483:GON917513 GYJ917483:GYJ917513 HIF917483:HIF917513 HSB917483:HSB917513 IBX917483:IBX917513 ILT917483:ILT917513 IVP917483:IVP917513 JFL917483:JFL917513 JPH917483:JPH917513 JZD917483:JZD917513 KIZ917483:KIZ917513 KSV917483:KSV917513 LCR917483:LCR917513 LMN917483:LMN917513 LWJ917483:LWJ917513 MGF917483:MGF917513 MQB917483:MQB917513 MZX917483:MZX917513 NJT917483:NJT917513 NTP917483:NTP917513 ODL917483:ODL917513 ONH917483:ONH917513 OXD917483:OXD917513 PGZ917483:PGZ917513 PQV917483:PQV917513 QAR917483:QAR917513 QKN917483:QKN917513 QUJ917483:QUJ917513 REF917483:REF917513 ROB917483:ROB917513 RXX917483:RXX917513 SHT917483:SHT917513 SRP917483:SRP917513 TBL917483:TBL917513 TLH917483:TLH917513 TVD917483:TVD917513 UEZ917483:UEZ917513 UOV917483:UOV917513 UYR917483:UYR917513 VIN917483:VIN917513 VSJ917483:VSJ917513 WCF917483:WCF917513 WMB917483:WMB917513 WVX917483:WVX917513 WVX983019:WVX983049 JL983019:JL983049 TH983019:TH983049 ADD983019:ADD983049 AMZ983019:AMZ983049 AWV983019:AWV983049 BGR983019:BGR983049 BQN983019:BQN983049 CAJ983019:CAJ983049 CKF983019:CKF983049 CUB983019:CUB983049 DDX983019:DDX983049 DNT983019:DNT983049 DXP983019:DXP983049 EHL983019:EHL983049 ERH983019:ERH983049 FBD983019:FBD983049 FKZ983019:FKZ983049 FUV983019:FUV983049 GER983019:GER983049 GON983019:GON983049 GYJ983019:GYJ983049 HIF983019:HIF983049 HSB983019:HSB983049 IBX983019:IBX983049 ILT983019:ILT983049 IVP983019:IVP983049 JFL983019:JFL983049 JPH983019:JPH983049 JZD983019:JZD983049 KIZ983019:KIZ983049 KSV983019:KSV983049 LCR983019:LCR983049 LMN983019:LMN983049 LWJ983019:LWJ983049 MGF983019:MGF983049 MQB983019:MQB983049 MZX983019:MZX983049 NJT983019:NJT983049 NTP983019:NTP983049 ODL983019:ODL983049 ONH983019:ONH983049 OXD983019:OXD983049 PGZ983019:PGZ983049 PQV983019:PQV983049 QAR983019:QAR983049 QKN983019:QKN983049 QUJ983019:QUJ983049 REF983019:REF983049 ROB983019:ROB983049 RXX983019:RXX983049 SHT983019:SHT983049 SRP983019:SRP983049 TBL983019:TBL983049 TLH983019:TLH983049 TVD983019:TVD983049 UEZ983019:UEZ983049 UOV983019:UOV983049 UYR983019:UYR983049 VIN983019:VIN983049 VSJ983019:VSJ983049 WCF983019:WCF983049 WMB983019:WMB983049 JL4:JL20 TH4:TH20 ADD4:ADD20 AMZ4:AMZ20 AWV4:AWV20 BGR4:BGR20 BQN4:BQN20 CAJ4:CAJ20 CKF4:CKF20 CUB4:CUB20 DDX4:DDX20 DNT4:DNT20 DXP4:DXP20 EHL4:EHL20 ERH4:ERH20 FBD4:FBD20 FKZ4:FKZ20 FUV4:FUV20 GER4:GER20 GON4:GON20 GYJ4:GYJ20 HIF4:HIF20 HSB4:HSB20 IBX4:IBX20 ILT4:ILT20 IVP4:IVP20 JFL4:JFL20 JPH4:JPH20 JZD4:JZD20 KIZ4:KIZ20 KSV4:KSV20 LCR4:LCR20 LMN4:LMN20 LWJ4:LWJ20 MGF4:MGF20 MQB4:MQB20 MZX4:MZX20 NJT4:NJT20 NTP4:NTP20 ODL4:ODL20 ONH4:ONH20 OXD4:OXD20 PGZ4:PGZ20 PQV4:PQV20 QAR4:QAR20 QKN4:QKN20 QUJ4:QUJ20 REF4:REF20 ROB4:ROB20 RXX4:RXX20 SHT4:SHT20 SRP4:SRP20 TBL4:TBL20 TLH4:TLH20 TVD4:TVD20 UEZ4:UEZ20 UOV4:UOV20 UYR4:UYR20 VIN4:VIN20 VSJ4:VSJ20 WCF4:WCF20 WMB4:WMB20 WVX4:WVX20" xr:uid="{00000000-0002-0000-0200-00000B000000}">
       <formula1>"1, 2, 3, 4, 5, 6"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JI65515:JI65545 TE65515:TE65545 ADA65515:ADA65545 AMW65515:AMW65545 AWS65515:AWS65545 BGO65515:BGO65545 BQK65515:BQK65545 CAG65515:CAG65545 CKC65515:CKC65545 CTY65515:CTY65545 DDU65515:DDU65545 DNQ65515:DNQ65545 DXM65515:DXM65545 EHI65515:EHI65545 ERE65515:ERE65545 FBA65515:FBA65545 FKW65515:FKW65545 FUS65515:FUS65545 GEO65515:GEO65545 GOK65515:GOK65545 GYG65515:GYG65545 HIC65515:HIC65545 HRY65515:HRY65545 IBU65515:IBU65545 ILQ65515:ILQ65545 IVM65515:IVM65545 JFI65515:JFI65545 JPE65515:JPE65545 JZA65515:JZA65545 KIW65515:KIW65545 KSS65515:KSS65545 LCO65515:LCO65545 LMK65515:LMK65545 LWG65515:LWG65545 MGC65515:MGC65545 MPY65515:MPY65545 MZU65515:MZU65545 NJQ65515:NJQ65545 NTM65515:NTM65545 ODI65515:ODI65545 ONE65515:ONE65545 OXA65515:OXA65545 PGW65515:PGW65545 PQS65515:PQS65545 QAO65515:QAO65545 QKK65515:QKK65545 QUG65515:QUG65545 REC65515:REC65545 RNY65515:RNY65545 RXU65515:RXU65545 SHQ65515:SHQ65545 SRM65515:SRM65545 TBI65515:TBI65545 TLE65515:TLE65545 TVA65515:TVA65545 UEW65515:UEW65545 UOS65515:UOS65545 UYO65515:UYO65545 VIK65515:VIK65545 VSG65515:VSG65545 WCC65515:WCC65545 WLY65515:WLY65545 WVU65515:WVU65545 JI131051:JI131081 TE131051:TE131081 ADA131051:ADA131081 AMW131051:AMW131081 AWS131051:AWS131081 BGO131051:BGO131081 BQK131051:BQK131081 CAG131051:CAG131081 CKC131051:CKC131081 CTY131051:CTY131081 DDU131051:DDU131081 DNQ131051:DNQ131081 DXM131051:DXM131081 EHI131051:EHI131081 ERE131051:ERE131081 FBA131051:FBA131081 FKW131051:FKW131081 FUS131051:FUS131081 GEO131051:GEO131081 GOK131051:GOK131081 GYG131051:GYG131081 HIC131051:HIC131081 HRY131051:HRY131081 IBU131051:IBU131081 ILQ131051:ILQ131081 IVM131051:IVM131081 JFI131051:JFI131081 JPE131051:JPE131081 JZA131051:JZA131081 KIW131051:KIW131081 KSS131051:KSS131081 LCO131051:LCO131081 LMK131051:LMK131081 LWG131051:LWG131081 MGC131051:MGC131081 MPY131051:MPY131081 MZU131051:MZU131081 NJQ131051:NJQ131081 NTM131051:NTM131081 ODI131051:ODI131081 ONE131051:ONE131081 OXA131051:OXA131081 PGW131051:PGW131081 PQS131051:PQS131081 QAO131051:QAO131081 QKK131051:QKK131081 QUG131051:QUG131081 REC131051:REC131081 RNY131051:RNY131081 RXU131051:RXU131081 SHQ131051:SHQ131081 SRM131051:SRM131081 TBI131051:TBI131081 TLE131051:TLE131081 TVA131051:TVA131081 UEW131051:UEW131081 UOS131051:UOS131081 UYO131051:UYO131081 VIK131051:VIK131081 VSG131051:VSG131081 WCC131051:WCC131081 WLY131051:WLY131081 WVU131051:WVU131081 JI196587:JI196617 TE196587:TE196617 ADA196587:ADA196617 AMW196587:AMW196617 AWS196587:AWS196617 BGO196587:BGO196617 BQK196587:BQK196617 CAG196587:CAG196617 CKC196587:CKC196617 CTY196587:CTY196617 DDU196587:DDU196617 DNQ196587:DNQ196617 DXM196587:DXM196617 EHI196587:EHI196617 ERE196587:ERE196617 FBA196587:FBA196617 FKW196587:FKW196617 FUS196587:FUS196617 GEO196587:GEO196617 GOK196587:GOK196617 GYG196587:GYG196617 HIC196587:HIC196617 HRY196587:HRY196617 IBU196587:IBU196617 ILQ196587:ILQ196617 IVM196587:IVM196617 JFI196587:JFI196617 JPE196587:JPE196617 JZA196587:JZA196617 KIW196587:KIW196617 KSS196587:KSS196617 LCO196587:LCO196617 LMK196587:LMK196617 LWG196587:LWG196617 MGC196587:MGC196617 MPY196587:MPY196617 MZU196587:MZU196617 NJQ196587:NJQ196617 NTM196587:NTM196617 ODI196587:ODI196617 ONE196587:ONE196617 OXA196587:OXA196617 PGW196587:PGW196617 PQS196587:PQS196617 QAO196587:QAO196617 QKK196587:QKK196617 QUG196587:QUG196617 REC196587:REC196617 RNY196587:RNY196617 RXU196587:RXU196617 SHQ196587:SHQ196617 SRM196587:SRM196617 TBI196587:TBI196617 TLE196587:TLE196617 TVA196587:TVA196617 UEW196587:UEW196617 UOS196587:UOS196617 UYO196587:UYO196617 VIK196587:VIK196617 VSG196587:VSG196617 WCC196587:WCC196617 WLY196587:WLY196617 WVU196587:WVU196617 JI262123:JI262153 TE262123:TE262153 ADA262123:ADA262153 AMW262123:AMW262153 AWS262123:AWS262153 BGO262123:BGO262153 BQK262123:BQK262153 CAG262123:CAG262153 CKC262123:CKC262153 CTY262123:CTY262153 DDU262123:DDU262153 DNQ262123:DNQ262153 DXM262123:DXM262153 EHI262123:EHI262153 ERE262123:ERE262153 FBA262123:FBA262153 FKW262123:FKW262153 FUS262123:FUS262153 GEO262123:GEO262153 GOK262123:GOK262153 GYG262123:GYG262153 HIC262123:HIC262153 HRY262123:HRY262153 IBU262123:IBU262153 ILQ262123:ILQ262153 IVM262123:IVM262153 JFI262123:JFI262153 JPE262123:JPE262153 JZA262123:JZA262153 KIW262123:KIW262153 KSS262123:KSS262153 LCO262123:LCO262153 LMK262123:LMK262153 LWG262123:LWG262153 MGC262123:MGC262153 MPY262123:MPY262153 MZU262123:MZU262153 NJQ262123:NJQ262153 NTM262123:NTM262153 ODI262123:ODI262153 ONE262123:ONE262153 OXA262123:OXA262153 PGW262123:PGW262153 PQS262123:PQS262153 QAO262123:QAO262153 QKK262123:QKK262153 QUG262123:QUG262153 REC262123:REC262153 RNY262123:RNY262153 RXU262123:RXU262153 SHQ262123:SHQ262153 SRM262123:SRM262153 TBI262123:TBI262153 TLE262123:TLE262153 TVA262123:TVA262153 UEW262123:UEW262153 UOS262123:UOS262153 UYO262123:UYO262153 VIK262123:VIK262153 VSG262123:VSG262153 WCC262123:WCC262153 WLY262123:WLY262153 WVU262123:WVU262153 JI327659:JI327689 TE327659:TE327689 ADA327659:ADA327689 AMW327659:AMW327689 AWS327659:AWS327689 BGO327659:BGO327689 BQK327659:BQK327689 CAG327659:CAG327689 CKC327659:CKC327689 CTY327659:CTY327689 DDU327659:DDU327689 DNQ327659:DNQ327689 DXM327659:DXM327689 EHI327659:EHI327689 ERE327659:ERE327689 FBA327659:FBA327689 FKW327659:FKW327689 FUS327659:FUS327689 GEO327659:GEO327689 GOK327659:GOK327689 GYG327659:GYG327689 HIC327659:HIC327689 HRY327659:HRY327689 IBU327659:IBU327689 ILQ327659:ILQ327689 IVM327659:IVM327689 JFI327659:JFI327689 JPE327659:JPE327689 JZA327659:JZA327689 KIW327659:KIW327689 KSS327659:KSS327689 LCO327659:LCO327689 LMK327659:LMK327689 LWG327659:LWG327689 MGC327659:MGC327689 MPY327659:MPY327689 MZU327659:MZU327689 NJQ327659:NJQ327689 NTM327659:NTM327689 ODI327659:ODI327689 ONE327659:ONE327689 OXA327659:OXA327689 PGW327659:PGW327689 PQS327659:PQS327689 QAO327659:QAO327689 QKK327659:QKK327689 QUG327659:QUG327689 REC327659:REC327689 RNY327659:RNY327689 RXU327659:RXU327689 SHQ327659:SHQ327689 SRM327659:SRM327689 TBI327659:TBI327689 TLE327659:TLE327689 TVA327659:TVA327689 UEW327659:UEW327689 UOS327659:UOS327689 UYO327659:UYO327689 VIK327659:VIK327689 VSG327659:VSG327689 WCC327659:WCC327689 WLY327659:WLY327689 WVU327659:WVU327689 JI393195:JI393225 TE393195:TE393225 ADA393195:ADA393225 AMW393195:AMW393225 AWS393195:AWS393225 BGO393195:BGO393225 BQK393195:BQK393225 CAG393195:CAG393225 CKC393195:CKC393225 CTY393195:CTY393225 DDU393195:DDU393225 DNQ393195:DNQ393225 DXM393195:DXM393225 EHI393195:EHI393225 ERE393195:ERE393225 FBA393195:FBA393225 FKW393195:FKW393225 FUS393195:FUS393225 GEO393195:GEO393225 GOK393195:GOK393225 GYG393195:GYG393225 HIC393195:HIC393225 HRY393195:HRY393225 IBU393195:IBU393225 ILQ393195:ILQ393225 IVM393195:IVM393225 JFI393195:JFI393225 JPE393195:JPE393225 JZA393195:JZA393225 KIW393195:KIW393225 KSS393195:KSS393225 LCO393195:LCO393225 LMK393195:LMK393225 LWG393195:LWG393225 MGC393195:MGC393225 MPY393195:MPY393225 MZU393195:MZU393225 NJQ393195:NJQ393225 NTM393195:NTM393225 ODI393195:ODI393225 ONE393195:ONE393225 OXA393195:OXA393225 PGW393195:PGW393225 PQS393195:PQS393225 QAO393195:QAO393225 QKK393195:QKK393225 QUG393195:QUG393225 REC393195:REC393225 RNY393195:RNY393225 RXU393195:RXU393225 SHQ393195:SHQ393225 SRM393195:SRM393225 TBI393195:TBI393225 TLE393195:TLE393225 TVA393195:TVA393225 UEW393195:UEW393225 UOS393195:UOS393225 UYO393195:UYO393225 VIK393195:VIK393225 VSG393195:VSG393225 WCC393195:WCC393225 WLY393195:WLY393225 WVU393195:WVU393225 JI458731:JI458761 TE458731:TE458761 ADA458731:ADA458761 AMW458731:AMW458761 AWS458731:AWS458761 BGO458731:BGO458761 BQK458731:BQK458761 CAG458731:CAG458761 CKC458731:CKC458761 CTY458731:CTY458761 DDU458731:DDU458761 DNQ458731:DNQ458761 DXM458731:DXM458761 EHI458731:EHI458761 ERE458731:ERE458761 FBA458731:FBA458761 FKW458731:FKW458761 FUS458731:FUS458761 GEO458731:GEO458761 GOK458731:GOK458761 GYG458731:GYG458761 HIC458731:HIC458761 HRY458731:HRY458761 IBU458731:IBU458761 ILQ458731:ILQ458761 IVM458731:IVM458761 JFI458731:JFI458761 JPE458731:JPE458761 JZA458731:JZA458761 KIW458731:KIW458761 KSS458731:KSS458761 LCO458731:LCO458761 LMK458731:LMK458761 LWG458731:LWG458761 MGC458731:MGC458761 MPY458731:MPY458761 MZU458731:MZU458761 NJQ458731:NJQ458761 NTM458731:NTM458761 ODI458731:ODI458761 ONE458731:ONE458761 OXA458731:OXA458761 PGW458731:PGW458761 PQS458731:PQS458761 QAO458731:QAO458761 QKK458731:QKK458761 QUG458731:QUG458761 REC458731:REC458761 RNY458731:RNY458761 RXU458731:RXU458761 SHQ458731:SHQ458761 SRM458731:SRM458761 TBI458731:TBI458761 TLE458731:TLE458761 TVA458731:TVA458761 UEW458731:UEW458761 UOS458731:UOS458761 UYO458731:UYO458761 VIK458731:VIK458761 VSG458731:VSG458761 WCC458731:WCC458761 WLY458731:WLY458761 WVU458731:WVU458761 JI524267:JI524297 TE524267:TE524297 ADA524267:ADA524297 AMW524267:AMW524297 AWS524267:AWS524297 BGO524267:BGO524297 BQK524267:BQK524297 CAG524267:CAG524297 CKC524267:CKC524297 CTY524267:CTY524297 DDU524267:DDU524297 DNQ524267:DNQ524297 DXM524267:DXM524297 EHI524267:EHI524297 ERE524267:ERE524297 FBA524267:FBA524297 FKW524267:FKW524297 FUS524267:FUS524297 GEO524267:GEO524297 GOK524267:GOK524297 GYG524267:GYG524297 HIC524267:HIC524297 HRY524267:HRY524297 IBU524267:IBU524297 ILQ524267:ILQ524297 IVM524267:IVM524297 JFI524267:JFI524297 JPE524267:JPE524297 JZA524267:JZA524297 KIW524267:KIW524297 KSS524267:KSS524297 LCO524267:LCO524297 LMK524267:LMK524297 LWG524267:LWG524297 MGC524267:MGC524297 MPY524267:MPY524297 MZU524267:MZU524297 NJQ524267:NJQ524297 NTM524267:NTM524297 ODI524267:ODI524297 ONE524267:ONE524297 OXA524267:OXA524297 PGW524267:PGW524297 PQS524267:PQS524297 QAO524267:QAO524297 QKK524267:QKK524297 QUG524267:QUG524297 REC524267:REC524297 RNY524267:RNY524297 RXU524267:RXU524297 SHQ524267:SHQ524297 SRM524267:SRM524297 TBI524267:TBI524297 TLE524267:TLE524297 TVA524267:TVA524297 UEW524267:UEW524297 UOS524267:UOS524297 UYO524267:UYO524297 VIK524267:VIK524297 VSG524267:VSG524297 WCC524267:WCC524297 WLY524267:WLY524297 WVU524267:WVU524297 JI589803:JI589833 TE589803:TE589833 ADA589803:ADA589833 AMW589803:AMW589833 AWS589803:AWS589833 BGO589803:BGO589833 BQK589803:BQK589833 CAG589803:CAG589833 CKC589803:CKC589833 CTY589803:CTY589833 DDU589803:DDU589833 DNQ589803:DNQ589833 DXM589803:DXM589833 EHI589803:EHI589833 ERE589803:ERE589833 FBA589803:FBA589833 FKW589803:FKW589833 FUS589803:FUS589833 GEO589803:GEO589833 GOK589803:GOK589833 GYG589803:GYG589833 HIC589803:HIC589833 HRY589803:HRY589833 IBU589803:IBU589833 ILQ589803:ILQ589833 IVM589803:IVM589833 JFI589803:JFI589833 JPE589803:JPE589833 JZA589803:JZA589833 KIW589803:KIW589833 KSS589803:KSS589833 LCO589803:LCO589833 LMK589803:LMK589833 LWG589803:LWG589833 MGC589803:MGC589833 MPY589803:MPY589833 MZU589803:MZU589833 NJQ589803:NJQ589833 NTM589803:NTM589833 ODI589803:ODI589833 ONE589803:ONE589833 OXA589803:OXA589833 PGW589803:PGW589833 PQS589803:PQS589833 QAO589803:QAO589833 QKK589803:QKK589833 QUG589803:QUG589833 REC589803:REC589833 RNY589803:RNY589833 RXU589803:RXU589833 SHQ589803:SHQ589833 SRM589803:SRM589833 TBI589803:TBI589833 TLE589803:TLE589833 TVA589803:TVA589833 UEW589803:UEW589833 UOS589803:UOS589833 UYO589803:UYO589833 VIK589803:VIK589833 VSG589803:VSG589833 WCC589803:WCC589833 WLY589803:WLY589833 WVU589803:WVU589833 JI655339:JI655369 TE655339:TE655369 ADA655339:ADA655369 AMW655339:AMW655369 AWS655339:AWS655369 BGO655339:BGO655369 BQK655339:BQK655369 CAG655339:CAG655369 CKC655339:CKC655369 CTY655339:CTY655369 DDU655339:DDU655369 DNQ655339:DNQ655369 DXM655339:DXM655369 EHI655339:EHI655369 ERE655339:ERE655369 FBA655339:FBA655369 FKW655339:FKW655369 FUS655339:FUS655369 GEO655339:GEO655369 GOK655339:GOK655369 GYG655339:GYG655369 HIC655339:HIC655369 HRY655339:HRY655369 IBU655339:IBU655369 ILQ655339:ILQ655369 IVM655339:IVM655369 JFI655339:JFI655369 JPE655339:JPE655369 JZA655339:JZA655369 KIW655339:KIW655369 KSS655339:KSS655369 LCO655339:LCO655369 LMK655339:LMK655369 LWG655339:LWG655369 MGC655339:MGC655369 MPY655339:MPY655369 MZU655339:MZU655369 NJQ655339:NJQ655369 NTM655339:NTM655369 ODI655339:ODI655369 ONE655339:ONE655369 OXA655339:OXA655369 PGW655339:PGW655369 PQS655339:PQS655369 QAO655339:QAO655369 QKK655339:QKK655369 QUG655339:QUG655369 REC655339:REC655369 RNY655339:RNY655369 RXU655339:RXU655369 SHQ655339:SHQ655369 SRM655339:SRM655369 TBI655339:TBI655369 TLE655339:TLE655369 TVA655339:TVA655369 UEW655339:UEW655369 UOS655339:UOS655369 UYO655339:UYO655369 VIK655339:VIK655369 VSG655339:VSG655369 WCC655339:WCC655369 WLY655339:WLY655369 WVU655339:WVU655369 JI720875:JI720905 TE720875:TE720905 ADA720875:ADA720905 AMW720875:AMW720905 AWS720875:AWS720905 BGO720875:BGO720905 BQK720875:BQK720905 CAG720875:CAG720905 CKC720875:CKC720905 CTY720875:CTY720905 DDU720875:DDU720905 DNQ720875:DNQ720905 DXM720875:DXM720905 EHI720875:EHI720905 ERE720875:ERE720905 FBA720875:FBA720905 FKW720875:FKW720905 FUS720875:FUS720905 GEO720875:GEO720905 GOK720875:GOK720905 GYG720875:GYG720905 HIC720875:HIC720905 HRY720875:HRY720905 IBU720875:IBU720905 ILQ720875:ILQ720905 IVM720875:IVM720905 JFI720875:JFI720905 JPE720875:JPE720905 JZA720875:JZA720905 KIW720875:KIW720905 KSS720875:KSS720905 LCO720875:LCO720905 LMK720875:LMK720905 LWG720875:LWG720905 MGC720875:MGC720905 MPY720875:MPY720905 MZU720875:MZU720905 NJQ720875:NJQ720905 NTM720875:NTM720905 ODI720875:ODI720905 ONE720875:ONE720905 OXA720875:OXA720905 PGW720875:PGW720905 PQS720875:PQS720905 QAO720875:QAO720905 QKK720875:QKK720905 QUG720875:QUG720905 REC720875:REC720905 RNY720875:RNY720905 RXU720875:RXU720905 SHQ720875:SHQ720905 SRM720875:SRM720905 TBI720875:TBI720905 TLE720875:TLE720905 TVA720875:TVA720905 UEW720875:UEW720905 UOS720875:UOS720905 UYO720875:UYO720905 VIK720875:VIK720905 VSG720875:VSG720905 WCC720875:WCC720905 WLY720875:WLY720905 WVU720875:WVU720905 JI786411:JI786441 TE786411:TE786441 ADA786411:ADA786441 AMW786411:AMW786441 AWS786411:AWS786441 BGO786411:BGO786441 BQK786411:BQK786441 CAG786411:CAG786441 CKC786411:CKC786441 CTY786411:CTY786441 DDU786411:DDU786441 DNQ786411:DNQ786441 DXM786411:DXM786441 EHI786411:EHI786441 ERE786411:ERE786441 FBA786411:FBA786441 FKW786411:FKW786441 FUS786411:FUS786441 GEO786411:GEO786441 GOK786411:GOK786441 GYG786411:GYG786441 HIC786411:HIC786441 HRY786411:HRY786441 IBU786411:IBU786441 ILQ786411:ILQ786441 IVM786411:IVM786441 JFI786411:JFI786441 JPE786411:JPE786441 JZA786411:JZA786441 KIW786411:KIW786441 KSS786411:KSS786441 LCO786411:LCO786441 LMK786411:LMK786441 LWG786411:LWG786441 MGC786411:MGC786441 MPY786411:MPY786441 MZU786411:MZU786441 NJQ786411:NJQ786441 NTM786411:NTM786441 ODI786411:ODI786441 ONE786411:ONE786441 OXA786411:OXA786441 PGW786411:PGW786441 PQS786411:PQS786441 QAO786411:QAO786441 QKK786411:QKK786441 QUG786411:QUG786441 REC786411:REC786441 RNY786411:RNY786441 RXU786411:RXU786441 SHQ786411:SHQ786441 SRM786411:SRM786441 TBI786411:TBI786441 TLE786411:TLE786441 TVA786411:TVA786441 UEW786411:UEW786441 UOS786411:UOS786441 UYO786411:UYO786441 VIK786411:VIK786441 VSG786411:VSG786441 WCC786411:WCC786441 WLY786411:WLY786441 WVU786411:WVU786441 JI851947:JI851977 TE851947:TE851977 ADA851947:ADA851977 AMW851947:AMW851977 AWS851947:AWS851977 BGO851947:BGO851977 BQK851947:BQK851977 CAG851947:CAG851977 CKC851947:CKC851977 CTY851947:CTY851977 DDU851947:DDU851977 DNQ851947:DNQ851977 DXM851947:DXM851977 EHI851947:EHI851977 ERE851947:ERE851977 FBA851947:FBA851977 FKW851947:FKW851977 FUS851947:FUS851977 GEO851947:GEO851977 GOK851947:GOK851977 GYG851947:GYG851977 HIC851947:HIC851977 HRY851947:HRY851977 IBU851947:IBU851977 ILQ851947:ILQ851977 IVM851947:IVM851977 JFI851947:JFI851977 JPE851947:JPE851977 JZA851947:JZA851977 KIW851947:KIW851977 KSS851947:KSS851977 LCO851947:LCO851977 LMK851947:LMK851977 LWG851947:LWG851977 MGC851947:MGC851977 MPY851947:MPY851977 MZU851947:MZU851977 NJQ851947:NJQ851977 NTM851947:NTM851977 ODI851947:ODI851977 ONE851947:ONE851977 OXA851947:OXA851977 PGW851947:PGW851977 PQS851947:PQS851977 QAO851947:QAO851977 QKK851947:QKK851977 QUG851947:QUG851977 REC851947:REC851977 RNY851947:RNY851977 RXU851947:RXU851977 SHQ851947:SHQ851977 SRM851947:SRM851977 TBI851947:TBI851977 TLE851947:TLE851977 TVA851947:TVA851977 UEW851947:UEW851977 UOS851947:UOS851977 UYO851947:UYO851977 VIK851947:VIK851977 VSG851947:VSG851977 WCC851947:WCC851977 WLY851947:WLY851977 WVU851947:WVU851977 JI917483:JI917513 TE917483:TE917513 ADA917483:ADA917513 AMW917483:AMW917513 AWS917483:AWS917513 BGO917483:BGO917513 BQK917483:BQK917513 CAG917483:CAG917513 CKC917483:CKC917513 CTY917483:CTY917513 DDU917483:DDU917513 DNQ917483:DNQ917513 DXM917483:DXM917513 EHI917483:EHI917513 ERE917483:ERE917513 FBA917483:FBA917513 FKW917483:FKW917513 FUS917483:FUS917513 GEO917483:GEO917513 GOK917483:GOK917513 GYG917483:GYG917513 HIC917483:HIC917513 HRY917483:HRY917513 IBU917483:IBU917513 ILQ917483:ILQ917513 IVM917483:IVM917513 JFI917483:JFI917513 JPE917483:JPE917513 JZA917483:JZA917513 KIW917483:KIW917513 KSS917483:KSS917513 LCO917483:LCO917513 LMK917483:LMK917513 LWG917483:LWG917513 MGC917483:MGC917513 MPY917483:MPY917513 MZU917483:MZU917513 NJQ917483:NJQ917513 NTM917483:NTM917513 ODI917483:ODI917513 ONE917483:ONE917513 OXA917483:OXA917513 PGW917483:PGW917513 PQS917483:PQS917513 QAO917483:QAO917513 QKK917483:QKK917513 QUG917483:QUG917513 REC917483:REC917513 RNY917483:RNY917513 RXU917483:RXU917513 SHQ917483:SHQ917513 SRM917483:SRM917513 TBI917483:TBI917513 TLE917483:TLE917513 TVA917483:TVA917513 UEW917483:UEW917513 UOS917483:UOS917513 UYO917483:UYO917513 VIK917483:VIK917513 VSG917483:VSG917513 WCC917483:WCC917513 WLY917483:WLY917513 WVU917483:WVU917513 JI983019:JI983049 TE983019:TE983049 ADA983019:ADA983049 AMW983019:AMW983049 AWS983019:AWS983049 BGO983019:BGO983049 BQK983019:BQK983049 CAG983019:CAG983049 CKC983019:CKC983049 CTY983019:CTY983049 DDU983019:DDU983049 DNQ983019:DNQ983049 DXM983019:DXM983049 EHI983019:EHI983049 ERE983019:ERE983049 FBA983019:FBA983049 FKW983019:FKW983049 FUS983019:FUS983049 GEO983019:GEO983049 GOK983019:GOK983049 GYG983019:GYG983049 HIC983019:HIC983049 HRY983019:HRY983049 IBU983019:IBU983049 ILQ983019:ILQ983049 IVM983019:IVM983049 JFI983019:JFI983049 JPE983019:JPE983049 JZA983019:JZA983049 KIW983019:KIW983049 KSS983019:KSS983049 LCO983019:LCO983049 LMK983019:LMK983049 LWG983019:LWG983049 MGC983019:MGC983049 MPY983019:MPY983049 MZU983019:MZU983049 NJQ983019:NJQ983049 NTM983019:NTM983049 ODI983019:ODI983049 ONE983019:ONE983049 OXA983019:OXA983049 PGW983019:PGW983049 PQS983019:PQS983049 QAO983019:QAO983049 QKK983019:QKK983049 QUG983019:QUG983049 REC983019:REC983049 RNY983019:RNY983049 RXU983019:RXU983049 SHQ983019:SHQ983049 SRM983019:SRM983049 TBI983019:TBI983049 TLE983019:TLE983049 TVA983019:TVA983049 UEW983019:UEW983049 UOS983019:UOS983049 UYO983019:UYO983049 VIK983019:VIK983049 VSG983019:VSG983049 WCC983019:WCC983049 WLY983019:WLY983049 WVU983019:WVU983049 T983019:T983049 T65515:T65545 T131051:T131081 T196587:T196617 T262123:T262153 T327659:T327689 T393195:T393225 T458731:T458761 T524267:T524297 T589803:T589833 T655339:T655369 T720875:T720905 T786411:T786441 T851947:T851977 T917483:T917513 WVU4:WVU20 WLY4:WLY20 WCC4:WCC20 VSG4:VSG20 VIK4:VIK20 UYO4:UYO20 UOS4:UOS20 UEW4:UEW20 TVA4:TVA20 TLE4:TLE20 TBI4:TBI20 SRM4:SRM20 SHQ4:SHQ20 RXU4:RXU20 RNY4:RNY20 REC4:REC20 QUG4:QUG20 QKK4:QKK20 QAO4:QAO20 PQS4:PQS20 PGW4:PGW20 OXA4:OXA20 ONE4:ONE20 ODI4:ODI20 NTM4:NTM20 NJQ4:NJQ20 MZU4:MZU20 MPY4:MPY20 MGC4:MGC20 LWG4:LWG20 LMK4:LMK20 LCO4:LCO20 KSS4:KSS20 KIW4:KIW20 JZA4:JZA20 JPE4:JPE20 JFI4:JFI20 IVM4:IVM20 ILQ4:ILQ20 IBU4:IBU20 HRY4:HRY20 HIC4:HIC20 GYG4:GYG20 GOK4:GOK20 GEO4:GEO20 FUS4:FUS20 FKW4:FKW20 FBA4:FBA20 ERE4:ERE20 EHI4:EHI20 DXM4:DXM20 DNQ4:DNQ20 DDU4:DDU20 CTY4:CTY20 CKC4:CKC20 CAG4:CAG20 BQK4:BQK20 BGO4:BGO20 AWS4:AWS20 AMW4:AMW20 ADA4:ADA20 TE4:TE20 JI4:JI20" xr:uid="{00000000-0002-0000-0200-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JI65515:JI65545 TE65515:TE65545 ADA65515:ADA65545 AMW65515:AMW65545 AWS65515:AWS65545 BGO65515:BGO65545 BQK65515:BQK65545 CAG65515:CAG65545 CKC65515:CKC65545 CTY65515:CTY65545 DDU65515:DDU65545 DNQ65515:DNQ65545 DXM65515:DXM65545 EHI65515:EHI65545 ERE65515:ERE65545 FBA65515:FBA65545 FKW65515:FKW65545 FUS65515:FUS65545 GEO65515:GEO65545 GOK65515:GOK65545 GYG65515:GYG65545 HIC65515:HIC65545 HRY65515:HRY65545 IBU65515:IBU65545 ILQ65515:ILQ65545 IVM65515:IVM65545 JFI65515:JFI65545 JPE65515:JPE65545 JZA65515:JZA65545 KIW65515:KIW65545 KSS65515:KSS65545 LCO65515:LCO65545 LMK65515:LMK65545 LWG65515:LWG65545 MGC65515:MGC65545 MPY65515:MPY65545 MZU65515:MZU65545 NJQ65515:NJQ65545 NTM65515:NTM65545 ODI65515:ODI65545 ONE65515:ONE65545 OXA65515:OXA65545 PGW65515:PGW65545 PQS65515:PQS65545 QAO65515:QAO65545 QKK65515:QKK65545 QUG65515:QUG65545 REC65515:REC65545 RNY65515:RNY65545 RXU65515:RXU65545 SHQ65515:SHQ65545 SRM65515:SRM65545 TBI65515:TBI65545 TLE65515:TLE65545 TVA65515:TVA65545 UEW65515:UEW65545 UOS65515:UOS65545 UYO65515:UYO65545 VIK65515:VIK65545 VSG65515:VSG65545 WCC65515:WCC65545 WLY65515:WLY65545 WVU65515:WVU65545 JI131051:JI131081 TE131051:TE131081 ADA131051:ADA131081 AMW131051:AMW131081 AWS131051:AWS131081 BGO131051:BGO131081 BQK131051:BQK131081 CAG131051:CAG131081 CKC131051:CKC131081 CTY131051:CTY131081 DDU131051:DDU131081 DNQ131051:DNQ131081 DXM131051:DXM131081 EHI131051:EHI131081 ERE131051:ERE131081 FBA131051:FBA131081 FKW131051:FKW131081 FUS131051:FUS131081 GEO131051:GEO131081 GOK131051:GOK131081 GYG131051:GYG131081 HIC131051:HIC131081 HRY131051:HRY131081 IBU131051:IBU131081 ILQ131051:ILQ131081 IVM131051:IVM131081 JFI131051:JFI131081 JPE131051:JPE131081 JZA131051:JZA131081 KIW131051:KIW131081 KSS131051:KSS131081 LCO131051:LCO131081 LMK131051:LMK131081 LWG131051:LWG131081 MGC131051:MGC131081 MPY131051:MPY131081 MZU131051:MZU131081 NJQ131051:NJQ131081 NTM131051:NTM131081 ODI131051:ODI131081 ONE131051:ONE131081 OXA131051:OXA131081 PGW131051:PGW131081 PQS131051:PQS131081 QAO131051:QAO131081 QKK131051:QKK131081 QUG131051:QUG131081 REC131051:REC131081 RNY131051:RNY131081 RXU131051:RXU131081 SHQ131051:SHQ131081 SRM131051:SRM131081 TBI131051:TBI131081 TLE131051:TLE131081 TVA131051:TVA131081 UEW131051:UEW131081 UOS131051:UOS131081 UYO131051:UYO131081 VIK131051:VIK131081 VSG131051:VSG131081 WCC131051:WCC131081 WLY131051:WLY131081 WVU131051:WVU131081 JI196587:JI196617 TE196587:TE196617 ADA196587:ADA196617 AMW196587:AMW196617 AWS196587:AWS196617 BGO196587:BGO196617 BQK196587:BQK196617 CAG196587:CAG196617 CKC196587:CKC196617 CTY196587:CTY196617 DDU196587:DDU196617 DNQ196587:DNQ196617 DXM196587:DXM196617 EHI196587:EHI196617 ERE196587:ERE196617 FBA196587:FBA196617 FKW196587:FKW196617 FUS196587:FUS196617 GEO196587:GEO196617 GOK196587:GOK196617 GYG196587:GYG196617 HIC196587:HIC196617 HRY196587:HRY196617 IBU196587:IBU196617 ILQ196587:ILQ196617 IVM196587:IVM196617 JFI196587:JFI196617 JPE196587:JPE196617 JZA196587:JZA196617 KIW196587:KIW196617 KSS196587:KSS196617 LCO196587:LCO196617 LMK196587:LMK196617 LWG196587:LWG196617 MGC196587:MGC196617 MPY196587:MPY196617 MZU196587:MZU196617 NJQ196587:NJQ196617 NTM196587:NTM196617 ODI196587:ODI196617 ONE196587:ONE196617 OXA196587:OXA196617 PGW196587:PGW196617 PQS196587:PQS196617 QAO196587:QAO196617 QKK196587:QKK196617 QUG196587:QUG196617 REC196587:REC196617 RNY196587:RNY196617 RXU196587:RXU196617 SHQ196587:SHQ196617 SRM196587:SRM196617 TBI196587:TBI196617 TLE196587:TLE196617 TVA196587:TVA196617 UEW196587:UEW196617 UOS196587:UOS196617 UYO196587:UYO196617 VIK196587:VIK196617 VSG196587:VSG196617 WCC196587:WCC196617 WLY196587:WLY196617 WVU196587:WVU196617 JI262123:JI262153 TE262123:TE262153 ADA262123:ADA262153 AMW262123:AMW262153 AWS262123:AWS262153 BGO262123:BGO262153 BQK262123:BQK262153 CAG262123:CAG262153 CKC262123:CKC262153 CTY262123:CTY262153 DDU262123:DDU262153 DNQ262123:DNQ262153 DXM262123:DXM262153 EHI262123:EHI262153 ERE262123:ERE262153 FBA262123:FBA262153 FKW262123:FKW262153 FUS262123:FUS262153 GEO262123:GEO262153 GOK262123:GOK262153 GYG262123:GYG262153 HIC262123:HIC262153 HRY262123:HRY262153 IBU262123:IBU262153 ILQ262123:ILQ262153 IVM262123:IVM262153 JFI262123:JFI262153 JPE262123:JPE262153 JZA262123:JZA262153 KIW262123:KIW262153 KSS262123:KSS262153 LCO262123:LCO262153 LMK262123:LMK262153 LWG262123:LWG262153 MGC262123:MGC262153 MPY262123:MPY262153 MZU262123:MZU262153 NJQ262123:NJQ262153 NTM262123:NTM262153 ODI262123:ODI262153 ONE262123:ONE262153 OXA262123:OXA262153 PGW262123:PGW262153 PQS262123:PQS262153 QAO262123:QAO262153 QKK262123:QKK262153 QUG262123:QUG262153 REC262123:REC262153 RNY262123:RNY262153 RXU262123:RXU262153 SHQ262123:SHQ262153 SRM262123:SRM262153 TBI262123:TBI262153 TLE262123:TLE262153 TVA262123:TVA262153 UEW262123:UEW262153 UOS262123:UOS262153 UYO262123:UYO262153 VIK262123:VIK262153 VSG262123:VSG262153 WCC262123:WCC262153 WLY262123:WLY262153 WVU262123:WVU262153 JI327659:JI327689 TE327659:TE327689 ADA327659:ADA327689 AMW327659:AMW327689 AWS327659:AWS327689 BGO327659:BGO327689 BQK327659:BQK327689 CAG327659:CAG327689 CKC327659:CKC327689 CTY327659:CTY327689 DDU327659:DDU327689 DNQ327659:DNQ327689 DXM327659:DXM327689 EHI327659:EHI327689 ERE327659:ERE327689 FBA327659:FBA327689 FKW327659:FKW327689 FUS327659:FUS327689 GEO327659:GEO327689 GOK327659:GOK327689 GYG327659:GYG327689 HIC327659:HIC327689 HRY327659:HRY327689 IBU327659:IBU327689 ILQ327659:ILQ327689 IVM327659:IVM327689 JFI327659:JFI327689 JPE327659:JPE327689 JZA327659:JZA327689 KIW327659:KIW327689 KSS327659:KSS327689 LCO327659:LCO327689 LMK327659:LMK327689 LWG327659:LWG327689 MGC327659:MGC327689 MPY327659:MPY327689 MZU327659:MZU327689 NJQ327659:NJQ327689 NTM327659:NTM327689 ODI327659:ODI327689 ONE327659:ONE327689 OXA327659:OXA327689 PGW327659:PGW327689 PQS327659:PQS327689 QAO327659:QAO327689 QKK327659:QKK327689 QUG327659:QUG327689 REC327659:REC327689 RNY327659:RNY327689 RXU327659:RXU327689 SHQ327659:SHQ327689 SRM327659:SRM327689 TBI327659:TBI327689 TLE327659:TLE327689 TVA327659:TVA327689 UEW327659:UEW327689 UOS327659:UOS327689 UYO327659:UYO327689 VIK327659:VIK327689 VSG327659:VSG327689 WCC327659:WCC327689 WLY327659:WLY327689 WVU327659:WVU327689 JI393195:JI393225 TE393195:TE393225 ADA393195:ADA393225 AMW393195:AMW393225 AWS393195:AWS393225 BGO393195:BGO393225 BQK393195:BQK393225 CAG393195:CAG393225 CKC393195:CKC393225 CTY393195:CTY393225 DDU393195:DDU393225 DNQ393195:DNQ393225 DXM393195:DXM393225 EHI393195:EHI393225 ERE393195:ERE393225 FBA393195:FBA393225 FKW393195:FKW393225 FUS393195:FUS393225 GEO393195:GEO393225 GOK393195:GOK393225 GYG393195:GYG393225 HIC393195:HIC393225 HRY393195:HRY393225 IBU393195:IBU393225 ILQ393195:ILQ393225 IVM393195:IVM393225 JFI393195:JFI393225 JPE393195:JPE393225 JZA393195:JZA393225 KIW393195:KIW393225 KSS393195:KSS393225 LCO393195:LCO393225 LMK393195:LMK393225 LWG393195:LWG393225 MGC393195:MGC393225 MPY393195:MPY393225 MZU393195:MZU393225 NJQ393195:NJQ393225 NTM393195:NTM393225 ODI393195:ODI393225 ONE393195:ONE393225 OXA393195:OXA393225 PGW393195:PGW393225 PQS393195:PQS393225 QAO393195:QAO393225 QKK393195:QKK393225 QUG393195:QUG393225 REC393195:REC393225 RNY393195:RNY393225 RXU393195:RXU393225 SHQ393195:SHQ393225 SRM393195:SRM393225 TBI393195:TBI393225 TLE393195:TLE393225 TVA393195:TVA393225 UEW393195:UEW393225 UOS393195:UOS393225 UYO393195:UYO393225 VIK393195:VIK393225 VSG393195:VSG393225 WCC393195:WCC393225 WLY393195:WLY393225 WVU393195:WVU393225 JI458731:JI458761 TE458731:TE458761 ADA458731:ADA458761 AMW458731:AMW458761 AWS458731:AWS458761 BGO458731:BGO458761 BQK458731:BQK458761 CAG458731:CAG458761 CKC458731:CKC458761 CTY458731:CTY458761 DDU458731:DDU458761 DNQ458731:DNQ458761 DXM458731:DXM458761 EHI458731:EHI458761 ERE458731:ERE458761 FBA458731:FBA458761 FKW458731:FKW458761 FUS458731:FUS458761 GEO458731:GEO458761 GOK458731:GOK458761 GYG458731:GYG458761 HIC458731:HIC458761 HRY458731:HRY458761 IBU458731:IBU458761 ILQ458731:ILQ458761 IVM458731:IVM458761 JFI458731:JFI458761 JPE458731:JPE458761 JZA458731:JZA458761 KIW458731:KIW458761 KSS458731:KSS458761 LCO458731:LCO458761 LMK458731:LMK458761 LWG458731:LWG458761 MGC458731:MGC458761 MPY458731:MPY458761 MZU458731:MZU458761 NJQ458731:NJQ458761 NTM458731:NTM458761 ODI458731:ODI458761 ONE458731:ONE458761 OXA458731:OXA458761 PGW458731:PGW458761 PQS458731:PQS458761 QAO458731:QAO458761 QKK458731:QKK458761 QUG458731:QUG458761 REC458731:REC458761 RNY458731:RNY458761 RXU458731:RXU458761 SHQ458731:SHQ458761 SRM458731:SRM458761 TBI458731:TBI458761 TLE458731:TLE458761 TVA458731:TVA458761 UEW458731:UEW458761 UOS458731:UOS458761 UYO458731:UYO458761 VIK458731:VIK458761 VSG458731:VSG458761 WCC458731:WCC458761 WLY458731:WLY458761 WVU458731:WVU458761 JI524267:JI524297 TE524267:TE524297 ADA524267:ADA524297 AMW524267:AMW524297 AWS524267:AWS524297 BGO524267:BGO524297 BQK524267:BQK524297 CAG524267:CAG524297 CKC524267:CKC524297 CTY524267:CTY524297 DDU524267:DDU524297 DNQ524267:DNQ524297 DXM524267:DXM524297 EHI524267:EHI524297 ERE524267:ERE524297 FBA524267:FBA524297 FKW524267:FKW524297 FUS524267:FUS524297 GEO524267:GEO524297 GOK524267:GOK524297 GYG524267:GYG524297 HIC524267:HIC524297 HRY524267:HRY524297 IBU524267:IBU524297 ILQ524267:ILQ524297 IVM524267:IVM524297 JFI524267:JFI524297 JPE524267:JPE524297 JZA524267:JZA524297 KIW524267:KIW524297 KSS524267:KSS524297 LCO524267:LCO524297 LMK524267:LMK524297 LWG524267:LWG524297 MGC524267:MGC524297 MPY524267:MPY524297 MZU524267:MZU524297 NJQ524267:NJQ524297 NTM524267:NTM524297 ODI524267:ODI524297 ONE524267:ONE524297 OXA524267:OXA524297 PGW524267:PGW524297 PQS524267:PQS524297 QAO524267:QAO524297 QKK524267:QKK524297 QUG524267:QUG524297 REC524267:REC524297 RNY524267:RNY524297 RXU524267:RXU524297 SHQ524267:SHQ524297 SRM524267:SRM524297 TBI524267:TBI524297 TLE524267:TLE524297 TVA524267:TVA524297 UEW524267:UEW524297 UOS524267:UOS524297 UYO524267:UYO524297 VIK524267:VIK524297 VSG524267:VSG524297 WCC524267:WCC524297 WLY524267:WLY524297 WVU524267:WVU524297 JI589803:JI589833 TE589803:TE589833 ADA589803:ADA589833 AMW589803:AMW589833 AWS589803:AWS589833 BGO589803:BGO589833 BQK589803:BQK589833 CAG589803:CAG589833 CKC589803:CKC589833 CTY589803:CTY589833 DDU589803:DDU589833 DNQ589803:DNQ589833 DXM589803:DXM589833 EHI589803:EHI589833 ERE589803:ERE589833 FBA589803:FBA589833 FKW589803:FKW589833 FUS589803:FUS589833 GEO589803:GEO589833 GOK589803:GOK589833 GYG589803:GYG589833 HIC589803:HIC589833 HRY589803:HRY589833 IBU589803:IBU589833 ILQ589803:ILQ589833 IVM589803:IVM589833 JFI589803:JFI589833 JPE589803:JPE589833 JZA589803:JZA589833 KIW589803:KIW589833 KSS589803:KSS589833 LCO589803:LCO589833 LMK589803:LMK589833 LWG589803:LWG589833 MGC589803:MGC589833 MPY589803:MPY589833 MZU589803:MZU589833 NJQ589803:NJQ589833 NTM589803:NTM589833 ODI589803:ODI589833 ONE589803:ONE589833 OXA589803:OXA589833 PGW589803:PGW589833 PQS589803:PQS589833 QAO589803:QAO589833 QKK589803:QKK589833 QUG589803:QUG589833 REC589803:REC589833 RNY589803:RNY589833 RXU589803:RXU589833 SHQ589803:SHQ589833 SRM589803:SRM589833 TBI589803:TBI589833 TLE589803:TLE589833 TVA589803:TVA589833 UEW589803:UEW589833 UOS589803:UOS589833 UYO589803:UYO589833 VIK589803:VIK589833 VSG589803:VSG589833 WCC589803:WCC589833 WLY589803:WLY589833 WVU589803:WVU589833 JI655339:JI655369 TE655339:TE655369 ADA655339:ADA655369 AMW655339:AMW655369 AWS655339:AWS655369 BGO655339:BGO655369 BQK655339:BQK655369 CAG655339:CAG655369 CKC655339:CKC655369 CTY655339:CTY655369 DDU655339:DDU655369 DNQ655339:DNQ655369 DXM655339:DXM655369 EHI655339:EHI655369 ERE655339:ERE655369 FBA655339:FBA655369 FKW655339:FKW655369 FUS655339:FUS655369 GEO655339:GEO655369 GOK655339:GOK655369 GYG655339:GYG655369 HIC655339:HIC655369 HRY655339:HRY655369 IBU655339:IBU655369 ILQ655339:ILQ655369 IVM655339:IVM655369 JFI655339:JFI655369 JPE655339:JPE655369 JZA655339:JZA655369 KIW655339:KIW655369 KSS655339:KSS655369 LCO655339:LCO655369 LMK655339:LMK655369 LWG655339:LWG655369 MGC655339:MGC655369 MPY655339:MPY655369 MZU655339:MZU655369 NJQ655339:NJQ655369 NTM655339:NTM655369 ODI655339:ODI655369 ONE655339:ONE655369 OXA655339:OXA655369 PGW655339:PGW655369 PQS655339:PQS655369 QAO655339:QAO655369 QKK655339:QKK655369 QUG655339:QUG655369 REC655339:REC655369 RNY655339:RNY655369 RXU655339:RXU655369 SHQ655339:SHQ655369 SRM655339:SRM655369 TBI655339:TBI655369 TLE655339:TLE655369 TVA655339:TVA655369 UEW655339:UEW655369 UOS655339:UOS655369 UYO655339:UYO655369 VIK655339:VIK655369 VSG655339:VSG655369 WCC655339:WCC655369 WLY655339:WLY655369 WVU655339:WVU655369 JI720875:JI720905 TE720875:TE720905 ADA720875:ADA720905 AMW720875:AMW720905 AWS720875:AWS720905 BGO720875:BGO720905 BQK720875:BQK720905 CAG720875:CAG720905 CKC720875:CKC720905 CTY720875:CTY720905 DDU720875:DDU720905 DNQ720875:DNQ720905 DXM720875:DXM720905 EHI720875:EHI720905 ERE720875:ERE720905 FBA720875:FBA720905 FKW720875:FKW720905 FUS720875:FUS720905 GEO720875:GEO720905 GOK720875:GOK720905 GYG720875:GYG720905 HIC720875:HIC720905 HRY720875:HRY720905 IBU720875:IBU720905 ILQ720875:ILQ720905 IVM720875:IVM720905 JFI720875:JFI720905 JPE720875:JPE720905 JZA720875:JZA720905 KIW720875:KIW720905 KSS720875:KSS720905 LCO720875:LCO720905 LMK720875:LMK720905 LWG720875:LWG720905 MGC720875:MGC720905 MPY720875:MPY720905 MZU720875:MZU720905 NJQ720875:NJQ720905 NTM720875:NTM720905 ODI720875:ODI720905 ONE720875:ONE720905 OXA720875:OXA720905 PGW720875:PGW720905 PQS720875:PQS720905 QAO720875:QAO720905 QKK720875:QKK720905 QUG720875:QUG720905 REC720875:REC720905 RNY720875:RNY720905 RXU720875:RXU720905 SHQ720875:SHQ720905 SRM720875:SRM720905 TBI720875:TBI720905 TLE720875:TLE720905 TVA720875:TVA720905 UEW720875:UEW720905 UOS720875:UOS720905 UYO720875:UYO720905 VIK720875:VIK720905 VSG720875:VSG720905 WCC720875:WCC720905 WLY720875:WLY720905 WVU720875:WVU720905 JI786411:JI786441 TE786411:TE786441 ADA786411:ADA786441 AMW786411:AMW786441 AWS786411:AWS786441 BGO786411:BGO786441 BQK786411:BQK786441 CAG786411:CAG786441 CKC786411:CKC786441 CTY786411:CTY786441 DDU786411:DDU786441 DNQ786411:DNQ786441 DXM786411:DXM786441 EHI786411:EHI786441 ERE786411:ERE786441 FBA786411:FBA786441 FKW786411:FKW786441 FUS786411:FUS786441 GEO786411:GEO786441 GOK786411:GOK786441 GYG786411:GYG786441 HIC786411:HIC786441 HRY786411:HRY786441 IBU786411:IBU786441 ILQ786411:ILQ786441 IVM786411:IVM786441 JFI786411:JFI786441 JPE786411:JPE786441 JZA786411:JZA786441 KIW786411:KIW786441 KSS786411:KSS786441 LCO786411:LCO786441 LMK786411:LMK786441 LWG786411:LWG786441 MGC786411:MGC786441 MPY786411:MPY786441 MZU786411:MZU786441 NJQ786411:NJQ786441 NTM786411:NTM786441 ODI786411:ODI786441 ONE786411:ONE786441 OXA786411:OXA786441 PGW786411:PGW786441 PQS786411:PQS786441 QAO786411:QAO786441 QKK786411:QKK786441 QUG786411:QUG786441 REC786411:REC786441 RNY786411:RNY786441 RXU786411:RXU786441 SHQ786411:SHQ786441 SRM786411:SRM786441 TBI786411:TBI786441 TLE786411:TLE786441 TVA786411:TVA786441 UEW786411:UEW786441 UOS786411:UOS786441 UYO786411:UYO786441 VIK786411:VIK786441 VSG786411:VSG786441 WCC786411:WCC786441 WLY786411:WLY786441 WVU786411:WVU786441 JI851947:JI851977 TE851947:TE851977 ADA851947:ADA851977 AMW851947:AMW851977 AWS851947:AWS851977 BGO851947:BGO851977 BQK851947:BQK851977 CAG851947:CAG851977 CKC851947:CKC851977 CTY851947:CTY851977 DDU851947:DDU851977 DNQ851947:DNQ851977 DXM851947:DXM851977 EHI851947:EHI851977 ERE851947:ERE851977 FBA851947:FBA851977 FKW851947:FKW851977 FUS851947:FUS851977 GEO851947:GEO851977 GOK851947:GOK851977 GYG851947:GYG851977 HIC851947:HIC851977 HRY851947:HRY851977 IBU851947:IBU851977 ILQ851947:ILQ851977 IVM851947:IVM851977 JFI851947:JFI851977 JPE851947:JPE851977 JZA851947:JZA851977 KIW851947:KIW851977 KSS851947:KSS851977 LCO851947:LCO851977 LMK851947:LMK851977 LWG851947:LWG851977 MGC851947:MGC851977 MPY851947:MPY851977 MZU851947:MZU851977 NJQ851947:NJQ851977 NTM851947:NTM851977 ODI851947:ODI851977 ONE851947:ONE851977 OXA851947:OXA851977 PGW851947:PGW851977 PQS851947:PQS851977 QAO851947:QAO851977 QKK851947:QKK851977 QUG851947:QUG851977 REC851947:REC851977 RNY851947:RNY851977 RXU851947:RXU851977 SHQ851947:SHQ851977 SRM851947:SRM851977 TBI851947:TBI851977 TLE851947:TLE851977 TVA851947:TVA851977 UEW851947:UEW851977 UOS851947:UOS851977 UYO851947:UYO851977 VIK851947:VIK851977 VSG851947:VSG851977 WCC851947:WCC851977 WLY851947:WLY851977 WVU851947:WVU851977 JI917483:JI917513 TE917483:TE917513 ADA917483:ADA917513 AMW917483:AMW917513 AWS917483:AWS917513 BGO917483:BGO917513 BQK917483:BQK917513 CAG917483:CAG917513 CKC917483:CKC917513 CTY917483:CTY917513 DDU917483:DDU917513 DNQ917483:DNQ917513 DXM917483:DXM917513 EHI917483:EHI917513 ERE917483:ERE917513 FBA917483:FBA917513 FKW917483:FKW917513 FUS917483:FUS917513 GEO917483:GEO917513 GOK917483:GOK917513 GYG917483:GYG917513 HIC917483:HIC917513 HRY917483:HRY917513 IBU917483:IBU917513 ILQ917483:ILQ917513 IVM917483:IVM917513 JFI917483:JFI917513 JPE917483:JPE917513 JZA917483:JZA917513 KIW917483:KIW917513 KSS917483:KSS917513 LCO917483:LCO917513 LMK917483:LMK917513 LWG917483:LWG917513 MGC917483:MGC917513 MPY917483:MPY917513 MZU917483:MZU917513 NJQ917483:NJQ917513 NTM917483:NTM917513 ODI917483:ODI917513 ONE917483:ONE917513 OXA917483:OXA917513 PGW917483:PGW917513 PQS917483:PQS917513 QAO917483:QAO917513 QKK917483:QKK917513 QUG917483:QUG917513 REC917483:REC917513 RNY917483:RNY917513 RXU917483:RXU917513 SHQ917483:SHQ917513 SRM917483:SRM917513 TBI917483:TBI917513 TLE917483:TLE917513 TVA917483:TVA917513 UEW917483:UEW917513 UOS917483:UOS917513 UYO917483:UYO917513 VIK917483:VIK917513 VSG917483:VSG917513 WCC917483:WCC917513 WLY917483:WLY917513 WVU917483:WVU917513 JI983019:JI983049 TE983019:TE983049 ADA983019:ADA983049 AMW983019:AMW983049 AWS983019:AWS983049 BGO983019:BGO983049 BQK983019:BQK983049 CAG983019:CAG983049 CKC983019:CKC983049 CTY983019:CTY983049 DDU983019:DDU983049 DNQ983019:DNQ983049 DXM983019:DXM983049 EHI983019:EHI983049 ERE983019:ERE983049 FBA983019:FBA983049 FKW983019:FKW983049 FUS983019:FUS983049 GEO983019:GEO983049 GOK983019:GOK983049 GYG983019:GYG983049 HIC983019:HIC983049 HRY983019:HRY983049 IBU983019:IBU983049 ILQ983019:ILQ983049 IVM983019:IVM983049 JFI983019:JFI983049 JPE983019:JPE983049 JZA983019:JZA983049 KIW983019:KIW983049 KSS983019:KSS983049 LCO983019:LCO983049 LMK983019:LMK983049 LWG983019:LWG983049 MGC983019:MGC983049 MPY983019:MPY983049 MZU983019:MZU983049 NJQ983019:NJQ983049 NTM983019:NTM983049 ODI983019:ODI983049 ONE983019:ONE983049 OXA983019:OXA983049 PGW983019:PGW983049 PQS983019:PQS983049 QAO983019:QAO983049 QKK983019:QKK983049 QUG983019:QUG983049 REC983019:REC983049 RNY983019:RNY983049 RXU983019:RXU983049 SHQ983019:SHQ983049 SRM983019:SRM983049 TBI983019:TBI983049 TLE983019:TLE983049 TVA983019:TVA983049 UEW983019:UEW983049 UOS983019:UOS983049 UYO983019:UYO983049 VIK983019:VIK983049 VSG983019:VSG983049 WCC983019:WCC983049 WLY983019:WLY983049 WVU983019:WVU983049 T983019:T983049 T65515:T65545 T131051:T131081 T196587:T196617 T262123:T262153 T327659:T327689 T393195:T393225 T458731:T458761 T524267:T524297 T589803:T589833 T655339:T655369 T720875:T720905 T786411:T786441 T851947:T851977 T917483:T917513 JI4:JI20 TE4:TE20 ADA4:ADA20 AMW4:AMW20 AWS4:AWS20 BGO4:BGO20 BQK4:BQK20 CAG4:CAG20 CKC4:CKC20 CTY4:CTY20 DDU4:DDU20 DNQ4:DNQ20 DXM4:DXM20 EHI4:EHI20 ERE4:ERE20 FBA4:FBA20 FKW4:FKW20 FUS4:FUS20 GEO4:GEO20 GOK4:GOK20 GYG4:GYG20 HIC4:HIC20 HRY4:HRY20 IBU4:IBU20 ILQ4:ILQ20 IVM4:IVM20 JFI4:JFI20 JPE4:JPE20 JZA4:JZA20 KIW4:KIW20 KSS4:KSS20 LCO4:LCO20 LMK4:LMK20 LWG4:LWG20 MGC4:MGC20 MPY4:MPY20 MZU4:MZU20 NJQ4:NJQ20 NTM4:NTM20 ODI4:ODI20 ONE4:ONE20 OXA4:OXA20 PGW4:PGW20 PQS4:PQS20 QAO4:QAO20 QKK4:QKK20 QUG4:QUG20 REC4:REC20 RNY4:RNY20 RXU4:RXU20 SHQ4:SHQ20 SRM4:SRM20 TBI4:TBI20 TLE4:TLE20 TVA4:TVA20 UEW4:UEW20 UOS4:UOS20 UYO4:UYO20 VIK4:VIK20 VSG4:VSG20 WCC4:WCC20 WLY4:WLY20 WVU4:WVU20" xr:uid="{00000000-0002-0000-0200-00000C000000}">
       <formula1>"Sin hijos, 1-2 hijos,3-5 hijos, más de 6 hijos"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVP983019:WVP983049 O65515:O65545 JD65515:JD65545 SZ65515:SZ65545 ACV65515:ACV65545 AMR65515:AMR65545 AWN65515:AWN65545 BGJ65515:BGJ65545 BQF65515:BQF65545 CAB65515:CAB65545 CJX65515:CJX65545 CTT65515:CTT65545 DDP65515:DDP65545 DNL65515:DNL65545 DXH65515:DXH65545 EHD65515:EHD65545 EQZ65515:EQZ65545 FAV65515:FAV65545 FKR65515:FKR65545 FUN65515:FUN65545 GEJ65515:GEJ65545 GOF65515:GOF65545 GYB65515:GYB65545 HHX65515:HHX65545 HRT65515:HRT65545 IBP65515:IBP65545 ILL65515:ILL65545 IVH65515:IVH65545 JFD65515:JFD65545 JOZ65515:JOZ65545 JYV65515:JYV65545 KIR65515:KIR65545 KSN65515:KSN65545 LCJ65515:LCJ65545 LMF65515:LMF65545 LWB65515:LWB65545 MFX65515:MFX65545 MPT65515:MPT65545 MZP65515:MZP65545 NJL65515:NJL65545 NTH65515:NTH65545 ODD65515:ODD65545 OMZ65515:OMZ65545 OWV65515:OWV65545 PGR65515:PGR65545 PQN65515:PQN65545 QAJ65515:QAJ65545 QKF65515:QKF65545 QUB65515:QUB65545 RDX65515:RDX65545 RNT65515:RNT65545 RXP65515:RXP65545 SHL65515:SHL65545 SRH65515:SRH65545 TBD65515:TBD65545 TKZ65515:TKZ65545 TUV65515:TUV65545 UER65515:UER65545 UON65515:UON65545 UYJ65515:UYJ65545 VIF65515:VIF65545 VSB65515:VSB65545 WBX65515:WBX65545 WLT65515:WLT65545 WVP65515:WVP65545 O131051:O131081 JD131051:JD131081 SZ131051:SZ131081 ACV131051:ACV131081 AMR131051:AMR131081 AWN131051:AWN131081 BGJ131051:BGJ131081 BQF131051:BQF131081 CAB131051:CAB131081 CJX131051:CJX131081 CTT131051:CTT131081 DDP131051:DDP131081 DNL131051:DNL131081 DXH131051:DXH131081 EHD131051:EHD131081 EQZ131051:EQZ131081 FAV131051:FAV131081 FKR131051:FKR131081 FUN131051:FUN131081 GEJ131051:GEJ131081 GOF131051:GOF131081 GYB131051:GYB131081 HHX131051:HHX131081 HRT131051:HRT131081 IBP131051:IBP131081 ILL131051:ILL131081 IVH131051:IVH131081 JFD131051:JFD131081 JOZ131051:JOZ131081 JYV131051:JYV131081 KIR131051:KIR131081 KSN131051:KSN131081 LCJ131051:LCJ131081 LMF131051:LMF131081 LWB131051:LWB131081 MFX131051:MFX131081 MPT131051:MPT131081 MZP131051:MZP131081 NJL131051:NJL131081 NTH131051:NTH131081 ODD131051:ODD131081 OMZ131051:OMZ131081 OWV131051:OWV131081 PGR131051:PGR131081 PQN131051:PQN131081 QAJ131051:QAJ131081 QKF131051:QKF131081 QUB131051:QUB131081 RDX131051:RDX131081 RNT131051:RNT131081 RXP131051:RXP131081 SHL131051:SHL131081 SRH131051:SRH131081 TBD131051:TBD131081 TKZ131051:TKZ131081 TUV131051:TUV131081 UER131051:UER131081 UON131051:UON131081 UYJ131051:UYJ131081 VIF131051:VIF131081 VSB131051:VSB131081 WBX131051:WBX131081 WLT131051:WLT131081 WVP131051:WVP131081 O196587:O196617 JD196587:JD196617 SZ196587:SZ196617 ACV196587:ACV196617 AMR196587:AMR196617 AWN196587:AWN196617 BGJ196587:BGJ196617 BQF196587:BQF196617 CAB196587:CAB196617 CJX196587:CJX196617 CTT196587:CTT196617 DDP196587:DDP196617 DNL196587:DNL196617 DXH196587:DXH196617 EHD196587:EHD196617 EQZ196587:EQZ196617 FAV196587:FAV196617 FKR196587:FKR196617 FUN196587:FUN196617 GEJ196587:GEJ196617 GOF196587:GOF196617 GYB196587:GYB196617 HHX196587:HHX196617 HRT196587:HRT196617 IBP196587:IBP196617 ILL196587:ILL196617 IVH196587:IVH196617 JFD196587:JFD196617 JOZ196587:JOZ196617 JYV196587:JYV196617 KIR196587:KIR196617 KSN196587:KSN196617 LCJ196587:LCJ196617 LMF196587:LMF196617 LWB196587:LWB196617 MFX196587:MFX196617 MPT196587:MPT196617 MZP196587:MZP196617 NJL196587:NJL196617 NTH196587:NTH196617 ODD196587:ODD196617 OMZ196587:OMZ196617 OWV196587:OWV196617 PGR196587:PGR196617 PQN196587:PQN196617 QAJ196587:QAJ196617 QKF196587:QKF196617 QUB196587:QUB196617 RDX196587:RDX196617 RNT196587:RNT196617 RXP196587:RXP196617 SHL196587:SHL196617 SRH196587:SRH196617 TBD196587:TBD196617 TKZ196587:TKZ196617 TUV196587:TUV196617 UER196587:UER196617 UON196587:UON196617 UYJ196587:UYJ196617 VIF196587:VIF196617 VSB196587:VSB196617 WBX196587:WBX196617 WLT196587:WLT196617 WVP196587:WVP196617 O262123:O262153 JD262123:JD262153 SZ262123:SZ262153 ACV262123:ACV262153 AMR262123:AMR262153 AWN262123:AWN262153 BGJ262123:BGJ262153 BQF262123:BQF262153 CAB262123:CAB262153 CJX262123:CJX262153 CTT262123:CTT262153 DDP262123:DDP262153 DNL262123:DNL262153 DXH262123:DXH262153 EHD262123:EHD262153 EQZ262123:EQZ262153 FAV262123:FAV262153 FKR262123:FKR262153 FUN262123:FUN262153 GEJ262123:GEJ262153 GOF262123:GOF262153 GYB262123:GYB262153 HHX262123:HHX262153 HRT262123:HRT262153 IBP262123:IBP262153 ILL262123:ILL262153 IVH262123:IVH262153 JFD262123:JFD262153 JOZ262123:JOZ262153 JYV262123:JYV262153 KIR262123:KIR262153 KSN262123:KSN262153 LCJ262123:LCJ262153 LMF262123:LMF262153 LWB262123:LWB262153 MFX262123:MFX262153 MPT262123:MPT262153 MZP262123:MZP262153 NJL262123:NJL262153 NTH262123:NTH262153 ODD262123:ODD262153 OMZ262123:OMZ262153 OWV262123:OWV262153 PGR262123:PGR262153 PQN262123:PQN262153 QAJ262123:QAJ262153 QKF262123:QKF262153 QUB262123:QUB262153 RDX262123:RDX262153 RNT262123:RNT262153 RXP262123:RXP262153 SHL262123:SHL262153 SRH262123:SRH262153 TBD262123:TBD262153 TKZ262123:TKZ262153 TUV262123:TUV262153 UER262123:UER262153 UON262123:UON262153 UYJ262123:UYJ262153 VIF262123:VIF262153 VSB262123:VSB262153 WBX262123:WBX262153 WLT262123:WLT262153 WVP262123:WVP262153 O327659:O327689 JD327659:JD327689 SZ327659:SZ327689 ACV327659:ACV327689 AMR327659:AMR327689 AWN327659:AWN327689 BGJ327659:BGJ327689 BQF327659:BQF327689 CAB327659:CAB327689 CJX327659:CJX327689 CTT327659:CTT327689 DDP327659:DDP327689 DNL327659:DNL327689 DXH327659:DXH327689 EHD327659:EHD327689 EQZ327659:EQZ327689 FAV327659:FAV327689 FKR327659:FKR327689 FUN327659:FUN327689 GEJ327659:GEJ327689 GOF327659:GOF327689 GYB327659:GYB327689 HHX327659:HHX327689 HRT327659:HRT327689 IBP327659:IBP327689 ILL327659:ILL327689 IVH327659:IVH327689 JFD327659:JFD327689 JOZ327659:JOZ327689 JYV327659:JYV327689 KIR327659:KIR327689 KSN327659:KSN327689 LCJ327659:LCJ327689 LMF327659:LMF327689 LWB327659:LWB327689 MFX327659:MFX327689 MPT327659:MPT327689 MZP327659:MZP327689 NJL327659:NJL327689 NTH327659:NTH327689 ODD327659:ODD327689 OMZ327659:OMZ327689 OWV327659:OWV327689 PGR327659:PGR327689 PQN327659:PQN327689 QAJ327659:QAJ327689 QKF327659:QKF327689 QUB327659:QUB327689 RDX327659:RDX327689 RNT327659:RNT327689 RXP327659:RXP327689 SHL327659:SHL327689 SRH327659:SRH327689 TBD327659:TBD327689 TKZ327659:TKZ327689 TUV327659:TUV327689 UER327659:UER327689 UON327659:UON327689 UYJ327659:UYJ327689 VIF327659:VIF327689 VSB327659:VSB327689 WBX327659:WBX327689 WLT327659:WLT327689 WVP327659:WVP327689 O393195:O393225 JD393195:JD393225 SZ393195:SZ393225 ACV393195:ACV393225 AMR393195:AMR393225 AWN393195:AWN393225 BGJ393195:BGJ393225 BQF393195:BQF393225 CAB393195:CAB393225 CJX393195:CJX393225 CTT393195:CTT393225 DDP393195:DDP393225 DNL393195:DNL393225 DXH393195:DXH393225 EHD393195:EHD393225 EQZ393195:EQZ393225 FAV393195:FAV393225 FKR393195:FKR393225 FUN393195:FUN393225 GEJ393195:GEJ393225 GOF393195:GOF393225 GYB393195:GYB393225 HHX393195:HHX393225 HRT393195:HRT393225 IBP393195:IBP393225 ILL393195:ILL393225 IVH393195:IVH393225 JFD393195:JFD393225 JOZ393195:JOZ393225 JYV393195:JYV393225 KIR393195:KIR393225 KSN393195:KSN393225 LCJ393195:LCJ393225 LMF393195:LMF393225 LWB393195:LWB393225 MFX393195:MFX393225 MPT393195:MPT393225 MZP393195:MZP393225 NJL393195:NJL393225 NTH393195:NTH393225 ODD393195:ODD393225 OMZ393195:OMZ393225 OWV393195:OWV393225 PGR393195:PGR393225 PQN393195:PQN393225 QAJ393195:QAJ393225 QKF393195:QKF393225 QUB393195:QUB393225 RDX393195:RDX393225 RNT393195:RNT393225 RXP393195:RXP393225 SHL393195:SHL393225 SRH393195:SRH393225 TBD393195:TBD393225 TKZ393195:TKZ393225 TUV393195:TUV393225 UER393195:UER393225 UON393195:UON393225 UYJ393195:UYJ393225 VIF393195:VIF393225 VSB393195:VSB393225 WBX393195:WBX393225 WLT393195:WLT393225 WVP393195:WVP393225 O458731:O458761 JD458731:JD458761 SZ458731:SZ458761 ACV458731:ACV458761 AMR458731:AMR458761 AWN458731:AWN458761 BGJ458731:BGJ458761 BQF458731:BQF458761 CAB458731:CAB458761 CJX458731:CJX458761 CTT458731:CTT458761 DDP458731:DDP458761 DNL458731:DNL458761 DXH458731:DXH458761 EHD458731:EHD458761 EQZ458731:EQZ458761 FAV458731:FAV458761 FKR458731:FKR458761 FUN458731:FUN458761 GEJ458731:GEJ458761 GOF458731:GOF458761 GYB458731:GYB458761 HHX458731:HHX458761 HRT458731:HRT458761 IBP458731:IBP458761 ILL458731:ILL458761 IVH458731:IVH458761 JFD458731:JFD458761 JOZ458731:JOZ458761 JYV458731:JYV458761 KIR458731:KIR458761 KSN458731:KSN458761 LCJ458731:LCJ458761 LMF458731:LMF458761 LWB458731:LWB458761 MFX458731:MFX458761 MPT458731:MPT458761 MZP458731:MZP458761 NJL458731:NJL458761 NTH458731:NTH458761 ODD458731:ODD458761 OMZ458731:OMZ458761 OWV458731:OWV458761 PGR458731:PGR458761 PQN458731:PQN458761 QAJ458731:QAJ458761 QKF458731:QKF458761 QUB458731:QUB458761 RDX458731:RDX458761 RNT458731:RNT458761 RXP458731:RXP458761 SHL458731:SHL458761 SRH458731:SRH458761 TBD458731:TBD458761 TKZ458731:TKZ458761 TUV458731:TUV458761 UER458731:UER458761 UON458731:UON458761 UYJ458731:UYJ458761 VIF458731:VIF458761 VSB458731:VSB458761 WBX458731:WBX458761 WLT458731:WLT458761 WVP458731:WVP458761 O524267:O524297 JD524267:JD524297 SZ524267:SZ524297 ACV524267:ACV524297 AMR524267:AMR524297 AWN524267:AWN524297 BGJ524267:BGJ524297 BQF524267:BQF524297 CAB524267:CAB524297 CJX524267:CJX524297 CTT524267:CTT524297 DDP524267:DDP524297 DNL524267:DNL524297 DXH524267:DXH524297 EHD524267:EHD524297 EQZ524267:EQZ524297 FAV524267:FAV524297 FKR524267:FKR524297 FUN524267:FUN524297 GEJ524267:GEJ524297 GOF524267:GOF524297 GYB524267:GYB524297 HHX524267:HHX524297 HRT524267:HRT524297 IBP524267:IBP524297 ILL524267:ILL524297 IVH524267:IVH524297 JFD524267:JFD524297 JOZ524267:JOZ524297 JYV524267:JYV524297 KIR524267:KIR524297 KSN524267:KSN524297 LCJ524267:LCJ524297 LMF524267:LMF524297 LWB524267:LWB524297 MFX524267:MFX524297 MPT524267:MPT524297 MZP524267:MZP524297 NJL524267:NJL524297 NTH524267:NTH524297 ODD524267:ODD524297 OMZ524267:OMZ524297 OWV524267:OWV524297 PGR524267:PGR524297 PQN524267:PQN524297 QAJ524267:QAJ524297 QKF524267:QKF524297 QUB524267:QUB524297 RDX524267:RDX524297 RNT524267:RNT524297 RXP524267:RXP524297 SHL524267:SHL524297 SRH524267:SRH524297 TBD524267:TBD524297 TKZ524267:TKZ524297 TUV524267:TUV524297 UER524267:UER524297 UON524267:UON524297 UYJ524267:UYJ524297 VIF524267:VIF524297 VSB524267:VSB524297 WBX524267:WBX524297 WLT524267:WLT524297 WVP524267:WVP524297 O589803:O589833 JD589803:JD589833 SZ589803:SZ589833 ACV589803:ACV589833 AMR589803:AMR589833 AWN589803:AWN589833 BGJ589803:BGJ589833 BQF589803:BQF589833 CAB589803:CAB589833 CJX589803:CJX589833 CTT589803:CTT589833 DDP589803:DDP589833 DNL589803:DNL589833 DXH589803:DXH589833 EHD589803:EHD589833 EQZ589803:EQZ589833 FAV589803:FAV589833 FKR589803:FKR589833 FUN589803:FUN589833 GEJ589803:GEJ589833 GOF589803:GOF589833 GYB589803:GYB589833 HHX589803:HHX589833 HRT589803:HRT589833 IBP589803:IBP589833 ILL589803:ILL589833 IVH589803:IVH589833 JFD589803:JFD589833 JOZ589803:JOZ589833 JYV589803:JYV589833 KIR589803:KIR589833 KSN589803:KSN589833 LCJ589803:LCJ589833 LMF589803:LMF589833 LWB589803:LWB589833 MFX589803:MFX589833 MPT589803:MPT589833 MZP589803:MZP589833 NJL589803:NJL589833 NTH589803:NTH589833 ODD589803:ODD589833 OMZ589803:OMZ589833 OWV589803:OWV589833 PGR589803:PGR589833 PQN589803:PQN589833 QAJ589803:QAJ589833 QKF589803:QKF589833 QUB589803:QUB589833 RDX589803:RDX589833 RNT589803:RNT589833 RXP589803:RXP589833 SHL589803:SHL589833 SRH589803:SRH589833 TBD589803:TBD589833 TKZ589803:TKZ589833 TUV589803:TUV589833 UER589803:UER589833 UON589803:UON589833 UYJ589803:UYJ589833 VIF589803:VIF589833 VSB589803:VSB589833 WBX589803:WBX589833 WLT589803:WLT589833 WVP589803:WVP589833 O655339:O655369 JD655339:JD655369 SZ655339:SZ655369 ACV655339:ACV655369 AMR655339:AMR655369 AWN655339:AWN655369 BGJ655339:BGJ655369 BQF655339:BQF655369 CAB655339:CAB655369 CJX655339:CJX655369 CTT655339:CTT655369 DDP655339:DDP655369 DNL655339:DNL655369 DXH655339:DXH655369 EHD655339:EHD655369 EQZ655339:EQZ655369 FAV655339:FAV655369 FKR655339:FKR655369 FUN655339:FUN655369 GEJ655339:GEJ655369 GOF655339:GOF655369 GYB655339:GYB655369 HHX655339:HHX655369 HRT655339:HRT655369 IBP655339:IBP655369 ILL655339:ILL655369 IVH655339:IVH655369 JFD655339:JFD655369 JOZ655339:JOZ655369 JYV655339:JYV655369 KIR655339:KIR655369 KSN655339:KSN655369 LCJ655339:LCJ655369 LMF655339:LMF655369 LWB655339:LWB655369 MFX655339:MFX655369 MPT655339:MPT655369 MZP655339:MZP655369 NJL655339:NJL655369 NTH655339:NTH655369 ODD655339:ODD655369 OMZ655339:OMZ655369 OWV655339:OWV655369 PGR655339:PGR655369 PQN655339:PQN655369 QAJ655339:QAJ655369 QKF655339:QKF655369 QUB655339:QUB655369 RDX655339:RDX655369 RNT655339:RNT655369 RXP655339:RXP655369 SHL655339:SHL655369 SRH655339:SRH655369 TBD655339:TBD655369 TKZ655339:TKZ655369 TUV655339:TUV655369 UER655339:UER655369 UON655339:UON655369 UYJ655339:UYJ655369 VIF655339:VIF655369 VSB655339:VSB655369 WBX655339:WBX655369 WLT655339:WLT655369 WVP655339:WVP655369 O720875:O720905 JD720875:JD720905 SZ720875:SZ720905 ACV720875:ACV720905 AMR720875:AMR720905 AWN720875:AWN720905 BGJ720875:BGJ720905 BQF720875:BQF720905 CAB720875:CAB720905 CJX720875:CJX720905 CTT720875:CTT720905 DDP720875:DDP720905 DNL720875:DNL720905 DXH720875:DXH720905 EHD720875:EHD720905 EQZ720875:EQZ720905 FAV720875:FAV720905 FKR720875:FKR720905 FUN720875:FUN720905 GEJ720875:GEJ720905 GOF720875:GOF720905 GYB720875:GYB720905 HHX720875:HHX720905 HRT720875:HRT720905 IBP720875:IBP720905 ILL720875:ILL720905 IVH720875:IVH720905 JFD720875:JFD720905 JOZ720875:JOZ720905 JYV720875:JYV720905 KIR720875:KIR720905 KSN720875:KSN720905 LCJ720875:LCJ720905 LMF720875:LMF720905 LWB720875:LWB720905 MFX720875:MFX720905 MPT720875:MPT720905 MZP720875:MZP720905 NJL720875:NJL720905 NTH720875:NTH720905 ODD720875:ODD720905 OMZ720875:OMZ720905 OWV720875:OWV720905 PGR720875:PGR720905 PQN720875:PQN720905 QAJ720875:QAJ720905 QKF720875:QKF720905 QUB720875:QUB720905 RDX720875:RDX720905 RNT720875:RNT720905 RXP720875:RXP720905 SHL720875:SHL720905 SRH720875:SRH720905 TBD720875:TBD720905 TKZ720875:TKZ720905 TUV720875:TUV720905 UER720875:UER720905 UON720875:UON720905 UYJ720875:UYJ720905 VIF720875:VIF720905 VSB720875:VSB720905 WBX720875:WBX720905 WLT720875:WLT720905 WVP720875:WVP720905 O786411:O786441 JD786411:JD786441 SZ786411:SZ786441 ACV786411:ACV786441 AMR786411:AMR786441 AWN786411:AWN786441 BGJ786411:BGJ786441 BQF786411:BQF786441 CAB786411:CAB786441 CJX786411:CJX786441 CTT786411:CTT786441 DDP786411:DDP786441 DNL786411:DNL786441 DXH786411:DXH786441 EHD786411:EHD786441 EQZ786411:EQZ786441 FAV786411:FAV786441 FKR786411:FKR786441 FUN786411:FUN786441 GEJ786411:GEJ786441 GOF786411:GOF786441 GYB786411:GYB786441 HHX786411:HHX786441 HRT786411:HRT786441 IBP786411:IBP786441 ILL786411:ILL786441 IVH786411:IVH786441 JFD786411:JFD786441 JOZ786411:JOZ786441 JYV786411:JYV786441 KIR786411:KIR786441 KSN786411:KSN786441 LCJ786411:LCJ786441 LMF786411:LMF786441 LWB786411:LWB786441 MFX786411:MFX786441 MPT786411:MPT786441 MZP786411:MZP786441 NJL786411:NJL786441 NTH786411:NTH786441 ODD786411:ODD786441 OMZ786411:OMZ786441 OWV786411:OWV786441 PGR786411:PGR786441 PQN786411:PQN786441 QAJ786411:QAJ786441 QKF786411:QKF786441 QUB786411:QUB786441 RDX786411:RDX786441 RNT786411:RNT786441 RXP786411:RXP786441 SHL786411:SHL786441 SRH786411:SRH786441 TBD786411:TBD786441 TKZ786411:TKZ786441 TUV786411:TUV786441 UER786411:UER786441 UON786411:UON786441 UYJ786411:UYJ786441 VIF786411:VIF786441 VSB786411:VSB786441 WBX786411:WBX786441 WLT786411:WLT786441 WVP786411:WVP786441 O851947:O851977 JD851947:JD851977 SZ851947:SZ851977 ACV851947:ACV851977 AMR851947:AMR851977 AWN851947:AWN851977 BGJ851947:BGJ851977 BQF851947:BQF851977 CAB851947:CAB851977 CJX851947:CJX851977 CTT851947:CTT851977 DDP851947:DDP851977 DNL851947:DNL851977 DXH851947:DXH851977 EHD851947:EHD851977 EQZ851947:EQZ851977 FAV851947:FAV851977 FKR851947:FKR851977 FUN851947:FUN851977 GEJ851947:GEJ851977 GOF851947:GOF851977 GYB851947:GYB851977 HHX851947:HHX851977 HRT851947:HRT851977 IBP851947:IBP851977 ILL851947:ILL851977 IVH851947:IVH851977 JFD851947:JFD851977 JOZ851947:JOZ851977 JYV851947:JYV851977 KIR851947:KIR851977 KSN851947:KSN851977 LCJ851947:LCJ851977 LMF851947:LMF851977 LWB851947:LWB851977 MFX851947:MFX851977 MPT851947:MPT851977 MZP851947:MZP851977 NJL851947:NJL851977 NTH851947:NTH851977 ODD851947:ODD851977 OMZ851947:OMZ851977 OWV851947:OWV851977 PGR851947:PGR851977 PQN851947:PQN851977 QAJ851947:QAJ851977 QKF851947:QKF851977 QUB851947:QUB851977 RDX851947:RDX851977 RNT851947:RNT851977 RXP851947:RXP851977 SHL851947:SHL851977 SRH851947:SRH851977 TBD851947:TBD851977 TKZ851947:TKZ851977 TUV851947:TUV851977 UER851947:UER851977 UON851947:UON851977 UYJ851947:UYJ851977 VIF851947:VIF851977 VSB851947:VSB851977 WBX851947:WBX851977 WLT851947:WLT851977 WVP851947:WVP851977 O917483:O917513 JD917483:JD917513 SZ917483:SZ917513 ACV917483:ACV917513 AMR917483:AMR917513 AWN917483:AWN917513 BGJ917483:BGJ917513 BQF917483:BQF917513 CAB917483:CAB917513 CJX917483:CJX917513 CTT917483:CTT917513 DDP917483:DDP917513 DNL917483:DNL917513 DXH917483:DXH917513 EHD917483:EHD917513 EQZ917483:EQZ917513 FAV917483:FAV917513 FKR917483:FKR917513 FUN917483:FUN917513 GEJ917483:GEJ917513 GOF917483:GOF917513 GYB917483:GYB917513 HHX917483:HHX917513 HRT917483:HRT917513 IBP917483:IBP917513 ILL917483:ILL917513 IVH917483:IVH917513 JFD917483:JFD917513 JOZ917483:JOZ917513 JYV917483:JYV917513 KIR917483:KIR917513 KSN917483:KSN917513 LCJ917483:LCJ917513 LMF917483:LMF917513 LWB917483:LWB917513 MFX917483:MFX917513 MPT917483:MPT917513 MZP917483:MZP917513 NJL917483:NJL917513 NTH917483:NTH917513 ODD917483:ODD917513 OMZ917483:OMZ917513 OWV917483:OWV917513 PGR917483:PGR917513 PQN917483:PQN917513 QAJ917483:QAJ917513 QKF917483:QKF917513 QUB917483:QUB917513 RDX917483:RDX917513 RNT917483:RNT917513 RXP917483:RXP917513 SHL917483:SHL917513 SRH917483:SRH917513 TBD917483:TBD917513 TKZ917483:TKZ917513 TUV917483:TUV917513 UER917483:UER917513 UON917483:UON917513 UYJ917483:UYJ917513 VIF917483:VIF917513 VSB917483:VSB917513 WBX917483:WBX917513 WLT917483:WLT917513 WVP917483:WVP917513 O983019:O983049 JD983019:JD983049 SZ983019:SZ983049 ACV983019:ACV983049 AMR983019:AMR983049 AWN983019:AWN983049 BGJ983019:BGJ983049 BQF983019:BQF983049 CAB983019:CAB983049 CJX983019:CJX983049 CTT983019:CTT983049 DDP983019:DDP983049 DNL983019:DNL983049 DXH983019:DXH983049 EHD983019:EHD983049 EQZ983019:EQZ983049 FAV983019:FAV983049 FKR983019:FKR983049 FUN983019:FUN983049 GEJ983019:GEJ983049 GOF983019:GOF983049 GYB983019:GYB983049 HHX983019:HHX983049 HRT983019:HRT983049 IBP983019:IBP983049 ILL983019:ILL983049 IVH983019:IVH983049 JFD983019:JFD983049 JOZ983019:JOZ983049 JYV983019:JYV983049 KIR983019:KIR983049 KSN983019:KSN983049 LCJ983019:LCJ983049 LMF983019:LMF983049 LWB983019:LWB983049 MFX983019:MFX983049 MPT983019:MPT983049 MZP983019:MZP983049 NJL983019:NJL983049 NTH983019:NTH983049 ODD983019:ODD983049 OMZ983019:OMZ983049 OWV983019:OWV983049 PGR983019:PGR983049 PQN983019:PQN983049 QAJ983019:QAJ983049 QKF983019:QKF983049 QUB983019:QUB983049 RDX983019:RDX983049 RNT983019:RNT983049 RXP983019:RXP983049 SHL983019:SHL983049 SRH983019:SRH983049 TBD983019:TBD983049 TKZ983019:TKZ983049 TUV983019:TUV983049 UER983019:UER983049 UON983019:UON983049 UYJ983019:UYJ983049 VIF983019:VIF983049 VSB983019:VSB983049 WBX983019:WBX983049 WLT983019:WLT983049 O13:O20 O11 O9 WVP4:WVP20 WLT4:WLT20 WBX4:WBX20 VSB4:VSB20 VIF4:VIF20 UYJ4:UYJ20 UON4:UON20 UER4:UER20 TUV4:TUV20 TKZ4:TKZ20 TBD4:TBD20 SRH4:SRH20 SHL4:SHL20 RXP4:RXP20 RNT4:RNT20 RDX4:RDX20 QUB4:QUB20 QKF4:QKF20 QAJ4:QAJ20 PQN4:PQN20 PGR4:PGR20 OWV4:OWV20 OMZ4:OMZ20 ODD4:ODD20 NTH4:NTH20 NJL4:NJL20 MZP4:MZP20 MPT4:MPT20 MFX4:MFX20 LWB4:LWB20 LMF4:LMF20 LCJ4:LCJ20 KSN4:KSN20 KIR4:KIR20 JYV4:JYV20 JOZ4:JOZ20 JFD4:JFD20 IVH4:IVH20 ILL4:ILL20 IBP4:IBP20 HRT4:HRT20 HHX4:HHX20 GYB4:GYB20 GOF4:GOF20 GEJ4:GEJ20 FUN4:FUN20 FKR4:FKR20 FAV4:FAV20 EQZ4:EQZ20 EHD4:EHD20 DXH4:DXH20 DNL4:DNL20 DDP4:DDP20 CTT4:CTT20 CJX4:CJX20 CAB4:CAB20 BQF4:BQF20 BGJ4:BGJ20 AWN4:AWN20 AMR4:AMR20 ACV4:ACV20 SZ4:SZ20 JD4:JD20" xr:uid="{00000000-0002-0000-0200-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVP983019:WVP983049 O65515:O65545 JD65515:JD65545 SZ65515:SZ65545 ACV65515:ACV65545 AMR65515:AMR65545 AWN65515:AWN65545 BGJ65515:BGJ65545 BQF65515:BQF65545 CAB65515:CAB65545 CJX65515:CJX65545 CTT65515:CTT65545 DDP65515:DDP65545 DNL65515:DNL65545 DXH65515:DXH65545 EHD65515:EHD65545 EQZ65515:EQZ65545 FAV65515:FAV65545 FKR65515:FKR65545 FUN65515:FUN65545 GEJ65515:GEJ65545 GOF65515:GOF65545 GYB65515:GYB65545 HHX65515:HHX65545 HRT65515:HRT65545 IBP65515:IBP65545 ILL65515:ILL65545 IVH65515:IVH65545 JFD65515:JFD65545 JOZ65515:JOZ65545 JYV65515:JYV65545 KIR65515:KIR65545 KSN65515:KSN65545 LCJ65515:LCJ65545 LMF65515:LMF65545 LWB65515:LWB65545 MFX65515:MFX65545 MPT65515:MPT65545 MZP65515:MZP65545 NJL65515:NJL65545 NTH65515:NTH65545 ODD65515:ODD65545 OMZ65515:OMZ65545 OWV65515:OWV65545 PGR65515:PGR65545 PQN65515:PQN65545 QAJ65515:QAJ65545 QKF65515:QKF65545 QUB65515:QUB65545 RDX65515:RDX65545 RNT65515:RNT65545 RXP65515:RXP65545 SHL65515:SHL65545 SRH65515:SRH65545 TBD65515:TBD65545 TKZ65515:TKZ65545 TUV65515:TUV65545 UER65515:UER65545 UON65515:UON65545 UYJ65515:UYJ65545 VIF65515:VIF65545 VSB65515:VSB65545 WBX65515:WBX65545 WLT65515:WLT65545 WVP65515:WVP65545 O131051:O131081 JD131051:JD131081 SZ131051:SZ131081 ACV131051:ACV131081 AMR131051:AMR131081 AWN131051:AWN131081 BGJ131051:BGJ131081 BQF131051:BQF131081 CAB131051:CAB131081 CJX131051:CJX131081 CTT131051:CTT131081 DDP131051:DDP131081 DNL131051:DNL131081 DXH131051:DXH131081 EHD131051:EHD131081 EQZ131051:EQZ131081 FAV131051:FAV131081 FKR131051:FKR131081 FUN131051:FUN131081 GEJ131051:GEJ131081 GOF131051:GOF131081 GYB131051:GYB131081 HHX131051:HHX131081 HRT131051:HRT131081 IBP131051:IBP131081 ILL131051:ILL131081 IVH131051:IVH131081 JFD131051:JFD131081 JOZ131051:JOZ131081 JYV131051:JYV131081 KIR131051:KIR131081 KSN131051:KSN131081 LCJ131051:LCJ131081 LMF131051:LMF131081 LWB131051:LWB131081 MFX131051:MFX131081 MPT131051:MPT131081 MZP131051:MZP131081 NJL131051:NJL131081 NTH131051:NTH131081 ODD131051:ODD131081 OMZ131051:OMZ131081 OWV131051:OWV131081 PGR131051:PGR131081 PQN131051:PQN131081 QAJ131051:QAJ131081 QKF131051:QKF131081 QUB131051:QUB131081 RDX131051:RDX131081 RNT131051:RNT131081 RXP131051:RXP131081 SHL131051:SHL131081 SRH131051:SRH131081 TBD131051:TBD131081 TKZ131051:TKZ131081 TUV131051:TUV131081 UER131051:UER131081 UON131051:UON131081 UYJ131051:UYJ131081 VIF131051:VIF131081 VSB131051:VSB131081 WBX131051:WBX131081 WLT131051:WLT131081 WVP131051:WVP131081 O196587:O196617 JD196587:JD196617 SZ196587:SZ196617 ACV196587:ACV196617 AMR196587:AMR196617 AWN196587:AWN196617 BGJ196587:BGJ196617 BQF196587:BQF196617 CAB196587:CAB196617 CJX196587:CJX196617 CTT196587:CTT196617 DDP196587:DDP196617 DNL196587:DNL196617 DXH196587:DXH196617 EHD196587:EHD196617 EQZ196587:EQZ196617 FAV196587:FAV196617 FKR196587:FKR196617 FUN196587:FUN196617 GEJ196587:GEJ196617 GOF196587:GOF196617 GYB196587:GYB196617 HHX196587:HHX196617 HRT196587:HRT196617 IBP196587:IBP196617 ILL196587:ILL196617 IVH196587:IVH196617 JFD196587:JFD196617 JOZ196587:JOZ196617 JYV196587:JYV196617 KIR196587:KIR196617 KSN196587:KSN196617 LCJ196587:LCJ196617 LMF196587:LMF196617 LWB196587:LWB196617 MFX196587:MFX196617 MPT196587:MPT196617 MZP196587:MZP196617 NJL196587:NJL196617 NTH196587:NTH196617 ODD196587:ODD196617 OMZ196587:OMZ196617 OWV196587:OWV196617 PGR196587:PGR196617 PQN196587:PQN196617 QAJ196587:QAJ196617 QKF196587:QKF196617 QUB196587:QUB196617 RDX196587:RDX196617 RNT196587:RNT196617 RXP196587:RXP196617 SHL196587:SHL196617 SRH196587:SRH196617 TBD196587:TBD196617 TKZ196587:TKZ196617 TUV196587:TUV196617 UER196587:UER196617 UON196587:UON196617 UYJ196587:UYJ196617 VIF196587:VIF196617 VSB196587:VSB196617 WBX196587:WBX196617 WLT196587:WLT196617 WVP196587:WVP196617 O262123:O262153 JD262123:JD262153 SZ262123:SZ262153 ACV262123:ACV262153 AMR262123:AMR262153 AWN262123:AWN262153 BGJ262123:BGJ262153 BQF262123:BQF262153 CAB262123:CAB262153 CJX262123:CJX262153 CTT262123:CTT262153 DDP262123:DDP262153 DNL262123:DNL262153 DXH262123:DXH262153 EHD262123:EHD262153 EQZ262123:EQZ262153 FAV262123:FAV262153 FKR262123:FKR262153 FUN262123:FUN262153 GEJ262123:GEJ262153 GOF262123:GOF262153 GYB262123:GYB262153 HHX262123:HHX262153 HRT262123:HRT262153 IBP262123:IBP262153 ILL262123:ILL262153 IVH262123:IVH262153 JFD262123:JFD262153 JOZ262123:JOZ262153 JYV262123:JYV262153 KIR262123:KIR262153 KSN262123:KSN262153 LCJ262123:LCJ262153 LMF262123:LMF262153 LWB262123:LWB262153 MFX262123:MFX262153 MPT262123:MPT262153 MZP262123:MZP262153 NJL262123:NJL262153 NTH262123:NTH262153 ODD262123:ODD262153 OMZ262123:OMZ262153 OWV262123:OWV262153 PGR262123:PGR262153 PQN262123:PQN262153 QAJ262123:QAJ262153 QKF262123:QKF262153 QUB262123:QUB262153 RDX262123:RDX262153 RNT262123:RNT262153 RXP262123:RXP262153 SHL262123:SHL262153 SRH262123:SRH262153 TBD262123:TBD262153 TKZ262123:TKZ262153 TUV262123:TUV262153 UER262123:UER262153 UON262123:UON262153 UYJ262123:UYJ262153 VIF262123:VIF262153 VSB262123:VSB262153 WBX262123:WBX262153 WLT262123:WLT262153 WVP262123:WVP262153 O327659:O327689 JD327659:JD327689 SZ327659:SZ327689 ACV327659:ACV327689 AMR327659:AMR327689 AWN327659:AWN327689 BGJ327659:BGJ327689 BQF327659:BQF327689 CAB327659:CAB327689 CJX327659:CJX327689 CTT327659:CTT327689 DDP327659:DDP327689 DNL327659:DNL327689 DXH327659:DXH327689 EHD327659:EHD327689 EQZ327659:EQZ327689 FAV327659:FAV327689 FKR327659:FKR327689 FUN327659:FUN327689 GEJ327659:GEJ327689 GOF327659:GOF327689 GYB327659:GYB327689 HHX327659:HHX327689 HRT327659:HRT327689 IBP327659:IBP327689 ILL327659:ILL327689 IVH327659:IVH327689 JFD327659:JFD327689 JOZ327659:JOZ327689 JYV327659:JYV327689 KIR327659:KIR327689 KSN327659:KSN327689 LCJ327659:LCJ327689 LMF327659:LMF327689 LWB327659:LWB327689 MFX327659:MFX327689 MPT327659:MPT327689 MZP327659:MZP327689 NJL327659:NJL327689 NTH327659:NTH327689 ODD327659:ODD327689 OMZ327659:OMZ327689 OWV327659:OWV327689 PGR327659:PGR327689 PQN327659:PQN327689 QAJ327659:QAJ327689 QKF327659:QKF327689 QUB327659:QUB327689 RDX327659:RDX327689 RNT327659:RNT327689 RXP327659:RXP327689 SHL327659:SHL327689 SRH327659:SRH327689 TBD327659:TBD327689 TKZ327659:TKZ327689 TUV327659:TUV327689 UER327659:UER327689 UON327659:UON327689 UYJ327659:UYJ327689 VIF327659:VIF327689 VSB327659:VSB327689 WBX327659:WBX327689 WLT327659:WLT327689 WVP327659:WVP327689 O393195:O393225 JD393195:JD393225 SZ393195:SZ393225 ACV393195:ACV393225 AMR393195:AMR393225 AWN393195:AWN393225 BGJ393195:BGJ393225 BQF393195:BQF393225 CAB393195:CAB393225 CJX393195:CJX393225 CTT393195:CTT393225 DDP393195:DDP393225 DNL393195:DNL393225 DXH393195:DXH393225 EHD393195:EHD393225 EQZ393195:EQZ393225 FAV393195:FAV393225 FKR393195:FKR393225 FUN393195:FUN393225 GEJ393195:GEJ393225 GOF393195:GOF393225 GYB393195:GYB393225 HHX393195:HHX393225 HRT393195:HRT393225 IBP393195:IBP393225 ILL393195:ILL393225 IVH393195:IVH393225 JFD393195:JFD393225 JOZ393195:JOZ393225 JYV393195:JYV393225 KIR393195:KIR393225 KSN393195:KSN393225 LCJ393195:LCJ393225 LMF393195:LMF393225 LWB393195:LWB393225 MFX393195:MFX393225 MPT393195:MPT393225 MZP393195:MZP393225 NJL393195:NJL393225 NTH393195:NTH393225 ODD393195:ODD393225 OMZ393195:OMZ393225 OWV393195:OWV393225 PGR393195:PGR393225 PQN393195:PQN393225 QAJ393195:QAJ393225 QKF393195:QKF393225 QUB393195:QUB393225 RDX393195:RDX393225 RNT393195:RNT393225 RXP393195:RXP393225 SHL393195:SHL393225 SRH393195:SRH393225 TBD393195:TBD393225 TKZ393195:TKZ393225 TUV393195:TUV393225 UER393195:UER393225 UON393195:UON393225 UYJ393195:UYJ393225 VIF393195:VIF393225 VSB393195:VSB393225 WBX393195:WBX393225 WLT393195:WLT393225 WVP393195:WVP393225 O458731:O458761 JD458731:JD458761 SZ458731:SZ458761 ACV458731:ACV458761 AMR458731:AMR458761 AWN458731:AWN458761 BGJ458731:BGJ458761 BQF458731:BQF458761 CAB458731:CAB458761 CJX458731:CJX458761 CTT458731:CTT458761 DDP458731:DDP458761 DNL458731:DNL458761 DXH458731:DXH458761 EHD458731:EHD458761 EQZ458731:EQZ458761 FAV458731:FAV458761 FKR458731:FKR458761 FUN458731:FUN458761 GEJ458731:GEJ458761 GOF458731:GOF458761 GYB458731:GYB458761 HHX458731:HHX458761 HRT458731:HRT458761 IBP458731:IBP458761 ILL458731:ILL458761 IVH458731:IVH458761 JFD458731:JFD458761 JOZ458731:JOZ458761 JYV458731:JYV458761 KIR458731:KIR458761 KSN458731:KSN458761 LCJ458731:LCJ458761 LMF458731:LMF458761 LWB458731:LWB458761 MFX458731:MFX458761 MPT458731:MPT458761 MZP458731:MZP458761 NJL458731:NJL458761 NTH458731:NTH458761 ODD458731:ODD458761 OMZ458731:OMZ458761 OWV458731:OWV458761 PGR458731:PGR458761 PQN458731:PQN458761 QAJ458731:QAJ458761 QKF458731:QKF458761 QUB458731:QUB458761 RDX458731:RDX458761 RNT458731:RNT458761 RXP458731:RXP458761 SHL458731:SHL458761 SRH458731:SRH458761 TBD458731:TBD458761 TKZ458731:TKZ458761 TUV458731:TUV458761 UER458731:UER458761 UON458731:UON458761 UYJ458731:UYJ458761 VIF458731:VIF458761 VSB458731:VSB458761 WBX458731:WBX458761 WLT458731:WLT458761 WVP458731:WVP458761 O524267:O524297 JD524267:JD524297 SZ524267:SZ524297 ACV524267:ACV524297 AMR524267:AMR524297 AWN524267:AWN524297 BGJ524267:BGJ524297 BQF524267:BQF524297 CAB524267:CAB524297 CJX524267:CJX524297 CTT524267:CTT524297 DDP524267:DDP524297 DNL524267:DNL524297 DXH524267:DXH524297 EHD524267:EHD524297 EQZ524267:EQZ524297 FAV524267:FAV524297 FKR524267:FKR524297 FUN524267:FUN524297 GEJ524267:GEJ524297 GOF524267:GOF524297 GYB524267:GYB524297 HHX524267:HHX524297 HRT524267:HRT524297 IBP524267:IBP524297 ILL524267:ILL524297 IVH524267:IVH524297 JFD524267:JFD524297 JOZ524267:JOZ524297 JYV524267:JYV524297 KIR524267:KIR524297 KSN524267:KSN524297 LCJ524267:LCJ524297 LMF524267:LMF524297 LWB524267:LWB524297 MFX524267:MFX524297 MPT524267:MPT524297 MZP524267:MZP524297 NJL524267:NJL524297 NTH524267:NTH524297 ODD524267:ODD524297 OMZ524267:OMZ524297 OWV524267:OWV524297 PGR524267:PGR524297 PQN524267:PQN524297 QAJ524267:QAJ524297 QKF524267:QKF524297 QUB524267:QUB524297 RDX524267:RDX524297 RNT524267:RNT524297 RXP524267:RXP524297 SHL524267:SHL524297 SRH524267:SRH524297 TBD524267:TBD524297 TKZ524267:TKZ524297 TUV524267:TUV524297 UER524267:UER524297 UON524267:UON524297 UYJ524267:UYJ524297 VIF524267:VIF524297 VSB524267:VSB524297 WBX524267:WBX524297 WLT524267:WLT524297 WVP524267:WVP524297 O589803:O589833 JD589803:JD589833 SZ589803:SZ589833 ACV589803:ACV589833 AMR589803:AMR589833 AWN589803:AWN589833 BGJ589803:BGJ589833 BQF589803:BQF589833 CAB589803:CAB589833 CJX589803:CJX589833 CTT589803:CTT589833 DDP589803:DDP589833 DNL589803:DNL589833 DXH589803:DXH589833 EHD589803:EHD589833 EQZ589803:EQZ589833 FAV589803:FAV589833 FKR589803:FKR589833 FUN589803:FUN589833 GEJ589803:GEJ589833 GOF589803:GOF589833 GYB589803:GYB589833 HHX589803:HHX589833 HRT589803:HRT589833 IBP589803:IBP589833 ILL589803:ILL589833 IVH589803:IVH589833 JFD589803:JFD589833 JOZ589803:JOZ589833 JYV589803:JYV589833 KIR589803:KIR589833 KSN589803:KSN589833 LCJ589803:LCJ589833 LMF589803:LMF589833 LWB589803:LWB589833 MFX589803:MFX589833 MPT589803:MPT589833 MZP589803:MZP589833 NJL589803:NJL589833 NTH589803:NTH589833 ODD589803:ODD589833 OMZ589803:OMZ589833 OWV589803:OWV589833 PGR589803:PGR589833 PQN589803:PQN589833 QAJ589803:QAJ589833 QKF589803:QKF589833 QUB589803:QUB589833 RDX589803:RDX589833 RNT589803:RNT589833 RXP589803:RXP589833 SHL589803:SHL589833 SRH589803:SRH589833 TBD589803:TBD589833 TKZ589803:TKZ589833 TUV589803:TUV589833 UER589803:UER589833 UON589803:UON589833 UYJ589803:UYJ589833 VIF589803:VIF589833 VSB589803:VSB589833 WBX589803:WBX589833 WLT589803:WLT589833 WVP589803:WVP589833 O655339:O655369 JD655339:JD655369 SZ655339:SZ655369 ACV655339:ACV655369 AMR655339:AMR655369 AWN655339:AWN655369 BGJ655339:BGJ655369 BQF655339:BQF655369 CAB655339:CAB655369 CJX655339:CJX655369 CTT655339:CTT655369 DDP655339:DDP655369 DNL655339:DNL655369 DXH655339:DXH655369 EHD655339:EHD655369 EQZ655339:EQZ655369 FAV655339:FAV655369 FKR655339:FKR655369 FUN655339:FUN655369 GEJ655339:GEJ655369 GOF655339:GOF655369 GYB655339:GYB655369 HHX655339:HHX655369 HRT655339:HRT655369 IBP655339:IBP655369 ILL655339:ILL655369 IVH655339:IVH655369 JFD655339:JFD655369 JOZ655339:JOZ655369 JYV655339:JYV655369 KIR655339:KIR655369 KSN655339:KSN655369 LCJ655339:LCJ655369 LMF655339:LMF655369 LWB655339:LWB655369 MFX655339:MFX655369 MPT655339:MPT655369 MZP655339:MZP655369 NJL655339:NJL655369 NTH655339:NTH655369 ODD655339:ODD655369 OMZ655339:OMZ655369 OWV655339:OWV655369 PGR655339:PGR655369 PQN655339:PQN655369 QAJ655339:QAJ655369 QKF655339:QKF655369 QUB655339:QUB655369 RDX655339:RDX655369 RNT655339:RNT655369 RXP655339:RXP655369 SHL655339:SHL655369 SRH655339:SRH655369 TBD655339:TBD655369 TKZ655339:TKZ655369 TUV655339:TUV655369 UER655339:UER655369 UON655339:UON655369 UYJ655339:UYJ655369 VIF655339:VIF655369 VSB655339:VSB655369 WBX655339:WBX655369 WLT655339:WLT655369 WVP655339:WVP655369 O720875:O720905 JD720875:JD720905 SZ720875:SZ720905 ACV720875:ACV720905 AMR720875:AMR720905 AWN720875:AWN720905 BGJ720875:BGJ720905 BQF720875:BQF720905 CAB720875:CAB720905 CJX720875:CJX720905 CTT720875:CTT720905 DDP720875:DDP720905 DNL720875:DNL720905 DXH720875:DXH720905 EHD720875:EHD720905 EQZ720875:EQZ720905 FAV720875:FAV720905 FKR720875:FKR720905 FUN720875:FUN720905 GEJ720875:GEJ720905 GOF720875:GOF720905 GYB720875:GYB720905 HHX720875:HHX720905 HRT720875:HRT720905 IBP720875:IBP720905 ILL720875:ILL720905 IVH720875:IVH720905 JFD720875:JFD720905 JOZ720875:JOZ720905 JYV720875:JYV720905 KIR720875:KIR720905 KSN720875:KSN720905 LCJ720875:LCJ720905 LMF720875:LMF720905 LWB720875:LWB720905 MFX720875:MFX720905 MPT720875:MPT720905 MZP720875:MZP720905 NJL720875:NJL720905 NTH720875:NTH720905 ODD720875:ODD720905 OMZ720875:OMZ720905 OWV720875:OWV720905 PGR720875:PGR720905 PQN720875:PQN720905 QAJ720875:QAJ720905 QKF720875:QKF720905 QUB720875:QUB720905 RDX720875:RDX720905 RNT720875:RNT720905 RXP720875:RXP720905 SHL720875:SHL720905 SRH720875:SRH720905 TBD720875:TBD720905 TKZ720875:TKZ720905 TUV720875:TUV720905 UER720875:UER720905 UON720875:UON720905 UYJ720875:UYJ720905 VIF720875:VIF720905 VSB720875:VSB720905 WBX720875:WBX720905 WLT720875:WLT720905 WVP720875:WVP720905 O786411:O786441 JD786411:JD786441 SZ786411:SZ786441 ACV786411:ACV786441 AMR786411:AMR786441 AWN786411:AWN786441 BGJ786411:BGJ786441 BQF786411:BQF786441 CAB786411:CAB786441 CJX786411:CJX786441 CTT786411:CTT786441 DDP786411:DDP786441 DNL786411:DNL786441 DXH786411:DXH786441 EHD786411:EHD786441 EQZ786411:EQZ786441 FAV786411:FAV786441 FKR786411:FKR786441 FUN786411:FUN786441 GEJ786411:GEJ786441 GOF786411:GOF786441 GYB786411:GYB786441 HHX786411:HHX786441 HRT786411:HRT786441 IBP786411:IBP786441 ILL786411:ILL786441 IVH786411:IVH786441 JFD786411:JFD786441 JOZ786411:JOZ786441 JYV786411:JYV786441 KIR786411:KIR786441 KSN786411:KSN786441 LCJ786411:LCJ786441 LMF786411:LMF786441 LWB786411:LWB786441 MFX786411:MFX786441 MPT786411:MPT786441 MZP786411:MZP786441 NJL786411:NJL786441 NTH786411:NTH786441 ODD786411:ODD786441 OMZ786411:OMZ786441 OWV786411:OWV786441 PGR786411:PGR786441 PQN786411:PQN786441 QAJ786411:QAJ786441 QKF786411:QKF786441 QUB786411:QUB786441 RDX786411:RDX786441 RNT786411:RNT786441 RXP786411:RXP786441 SHL786411:SHL786441 SRH786411:SRH786441 TBD786411:TBD786441 TKZ786411:TKZ786441 TUV786411:TUV786441 UER786411:UER786441 UON786411:UON786441 UYJ786411:UYJ786441 VIF786411:VIF786441 VSB786411:VSB786441 WBX786411:WBX786441 WLT786411:WLT786441 WVP786411:WVP786441 O851947:O851977 JD851947:JD851977 SZ851947:SZ851977 ACV851947:ACV851977 AMR851947:AMR851977 AWN851947:AWN851977 BGJ851947:BGJ851977 BQF851947:BQF851977 CAB851947:CAB851977 CJX851947:CJX851977 CTT851947:CTT851977 DDP851947:DDP851977 DNL851947:DNL851977 DXH851947:DXH851977 EHD851947:EHD851977 EQZ851947:EQZ851977 FAV851947:FAV851977 FKR851947:FKR851977 FUN851947:FUN851977 GEJ851947:GEJ851977 GOF851947:GOF851977 GYB851947:GYB851977 HHX851947:HHX851977 HRT851947:HRT851977 IBP851947:IBP851977 ILL851947:ILL851977 IVH851947:IVH851977 JFD851947:JFD851977 JOZ851947:JOZ851977 JYV851947:JYV851977 KIR851947:KIR851977 KSN851947:KSN851977 LCJ851947:LCJ851977 LMF851947:LMF851977 LWB851947:LWB851977 MFX851947:MFX851977 MPT851947:MPT851977 MZP851947:MZP851977 NJL851947:NJL851977 NTH851947:NTH851977 ODD851947:ODD851977 OMZ851947:OMZ851977 OWV851947:OWV851977 PGR851947:PGR851977 PQN851947:PQN851977 QAJ851947:QAJ851977 QKF851947:QKF851977 QUB851947:QUB851977 RDX851947:RDX851977 RNT851947:RNT851977 RXP851947:RXP851977 SHL851947:SHL851977 SRH851947:SRH851977 TBD851947:TBD851977 TKZ851947:TKZ851977 TUV851947:TUV851977 UER851947:UER851977 UON851947:UON851977 UYJ851947:UYJ851977 VIF851947:VIF851977 VSB851947:VSB851977 WBX851947:WBX851977 WLT851947:WLT851977 WVP851947:WVP851977 O917483:O917513 JD917483:JD917513 SZ917483:SZ917513 ACV917483:ACV917513 AMR917483:AMR917513 AWN917483:AWN917513 BGJ917483:BGJ917513 BQF917483:BQF917513 CAB917483:CAB917513 CJX917483:CJX917513 CTT917483:CTT917513 DDP917483:DDP917513 DNL917483:DNL917513 DXH917483:DXH917513 EHD917483:EHD917513 EQZ917483:EQZ917513 FAV917483:FAV917513 FKR917483:FKR917513 FUN917483:FUN917513 GEJ917483:GEJ917513 GOF917483:GOF917513 GYB917483:GYB917513 HHX917483:HHX917513 HRT917483:HRT917513 IBP917483:IBP917513 ILL917483:ILL917513 IVH917483:IVH917513 JFD917483:JFD917513 JOZ917483:JOZ917513 JYV917483:JYV917513 KIR917483:KIR917513 KSN917483:KSN917513 LCJ917483:LCJ917513 LMF917483:LMF917513 LWB917483:LWB917513 MFX917483:MFX917513 MPT917483:MPT917513 MZP917483:MZP917513 NJL917483:NJL917513 NTH917483:NTH917513 ODD917483:ODD917513 OMZ917483:OMZ917513 OWV917483:OWV917513 PGR917483:PGR917513 PQN917483:PQN917513 QAJ917483:QAJ917513 QKF917483:QKF917513 QUB917483:QUB917513 RDX917483:RDX917513 RNT917483:RNT917513 RXP917483:RXP917513 SHL917483:SHL917513 SRH917483:SRH917513 TBD917483:TBD917513 TKZ917483:TKZ917513 TUV917483:TUV917513 UER917483:UER917513 UON917483:UON917513 UYJ917483:UYJ917513 VIF917483:VIF917513 VSB917483:VSB917513 WBX917483:WBX917513 WLT917483:WLT917513 WVP917483:WVP917513 O983019:O983049 JD983019:JD983049 SZ983019:SZ983049 ACV983019:ACV983049 AMR983019:AMR983049 AWN983019:AWN983049 BGJ983019:BGJ983049 BQF983019:BQF983049 CAB983019:CAB983049 CJX983019:CJX983049 CTT983019:CTT983049 DDP983019:DDP983049 DNL983019:DNL983049 DXH983019:DXH983049 EHD983019:EHD983049 EQZ983019:EQZ983049 FAV983019:FAV983049 FKR983019:FKR983049 FUN983019:FUN983049 GEJ983019:GEJ983049 GOF983019:GOF983049 GYB983019:GYB983049 HHX983019:HHX983049 HRT983019:HRT983049 IBP983019:IBP983049 ILL983019:ILL983049 IVH983019:IVH983049 JFD983019:JFD983049 JOZ983019:JOZ983049 JYV983019:JYV983049 KIR983019:KIR983049 KSN983019:KSN983049 LCJ983019:LCJ983049 LMF983019:LMF983049 LWB983019:LWB983049 MFX983019:MFX983049 MPT983019:MPT983049 MZP983019:MZP983049 NJL983019:NJL983049 NTH983019:NTH983049 ODD983019:ODD983049 OMZ983019:OMZ983049 OWV983019:OWV983049 PGR983019:PGR983049 PQN983019:PQN983049 QAJ983019:QAJ983049 QKF983019:QKF983049 QUB983019:QUB983049 RDX983019:RDX983049 RNT983019:RNT983049 RXP983019:RXP983049 SHL983019:SHL983049 SRH983019:SRH983049 TBD983019:TBD983049 TKZ983019:TKZ983049 TUV983019:TUV983049 UER983019:UER983049 UON983019:UON983049 UYJ983019:UYJ983049 VIF983019:VIF983049 VSB983019:VSB983049 WBX983019:WBX983049 WLT983019:WLT983049 O13:O20 JD4:JD20 SZ4:SZ20 ACV4:ACV20 AMR4:AMR20 AWN4:AWN20 BGJ4:BGJ20 BQF4:BQF20 CAB4:CAB20 CJX4:CJX20 CTT4:CTT20 DDP4:DDP20 DNL4:DNL20 DXH4:DXH20 EHD4:EHD20 EQZ4:EQZ20 FAV4:FAV20 FKR4:FKR20 FUN4:FUN20 GEJ4:GEJ20 GOF4:GOF20 GYB4:GYB20 HHX4:HHX20 HRT4:HRT20 IBP4:IBP20 ILL4:ILL20 IVH4:IVH20 JFD4:JFD20 JOZ4:JOZ20 JYV4:JYV20 KIR4:KIR20 KSN4:KSN20 LCJ4:LCJ20 LMF4:LMF20 LWB4:LWB20 MFX4:MFX20 MPT4:MPT20 MZP4:MZP20 NJL4:NJL20 NTH4:NTH20 ODD4:ODD20 OMZ4:OMZ20 OWV4:OWV20 PGR4:PGR20 PQN4:PQN20 QAJ4:QAJ20 QKF4:QKF20 QUB4:QUB20 RDX4:RDX20 RNT4:RNT20 RXP4:RXP20 SHL4:SHL20 SRH4:SRH20 TBD4:TBD20 TKZ4:TKZ20 TUV4:TUV20 UER4:UER20 UON4:UON20 UYJ4:UYJ20 VIF4:VIF20 VSB4:VSB20 WBX4:WBX20 WLT4:WLT20 WVP4:WVP20 O9 O11" xr:uid="{00000000-0002-0000-0200-00000D000000}">
       <formula1>"18-25 años,26-35 años,36-45 años,46 a 55 años,55-65 años, mayor de 65 años"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JA65515:JA65545 SW65515:SW65545 ACS65515:ACS65545 AMO65515:AMO65545 AWK65515:AWK65545 BGG65515:BGG65545 BQC65515:BQC65545 BZY65515:BZY65545 CJU65515:CJU65545 CTQ65515:CTQ65545 DDM65515:DDM65545 DNI65515:DNI65545 DXE65515:DXE65545 EHA65515:EHA65545 EQW65515:EQW65545 FAS65515:FAS65545 FKO65515:FKO65545 FUK65515:FUK65545 GEG65515:GEG65545 GOC65515:GOC65545 GXY65515:GXY65545 HHU65515:HHU65545 HRQ65515:HRQ65545 IBM65515:IBM65545 ILI65515:ILI65545 IVE65515:IVE65545 JFA65515:JFA65545 JOW65515:JOW65545 JYS65515:JYS65545 KIO65515:KIO65545 KSK65515:KSK65545 LCG65515:LCG65545 LMC65515:LMC65545 LVY65515:LVY65545 MFU65515:MFU65545 MPQ65515:MPQ65545 MZM65515:MZM65545 NJI65515:NJI65545 NTE65515:NTE65545 ODA65515:ODA65545 OMW65515:OMW65545 OWS65515:OWS65545 PGO65515:PGO65545 PQK65515:PQK65545 QAG65515:QAG65545 QKC65515:QKC65545 QTY65515:QTY65545 RDU65515:RDU65545 RNQ65515:RNQ65545 RXM65515:RXM65545 SHI65515:SHI65545 SRE65515:SRE65545 TBA65515:TBA65545 TKW65515:TKW65545 TUS65515:TUS65545 UEO65515:UEO65545 UOK65515:UOK65545 UYG65515:UYG65545 VIC65515:VIC65545 VRY65515:VRY65545 WBU65515:WBU65545 WLQ65515:WLQ65545 WVM65515:WVM65545 JA131051:JA131081 SW131051:SW131081 ACS131051:ACS131081 AMO131051:AMO131081 AWK131051:AWK131081 BGG131051:BGG131081 BQC131051:BQC131081 BZY131051:BZY131081 CJU131051:CJU131081 CTQ131051:CTQ131081 DDM131051:DDM131081 DNI131051:DNI131081 DXE131051:DXE131081 EHA131051:EHA131081 EQW131051:EQW131081 FAS131051:FAS131081 FKO131051:FKO131081 FUK131051:FUK131081 GEG131051:GEG131081 GOC131051:GOC131081 GXY131051:GXY131081 HHU131051:HHU131081 HRQ131051:HRQ131081 IBM131051:IBM131081 ILI131051:ILI131081 IVE131051:IVE131081 JFA131051:JFA131081 JOW131051:JOW131081 JYS131051:JYS131081 KIO131051:KIO131081 KSK131051:KSK131081 LCG131051:LCG131081 LMC131051:LMC131081 LVY131051:LVY131081 MFU131051:MFU131081 MPQ131051:MPQ131081 MZM131051:MZM131081 NJI131051:NJI131081 NTE131051:NTE131081 ODA131051:ODA131081 OMW131051:OMW131081 OWS131051:OWS131081 PGO131051:PGO131081 PQK131051:PQK131081 QAG131051:QAG131081 QKC131051:QKC131081 QTY131051:QTY131081 RDU131051:RDU131081 RNQ131051:RNQ131081 RXM131051:RXM131081 SHI131051:SHI131081 SRE131051:SRE131081 TBA131051:TBA131081 TKW131051:TKW131081 TUS131051:TUS131081 UEO131051:UEO131081 UOK131051:UOK131081 UYG131051:UYG131081 VIC131051:VIC131081 VRY131051:VRY131081 WBU131051:WBU131081 WLQ131051:WLQ131081 WVM131051:WVM131081 JA196587:JA196617 SW196587:SW196617 ACS196587:ACS196617 AMO196587:AMO196617 AWK196587:AWK196617 BGG196587:BGG196617 BQC196587:BQC196617 BZY196587:BZY196617 CJU196587:CJU196617 CTQ196587:CTQ196617 DDM196587:DDM196617 DNI196587:DNI196617 DXE196587:DXE196617 EHA196587:EHA196617 EQW196587:EQW196617 FAS196587:FAS196617 FKO196587:FKO196617 FUK196587:FUK196617 GEG196587:GEG196617 GOC196587:GOC196617 GXY196587:GXY196617 HHU196587:HHU196617 HRQ196587:HRQ196617 IBM196587:IBM196617 ILI196587:ILI196617 IVE196587:IVE196617 JFA196587:JFA196617 JOW196587:JOW196617 JYS196587:JYS196617 KIO196587:KIO196617 KSK196587:KSK196617 LCG196587:LCG196617 LMC196587:LMC196617 LVY196587:LVY196617 MFU196587:MFU196617 MPQ196587:MPQ196617 MZM196587:MZM196617 NJI196587:NJI196617 NTE196587:NTE196617 ODA196587:ODA196617 OMW196587:OMW196617 OWS196587:OWS196617 PGO196587:PGO196617 PQK196587:PQK196617 QAG196587:QAG196617 QKC196587:QKC196617 QTY196587:QTY196617 RDU196587:RDU196617 RNQ196587:RNQ196617 RXM196587:RXM196617 SHI196587:SHI196617 SRE196587:SRE196617 TBA196587:TBA196617 TKW196587:TKW196617 TUS196587:TUS196617 UEO196587:UEO196617 UOK196587:UOK196617 UYG196587:UYG196617 VIC196587:VIC196617 VRY196587:VRY196617 WBU196587:WBU196617 WLQ196587:WLQ196617 WVM196587:WVM196617 JA262123:JA262153 SW262123:SW262153 ACS262123:ACS262153 AMO262123:AMO262153 AWK262123:AWK262153 BGG262123:BGG262153 BQC262123:BQC262153 BZY262123:BZY262153 CJU262123:CJU262153 CTQ262123:CTQ262153 DDM262123:DDM262153 DNI262123:DNI262153 DXE262123:DXE262153 EHA262123:EHA262153 EQW262123:EQW262153 FAS262123:FAS262153 FKO262123:FKO262153 FUK262123:FUK262153 GEG262123:GEG262153 GOC262123:GOC262153 GXY262123:GXY262153 HHU262123:HHU262153 HRQ262123:HRQ262153 IBM262123:IBM262153 ILI262123:ILI262153 IVE262123:IVE262153 JFA262123:JFA262153 JOW262123:JOW262153 JYS262123:JYS262153 KIO262123:KIO262153 KSK262123:KSK262153 LCG262123:LCG262153 LMC262123:LMC262153 LVY262123:LVY262153 MFU262123:MFU262153 MPQ262123:MPQ262153 MZM262123:MZM262153 NJI262123:NJI262153 NTE262123:NTE262153 ODA262123:ODA262153 OMW262123:OMW262153 OWS262123:OWS262153 PGO262123:PGO262153 PQK262123:PQK262153 QAG262123:QAG262153 QKC262123:QKC262153 QTY262123:QTY262153 RDU262123:RDU262153 RNQ262123:RNQ262153 RXM262123:RXM262153 SHI262123:SHI262153 SRE262123:SRE262153 TBA262123:TBA262153 TKW262123:TKW262153 TUS262123:TUS262153 UEO262123:UEO262153 UOK262123:UOK262153 UYG262123:UYG262153 VIC262123:VIC262153 VRY262123:VRY262153 WBU262123:WBU262153 WLQ262123:WLQ262153 WVM262123:WVM262153 JA327659:JA327689 SW327659:SW327689 ACS327659:ACS327689 AMO327659:AMO327689 AWK327659:AWK327689 BGG327659:BGG327689 BQC327659:BQC327689 BZY327659:BZY327689 CJU327659:CJU327689 CTQ327659:CTQ327689 DDM327659:DDM327689 DNI327659:DNI327689 DXE327659:DXE327689 EHA327659:EHA327689 EQW327659:EQW327689 FAS327659:FAS327689 FKO327659:FKO327689 FUK327659:FUK327689 GEG327659:GEG327689 GOC327659:GOC327689 GXY327659:GXY327689 HHU327659:HHU327689 HRQ327659:HRQ327689 IBM327659:IBM327689 ILI327659:ILI327689 IVE327659:IVE327689 JFA327659:JFA327689 JOW327659:JOW327689 JYS327659:JYS327689 KIO327659:KIO327689 KSK327659:KSK327689 LCG327659:LCG327689 LMC327659:LMC327689 LVY327659:LVY327689 MFU327659:MFU327689 MPQ327659:MPQ327689 MZM327659:MZM327689 NJI327659:NJI327689 NTE327659:NTE327689 ODA327659:ODA327689 OMW327659:OMW327689 OWS327659:OWS327689 PGO327659:PGO327689 PQK327659:PQK327689 QAG327659:QAG327689 QKC327659:QKC327689 QTY327659:QTY327689 RDU327659:RDU327689 RNQ327659:RNQ327689 RXM327659:RXM327689 SHI327659:SHI327689 SRE327659:SRE327689 TBA327659:TBA327689 TKW327659:TKW327689 TUS327659:TUS327689 UEO327659:UEO327689 UOK327659:UOK327689 UYG327659:UYG327689 VIC327659:VIC327689 VRY327659:VRY327689 WBU327659:WBU327689 WLQ327659:WLQ327689 WVM327659:WVM327689 JA393195:JA393225 SW393195:SW393225 ACS393195:ACS393225 AMO393195:AMO393225 AWK393195:AWK393225 BGG393195:BGG393225 BQC393195:BQC393225 BZY393195:BZY393225 CJU393195:CJU393225 CTQ393195:CTQ393225 DDM393195:DDM393225 DNI393195:DNI393225 DXE393195:DXE393225 EHA393195:EHA393225 EQW393195:EQW393225 FAS393195:FAS393225 FKO393195:FKO393225 FUK393195:FUK393225 GEG393195:GEG393225 GOC393195:GOC393225 GXY393195:GXY393225 HHU393195:HHU393225 HRQ393195:HRQ393225 IBM393195:IBM393225 ILI393195:ILI393225 IVE393195:IVE393225 JFA393195:JFA393225 JOW393195:JOW393225 JYS393195:JYS393225 KIO393195:KIO393225 KSK393195:KSK393225 LCG393195:LCG393225 LMC393195:LMC393225 LVY393195:LVY393225 MFU393195:MFU393225 MPQ393195:MPQ393225 MZM393195:MZM393225 NJI393195:NJI393225 NTE393195:NTE393225 ODA393195:ODA393225 OMW393195:OMW393225 OWS393195:OWS393225 PGO393195:PGO393225 PQK393195:PQK393225 QAG393195:QAG393225 QKC393195:QKC393225 QTY393195:QTY393225 RDU393195:RDU393225 RNQ393195:RNQ393225 RXM393195:RXM393225 SHI393195:SHI393225 SRE393195:SRE393225 TBA393195:TBA393225 TKW393195:TKW393225 TUS393195:TUS393225 UEO393195:UEO393225 UOK393195:UOK393225 UYG393195:UYG393225 VIC393195:VIC393225 VRY393195:VRY393225 WBU393195:WBU393225 WLQ393195:WLQ393225 WVM393195:WVM393225 JA458731:JA458761 SW458731:SW458761 ACS458731:ACS458761 AMO458731:AMO458761 AWK458731:AWK458761 BGG458731:BGG458761 BQC458731:BQC458761 BZY458731:BZY458761 CJU458731:CJU458761 CTQ458731:CTQ458761 DDM458731:DDM458761 DNI458731:DNI458761 DXE458731:DXE458761 EHA458731:EHA458761 EQW458731:EQW458761 FAS458731:FAS458761 FKO458731:FKO458761 FUK458731:FUK458761 GEG458731:GEG458761 GOC458731:GOC458761 GXY458731:GXY458761 HHU458731:HHU458761 HRQ458731:HRQ458761 IBM458731:IBM458761 ILI458731:ILI458761 IVE458731:IVE458761 JFA458731:JFA458761 JOW458731:JOW458761 JYS458731:JYS458761 KIO458731:KIO458761 KSK458731:KSK458761 LCG458731:LCG458761 LMC458731:LMC458761 LVY458731:LVY458761 MFU458731:MFU458761 MPQ458731:MPQ458761 MZM458731:MZM458761 NJI458731:NJI458761 NTE458731:NTE458761 ODA458731:ODA458761 OMW458731:OMW458761 OWS458731:OWS458761 PGO458731:PGO458761 PQK458731:PQK458761 QAG458731:QAG458761 QKC458731:QKC458761 QTY458731:QTY458761 RDU458731:RDU458761 RNQ458731:RNQ458761 RXM458731:RXM458761 SHI458731:SHI458761 SRE458731:SRE458761 TBA458731:TBA458761 TKW458731:TKW458761 TUS458731:TUS458761 UEO458731:UEO458761 UOK458731:UOK458761 UYG458731:UYG458761 VIC458731:VIC458761 VRY458731:VRY458761 WBU458731:WBU458761 WLQ458731:WLQ458761 WVM458731:WVM458761 JA524267:JA524297 SW524267:SW524297 ACS524267:ACS524297 AMO524267:AMO524297 AWK524267:AWK524297 BGG524267:BGG524297 BQC524267:BQC524297 BZY524267:BZY524297 CJU524267:CJU524297 CTQ524267:CTQ524297 DDM524267:DDM524297 DNI524267:DNI524297 DXE524267:DXE524297 EHA524267:EHA524297 EQW524267:EQW524297 FAS524267:FAS524297 FKO524267:FKO524297 FUK524267:FUK524297 GEG524267:GEG524297 GOC524267:GOC524297 GXY524267:GXY524297 HHU524267:HHU524297 HRQ524267:HRQ524297 IBM524267:IBM524297 ILI524267:ILI524297 IVE524267:IVE524297 JFA524267:JFA524297 JOW524267:JOW524297 JYS524267:JYS524297 KIO524267:KIO524297 KSK524267:KSK524297 LCG524267:LCG524297 LMC524267:LMC524297 LVY524267:LVY524297 MFU524267:MFU524297 MPQ524267:MPQ524297 MZM524267:MZM524297 NJI524267:NJI524297 NTE524267:NTE524297 ODA524267:ODA524297 OMW524267:OMW524297 OWS524267:OWS524297 PGO524267:PGO524297 PQK524267:PQK524297 QAG524267:QAG524297 QKC524267:QKC524297 QTY524267:QTY524297 RDU524267:RDU524297 RNQ524267:RNQ524297 RXM524267:RXM524297 SHI524267:SHI524297 SRE524267:SRE524297 TBA524267:TBA524297 TKW524267:TKW524297 TUS524267:TUS524297 UEO524267:UEO524297 UOK524267:UOK524297 UYG524267:UYG524297 VIC524267:VIC524297 VRY524267:VRY524297 WBU524267:WBU524297 WLQ524267:WLQ524297 WVM524267:WVM524297 JA589803:JA589833 SW589803:SW589833 ACS589803:ACS589833 AMO589803:AMO589833 AWK589803:AWK589833 BGG589803:BGG589833 BQC589803:BQC589833 BZY589803:BZY589833 CJU589803:CJU589833 CTQ589803:CTQ589833 DDM589803:DDM589833 DNI589803:DNI589833 DXE589803:DXE589833 EHA589803:EHA589833 EQW589803:EQW589833 FAS589803:FAS589833 FKO589803:FKO589833 FUK589803:FUK589833 GEG589803:GEG589833 GOC589803:GOC589833 GXY589803:GXY589833 HHU589803:HHU589833 HRQ589803:HRQ589833 IBM589803:IBM589833 ILI589803:ILI589833 IVE589803:IVE589833 JFA589803:JFA589833 JOW589803:JOW589833 JYS589803:JYS589833 KIO589803:KIO589833 KSK589803:KSK589833 LCG589803:LCG589833 LMC589803:LMC589833 LVY589803:LVY589833 MFU589803:MFU589833 MPQ589803:MPQ589833 MZM589803:MZM589833 NJI589803:NJI589833 NTE589803:NTE589833 ODA589803:ODA589833 OMW589803:OMW589833 OWS589803:OWS589833 PGO589803:PGO589833 PQK589803:PQK589833 QAG589803:QAG589833 QKC589803:QKC589833 QTY589803:QTY589833 RDU589803:RDU589833 RNQ589803:RNQ589833 RXM589803:RXM589833 SHI589803:SHI589833 SRE589803:SRE589833 TBA589803:TBA589833 TKW589803:TKW589833 TUS589803:TUS589833 UEO589803:UEO589833 UOK589803:UOK589833 UYG589803:UYG589833 VIC589803:VIC589833 VRY589803:VRY589833 WBU589803:WBU589833 WLQ589803:WLQ589833 WVM589803:WVM589833 JA655339:JA655369 SW655339:SW655369 ACS655339:ACS655369 AMO655339:AMO655369 AWK655339:AWK655369 BGG655339:BGG655369 BQC655339:BQC655369 BZY655339:BZY655369 CJU655339:CJU655369 CTQ655339:CTQ655369 DDM655339:DDM655369 DNI655339:DNI655369 DXE655339:DXE655369 EHA655339:EHA655369 EQW655339:EQW655369 FAS655339:FAS655369 FKO655339:FKO655369 FUK655339:FUK655369 GEG655339:GEG655369 GOC655339:GOC655369 GXY655339:GXY655369 HHU655339:HHU655369 HRQ655339:HRQ655369 IBM655339:IBM655369 ILI655339:ILI655369 IVE655339:IVE655369 JFA655339:JFA655369 JOW655339:JOW655369 JYS655339:JYS655369 KIO655339:KIO655369 KSK655339:KSK655369 LCG655339:LCG655369 LMC655339:LMC655369 LVY655339:LVY655369 MFU655339:MFU655369 MPQ655339:MPQ655369 MZM655339:MZM655369 NJI655339:NJI655369 NTE655339:NTE655369 ODA655339:ODA655369 OMW655339:OMW655369 OWS655339:OWS655369 PGO655339:PGO655369 PQK655339:PQK655369 QAG655339:QAG655369 QKC655339:QKC655369 QTY655339:QTY655369 RDU655339:RDU655369 RNQ655339:RNQ655369 RXM655339:RXM655369 SHI655339:SHI655369 SRE655339:SRE655369 TBA655339:TBA655369 TKW655339:TKW655369 TUS655339:TUS655369 UEO655339:UEO655369 UOK655339:UOK655369 UYG655339:UYG655369 VIC655339:VIC655369 VRY655339:VRY655369 WBU655339:WBU655369 WLQ655339:WLQ655369 WVM655339:WVM655369 JA720875:JA720905 SW720875:SW720905 ACS720875:ACS720905 AMO720875:AMO720905 AWK720875:AWK720905 BGG720875:BGG720905 BQC720875:BQC720905 BZY720875:BZY720905 CJU720875:CJU720905 CTQ720875:CTQ720905 DDM720875:DDM720905 DNI720875:DNI720905 DXE720875:DXE720905 EHA720875:EHA720905 EQW720875:EQW720905 FAS720875:FAS720905 FKO720875:FKO720905 FUK720875:FUK720905 GEG720875:GEG720905 GOC720875:GOC720905 GXY720875:GXY720905 HHU720875:HHU720905 HRQ720875:HRQ720905 IBM720875:IBM720905 ILI720875:ILI720905 IVE720875:IVE720905 JFA720875:JFA720905 JOW720875:JOW720905 JYS720875:JYS720905 KIO720875:KIO720905 KSK720875:KSK720905 LCG720875:LCG720905 LMC720875:LMC720905 LVY720875:LVY720905 MFU720875:MFU720905 MPQ720875:MPQ720905 MZM720875:MZM720905 NJI720875:NJI720905 NTE720875:NTE720905 ODA720875:ODA720905 OMW720875:OMW720905 OWS720875:OWS720905 PGO720875:PGO720905 PQK720875:PQK720905 QAG720875:QAG720905 QKC720875:QKC720905 QTY720875:QTY720905 RDU720875:RDU720905 RNQ720875:RNQ720905 RXM720875:RXM720905 SHI720875:SHI720905 SRE720875:SRE720905 TBA720875:TBA720905 TKW720875:TKW720905 TUS720875:TUS720905 UEO720875:UEO720905 UOK720875:UOK720905 UYG720875:UYG720905 VIC720875:VIC720905 VRY720875:VRY720905 WBU720875:WBU720905 WLQ720875:WLQ720905 WVM720875:WVM720905 JA786411:JA786441 SW786411:SW786441 ACS786411:ACS786441 AMO786411:AMO786441 AWK786411:AWK786441 BGG786411:BGG786441 BQC786411:BQC786441 BZY786411:BZY786441 CJU786411:CJU786441 CTQ786411:CTQ786441 DDM786411:DDM786441 DNI786411:DNI786441 DXE786411:DXE786441 EHA786411:EHA786441 EQW786411:EQW786441 FAS786411:FAS786441 FKO786411:FKO786441 FUK786411:FUK786441 GEG786411:GEG786441 GOC786411:GOC786441 GXY786411:GXY786441 HHU786411:HHU786441 HRQ786411:HRQ786441 IBM786411:IBM786441 ILI786411:ILI786441 IVE786411:IVE786441 JFA786411:JFA786441 JOW786411:JOW786441 JYS786411:JYS786441 KIO786411:KIO786441 KSK786411:KSK786441 LCG786411:LCG786441 LMC786411:LMC786441 LVY786411:LVY786441 MFU786411:MFU786441 MPQ786411:MPQ786441 MZM786411:MZM786441 NJI786411:NJI786441 NTE786411:NTE786441 ODA786411:ODA786441 OMW786411:OMW786441 OWS786411:OWS786441 PGO786411:PGO786441 PQK786411:PQK786441 QAG786411:QAG786441 QKC786411:QKC786441 QTY786411:QTY786441 RDU786411:RDU786441 RNQ786411:RNQ786441 RXM786411:RXM786441 SHI786411:SHI786441 SRE786411:SRE786441 TBA786411:TBA786441 TKW786411:TKW786441 TUS786411:TUS786441 UEO786411:UEO786441 UOK786411:UOK786441 UYG786411:UYG786441 VIC786411:VIC786441 VRY786411:VRY786441 WBU786411:WBU786441 WLQ786411:WLQ786441 WVM786411:WVM786441 JA851947:JA851977 SW851947:SW851977 ACS851947:ACS851977 AMO851947:AMO851977 AWK851947:AWK851977 BGG851947:BGG851977 BQC851947:BQC851977 BZY851947:BZY851977 CJU851947:CJU851977 CTQ851947:CTQ851977 DDM851947:DDM851977 DNI851947:DNI851977 DXE851947:DXE851977 EHA851947:EHA851977 EQW851947:EQW851977 FAS851947:FAS851977 FKO851947:FKO851977 FUK851947:FUK851977 GEG851947:GEG851977 GOC851947:GOC851977 GXY851947:GXY851977 HHU851947:HHU851977 HRQ851947:HRQ851977 IBM851947:IBM851977 ILI851947:ILI851977 IVE851947:IVE851977 JFA851947:JFA851977 JOW851947:JOW851977 JYS851947:JYS851977 KIO851947:KIO851977 KSK851947:KSK851977 LCG851947:LCG851977 LMC851947:LMC851977 LVY851947:LVY851977 MFU851947:MFU851977 MPQ851947:MPQ851977 MZM851947:MZM851977 NJI851947:NJI851977 NTE851947:NTE851977 ODA851947:ODA851977 OMW851947:OMW851977 OWS851947:OWS851977 PGO851947:PGO851977 PQK851947:PQK851977 QAG851947:QAG851977 QKC851947:QKC851977 QTY851947:QTY851977 RDU851947:RDU851977 RNQ851947:RNQ851977 RXM851947:RXM851977 SHI851947:SHI851977 SRE851947:SRE851977 TBA851947:TBA851977 TKW851947:TKW851977 TUS851947:TUS851977 UEO851947:UEO851977 UOK851947:UOK851977 UYG851947:UYG851977 VIC851947:VIC851977 VRY851947:VRY851977 WBU851947:WBU851977 WLQ851947:WLQ851977 WVM851947:WVM851977 JA917483:JA917513 SW917483:SW917513 ACS917483:ACS917513 AMO917483:AMO917513 AWK917483:AWK917513 BGG917483:BGG917513 BQC917483:BQC917513 BZY917483:BZY917513 CJU917483:CJU917513 CTQ917483:CTQ917513 DDM917483:DDM917513 DNI917483:DNI917513 DXE917483:DXE917513 EHA917483:EHA917513 EQW917483:EQW917513 FAS917483:FAS917513 FKO917483:FKO917513 FUK917483:FUK917513 GEG917483:GEG917513 GOC917483:GOC917513 GXY917483:GXY917513 HHU917483:HHU917513 HRQ917483:HRQ917513 IBM917483:IBM917513 ILI917483:ILI917513 IVE917483:IVE917513 JFA917483:JFA917513 JOW917483:JOW917513 JYS917483:JYS917513 KIO917483:KIO917513 KSK917483:KSK917513 LCG917483:LCG917513 LMC917483:LMC917513 LVY917483:LVY917513 MFU917483:MFU917513 MPQ917483:MPQ917513 MZM917483:MZM917513 NJI917483:NJI917513 NTE917483:NTE917513 ODA917483:ODA917513 OMW917483:OMW917513 OWS917483:OWS917513 PGO917483:PGO917513 PQK917483:PQK917513 QAG917483:QAG917513 QKC917483:QKC917513 QTY917483:QTY917513 RDU917483:RDU917513 RNQ917483:RNQ917513 RXM917483:RXM917513 SHI917483:SHI917513 SRE917483:SRE917513 TBA917483:TBA917513 TKW917483:TKW917513 TUS917483:TUS917513 UEO917483:UEO917513 UOK917483:UOK917513 UYG917483:UYG917513 VIC917483:VIC917513 VRY917483:VRY917513 WBU917483:WBU917513 WLQ917483:WLQ917513 WVM917483:WVM917513 JA983019:JA983049 SW983019:SW983049 ACS983019:ACS983049 AMO983019:AMO983049 AWK983019:AWK983049 BGG983019:BGG983049 BQC983019:BQC983049 BZY983019:BZY983049 CJU983019:CJU983049 CTQ983019:CTQ983049 DDM983019:DDM983049 DNI983019:DNI983049 DXE983019:DXE983049 EHA983019:EHA983049 EQW983019:EQW983049 FAS983019:FAS983049 FKO983019:FKO983049 FUK983019:FUK983049 GEG983019:GEG983049 GOC983019:GOC983049 GXY983019:GXY983049 HHU983019:HHU983049 HRQ983019:HRQ983049 IBM983019:IBM983049 ILI983019:ILI983049 IVE983019:IVE983049 JFA983019:JFA983049 JOW983019:JOW983049 JYS983019:JYS983049 KIO983019:KIO983049 KSK983019:KSK983049 LCG983019:LCG983049 LMC983019:LMC983049 LVY983019:LVY983049 MFU983019:MFU983049 MPQ983019:MPQ983049 MZM983019:MZM983049 NJI983019:NJI983049 NTE983019:NTE983049 ODA983019:ODA983049 OMW983019:OMW983049 OWS983019:OWS983049 PGO983019:PGO983049 PQK983019:PQK983049 QAG983019:QAG983049 QKC983019:QKC983049 QTY983019:QTY983049 RDU983019:RDU983049 RNQ983019:RNQ983049 RXM983019:RXM983049 SHI983019:SHI983049 SRE983019:SRE983049 TBA983019:TBA983049 TKW983019:TKW983049 TUS983019:TUS983049 UEO983019:UEO983049 UOK983019:UOK983049 UYG983019:UYG983049 VIC983019:VIC983049 VRY983019:VRY983049 WBU983019:WBU983049 WLQ983019:WLQ983049 WVM983019:WVM983049 A983019:B983049 A65515:B65545 A131051:B131081 A196587:B196617 A262123:B262153 A327659:B327689 A393195:B393225 A458731:B458761 A524267:B524297 A589803:B589833 A655339:B655369 A720875:B720905 A786411:B786441 A851947:B851977 A917483:B917513 WVM4:WVM20 WLQ4:WLQ20 WBU4:WBU20 VRY4:VRY20 VIC4:VIC20 UYG4:UYG20 UOK4:UOK20 UEO4:UEO20 TUS4:TUS20 TKW4:TKW20 TBA4:TBA20 SRE4:SRE20 SHI4:SHI20 RXM4:RXM20 RNQ4:RNQ20 RDU4:RDU20 QTY4:QTY20 QKC4:QKC20 QAG4:QAG20 PQK4:PQK20 PGO4:PGO20 OWS4:OWS20 OMW4:OMW20 ODA4:ODA20 NTE4:NTE20 NJI4:NJI20 MZM4:MZM20 MPQ4:MPQ20 MFU4:MFU20 LVY4:LVY20 LMC4:LMC20 LCG4:LCG20 KSK4:KSK20 KIO4:KIO20 JYS4:JYS20 JOW4:JOW20 JFA4:JFA20 IVE4:IVE20 ILI4:ILI20 IBM4:IBM20 HRQ4:HRQ20 HHU4:HHU20 GXY4:GXY20 GOC4:GOC20 GEG4:GEG20 FUK4:FUK20 FKO4:FKO20 FAS4:FAS20 EQW4:EQW20 EHA4:EHA20 DXE4:DXE20 DNI4:DNI20 DDM4:DDM20 CTQ4:CTQ20 CJU4:CJU20 BZY4:BZY20 BQC4:BQC20 BGG4:BGG20 AWK4:AWK20 AMO4:AMO20 ACS4:ACS20 SW4:SW20 JA4:JA20" xr:uid="{00000000-0002-0000-0200-00000E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JA65515:JA65545 SW65515:SW65545 ACS65515:ACS65545 AMO65515:AMO65545 AWK65515:AWK65545 BGG65515:BGG65545 BQC65515:BQC65545 BZY65515:BZY65545 CJU65515:CJU65545 CTQ65515:CTQ65545 DDM65515:DDM65545 DNI65515:DNI65545 DXE65515:DXE65545 EHA65515:EHA65545 EQW65515:EQW65545 FAS65515:FAS65545 FKO65515:FKO65545 FUK65515:FUK65545 GEG65515:GEG65545 GOC65515:GOC65545 GXY65515:GXY65545 HHU65515:HHU65545 HRQ65515:HRQ65545 IBM65515:IBM65545 ILI65515:ILI65545 IVE65515:IVE65545 JFA65515:JFA65545 JOW65515:JOW65545 JYS65515:JYS65545 KIO65515:KIO65545 KSK65515:KSK65545 LCG65515:LCG65545 LMC65515:LMC65545 LVY65515:LVY65545 MFU65515:MFU65545 MPQ65515:MPQ65545 MZM65515:MZM65545 NJI65515:NJI65545 NTE65515:NTE65545 ODA65515:ODA65545 OMW65515:OMW65545 OWS65515:OWS65545 PGO65515:PGO65545 PQK65515:PQK65545 QAG65515:QAG65545 QKC65515:QKC65545 QTY65515:QTY65545 RDU65515:RDU65545 RNQ65515:RNQ65545 RXM65515:RXM65545 SHI65515:SHI65545 SRE65515:SRE65545 TBA65515:TBA65545 TKW65515:TKW65545 TUS65515:TUS65545 UEO65515:UEO65545 UOK65515:UOK65545 UYG65515:UYG65545 VIC65515:VIC65545 VRY65515:VRY65545 WBU65515:WBU65545 WLQ65515:WLQ65545 WVM65515:WVM65545 JA131051:JA131081 SW131051:SW131081 ACS131051:ACS131081 AMO131051:AMO131081 AWK131051:AWK131081 BGG131051:BGG131081 BQC131051:BQC131081 BZY131051:BZY131081 CJU131051:CJU131081 CTQ131051:CTQ131081 DDM131051:DDM131081 DNI131051:DNI131081 DXE131051:DXE131081 EHA131051:EHA131081 EQW131051:EQW131081 FAS131051:FAS131081 FKO131051:FKO131081 FUK131051:FUK131081 GEG131051:GEG131081 GOC131051:GOC131081 GXY131051:GXY131081 HHU131051:HHU131081 HRQ131051:HRQ131081 IBM131051:IBM131081 ILI131051:ILI131081 IVE131051:IVE131081 JFA131051:JFA131081 JOW131051:JOW131081 JYS131051:JYS131081 KIO131051:KIO131081 KSK131051:KSK131081 LCG131051:LCG131081 LMC131051:LMC131081 LVY131051:LVY131081 MFU131051:MFU131081 MPQ131051:MPQ131081 MZM131051:MZM131081 NJI131051:NJI131081 NTE131051:NTE131081 ODA131051:ODA131081 OMW131051:OMW131081 OWS131051:OWS131081 PGO131051:PGO131081 PQK131051:PQK131081 QAG131051:QAG131081 QKC131051:QKC131081 QTY131051:QTY131081 RDU131051:RDU131081 RNQ131051:RNQ131081 RXM131051:RXM131081 SHI131051:SHI131081 SRE131051:SRE131081 TBA131051:TBA131081 TKW131051:TKW131081 TUS131051:TUS131081 UEO131051:UEO131081 UOK131051:UOK131081 UYG131051:UYG131081 VIC131051:VIC131081 VRY131051:VRY131081 WBU131051:WBU131081 WLQ131051:WLQ131081 WVM131051:WVM131081 JA196587:JA196617 SW196587:SW196617 ACS196587:ACS196617 AMO196587:AMO196617 AWK196587:AWK196617 BGG196587:BGG196617 BQC196587:BQC196617 BZY196587:BZY196617 CJU196587:CJU196617 CTQ196587:CTQ196617 DDM196587:DDM196617 DNI196587:DNI196617 DXE196587:DXE196617 EHA196587:EHA196617 EQW196587:EQW196617 FAS196587:FAS196617 FKO196587:FKO196617 FUK196587:FUK196617 GEG196587:GEG196617 GOC196587:GOC196617 GXY196587:GXY196617 HHU196587:HHU196617 HRQ196587:HRQ196617 IBM196587:IBM196617 ILI196587:ILI196617 IVE196587:IVE196617 JFA196587:JFA196617 JOW196587:JOW196617 JYS196587:JYS196617 KIO196587:KIO196617 KSK196587:KSK196617 LCG196587:LCG196617 LMC196587:LMC196617 LVY196587:LVY196617 MFU196587:MFU196617 MPQ196587:MPQ196617 MZM196587:MZM196617 NJI196587:NJI196617 NTE196587:NTE196617 ODA196587:ODA196617 OMW196587:OMW196617 OWS196587:OWS196617 PGO196587:PGO196617 PQK196587:PQK196617 QAG196587:QAG196617 QKC196587:QKC196617 QTY196587:QTY196617 RDU196587:RDU196617 RNQ196587:RNQ196617 RXM196587:RXM196617 SHI196587:SHI196617 SRE196587:SRE196617 TBA196587:TBA196617 TKW196587:TKW196617 TUS196587:TUS196617 UEO196587:UEO196617 UOK196587:UOK196617 UYG196587:UYG196617 VIC196587:VIC196617 VRY196587:VRY196617 WBU196587:WBU196617 WLQ196587:WLQ196617 WVM196587:WVM196617 JA262123:JA262153 SW262123:SW262153 ACS262123:ACS262153 AMO262123:AMO262153 AWK262123:AWK262153 BGG262123:BGG262153 BQC262123:BQC262153 BZY262123:BZY262153 CJU262123:CJU262153 CTQ262123:CTQ262153 DDM262123:DDM262153 DNI262123:DNI262153 DXE262123:DXE262153 EHA262123:EHA262153 EQW262123:EQW262153 FAS262123:FAS262153 FKO262123:FKO262153 FUK262123:FUK262153 GEG262123:GEG262153 GOC262123:GOC262153 GXY262123:GXY262153 HHU262123:HHU262153 HRQ262123:HRQ262153 IBM262123:IBM262153 ILI262123:ILI262153 IVE262123:IVE262153 JFA262123:JFA262153 JOW262123:JOW262153 JYS262123:JYS262153 KIO262123:KIO262153 KSK262123:KSK262153 LCG262123:LCG262153 LMC262123:LMC262153 LVY262123:LVY262153 MFU262123:MFU262153 MPQ262123:MPQ262153 MZM262123:MZM262153 NJI262123:NJI262153 NTE262123:NTE262153 ODA262123:ODA262153 OMW262123:OMW262153 OWS262123:OWS262153 PGO262123:PGO262153 PQK262123:PQK262153 QAG262123:QAG262153 QKC262123:QKC262153 QTY262123:QTY262153 RDU262123:RDU262153 RNQ262123:RNQ262153 RXM262123:RXM262153 SHI262123:SHI262153 SRE262123:SRE262153 TBA262123:TBA262153 TKW262123:TKW262153 TUS262123:TUS262153 UEO262123:UEO262153 UOK262123:UOK262153 UYG262123:UYG262153 VIC262123:VIC262153 VRY262123:VRY262153 WBU262123:WBU262153 WLQ262123:WLQ262153 WVM262123:WVM262153 JA327659:JA327689 SW327659:SW327689 ACS327659:ACS327689 AMO327659:AMO327689 AWK327659:AWK327689 BGG327659:BGG327689 BQC327659:BQC327689 BZY327659:BZY327689 CJU327659:CJU327689 CTQ327659:CTQ327689 DDM327659:DDM327689 DNI327659:DNI327689 DXE327659:DXE327689 EHA327659:EHA327689 EQW327659:EQW327689 FAS327659:FAS327689 FKO327659:FKO327689 FUK327659:FUK327689 GEG327659:GEG327689 GOC327659:GOC327689 GXY327659:GXY327689 HHU327659:HHU327689 HRQ327659:HRQ327689 IBM327659:IBM327689 ILI327659:ILI327689 IVE327659:IVE327689 JFA327659:JFA327689 JOW327659:JOW327689 JYS327659:JYS327689 KIO327659:KIO327689 KSK327659:KSK327689 LCG327659:LCG327689 LMC327659:LMC327689 LVY327659:LVY327689 MFU327659:MFU327689 MPQ327659:MPQ327689 MZM327659:MZM327689 NJI327659:NJI327689 NTE327659:NTE327689 ODA327659:ODA327689 OMW327659:OMW327689 OWS327659:OWS327689 PGO327659:PGO327689 PQK327659:PQK327689 QAG327659:QAG327689 QKC327659:QKC327689 QTY327659:QTY327689 RDU327659:RDU327689 RNQ327659:RNQ327689 RXM327659:RXM327689 SHI327659:SHI327689 SRE327659:SRE327689 TBA327659:TBA327689 TKW327659:TKW327689 TUS327659:TUS327689 UEO327659:UEO327689 UOK327659:UOK327689 UYG327659:UYG327689 VIC327659:VIC327689 VRY327659:VRY327689 WBU327659:WBU327689 WLQ327659:WLQ327689 WVM327659:WVM327689 JA393195:JA393225 SW393195:SW393225 ACS393195:ACS393225 AMO393195:AMO393225 AWK393195:AWK393225 BGG393195:BGG393225 BQC393195:BQC393225 BZY393195:BZY393225 CJU393195:CJU393225 CTQ393195:CTQ393225 DDM393195:DDM393225 DNI393195:DNI393225 DXE393195:DXE393225 EHA393195:EHA393225 EQW393195:EQW393225 FAS393195:FAS393225 FKO393195:FKO393225 FUK393195:FUK393225 GEG393195:GEG393225 GOC393195:GOC393225 GXY393195:GXY393225 HHU393195:HHU393225 HRQ393195:HRQ393225 IBM393195:IBM393225 ILI393195:ILI393225 IVE393195:IVE393225 JFA393195:JFA393225 JOW393195:JOW393225 JYS393195:JYS393225 KIO393195:KIO393225 KSK393195:KSK393225 LCG393195:LCG393225 LMC393195:LMC393225 LVY393195:LVY393225 MFU393195:MFU393225 MPQ393195:MPQ393225 MZM393195:MZM393225 NJI393195:NJI393225 NTE393195:NTE393225 ODA393195:ODA393225 OMW393195:OMW393225 OWS393195:OWS393225 PGO393195:PGO393225 PQK393195:PQK393225 QAG393195:QAG393225 QKC393195:QKC393225 QTY393195:QTY393225 RDU393195:RDU393225 RNQ393195:RNQ393225 RXM393195:RXM393225 SHI393195:SHI393225 SRE393195:SRE393225 TBA393195:TBA393225 TKW393195:TKW393225 TUS393195:TUS393225 UEO393195:UEO393225 UOK393195:UOK393225 UYG393195:UYG393225 VIC393195:VIC393225 VRY393195:VRY393225 WBU393195:WBU393225 WLQ393195:WLQ393225 WVM393195:WVM393225 JA458731:JA458761 SW458731:SW458761 ACS458731:ACS458761 AMO458731:AMO458761 AWK458731:AWK458761 BGG458731:BGG458761 BQC458731:BQC458761 BZY458731:BZY458761 CJU458731:CJU458761 CTQ458731:CTQ458761 DDM458731:DDM458761 DNI458731:DNI458761 DXE458731:DXE458761 EHA458731:EHA458761 EQW458731:EQW458761 FAS458731:FAS458761 FKO458731:FKO458761 FUK458731:FUK458761 GEG458731:GEG458761 GOC458731:GOC458761 GXY458731:GXY458761 HHU458731:HHU458761 HRQ458731:HRQ458761 IBM458731:IBM458761 ILI458731:ILI458761 IVE458731:IVE458761 JFA458731:JFA458761 JOW458731:JOW458761 JYS458731:JYS458761 KIO458731:KIO458761 KSK458731:KSK458761 LCG458731:LCG458761 LMC458731:LMC458761 LVY458731:LVY458761 MFU458731:MFU458761 MPQ458731:MPQ458761 MZM458731:MZM458761 NJI458731:NJI458761 NTE458731:NTE458761 ODA458731:ODA458761 OMW458731:OMW458761 OWS458731:OWS458761 PGO458731:PGO458761 PQK458731:PQK458761 QAG458731:QAG458761 QKC458731:QKC458761 QTY458731:QTY458761 RDU458731:RDU458761 RNQ458731:RNQ458761 RXM458731:RXM458761 SHI458731:SHI458761 SRE458731:SRE458761 TBA458731:TBA458761 TKW458731:TKW458761 TUS458731:TUS458761 UEO458731:UEO458761 UOK458731:UOK458761 UYG458731:UYG458761 VIC458731:VIC458761 VRY458731:VRY458761 WBU458731:WBU458761 WLQ458731:WLQ458761 WVM458731:WVM458761 JA524267:JA524297 SW524267:SW524297 ACS524267:ACS524297 AMO524267:AMO524297 AWK524267:AWK524297 BGG524267:BGG524297 BQC524267:BQC524297 BZY524267:BZY524297 CJU524267:CJU524297 CTQ524267:CTQ524297 DDM524267:DDM524297 DNI524267:DNI524297 DXE524267:DXE524297 EHA524267:EHA524297 EQW524267:EQW524297 FAS524267:FAS524297 FKO524267:FKO524297 FUK524267:FUK524297 GEG524267:GEG524297 GOC524267:GOC524297 GXY524267:GXY524297 HHU524267:HHU524297 HRQ524267:HRQ524297 IBM524267:IBM524297 ILI524267:ILI524297 IVE524267:IVE524297 JFA524267:JFA524297 JOW524267:JOW524297 JYS524267:JYS524297 KIO524267:KIO524297 KSK524267:KSK524297 LCG524267:LCG524297 LMC524267:LMC524297 LVY524267:LVY524297 MFU524267:MFU524297 MPQ524267:MPQ524297 MZM524267:MZM524297 NJI524267:NJI524297 NTE524267:NTE524297 ODA524267:ODA524297 OMW524267:OMW524297 OWS524267:OWS524297 PGO524267:PGO524297 PQK524267:PQK524297 QAG524267:QAG524297 QKC524267:QKC524297 QTY524267:QTY524297 RDU524267:RDU524297 RNQ524267:RNQ524297 RXM524267:RXM524297 SHI524267:SHI524297 SRE524267:SRE524297 TBA524267:TBA524297 TKW524267:TKW524297 TUS524267:TUS524297 UEO524267:UEO524297 UOK524267:UOK524297 UYG524267:UYG524297 VIC524267:VIC524297 VRY524267:VRY524297 WBU524267:WBU524297 WLQ524267:WLQ524297 WVM524267:WVM524297 JA589803:JA589833 SW589803:SW589833 ACS589803:ACS589833 AMO589803:AMO589833 AWK589803:AWK589833 BGG589803:BGG589833 BQC589803:BQC589833 BZY589803:BZY589833 CJU589803:CJU589833 CTQ589803:CTQ589833 DDM589803:DDM589833 DNI589803:DNI589833 DXE589803:DXE589833 EHA589803:EHA589833 EQW589803:EQW589833 FAS589803:FAS589833 FKO589803:FKO589833 FUK589803:FUK589833 GEG589803:GEG589833 GOC589803:GOC589833 GXY589803:GXY589833 HHU589803:HHU589833 HRQ589803:HRQ589833 IBM589803:IBM589833 ILI589803:ILI589833 IVE589803:IVE589833 JFA589803:JFA589833 JOW589803:JOW589833 JYS589803:JYS589833 KIO589803:KIO589833 KSK589803:KSK589833 LCG589803:LCG589833 LMC589803:LMC589833 LVY589803:LVY589833 MFU589803:MFU589833 MPQ589803:MPQ589833 MZM589803:MZM589833 NJI589803:NJI589833 NTE589803:NTE589833 ODA589803:ODA589833 OMW589803:OMW589833 OWS589803:OWS589833 PGO589803:PGO589833 PQK589803:PQK589833 QAG589803:QAG589833 QKC589803:QKC589833 QTY589803:QTY589833 RDU589803:RDU589833 RNQ589803:RNQ589833 RXM589803:RXM589833 SHI589803:SHI589833 SRE589803:SRE589833 TBA589803:TBA589833 TKW589803:TKW589833 TUS589803:TUS589833 UEO589803:UEO589833 UOK589803:UOK589833 UYG589803:UYG589833 VIC589803:VIC589833 VRY589803:VRY589833 WBU589803:WBU589833 WLQ589803:WLQ589833 WVM589803:WVM589833 JA655339:JA655369 SW655339:SW655369 ACS655339:ACS655369 AMO655339:AMO655369 AWK655339:AWK655369 BGG655339:BGG655369 BQC655339:BQC655369 BZY655339:BZY655369 CJU655339:CJU655369 CTQ655339:CTQ655369 DDM655339:DDM655369 DNI655339:DNI655369 DXE655339:DXE655369 EHA655339:EHA655369 EQW655339:EQW655369 FAS655339:FAS655369 FKO655339:FKO655369 FUK655339:FUK655369 GEG655339:GEG655369 GOC655339:GOC655369 GXY655339:GXY655369 HHU655339:HHU655369 HRQ655339:HRQ655369 IBM655339:IBM655369 ILI655339:ILI655369 IVE655339:IVE655369 JFA655339:JFA655369 JOW655339:JOW655369 JYS655339:JYS655369 KIO655339:KIO655369 KSK655339:KSK655369 LCG655339:LCG655369 LMC655339:LMC655369 LVY655339:LVY655369 MFU655339:MFU655369 MPQ655339:MPQ655369 MZM655339:MZM655369 NJI655339:NJI655369 NTE655339:NTE655369 ODA655339:ODA655369 OMW655339:OMW655369 OWS655339:OWS655369 PGO655339:PGO655369 PQK655339:PQK655369 QAG655339:QAG655369 QKC655339:QKC655369 QTY655339:QTY655369 RDU655339:RDU655369 RNQ655339:RNQ655369 RXM655339:RXM655369 SHI655339:SHI655369 SRE655339:SRE655369 TBA655339:TBA655369 TKW655339:TKW655369 TUS655339:TUS655369 UEO655339:UEO655369 UOK655339:UOK655369 UYG655339:UYG655369 VIC655339:VIC655369 VRY655339:VRY655369 WBU655339:WBU655369 WLQ655339:WLQ655369 WVM655339:WVM655369 JA720875:JA720905 SW720875:SW720905 ACS720875:ACS720905 AMO720875:AMO720905 AWK720875:AWK720905 BGG720875:BGG720905 BQC720875:BQC720905 BZY720875:BZY720905 CJU720875:CJU720905 CTQ720875:CTQ720905 DDM720875:DDM720905 DNI720875:DNI720905 DXE720875:DXE720905 EHA720875:EHA720905 EQW720875:EQW720905 FAS720875:FAS720905 FKO720875:FKO720905 FUK720875:FUK720905 GEG720875:GEG720905 GOC720875:GOC720905 GXY720875:GXY720905 HHU720875:HHU720905 HRQ720875:HRQ720905 IBM720875:IBM720905 ILI720875:ILI720905 IVE720875:IVE720905 JFA720875:JFA720905 JOW720875:JOW720905 JYS720875:JYS720905 KIO720875:KIO720905 KSK720875:KSK720905 LCG720875:LCG720905 LMC720875:LMC720905 LVY720875:LVY720905 MFU720875:MFU720905 MPQ720875:MPQ720905 MZM720875:MZM720905 NJI720875:NJI720905 NTE720875:NTE720905 ODA720875:ODA720905 OMW720875:OMW720905 OWS720875:OWS720905 PGO720875:PGO720905 PQK720875:PQK720905 QAG720875:QAG720905 QKC720875:QKC720905 QTY720875:QTY720905 RDU720875:RDU720905 RNQ720875:RNQ720905 RXM720875:RXM720905 SHI720875:SHI720905 SRE720875:SRE720905 TBA720875:TBA720905 TKW720875:TKW720905 TUS720875:TUS720905 UEO720875:UEO720905 UOK720875:UOK720905 UYG720875:UYG720905 VIC720875:VIC720905 VRY720875:VRY720905 WBU720875:WBU720905 WLQ720875:WLQ720905 WVM720875:WVM720905 JA786411:JA786441 SW786411:SW786441 ACS786411:ACS786441 AMO786411:AMO786441 AWK786411:AWK786441 BGG786411:BGG786441 BQC786411:BQC786441 BZY786411:BZY786441 CJU786411:CJU786441 CTQ786411:CTQ786441 DDM786411:DDM786441 DNI786411:DNI786441 DXE786411:DXE786441 EHA786411:EHA786441 EQW786411:EQW786441 FAS786411:FAS786441 FKO786411:FKO786441 FUK786411:FUK786441 GEG786411:GEG786441 GOC786411:GOC786441 GXY786411:GXY786441 HHU786411:HHU786441 HRQ786411:HRQ786441 IBM786411:IBM786441 ILI786411:ILI786441 IVE786411:IVE786441 JFA786411:JFA786441 JOW786411:JOW786441 JYS786411:JYS786441 KIO786411:KIO786441 KSK786411:KSK786441 LCG786411:LCG786441 LMC786411:LMC786441 LVY786411:LVY786441 MFU786411:MFU786441 MPQ786411:MPQ786441 MZM786411:MZM786441 NJI786411:NJI786441 NTE786411:NTE786441 ODA786411:ODA786441 OMW786411:OMW786441 OWS786411:OWS786441 PGO786411:PGO786441 PQK786411:PQK786441 QAG786411:QAG786441 QKC786411:QKC786441 QTY786411:QTY786441 RDU786411:RDU786441 RNQ786411:RNQ786441 RXM786411:RXM786441 SHI786411:SHI786441 SRE786411:SRE786441 TBA786411:TBA786441 TKW786411:TKW786441 TUS786411:TUS786441 UEO786411:UEO786441 UOK786411:UOK786441 UYG786411:UYG786441 VIC786411:VIC786441 VRY786411:VRY786441 WBU786411:WBU786441 WLQ786411:WLQ786441 WVM786411:WVM786441 JA851947:JA851977 SW851947:SW851977 ACS851947:ACS851977 AMO851947:AMO851977 AWK851947:AWK851977 BGG851947:BGG851977 BQC851947:BQC851977 BZY851947:BZY851977 CJU851947:CJU851977 CTQ851947:CTQ851977 DDM851947:DDM851977 DNI851947:DNI851977 DXE851947:DXE851977 EHA851947:EHA851977 EQW851947:EQW851977 FAS851947:FAS851977 FKO851947:FKO851977 FUK851947:FUK851977 GEG851947:GEG851977 GOC851947:GOC851977 GXY851947:GXY851977 HHU851947:HHU851977 HRQ851947:HRQ851977 IBM851947:IBM851977 ILI851947:ILI851977 IVE851947:IVE851977 JFA851947:JFA851977 JOW851947:JOW851977 JYS851947:JYS851977 KIO851947:KIO851977 KSK851947:KSK851977 LCG851947:LCG851977 LMC851947:LMC851977 LVY851947:LVY851977 MFU851947:MFU851977 MPQ851947:MPQ851977 MZM851947:MZM851977 NJI851947:NJI851977 NTE851947:NTE851977 ODA851947:ODA851977 OMW851947:OMW851977 OWS851947:OWS851977 PGO851947:PGO851977 PQK851947:PQK851977 QAG851947:QAG851977 QKC851947:QKC851977 QTY851947:QTY851977 RDU851947:RDU851977 RNQ851947:RNQ851977 RXM851947:RXM851977 SHI851947:SHI851977 SRE851947:SRE851977 TBA851947:TBA851977 TKW851947:TKW851977 TUS851947:TUS851977 UEO851947:UEO851977 UOK851947:UOK851977 UYG851947:UYG851977 VIC851947:VIC851977 VRY851947:VRY851977 WBU851947:WBU851977 WLQ851947:WLQ851977 WVM851947:WVM851977 JA917483:JA917513 SW917483:SW917513 ACS917483:ACS917513 AMO917483:AMO917513 AWK917483:AWK917513 BGG917483:BGG917513 BQC917483:BQC917513 BZY917483:BZY917513 CJU917483:CJU917513 CTQ917483:CTQ917513 DDM917483:DDM917513 DNI917483:DNI917513 DXE917483:DXE917513 EHA917483:EHA917513 EQW917483:EQW917513 FAS917483:FAS917513 FKO917483:FKO917513 FUK917483:FUK917513 GEG917483:GEG917513 GOC917483:GOC917513 GXY917483:GXY917513 HHU917483:HHU917513 HRQ917483:HRQ917513 IBM917483:IBM917513 ILI917483:ILI917513 IVE917483:IVE917513 JFA917483:JFA917513 JOW917483:JOW917513 JYS917483:JYS917513 KIO917483:KIO917513 KSK917483:KSK917513 LCG917483:LCG917513 LMC917483:LMC917513 LVY917483:LVY917513 MFU917483:MFU917513 MPQ917483:MPQ917513 MZM917483:MZM917513 NJI917483:NJI917513 NTE917483:NTE917513 ODA917483:ODA917513 OMW917483:OMW917513 OWS917483:OWS917513 PGO917483:PGO917513 PQK917483:PQK917513 QAG917483:QAG917513 QKC917483:QKC917513 QTY917483:QTY917513 RDU917483:RDU917513 RNQ917483:RNQ917513 RXM917483:RXM917513 SHI917483:SHI917513 SRE917483:SRE917513 TBA917483:TBA917513 TKW917483:TKW917513 TUS917483:TUS917513 UEO917483:UEO917513 UOK917483:UOK917513 UYG917483:UYG917513 VIC917483:VIC917513 VRY917483:VRY917513 WBU917483:WBU917513 WLQ917483:WLQ917513 WVM917483:WVM917513 JA983019:JA983049 SW983019:SW983049 ACS983019:ACS983049 AMO983019:AMO983049 AWK983019:AWK983049 BGG983019:BGG983049 BQC983019:BQC983049 BZY983019:BZY983049 CJU983019:CJU983049 CTQ983019:CTQ983049 DDM983019:DDM983049 DNI983019:DNI983049 DXE983019:DXE983049 EHA983019:EHA983049 EQW983019:EQW983049 FAS983019:FAS983049 FKO983019:FKO983049 FUK983019:FUK983049 GEG983019:GEG983049 GOC983019:GOC983049 GXY983019:GXY983049 HHU983019:HHU983049 HRQ983019:HRQ983049 IBM983019:IBM983049 ILI983019:ILI983049 IVE983019:IVE983049 JFA983019:JFA983049 JOW983019:JOW983049 JYS983019:JYS983049 KIO983019:KIO983049 KSK983019:KSK983049 LCG983019:LCG983049 LMC983019:LMC983049 LVY983019:LVY983049 MFU983019:MFU983049 MPQ983019:MPQ983049 MZM983019:MZM983049 NJI983019:NJI983049 NTE983019:NTE983049 ODA983019:ODA983049 OMW983019:OMW983049 OWS983019:OWS983049 PGO983019:PGO983049 PQK983019:PQK983049 QAG983019:QAG983049 QKC983019:QKC983049 QTY983019:QTY983049 RDU983019:RDU983049 RNQ983019:RNQ983049 RXM983019:RXM983049 SHI983019:SHI983049 SRE983019:SRE983049 TBA983019:TBA983049 TKW983019:TKW983049 TUS983019:TUS983049 UEO983019:UEO983049 UOK983019:UOK983049 UYG983019:UYG983049 VIC983019:VIC983049 VRY983019:VRY983049 WBU983019:WBU983049 WLQ983019:WLQ983049 WVM983019:WVM983049 A983019:B983049 A65515:B65545 A131051:B131081 A196587:B196617 A262123:B262153 A327659:B327689 A393195:B393225 A458731:B458761 A524267:B524297 A589803:B589833 A655339:B655369 A720875:B720905 A786411:B786441 A851947:B851977 A917483:B917513 JA4:JA20 SW4:SW20 ACS4:ACS20 AMO4:AMO20 AWK4:AWK20 BGG4:BGG20 BQC4:BQC20 BZY4:BZY20 CJU4:CJU20 CTQ4:CTQ20 DDM4:DDM20 DNI4:DNI20 DXE4:DXE20 EHA4:EHA20 EQW4:EQW20 FAS4:FAS20 FKO4:FKO20 FUK4:FUK20 GEG4:GEG20 GOC4:GOC20 GXY4:GXY20 HHU4:HHU20 HRQ4:HRQ20 IBM4:IBM20 ILI4:ILI20 IVE4:IVE20 JFA4:JFA20 JOW4:JOW20 JYS4:JYS20 KIO4:KIO20 KSK4:KSK20 LCG4:LCG20 LMC4:LMC20 LVY4:LVY20 MFU4:MFU20 MPQ4:MPQ20 MZM4:MZM20 NJI4:NJI20 NTE4:NTE20 ODA4:ODA20 OMW4:OMW20 OWS4:OWS20 PGO4:PGO20 PQK4:PQK20 QAG4:QAG20 QKC4:QKC20 QTY4:QTY20 RDU4:RDU20 RNQ4:RNQ20 RXM4:RXM20 SHI4:SHI20 SRE4:SRE20 TBA4:TBA20 TKW4:TKW20 TUS4:TUS20 UEO4:UEO20 UOK4:UOK20 UYG4:UYG20 VIC4:VIC20 VRY4:VRY20 WBU4:WBU20 WLQ4:WLQ20 WVM4:WVM20" xr:uid="{00000000-0002-0000-0200-00000E000000}">
       <formula1>"Femenino,Masculino"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JC65515:JC65545 SY65515:SY65545 ACU65515:ACU65545 AMQ65515:AMQ65545 AWM65515:AWM65545 BGI65515:BGI65545 BQE65515:BQE65545 CAA65515:CAA65545 CJW65515:CJW65545 CTS65515:CTS65545 DDO65515:DDO65545 DNK65515:DNK65545 DXG65515:DXG65545 EHC65515:EHC65545 EQY65515:EQY65545 FAU65515:FAU65545 FKQ65515:FKQ65545 FUM65515:FUM65545 GEI65515:GEI65545 GOE65515:GOE65545 GYA65515:GYA65545 HHW65515:HHW65545 HRS65515:HRS65545 IBO65515:IBO65545 ILK65515:ILK65545 IVG65515:IVG65545 JFC65515:JFC65545 JOY65515:JOY65545 JYU65515:JYU65545 KIQ65515:KIQ65545 KSM65515:KSM65545 LCI65515:LCI65545 LME65515:LME65545 LWA65515:LWA65545 MFW65515:MFW65545 MPS65515:MPS65545 MZO65515:MZO65545 NJK65515:NJK65545 NTG65515:NTG65545 ODC65515:ODC65545 OMY65515:OMY65545 OWU65515:OWU65545 PGQ65515:PGQ65545 PQM65515:PQM65545 QAI65515:QAI65545 QKE65515:QKE65545 QUA65515:QUA65545 RDW65515:RDW65545 RNS65515:RNS65545 RXO65515:RXO65545 SHK65515:SHK65545 SRG65515:SRG65545 TBC65515:TBC65545 TKY65515:TKY65545 TUU65515:TUU65545 UEQ65515:UEQ65545 UOM65515:UOM65545 UYI65515:UYI65545 VIE65515:VIE65545 VSA65515:VSA65545 WBW65515:WBW65545 WLS65515:WLS65545 WVO65515:WVO65545 JC131051:JC131081 SY131051:SY131081 ACU131051:ACU131081 AMQ131051:AMQ131081 AWM131051:AWM131081 BGI131051:BGI131081 BQE131051:BQE131081 CAA131051:CAA131081 CJW131051:CJW131081 CTS131051:CTS131081 DDO131051:DDO131081 DNK131051:DNK131081 DXG131051:DXG131081 EHC131051:EHC131081 EQY131051:EQY131081 FAU131051:FAU131081 FKQ131051:FKQ131081 FUM131051:FUM131081 GEI131051:GEI131081 GOE131051:GOE131081 GYA131051:GYA131081 HHW131051:HHW131081 HRS131051:HRS131081 IBO131051:IBO131081 ILK131051:ILK131081 IVG131051:IVG131081 JFC131051:JFC131081 JOY131051:JOY131081 JYU131051:JYU131081 KIQ131051:KIQ131081 KSM131051:KSM131081 LCI131051:LCI131081 LME131051:LME131081 LWA131051:LWA131081 MFW131051:MFW131081 MPS131051:MPS131081 MZO131051:MZO131081 NJK131051:NJK131081 NTG131051:NTG131081 ODC131051:ODC131081 OMY131051:OMY131081 OWU131051:OWU131081 PGQ131051:PGQ131081 PQM131051:PQM131081 QAI131051:QAI131081 QKE131051:QKE131081 QUA131051:QUA131081 RDW131051:RDW131081 RNS131051:RNS131081 RXO131051:RXO131081 SHK131051:SHK131081 SRG131051:SRG131081 TBC131051:TBC131081 TKY131051:TKY131081 TUU131051:TUU131081 UEQ131051:UEQ131081 UOM131051:UOM131081 UYI131051:UYI131081 VIE131051:VIE131081 VSA131051:VSA131081 WBW131051:WBW131081 WLS131051:WLS131081 WVO131051:WVO131081 JC196587:JC196617 SY196587:SY196617 ACU196587:ACU196617 AMQ196587:AMQ196617 AWM196587:AWM196617 BGI196587:BGI196617 BQE196587:BQE196617 CAA196587:CAA196617 CJW196587:CJW196617 CTS196587:CTS196617 DDO196587:DDO196617 DNK196587:DNK196617 DXG196587:DXG196617 EHC196587:EHC196617 EQY196587:EQY196617 FAU196587:FAU196617 FKQ196587:FKQ196617 FUM196587:FUM196617 GEI196587:GEI196617 GOE196587:GOE196617 GYA196587:GYA196617 HHW196587:HHW196617 HRS196587:HRS196617 IBO196587:IBO196617 ILK196587:ILK196617 IVG196587:IVG196617 JFC196587:JFC196617 JOY196587:JOY196617 JYU196587:JYU196617 KIQ196587:KIQ196617 KSM196587:KSM196617 LCI196587:LCI196617 LME196587:LME196617 LWA196587:LWA196617 MFW196587:MFW196617 MPS196587:MPS196617 MZO196587:MZO196617 NJK196587:NJK196617 NTG196587:NTG196617 ODC196587:ODC196617 OMY196587:OMY196617 OWU196587:OWU196617 PGQ196587:PGQ196617 PQM196587:PQM196617 QAI196587:QAI196617 QKE196587:QKE196617 QUA196587:QUA196617 RDW196587:RDW196617 RNS196587:RNS196617 RXO196587:RXO196617 SHK196587:SHK196617 SRG196587:SRG196617 TBC196587:TBC196617 TKY196587:TKY196617 TUU196587:TUU196617 UEQ196587:UEQ196617 UOM196587:UOM196617 UYI196587:UYI196617 VIE196587:VIE196617 VSA196587:VSA196617 WBW196587:WBW196617 WLS196587:WLS196617 WVO196587:WVO196617 JC262123:JC262153 SY262123:SY262153 ACU262123:ACU262153 AMQ262123:AMQ262153 AWM262123:AWM262153 BGI262123:BGI262153 BQE262123:BQE262153 CAA262123:CAA262153 CJW262123:CJW262153 CTS262123:CTS262153 DDO262123:DDO262153 DNK262123:DNK262153 DXG262123:DXG262153 EHC262123:EHC262153 EQY262123:EQY262153 FAU262123:FAU262153 FKQ262123:FKQ262153 FUM262123:FUM262153 GEI262123:GEI262153 GOE262123:GOE262153 GYA262123:GYA262153 HHW262123:HHW262153 HRS262123:HRS262153 IBO262123:IBO262153 ILK262123:ILK262153 IVG262123:IVG262153 JFC262123:JFC262153 JOY262123:JOY262153 JYU262123:JYU262153 KIQ262123:KIQ262153 KSM262123:KSM262153 LCI262123:LCI262153 LME262123:LME262153 LWA262123:LWA262153 MFW262123:MFW262153 MPS262123:MPS262153 MZO262123:MZO262153 NJK262123:NJK262153 NTG262123:NTG262153 ODC262123:ODC262153 OMY262123:OMY262153 OWU262123:OWU262153 PGQ262123:PGQ262153 PQM262123:PQM262153 QAI262123:QAI262153 QKE262123:QKE262153 QUA262123:QUA262153 RDW262123:RDW262153 RNS262123:RNS262153 RXO262123:RXO262153 SHK262123:SHK262153 SRG262123:SRG262153 TBC262123:TBC262153 TKY262123:TKY262153 TUU262123:TUU262153 UEQ262123:UEQ262153 UOM262123:UOM262153 UYI262123:UYI262153 VIE262123:VIE262153 VSA262123:VSA262153 WBW262123:WBW262153 WLS262123:WLS262153 WVO262123:WVO262153 JC327659:JC327689 SY327659:SY327689 ACU327659:ACU327689 AMQ327659:AMQ327689 AWM327659:AWM327689 BGI327659:BGI327689 BQE327659:BQE327689 CAA327659:CAA327689 CJW327659:CJW327689 CTS327659:CTS327689 DDO327659:DDO327689 DNK327659:DNK327689 DXG327659:DXG327689 EHC327659:EHC327689 EQY327659:EQY327689 FAU327659:FAU327689 FKQ327659:FKQ327689 FUM327659:FUM327689 GEI327659:GEI327689 GOE327659:GOE327689 GYA327659:GYA327689 HHW327659:HHW327689 HRS327659:HRS327689 IBO327659:IBO327689 ILK327659:ILK327689 IVG327659:IVG327689 JFC327659:JFC327689 JOY327659:JOY327689 JYU327659:JYU327689 KIQ327659:KIQ327689 KSM327659:KSM327689 LCI327659:LCI327689 LME327659:LME327689 LWA327659:LWA327689 MFW327659:MFW327689 MPS327659:MPS327689 MZO327659:MZO327689 NJK327659:NJK327689 NTG327659:NTG327689 ODC327659:ODC327689 OMY327659:OMY327689 OWU327659:OWU327689 PGQ327659:PGQ327689 PQM327659:PQM327689 QAI327659:QAI327689 QKE327659:QKE327689 QUA327659:QUA327689 RDW327659:RDW327689 RNS327659:RNS327689 RXO327659:RXO327689 SHK327659:SHK327689 SRG327659:SRG327689 TBC327659:TBC327689 TKY327659:TKY327689 TUU327659:TUU327689 UEQ327659:UEQ327689 UOM327659:UOM327689 UYI327659:UYI327689 VIE327659:VIE327689 VSA327659:VSA327689 WBW327659:WBW327689 WLS327659:WLS327689 WVO327659:WVO327689 JC393195:JC393225 SY393195:SY393225 ACU393195:ACU393225 AMQ393195:AMQ393225 AWM393195:AWM393225 BGI393195:BGI393225 BQE393195:BQE393225 CAA393195:CAA393225 CJW393195:CJW393225 CTS393195:CTS393225 DDO393195:DDO393225 DNK393195:DNK393225 DXG393195:DXG393225 EHC393195:EHC393225 EQY393195:EQY393225 FAU393195:FAU393225 FKQ393195:FKQ393225 FUM393195:FUM393225 GEI393195:GEI393225 GOE393195:GOE393225 GYA393195:GYA393225 HHW393195:HHW393225 HRS393195:HRS393225 IBO393195:IBO393225 ILK393195:ILK393225 IVG393195:IVG393225 JFC393195:JFC393225 JOY393195:JOY393225 JYU393195:JYU393225 KIQ393195:KIQ393225 KSM393195:KSM393225 LCI393195:LCI393225 LME393195:LME393225 LWA393195:LWA393225 MFW393195:MFW393225 MPS393195:MPS393225 MZO393195:MZO393225 NJK393195:NJK393225 NTG393195:NTG393225 ODC393195:ODC393225 OMY393195:OMY393225 OWU393195:OWU393225 PGQ393195:PGQ393225 PQM393195:PQM393225 QAI393195:QAI393225 QKE393195:QKE393225 QUA393195:QUA393225 RDW393195:RDW393225 RNS393195:RNS393225 RXO393195:RXO393225 SHK393195:SHK393225 SRG393195:SRG393225 TBC393195:TBC393225 TKY393195:TKY393225 TUU393195:TUU393225 UEQ393195:UEQ393225 UOM393195:UOM393225 UYI393195:UYI393225 VIE393195:VIE393225 VSA393195:VSA393225 WBW393195:WBW393225 WLS393195:WLS393225 WVO393195:WVO393225 JC458731:JC458761 SY458731:SY458761 ACU458731:ACU458761 AMQ458731:AMQ458761 AWM458731:AWM458761 BGI458731:BGI458761 BQE458731:BQE458761 CAA458731:CAA458761 CJW458731:CJW458761 CTS458731:CTS458761 DDO458731:DDO458761 DNK458731:DNK458761 DXG458731:DXG458761 EHC458731:EHC458761 EQY458731:EQY458761 FAU458731:FAU458761 FKQ458731:FKQ458761 FUM458731:FUM458761 GEI458731:GEI458761 GOE458731:GOE458761 GYA458731:GYA458761 HHW458731:HHW458761 HRS458731:HRS458761 IBO458731:IBO458761 ILK458731:ILK458761 IVG458731:IVG458761 JFC458731:JFC458761 JOY458731:JOY458761 JYU458731:JYU458761 KIQ458731:KIQ458761 KSM458731:KSM458761 LCI458731:LCI458761 LME458731:LME458761 LWA458731:LWA458761 MFW458731:MFW458761 MPS458731:MPS458761 MZO458731:MZO458761 NJK458731:NJK458761 NTG458731:NTG458761 ODC458731:ODC458761 OMY458731:OMY458761 OWU458731:OWU458761 PGQ458731:PGQ458761 PQM458731:PQM458761 QAI458731:QAI458761 QKE458731:QKE458761 QUA458731:QUA458761 RDW458731:RDW458761 RNS458731:RNS458761 RXO458731:RXO458761 SHK458731:SHK458761 SRG458731:SRG458761 TBC458731:TBC458761 TKY458731:TKY458761 TUU458731:TUU458761 UEQ458731:UEQ458761 UOM458731:UOM458761 UYI458731:UYI458761 VIE458731:VIE458761 VSA458731:VSA458761 WBW458731:WBW458761 WLS458731:WLS458761 WVO458731:WVO458761 JC524267:JC524297 SY524267:SY524297 ACU524267:ACU524297 AMQ524267:AMQ524297 AWM524267:AWM524297 BGI524267:BGI524297 BQE524267:BQE524297 CAA524267:CAA524297 CJW524267:CJW524297 CTS524267:CTS524297 DDO524267:DDO524297 DNK524267:DNK524297 DXG524267:DXG524297 EHC524267:EHC524297 EQY524267:EQY524297 FAU524267:FAU524297 FKQ524267:FKQ524297 FUM524267:FUM524297 GEI524267:GEI524297 GOE524267:GOE524297 GYA524267:GYA524297 HHW524267:HHW524297 HRS524267:HRS524297 IBO524267:IBO524297 ILK524267:ILK524297 IVG524267:IVG524297 JFC524267:JFC524297 JOY524267:JOY524297 JYU524267:JYU524297 KIQ524267:KIQ524297 KSM524267:KSM524297 LCI524267:LCI524297 LME524267:LME524297 LWA524267:LWA524297 MFW524267:MFW524297 MPS524267:MPS524297 MZO524267:MZO524297 NJK524267:NJK524297 NTG524267:NTG524297 ODC524267:ODC524297 OMY524267:OMY524297 OWU524267:OWU524297 PGQ524267:PGQ524297 PQM524267:PQM524297 QAI524267:QAI524297 QKE524267:QKE524297 QUA524267:QUA524297 RDW524267:RDW524297 RNS524267:RNS524297 RXO524267:RXO524297 SHK524267:SHK524297 SRG524267:SRG524297 TBC524267:TBC524297 TKY524267:TKY524297 TUU524267:TUU524297 UEQ524267:UEQ524297 UOM524267:UOM524297 UYI524267:UYI524297 VIE524267:VIE524297 VSA524267:VSA524297 WBW524267:WBW524297 WLS524267:WLS524297 WVO524267:WVO524297 JC589803:JC589833 SY589803:SY589833 ACU589803:ACU589833 AMQ589803:AMQ589833 AWM589803:AWM589833 BGI589803:BGI589833 BQE589803:BQE589833 CAA589803:CAA589833 CJW589803:CJW589833 CTS589803:CTS589833 DDO589803:DDO589833 DNK589803:DNK589833 DXG589803:DXG589833 EHC589803:EHC589833 EQY589803:EQY589833 FAU589803:FAU589833 FKQ589803:FKQ589833 FUM589803:FUM589833 GEI589803:GEI589833 GOE589803:GOE589833 GYA589803:GYA589833 HHW589803:HHW589833 HRS589803:HRS589833 IBO589803:IBO589833 ILK589803:ILK589833 IVG589803:IVG589833 JFC589803:JFC589833 JOY589803:JOY589833 JYU589803:JYU589833 KIQ589803:KIQ589833 KSM589803:KSM589833 LCI589803:LCI589833 LME589803:LME589833 LWA589803:LWA589833 MFW589803:MFW589833 MPS589803:MPS589833 MZO589803:MZO589833 NJK589803:NJK589833 NTG589803:NTG589833 ODC589803:ODC589833 OMY589803:OMY589833 OWU589803:OWU589833 PGQ589803:PGQ589833 PQM589803:PQM589833 QAI589803:QAI589833 QKE589803:QKE589833 QUA589803:QUA589833 RDW589803:RDW589833 RNS589803:RNS589833 RXO589803:RXO589833 SHK589803:SHK589833 SRG589803:SRG589833 TBC589803:TBC589833 TKY589803:TKY589833 TUU589803:TUU589833 UEQ589803:UEQ589833 UOM589803:UOM589833 UYI589803:UYI589833 VIE589803:VIE589833 VSA589803:VSA589833 WBW589803:WBW589833 WLS589803:WLS589833 WVO589803:WVO589833 JC655339:JC655369 SY655339:SY655369 ACU655339:ACU655369 AMQ655339:AMQ655369 AWM655339:AWM655369 BGI655339:BGI655369 BQE655339:BQE655369 CAA655339:CAA655369 CJW655339:CJW655369 CTS655339:CTS655369 DDO655339:DDO655369 DNK655339:DNK655369 DXG655339:DXG655369 EHC655339:EHC655369 EQY655339:EQY655369 FAU655339:FAU655369 FKQ655339:FKQ655369 FUM655339:FUM655369 GEI655339:GEI655369 GOE655339:GOE655369 GYA655339:GYA655369 HHW655339:HHW655369 HRS655339:HRS655369 IBO655339:IBO655369 ILK655339:ILK655369 IVG655339:IVG655369 JFC655339:JFC655369 JOY655339:JOY655369 JYU655339:JYU655369 KIQ655339:KIQ655369 KSM655339:KSM655369 LCI655339:LCI655369 LME655339:LME655369 LWA655339:LWA655369 MFW655339:MFW655369 MPS655339:MPS655369 MZO655339:MZO655369 NJK655339:NJK655369 NTG655339:NTG655369 ODC655339:ODC655369 OMY655339:OMY655369 OWU655339:OWU655369 PGQ655339:PGQ655369 PQM655339:PQM655369 QAI655339:QAI655369 QKE655339:QKE655369 QUA655339:QUA655369 RDW655339:RDW655369 RNS655339:RNS655369 RXO655339:RXO655369 SHK655339:SHK655369 SRG655339:SRG655369 TBC655339:TBC655369 TKY655339:TKY655369 TUU655339:TUU655369 UEQ655339:UEQ655369 UOM655339:UOM655369 UYI655339:UYI655369 VIE655339:VIE655369 VSA655339:VSA655369 WBW655339:WBW655369 WLS655339:WLS655369 WVO655339:WVO655369 JC720875:JC720905 SY720875:SY720905 ACU720875:ACU720905 AMQ720875:AMQ720905 AWM720875:AWM720905 BGI720875:BGI720905 BQE720875:BQE720905 CAA720875:CAA720905 CJW720875:CJW720905 CTS720875:CTS720905 DDO720875:DDO720905 DNK720875:DNK720905 DXG720875:DXG720905 EHC720875:EHC720905 EQY720875:EQY720905 FAU720875:FAU720905 FKQ720875:FKQ720905 FUM720875:FUM720905 GEI720875:GEI720905 GOE720875:GOE720905 GYA720875:GYA720905 HHW720875:HHW720905 HRS720875:HRS720905 IBO720875:IBO720905 ILK720875:ILK720905 IVG720875:IVG720905 JFC720875:JFC720905 JOY720875:JOY720905 JYU720875:JYU720905 KIQ720875:KIQ720905 KSM720875:KSM720905 LCI720875:LCI720905 LME720875:LME720905 LWA720875:LWA720905 MFW720875:MFW720905 MPS720875:MPS720905 MZO720875:MZO720905 NJK720875:NJK720905 NTG720875:NTG720905 ODC720875:ODC720905 OMY720875:OMY720905 OWU720875:OWU720905 PGQ720875:PGQ720905 PQM720875:PQM720905 QAI720875:QAI720905 QKE720875:QKE720905 QUA720875:QUA720905 RDW720875:RDW720905 RNS720875:RNS720905 RXO720875:RXO720905 SHK720875:SHK720905 SRG720875:SRG720905 TBC720875:TBC720905 TKY720875:TKY720905 TUU720875:TUU720905 UEQ720875:UEQ720905 UOM720875:UOM720905 UYI720875:UYI720905 VIE720875:VIE720905 VSA720875:VSA720905 WBW720875:WBW720905 WLS720875:WLS720905 WVO720875:WVO720905 JC786411:JC786441 SY786411:SY786441 ACU786411:ACU786441 AMQ786411:AMQ786441 AWM786411:AWM786441 BGI786411:BGI786441 BQE786411:BQE786441 CAA786411:CAA786441 CJW786411:CJW786441 CTS786411:CTS786441 DDO786411:DDO786441 DNK786411:DNK786441 DXG786411:DXG786441 EHC786411:EHC786441 EQY786411:EQY786441 FAU786411:FAU786441 FKQ786411:FKQ786441 FUM786411:FUM786441 GEI786411:GEI786441 GOE786411:GOE786441 GYA786411:GYA786441 HHW786411:HHW786441 HRS786411:HRS786441 IBO786411:IBO786441 ILK786411:ILK786441 IVG786411:IVG786441 JFC786411:JFC786441 JOY786411:JOY786441 JYU786411:JYU786441 KIQ786411:KIQ786441 KSM786411:KSM786441 LCI786411:LCI786441 LME786411:LME786441 LWA786411:LWA786441 MFW786411:MFW786441 MPS786411:MPS786441 MZO786411:MZO786441 NJK786411:NJK786441 NTG786411:NTG786441 ODC786411:ODC786441 OMY786411:OMY786441 OWU786411:OWU786441 PGQ786411:PGQ786441 PQM786411:PQM786441 QAI786411:QAI786441 QKE786411:QKE786441 QUA786411:QUA786441 RDW786411:RDW786441 RNS786411:RNS786441 RXO786411:RXO786441 SHK786411:SHK786441 SRG786411:SRG786441 TBC786411:TBC786441 TKY786411:TKY786441 TUU786411:TUU786441 UEQ786411:UEQ786441 UOM786411:UOM786441 UYI786411:UYI786441 VIE786411:VIE786441 VSA786411:VSA786441 WBW786411:WBW786441 WLS786411:WLS786441 WVO786411:WVO786441 JC851947:JC851977 SY851947:SY851977 ACU851947:ACU851977 AMQ851947:AMQ851977 AWM851947:AWM851977 BGI851947:BGI851977 BQE851947:BQE851977 CAA851947:CAA851977 CJW851947:CJW851977 CTS851947:CTS851977 DDO851947:DDO851977 DNK851947:DNK851977 DXG851947:DXG851977 EHC851947:EHC851977 EQY851947:EQY851977 FAU851947:FAU851977 FKQ851947:FKQ851977 FUM851947:FUM851977 GEI851947:GEI851977 GOE851947:GOE851977 GYA851947:GYA851977 HHW851947:HHW851977 HRS851947:HRS851977 IBO851947:IBO851977 ILK851947:ILK851977 IVG851947:IVG851977 JFC851947:JFC851977 JOY851947:JOY851977 JYU851947:JYU851977 KIQ851947:KIQ851977 KSM851947:KSM851977 LCI851947:LCI851977 LME851947:LME851977 LWA851947:LWA851977 MFW851947:MFW851977 MPS851947:MPS851977 MZO851947:MZO851977 NJK851947:NJK851977 NTG851947:NTG851977 ODC851947:ODC851977 OMY851947:OMY851977 OWU851947:OWU851977 PGQ851947:PGQ851977 PQM851947:PQM851977 QAI851947:QAI851977 QKE851947:QKE851977 QUA851947:QUA851977 RDW851947:RDW851977 RNS851947:RNS851977 RXO851947:RXO851977 SHK851947:SHK851977 SRG851947:SRG851977 TBC851947:TBC851977 TKY851947:TKY851977 TUU851947:TUU851977 UEQ851947:UEQ851977 UOM851947:UOM851977 UYI851947:UYI851977 VIE851947:VIE851977 VSA851947:VSA851977 WBW851947:WBW851977 WLS851947:WLS851977 WVO851947:WVO851977 JC917483:JC917513 SY917483:SY917513 ACU917483:ACU917513 AMQ917483:AMQ917513 AWM917483:AWM917513 BGI917483:BGI917513 BQE917483:BQE917513 CAA917483:CAA917513 CJW917483:CJW917513 CTS917483:CTS917513 DDO917483:DDO917513 DNK917483:DNK917513 DXG917483:DXG917513 EHC917483:EHC917513 EQY917483:EQY917513 FAU917483:FAU917513 FKQ917483:FKQ917513 FUM917483:FUM917513 GEI917483:GEI917513 GOE917483:GOE917513 GYA917483:GYA917513 HHW917483:HHW917513 HRS917483:HRS917513 IBO917483:IBO917513 ILK917483:ILK917513 IVG917483:IVG917513 JFC917483:JFC917513 JOY917483:JOY917513 JYU917483:JYU917513 KIQ917483:KIQ917513 KSM917483:KSM917513 LCI917483:LCI917513 LME917483:LME917513 LWA917483:LWA917513 MFW917483:MFW917513 MPS917483:MPS917513 MZO917483:MZO917513 NJK917483:NJK917513 NTG917483:NTG917513 ODC917483:ODC917513 OMY917483:OMY917513 OWU917483:OWU917513 PGQ917483:PGQ917513 PQM917483:PQM917513 QAI917483:QAI917513 QKE917483:QKE917513 QUA917483:QUA917513 RDW917483:RDW917513 RNS917483:RNS917513 RXO917483:RXO917513 SHK917483:SHK917513 SRG917483:SRG917513 TBC917483:TBC917513 TKY917483:TKY917513 TUU917483:TUU917513 UEQ917483:UEQ917513 UOM917483:UOM917513 UYI917483:UYI917513 VIE917483:VIE917513 VSA917483:VSA917513 WBW917483:WBW917513 WLS917483:WLS917513 WVO917483:WVO917513 JC983019:JC983049 SY983019:SY983049 ACU983019:ACU983049 AMQ983019:AMQ983049 AWM983019:AWM983049 BGI983019:BGI983049 BQE983019:BQE983049 CAA983019:CAA983049 CJW983019:CJW983049 CTS983019:CTS983049 DDO983019:DDO983049 DNK983019:DNK983049 DXG983019:DXG983049 EHC983019:EHC983049 EQY983019:EQY983049 FAU983019:FAU983049 FKQ983019:FKQ983049 FUM983019:FUM983049 GEI983019:GEI983049 GOE983019:GOE983049 GYA983019:GYA983049 HHW983019:HHW983049 HRS983019:HRS983049 IBO983019:IBO983049 ILK983019:ILK983049 IVG983019:IVG983049 JFC983019:JFC983049 JOY983019:JOY983049 JYU983019:JYU983049 KIQ983019:KIQ983049 KSM983019:KSM983049 LCI983019:LCI983049 LME983019:LME983049 LWA983019:LWA983049 MFW983019:MFW983049 MPS983019:MPS983049 MZO983019:MZO983049 NJK983019:NJK983049 NTG983019:NTG983049 ODC983019:ODC983049 OMY983019:OMY983049 OWU983019:OWU983049 PGQ983019:PGQ983049 PQM983019:PQM983049 QAI983019:QAI983049 QKE983019:QKE983049 QUA983019:QUA983049 RDW983019:RDW983049 RNS983019:RNS983049 RXO983019:RXO983049 SHK983019:SHK983049 SRG983019:SRG983049 TBC983019:TBC983049 TKY983019:TKY983049 TUU983019:TUU983049 UEQ983019:UEQ983049 UOM983019:UOM983049 UYI983019:UYI983049 VIE983019:VIE983049 VSA983019:VSA983049 WBW983019:WBW983049 WLS983019:WLS983049 WVO983019:WVO983049 K983019:K983049 K65515:K65545 K131051:K131081 K196587:K196617 K262123:K262153 K327659:K327689 K393195:K393225 K458731:K458761 K524267:K524297 K589803:K589833 K655339:K655369 K720875:K720905 K786411:K786441 K851947:K851977 K917483:K917513 WVO4:WVO20 WLS4:WLS20 WBW4:WBW20 VSA4:VSA20 VIE4:VIE20 UYI4:UYI20 UOM4:UOM20 UEQ4:UEQ20 TUU4:TUU20 TKY4:TKY20 TBC4:TBC20 SRG4:SRG20 SHK4:SHK20 RXO4:RXO20 RNS4:RNS20 RDW4:RDW20 QUA4:QUA20 QKE4:QKE20 QAI4:QAI20 PQM4:PQM20 PGQ4:PGQ20 OWU4:OWU20 OMY4:OMY20 ODC4:ODC20 NTG4:NTG20 NJK4:NJK20 MZO4:MZO20 MPS4:MPS20 MFW4:MFW20 LWA4:LWA20 LME4:LME20 LCI4:LCI20 KSM4:KSM20 KIQ4:KIQ20 JYU4:JYU20 JOY4:JOY20 JFC4:JFC20 IVG4:IVG20 ILK4:ILK20 IBO4:IBO20 HRS4:HRS20 HHW4:HHW20 GYA4:GYA20 GOE4:GOE20 GEI4:GEI20 FUM4:FUM20 FKQ4:FKQ20 FAU4:FAU20 EQY4:EQY20 EHC4:EHC20 DXG4:DXG20 DNK4:DNK20 DDO4:DDO20 CTS4:CTS20 CJW4:CJW20 CAA4:CAA20 BQE4:BQE20 BGI4:BGI20 AWM4:AWM20 AMQ4:AMQ20 ACU4:ACU20 SY4:SY20 JC4:JC20" xr:uid="{00000000-0002-0000-0200-00000F000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JC65515:JC65545 SY65515:SY65545 ACU65515:ACU65545 AMQ65515:AMQ65545 AWM65515:AWM65545 BGI65515:BGI65545 BQE65515:BQE65545 CAA65515:CAA65545 CJW65515:CJW65545 CTS65515:CTS65545 DDO65515:DDO65545 DNK65515:DNK65545 DXG65515:DXG65545 EHC65515:EHC65545 EQY65515:EQY65545 FAU65515:FAU65545 FKQ65515:FKQ65545 FUM65515:FUM65545 GEI65515:GEI65545 GOE65515:GOE65545 GYA65515:GYA65545 HHW65515:HHW65545 HRS65515:HRS65545 IBO65515:IBO65545 ILK65515:ILK65545 IVG65515:IVG65545 JFC65515:JFC65545 JOY65515:JOY65545 JYU65515:JYU65545 KIQ65515:KIQ65545 KSM65515:KSM65545 LCI65515:LCI65545 LME65515:LME65545 LWA65515:LWA65545 MFW65515:MFW65545 MPS65515:MPS65545 MZO65515:MZO65545 NJK65515:NJK65545 NTG65515:NTG65545 ODC65515:ODC65545 OMY65515:OMY65545 OWU65515:OWU65545 PGQ65515:PGQ65545 PQM65515:PQM65545 QAI65515:QAI65545 QKE65515:QKE65545 QUA65515:QUA65545 RDW65515:RDW65545 RNS65515:RNS65545 RXO65515:RXO65545 SHK65515:SHK65545 SRG65515:SRG65545 TBC65515:TBC65545 TKY65515:TKY65545 TUU65515:TUU65545 UEQ65515:UEQ65545 UOM65515:UOM65545 UYI65515:UYI65545 VIE65515:VIE65545 VSA65515:VSA65545 WBW65515:WBW65545 WLS65515:WLS65545 WVO65515:WVO65545 JC131051:JC131081 SY131051:SY131081 ACU131051:ACU131081 AMQ131051:AMQ131081 AWM131051:AWM131081 BGI131051:BGI131081 BQE131051:BQE131081 CAA131051:CAA131081 CJW131051:CJW131081 CTS131051:CTS131081 DDO131051:DDO131081 DNK131051:DNK131081 DXG131051:DXG131081 EHC131051:EHC131081 EQY131051:EQY131081 FAU131051:FAU131081 FKQ131051:FKQ131081 FUM131051:FUM131081 GEI131051:GEI131081 GOE131051:GOE131081 GYA131051:GYA131081 HHW131051:HHW131081 HRS131051:HRS131081 IBO131051:IBO131081 ILK131051:ILK131081 IVG131051:IVG131081 JFC131051:JFC131081 JOY131051:JOY131081 JYU131051:JYU131081 KIQ131051:KIQ131081 KSM131051:KSM131081 LCI131051:LCI131081 LME131051:LME131081 LWA131051:LWA131081 MFW131051:MFW131081 MPS131051:MPS131081 MZO131051:MZO131081 NJK131051:NJK131081 NTG131051:NTG131081 ODC131051:ODC131081 OMY131051:OMY131081 OWU131051:OWU131081 PGQ131051:PGQ131081 PQM131051:PQM131081 QAI131051:QAI131081 QKE131051:QKE131081 QUA131051:QUA131081 RDW131051:RDW131081 RNS131051:RNS131081 RXO131051:RXO131081 SHK131051:SHK131081 SRG131051:SRG131081 TBC131051:TBC131081 TKY131051:TKY131081 TUU131051:TUU131081 UEQ131051:UEQ131081 UOM131051:UOM131081 UYI131051:UYI131081 VIE131051:VIE131081 VSA131051:VSA131081 WBW131051:WBW131081 WLS131051:WLS131081 WVO131051:WVO131081 JC196587:JC196617 SY196587:SY196617 ACU196587:ACU196617 AMQ196587:AMQ196617 AWM196587:AWM196617 BGI196587:BGI196617 BQE196587:BQE196617 CAA196587:CAA196617 CJW196587:CJW196617 CTS196587:CTS196617 DDO196587:DDO196617 DNK196587:DNK196617 DXG196587:DXG196617 EHC196587:EHC196617 EQY196587:EQY196617 FAU196587:FAU196617 FKQ196587:FKQ196617 FUM196587:FUM196617 GEI196587:GEI196617 GOE196587:GOE196617 GYA196587:GYA196617 HHW196587:HHW196617 HRS196587:HRS196617 IBO196587:IBO196617 ILK196587:ILK196617 IVG196587:IVG196617 JFC196587:JFC196617 JOY196587:JOY196617 JYU196587:JYU196617 KIQ196587:KIQ196617 KSM196587:KSM196617 LCI196587:LCI196617 LME196587:LME196617 LWA196587:LWA196617 MFW196587:MFW196617 MPS196587:MPS196617 MZO196587:MZO196617 NJK196587:NJK196617 NTG196587:NTG196617 ODC196587:ODC196617 OMY196587:OMY196617 OWU196587:OWU196617 PGQ196587:PGQ196617 PQM196587:PQM196617 QAI196587:QAI196617 QKE196587:QKE196617 QUA196587:QUA196617 RDW196587:RDW196617 RNS196587:RNS196617 RXO196587:RXO196617 SHK196587:SHK196617 SRG196587:SRG196617 TBC196587:TBC196617 TKY196587:TKY196617 TUU196587:TUU196617 UEQ196587:UEQ196617 UOM196587:UOM196617 UYI196587:UYI196617 VIE196587:VIE196617 VSA196587:VSA196617 WBW196587:WBW196617 WLS196587:WLS196617 WVO196587:WVO196617 JC262123:JC262153 SY262123:SY262153 ACU262123:ACU262153 AMQ262123:AMQ262153 AWM262123:AWM262153 BGI262123:BGI262153 BQE262123:BQE262153 CAA262123:CAA262153 CJW262123:CJW262153 CTS262123:CTS262153 DDO262123:DDO262153 DNK262123:DNK262153 DXG262123:DXG262153 EHC262123:EHC262153 EQY262123:EQY262153 FAU262123:FAU262153 FKQ262123:FKQ262153 FUM262123:FUM262153 GEI262123:GEI262153 GOE262123:GOE262153 GYA262123:GYA262153 HHW262123:HHW262153 HRS262123:HRS262153 IBO262123:IBO262153 ILK262123:ILK262153 IVG262123:IVG262153 JFC262123:JFC262153 JOY262123:JOY262153 JYU262123:JYU262153 KIQ262123:KIQ262153 KSM262123:KSM262153 LCI262123:LCI262153 LME262123:LME262153 LWA262123:LWA262153 MFW262123:MFW262153 MPS262123:MPS262153 MZO262123:MZO262153 NJK262123:NJK262153 NTG262123:NTG262153 ODC262123:ODC262153 OMY262123:OMY262153 OWU262123:OWU262153 PGQ262123:PGQ262153 PQM262123:PQM262153 QAI262123:QAI262153 QKE262123:QKE262153 QUA262123:QUA262153 RDW262123:RDW262153 RNS262123:RNS262153 RXO262123:RXO262153 SHK262123:SHK262153 SRG262123:SRG262153 TBC262123:TBC262153 TKY262123:TKY262153 TUU262123:TUU262153 UEQ262123:UEQ262153 UOM262123:UOM262153 UYI262123:UYI262153 VIE262123:VIE262153 VSA262123:VSA262153 WBW262123:WBW262153 WLS262123:WLS262153 WVO262123:WVO262153 JC327659:JC327689 SY327659:SY327689 ACU327659:ACU327689 AMQ327659:AMQ327689 AWM327659:AWM327689 BGI327659:BGI327689 BQE327659:BQE327689 CAA327659:CAA327689 CJW327659:CJW327689 CTS327659:CTS327689 DDO327659:DDO327689 DNK327659:DNK327689 DXG327659:DXG327689 EHC327659:EHC327689 EQY327659:EQY327689 FAU327659:FAU327689 FKQ327659:FKQ327689 FUM327659:FUM327689 GEI327659:GEI327689 GOE327659:GOE327689 GYA327659:GYA327689 HHW327659:HHW327689 HRS327659:HRS327689 IBO327659:IBO327689 ILK327659:ILK327689 IVG327659:IVG327689 JFC327659:JFC327689 JOY327659:JOY327689 JYU327659:JYU327689 KIQ327659:KIQ327689 KSM327659:KSM327689 LCI327659:LCI327689 LME327659:LME327689 LWA327659:LWA327689 MFW327659:MFW327689 MPS327659:MPS327689 MZO327659:MZO327689 NJK327659:NJK327689 NTG327659:NTG327689 ODC327659:ODC327689 OMY327659:OMY327689 OWU327659:OWU327689 PGQ327659:PGQ327689 PQM327659:PQM327689 QAI327659:QAI327689 QKE327659:QKE327689 QUA327659:QUA327689 RDW327659:RDW327689 RNS327659:RNS327689 RXO327659:RXO327689 SHK327659:SHK327689 SRG327659:SRG327689 TBC327659:TBC327689 TKY327659:TKY327689 TUU327659:TUU327689 UEQ327659:UEQ327689 UOM327659:UOM327689 UYI327659:UYI327689 VIE327659:VIE327689 VSA327659:VSA327689 WBW327659:WBW327689 WLS327659:WLS327689 WVO327659:WVO327689 JC393195:JC393225 SY393195:SY393225 ACU393195:ACU393225 AMQ393195:AMQ393225 AWM393195:AWM393225 BGI393195:BGI393225 BQE393195:BQE393225 CAA393195:CAA393225 CJW393195:CJW393225 CTS393195:CTS393225 DDO393195:DDO393225 DNK393195:DNK393225 DXG393195:DXG393225 EHC393195:EHC393225 EQY393195:EQY393225 FAU393195:FAU393225 FKQ393195:FKQ393225 FUM393195:FUM393225 GEI393195:GEI393225 GOE393195:GOE393225 GYA393195:GYA393225 HHW393195:HHW393225 HRS393195:HRS393225 IBO393195:IBO393225 ILK393195:ILK393225 IVG393195:IVG393225 JFC393195:JFC393225 JOY393195:JOY393225 JYU393195:JYU393225 KIQ393195:KIQ393225 KSM393195:KSM393225 LCI393195:LCI393225 LME393195:LME393225 LWA393195:LWA393225 MFW393195:MFW393225 MPS393195:MPS393225 MZO393195:MZO393225 NJK393195:NJK393225 NTG393195:NTG393225 ODC393195:ODC393225 OMY393195:OMY393225 OWU393195:OWU393225 PGQ393195:PGQ393225 PQM393195:PQM393225 QAI393195:QAI393225 QKE393195:QKE393225 QUA393195:QUA393225 RDW393195:RDW393225 RNS393195:RNS393225 RXO393195:RXO393225 SHK393195:SHK393225 SRG393195:SRG393225 TBC393195:TBC393225 TKY393195:TKY393225 TUU393195:TUU393225 UEQ393195:UEQ393225 UOM393195:UOM393225 UYI393195:UYI393225 VIE393195:VIE393225 VSA393195:VSA393225 WBW393195:WBW393225 WLS393195:WLS393225 WVO393195:WVO393225 JC458731:JC458761 SY458731:SY458761 ACU458731:ACU458761 AMQ458731:AMQ458761 AWM458731:AWM458761 BGI458731:BGI458761 BQE458731:BQE458761 CAA458731:CAA458761 CJW458731:CJW458761 CTS458731:CTS458761 DDO458731:DDO458761 DNK458731:DNK458761 DXG458731:DXG458761 EHC458731:EHC458761 EQY458731:EQY458761 FAU458731:FAU458761 FKQ458731:FKQ458761 FUM458731:FUM458761 GEI458731:GEI458761 GOE458731:GOE458761 GYA458731:GYA458761 HHW458731:HHW458761 HRS458731:HRS458761 IBO458731:IBO458761 ILK458731:ILK458761 IVG458731:IVG458761 JFC458731:JFC458761 JOY458731:JOY458761 JYU458731:JYU458761 KIQ458731:KIQ458761 KSM458731:KSM458761 LCI458731:LCI458761 LME458731:LME458761 LWA458731:LWA458761 MFW458731:MFW458761 MPS458731:MPS458761 MZO458731:MZO458761 NJK458731:NJK458761 NTG458731:NTG458761 ODC458731:ODC458761 OMY458731:OMY458761 OWU458731:OWU458761 PGQ458731:PGQ458761 PQM458731:PQM458761 QAI458731:QAI458761 QKE458731:QKE458761 QUA458731:QUA458761 RDW458731:RDW458761 RNS458731:RNS458761 RXO458731:RXO458761 SHK458731:SHK458761 SRG458731:SRG458761 TBC458731:TBC458761 TKY458731:TKY458761 TUU458731:TUU458761 UEQ458731:UEQ458761 UOM458731:UOM458761 UYI458731:UYI458761 VIE458731:VIE458761 VSA458731:VSA458761 WBW458731:WBW458761 WLS458731:WLS458761 WVO458731:WVO458761 JC524267:JC524297 SY524267:SY524297 ACU524267:ACU524297 AMQ524267:AMQ524297 AWM524267:AWM524297 BGI524267:BGI524297 BQE524267:BQE524297 CAA524267:CAA524297 CJW524267:CJW524297 CTS524267:CTS524297 DDO524267:DDO524297 DNK524267:DNK524297 DXG524267:DXG524297 EHC524267:EHC524297 EQY524267:EQY524297 FAU524267:FAU524297 FKQ524267:FKQ524297 FUM524267:FUM524297 GEI524267:GEI524297 GOE524267:GOE524297 GYA524267:GYA524297 HHW524267:HHW524297 HRS524267:HRS524297 IBO524267:IBO524297 ILK524267:ILK524297 IVG524267:IVG524297 JFC524267:JFC524297 JOY524267:JOY524297 JYU524267:JYU524297 KIQ524267:KIQ524297 KSM524267:KSM524297 LCI524267:LCI524297 LME524267:LME524297 LWA524267:LWA524297 MFW524267:MFW524297 MPS524267:MPS524297 MZO524267:MZO524297 NJK524267:NJK524297 NTG524267:NTG524297 ODC524267:ODC524297 OMY524267:OMY524297 OWU524267:OWU524297 PGQ524267:PGQ524297 PQM524267:PQM524297 QAI524267:QAI524297 QKE524267:QKE524297 QUA524267:QUA524297 RDW524267:RDW524297 RNS524267:RNS524297 RXO524267:RXO524297 SHK524267:SHK524297 SRG524267:SRG524297 TBC524267:TBC524297 TKY524267:TKY524297 TUU524267:TUU524297 UEQ524267:UEQ524297 UOM524267:UOM524297 UYI524267:UYI524297 VIE524267:VIE524297 VSA524267:VSA524297 WBW524267:WBW524297 WLS524267:WLS524297 WVO524267:WVO524297 JC589803:JC589833 SY589803:SY589833 ACU589803:ACU589833 AMQ589803:AMQ589833 AWM589803:AWM589833 BGI589803:BGI589833 BQE589803:BQE589833 CAA589803:CAA589833 CJW589803:CJW589833 CTS589803:CTS589833 DDO589803:DDO589833 DNK589803:DNK589833 DXG589803:DXG589833 EHC589803:EHC589833 EQY589803:EQY589833 FAU589803:FAU589833 FKQ589803:FKQ589833 FUM589803:FUM589833 GEI589803:GEI589833 GOE589803:GOE589833 GYA589803:GYA589833 HHW589803:HHW589833 HRS589803:HRS589833 IBO589803:IBO589833 ILK589803:ILK589833 IVG589803:IVG589833 JFC589803:JFC589833 JOY589803:JOY589833 JYU589803:JYU589833 KIQ589803:KIQ589833 KSM589803:KSM589833 LCI589803:LCI589833 LME589803:LME589833 LWA589803:LWA589833 MFW589803:MFW589833 MPS589803:MPS589833 MZO589803:MZO589833 NJK589803:NJK589833 NTG589803:NTG589833 ODC589803:ODC589833 OMY589803:OMY589833 OWU589803:OWU589833 PGQ589803:PGQ589833 PQM589803:PQM589833 QAI589803:QAI589833 QKE589803:QKE589833 QUA589803:QUA589833 RDW589803:RDW589833 RNS589803:RNS589833 RXO589803:RXO589833 SHK589803:SHK589833 SRG589803:SRG589833 TBC589803:TBC589833 TKY589803:TKY589833 TUU589803:TUU589833 UEQ589803:UEQ589833 UOM589803:UOM589833 UYI589803:UYI589833 VIE589803:VIE589833 VSA589803:VSA589833 WBW589803:WBW589833 WLS589803:WLS589833 WVO589803:WVO589833 JC655339:JC655369 SY655339:SY655369 ACU655339:ACU655369 AMQ655339:AMQ655369 AWM655339:AWM655369 BGI655339:BGI655369 BQE655339:BQE655369 CAA655339:CAA655369 CJW655339:CJW655369 CTS655339:CTS655369 DDO655339:DDO655369 DNK655339:DNK655369 DXG655339:DXG655369 EHC655339:EHC655369 EQY655339:EQY655369 FAU655339:FAU655369 FKQ655339:FKQ655369 FUM655339:FUM655369 GEI655339:GEI655369 GOE655339:GOE655369 GYA655339:GYA655369 HHW655339:HHW655369 HRS655339:HRS655369 IBO655339:IBO655369 ILK655339:ILK655369 IVG655339:IVG655369 JFC655339:JFC655369 JOY655339:JOY655369 JYU655339:JYU655369 KIQ655339:KIQ655369 KSM655339:KSM655369 LCI655339:LCI655369 LME655339:LME655369 LWA655339:LWA655369 MFW655339:MFW655369 MPS655339:MPS655369 MZO655339:MZO655369 NJK655339:NJK655369 NTG655339:NTG655369 ODC655339:ODC655369 OMY655339:OMY655369 OWU655339:OWU655369 PGQ655339:PGQ655369 PQM655339:PQM655369 QAI655339:QAI655369 QKE655339:QKE655369 QUA655339:QUA655369 RDW655339:RDW655369 RNS655339:RNS655369 RXO655339:RXO655369 SHK655339:SHK655369 SRG655339:SRG655369 TBC655339:TBC655369 TKY655339:TKY655369 TUU655339:TUU655369 UEQ655339:UEQ655369 UOM655339:UOM655369 UYI655339:UYI655369 VIE655339:VIE655369 VSA655339:VSA655369 WBW655339:WBW655369 WLS655339:WLS655369 WVO655339:WVO655369 JC720875:JC720905 SY720875:SY720905 ACU720875:ACU720905 AMQ720875:AMQ720905 AWM720875:AWM720905 BGI720875:BGI720905 BQE720875:BQE720905 CAA720875:CAA720905 CJW720875:CJW720905 CTS720875:CTS720905 DDO720875:DDO720905 DNK720875:DNK720905 DXG720875:DXG720905 EHC720875:EHC720905 EQY720875:EQY720905 FAU720875:FAU720905 FKQ720875:FKQ720905 FUM720875:FUM720905 GEI720875:GEI720905 GOE720875:GOE720905 GYA720875:GYA720905 HHW720875:HHW720905 HRS720875:HRS720905 IBO720875:IBO720905 ILK720875:ILK720905 IVG720875:IVG720905 JFC720875:JFC720905 JOY720875:JOY720905 JYU720875:JYU720905 KIQ720875:KIQ720905 KSM720875:KSM720905 LCI720875:LCI720905 LME720875:LME720905 LWA720875:LWA720905 MFW720875:MFW720905 MPS720875:MPS720905 MZO720875:MZO720905 NJK720875:NJK720905 NTG720875:NTG720905 ODC720875:ODC720905 OMY720875:OMY720905 OWU720875:OWU720905 PGQ720875:PGQ720905 PQM720875:PQM720905 QAI720875:QAI720905 QKE720875:QKE720905 QUA720875:QUA720905 RDW720875:RDW720905 RNS720875:RNS720905 RXO720875:RXO720905 SHK720875:SHK720905 SRG720875:SRG720905 TBC720875:TBC720905 TKY720875:TKY720905 TUU720875:TUU720905 UEQ720875:UEQ720905 UOM720875:UOM720905 UYI720875:UYI720905 VIE720875:VIE720905 VSA720875:VSA720905 WBW720875:WBW720905 WLS720875:WLS720905 WVO720875:WVO720905 JC786411:JC786441 SY786411:SY786441 ACU786411:ACU786441 AMQ786411:AMQ786441 AWM786411:AWM786441 BGI786411:BGI786441 BQE786411:BQE786441 CAA786411:CAA786441 CJW786411:CJW786441 CTS786411:CTS786441 DDO786411:DDO786441 DNK786411:DNK786441 DXG786411:DXG786441 EHC786411:EHC786441 EQY786411:EQY786441 FAU786411:FAU786441 FKQ786411:FKQ786441 FUM786411:FUM786441 GEI786411:GEI786441 GOE786411:GOE786441 GYA786411:GYA786441 HHW786411:HHW786441 HRS786411:HRS786441 IBO786411:IBO786441 ILK786411:ILK786441 IVG786411:IVG786441 JFC786411:JFC786441 JOY786411:JOY786441 JYU786411:JYU786441 KIQ786411:KIQ786441 KSM786411:KSM786441 LCI786411:LCI786441 LME786411:LME786441 LWA786411:LWA786441 MFW786411:MFW786441 MPS786411:MPS786441 MZO786411:MZO786441 NJK786411:NJK786441 NTG786411:NTG786441 ODC786411:ODC786441 OMY786411:OMY786441 OWU786411:OWU786441 PGQ786411:PGQ786441 PQM786411:PQM786441 QAI786411:QAI786441 QKE786411:QKE786441 QUA786411:QUA786441 RDW786411:RDW786441 RNS786411:RNS786441 RXO786411:RXO786441 SHK786411:SHK786441 SRG786411:SRG786441 TBC786411:TBC786441 TKY786411:TKY786441 TUU786411:TUU786441 UEQ786411:UEQ786441 UOM786411:UOM786441 UYI786411:UYI786441 VIE786411:VIE786441 VSA786411:VSA786441 WBW786411:WBW786441 WLS786411:WLS786441 WVO786411:WVO786441 JC851947:JC851977 SY851947:SY851977 ACU851947:ACU851977 AMQ851947:AMQ851977 AWM851947:AWM851977 BGI851947:BGI851977 BQE851947:BQE851977 CAA851947:CAA851977 CJW851947:CJW851977 CTS851947:CTS851977 DDO851947:DDO851977 DNK851947:DNK851977 DXG851947:DXG851977 EHC851947:EHC851977 EQY851947:EQY851977 FAU851947:FAU851977 FKQ851947:FKQ851977 FUM851947:FUM851977 GEI851947:GEI851977 GOE851947:GOE851977 GYA851947:GYA851977 HHW851947:HHW851977 HRS851947:HRS851977 IBO851947:IBO851977 ILK851947:ILK851977 IVG851947:IVG851977 JFC851947:JFC851977 JOY851947:JOY851977 JYU851947:JYU851977 KIQ851947:KIQ851977 KSM851947:KSM851977 LCI851947:LCI851977 LME851947:LME851977 LWA851947:LWA851977 MFW851947:MFW851977 MPS851947:MPS851977 MZO851947:MZO851977 NJK851947:NJK851977 NTG851947:NTG851977 ODC851947:ODC851977 OMY851947:OMY851977 OWU851947:OWU851977 PGQ851947:PGQ851977 PQM851947:PQM851977 QAI851947:QAI851977 QKE851947:QKE851977 QUA851947:QUA851977 RDW851947:RDW851977 RNS851947:RNS851977 RXO851947:RXO851977 SHK851947:SHK851977 SRG851947:SRG851977 TBC851947:TBC851977 TKY851947:TKY851977 TUU851947:TUU851977 UEQ851947:UEQ851977 UOM851947:UOM851977 UYI851947:UYI851977 VIE851947:VIE851977 VSA851947:VSA851977 WBW851947:WBW851977 WLS851947:WLS851977 WVO851947:WVO851977 JC917483:JC917513 SY917483:SY917513 ACU917483:ACU917513 AMQ917483:AMQ917513 AWM917483:AWM917513 BGI917483:BGI917513 BQE917483:BQE917513 CAA917483:CAA917513 CJW917483:CJW917513 CTS917483:CTS917513 DDO917483:DDO917513 DNK917483:DNK917513 DXG917483:DXG917513 EHC917483:EHC917513 EQY917483:EQY917513 FAU917483:FAU917513 FKQ917483:FKQ917513 FUM917483:FUM917513 GEI917483:GEI917513 GOE917483:GOE917513 GYA917483:GYA917513 HHW917483:HHW917513 HRS917483:HRS917513 IBO917483:IBO917513 ILK917483:ILK917513 IVG917483:IVG917513 JFC917483:JFC917513 JOY917483:JOY917513 JYU917483:JYU917513 KIQ917483:KIQ917513 KSM917483:KSM917513 LCI917483:LCI917513 LME917483:LME917513 LWA917483:LWA917513 MFW917483:MFW917513 MPS917483:MPS917513 MZO917483:MZO917513 NJK917483:NJK917513 NTG917483:NTG917513 ODC917483:ODC917513 OMY917483:OMY917513 OWU917483:OWU917513 PGQ917483:PGQ917513 PQM917483:PQM917513 QAI917483:QAI917513 QKE917483:QKE917513 QUA917483:QUA917513 RDW917483:RDW917513 RNS917483:RNS917513 RXO917483:RXO917513 SHK917483:SHK917513 SRG917483:SRG917513 TBC917483:TBC917513 TKY917483:TKY917513 TUU917483:TUU917513 UEQ917483:UEQ917513 UOM917483:UOM917513 UYI917483:UYI917513 VIE917483:VIE917513 VSA917483:VSA917513 WBW917483:WBW917513 WLS917483:WLS917513 WVO917483:WVO917513 JC983019:JC983049 SY983019:SY983049 ACU983019:ACU983049 AMQ983019:AMQ983049 AWM983019:AWM983049 BGI983019:BGI983049 BQE983019:BQE983049 CAA983019:CAA983049 CJW983019:CJW983049 CTS983019:CTS983049 DDO983019:DDO983049 DNK983019:DNK983049 DXG983019:DXG983049 EHC983019:EHC983049 EQY983019:EQY983049 FAU983019:FAU983049 FKQ983019:FKQ983049 FUM983019:FUM983049 GEI983019:GEI983049 GOE983019:GOE983049 GYA983019:GYA983049 HHW983019:HHW983049 HRS983019:HRS983049 IBO983019:IBO983049 ILK983019:ILK983049 IVG983019:IVG983049 JFC983019:JFC983049 JOY983019:JOY983049 JYU983019:JYU983049 KIQ983019:KIQ983049 KSM983019:KSM983049 LCI983019:LCI983049 LME983019:LME983049 LWA983019:LWA983049 MFW983019:MFW983049 MPS983019:MPS983049 MZO983019:MZO983049 NJK983019:NJK983049 NTG983019:NTG983049 ODC983019:ODC983049 OMY983019:OMY983049 OWU983019:OWU983049 PGQ983019:PGQ983049 PQM983019:PQM983049 QAI983019:QAI983049 QKE983019:QKE983049 QUA983019:QUA983049 RDW983019:RDW983049 RNS983019:RNS983049 RXO983019:RXO983049 SHK983019:SHK983049 SRG983019:SRG983049 TBC983019:TBC983049 TKY983019:TKY983049 TUU983019:TUU983049 UEQ983019:UEQ983049 UOM983019:UOM983049 UYI983019:UYI983049 VIE983019:VIE983049 VSA983019:VSA983049 WBW983019:WBW983049 WLS983019:WLS983049 WVO983019:WVO983049 K983019:K983049 K65515:K65545 K131051:K131081 K196587:K196617 K262123:K262153 K327659:K327689 K393195:K393225 K458731:K458761 K524267:K524297 K589803:K589833 K655339:K655369 K720875:K720905 K786411:K786441 K851947:K851977 K917483:K917513 JC4:JC20 SY4:SY20 ACU4:ACU20 AMQ4:AMQ20 AWM4:AWM20 BGI4:BGI20 BQE4:BQE20 CAA4:CAA20 CJW4:CJW20 CTS4:CTS20 DDO4:DDO20 DNK4:DNK20 DXG4:DXG20 EHC4:EHC20 EQY4:EQY20 FAU4:FAU20 FKQ4:FKQ20 FUM4:FUM20 GEI4:GEI20 GOE4:GOE20 GYA4:GYA20 HHW4:HHW20 HRS4:HRS20 IBO4:IBO20 ILK4:ILK20 IVG4:IVG20 JFC4:JFC20 JOY4:JOY20 JYU4:JYU20 KIQ4:KIQ20 KSM4:KSM20 LCI4:LCI20 LME4:LME20 LWA4:LWA20 MFW4:MFW20 MPS4:MPS20 MZO4:MZO20 NJK4:NJK20 NTG4:NTG20 ODC4:ODC20 OMY4:OMY20 OWU4:OWU20 PGQ4:PGQ20 PQM4:PQM20 QAI4:QAI20 QKE4:QKE20 QUA4:QUA20 RDW4:RDW20 RNS4:RNS20 RXO4:RXO20 SHK4:SHK20 SRG4:SRG20 TBC4:TBC20 TKY4:TKY20 TUU4:TUU20 UEQ4:UEQ20 UOM4:UOM20 UYI4:UYI20 VIE4:VIE20 VSA4:VSA20 WBW4:WBW20 WLS4:WLS20 WVO4:WVO20" xr:uid="{00000000-0002-0000-0200-00000F000000}">
       <formula1>"Vinculado Directo,Temporal,Asociado (Cooperativa),Contratista,Independiente,Otro"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R65515:S65545 R131051:S131081 JJ65515:JJ65545 TF65515:TF65545 ADB65515:ADB65545 AMX65515:AMX65545 AWT65515:AWT65545 BGP65515:BGP65545 BQL65515:BQL65545 CAH65515:CAH65545 CKD65515:CKD65545 CTZ65515:CTZ65545 DDV65515:DDV65545 DNR65515:DNR65545 DXN65515:DXN65545 EHJ65515:EHJ65545 ERF65515:ERF65545 FBB65515:FBB65545 FKX65515:FKX65545 FUT65515:FUT65545 GEP65515:GEP65545 GOL65515:GOL65545 GYH65515:GYH65545 HID65515:HID65545 HRZ65515:HRZ65545 IBV65515:IBV65545 ILR65515:ILR65545 IVN65515:IVN65545 JFJ65515:JFJ65545 JPF65515:JPF65545 JZB65515:JZB65545 KIX65515:KIX65545 KST65515:KST65545 LCP65515:LCP65545 LML65515:LML65545 LWH65515:LWH65545 MGD65515:MGD65545 MPZ65515:MPZ65545 MZV65515:MZV65545 NJR65515:NJR65545 NTN65515:NTN65545 ODJ65515:ODJ65545 ONF65515:ONF65545 OXB65515:OXB65545 PGX65515:PGX65545 PQT65515:PQT65545 QAP65515:QAP65545 QKL65515:QKL65545 QUH65515:QUH65545 RED65515:RED65545 RNZ65515:RNZ65545 RXV65515:RXV65545 SHR65515:SHR65545 SRN65515:SRN65545 TBJ65515:TBJ65545 TLF65515:TLF65545 TVB65515:TVB65545 UEX65515:UEX65545 UOT65515:UOT65545 UYP65515:UYP65545 VIL65515:VIL65545 VSH65515:VSH65545 WCD65515:WCD65545 WLZ65515:WLZ65545 WVV65515:WVV65545 R196587:S196617 JJ131051:JJ131081 TF131051:TF131081 ADB131051:ADB131081 AMX131051:AMX131081 AWT131051:AWT131081 BGP131051:BGP131081 BQL131051:BQL131081 CAH131051:CAH131081 CKD131051:CKD131081 CTZ131051:CTZ131081 DDV131051:DDV131081 DNR131051:DNR131081 DXN131051:DXN131081 EHJ131051:EHJ131081 ERF131051:ERF131081 FBB131051:FBB131081 FKX131051:FKX131081 FUT131051:FUT131081 GEP131051:GEP131081 GOL131051:GOL131081 GYH131051:GYH131081 HID131051:HID131081 HRZ131051:HRZ131081 IBV131051:IBV131081 ILR131051:ILR131081 IVN131051:IVN131081 JFJ131051:JFJ131081 JPF131051:JPF131081 JZB131051:JZB131081 KIX131051:KIX131081 KST131051:KST131081 LCP131051:LCP131081 LML131051:LML131081 LWH131051:LWH131081 MGD131051:MGD131081 MPZ131051:MPZ131081 MZV131051:MZV131081 NJR131051:NJR131081 NTN131051:NTN131081 ODJ131051:ODJ131081 ONF131051:ONF131081 OXB131051:OXB131081 PGX131051:PGX131081 PQT131051:PQT131081 QAP131051:QAP131081 QKL131051:QKL131081 QUH131051:QUH131081 RED131051:RED131081 RNZ131051:RNZ131081 RXV131051:RXV131081 SHR131051:SHR131081 SRN131051:SRN131081 TBJ131051:TBJ131081 TLF131051:TLF131081 TVB131051:TVB131081 UEX131051:UEX131081 UOT131051:UOT131081 UYP131051:UYP131081 VIL131051:VIL131081 VSH131051:VSH131081 WCD131051:WCD131081 WLZ131051:WLZ131081 WVV131051:WVV131081 R262123:S262153 JJ196587:JJ196617 TF196587:TF196617 ADB196587:ADB196617 AMX196587:AMX196617 AWT196587:AWT196617 BGP196587:BGP196617 BQL196587:BQL196617 CAH196587:CAH196617 CKD196587:CKD196617 CTZ196587:CTZ196617 DDV196587:DDV196617 DNR196587:DNR196617 DXN196587:DXN196617 EHJ196587:EHJ196617 ERF196587:ERF196617 FBB196587:FBB196617 FKX196587:FKX196617 FUT196587:FUT196617 GEP196587:GEP196617 GOL196587:GOL196617 GYH196587:GYH196617 HID196587:HID196617 HRZ196587:HRZ196617 IBV196587:IBV196617 ILR196587:ILR196617 IVN196587:IVN196617 JFJ196587:JFJ196617 JPF196587:JPF196617 JZB196587:JZB196617 KIX196587:KIX196617 KST196587:KST196617 LCP196587:LCP196617 LML196587:LML196617 LWH196587:LWH196617 MGD196587:MGD196617 MPZ196587:MPZ196617 MZV196587:MZV196617 NJR196587:NJR196617 NTN196587:NTN196617 ODJ196587:ODJ196617 ONF196587:ONF196617 OXB196587:OXB196617 PGX196587:PGX196617 PQT196587:PQT196617 QAP196587:QAP196617 QKL196587:QKL196617 QUH196587:QUH196617 RED196587:RED196617 RNZ196587:RNZ196617 RXV196587:RXV196617 SHR196587:SHR196617 SRN196587:SRN196617 TBJ196587:TBJ196617 TLF196587:TLF196617 TVB196587:TVB196617 UEX196587:UEX196617 UOT196587:UOT196617 UYP196587:UYP196617 VIL196587:VIL196617 VSH196587:VSH196617 WCD196587:WCD196617 WLZ196587:WLZ196617 WVV196587:WVV196617 R327659:S327689 JJ262123:JJ262153 TF262123:TF262153 ADB262123:ADB262153 AMX262123:AMX262153 AWT262123:AWT262153 BGP262123:BGP262153 BQL262123:BQL262153 CAH262123:CAH262153 CKD262123:CKD262153 CTZ262123:CTZ262153 DDV262123:DDV262153 DNR262123:DNR262153 DXN262123:DXN262153 EHJ262123:EHJ262153 ERF262123:ERF262153 FBB262123:FBB262153 FKX262123:FKX262153 FUT262123:FUT262153 GEP262123:GEP262153 GOL262123:GOL262153 GYH262123:GYH262153 HID262123:HID262153 HRZ262123:HRZ262153 IBV262123:IBV262153 ILR262123:ILR262153 IVN262123:IVN262153 JFJ262123:JFJ262153 JPF262123:JPF262153 JZB262123:JZB262153 KIX262123:KIX262153 KST262123:KST262153 LCP262123:LCP262153 LML262123:LML262153 LWH262123:LWH262153 MGD262123:MGD262153 MPZ262123:MPZ262153 MZV262123:MZV262153 NJR262123:NJR262153 NTN262123:NTN262153 ODJ262123:ODJ262153 ONF262123:ONF262153 OXB262123:OXB262153 PGX262123:PGX262153 PQT262123:PQT262153 QAP262123:QAP262153 QKL262123:QKL262153 QUH262123:QUH262153 RED262123:RED262153 RNZ262123:RNZ262153 RXV262123:RXV262153 SHR262123:SHR262153 SRN262123:SRN262153 TBJ262123:TBJ262153 TLF262123:TLF262153 TVB262123:TVB262153 UEX262123:UEX262153 UOT262123:UOT262153 UYP262123:UYP262153 VIL262123:VIL262153 VSH262123:VSH262153 WCD262123:WCD262153 WLZ262123:WLZ262153 WVV262123:WVV262153 R393195:S393225 JJ327659:JJ327689 TF327659:TF327689 ADB327659:ADB327689 AMX327659:AMX327689 AWT327659:AWT327689 BGP327659:BGP327689 BQL327659:BQL327689 CAH327659:CAH327689 CKD327659:CKD327689 CTZ327659:CTZ327689 DDV327659:DDV327689 DNR327659:DNR327689 DXN327659:DXN327689 EHJ327659:EHJ327689 ERF327659:ERF327689 FBB327659:FBB327689 FKX327659:FKX327689 FUT327659:FUT327689 GEP327659:GEP327689 GOL327659:GOL327689 GYH327659:GYH327689 HID327659:HID327689 HRZ327659:HRZ327689 IBV327659:IBV327689 ILR327659:ILR327689 IVN327659:IVN327689 JFJ327659:JFJ327689 JPF327659:JPF327689 JZB327659:JZB327689 KIX327659:KIX327689 KST327659:KST327689 LCP327659:LCP327689 LML327659:LML327689 LWH327659:LWH327689 MGD327659:MGD327689 MPZ327659:MPZ327689 MZV327659:MZV327689 NJR327659:NJR327689 NTN327659:NTN327689 ODJ327659:ODJ327689 ONF327659:ONF327689 OXB327659:OXB327689 PGX327659:PGX327689 PQT327659:PQT327689 QAP327659:QAP327689 QKL327659:QKL327689 QUH327659:QUH327689 RED327659:RED327689 RNZ327659:RNZ327689 RXV327659:RXV327689 SHR327659:SHR327689 SRN327659:SRN327689 TBJ327659:TBJ327689 TLF327659:TLF327689 TVB327659:TVB327689 UEX327659:UEX327689 UOT327659:UOT327689 UYP327659:UYP327689 VIL327659:VIL327689 VSH327659:VSH327689 WCD327659:WCD327689 WLZ327659:WLZ327689 WVV327659:WVV327689 R458731:S458761 JJ393195:JJ393225 TF393195:TF393225 ADB393195:ADB393225 AMX393195:AMX393225 AWT393195:AWT393225 BGP393195:BGP393225 BQL393195:BQL393225 CAH393195:CAH393225 CKD393195:CKD393225 CTZ393195:CTZ393225 DDV393195:DDV393225 DNR393195:DNR393225 DXN393195:DXN393225 EHJ393195:EHJ393225 ERF393195:ERF393225 FBB393195:FBB393225 FKX393195:FKX393225 FUT393195:FUT393225 GEP393195:GEP393225 GOL393195:GOL393225 GYH393195:GYH393225 HID393195:HID393225 HRZ393195:HRZ393225 IBV393195:IBV393225 ILR393195:ILR393225 IVN393195:IVN393225 JFJ393195:JFJ393225 JPF393195:JPF393225 JZB393195:JZB393225 KIX393195:KIX393225 KST393195:KST393225 LCP393195:LCP393225 LML393195:LML393225 LWH393195:LWH393225 MGD393195:MGD393225 MPZ393195:MPZ393225 MZV393195:MZV393225 NJR393195:NJR393225 NTN393195:NTN393225 ODJ393195:ODJ393225 ONF393195:ONF393225 OXB393195:OXB393225 PGX393195:PGX393225 PQT393195:PQT393225 QAP393195:QAP393225 QKL393195:QKL393225 QUH393195:QUH393225 RED393195:RED393225 RNZ393195:RNZ393225 RXV393195:RXV393225 SHR393195:SHR393225 SRN393195:SRN393225 TBJ393195:TBJ393225 TLF393195:TLF393225 TVB393195:TVB393225 UEX393195:UEX393225 UOT393195:UOT393225 UYP393195:UYP393225 VIL393195:VIL393225 VSH393195:VSH393225 WCD393195:WCD393225 WLZ393195:WLZ393225 WVV393195:WVV393225 R524267:S524297 JJ458731:JJ458761 TF458731:TF458761 ADB458731:ADB458761 AMX458731:AMX458761 AWT458731:AWT458761 BGP458731:BGP458761 BQL458731:BQL458761 CAH458731:CAH458761 CKD458731:CKD458761 CTZ458731:CTZ458761 DDV458731:DDV458761 DNR458731:DNR458761 DXN458731:DXN458761 EHJ458731:EHJ458761 ERF458731:ERF458761 FBB458731:FBB458761 FKX458731:FKX458761 FUT458731:FUT458761 GEP458731:GEP458761 GOL458731:GOL458761 GYH458731:GYH458761 HID458731:HID458761 HRZ458731:HRZ458761 IBV458731:IBV458761 ILR458731:ILR458761 IVN458731:IVN458761 JFJ458731:JFJ458761 JPF458731:JPF458761 JZB458731:JZB458761 KIX458731:KIX458761 KST458731:KST458761 LCP458731:LCP458761 LML458731:LML458761 LWH458731:LWH458761 MGD458731:MGD458761 MPZ458731:MPZ458761 MZV458731:MZV458761 NJR458731:NJR458761 NTN458731:NTN458761 ODJ458731:ODJ458761 ONF458731:ONF458761 OXB458731:OXB458761 PGX458731:PGX458761 PQT458731:PQT458761 QAP458731:QAP458761 QKL458731:QKL458761 QUH458731:QUH458761 RED458731:RED458761 RNZ458731:RNZ458761 RXV458731:RXV458761 SHR458731:SHR458761 SRN458731:SRN458761 TBJ458731:TBJ458761 TLF458731:TLF458761 TVB458731:TVB458761 UEX458731:UEX458761 UOT458731:UOT458761 UYP458731:UYP458761 VIL458731:VIL458761 VSH458731:VSH458761 WCD458731:WCD458761 WLZ458731:WLZ458761 WVV458731:WVV458761 R589803:S589833 JJ524267:JJ524297 TF524267:TF524297 ADB524267:ADB524297 AMX524267:AMX524297 AWT524267:AWT524297 BGP524267:BGP524297 BQL524267:BQL524297 CAH524267:CAH524297 CKD524267:CKD524297 CTZ524267:CTZ524297 DDV524267:DDV524297 DNR524267:DNR524297 DXN524267:DXN524297 EHJ524267:EHJ524297 ERF524267:ERF524297 FBB524267:FBB524297 FKX524267:FKX524297 FUT524267:FUT524297 GEP524267:GEP524297 GOL524267:GOL524297 GYH524267:GYH524297 HID524267:HID524297 HRZ524267:HRZ524297 IBV524267:IBV524297 ILR524267:ILR524297 IVN524267:IVN524297 JFJ524267:JFJ524297 JPF524267:JPF524297 JZB524267:JZB524297 KIX524267:KIX524297 KST524267:KST524297 LCP524267:LCP524297 LML524267:LML524297 LWH524267:LWH524297 MGD524267:MGD524297 MPZ524267:MPZ524297 MZV524267:MZV524297 NJR524267:NJR524297 NTN524267:NTN524297 ODJ524267:ODJ524297 ONF524267:ONF524297 OXB524267:OXB524297 PGX524267:PGX524297 PQT524267:PQT524297 QAP524267:QAP524297 QKL524267:QKL524297 QUH524267:QUH524297 RED524267:RED524297 RNZ524267:RNZ524297 RXV524267:RXV524297 SHR524267:SHR524297 SRN524267:SRN524297 TBJ524267:TBJ524297 TLF524267:TLF524297 TVB524267:TVB524297 UEX524267:UEX524297 UOT524267:UOT524297 UYP524267:UYP524297 VIL524267:VIL524297 VSH524267:VSH524297 WCD524267:WCD524297 WLZ524267:WLZ524297 WVV524267:WVV524297 R655339:S655369 JJ589803:JJ589833 TF589803:TF589833 ADB589803:ADB589833 AMX589803:AMX589833 AWT589803:AWT589833 BGP589803:BGP589833 BQL589803:BQL589833 CAH589803:CAH589833 CKD589803:CKD589833 CTZ589803:CTZ589833 DDV589803:DDV589833 DNR589803:DNR589833 DXN589803:DXN589833 EHJ589803:EHJ589833 ERF589803:ERF589833 FBB589803:FBB589833 FKX589803:FKX589833 FUT589803:FUT589833 GEP589803:GEP589833 GOL589803:GOL589833 GYH589803:GYH589833 HID589803:HID589833 HRZ589803:HRZ589833 IBV589803:IBV589833 ILR589803:ILR589833 IVN589803:IVN589833 JFJ589803:JFJ589833 JPF589803:JPF589833 JZB589803:JZB589833 KIX589803:KIX589833 KST589803:KST589833 LCP589803:LCP589833 LML589803:LML589833 LWH589803:LWH589833 MGD589803:MGD589833 MPZ589803:MPZ589833 MZV589803:MZV589833 NJR589803:NJR589833 NTN589803:NTN589833 ODJ589803:ODJ589833 ONF589803:ONF589833 OXB589803:OXB589833 PGX589803:PGX589833 PQT589803:PQT589833 QAP589803:QAP589833 QKL589803:QKL589833 QUH589803:QUH589833 RED589803:RED589833 RNZ589803:RNZ589833 RXV589803:RXV589833 SHR589803:SHR589833 SRN589803:SRN589833 TBJ589803:TBJ589833 TLF589803:TLF589833 TVB589803:TVB589833 UEX589803:UEX589833 UOT589803:UOT589833 UYP589803:UYP589833 VIL589803:VIL589833 VSH589803:VSH589833 WCD589803:WCD589833 WLZ589803:WLZ589833 WVV589803:WVV589833 R720875:S720905 JJ655339:JJ655369 TF655339:TF655369 ADB655339:ADB655369 AMX655339:AMX655369 AWT655339:AWT655369 BGP655339:BGP655369 BQL655339:BQL655369 CAH655339:CAH655369 CKD655339:CKD655369 CTZ655339:CTZ655369 DDV655339:DDV655369 DNR655339:DNR655369 DXN655339:DXN655369 EHJ655339:EHJ655369 ERF655339:ERF655369 FBB655339:FBB655369 FKX655339:FKX655369 FUT655339:FUT655369 GEP655339:GEP655369 GOL655339:GOL655369 GYH655339:GYH655369 HID655339:HID655369 HRZ655339:HRZ655369 IBV655339:IBV655369 ILR655339:ILR655369 IVN655339:IVN655369 JFJ655339:JFJ655369 JPF655339:JPF655369 JZB655339:JZB655369 KIX655339:KIX655369 KST655339:KST655369 LCP655339:LCP655369 LML655339:LML655369 LWH655339:LWH655369 MGD655339:MGD655369 MPZ655339:MPZ655369 MZV655339:MZV655369 NJR655339:NJR655369 NTN655339:NTN655369 ODJ655339:ODJ655369 ONF655339:ONF655369 OXB655339:OXB655369 PGX655339:PGX655369 PQT655339:PQT655369 QAP655339:QAP655369 QKL655339:QKL655369 QUH655339:QUH655369 RED655339:RED655369 RNZ655339:RNZ655369 RXV655339:RXV655369 SHR655339:SHR655369 SRN655339:SRN655369 TBJ655339:TBJ655369 TLF655339:TLF655369 TVB655339:TVB655369 UEX655339:UEX655369 UOT655339:UOT655369 UYP655339:UYP655369 VIL655339:VIL655369 VSH655339:VSH655369 WCD655339:WCD655369 WLZ655339:WLZ655369 WVV655339:WVV655369 R786411:S786441 JJ720875:JJ720905 TF720875:TF720905 ADB720875:ADB720905 AMX720875:AMX720905 AWT720875:AWT720905 BGP720875:BGP720905 BQL720875:BQL720905 CAH720875:CAH720905 CKD720875:CKD720905 CTZ720875:CTZ720905 DDV720875:DDV720905 DNR720875:DNR720905 DXN720875:DXN720905 EHJ720875:EHJ720905 ERF720875:ERF720905 FBB720875:FBB720905 FKX720875:FKX720905 FUT720875:FUT720905 GEP720875:GEP720905 GOL720875:GOL720905 GYH720875:GYH720905 HID720875:HID720905 HRZ720875:HRZ720905 IBV720875:IBV720905 ILR720875:ILR720905 IVN720875:IVN720905 JFJ720875:JFJ720905 JPF720875:JPF720905 JZB720875:JZB720905 KIX720875:KIX720905 KST720875:KST720905 LCP720875:LCP720905 LML720875:LML720905 LWH720875:LWH720905 MGD720875:MGD720905 MPZ720875:MPZ720905 MZV720875:MZV720905 NJR720875:NJR720905 NTN720875:NTN720905 ODJ720875:ODJ720905 ONF720875:ONF720905 OXB720875:OXB720905 PGX720875:PGX720905 PQT720875:PQT720905 QAP720875:QAP720905 QKL720875:QKL720905 QUH720875:QUH720905 RED720875:RED720905 RNZ720875:RNZ720905 RXV720875:RXV720905 SHR720875:SHR720905 SRN720875:SRN720905 TBJ720875:TBJ720905 TLF720875:TLF720905 TVB720875:TVB720905 UEX720875:UEX720905 UOT720875:UOT720905 UYP720875:UYP720905 VIL720875:VIL720905 VSH720875:VSH720905 WCD720875:WCD720905 WLZ720875:WLZ720905 WVV720875:WVV720905 R851947:S851977 JJ786411:JJ786441 TF786411:TF786441 ADB786411:ADB786441 AMX786411:AMX786441 AWT786411:AWT786441 BGP786411:BGP786441 BQL786411:BQL786441 CAH786411:CAH786441 CKD786411:CKD786441 CTZ786411:CTZ786441 DDV786411:DDV786441 DNR786411:DNR786441 DXN786411:DXN786441 EHJ786411:EHJ786441 ERF786411:ERF786441 FBB786411:FBB786441 FKX786411:FKX786441 FUT786411:FUT786441 GEP786411:GEP786441 GOL786411:GOL786441 GYH786411:GYH786441 HID786411:HID786441 HRZ786411:HRZ786441 IBV786411:IBV786441 ILR786411:ILR786441 IVN786411:IVN786441 JFJ786411:JFJ786441 JPF786411:JPF786441 JZB786411:JZB786441 KIX786411:KIX786441 KST786411:KST786441 LCP786411:LCP786441 LML786411:LML786441 LWH786411:LWH786441 MGD786411:MGD786441 MPZ786411:MPZ786441 MZV786411:MZV786441 NJR786411:NJR786441 NTN786411:NTN786441 ODJ786411:ODJ786441 ONF786411:ONF786441 OXB786411:OXB786441 PGX786411:PGX786441 PQT786411:PQT786441 QAP786411:QAP786441 QKL786411:QKL786441 QUH786411:QUH786441 RED786411:RED786441 RNZ786411:RNZ786441 RXV786411:RXV786441 SHR786411:SHR786441 SRN786411:SRN786441 TBJ786411:TBJ786441 TLF786411:TLF786441 TVB786411:TVB786441 UEX786411:UEX786441 UOT786411:UOT786441 UYP786411:UYP786441 VIL786411:VIL786441 VSH786411:VSH786441 WCD786411:WCD786441 WLZ786411:WLZ786441 WVV786411:WVV786441 R917483:S917513 JJ851947:JJ851977 TF851947:TF851977 ADB851947:ADB851977 AMX851947:AMX851977 AWT851947:AWT851977 BGP851947:BGP851977 BQL851947:BQL851977 CAH851947:CAH851977 CKD851947:CKD851977 CTZ851947:CTZ851977 DDV851947:DDV851977 DNR851947:DNR851977 DXN851947:DXN851977 EHJ851947:EHJ851977 ERF851947:ERF851977 FBB851947:FBB851977 FKX851947:FKX851977 FUT851947:FUT851977 GEP851947:GEP851977 GOL851947:GOL851977 GYH851947:GYH851977 HID851947:HID851977 HRZ851947:HRZ851977 IBV851947:IBV851977 ILR851947:ILR851977 IVN851947:IVN851977 JFJ851947:JFJ851977 JPF851947:JPF851977 JZB851947:JZB851977 KIX851947:KIX851977 KST851947:KST851977 LCP851947:LCP851977 LML851947:LML851977 LWH851947:LWH851977 MGD851947:MGD851977 MPZ851947:MPZ851977 MZV851947:MZV851977 NJR851947:NJR851977 NTN851947:NTN851977 ODJ851947:ODJ851977 ONF851947:ONF851977 OXB851947:OXB851977 PGX851947:PGX851977 PQT851947:PQT851977 QAP851947:QAP851977 QKL851947:QKL851977 QUH851947:QUH851977 RED851947:RED851977 RNZ851947:RNZ851977 RXV851947:RXV851977 SHR851947:SHR851977 SRN851947:SRN851977 TBJ851947:TBJ851977 TLF851947:TLF851977 TVB851947:TVB851977 UEX851947:UEX851977 UOT851947:UOT851977 UYP851947:UYP851977 VIL851947:VIL851977 VSH851947:VSH851977 WCD851947:WCD851977 WLZ851947:WLZ851977 WVV851947:WVV851977 R983019:S983049 JJ917483:JJ917513 TF917483:TF917513 ADB917483:ADB917513 AMX917483:AMX917513 AWT917483:AWT917513 BGP917483:BGP917513 BQL917483:BQL917513 CAH917483:CAH917513 CKD917483:CKD917513 CTZ917483:CTZ917513 DDV917483:DDV917513 DNR917483:DNR917513 DXN917483:DXN917513 EHJ917483:EHJ917513 ERF917483:ERF917513 FBB917483:FBB917513 FKX917483:FKX917513 FUT917483:FUT917513 GEP917483:GEP917513 GOL917483:GOL917513 GYH917483:GYH917513 HID917483:HID917513 HRZ917483:HRZ917513 IBV917483:IBV917513 ILR917483:ILR917513 IVN917483:IVN917513 JFJ917483:JFJ917513 JPF917483:JPF917513 JZB917483:JZB917513 KIX917483:KIX917513 KST917483:KST917513 LCP917483:LCP917513 LML917483:LML917513 LWH917483:LWH917513 MGD917483:MGD917513 MPZ917483:MPZ917513 MZV917483:MZV917513 NJR917483:NJR917513 NTN917483:NTN917513 ODJ917483:ODJ917513 ONF917483:ONF917513 OXB917483:OXB917513 PGX917483:PGX917513 PQT917483:PQT917513 QAP917483:QAP917513 QKL917483:QKL917513 QUH917483:QUH917513 RED917483:RED917513 RNZ917483:RNZ917513 RXV917483:RXV917513 SHR917483:SHR917513 SRN917483:SRN917513 TBJ917483:TBJ917513 TLF917483:TLF917513 TVB917483:TVB917513 UEX917483:UEX917513 UOT917483:UOT917513 UYP917483:UYP917513 VIL917483:VIL917513 VSH917483:VSH917513 WCD917483:WCD917513 WLZ917483:WLZ917513 WVV917483:WVV917513 WVV983019:WVV983049 JJ983019:JJ983049 TF983019:TF983049 ADB983019:ADB983049 AMX983019:AMX983049 AWT983019:AWT983049 BGP983019:BGP983049 BQL983019:BQL983049 CAH983019:CAH983049 CKD983019:CKD983049 CTZ983019:CTZ983049 DDV983019:DDV983049 DNR983019:DNR983049 DXN983019:DXN983049 EHJ983019:EHJ983049 ERF983019:ERF983049 FBB983019:FBB983049 FKX983019:FKX983049 FUT983019:FUT983049 GEP983019:GEP983049 GOL983019:GOL983049 GYH983019:GYH983049 HID983019:HID983049 HRZ983019:HRZ983049 IBV983019:IBV983049 ILR983019:ILR983049 IVN983019:IVN983049 JFJ983019:JFJ983049 JPF983019:JPF983049 JZB983019:JZB983049 KIX983019:KIX983049 KST983019:KST983049 LCP983019:LCP983049 LML983019:LML983049 LWH983019:LWH983049 MGD983019:MGD983049 MPZ983019:MPZ983049 MZV983019:MZV983049 NJR983019:NJR983049 NTN983019:NTN983049 ODJ983019:ODJ983049 ONF983019:ONF983049 OXB983019:OXB983049 PGX983019:PGX983049 PQT983019:PQT983049 QAP983019:QAP983049 QKL983019:QKL983049 QUH983019:QUH983049 RED983019:RED983049 RNZ983019:RNZ983049 RXV983019:RXV983049 SHR983019:SHR983049 SRN983019:SRN983049 TBJ983019:TBJ983049 TLF983019:TLF983049 TVB983019:TVB983049 UEX983019:UEX983049 UOT983019:UOT983049 UYP983019:UYP983049 VIL983019:VIL983049 VSH983019:VSH983049 WCD983019:WCD983049 WLZ983019:WLZ983049 WLZ4:WLZ20 WCD4:WCD20 VSH4:VSH20 VIL4:VIL20 UYP4:UYP20 UOT4:UOT20 UEX4:UEX20 TVB4:TVB20 TLF4:TLF20 TBJ4:TBJ20 SRN4:SRN20 SHR4:SHR20 RXV4:RXV20 RNZ4:RNZ20 RED4:RED20 QUH4:QUH20 QKL4:QKL20 QAP4:QAP20 PQT4:PQT20 PGX4:PGX20 OXB4:OXB20 ONF4:ONF20 ODJ4:ODJ20 NTN4:NTN20 NJR4:NJR20 MZV4:MZV20 MPZ4:MPZ20 MGD4:MGD20 LWH4:LWH20 LML4:LML20 LCP4:LCP20 KST4:KST20 KIX4:KIX20 JZB4:JZB20 JPF4:JPF20 JFJ4:JFJ20 IVN4:IVN20 ILR4:ILR20 IBV4:IBV20 HRZ4:HRZ20 HID4:HID20 GYH4:GYH20 GOL4:GOL20 GEP4:GEP20 FUT4:FUT20 FKX4:FKX20 FBB4:FBB20 ERF4:ERF20 EHJ4:EHJ20 DXN4:DXN20 DNR4:DNR20 DDV4:DDV20 CTZ4:CTZ20 CKD4:CKD20 CAH4:CAH20 BQL4:BQL20 BGP4:BGP20 AWT4:AWT20 AMX4:AMX20 ADB4:ADB20 TF4:TF20 JJ4:JJ20 WVV4:WVV20 R9:R20" xr:uid="{00000000-0002-0000-0200-000010000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R65515:S65545 R131051:S131081 JJ65515:JJ65545 TF65515:TF65545 ADB65515:ADB65545 AMX65515:AMX65545 AWT65515:AWT65545 BGP65515:BGP65545 BQL65515:BQL65545 CAH65515:CAH65545 CKD65515:CKD65545 CTZ65515:CTZ65545 DDV65515:DDV65545 DNR65515:DNR65545 DXN65515:DXN65545 EHJ65515:EHJ65545 ERF65515:ERF65545 FBB65515:FBB65545 FKX65515:FKX65545 FUT65515:FUT65545 GEP65515:GEP65545 GOL65515:GOL65545 GYH65515:GYH65545 HID65515:HID65545 HRZ65515:HRZ65545 IBV65515:IBV65545 ILR65515:ILR65545 IVN65515:IVN65545 JFJ65515:JFJ65545 JPF65515:JPF65545 JZB65515:JZB65545 KIX65515:KIX65545 KST65515:KST65545 LCP65515:LCP65545 LML65515:LML65545 LWH65515:LWH65545 MGD65515:MGD65545 MPZ65515:MPZ65545 MZV65515:MZV65545 NJR65515:NJR65545 NTN65515:NTN65545 ODJ65515:ODJ65545 ONF65515:ONF65545 OXB65515:OXB65545 PGX65515:PGX65545 PQT65515:PQT65545 QAP65515:QAP65545 QKL65515:QKL65545 QUH65515:QUH65545 RED65515:RED65545 RNZ65515:RNZ65545 RXV65515:RXV65545 SHR65515:SHR65545 SRN65515:SRN65545 TBJ65515:TBJ65545 TLF65515:TLF65545 TVB65515:TVB65545 UEX65515:UEX65545 UOT65515:UOT65545 UYP65515:UYP65545 VIL65515:VIL65545 VSH65515:VSH65545 WCD65515:WCD65545 WLZ65515:WLZ65545 WVV65515:WVV65545 R196587:S196617 JJ131051:JJ131081 TF131051:TF131081 ADB131051:ADB131081 AMX131051:AMX131081 AWT131051:AWT131081 BGP131051:BGP131081 BQL131051:BQL131081 CAH131051:CAH131081 CKD131051:CKD131081 CTZ131051:CTZ131081 DDV131051:DDV131081 DNR131051:DNR131081 DXN131051:DXN131081 EHJ131051:EHJ131081 ERF131051:ERF131081 FBB131051:FBB131081 FKX131051:FKX131081 FUT131051:FUT131081 GEP131051:GEP131081 GOL131051:GOL131081 GYH131051:GYH131081 HID131051:HID131081 HRZ131051:HRZ131081 IBV131051:IBV131081 ILR131051:ILR131081 IVN131051:IVN131081 JFJ131051:JFJ131081 JPF131051:JPF131081 JZB131051:JZB131081 KIX131051:KIX131081 KST131051:KST131081 LCP131051:LCP131081 LML131051:LML131081 LWH131051:LWH131081 MGD131051:MGD131081 MPZ131051:MPZ131081 MZV131051:MZV131081 NJR131051:NJR131081 NTN131051:NTN131081 ODJ131051:ODJ131081 ONF131051:ONF131081 OXB131051:OXB131081 PGX131051:PGX131081 PQT131051:PQT131081 QAP131051:QAP131081 QKL131051:QKL131081 QUH131051:QUH131081 RED131051:RED131081 RNZ131051:RNZ131081 RXV131051:RXV131081 SHR131051:SHR131081 SRN131051:SRN131081 TBJ131051:TBJ131081 TLF131051:TLF131081 TVB131051:TVB131081 UEX131051:UEX131081 UOT131051:UOT131081 UYP131051:UYP131081 VIL131051:VIL131081 VSH131051:VSH131081 WCD131051:WCD131081 WLZ131051:WLZ131081 WVV131051:WVV131081 R262123:S262153 JJ196587:JJ196617 TF196587:TF196617 ADB196587:ADB196617 AMX196587:AMX196617 AWT196587:AWT196617 BGP196587:BGP196617 BQL196587:BQL196617 CAH196587:CAH196617 CKD196587:CKD196617 CTZ196587:CTZ196617 DDV196587:DDV196617 DNR196587:DNR196617 DXN196587:DXN196617 EHJ196587:EHJ196617 ERF196587:ERF196617 FBB196587:FBB196617 FKX196587:FKX196617 FUT196587:FUT196617 GEP196587:GEP196617 GOL196587:GOL196617 GYH196587:GYH196617 HID196587:HID196617 HRZ196587:HRZ196617 IBV196587:IBV196617 ILR196587:ILR196617 IVN196587:IVN196617 JFJ196587:JFJ196617 JPF196587:JPF196617 JZB196587:JZB196617 KIX196587:KIX196617 KST196587:KST196617 LCP196587:LCP196617 LML196587:LML196617 LWH196587:LWH196617 MGD196587:MGD196617 MPZ196587:MPZ196617 MZV196587:MZV196617 NJR196587:NJR196617 NTN196587:NTN196617 ODJ196587:ODJ196617 ONF196587:ONF196617 OXB196587:OXB196617 PGX196587:PGX196617 PQT196587:PQT196617 QAP196587:QAP196617 QKL196587:QKL196617 QUH196587:QUH196617 RED196587:RED196617 RNZ196587:RNZ196617 RXV196587:RXV196617 SHR196587:SHR196617 SRN196587:SRN196617 TBJ196587:TBJ196617 TLF196587:TLF196617 TVB196587:TVB196617 UEX196587:UEX196617 UOT196587:UOT196617 UYP196587:UYP196617 VIL196587:VIL196617 VSH196587:VSH196617 WCD196587:WCD196617 WLZ196587:WLZ196617 WVV196587:WVV196617 R327659:S327689 JJ262123:JJ262153 TF262123:TF262153 ADB262123:ADB262153 AMX262123:AMX262153 AWT262123:AWT262153 BGP262123:BGP262153 BQL262123:BQL262153 CAH262123:CAH262153 CKD262123:CKD262153 CTZ262123:CTZ262153 DDV262123:DDV262153 DNR262123:DNR262153 DXN262123:DXN262153 EHJ262123:EHJ262153 ERF262123:ERF262153 FBB262123:FBB262153 FKX262123:FKX262153 FUT262123:FUT262153 GEP262123:GEP262153 GOL262123:GOL262153 GYH262123:GYH262153 HID262123:HID262153 HRZ262123:HRZ262153 IBV262123:IBV262153 ILR262123:ILR262153 IVN262123:IVN262153 JFJ262123:JFJ262153 JPF262123:JPF262153 JZB262123:JZB262153 KIX262123:KIX262153 KST262123:KST262153 LCP262123:LCP262153 LML262123:LML262153 LWH262123:LWH262153 MGD262123:MGD262153 MPZ262123:MPZ262153 MZV262123:MZV262153 NJR262123:NJR262153 NTN262123:NTN262153 ODJ262123:ODJ262153 ONF262123:ONF262153 OXB262123:OXB262153 PGX262123:PGX262153 PQT262123:PQT262153 QAP262123:QAP262153 QKL262123:QKL262153 QUH262123:QUH262153 RED262123:RED262153 RNZ262123:RNZ262153 RXV262123:RXV262153 SHR262123:SHR262153 SRN262123:SRN262153 TBJ262123:TBJ262153 TLF262123:TLF262153 TVB262123:TVB262153 UEX262123:UEX262153 UOT262123:UOT262153 UYP262123:UYP262153 VIL262123:VIL262153 VSH262123:VSH262153 WCD262123:WCD262153 WLZ262123:WLZ262153 WVV262123:WVV262153 R393195:S393225 JJ327659:JJ327689 TF327659:TF327689 ADB327659:ADB327689 AMX327659:AMX327689 AWT327659:AWT327689 BGP327659:BGP327689 BQL327659:BQL327689 CAH327659:CAH327689 CKD327659:CKD327689 CTZ327659:CTZ327689 DDV327659:DDV327689 DNR327659:DNR327689 DXN327659:DXN327689 EHJ327659:EHJ327689 ERF327659:ERF327689 FBB327659:FBB327689 FKX327659:FKX327689 FUT327659:FUT327689 GEP327659:GEP327689 GOL327659:GOL327689 GYH327659:GYH327689 HID327659:HID327689 HRZ327659:HRZ327689 IBV327659:IBV327689 ILR327659:ILR327689 IVN327659:IVN327689 JFJ327659:JFJ327689 JPF327659:JPF327689 JZB327659:JZB327689 KIX327659:KIX327689 KST327659:KST327689 LCP327659:LCP327689 LML327659:LML327689 LWH327659:LWH327689 MGD327659:MGD327689 MPZ327659:MPZ327689 MZV327659:MZV327689 NJR327659:NJR327689 NTN327659:NTN327689 ODJ327659:ODJ327689 ONF327659:ONF327689 OXB327659:OXB327689 PGX327659:PGX327689 PQT327659:PQT327689 QAP327659:QAP327689 QKL327659:QKL327689 QUH327659:QUH327689 RED327659:RED327689 RNZ327659:RNZ327689 RXV327659:RXV327689 SHR327659:SHR327689 SRN327659:SRN327689 TBJ327659:TBJ327689 TLF327659:TLF327689 TVB327659:TVB327689 UEX327659:UEX327689 UOT327659:UOT327689 UYP327659:UYP327689 VIL327659:VIL327689 VSH327659:VSH327689 WCD327659:WCD327689 WLZ327659:WLZ327689 WVV327659:WVV327689 R458731:S458761 JJ393195:JJ393225 TF393195:TF393225 ADB393195:ADB393225 AMX393195:AMX393225 AWT393195:AWT393225 BGP393195:BGP393225 BQL393195:BQL393225 CAH393195:CAH393225 CKD393195:CKD393225 CTZ393195:CTZ393225 DDV393195:DDV393225 DNR393195:DNR393225 DXN393195:DXN393225 EHJ393195:EHJ393225 ERF393195:ERF393225 FBB393195:FBB393225 FKX393195:FKX393225 FUT393195:FUT393225 GEP393195:GEP393225 GOL393195:GOL393225 GYH393195:GYH393225 HID393195:HID393225 HRZ393195:HRZ393225 IBV393195:IBV393225 ILR393195:ILR393225 IVN393195:IVN393225 JFJ393195:JFJ393225 JPF393195:JPF393225 JZB393195:JZB393225 KIX393195:KIX393225 KST393195:KST393225 LCP393195:LCP393225 LML393195:LML393225 LWH393195:LWH393225 MGD393195:MGD393225 MPZ393195:MPZ393225 MZV393195:MZV393225 NJR393195:NJR393225 NTN393195:NTN393225 ODJ393195:ODJ393225 ONF393195:ONF393225 OXB393195:OXB393225 PGX393195:PGX393225 PQT393195:PQT393225 QAP393195:QAP393225 QKL393195:QKL393225 QUH393195:QUH393225 RED393195:RED393225 RNZ393195:RNZ393225 RXV393195:RXV393225 SHR393195:SHR393225 SRN393195:SRN393225 TBJ393195:TBJ393225 TLF393195:TLF393225 TVB393195:TVB393225 UEX393195:UEX393225 UOT393195:UOT393225 UYP393195:UYP393225 VIL393195:VIL393225 VSH393195:VSH393225 WCD393195:WCD393225 WLZ393195:WLZ393225 WVV393195:WVV393225 R524267:S524297 JJ458731:JJ458761 TF458731:TF458761 ADB458731:ADB458761 AMX458731:AMX458761 AWT458731:AWT458761 BGP458731:BGP458761 BQL458731:BQL458761 CAH458731:CAH458761 CKD458731:CKD458761 CTZ458731:CTZ458761 DDV458731:DDV458761 DNR458731:DNR458761 DXN458731:DXN458761 EHJ458731:EHJ458761 ERF458731:ERF458761 FBB458731:FBB458761 FKX458731:FKX458761 FUT458731:FUT458761 GEP458731:GEP458761 GOL458731:GOL458761 GYH458731:GYH458761 HID458731:HID458761 HRZ458731:HRZ458761 IBV458731:IBV458761 ILR458731:ILR458761 IVN458731:IVN458761 JFJ458731:JFJ458761 JPF458731:JPF458761 JZB458731:JZB458761 KIX458731:KIX458761 KST458731:KST458761 LCP458731:LCP458761 LML458731:LML458761 LWH458731:LWH458761 MGD458731:MGD458761 MPZ458731:MPZ458761 MZV458731:MZV458761 NJR458731:NJR458761 NTN458731:NTN458761 ODJ458731:ODJ458761 ONF458731:ONF458761 OXB458731:OXB458761 PGX458731:PGX458761 PQT458731:PQT458761 QAP458731:QAP458761 QKL458731:QKL458761 QUH458731:QUH458761 RED458731:RED458761 RNZ458731:RNZ458761 RXV458731:RXV458761 SHR458731:SHR458761 SRN458731:SRN458761 TBJ458731:TBJ458761 TLF458731:TLF458761 TVB458731:TVB458761 UEX458731:UEX458761 UOT458731:UOT458761 UYP458731:UYP458761 VIL458731:VIL458761 VSH458731:VSH458761 WCD458731:WCD458761 WLZ458731:WLZ458761 WVV458731:WVV458761 R589803:S589833 JJ524267:JJ524297 TF524267:TF524297 ADB524267:ADB524297 AMX524267:AMX524297 AWT524267:AWT524297 BGP524267:BGP524297 BQL524267:BQL524297 CAH524267:CAH524297 CKD524267:CKD524297 CTZ524267:CTZ524297 DDV524267:DDV524297 DNR524267:DNR524297 DXN524267:DXN524297 EHJ524267:EHJ524297 ERF524267:ERF524297 FBB524267:FBB524297 FKX524267:FKX524297 FUT524267:FUT524297 GEP524267:GEP524297 GOL524267:GOL524297 GYH524267:GYH524297 HID524267:HID524297 HRZ524267:HRZ524297 IBV524267:IBV524297 ILR524267:ILR524297 IVN524267:IVN524297 JFJ524267:JFJ524297 JPF524267:JPF524297 JZB524267:JZB524297 KIX524267:KIX524297 KST524267:KST524297 LCP524267:LCP524297 LML524267:LML524297 LWH524267:LWH524297 MGD524267:MGD524297 MPZ524267:MPZ524297 MZV524267:MZV524297 NJR524267:NJR524297 NTN524267:NTN524297 ODJ524267:ODJ524297 ONF524267:ONF524297 OXB524267:OXB524297 PGX524267:PGX524297 PQT524267:PQT524297 QAP524267:QAP524297 QKL524267:QKL524297 QUH524267:QUH524297 RED524267:RED524297 RNZ524267:RNZ524297 RXV524267:RXV524297 SHR524267:SHR524297 SRN524267:SRN524297 TBJ524267:TBJ524297 TLF524267:TLF524297 TVB524267:TVB524297 UEX524267:UEX524297 UOT524267:UOT524297 UYP524267:UYP524297 VIL524267:VIL524297 VSH524267:VSH524297 WCD524267:WCD524297 WLZ524267:WLZ524297 WVV524267:WVV524297 R655339:S655369 JJ589803:JJ589833 TF589803:TF589833 ADB589803:ADB589833 AMX589803:AMX589833 AWT589803:AWT589833 BGP589803:BGP589833 BQL589803:BQL589833 CAH589803:CAH589833 CKD589803:CKD589833 CTZ589803:CTZ589833 DDV589803:DDV589833 DNR589803:DNR589833 DXN589803:DXN589833 EHJ589803:EHJ589833 ERF589803:ERF589833 FBB589803:FBB589833 FKX589803:FKX589833 FUT589803:FUT589833 GEP589803:GEP589833 GOL589803:GOL589833 GYH589803:GYH589833 HID589803:HID589833 HRZ589803:HRZ589833 IBV589803:IBV589833 ILR589803:ILR589833 IVN589803:IVN589833 JFJ589803:JFJ589833 JPF589803:JPF589833 JZB589803:JZB589833 KIX589803:KIX589833 KST589803:KST589833 LCP589803:LCP589833 LML589803:LML589833 LWH589803:LWH589833 MGD589803:MGD589833 MPZ589803:MPZ589833 MZV589803:MZV589833 NJR589803:NJR589833 NTN589803:NTN589833 ODJ589803:ODJ589833 ONF589803:ONF589833 OXB589803:OXB589833 PGX589803:PGX589833 PQT589803:PQT589833 QAP589803:QAP589833 QKL589803:QKL589833 QUH589803:QUH589833 RED589803:RED589833 RNZ589803:RNZ589833 RXV589803:RXV589833 SHR589803:SHR589833 SRN589803:SRN589833 TBJ589803:TBJ589833 TLF589803:TLF589833 TVB589803:TVB589833 UEX589803:UEX589833 UOT589803:UOT589833 UYP589803:UYP589833 VIL589803:VIL589833 VSH589803:VSH589833 WCD589803:WCD589833 WLZ589803:WLZ589833 WVV589803:WVV589833 R720875:S720905 JJ655339:JJ655369 TF655339:TF655369 ADB655339:ADB655369 AMX655339:AMX655369 AWT655339:AWT655369 BGP655339:BGP655369 BQL655339:BQL655369 CAH655339:CAH655369 CKD655339:CKD655369 CTZ655339:CTZ655369 DDV655339:DDV655369 DNR655339:DNR655369 DXN655339:DXN655369 EHJ655339:EHJ655369 ERF655339:ERF655369 FBB655339:FBB655369 FKX655339:FKX655369 FUT655339:FUT655369 GEP655339:GEP655369 GOL655339:GOL655369 GYH655339:GYH655369 HID655339:HID655369 HRZ655339:HRZ655369 IBV655339:IBV655369 ILR655339:ILR655369 IVN655339:IVN655369 JFJ655339:JFJ655369 JPF655339:JPF655369 JZB655339:JZB655369 KIX655339:KIX655369 KST655339:KST655369 LCP655339:LCP655369 LML655339:LML655369 LWH655339:LWH655369 MGD655339:MGD655369 MPZ655339:MPZ655369 MZV655339:MZV655369 NJR655339:NJR655369 NTN655339:NTN655369 ODJ655339:ODJ655369 ONF655339:ONF655369 OXB655339:OXB655369 PGX655339:PGX655369 PQT655339:PQT655369 QAP655339:QAP655369 QKL655339:QKL655369 QUH655339:QUH655369 RED655339:RED655369 RNZ655339:RNZ655369 RXV655339:RXV655369 SHR655339:SHR655369 SRN655339:SRN655369 TBJ655339:TBJ655369 TLF655339:TLF655369 TVB655339:TVB655369 UEX655339:UEX655369 UOT655339:UOT655369 UYP655339:UYP655369 VIL655339:VIL655369 VSH655339:VSH655369 WCD655339:WCD655369 WLZ655339:WLZ655369 WVV655339:WVV655369 R786411:S786441 JJ720875:JJ720905 TF720875:TF720905 ADB720875:ADB720905 AMX720875:AMX720905 AWT720875:AWT720905 BGP720875:BGP720905 BQL720875:BQL720905 CAH720875:CAH720905 CKD720875:CKD720905 CTZ720875:CTZ720905 DDV720875:DDV720905 DNR720875:DNR720905 DXN720875:DXN720905 EHJ720875:EHJ720905 ERF720875:ERF720905 FBB720875:FBB720905 FKX720875:FKX720905 FUT720875:FUT720905 GEP720875:GEP720905 GOL720875:GOL720905 GYH720875:GYH720905 HID720875:HID720905 HRZ720875:HRZ720905 IBV720875:IBV720905 ILR720875:ILR720905 IVN720875:IVN720905 JFJ720875:JFJ720905 JPF720875:JPF720905 JZB720875:JZB720905 KIX720875:KIX720905 KST720875:KST720905 LCP720875:LCP720905 LML720875:LML720905 LWH720875:LWH720905 MGD720875:MGD720905 MPZ720875:MPZ720905 MZV720875:MZV720905 NJR720875:NJR720905 NTN720875:NTN720905 ODJ720875:ODJ720905 ONF720875:ONF720905 OXB720875:OXB720905 PGX720875:PGX720905 PQT720875:PQT720905 QAP720875:QAP720905 QKL720875:QKL720905 QUH720875:QUH720905 RED720875:RED720905 RNZ720875:RNZ720905 RXV720875:RXV720905 SHR720875:SHR720905 SRN720875:SRN720905 TBJ720875:TBJ720905 TLF720875:TLF720905 TVB720875:TVB720905 UEX720875:UEX720905 UOT720875:UOT720905 UYP720875:UYP720905 VIL720875:VIL720905 VSH720875:VSH720905 WCD720875:WCD720905 WLZ720875:WLZ720905 WVV720875:WVV720905 R851947:S851977 JJ786411:JJ786441 TF786411:TF786441 ADB786411:ADB786441 AMX786411:AMX786441 AWT786411:AWT786441 BGP786411:BGP786441 BQL786411:BQL786441 CAH786411:CAH786441 CKD786411:CKD786441 CTZ786411:CTZ786441 DDV786411:DDV786441 DNR786411:DNR786441 DXN786411:DXN786441 EHJ786411:EHJ786441 ERF786411:ERF786441 FBB786411:FBB786441 FKX786411:FKX786441 FUT786411:FUT786441 GEP786411:GEP786441 GOL786411:GOL786441 GYH786411:GYH786441 HID786411:HID786441 HRZ786411:HRZ786441 IBV786411:IBV786441 ILR786411:ILR786441 IVN786411:IVN786441 JFJ786411:JFJ786441 JPF786411:JPF786441 JZB786411:JZB786441 KIX786411:KIX786441 KST786411:KST786441 LCP786411:LCP786441 LML786411:LML786441 LWH786411:LWH786441 MGD786411:MGD786441 MPZ786411:MPZ786441 MZV786411:MZV786441 NJR786411:NJR786441 NTN786411:NTN786441 ODJ786411:ODJ786441 ONF786411:ONF786441 OXB786411:OXB786441 PGX786411:PGX786441 PQT786411:PQT786441 QAP786411:QAP786441 QKL786411:QKL786441 QUH786411:QUH786441 RED786411:RED786441 RNZ786411:RNZ786441 RXV786411:RXV786441 SHR786411:SHR786441 SRN786411:SRN786441 TBJ786411:TBJ786441 TLF786411:TLF786441 TVB786411:TVB786441 UEX786411:UEX786441 UOT786411:UOT786441 UYP786411:UYP786441 VIL786411:VIL786441 VSH786411:VSH786441 WCD786411:WCD786441 WLZ786411:WLZ786441 WVV786411:WVV786441 R917483:S917513 JJ851947:JJ851977 TF851947:TF851977 ADB851947:ADB851977 AMX851947:AMX851977 AWT851947:AWT851977 BGP851947:BGP851977 BQL851947:BQL851977 CAH851947:CAH851977 CKD851947:CKD851977 CTZ851947:CTZ851977 DDV851947:DDV851977 DNR851947:DNR851977 DXN851947:DXN851977 EHJ851947:EHJ851977 ERF851947:ERF851977 FBB851947:FBB851977 FKX851947:FKX851977 FUT851947:FUT851977 GEP851947:GEP851977 GOL851947:GOL851977 GYH851947:GYH851977 HID851947:HID851977 HRZ851947:HRZ851977 IBV851947:IBV851977 ILR851947:ILR851977 IVN851947:IVN851977 JFJ851947:JFJ851977 JPF851947:JPF851977 JZB851947:JZB851977 KIX851947:KIX851977 KST851947:KST851977 LCP851947:LCP851977 LML851947:LML851977 LWH851947:LWH851977 MGD851947:MGD851977 MPZ851947:MPZ851977 MZV851947:MZV851977 NJR851947:NJR851977 NTN851947:NTN851977 ODJ851947:ODJ851977 ONF851947:ONF851977 OXB851947:OXB851977 PGX851947:PGX851977 PQT851947:PQT851977 QAP851947:QAP851977 QKL851947:QKL851977 QUH851947:QUH851977 RED851947:RED851977 RNZ851947:RNZ851977 RXV851947:RXV851977 SHR851947:SHR851977 SRN851947:SRN851977 TBJ851947:TBJ851977 TLF851947:TLF851977 TVB851947:TVB851977 UEX851947:UEX851977 UOT851947:UOT851977 UYP851947:UYP851977 VIL851947:VIL851977 VSH851947:VSH851977 WCD851947:WCD851977 WLZ851947:WLZ851977 WVV851947:WVV851977 R983019:S983049 JJ917483:JJ917513 TF917483:TF917513 ADB917483:ADB917513 AMX917483:AMX917513 AWT917483:AWT917513 BGP917483:BGP917513 BQL917483:BQL917513 CAH917483:CAH917513 CKD917483:CKD917513 CTZ917483:CTZ917513 DDV917483:DDV917513 DNR917483:DNR917513 DXN917483:DXN917513 EHJ917483:EHJ917513 ERF917483:ERF917513 FBB917483:FBB917513 FKX917483:FKX917513 FUT917483:FUT917513 GEP917483:GEP917513 GOL917483:GOL917513 GYH917483:GYH917513 HID917483:HID917513 HRZ917483:HRZ917513 IBV917483:IBV917513 ILR917483:ILR917513 IVN917483:IVN917513 JFJ917483:JFJ917513 JPF917483:JPF917513 JZB917483:JZB917513 KIX917483:KIX917513 KST917483:KST917513 LCP917483:LCP917513 LML917483:LML917513 LWH917483:LWH917513 MGD917483:MGD917513 MPZ917483:MPZ917513 MZV917483:MZV917513 NJR917483:NJR917513 NTN917483:NTN917513 ODJ917483:ODJ917513 ONF917483:ONF917513 OXB917483:OXB917513 PGX917483:PGX917513 PQT917483:PQT917513 QAP917483:QAP917513 QKL917483:QKL917513 QUH917483:QUH917513 RED917483:RED917513 RNZ917483:RNZ917513 RXV917483:RXV917513 SHR917483:SHR917513 SRN917483:SRN917513 TBJ917483:TBJ917513 TLF917483:TLF917513 TVB917483:TVB917513 UEX917483:UEX917513 UOT917483:UOT917513 UYP917483:UYP917513 VIL917483:VIL917513 VSH917483:VSH917513 WCD917483:WCD917513 WLZ917483:WLZ917513 WVV917483:WVV917513 WVV983019:WVV983049 JJ983019:JJ983049 TF983019:TF983049 ADB983019:ADB983049 AMX983019:AMX983049 AWT983019:AWT983049 BGP983019:BGP983049 BQL983019:BQL983049 CAH983019:CAH983049 CKD983019:CKD983049 CTZ983019:CTZ983049 DDV983019:DDV983049 DNR983019:DNR983049 DXN983019:DXN983049 EHJ983019:EHJ983049 ERF983019:ERF983049 FBB983019:FBB983049 FKX983019:FKX983049 FUT983019:FUT983049 GEP983019:GEP983049 GOL983019:GOL983049 GYH983019:GYH983049 HID983019:HID983049 HRZ983019:HRZ983049 IBV983019:IBV983049 ILR983019:ILR983049 IVN983019:IVN983049 JFJ983019:JFJ983049 JPF983019:JPF983049 JZB983019:JZB983049 KIX983019:KIX983049 KST983019:KST983049 LCP983019:LCP983049 LML983019:LML983049 LWH983019:LWH983049 MGD983019:MGD983049 MPZ983019:MPZ983049 MZV983019:MZV983049 NJR983019:NJR983049 NTN983019:NTN983049 ODJ983019:ODJ983049 ONF983019:ONF983049 OXB983019:OXB983049 PGX983019:PGX983049 PQT983019:PQT983049 QAP983019:QAP983049 QKL983019:QKL983049 QUH983019:QUH983049 RED983019:RED983049 RNZ983019:RNZ983049 RXV983019:RXV983049 SHR983019:SHR983049 SRN983019:SRN983049 TBJ983019:TBJ983049 TLF983019:TLF983049 TVB983019:TVB983049 UEX983019:UEX983049 UOT983019:UOT983049 UYP983019:UYP983049 VIL983019:VIL983049 VSH983019:VSH983049 WCD983019:WCD983049 WLZ983019:WLZ983049 R5:R6 WVV4:WVV20 JJ4:JJ20 TF4:TF20 ADB4:ADB20 AMX4:AMX20 AWT4:AWT20 BGP4:BGP20 BQL4:BQL20 CAH4:CAH20 CKD4:CKD20 CTZ4:CTZ20 DDV4:DDV20 DNR4:DNR20 DXN4:DXN20 EHJ4:EHJ20 ERF4:ERF20 FBB4:FBB20 FKX4:FKX20 FUT4:FUT20 GEP4:GEP20 GOL4:GOL20 GYH4:GYH20 HID4:HID20 HRZ4:HRZ20 IBV4:IBV20 ILR4:ILR20 IVN4:IVN20 JFJ4:JFJ20 JPF4:JPF20 JZB4:JZB20 KIX4:KIX20 KST4:KST20 LCP4:LCP20 LML4:LML20 LWH4:LWH20 MGD4:MGD20 MPZ4:MPZ20 MZV4:MZV20 NJR4:NJR20 NTN4:NTN20 ODJ4:ODJ20 ONF4:ONF20 OXB4:OXB20 PGX4:PGX20 PQT4:PQT20 QAP4:QAP20 QKL4:QKL20 QUH4:QUH20 RED4:RED20 RNZ4:RNZ20 RXV4:RXV20 SHR4:SHR20 SRN4:SRN20 TBJ4:TBJ20 TLF4:TLF20 TVB4:TVB20 UEX4:UEX20 UOT4:UOT20 UYP4:UYP20 VIL4:VIL20 VSH4:VSH20 WCD4:WCD20 WLZ4:WLZ20 R8:R20" xr:uid="{00000000-0002-0000-0200-000010000000}">
       <formula1>"Soltero,Casado,Unión Libre,Separado,Viudo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JF65515:JF65545 TB65515:TB65545 ACX65515:ACX65545 AMT65515:AMT65545 AWP65515:AWP65545 BGL65515:BGL65545 BQH65515:BQH65545 CAD65515:CAD65545 CJZ65515:CJZ65545 CTV65515:CTV65545 DDR65515:DDR65545 DNN65515:DNN65545 DXJ65515:DXJ65545 EHF65515:EHF65545 ERB65515:ERB65545 FAX65515:FAX65545 FKT65515:FKT65545 FUP65515:FUP65545 GEL65515:GEL65545 GOH65515:GOH65545 GYD65515:GYD65545 HHZ65515:HHZ65545 HRV65515:HRV65545 IBR65515:IBR65545 ILN65515:ILN65545 IVJ65515:IVJ65545 JFF65515:JFF65545 JPB65515:JPB65545 JYX65515:JYX65545 KIT65515:KIT65545 KSP65515:KSP65545 LCL65515:LCL65545 LMH65515:LMH65545 LWD65515:LWD65545 MFZ65515:MFZ65545 MPV65515:MPV65545 MZR65515:MZR65545 NJN65515:NJN65545 NTJ65515:NTJ65545 ODF65515:ODF65545 ONB65515:ONB65545 OWX65515:OWX65545 PGT65515:PGT65545 PQP65515:PQP65545 QAL65515:QAL65545 QKH65515:QKH65545 QUD65515:QUD65545 RDZ65515:RDZ65545 RNV65515:RNV65545 RXR65515:RXR65545 SHN65515:SHN65545 SRJ65515:SRJ65545 TBF65515:TBF65545 TLB65515:TLB65545 TUX65515:TUX65545 UET65515:UET65545 UOP65515:UOP65545 UYL65515:UYL65545 VIH65515:VIH65545 VSD65515:VSD65545 WBZ65515:WBZ65545 WLV65515:WLV65545 WVR65515:WVR65545 JF131051:JF131081 TB131051:TB131081 ACX131051:ACX131081 AMT131051:AMT131081 AWP131051:AWP131081 BGL131051:BGL131081 BQH131051:BQH131081 CAD131051:CAD131081 CJZ131051:CJZ131081 CTV131051:CTV131081 DDR131051:DDR131081 DNN131051:DNN131081 DXJ131051:DXJ131081 EHF131051:EHF131081 ERB131051:ERB131081 FAX131051:FAX131081 FKT131051:FKT131081 FUP131051:FUP131081 GEL131051:GEL131081 GOH131051:GOH131081 GYD131051:GYD131081 HHZ131051:HHZ131081 HRV131051:HRV131081 IBR131051:IBR131081 ILN131051:ILN131081 IVJ131051:IVJ131081 JFF131051:JFF131081 JPB131051:JPB131081 JYX131051:JYX131081 KIT131051:KIT131081 KSP131051:KSP131081 LCL131051:LCL131081 LMH131051:LMH131081 LWD131051:LWD131081 MFZ131051:MFZ131081 MPV131051:MPV131081 MZR131051:MZR131081 NJN131051:NJN131081 NTJ131051:NTJ131081 ODF131051:ODF131081 ONB131051:ONB131081 OWX131051:OWX131081 PGT131051:PGT131081 PQP131051:PQP131081 QAL131051:QAL131081 QKH131051:QKH131081 QUD131051:QUD131081 RDZ131051:RDZ131081 RNV131051:RNV131081 RXR131051:RXR131081 SHN131051:SHN131081 SRJ131051:SRJ131081 TBF131051:TBF131081 TLB131051:TLB131081 TUX131051:TUX131081 UET131051:UET131081 UOP131051:UOP131081 UYL131051:UYL131081 VIH131051:VIH131081 VSD131051:VSD131081 WBZ131051:WBZ131081 WLV131051:WLV131081 WVR131051:WVR131081 JF196587:JF196617 TB196587:TB196617 ACX196587:ACX196617 AMT196587:AMT196617 AWP196587:AWP196617 BGL196587:BGL196617 BQH196587:BQH196617 CAD196587:CAD196617 CJZ196587:CJZ196617 CTV196587:CTV196617 DDR196587:DDR196617 DNN196587:DNN196617 DXJ196587:DXJ196617 EHF196587:EHF196617 ERB196587:ERB196617 FAX196587:FAX196617 FKT196587:FKT196617 FUP196587:FUP196617 GEL196587:GEL196617 GOH196587:GOH196617 GYD196587:GYD196617 HHZ196587:HHZ196617 HRV196587:HRV196617 IBR196587:IBR196617 ILN196587:ILN196617 IVJ196587:IVJ196617 JFF196587:JFF196617 JPB196587:JPB196617 JYX196587:JYX196617 KIT196587:KIT196617 KSP196587:KSP196617 LCL196587:LCL196617 LMH196587:LMH196617 LWD196587:LWD196617 MFZ196587:MFZ196617 MPV196587:MPV196617 MZR196587:MZR196617 NJN196587:NJN196617 NTJ196587:NTJ196617 ODF196587:ODF196617 ONB196587:ONB196617 OWX196587:OWX196617 PGT196587:PGT196617 PQP196587:PQP196617 QAL196587:QAL196617 QKH196587:QKH196617 QUD196587:QUD196617 RDZ196587:RDZ196617 RNV196587:RNV196617 RXR196587:RXR196617 SHN196587:SHN196617 SRJ196587:SRJ196617 TBF196587:TBF196617 TLB196587:TLB196617 TUX196587:TUX196617 UET196587:UET196617 UOP196587:UOP196617 UYL196587:UYL196617 VIH196587:VIH196617 VSD196587:VSD196617 WBZ196587:WBZ196617 WLV196587:WLV196617 WVR196587:WVR196617 JF262123:JF262153 TB262123:TB262153 ACX262123:ACX262153 AMT262123:AMT262153 AWP262123:AWP262153 BGL262123:BGL262153 BQH262123:BQH262153 CAD262123:CAD262153 CJZ262123:CJZ262153 CTV262123:CTV262153 DDR262123:DDR262153 DNN262123:DNN262153 DXJ262123:DXJ262153 EHF262123:EHF262153 ERB262123:ERB262153 FAX262123:FAX262153 FKT262123:FKT262153 FUP262123:FUP262153 GEL262123:GEL262153 GOH262123:GOH262153 GYD262123:GYD262153 HHZ262123:HHZ262153 HRV262123:HRV262153 IBR262123:IBR262153 ILN262123:ILN262153 IVJ262123:IVJ262153 JFF262123:JFF262153 JPB262123:JPB262153 JYX262123:JYX262153 KIT262123:KIT262153 KSP262123:KSP262153 LCL262123:LCL262153 LMH262123:LMH262153 LWD262123:LWD262153 MFZ262123:MFZ262153 MPV262123:MPV262153 MZR262123:MZR262153 NJN262123:NJN262153 NTJ262123:NTJ262153 ODF262123:ODF262153 ONB262123:ONB262153 OWX262123:OWX262153 PGT262123:PGT262153 PQP262123:PQP262153 QAL262123:QAL262153 QKH262123:QKH262153 QUD262123:QUD262153 RDZ262123:RDZ262153 RNV262123:RNV262153 RXR262123:RXR262153 SHN262123:SHN262153 SRJ262123:SRJ262153 TBF262123:TBF262153 TLB262123:TLB262153 TUX262123:TUX262153 UET262123:UET262153 UOP262123:UOP262153 UYL262123:UYL262153 VIH262123:VIH262153 VSD262123:VSD262153 WBZ262123:WBZ262153 WLV262123:WLV262153 WVR262123:WVR262153 JF327659:JF327689 TB327659:TB327689 ACX327659:ACX327689 AMT327659:AMT327689 AWP327659:AWP327689 BGL327659:BGL327689 BQH327659:BQH327689 CAD327659:CAD327689 CJZ327659:CJZ327689 CTV327659:CTV327689 DDR327659:DDR327689 DNN327659:DNN327689 DXJ327659:DXJ327689 EHF327659:EHF327689 ERB327659:ERB327689 FAX327659:FAX327689 FKT327659:FKT327689 FUP327659:FUP327689 GEL327659:GEL327689 GOH327659:GOH327689 GYD327659:GYD327689 HHZ327659:HHZ327689 HRV327659:HRV327689 IBR327659:IBR327689 ILN327659:ILN327689 IVJ327659:IVJ327689 JFF327659:JFF327689 JPB327659:JPB327689 JYX327659:JYX327689 KIT327659:KIT327689 KSP327659:KSP327689 LCL327659:LCL327689 LMH327659:LMH327689 LWD327659:LWD327689 MFZ327659:MFZ327689 MPV327659:MPV327689 MZR327659:MZR327689 NJN327659:NJN327689 NTJ327659:NTJ327689 ODF327659:ODF327689 ONB327659:ONB327689 OWX327659:OWX327689 PGT327659:PGT327689 PQP327659:PQP327689 QAL327659:QAL327689 QKH327659:QKH327689 QUD327659:QUD327689 RDZ327659:RDZ327689 RNV327659:RNV327689 RXR327659:RXR327689 SHN327659:SHN327689 SRJ327659:SRJ327689 TBF327659:TBF327689 TLB327659:TLB327689 TUX327659:TUX327689 UET327659:UET327689 UOP327659:UOP327689 UYL327659:UYL327689 VIH327659:VIH327689 VSD327659:VSD327689 WBZ327659:WBZ327689 WLV327659:WLV327689 WVR327659:WVR327689 JF393195:JF393225 TB393195:TB393225 ACX393195:ACX393225 AMT393195:AMT393225 AWP393195:AWP393225 BGL393195:BGL393225 BQH393195:BQH393225 CAD393195:CAD393225 CJZ393195:CJZ393225 CTV393195:CTV393225 DDR393195:DDR393225 DNN393195:DNN393225 DXJ393195:DXJ393225 EHF393195:EHF393225 ERB393195:ERB393225 FAX393195:FAX393225 FKT393195:FKT393225 FUP393195:FUP393225 GEL393195:GEL393225 GOH393195:GOH393225 GYD393195:GYD393225 HHZ393195:HHZ393225 HRV393195:HRV393225 IBR393195:IBR393225 ILN393195:ILN393225 IVJ393195:IVJ393225 JFF393195:JFF393225 JPB393195:JPB393225 JYX393195:JYX393225 KIT393195:KIT393225 KSP393195:KSP393225 LCL393195:LCL393225 LMH393195:LMH393225 LWD393195:LWD393225 MFZ393195:MFZ393225 MPV393195:MPV393225 MZR393195:MZR393225 NJN393195:NJN393225 NTJ393195:NTJ393225 ODF393195:ODF393225 ONB393195:ONB393225 OWX393195:OWX393225 PGT393195:PGT393225 PQP393195:PQP393225 QAL393195:QAL393225 QKH393195:QKH393225 QUD393195:QUD393225 RDZ393195:RDZ393225 RNV393195:RNV393225 RXR393195:RXR393225 SHN393195:SHN393225 SRJ393195:SRJ393225 TBF393195:TBF393225 TLB393195:TLB393225 TUX393195:TUX393225 UET393195:UET393225 UOP393195:UOP393225 UYL393195:UYL393225 VIH393195:VIH393225 VSD393195:VSD393225 WBZ393195:WBZ393225 WLV393195:WLV393225 WVR393195:WVR393225 JF458731:JF458761 TB458731:TB458761 ACX458731:ACX458761 AMT458731:AMT458761 AWP458731:AWP458761 BGL458731:BGL458761 BQH458731:BQH458761 CAD458731:CAD458761 CJZ458731:CJZ458761 CTV458731:CTV458761 DDR458731:DDR458761 DNN458731:DNN458761 DXJ458731:DXJ458761 EHF458731:EHF458761 ERB458731:ERB458761 FAX458731:FAX458761 FKT458731:FKT458761 FUP458731:FUP458761 GEL458731:GEL458761 GOH458731:GOH458761 GYD458731:GYD458761 HHZ458731:HHZ458761 HRV458731:HRV458761 IBR458731:IBR458761 ILN458731:ILN458761 IVJ458731:IVJ458761 JFF458731:JFF458761 JPB458731:JPB458761 JYX458731:JYX458761 KIT458731:KIT458761 KSP458731:KSP458761 LCL458731:LCL458761 LMH458731:LMH458761 LWD458731:LWD458761 MFZ458731:MFZ458761 MPV458731:MPV458761 MZR458731:MZR458761 NJN458731:NJN458761 NTJ458731:NTJ458761 ODF458731:ODF458761 ONB458731:ONB458761 OWX458731:OWX458761 PGT458731:PGT458761 PQP458731:PQP458761 QAL458731:QAL458761 QKH458731:QKH458761 QUD458731:QUD458761 RDZ458731:RDZ458761 RNV458731:RNV458761 RXR458731:RXR458761 SHN458731:SHN458761 SRJ458731:SRJ458761 TBF458731:TBF458761 TLB458731:TLB458761 TUX458731:TUX458761 UET458731:UET458761 UOP458731:UOP458761 UYL458731:UYL458761 VIH458731:VIH458761 VSD458731:VSD458761 WBZ458731:WBZ458761 WLV458731:WLV458761 WVR458731:WVR458761 JF524267:JF524297 TB524267:TB524297 ACX524267:ACX524297 AMT524267:AMT524297 AWP524267:AWP524297 BGL524267:BGL524297 BQH524267:BQH524297 CAD524267:CAD524297 CJZ524267:CJZ524297 CTV524267:CTV524297 DDR524267:DDR524297 DNN524267:DNN524297 DXJ524267:DXJ524297 EHF524267:EHF524297 ERB524267:ERB524297 FAX524267:FAX524297 FKT524267:FKT524297 FUP524267:FUP524297 GEL524267:GEL524297 GOH524267:GOH524297 GYD524267:GYD524297 HHZ524267:HHZ524297 HRV524267:HRV524297 IBR524267:IBR524297 ILN524267:ILN524297 IVJ524267:IVJ524297 JFF524267:JFF524297 JPB524267:JPB524297 JYX524267:JYX524297 KIT524267:KIT524297 KSP524267:KSP524297 LCL524267:LCL524297 LMH524267:LMH524297 LWD524267:LWD524297 MFZ524267:MFZ524297 MPV524267:MPV524297 MZR524267:MZR524297 NJN524267:NJN524297 NTJ524267:NTJ524297 ODF524267:ODF524297 ONB524267:ONB524297 OWX524267:OWX524297 PGT524267:PGT524297 PQP524267:PQP524297 QAL524267:QAL524297 QKH524267:QKH524297 QUD524267:QUD524297 RDZ524267:RDZ524297 RNV524267:RNV524297 RXR524267:RXR524297 SHN524267:SHN524297 SRJ524267:SRJ524297 TBF524267:TBF524297 TLB524267:TLB524297 TUX524267:TUX524297 UET524267:UET524297 UOP524267:UOP524297 UYL524267:UYL524297 VIH524267:VIH524297 VSD524267:VSD524297 WBZ524267:WBZ524297 WLV524267:WLV524297 WVR524267:WVR524297 JF589803:JF589833 TB589803:TB589833 ACX589803:ACX589833 AMT589803:AMT589833 AWP589803:AWP589833 BGL589803:BGL589833 BQH589803:BQH589833 CAD589803:CAD589833 CJZ589803:CJZ589833 CTV589803:CTV589833 DDR589803:DDR589833 DNN589803:DNN589833 DXJ589803:DXJ589833 EHF589803:EHF589833 ERB589803:ERB589833 FAX589803:FAX589833 FKT589803:FKT589833 FUP589803:FUP589833 GEL589803:GEL589833 GOH589803:GOH589833 GYD589803:GYD589833 HHZ589803:HHZ589833 HRV589803:HRV589833 IBR589803:IBR589833 ILN589803:ILN589833 IVJ589803:IVJ589833 JFF589803:JFF589833 JPB589803:JPB589833 JYX589803:JYX589833 KIT589803:KIT589833 KSP589803:KSP589833 LCL589803:LCL589833 LMH589803:LMH589833 LWD589803:LWD589833 MFZ589803:MFZ589833 MPV589803:MPV589833 MZR589803:MZR589833 NJN589803:NJN589833 NTJ589803:NTJ589833 ODF589803:ODF589833 ONB589803:ONB589833 OWX589803:OWX589833 PGT589803:PGT589833 PQP589803:PQP589833 QAL589803:QAL589833 QKH589803:QKH589833 QUD589803:QUD589833 RDZ589803:RDZ589833 RNV589803:RNV589833 RXR589803:RXR589833 SHN589803:SHN589833 SRJ589803:SRJ589833 TBF589803:TBF589833 TLB589803:TLB589833 TUX589803:TUX589833 UET589803:UET589833 UOP589803:UOP589833 UYL589803:UYL589833 VIH589803:VIH589833 VSD589803:VSD589833 WBZ589803:WBZ589833 WLV589803:WLV589833 WVR589803:WVR589833 JF655339:JF655369 TB655339:TB655369 ACX655339:ACX655369 AMT655339:AMT655369 AWP655339:AWP655369 BGL655339:BGL655369 BQH655339:BQH655369 CAD655339:CAD655369 CJZ655339:CJZ655369 CTV655339:CTV655369 DDR655339:DDR655369 DNN655339:DNN655369 DXJ655339:DXJ655369 EHF655339:EHF655369 ERB655339:ERB655369 FAX655339:FAX655369 FKT655339:FKT655369 FUP655339:FUP655369 GEL655339:GEL655369 GOH655339:GOH655369 GYD655339:GYD655369 HHZ655339:HHZ655369 HRV655339:HRV655369 IBR655339:IBR655369 ILN655339:ILN655369 IVJ655339:IVJ655369 JFF655339:JFF655369 JPB655339:JPB655369 JYX655339:JYX655369 KIT655339:KIT655369 KSP655339:KSP655369 LCL655339:LCL655369 LMH655339:LMH655369 LWD655339:LWD655369 MFZ655339:MFZ655369 MPV655339:MPV655369 MZR655339:MZR655369 NJN655339:NJN655369 NTJ655339:NTJ655369 ODF655339:ODF655369 ONB655339:ONB655369 OWX655339:OWX655369 PGT655339:PGT655369 PQP655339:PQP655369 QAL655339:QAL655369 QKH655339:QKH655369 QUD655339:QUD655369 RDZ655339:RDZ655369 RNV655339:RNV655369 RXR655339:RXR655369 SHN655339:SHN655369 SRJ655339:SRJ655369 TBF655339:TBF655369 TLB655339:TLB655369 TUX655339:TUX655369 UET655339:UET655369 UOP655339:UOP655369 UYL655339:UYL655369 VIH655339:VIH655369 VSD655339:VSD655369 WBZ655339:WBZ655369 WLV655339:WLV655369 WVR655339:WVR655369 JF720875:JF720905 TB720875:TB720905 ACX720875:ACX720905 AMT720875:AMT720905 AWP720875:AWP720905 BGL720875:BGL720905 BQH720875:BQH720905 CAD720875:CAD720905 CJZ720875:CJZ720905 CTV720875:CTV720905 DDR720875:DDR720905 DNN720875:DNN720905 DXJ720875:DXJ720905 EHF720875:EHF720905 ERB720875:ERB720905 FAX720875:FAX720905 FKT720875:FKT720905 FUP720875:FUP720905 GEL720875:GEL720905 GOH720875:GOH720905 GYD720875:GYD720905 HHZ720875:HHZ720905 HRV720875:HRV720905 IBR720875:IBR720905 ILN720875:ILN720905 IVJ720875:IVJ720905 JFF720875:JFF720905 JPB720875:JPB720905 JYX720875:JYX720905 KIT720875:KIT720905 KSP720875:KSP720905 LCL720875:LCL720905 LMH720875:LMH720905 LWD720875:LWD720905 MFZ720875:MFZ720905 MPV720875:MPV720905 MZR720875:MZR720905 NJN720875:NJN720905 NTJ720875:NTJ720905 ODF720875:ODF720905 ONB720875:ONB720905 OWX720875:OWX720905 PGT720875:PGT720905 PQP720875:PQP720905 QAL720875:QAL720905 QKH720875:QKH720905 QUD720875:QUD720905 RDZ720875:RDZ720905 RNV720875:RNV720905 RXR720875:RXR720905 SHN720875:SHN720905 SRJ720875:SRJ720905 TBF720875:TBF720905 TLB720875:TLB720905 TUX720875:TUX720905 UET720875:UET720905 UOP720875:UOP720905 UYL720875:UYL720905 VIH720875:VIH720905 VSD720875:VSD720905 WBZ720875:WBZ720905 WLV720875:WLV720905 WVR720875:WVR720905 JF786411:JF786441 TB786411:TB786441 ACX786411:ACX786441 AMT786411:AMT786441 AWP786411:AWP786441 BGL786411:BGL786441 BQH786411:BQH786441 CAD786411:CAD786441 CJZ786411:CJZ786441 CTV786411:CTV786441 DDR786411:DDR786441 DNN786411:DNN786441 DXJ786411:DXJ786441 EHF786411:EHF786441 ERB786411:ERB786441 FAX786411:FAX786441 FKT786411:FKT786441 FUP786411:FUP786441 GEL786411:GEL786441 GOH786411:GOH786441 GYD786411:GYD786441 HHZ786411:HHZ786441 HRV786411:HRV786441 IBR786411:IBR786441 ILN786411:ILN786441 IVJ786411:IVJ786441 JFF786411:JFF786441 JPB786411:JPB786441 JYX786411:JYX786441 KIT786411:KIT786441 KSP786411:KSP786441 LCL786411:LCL786441 LMH786411:LMH786441 LWD786411:LWD786441 MFZ786411:MFZ786441 MPV786411:MPV786441 MZR786411:MZR786441 NJN786411:NJN786441 NTJ786411:NTJ786441 ODF786411:ODF786441 ONB786411:ONB786441 OWX786411:OWX786441 PGT786411:PGT786441 PQP786411:PQP786441 QAL786411:QAL786441 QKH786411:QKH786441 QUD786411:QUD786441 RDZ786411:RDZ786441 RNV786411:RNV786441 RXR786411:RXR786441 SHN786411:SHN786441 SRJ786411:SRJ786441 TBF786411:TBF786441 TLB786411:TLB786441 TUX786411:TUX786441 UET786411:UET786441 UOP786411:UOP786441 UYL786411:UYL786441 VIH786411:VIH786441 VSD786411:VSD786441 WBZ786411:WBZ786441 WLV786411:WLV786441 WVR786411:WVR786441 JF851947:JF851977 TB851947:TB851977 ACX851947:ACX851977 AMT851947:AMT851977 AWP851947:AWP851977 BGL851947:BGL851977 BQH851947:BQH851977 CAD851947:CAD851977 CJZ851947:CJZ851977 CTV851947:CTV851977 DDR851947:DDR851977 DNN851947:DNN851977 DXJ851947:DXJ851977 EHF851947:EHF851977 ERB851947:ERB851977 FAX851947:FAX851977 FKT851947:FKT851977 FUP851947:FUP851977 GEL851947:GEL851977 GOH851947:GOH851977 GYD851947:GYD851977 HHZ851947:HHZ851977 HRV851947:HRV851977 IBR851947:IBR851977 ILN851947:ILN851977 IVJ851947:IVJ851977 JFF851947:JFF851977 JPB851947:JPB851977 JYX851947:JYX851977 KIT851947:KIT851977 KSP851947:KSP851977 LCL851947:LCL851977 LMH851947:LMH851977 LWD851947:LWD851977 MFZ851947:MFZ851977 MPV851947:MPV851977 MZR851947:MZR851977 NJN851947:NJN851977 NTJ851947:NTJ851977 ODF851947:ODF851977 ONB851947:ONB851977 OWX851947:OWX851977 PGT851947:PGT851977 PQP851947:PQP851977 QAL851947:QAL851977 QKH851947:QKH851977 QUD851947:QUD851977 RDZ851947:RDZ851977 RNV851947:RNV851977 RXR851947:RXR851977 SHN851947:SHN851977 SRJ851947:SRJ851977 TBF851947:TBF851977 TLB851947:TLB851977 TUX851947:TUX851977 UET851947:UET851977 UOP851947:UOP851977 UYL851947:UYL851977 VIH851947:VIH851977 VSD851947:VSD851977 WBZ851947:WBZ851977 WLV851947:WLV851977 WVR851947:WVR851977 JF917483:JF917513 TB917483:TB917513 ACX917483:ACX917513 AMT917483:AMT917513 AWP917483:AWP917513 BGL917483:BGL917513 BQH917483:BQH917513 CAD917483:CAD917513 CJZ917483:CJZ917513 CTV917483:CTV917513 DDR917483:DDR917513 DNN917483:DNN917513 DXJ917483:DXJ917513 EHF917483:EHF917513 ERB917483:ERB917513 FAX917483:FAX917513 FKT917483:FKT917513 FUP917483:FUP917513 GEL917483:GEL917513 GOH917483:GOH917513 GYD917483:GYD917513 HHZ917483:HHZ917513 HRV917483:HRV917513 IBR917483:IBR917513 ILN917483:ILN917513 IVJ917483:IVJ917513 JFF917483:JFF917513 JPB917483:JPB917513 JYX917483:JYX917513 KIT917483:KIT917513 KSP917483:KSP917513 LCL917483:LCL917513 LMH917483:LMH917513 LWD917483:LWD917513 MFZ917483:MFZ917513 MPV917483:MPV917513 MZR917483:MZR917513 NJN917483:NJN917513 NTJ917483:NTJ917513 ODF917483:ODF917513 ONB917483:ONB917513 OWX917483:OWX917513 PGT917483:PGT917513 PQP917483:PQP917513 QAL917483:QAL917513 QKH917483:QKH917513 QUD917483:QUD917513 RDZ917483:RDZ917513 RNV917483:RNV917513 RXR917483:RXR917513 SHN917483:SHN917513 SRJ917483:SRJ917513 TBF917483:TBF917513 TLB917483:TLB917513 TUX917483:TUX917513 UET917483:UET917513 UOP917483:UOP917513 UYL917483:UYL917513 VIH917483:VIH917513 VSD917483:VSD917513 WBZ917483:WBZ917513 WLV917483:WLV917513 WVR917483:WVR917513 JF983019:JF983049 TB983019:TB983049 ACX983019:ACX983049 AMT983019:AMT983049 AWP983019:AWP983049 BGL983019:BGL983049 BQH983019:BQH983049 CAD983019:CAD983049 CJZ983019:CJZ983049 CTV983019:CTV983049 DDR983019:DDR983049 DNN983019:DNN983049 DXJ983019:DXJ983049 EHF983019:EHF983049 ERB983019:ERB983049 FAX983019:FAX983049 FKT983019:FKT983049 FUP983019:FUP983049 GEL983019:GEL983049 GOH983019:GOH983049 GYD983019:GYD983049 HHZ983019:HHZ983049 HRV983019:HRV983049 IBR983019:IBR983049 ILN983019:ILN983049 IVJ983019:IVJ983049 JFF983019:JFF983049 JPB983019:JPB983049 JYX983019:JYX983049 KIT983019:KIT983049 KSP983019:KSP983049 LCL983019:LCL983049 LMH983019:LMH983049 LWD983019:LWD983049 MFZ983019:MFZ983049 MPV983019:MPV983049 MZR983019:MZR983049 NJN983019:NJN983049 NTJ983019:NTJ983049 ODF983019:ODF983049 ONB983019:ONB983049 OWX983019:OWX983049 PGT983019:PGT983049 PQP983019:PQP983049 QAL983019:QAL983049 QKH983019:QKH983049 QUD983019:QUD983049 RDZ983019:RDZ983049 RNV983019:RNV983049 RXR983019:RXR983049 SHN983019:SHN983049 SRJ983019:SRJ983049 TBF983019:TBF983049 TLB983019:TLB983049 TUX983019:TUX983049 UET983019:UET983049 UOP983019:UOP983049 UYL983019:UYL983049 VIH983019:VIH983049 VSD983019:VSD983049 WBZ983019:WBZ983049 WLV983019:WLV983049 WVR983019:WVR983049 G65515:H65545 G131051:H131081 G196587:H196617 G262123:H262153 G327659:H327689 G393195:H393225 G458731:H458761 G524267:H524297 G589803:H589833 G655339:H655369 G720875:H720905 G786411:H786441 G851947:H851977 G917483:H917513 G983019:H983049 WVR4:WVR20 WLV4:WLV20 WBZ4:WBZ20 VSD4:VSD20 VIH4:VIH20 UYL4:UYL20 UOP4:UOP20 UET4:UET20 TUX4:TUX20 TLB4:TLB20 TBF4:TBF20 SRJ4:SRJ20 SHN4:SHN20 RXR4:RXR20 RNV4:RNV20 RDZ4:RDZ20 QUD4:QUD20 QKH4:QKH20 QAL4:QAL20 PQP4:PQP20 PGT4:PGT20 OWX4:OWX20 ONB4:ONB20 ODF4:ODF20 NTJ4:NTJ20 NJN4:NJN20 MZR4:MZR20 MPV4:MPV20 MFZ4:MFZ20 LWD4:LWD20 LMH4:LMH20 LCL4:LCL20 KSP4:KSP20 KIT4:KIT20 JYX4:JYX20 JPB4:JPB20 JFF4:JFF20 IVJ4:IVJ20 ILN4:ILN20 IBR4:IBR20 HRV4:HRV20 HHZ4:HHZ20 GYD4:GYD20 GOH4:GOH20 GEL4:GEL20 FUP4:FUP20 FKT4:FKT20 FAX4:FAX20 ERB4:ERB20 EHF4:EHF20 DXJ4:DXJ20 DNN4:DNN20 DDR4:DDR20 CTV4:CTV20 CJZ4:CJZ20 CAD4:CAD20 BQH4:BQH20 BGL4:BGL20 AWP4:AWP20 AMT4:AMT20 ACX4:ACX20 TB4:TB20 JF4:JF20" xr:uid="{00000000-0002-0000-0200-000011000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JF65515:JF65545 TB65515:TB65545 ACX65515:ACX65545 AMT65515:AMT65545 AWP65515:AWP65545 BGL65515:BGL65545 BQH65515:BQH65545 CAD65515:CAD65545 CJZ65515:CJZ65545 CTV65515:CTV65545 DDR65515:DDR65545 DNN65515:DNN65545 DXJ65515:DXJ65545 EHF65515:EHF65545 ERB65515:ERB65545 FAX65515:FAX65545 FKT65515:FKT65545 FUP65515:FUP65545 GEL65515:GEL65545 GOH65515:GOH65545 GYD65515:GYD65545 HHZ65515:HHZ65545 HRV65515:HRV65545 IBR65515:IBR65545 ILN65515:ILN65545 IVJ65515:IVJ65545 JFF65515:JFF65545 JPB65515:JPB65545 JYX65515:JYX65545 KIT65515:KIT65545 KSP65515:KSP65545 LCL65515:LCL65545 LMH65515:LMH65545 LWD65515:LWD65545 MFZ65515:MFZ65545 MPV65515:MPV65545 MZR65515:MZR65545 NJN65515:NJN65545 NTJ65515:NTJ65545 ODF65515:ODF65545 ONB65515:ONB65545 OWX65515:OWX65545 PGT65515:PGT65545 PQP65515:PQP65545 QAL65515:QAL65545 QKH65515:QKH65545 QUD65515:QUD65545 RDZ65515:RDZ65545 RNV65515:RNV65545 RXR65515:RXR65545 SHN65515:SHN65545 SRJ65515:SRJ65545 TBF65515:TBF65545 TLB65515:TLB65545 TUX65515:TUX65545 UET65515:UET65545 UOP65515:UOP65545 UYL65515:UYL65545 VIH65515:VIH65545 VSD65515:VSD65545 WBZ65515:WBZ65545 WLV65515:WLV65545 WVR65515:WVR65545 JF131051:JF131081 TB131051:TB131081 ACX131051:ACX131081 AMT131051:AMT131081 AWP131051:AWP131081 BGL131051:BGL131081 BQH131051:BQH131081 CAD131051:CAD131081 CJZ131051:CJZ131081 CTV131051:CTV131081 DDR131051:DDR131081 DNN131051:DNN131081 DXJ131051:DXJ131081 EHF131051:EHF131081 ERB131051:ERB131081 FAX131051:FAX131081 FKT131051:FKT131081 FUP131051:FUP131081 GEL131051:GEL131081 GOH131051:GOH131081 GYD131051:GYD131081 HHZ131051:HHZ131081 HRV131051:HRV131081 IBR131051:IBR131081 ILN131051:ILN131081 IVJ131051:IVJ131081 JFF131051:JFF131081 JPB131051:JPB131081 JYX131051:JYX131081 KIT131051:KIT131081 KSP131051:KSP131081 LCL131051:LCL131081 LMH131051:LMH131081 LWD131051:LWD131081 MFZ131051:MFZ131081 MPV131051:MPV131081 MZR131051:MZR131081 NJN131051:NJN131081 NTJ131051:NTJ131081 ODF131051:ODF131081 ONB131051:ONB131081 OWX131051:OWX131081 PGT131051:PGT131081 PQP131051:PQP131081 QAL131051:QAL131081 QKH131051:QKH131081 QUD131051:QUD131081 RDZ131051:RDZ131081 RNV131051:RNV131081 RXR131051:RXR131081 SHN131051:SHN131081 SRJ131051:SRJ131081 TBF131051:TBF131081 TLB131051:TLB131081 TUX131051:TUX131081 UET131051:UET131081 UOP131051:UOP131081 UYL131051:UYL131081 VIH131051:VIH131081 VSD131051:VSD131081 WBZ131051:WBZ131081 WLV131051:WLV131081 WVR131051:WVR131081 JF196587:JF196617 TB196587:TB196617 ACX196587:ACX196617 AMT196587:AMT196617 AWP196587:AWP196617 BGL196587:BGL196617 BQH196587:BQH196617 CAD196587:CAD196617 CJZ196587:CJZ196617 CTV196587:CTV196617 DDR196587:DDR196617 DNN196587:DNN196617 DXJ196587:DXJ196617 EHF196587:EHF196617 ERB196587:ERB196617 FAX196587:FAX196617 FKT196587:FKT196617 FUP196587:FUP196617 GEL196587:GEL196617 GOH196587:GOH196617 GYD196587:GYD196617 HHZ196587:HHZ196617 HRV196587:HRV196617 IBR196587:IBR196617 ILN196587:ILN196617 IVJ196587:IVJ196617 JFF196587:JFF196617 JPB196587:JPB196617 JYX196587:JYX196617 KIT196587:KIT196617 KSP196587:KSP196617 LCL196587:LCL196617 LMH196587:LMH196617 LWD196587:LWD196617 MFZ196587:MFZ196617 MPV196587:MPV196617 MZR196587:MZR196617 NJN196587:NJN196617 NTJ196587:NTJ196617 ODF196587:ODF196617 ONB196587:ONB196617 OWX196587:OWX196617 PGT196587:PGT196617 PQP196587:PQP196617 QAL196587:QAL196617 QKH196587:QKH196617 QUD196587:QUD196617 RDZ196587:RDZ196617 RNV196587:RNV196617 RXR196587:RXR196617 SHN196587:SHN196617 SRJ196587:SRJ196617 TBF196587:TBF196617 TLB196587:TLB196617 TUX196587:TUX196617 UET196587:UET196617 UOP196587:UOP196617 UYL196587:UYL196617 VIH196587:VIH196617 VSD196587:VSD196617 WBZ196587:WBZ196617 WLV196587:WLV196617 WVR196587:WVR196617 JF262123:JF262153 TB262123:TB262153 ACX262123:ACX262153 AMT262123:AMT262153 AWP262123:AWP262153 BGL262123:BGL262153 BQH262123:BQH262153 CAD262123:CAD262153 CJZ262123:CJZ262153 CTV262123:CTV262153 DDR262123:DDR262153 DNN262123:DNN262153 DXJ262123:DXJ262153 EHF262123:EHF262153 ERB262123:ERB262153 FAX262123:FAX262153 FKT262123:FKT262153 FUP262123:FUP262153 GEL262123:GEL262153 GOH262123:GOH262153 GYD262123:GYD262153 HHZ262123:HHZ262153 HRV262123:HRV262153 IBR262123:IBR262153 ILN262123:ILN262153 IVJ262123:IVJ262153 JFF262123:JFF262153 JPB262123:JPB262153 JYX262123:JYX262153 KIT262123:KIT262153 KSP262123:KSP262153 LCL262123:LCL262153 LMH262123:LMH262153 LWD262123:LWD262153 MFZ262123:MFZ262153 MPV262123:MPV262153 MZR262123:MZR262153 NJN262123:NJN262153 NTJ262123:NTJ262153 ODF262123:ODF262153 ONB262123:ONB262153 OWX262123:OWX262153 PGT262123:PGT262153 PQP262123:PQP262153 QAL262123:QAL262153 QKH262123:QKH262153 QUD262123:QUD262153 RDZ262123:RDZ262153 RNV262123:RNV262153 RXR262123:RXR262153 SHN262123:SHN262153 SRJ262123:SRJ262153 TBF262123:TBF262153 TLB262123:TLB262153 TUX262123:TUX262153 UET262123:UET262153 UOP262123:UOP262153 UYL262123:UYL262153 VIH262123:VIH262153 VSD262123:VSD262153 WBZ262123:WBZ262153 WLV262123:WLV262153 WVR262123:WVR262153 JF327659:JF327689 TB327659:TB327689 ACX327659:ACX327689 AMT327659:AMT327689 AWP327659:AWP327689 BGL327659:BGL327689 BQH327659:BQH327689 CAD327659:CAD327689 CJZ327659:CJZ327689 CTV327659:CTV327689 DDR327659:DDR327689 DNN327659:DNN327689 DXJ327659:DXJ327689 EHF327659:EHF327689 ERB327659:ERB327689 FAX327659:FAX327689 FKT327659:FKT327689 FUP327659:FUP327689 GEL327659:GEL327689 GOH327659:GOH327689 GYD327659:GYD327689 HHZ327659:HHZ327689 HRV327659:HRV327689 IBR327659:IBR327689 ILN327659:ILN327689 IVJ327659:IVJ327689 JFF327659:JFF327689 JPB327659:JPB327689 JYX327659:JYX327689 KIT327659:KIT327689 KSP327659:KSP327689 LCL327659:LCL327689 LMH327659:LMH327689 LWD327659:LWD327689 MFZ327659:MFZ327689 MPV327659:MPV327689 MZR327659:MZR327689 NJN327659:NJN327689 NTJ327659:NTJ327689 ODF327659:ODF327689 ONB327659:ONB327689 OWX327659:OWX327689 PGT327659:PGT327689 PQP327659:PQP327689 QAL327659:QAL327689 QKH327659:QKH327689 QUD327659:QUD327689 RDZ327659:RDZ327689 RNV327659:RNV327689 RXR327659:RXR327689 SHN327659:SHN327689 SRJ327659:SRJ327689 TBF327659:TBF327689 TLB327659:TLB327689 TUX327659:TUX327689 UET327659:UET327689 UOP327659:UOP327689 UYL327659:UYL327689 VIH327659:VIH327689 VSD327659:VSD327689 WBZ327659:WBZ327689 WLV327659:WLV327689 WVR327659:WVR327689 JF393195:JF393225 TB393195:TB393225 ACX393195:ACX393225 AMT393195:AMT393225 AWP393195:AWP393225 BGL393195:BGL393225 BQH393195:BQH393225 CAD393195:CAD393225 CJZ393195:CJZ393225 CTV393195:CTV393225 DDR393195:DDR393225 DNN393195:DNN393225 DXJ393195:DXJ393225 EHF393195:EHF393225 ERB393195:ERB393225 FAX393195:FAX393225 FKT393195:FKT393225 FUP393195:FUP393225 GEL393195:GEL393225 GOH393195:GOH393225 GYD393195:GYD393225 HHZ393195:HHZ393225 HRV393195:HRV393225 IBR393195:IBR393225 ILN393195:ILN393225 IVJ393195:IVJ393225 JFF393195:JFF393225 JPB393195:JPB393225 JYX393195:JYX393225 KIT393195:KIT393225 KSP393195:KSP393225 LCL393195:LCL393225 LMH393195:LMH393225 LWD393195:LWD393225 MFZ393195:MFZ393225 MPV393195:MPV393225 MZR393195:MZR393225 NJN393195:NJN393225 NTJ393195:NTJ393225 ODF393195:ODF393225 ONB393195:ONB393225 OWX393195:OWX393225 PGT393195:PGT393225 PQP393195:PQP393225 QAL393195:QAL393225 QKH393195:QKH393225 QUD393195:QUD393225 RDZ393195:RDZ393225 RNV393195:RNV393225 RXR393195:RXR393225 SHN393195:SHN393225 SRJ393195:SRJ393225 TBF393195:TBF393225 TLB393195:TLB393225 TUX393195:TUX393225 UET393195:UET393225 UOP393195:UOP393225 UYL393195:UYL393225 VIH393195:VIH393225 VSD393195:VSD393225 WBZ393195:WBZ393225 WLV393195:WLV393225 WVR393195:WVR393225 JF458731:JF458761 TB458731:TB458761 ACX458731:ACX458761 AMT458731:AMT458761 AWP458731:AWP458761 BGL458731:BGL458761 BQH458731:BQH458761 CAD458731:CAD458761 CJZ458731:CJZ458761 CTV458731:CTV458761 DDR458731:DDR458761 DNN458731:DNN458761 DXJ458731:DXJ458761 EHF458731:EHF458761 ERB458731:ERB458761 FAX458731:FAX458761 FKT458731:FKT458761 FUP458731:FUP458761 GEL458731:GEL458761 GOH458731:GOH458761 GYD458731:GYD458761 HHZ458731:HHZ458761 HRV458731:HRV458761 IBR458731:IBR458761 ILN458731:ILN458761 IVJ458731:IVJ458761 JFF458731:JFF458761 JPB458731:JPB458761 JYX458731:JYX458761 KIT458731:KIT458761 KSP458731:KSP458761 LCL458731:LCL458761 LMH458731:LMH458761 LWD458731:LWD458761 MFZ458731:MFZ458761 MPV458731:MPV458761 MZR458731:MZR458761 NJN458731:NJN458761 NTJ458731:NTJ458761 ODF458731:ODF458761 ONB458731:ONB458761 OWX458731:OWX458761 PGT458731:PGT458761 PQP458731:PQP458761 QAL458731:QAL458761 QKH458731:QKH458761 QUD458731:QUD458761 RDZ458731:RDZ458761 RNV458731:RNV458761 RXR458731:RXR458761 SHN458731:SHN458761 SRJ458731:SRJ458761 TBF458731:TBF458761 TLB458731:TLB458761 TUX458731:TUX458761 UET458731:UET458761 UOP458731:UOP458761 UYL458731:UYL458761 VIH458731:VIH458761 VSD458731:VSD458761 WBZ458731:WBZ458761 WLV458731:WLV458761 WVR458731:WVR458761 JF524267:JF524297 TB524267:TB524297 ACX524267:ACX524297 AMT524267:AMT524297 AWP524267:AWP524297 BGL524267:BGL524297 BQH524267:BQH524297 CAD524267:CAD524297 CJZ524267:CJZ524297 CTV524267:CTV524297 DDR524267:DDR524297 DNN524267:DNN524297 DXJ524267:DXJ524297 EHF524267:EHF524297 ERB524267:ERB524297 FAX524267:FAX524297 FKT524267:FKT524297 FUP524267:FUP524297 GEL524267:GEL524297 GOH524267:GOH524297 GYD524267:GYD524297 HHZ524267:HHZ524297 HRV524267:HRV524297 IBR524267:IBR524297 ILN524267:ILN524297 IVJ524267:IVJ524297 JFF524267:JFF524297 JPB524267:JPB524297 JYX524267:JYX524297 KIT524267:KIT524297 KSP524267:KSP524297 LCL524267:LCL524297 LMH524267:LMH524297 LWD524267:LWD524297 MFZ524267:MFZ524297 MPV524267:MPV524297 MZR524267:MZR524297 NJN524267:NJN524297 NTJ524267:NTJ524297 ODF524267:ODF524297 ONB524267:ONB524297 OWX524267:OWX524297 PGT524267:PGT524297 PQP524267:PQP524297 QAL524267:QAL524297 QKH524267:QKH524297 QUD524267:QUD524297 RDZ524267:RDZ524297 RNV524267:RNV524297 RXR524267:RXR524297 SHN524267:SHN524297 SRJ524267:SRJ524297 TBF524267:TBF524297 TLB524267:TLB524297 TUX524267:TUX524297 UET524267:UET524297 UOP524267:UOP524297 UYL524267:UYL524297 VIH524267:VIH524297 VSD524267:VSD524297 WBZ524267:WBZ524297 WLV524267:WLV524297 WVR524267:WVR524297 JF589803:JF589833 TB589803:TB589833 ACX589803:ACX589833 AMT589803:AMT589833 AWP589803:AWP589833 BGL589803:BGL589833 BQH589803:BQH589833 CAD589803:CAD589833 CJZ589803:CJZ589833 CTV589803:CTV589833 DDR589803:DDR589833 DNN589803:DNN589833 DXJ589803:DXJ589833 EHF589803:EHF589833 ERB589803:ERB589833 FAX589803:FAX589833 FKT589803:FKT589833 FUP589803:FUP589833 GEL589803:GEL589833 GOH589803:GOH589833 GYD589803:GYD589833 HHZ589803:HHZ589833 HRV589803:HRV589833 IBR589803:IBR589833 ILN589803:ILN589833 IVJ589803:IVJ589833 JFF589803:JFF589833 JPB589803:JPB589833 JYX589803:JYX589833 KIT589803:KIT589833 KSP589803:KSP589833 LCL589803:LCL589833 LMH589803:LMH589833 LWD589803:LWD589833 MFZ589803:MFZ589833 MPV589803:MPV589833 MZR589803:MZR589833 NJN589803:NJN589833 NTJ589803:NTJ589833 ODF589803:ODF589833 ONB589803:ONB589833 OWX589803:OWX589833 PGT589803:PGT589833 PQP589803:PQP589833 QAL589803:QAL589833 QKH589803:QKH589833 QUD589803:QUD589833 RDZ589803:RDZ589833 RNV589803:RNV589833 RXR589803:RXR589833 SHN589803:SHN589833 SRJ589803:SRJ589833 TBF589803:TBF589833 TLB589803:TLB589833 TUX589803:TUX589833 UET589803:UET589833 UOP589803:UOP589833 UYL589803:UYL589833 VIH589803:VIH589833 VSD589803:VSD589833 WBZ589803:WBZ589833 WLV589803:WLV589833 WVR589803:WVR589833 JF655339:JF655369 TB655339:TB655369 ACX655339:ACX655369 AMT655339:AMT655369 AWP655339:AWP655369 BGL655339:BGL655369 BQH655339:BQH655369 CAD655339:CAD655369 CJZ655339:CJZ655369 CTV655339:CTV655369 DDR655339:DDR655369 DNN655339:DNN655369 DXJ655339:DXJ655369 EHF655339:EHF655369 ERB655339:ERB655369 FAX655339:FAX655369 FKT655339:FKT655369 FUP655339:FUP655369 GEL655339:GEL655369 GOH655339:GOH655369 GYD655339:GYD655369 HHZ655339:HHZ655369 HRV655339:HRV655369 IBR655339:IBR655369 ILN655339:ILN655369 IVJ655339:IVJ655369 JFF655339:JFF655369 JPB655339:JPB655369 JYX655339:JYX655369 KIT655339:KIT655369 KSP655339:KSP655369 LCL655339:LCL655369 LMH655339:LMH655369 LWD655339:LWD655369 MFZ655339:MFZ655369 MPV655339:MPV655369 MZR655339:MZR655369 NJN655339:NJN655369 NTJ655339:NTJ655369 ODF655339:ODF655369 ONB655339:ONB655369 OWX655339:OWX655369 PGT655339:PGT655369 PQP655339:PQP655369 QAL655339:QAL655369 QKH655339:QKH655369 QUD655339:QUD655369 RDZ655339:RDZ655369 RNV655339:RNV655369 RXR655339:RXR655369 SHN655339:SHN655369 SRJ655339:SRJ655369 TBF655339:TBF655369 TLB655339:TLB655369 TUX655339:TUX655369 UET655339:UET655369 UOP655339:UOP655369 UYL655339:UYL655369 VIH655339:VIH655369 VSD655339:VSD655369 WBZ655339:WBZ655369 WLV655339:WLV655369 WVR655339:WVR655369 JF720875:JF720905 TB720875:TB720905 ACX720875:ACX720905 AMT720875:AMT720905 AWP720875:AWP720905 BGL720875:BGL720905 BQH720875:BQH720905 CAD720875:CAD720905 CJZ720875:CJZ720905 CTV720875:CTV720905 DDR720875:DDR720905 DNN720875:DNN720905 DXJ720875:DXJ720905 EHF720875:EHF720905 ERB720875:ERB720905 FAX720875:FAX720905 FKT720875:FKT720905 FUP720875:FUP720905 GEL720875:GEL720905 GOH720875:GOH720905 GYD720875:GYD720905 HHZ720875:HHZ720905 HRV720875:HRV720905 IBR720875:IBR720905 ILN720875:ILN720905 IVJ720875:IVJ720905 JFF720875:JFF720905 JPB720875:JPB720905 JYX720875:JYX720905 KIT720875:KIT720905 KSP720875:KSP720905 LCL720875:LCL720905 LMH720875:LMH720905 LWD720875:LWD720905 MFZ720875:MFZ720905 MPV720875:MPV720905 MZR720875:MZR720905 NJN720875:NJN720905 NTJ720875:NTJ720905 ODF720875:ODF720905 ONB720875:ONB720905 OWX720875:OWX720905 PGT720875:PGT720905 PQP720875:PQP720905 QAL720875:QAL720905 QKH720875:QKH720905 QUD720875:QUD720905 RDZ720875:RDZ720905 RNV720875:RNV720905 RXR720875:RXR720905 SHN720875:SHN720905 SRJ720875:SRJ720905 TBF720875:TBF720905 TLB720875:TLB720905 TUX720875:TUX720905 UET720875:UET720905 UOP720875:UOP720905 UYL720875:UYL720905 VIH720875:VIH720905 VSD720875:VSD720905 WBZ720875:WBZ720905 WLV720875:WLV720905 WVR720875:WVR720905 JF786411:JF786441 TB786411:TB786441 ACX786411:ACX786441 AMT786411:AMT786441 AWP786411:AWP786441 BGL786411:BGL786441 BQH786411:BQH786441 CAD786411:CAD786441 CJZ786411:CJZ786441 CTV786411:CTV786441 DDR786411:DDR786441 DNN786411:DNN786441 DXJ786411:DXJ786441 EHF786411:EHF786441 ERB786411:ERB786441 FAX786411:FAX786441 FKT786411:FKT786441 FUP786411:FUP786441 GEL786411:GEL786441 GOH786411:GOH786441 GYD786411:GYD786441 HHZ786411:HHZ786441 HRV786411:HRV786441 IBR786411:IBR786441 ILN786411:ILN786441 IVJ786411:IVJ786441 JFF786411:JFF786441 JPB786411:JPB786441 JYX786411:JYX786441 KIT786411:KIT786441 KSP786411:KSP786441 LCL786411:LCL786441 LMH786411:LMH786441 LWD786411:LWD786441 MFZ786411:MFZ786441 MPV786411:MPV786441 MZR786411:MZR786441 NJN786411:NJN786441 NTJ786411:NTJ786441 ODF786411:ODF786441 ONB786411:ONB786441 OWX786411:OWX786441 PGT786411:PGT786441 PQP786411:PQP786441 QAL786411:QAL786441 QKH786411:QKH786441 QUD786411:QUD786441 RDZ786411:RDZ786441 RNV786411:RNV786441 RXR786411:RXR786441 SHN786411:SHN786441 SRJ786411:SRJ786441 TBF786411:TBF786441 TLB786411:TLB786441 TUX786411:TUX786441 UET786411:UET786441 UOP786411:UOP786441 UYL786411:UYL786441 VIH786411:VIH786441 VSD786411:VSD786441 WBZ786411:WBZ786441 WLV786411:WLV786441 WVR786411:WVR786441 JF851947:JF851977 TB851947:TB851977 ACX851947:ACX851977 AMT851947:AMT851977 AWP851947:AWP851977 BGL851947:BGL851977 BQH851947:BQH851977 CAD851947:CAD851977 CJZ851947:CJZ851977 CTV851947:CTV851977 DDR851947:DDR851977 DNN851947:DNN851977 DXJ851947:DXJ851977 EHF851947:EHF851977 ERB851947:ERB851977 FAX851947:FAX851977 FKT851947:FKT851977 FUP851947:FUP851977 GEL851947:GEL851977 GOH851947:GOH851977 GYD851947:GYD851977 HHZ851947:HHZ851977 HRV851947:HRV851977 IBR851947:IBR851977 ILN851947:ILN851977 IVJ851947:IVJ851977 JFF851947:JFF851977 JPB851947:JPB851977 JYX851947:JYX851977 KIT851947:KIT851977 KSP851947:KSP851977 LCL851947:LCL851977 LMH851947:LMH851977 LWD851947:LWD851977 MFZ851947:MFZ851977 MPV851947:MPV851977 MZR851947:MZR851977 NJN851947:NJN851977 NTJ851947:NTJ851977 ODF851947:ODF851977 ONB851947:ONB851977 OWX851947:OWX851977 PGT851947:PGT851977 PQP851947:PQP851977 QAL851947:QAL851977 QKH851947:QKH851977 QUD851947:QUD851977 RDZ851947:RDZ851977 RNV851947:RNV851977 RXR851947:RXR851977 SHN851947:SHN851977 SRJ851947:SRJ851977 TBF851947:TBF851977 TLB851947:TLB851977 TUX851947:TUX851977 UET851947:UET851977 UOP851947:UOP851977 UYL851947:UYL851977 VIH851947:VIH851977 VSD851947:VSD851977 WBZ851947:WBZ851977 WLV851947:WLV851977 WVR851947:WVR851977 JF917483:JF917513 TB917483:TB917513 ACX917483:ACX917513 AMT917483:AMT917513 AWP917483:AWP917513 BGL917483:BGL917513 BQH917483:BQH917513 CAD917483:CAD917513 CJZ917483:CJZ917513 CTV917483:CTV917513 DDR917483:DDR917513 DNN917483:DNN917513 DXJ917483:DXJ917513 EHF917483:EHF917513 ERB917483:ERB917513 FAX917483:FAX917513 FKT917483:FKT917513 FUP917483:FUP917513 GEL917483:GEL917513 GOH917483:GOH917513 GYD917483:GYD917513 HHZ917483:HHZ917513 HRV917483:HRV917513 IBR917483:IBR917513 ILN917483:ILN917513 IVJ917483:IVJ917513 JFF917483:JFF917513 JPB917483:JPB917513 JYX917483:JYX917513 KIT917483:KIT917513 KSP917483:KSP917513 LCL917483:LCL917513 LMH917483:LMH917513 LWD917483:LWD917513 MFZ917483:MFZ917513 MPV917483:MPV917513 MZR917483:MZR917513 NJN917483:NJN917513 NTJ917483:NTJ917513 ODF917483:ODF917513 ONB917483:ONB917513 OWX917483:OWX917513 PGT917483:PGT917513 PQP917483:PQP917513 QAL917483:QAL917513 QKH917483:QKH917513 QUD917483:QUD917513 RDZ917483:RDZ917513 RNV917483:RNV917513 RXR917483:RXR917513 SHN917483:SHN917513 SRJ917483:SRJ917513 TBF917483:TBF917513 TLB917483:TLB917513 TUX917483:TUX917513 UET917483:UET917513 UOP917483:UOP917513 UYL917483:UYL917513 VIH917483:VIH917513 VSD917483:VSD917513 WBZ917483:WBZ917513 WLV917483:WLV917513 WVR917483:WVR917513 JF983019:JF983049 TB983019:TB983049 ACX983019:ACX983049 AMT983019:AMT983049 AWP983019:AWP983049 BGL983019:BGL983049 BQH983019:BQH983049 CAD983019:CAD983049 CJZ983019:CJZ983049 CTV983019:CTV983049 DDR983019:DDR983049 DNN983019:DNN983049 DXJ983019:DXJ983049 EHF983019:EHF983049 ERB983019:ERB983049 FAX983019:FAX983049 FKT983019:FKT983049 FUP983019:FUP983049 GEL983019:GEL983049 GOH983019:GOH983049 GYD983019:GYD983049 HHZ983019:HHZ983049 HRV983019:HRV983049 IBR983019:IBR983049 ILN983019:ILN983049 IVJ983019:IVJ983049 JFF983019:JFF983049 JPB983019:JPB983049 JYX983019:JYX983049 KIT983019:KIT983049 KSP983019:KSP983049 LCL983019:LCL983049 LMH983019:LMH983049 LWD983019:LWD983049 MFZ983019:MFZ983049 MPV983019:MPV983049 MZR983019:MZR983049 NJN983019:NJN983049 NTJ983019:NTJ983049 ODF983019:ODF983049 ONB983019:ONB983049 OWX983019:OWX983049 PGT983019:PGT983049 PQP983019:PQP983049 QAL983019:QAL983049 QKH983019:QKH983049 QUD983019:QUD983049 RDZ983019:RDZ983049 RNV983019:RNV983049 RXR983019:RXR983049 SHN983019:SHN983049 SRJ983019:SRJ983049 TBF983019:TBF983049 TLB983019:TLB983049 TUX983019:TUX983049 UET983019:UET983049 UOP983019:UOP983049 UYL983019:UYL983049 VIH983019:VIH983049 VSD983019:VSD983049 WBZ983019:WBZ983049 WLV983019:WLV983049 WVR983019:WVR983049 G65515:H65545 G131051:H131081 G196587:H196617 G262123:H262153 G327659:H327689 G393195:H393225 G458731:H458761 G524267:H524297 G589803:H589833 G655339:H655369 G720875:H720905 G786411:H786441 G851947:H851977 G917483:H917513 G983019:H983049 JF4:JF20 TB4:TB20 ACX4:ACX20 AMT4:AMT20 AWP4:AWP20 BGL4:BGL20 BQH4:BQH20 CAD4:CAD20 CJZ4:CJZ20 CTV4:CTV20 DDR4:DDR20 DNN4:DNN20 DXJ4:DXJ20 EHF4:EHF20 ERB4:ERB20 FAX4:FAX20 FKT4:FKT20 FUP4:FUP20 GEL4:GEL20 GOH4:GOH20 GYD4:GYD20 HHZ4:HHZ20 HRV4:HRV20 IBR4:IBR20 ILN4:ILN20 IVJ4:IVJ20 JFF4:JFF20 JPB4:JPB20 JYX4:JYX20 KIT4:KIT20 KSP4:KSP20 LCL4:LCL20 LMH4:LMH20 LWD4:LWD20 MFZ4:MFZ20 MPV4:MPV20 MZR4:MZR20 NJN4:NJN20 NTJ4:NTJ20 ODF4:ODF20 ONB4:ONB20 OWX4:OWX20 PGT4:PGT20 PQP4:PQP20 QAL4:QAL20 QKH4:QKH20 QUD4:QUD20 RDZ4:RDZ20 RNV4:RNV20 RXR4:RXR20 SHN4:SHN20 SRJ4:SRJ20 TBF4:TBF20 TLB4:TLB20 TUX4:TUX20 UET4:UET20 UOP4:UOP20 UYL4:UYL20 VIH4:VIH20 VSD4:VSD20 WBZ4:WBZ20 WLV4:WLV20 WVR4:WVR20" xr:uid="{00000000-0002-0000-0200-000011000000}">
       <formula1>"Primaria Incompleta,Primaria Completa,Secundaria Incompleta,Secundaria Completa,Técnico,Tecnólogo,Profesional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G8" xr:uid="{00000000-0002-0000-0200-000012000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4" xr:uid="{00000000-0002-0000-0200-000012000000}">
       <formula1>$E$140:$E$146</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4:N8" xr:uid="{00000000-0002-0000-0200-000013000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4" xr:uid="{00000000-0002-0000-0200-000013000000}">
       <formula1>$E$179:$E$182</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4:M8" xr:uid="{00000000-0002-0000-0200-000014000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4" xr:uid="{00000000-0002-0000-0200-000014000000}">
       <formula1>$E$171:$E$177</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4:U8" xr:uid="{00000000-0002-0000-0200-000015000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4" xr:uid="{00000000-0002-0000-0200-000015000000}">
       <formula1>$E$218:$E$223</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4:T8" xr:uid="{00000000-0002-0000-0200-000016000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4" xr:uid="{00000000-0002-0000-0200-000016000000}">
       <formula1>$E$210:$E$216</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R4:R8" xr:uid="{00000000-0002-0000-0200-000017000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R4" xr:uid="{00000000-0002-0000-0200-000017000000}">
       <formula1>$E$205:$E$208</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P4:P8" xr:uid="{00000000-0002-0000-0200-000018000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P4" xr:uid="{00000000-0002-0000-0200-000018000000}">
       <formula1>$E$191:$E$198</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O4:O8" xr:uid="{00000000-0002-0000-0200-000019000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O4" xr:uid="{00000000-0002-0000-0200-000019000000}">
       <formula1>$E$184:$E$189</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L8" xr:uid="{00000000-0002-0000-0200-00001A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4" xr:uid="{00000000-0002-0000-0200-00001A000000}">
       <formula1>$E$229:$E$231</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K8" xr:uid="{00000000-0002-0000-0200-00001B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4" xr:uid="{00000000-0002-0000-0200-00001B000000}">
       <formula1>$E$161:$E$165</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J8" xr:uid="{00000000-0002-0000-0200-00001C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4" xr:uid="{00000000-0002-0000-0200-00001C000000}">
       <formula1>$E$154:$E$159</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9" xr:uid="{00000000-0002-0000-0200-00001D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 G9" xr:uid="{00000000-0002-0000-0200-00001D000000}">
       <formula1>$E$150:$E$156</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10" xr:uid="{00000000-0002-0000-0200-00001E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6 G10" xr:uid="{00000000-0002-0000-0200-00001E000000}">
       <formula1>$E$149:$E$155</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:T20" xr:uid="{00000000-0002-0000-0200-000022000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8" xr:uid="{00000000-0002-0000-0200-00001F000000}">
+      <formula1>$E$147:$E$153</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N8" xr:uid="{00000000-0002-0000-0200-000020000000}">
+      <formula1>$E$186:$E$189</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8" xr:uid="{00000000-0002-0000-0200-000021000000}">
+      <formula1>$E$178:$E$184</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T20" xr:uid="{00000000-0002-0000-0200-000022000000}">
       <formula1>"Sin hijos, 1 hijo,2 hijos,3 hijos,4 Hijos, más de 6 hijos"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P9:P20" xr:uid="{00000000-0002-0000-0200-000023000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5:P20" xr:uid="{00000000-0002-0000-0200-000023000000}">
       <formula1>"AB+,AB-,A+,A-,B+,B-,O+,O-"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9" xr:uid="{00000000-0002-0000-0200-000024000000}">
@@ -11789,15 +11545,8 @@
       <formula1>$E$187:$E$190</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="X4" r:id="rId1" xr:uid="{BB2ECF9D-0DC3-4734-B15E-1CAC87B35D11}"/>
-    <hyperlink ref="X5" r:id="rId2" xr:uid="{A576F27C-6D9C-4039-8C3D-A965E819CF62}"/>
-    <hyperlink ref="X6" r:id="rId3" xr:uid="{5D6F39B8-EDD4-48D5-ABBD-9408C420FFE4}"/>
-    <hyperlink ref="X7" r:id="rId4" xr:uid="{EA55B677-B724-41CB-8B3D-62B6CA1A5206}"/>
-    <hyperlink ref="X8" r:id="rId5" xr:uid="{3C25CD9B-A220-4212-A315-5D99D43BDD18}"/>
-  </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="138" scale="70" orientation="landscape" r:id="rId6"/>
+  <pageSetup paperSize="138" scale="70" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">

</xml_diff>